<commit_message>
Updated testing data for 2020-05-02
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="498">
   <si>
     <t xml:space="preserve">Entity</t>
   </si>
@@ -83,7 +83,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/04/coronavirus-covid-19-at-a-glance-30-april-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/05/coronavirus-covid-19-at-a-glance-1-may-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200501145322/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200502151038/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -124,7 +124,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200501145324/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200502151040/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -166,7 +166,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-28-krasavika-vypisanyya-1993-patsyenta/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-vyzdoroveli-i-vypisany-2918-patsientov/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -220,7 +220,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200501112313/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200502151045/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -240,7 +240,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200501081525/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200501173328/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -316,7 +316,7 @@
     <t xml:space="preserve">Croatia - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200501145333/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200502151051/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -416,7 +416,7 @@
     <t xml:space="preserve">Government of El Salvador</t>
   </si>
   <si>
-    <t xml:space="preserve">updated at 11:08pm local time on 2020-04-29.</t>
+    <t xml:space="preserve">updated at 10:58am local time on 2020-05-01.</t>
   </si>
   <si>
     <t xml:space="preserve">The government of El Salvador publishes an online dashboard with figures and graphs about the epidemic, including the number of tests performed ("pruebas COVID19 realizadas hasta hoy"). No information is given on the geographical scope and number of labs included.</t>
@@ -560,16 +560,16 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200502/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National Organization of Public Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The National Organization of Public Health</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://eody.gov.gr/epidimiologika-statistika-dedomena/imerisies-ektheseis-covid-19/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">National Organization of Public Health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Made available on Github by Covid-19 Response Greece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The National Organization of Public Health</t>
   </si>
   <si>
     <t xml:space="preserve">The Greek National Organization of Public Health publishes daily COVID-19 reports on confirmed cases, deaths and samples tested. 
@@ -582,7 +582,7 @@
     <t xml:space="preserve">Hong Kong - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://data.gov.hk/en-data/dataset/hk-dh-chpsebcddr-novel-infectious-agent/resource/a88635eb-1a6d-4dba-952f-f37cb165c24f</t>
+    <t xml:space="preserve">https://data.gov.hk/en-data/dataset/hk-dh-chpsebcddr-novel-infectious-agent/resource/000cc801-6294-4ea9-b505-f5f1633a53b9</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Health</t>
@@ -813,7 +813,7 @@
     <t xml:space="preserve">Kenya - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1255840194357604352</t>
+    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1256225780822093824</t>
   </si>
   <si>
     <t xml:space="preserve">Kenya Ministry of Health</t>
@@ -848,7 +848,7 @@
     <t xml:space="preserve">Lithuania - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200501082406/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200502151129/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -861,7 +861,7 @@
     <t xml:space="preserve">Luxembourg - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200502161051/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg Government situation update</t>
@@ -879,7 +879,7 @@
     <t xml:space="preserve">Malaysia - cases tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200501145427/https://www.moh.gov.my/index.php/pages/view/2019-ncov-wuhan</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200502151137/https://www.moh.gov.my/index.php/pages/view/2019-ncov-wuhan</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -940,6 +940,9 @@
     <t xml:space="preserve">Myanmar Ministry of Health and Sports</t>
   </si>
   <si>
+    <t xml:space="preserve">This figure is taken from the live dashboard and should be updated using the PDF Situation Report once it is available</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://mohs.gov.mm/Home</t>
   </si>
   <si>
@@ -970,10 +973,10 @@
     <t xml:space="preserve">Netherlands - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-04/COVID-19_WebSite_rapport_20200430_1215.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 30 April 2020 update</t>
+    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-05/COVID-19_WebSite_rapport_20200501_1150.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 1 May 2020 update</t>
   </si>
   <si>
     <t xml:space="preserve">Dutch National Institute for Public Health and the Environment</t>
@@ -1003,7 +1006,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200430195121/http://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200501155337/http://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1042,7 +1045,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200501082450/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200502151159/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1099,7 +1102,7 @@
     <t xml:space="preserve">Peru - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/143118-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-36-976-en-el-peru-comunicado-n-82</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/143593-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-40-459-en-el-peru-comunicado-n-84</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1173,7 +1176,7 @@
     <t xml:space="preserve">Qatar - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200501145525/https://www.moph.gov.qa/english/Pages/Coronavirus2019.aspx</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200502151207/https://www.moph.gov.qa/english/Pages/Coronavirus2019.aspx</t>
   </si>
   <si>
     <t xml:space="preserve">Qatar Ministry of Public Health</t>
@@ -1205,7 +1208,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14368</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14371</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1222,7 +1225,7 @@
     <t xml:space="preserve">Rwanda - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1255573506294767619</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1255954649879851009</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1295,7 +1298,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200501082509/https://www.korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200502151233/https://www.korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Center of Health Information and the Office of the Government of the Slovak Republic</t>
@@ -1360,7 +1363,7 @@
     <t xml:space="preserve">South Korea - cases tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367062&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367066&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1437,7 +1440,7 @@
     <t xml:space="preserve">Taiwan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/Xu8MOuQTDD1uAXvY9riyRw?typeid=9</t>
+    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/bJVsQHE6lCY1CMTi1gMcpQ?typeid=9</t>
   </si>
   <si>
     <t xml:space="preserve">Taiwan Centers for Disease Control (CDC)</t>
@@ -1457,7 +1460,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200501145612/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200502151250/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1498,10 +1501,13 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
+    <t xml:space="preserve">https://web.archive.org/web/20200501173455/https://covid19.saglik.gov.tr/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turkish Ministry of Health</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://covid19.saglik.gov.tr/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turkish Ministry of Health</t>
   </si>
   <si>
     <t xml:space="preserve">The total number of tests.</t>
@@ -1536,7 +1542,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200430155239/https://covid19.gov.ua/en/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200502151255/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1555,7 +1561,7 @@
     <t xml:space="preserve">United Kingdom - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200430190452/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200501173458/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
@@ -1571,13 +1577,17 @@
 Pillar 2: swab testing for health, social care and other essential workers and their households
 Pillar 4: serology and swab testing: a national surveillance programme supported by PHE, ONS and Biobank to learn more about the prevalence and spread of the virus
 As of 30 April, there were no people tested under Pillar 4 included in this series.
-(As discussed in the Govenerment's [national testing strategy document](https://www.gov.uk/government/publications/coronavirus-covid-19-scaling-up-testing-programmes), Pillar 3 relates to antibody tests – but these are currently not reported within the figures above).</t>
+(As discussed in the Govenerment's [national testing strategy document](https://www.gov.uk/government/publications/coronavirus-covid-19-scaling-up-testing-programmes), Pillar 3 relates to antibody tests – but these are currently not reported within the figures above).
+The Health Service Journal highlighted in [an article published on 1 May 2020](https://www.hsj.co.uk/quality-and-performance/revealed-how-government-changed-the-rules-to-hit-100000-tests-target/7027544.article) that “the Department of Health and Social Care [was] now including tests that have been posted or delivered to people’s homes in its figures. This means tests which are sent to people are counted before the recipient has provided and returned their sample to a laboratory.” No data is made available by the UK government on how many of these mailed tests have been returned and processed, but this could represent a significant number for recent days. As far as we know, the “People tested” figures are not affected by this issue.</t>
   </si>
   <si>
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200430190453/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200501173558/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of tests performed, including tests posted or delivered but not yet returned and/or processed.</t>
   </si>
   <si>
     <t xml:space="preserve">A time series is not yet released. The figures we provide relate to the daily updates provided for the cumulative total and daily number of tests performed. It is not clear the exact date that the cumulative figures date back to.
@@ -1586,8 +1596,9 @@
 Pillar 1: swab testing in PHE labs and NHS hospitals for those with a clinical need, and health and care workers
 Pillar 2: swab testing for health, social care and other essential workers and their households
 Pillar 4: serology and swab testing: a national surveillance programme supported by PHE, ONS and Biobank to learn more about the prevalence and spread of the virus
- As of 30 April, around 10% of the total number of tests were reported under Pillar 4. How these further breakdown between serology and swab testing is not known.
-As discussed in the Govenerment's [national testing strategy document](https://www.gov.uk/government/publications/coronavirus-covid-19-scaling-up-testing-programmes), Pillar 3 relates to antibody tests – but these are currently not reported within the figures above.</t>
+As of 30 April, around 10% of the total number of tests were reported under Pillar 4. How these further breakdown between serology and swab testing is not known.
+As discussed in the Govenerment's [national testing strategy document](https://www.gov.uk/government/publications/coronavirus-covid-19-scaling-up-testing-programmes), Pillar 3 relates to antibody tests – but these are currently not reported within the figures above.
+The Health Service Journal highlighted in [an article published on 1 May 2020](https://www.hsj.co.uk/quality-and-performance/revealed-how-government-changed-the-rules-to-hit-100000-tests-target/7027544.article) that “the Department of Health and Social Care [was] now including tests that have been posted or delivered to people’s homes in its figures. This means tests which are sent to people are counted before the recipient has provided and returned their sample to a laboratory.” No data is made available by the UK government on how many of these mailed tests have been returned and processed, but this could represent a significant number for recent days. As far as we know, the “People tested” figures are not affected by this issue.</t>
   </si>
   <si>
     <t xml:space="preserve">United States - inconsistent units (COVID Tracking Project)</t>
@@ -1641,7 +1652,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-11</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-12</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -1674,7 +1685,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1255674098446974983</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1256124142803353600</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -2117,7 +2128,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
@@ -2127,25 +2138,25 @@
       </c>
       <c r="E3"/>
       <c r="F3" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G3" t="n">
-        <v>563641</v>
+        <v>588868</v>
       </c>
       <c r="H3" t="n">
-        <v>22.104</v>
+        <v>23.093</v>
       </c>
       <c r="I3" t="n">
-        <v>19231</v>
+        <v>25227</v>
       </c>
       <c r="J3" t="n">
-        <v>0.754</v>
+        <v>0.989</v>
       </c>
       <c r="K3" t="n">
-        <v>15526</v>
+        <v>19396.333</v>
       </c>
       <c r="L3" t="n">
-        <v>0.609</v>
+        <v>0.76</v>
       </c>
       <c r="M3" t="s">
         <v>24</v>
@@ -2165,7 +2176,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -2175,25 +2186,25 @@
       </c>
       <c r="E4"/>
       <c r="F4" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G4" t="n">
-        <v>264079</v>
+        <v>269619</v>
       </c>
       <c r="H4" t="n">
-        <v>29.321</v>
+        <v>29.936</v>
       </c>
       <c r="I4" t="n">
-        <v>7680</v>
+        <v>5540</v>
       </c>
       <c r="J4" t="n">
-        <v>0.853</v>
+        <v>0.615</v>
       </c>
       <c r="K4" t="n">
-        <v>8167</v>
+        <v>7288.333</v>
       </c>
       <c r="L4" t="n">
-        <v>0.907</v>
+        <v>0.809</v>
       </c>
       <c r="M4" t="s">
         <v>30</v>
@@ -2213,7 +2224,7 @@
         <v>34</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -2223,25 +2234,25 @@
       </c>
       <c r="E5"/>
       <c r="F5" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G5" t="n">
-        <v>134082</v>
+        <v>138278</v>
       </c>
       <c r="H5" t="n">
-        <v>78.798</v>
+        <v>81.264</v>
       </c>
       <c r="I5" t="n">
-        <v>4388</v>
+        <v>4196</v>
       </c>
       <c r="J5" t="n">
-        <v>2.579</v>
+        <v>2.466</v>
       </c>
       <c r="K5" t="n">
-        <v>4125.333</v>
+        <v>3791</v>
       </c>
       <c r="L5" t="n">
-        <v>2.424</v>
+        <v>2.228</v>
       </c>
       <c r="M5" t="s">
         <v>37</v>
@@ -2261,7 +2272,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C6" t="s">
         <v>42</v>
@@ -2271,25 +2282,25 @@
       </c>
       <c r="E6"/>
       <c r="F6" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G6" t="n">
-        <v>64666</v>
+        <v>70239</v>
       </c>
       <c r="H6" t="n">
-        <v>0.393</v>
+        <v>0.426</v>
       </c>
       <c r="I6" t="n">
-        <v>4965</v>
+        <v>5573</v>
       </c>
       <c r="J6" t="n">
-        <v>0.03</v>
+        <v>0.034</v>
       </c>
       <c r="K6" t="n">
-        <v>4789.667</v>
+        <v>5168.667</v>
       </c>
       <c r="L6" t="n">
-        <v>0.029</v>
+        <v>0.031</v>
       </c>
       <c r="M6" t="s">
         <v>43</v>
@@ -2309,7 +2320,7 @@
         <v>47</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>43949</v>
+        <v>43952</v>
       </c>
       <c r="C7" t="s">
         <v>48</v>
@@ -2319,26 +2330,18 @@
       </c>
       <c r="E7"/>
       <c r="F7" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G7" t="n">
-        <v>161028</v>
+        <v>186262</v>
       </c>
       <c r="H7" t="n">
-        <v>17.041</v>
-      </c>
-      <c r="I7" t="n">
-        <v>7228</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.765</v>
-      </c>
-      <c r="K7" t="n">
-        <v>7244.333</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.767</v>
-      </c>
+        <v>19.712</v>
+      </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
       <c r="M7" t="s">
         <v>49</v>
       </c>
@@ -2357,7 +2360,7 @@
         <v>52</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>43950</v>
+        <v>43951</v>
       </c>
       <c r="C8" t="s">
         <v>53</v>
@@ -2367,25 +2370,25 @@
       </c>
       <c r="E8"/>
       <c r="F8" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G8" t="n">
-        <v>306936</v>
+        <v>327653</v>
       </c>
       <c r="H8" t="n">
-        <v>26.484</v>
+        <v>28.271</v>
       </c>
       <c r="I8" t="n">
-        <v>19120</v>
+        <v>20718</v>
       </c>
       <c r="J8" t="n">
-        <v>1.65</v>
+        <v>1.788</v>
       </c>
       <c r="K8" t="n">
-        <v>16904.333</v>
+        <v>19130</v>
       </c>
       <c r="L8" t="n">
-        <v>1.459</v>
+        <v>1.651</v>
       </c>
       <c r="M8" t="s">
         <v>54</v>
@@ -2405,7 +2408,7 @@
         <v>58</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C9" t="s">
         <v>59</v>
@@ -2417,21 +2420,21 @@
         <v>60</v>
       </c>
       <c r="F9" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G9" t="n">
-        <v>6551</v>
+        <v>6613</v>
       </c>
       <c r="H9" t="n">
-        <v>0.561</v>
+        <v>0.567</v>
       </c>
       <c r="I9"/>
       <c r="J9" t="n">
-        <v>0.012</v>
+        <v>0.005</v>
       </c>
       <c r="K9"/>
       <c r="L9" t="n">
-        <v>0.016</v>
+        <v>0.014</v>
       </c>
       <c r="M9" t="s">
         <v>36</v>
@@ -2451,7 +2454,7 @@
         <v>64</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C10" t="s">
         <v>65</v>
@@ -2461,16 +2464,20 @@
       </c>
       <c r="E10"/>
       <c r="F10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G10" t="n">
-        <v>46510</v>
+        <v>47636</v>
       </c>
       <c r="H10" t="n">
-        <v>6.694</v>
-      </c>
-      <c r="I10"/>
-      <c r="J10"/>
+        <v>6.856</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1126</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.162</v>
+      </c>
       <c r="K10"/>
       <c r="L10"/>
       <c r="M10" t="s">
@@ -2504,22 +2511,22 @@
         <v>44</v>
       </c>
       <c r="G11" t="n">
-        <v>806449</v>
+        <v>832222</v>
       </c>
       <c r="H11" t="n">
-        <v>21.367</v>
+        <v>22.05</v>
       </c>
       <c r="I11" t="n">
-        <v>18166</v>
+        <v>43939</v>
       </c>
       <c r="J11" t="n">
-        <v>0.481</v>
+        <v>1.164</v>
       </c>
       <c r="K11" t="n">
-        <v>21863.333</v>
+        <v>30454.333</v>
       </c>
       <c r="L11" t="n">
-        <v>0.579</v>
+        <v>0.807</v>
       </c>
       <c r="M11" t="s">
         <v>72</v>
@@ -2539,7 +2546,7 @@
         <v>76</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C12" t="s">
         <v>77</v>
@@ -2551,25 +2558,25 @@
         <v>78</v>
       </c>
       <c r="F12" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G12" t="n">
-        <v>180517</v>
+        <v>189433</v>
       </c>
       <c r="H12" t="n">
-        <v>9.443</v>
+        <v>9.91</v>
       </c>
       <c r="I12" t="n">
-        <v>7898</v>
+        <v>8916</v>
       </c>
       <c r="J12" t="n">
-        <v>0.413</v>
+        <v>0.466</v>
       </c>
       <c r="K12" t="n">
-        <v>6427.333</v>
+        <v>7756</v>
       </c>
       <c r="L12" t="n">
-        <v>0.336</v>
+        <v>0.406</v>
       </c>
       <c r="M12" t="s">
         <v>79</v>
@@ -2589,7 +2596,7 @@
         <v>82</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C13" t="s">
         <v>83</v>
@@ -2602,22 +2609,22 @@
         <v>58</v>
       </c>
       <c r="G13" t="n">
-        <v>104657</v>
+        <v>108950</v>
       </c>
       <c r="H13" t="n">
-        <v>2.057</v>
+        <v>2.141</v>
       </c>
       <c r="I13" t="n">
-        <v>2520</v>
+        <v>4293</v>
       </c>
       <c r="J13" t="n">
-        <v>0.05</v>
+        <v>0.084</v>
       </c>
       <c r="K13" t="n">
-        <v>3073</v>
+        <v>4621.667</v>
       </c>
       <c r="L13" t="n">
-        <v>0.06</v>
+        <v>0.091</v>
       </c>
       <c r="M13" t="s">
         <v>84</v>
@@ -2637,7 +2644,7 @@
         <v>88</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C14" t="s">
         <v>89</v>
@@ -2647,21 +2654,25 @@
       </c>
       <c r="E14"/>
       <c r="F14" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G14" t="n">
-        <v>9335</v>
+        <v>9502</v>
       </c>
       <c r="H14" t="n">
-        <v>1.833</v>
-      </c>
-      <c r="I14"/>
+        <v>1.865</v>
+      </c>
+      <c r="I14" t="n">
+        <v>167</v>
+      </c>
       <c r="J14" t="n">
-        <v>0.021</v>
-      </c>
-      <c r="K14"/>
+        <v>0.033</v>
+      </c>
+      <c r="K14" t="n">
+        <v>171</v>
+      </c>
       <c r="L14" t="n">
-        <v>0.027</v>
+        <v>0.034</v>
       </c>
       <c r="M14" t="s">
         <v>90</v>
@@ -2681,7 +2692,7 @@
         <v>93</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>43951</v>
+        <v>43953</v>
       </c>
       <c r="C15" t="s">
         <v>94</v>
@@ -2691,26 +2702,18 @@
       </c>
       <c r="E15"/>
       <c r="F15" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G15" t="n">
-        <v>36917</v>
+        <v>37557</v>
       </c>
       <c r="H15" t="n">
-        <v>8.993</v>
-      </c>
-      <c r="I15" t="n">
-        <v>2441</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0.595</v>
-      </c>
-      <c r="K15" t="n">
-        <v>1366.667</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0.333</v>
-      </c>
+        <v>9.148</v>
+      </c>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
       <c r="M15" t="s">
         <v>95</v>
       </c>
@@ -2729,7 +2732,7 @@
         <v>99</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>43950</v>
+        <v>43951</v>
       </c>
       <c r="C16" t="s">
         <v>100</v>
@@ -2741,25 +2744,25 @@
         <v>102</v>
       </c>
       <c r="F16" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G16" t="n">
-        <v>47347</v>
+        <v>49409</v>
       </c>
       <c r="H16" t="n">
-        <v>4.18</v>
+        <v>4.362</v>
       </c>
       <c r="I16" t="n">
-        <v>2003</v>
+        <v>2062</v>
       </c>
       <c r="J16" t="n">
-        <v>0.177</v>
+        <v>0.182</v>
       </c>
       <c r="K16" t="n">
-        <v>1898.667</v>
+        <v>1967</v>
       </c>
       <c r="L16" t="n">
-        <v>0.168</v>
+        <v>0.174</v>
       </c>
       <c r="M16" t="s">
         <v>101</v>
@@ -2779,7 +2782,7 @@
         <v>105</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C17" t="s">
         <v>106</v>
@@ -2789,25 +2792,25 @@
       </c>
       <c r="E17"/>
       <c r="F17" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G17" t="n">
-        <v>249634</v>
+        <v>253826</v>
       </c>
       <c r="H17" t="n">
-        <v>23.311</v>
+        <v>23.702</v>
       </c>
       <c r="I17" t="n">
-        <v>7250</v>
+        <v>4192</v>
       </c>
       <c r="J17" t="n">
-        <v>0.677</v>
+        <v>0.391</v>
       </c>
       <c r="K17" t="n">
-        <v>7771.333</v>
+        <v>6253.667</v>
       </c>
       <c r="L17" t="n">
-        <v>0.726</v>
+        <v>0.584</v>
       </c>
       <c r="M17" t="s">
         <v>36</v>
@@ -2923,7 +2926,7 @@
         <v>122</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>43950</v>
+        <v>43952</v>
       </c>
       <c r="C20" t="s">
         <v>123</v>
@@ -2935,13 +2938,13 @@
         <v>125</v>
       </c>
       <c r="F20" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G20" t="n">
-        <v>24057</v>
+        <v>25492</v>
       </c>
       <c r="H20" t="n">
-        <v>3.709</v>
+        <v>3.93</v>
       </c>
       <c r="I20"/>
       <c r="J20"/>
@@ -2965,7 +2968,7 @@
         <v>127</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C21" t="s">
         <v>128</v>
@@ -2975,25 +2978,25 @@
       </c>
       <c r="E21"/>
       <c r="F21" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G21" t="n">
-        <v>53767</v>
+        <v>54464</v>
       </c>
       <c r="H21" t="n">
-        <v>40.532</v>
+        <v>41.057</v>
       </c>
       <c r="I21" t="n">
-        <v>1031</v>
+        <v>697</v>
       </c>
       <c r="J21" t="n">
-        <v>0.777</v>
+        <v>0.525</v>
       </c>
       <c r="K21" t="n">
-        <v>1421</v>
+        <v>1096.333</v>
       </c>
       <c r="L21" t="n">
-        <v>1.071</v>
+        <v>0.826</v>
       </c>
       <c r="M21" t="s">
         <v>130</v>
@@ -3189,7 +3192,7 @@
         <v>157</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>43949</v>
+        <v>43952</v>
       </c>
       <c r="C26" t="s">
         <v>158</v>
@@ -3199,20 +3202,16 @@
       </c>
       <c r="E26"/>
       <c r="F26" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G26" t="n">
-        <v>113497</v>
+        <v>117049</v>
       </c>
       <c r="H26" t="n">
-        <v>3.653</v>
-      </c>
-      <c r="I26" t="n">
-        <v>7407</v>
-      </c>
-      <c r="J26" t="n">
-        <v>0.238</v>
-      </c>
+        <v>3.767</v>
+      </c>
+      <c r="I26"/>
+      <c r="J26"/>
       <c r="K26"/>
       <c r="L26"/>
       <c r="M26" t="s">
@@ -3233,7 +3232,7 @@
         <v>164</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>43951</v>
+        <v>43953</v>
       </c>
       <c r="C27" t="s">
         <v>165</v>
@@ -3241,35 +3240,29 @@
       <c r="D27" t="s">
         <v>166</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27"/>
+      <c r="F27" t="n">
+        <v>42</v>
+      </c>
+      <c r="G27" t="n">
+        <v>78207</v>
+      </c>
+      <c r="H27" t="n">
+        <v>7.503</v>
+      </c>
+      <c r="I27"/>
+      <c r="J27" t="n">
+        <v>0.092</v>
+      </c>
+      <c r="K27"/>
+      <c r="L27" t="n">
+        <v>0.195</v>
+      </c>
+      <c r="M27" t="s">
         <v>167</v>
       </c>
-      <c r="F27" t="n">
-        <v>40</v>
-      </c>
-      <c r="G27" t="n">
-        <v>75170</v>
-      </c>
-      <c r="H27" t="n">
-        <v>7.212</v>
-      </c>
-      <c r="I27" t="n">
-        <v>3040</v>
-      </c>
-      <c r="J27" t="n">
-        <v>0.292</v>
-      </c>
-      <c r="K27" t="n">
-        <v>3025.333</v>
-      </c>
-      <c r="L27" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>168</v>
-      </c>
-      <c r="N27" t="s">
-        <v>165</v>
       </c>
       <c r="O27" t="s">
         <v>74</v>
@@ -3323,7 +3316,7 @@
         <v>176</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C29" t="s">
         <v>177</v>
@@ -3335,25 +3328,25 @@
         <v>179</v>
       </c>
       <c r="F29" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G29" t="n">
-        <v>76331</v>
+        <v>79551</v>
       </c>
       <c r="H29" t="n">
-        <v>7.901</v>
+        <v>8.235</v>
       </c>
       <c r="I29" t="n">
-        <v>3380</v>
+        <v>3220</v>
       </c>
       <c r="J29" t="n">
-        <v>0.35</v>
+        <v>0.333</v>
       </c>
       <c r="K29" t="n">
-        <v>3053</v>
+        <v>3083.667</v>
       </c>
       <c r="L29" t="n">
-        <v>0.316</v>
+        <v>0.319</v>
       </c>
       <c r="M29" t="s">
         <v>178</v>
@@ -3373,7 +3366,7 @@
         <v>183</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C30" t="s">
         <v>184</v>
@@ -3383,25 +3376,25 @@
       </c>
       <c r="E30"/>
       <c r="F30" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G30" t="n">
-        <v>49094</v>
+        <v>49961</v>
       </c>
       <c r="H30" t="n">
-        <v>143.865</v>
+        <v>146.406</v>
       </c>
       <c r="I30" t="n">
-        <v>722</v>
+        <v>867</v>
       </c>
       <c r="J30" t="n">
-        <v>2.116</v>
+        <v>2.541</v>
       </c>
       <c r="K30" t="n">
-        <v>690</v>
+        <v>809.667</v>
       </c>
       <c r="L30" t="n">
-        <v>2.022</v>
+        <v>2.373</v>
       </c>
       <c r="M30" t="s">
         <v>185</v>
@@ -3467,7 +3460,7 @@
         <v>193</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C32" t="s">
         <v>189</v>
@@ -3479,25 +3472,25 @@
         <v>191</v>
       </c>
       <c r="F32" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G32" t="n">
-        <v>902654</v>
+        <v>976363</v>
       </c>
       <c r="H32" t="n">
-        <v>0.654</v>
+        <v>0.708</v>
       </c>
       <c r="I32" t="n">
-        <v>72453</v>
+        <v>73709</v>
       </c>
       <c r="J32" t="n">
         <v>0.053</v>
       </c>
       <c r="K32" t="n">
-        <v>61973.667</v>
+        <v>68533</v>
       </c>
       <c r="L32" t="n">
-        <v>0.045</v>
+        <v>0.05</v>
       </c>
       <c r="M32" t="s">
         <v>190</v>
@@ -3517,7 +3510,7 @@
         <v>194</v>
       </c>
       <c r="B33" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C33" t="s">
         <v>195</v>
@@ -3527,25 +3520,25 @@
       </c>
       <c r="E33"/>
       <c r="F33" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G33" t="n">
-        <v>76538</v>
+        <v>79868</v>
       </c>
       <c r="H33" t="n">
-        <v>0.28</v>
+        <v>0.292</v>
       </c>
       <c r="I33" t="n">
-        <v>4187</v>
+        <v>3330</v>
       </c>
       <c r="J33" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="K33" t="n">
+        <v>4028</v>
+      </c>
+      <c r="L33" t="n">
         <v>0.015</v>
-      </c>
-      <c r="K33" t="n">
-        <v>4664.667</v>
-      </c>
-      <c r="L33" t="n">
-        <v>0.017</v>
       </c>
       <c r="M33" t="s">
         <v>196</v>
@@ -3649,7 +3642,7 @@
         <v>209</v>
       </c>
       <c r="B36" s="1" t="n">
-        <v>43949</v>
+        <v>43953</v>
       </c>
       <c r="C36" t="s">
         <v>210</v>
@@ -3661,25 +3654,25 @@
         <v>212</v>
       </c>
       <c r="F36" t="n">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G36" t="n">
-        <v>354857</v>
+        <v>392660</v>
       </c>
       <c r="H36" t="n">
-        <v>40.998</v>
+        <v>45.365</v>
       </c>
       <c r="I36" t="n">
-        <v>10476</v>
+        <v>6738</v>
       </c>
       <c r="J36" t="n">
-        <v>1.21</v>
+        <v>0.778</v>
       </c>
       <c r="K36" t="n">
-        <v>9916.667</v>
+        <v>8899.667</v>
       </c>
       <c r="L36" t="n">
-        <v>1.146</v>
+        <v>1.028</v>
       </c>
       <c r="M36" t="s">
         <v>36</v>
@@ -3699,7 +3692,7 @@
         <v>215</v>
       </c>
       <c r="B37" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C37" t="s">
         <v>216</v>
@@ -3711,25 +3704,25 @@
         <v>218</v>
       </c>
       <c r="F37" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G37" t="n">
-        <v>1354901</v>
+        <v>1398633</v>
       </c>
       <c r="H37" t="n">
-        <v>22.409</v>
+        <v>23.132</v>
       </c>
       <c r="I37" t="n">
-        <v>41441</v>
+        <v>43732</v>
       </c>
       <c r="J37" t="n">
-        <v>0.685</v>
+        <v>0.723</v>
       </c>
       <c r="K37" t="n">
-        <v>39194.667</v>
+        <v>41254</v>
       </c>
       <c r="L37" t="n">
-        <v>0.648</v>
+        <v>0.682</v>
       </c>
       <c r="M37" t="s">
         <v>219</v>
@@ -3749,7 +3742,7 @@
         <v>222</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C38" t="s">
         <v>216</v>
@@ -3761,25 +3754,25 @@
         <v>218</v>
       </c>
       <c r="F38" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G38" t="n">
-        <v>1979217</v>
+        <v>2053425</v>
       </c>
       <c r="H38" t="n">
-        <v>32.735</v>
+        <v>33.962</v>
       </c>
       <c r="I38" t="n">
-        <v>68456</v>
+        <v>74208</v>
       </c>
       <c r="J38" t="n">
-        <v>1.132</v>
+        <v>1.227</v>
       </c>
       <c r="K38" t="n">
-        <v>63185</v>
+        <v>68830.333</v>
       </c>
       <c r="L38" t="n">
-        <v>1.045</v>
+        <v>1.138</v>
       </c>
       <c r="M38" t="s">
         <v>219</v>
@@ -3799,7 +3792,7 @@
         <v>224</v>
       </c>
       <c r="B39" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C39" t="s">
         <v>225</v>
@@ -3811,13 +3804,13 @@
         <v>227</v>
       </c>
       <c r="F39" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G39" t="n">
-        <v>174150</v>
+        <v>181527</v>
       </c>
       <c r="H39" t="n">
-        <v>1.377</v>
+        <v>1.435</v>
       </c>
       <c r="I39"/>
       <c r="J39"/>
@@ -3891,7 +3884,7 @@
         <v>234</v>
       </c>
       <c r="B41" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C41" t="s">
         <v>235</v>
@@ -3901,25 +3894,25 @@
       </c>
       <c r="E41"/>
       <c r="F41" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G41" t="n">
-        <v>249527</v>
+        <v>268534</v>
       </c>
       <c r="H41" t="n">
-        <v>13.289</v>
+        <v>14.301</v>
       </c>
       <c r="I41" t="n">
-        <v>17112</v>
+        <v>19007</v>
       </c>
       <c r="J41" t="n">
-        <v>0.911</v>
+        <v>1.012</v>
       </c>
       <c r="K41" t="n">
-        <v>14655.667</v>
+        <v>17419.333</v>
       </c>
       <c r="L41" t="n">
-        <v>0.781</v>
+        <v>0.928</v>
       </c>
       <c r="M41" t="s">
         <v>236</v>
@@ -3939,7 +3932,7 @@
         <v>238</v>
       </c>
       <c r="B42" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C42" t="s">
         <v>239</v>
@@ -3949,22 +3942,26 @@
       </c>
       <c r="E42"/>
       <c r="F42" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G42" t="n">
-        <v>20268</v>
+        <v>21702</v>
       </c>
       <c r="H42" t="n">
-        <v>0.377</v>
+        <v>0.404</v>
       </c>
       <c r="I42" t="n">
-        <v>2433</v>
+        <v>1434</v>
       </c>
       <c r="J42" t="n">
-        <v>0.045</v>
-      </c>
-      <c r="K42"/>
-      <c r="L42"/>
+        <v>0.027</v>
+      </c>
+      <c r="K42" t="n">
+        <v>1458.333</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0.027</v>
+      </c>
       <c r="M42" t="s">
         <v>36</v>
       </c>
@@ -3983,7 +3980,7 @@
         <v>244</v>
       </c>
       <c r="B43" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C43" t="s">
         <v>245</v>
@@ -3995,25 +3992,25 @@
         <v>247</v>
       </c>
       <c r="F43" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G43" t="n">
-        <v>61120</v>
+        <v>63102</v>
       </c>
       <c r="H43" t="n">
-        <v>32.404</v>
+        <v>33.455</v>
       </c>
       <c r="I43" t="n">
-        <v>3234</v>
+        <v>1982</v>
       </c>
       <c r="J43" t="n">
-        <v>1.715</v>
+        <v>1.051</v>
       </c>
       <c r="K43" t="n">
-        <v>3186.333</v>
+        <v>2763.667</v>
       </c>
       <c r="L43" t="n">
-        <v>1.689</v>
+        <v>1.465</v>
       </c>
       <c r="M43" t="s">
         <v>246</v>
@@ -4033,7 +4030,7 @@
         <v>249</v>
       </c>
       <c r="B44" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C44" t="s">
         <v>250</v>
@@ -4043,25 +4040,25 @@
       </c>
       <c r="E44"/>
       <c r="F44" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G44" t="n">
-        <v>132768</v>
+        <v>138270</v>
       </c>
       <c r="H44" t="n">
-        <v>48.771</v>
+        <v>50.792</v>
       </c>
       <c r="I44" t="n">
-        <v>7213</v>
+        <v>5502</v>
       </c>
       <c r="J44" t="n">
-        <v>2.65</v>
+        <v>2.021</v>
       </c>
       <c r="K44" t="n">
-        <v>6986.333</v>
+        <v>6689.667</v>
       </c>
       <c r="L44" t="n">
-        <v>2.566</v>
+        <v>2.457</v>
       </c>
       <c r="M44" t="s">
         <v>36</v>
@@ -4081,7 +4078,7 @@
         <v>253</v>
       </c>
       <c r="B45" s="1" t="n">
-        <v>43951</v>
+        <v>43953</v>
       </c>
       <c r="C45" t="s">
         <v>254</v>
@@ -4091,21 +4088,25 @@
       </c>
       <c r="E45"/>
       <c r="F45" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G45" t="n">
-        <v>42643</v>
+        <v>47460</v>
       </c>
       <c r="H45" t="n">
-        <v>68.122</v>
-      </c>
-      <c r="I45"/>
+        <v>75.818</v>
+      </c>
+      <c r="I45" t="n">
+        <v>2565</v>
+      </c>
       <c r="J45" t="n">
-        <v>1.414</v>
-      </c>
-      <c r="K45"/>
+        <v>4.098</v>
+      </c>
+      <c r="K45" t="n">
+        <v>1900.667</v>
+      </c>
       <c r="L45" t="n">
-        <v>1.886</v>
+        <v>3.037</v>
       </c>
       <c r="M45" t="s">
         <v>255</v>
@@ -4125,7 +4126,7 @@
         <v>258</v>
       </c>
       <c r="B46" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C46" t="s">
         <v>259</v>
@@ -4135,16 +4136,20 @@
       </c>
       <c r="E46"/>
       <c r="F46" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G46" t="n">
-        <v>168784</v>
+        <v>184213</v>
       </c>
       <c r="H46" t="n">
-        <v>5.215</v>
-      </c>
-      <c r="I46"/>
-      <c r="J46"/>
+        <v>5.692</v>
+      </c>
+      <c r="I46" t="n">
+        <v>15429</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.477</v>
+      </c>
       <c r="K46"/>
       <c r="L46"/>
       <c r="M46" t="s">
@@ -4165,7 +4170,7 @@
         <v>264</v>
       </c>
       <c r="B47" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C47" t="s">
         <v>265</v>
@@ -4175,13 +4180,13 @@
       </c>
       <c r="E47"/>
       <c r="F47" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G47" t="n">
-        <v>71852</v>
+        <v>75742</v>
       </c>
       <c r="H47" t="n">
-        <v>0.557</v>
+        <v>0.587</v>
       </c>
       <c r="I47"/>
       <c r="J47" t="n">
@@ -4209,7 +4214,7 @@
         <v>268</v>
       </c>
       <c r="B48" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C48" t="s">
         <v>269</v>
@@ -4221,25 +4226,25 @@
         <v>271</v>
       </c>
       <c r="F48" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G48" t="n">
-        <v>34841</v>
+        <v>37006</v>
       </c>
       <c r="H48" t="n">
-        <v>0.944</v>
+        <v>1.003</v>
       </c>
       <c r="I48" t="n">
-        <v>1911</v>
+        <v>2165</v>
       </c>
       <c r="J48" t="n">
+        <v>0.059</v>
+      </c>
+      <c r="K48" t="n">
+        <v>1918.667</v>
+      </c>
+      <c r="L48" t="n">
         <v>0.052</v>
-      </c>
-      <c r="K48" t="n">
-        <v>1862.333</v>
-      </c>
-      <c r="L48" t="n">
-        <v>0.051</v>
       </c>
       <c r="M48" t="s">
         <v>270</v>
@@ -4259,7 +4264,7 @@
         <v>274</v>
       </c>
       <c r="B49" s="1" t="n">
-        <v>43950</v>
+        <v>43952</v>
       </c>
       <c r="C49" t="s">
         <v>275</v>
@@ -4267,243 +4272,241 @@
       <c r="D49" t="s">
         <v>276</v>
       </c>
-      <c r="E49"/>
+      <c r="E49" t="s">
+        <v>277</v>
+      </c>
       <c r="F49" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G49" t="n">
-        <v>7890</v>
+        <v>8281</v>
       </c>
       <c r="H49" t="n">
-        <v>0.145</v>
+        <v>0.152</v>
       </c>
       <c r="I49" t="n">
-        <v>282</v>
+        <v>196</v>
       </c>
       <c r="J49" t="n">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="K49" t="n">
-        <v>404</v>
+        <v>224.333</v>
       </c>
       <c r="L49" t="n">
-        <v>0.007</v>
+        <v>0.004</v>
       </c>
       <c r="M49" t="s">
         <v>276</v>
       </c>
       <c r="N49" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="O49" t="s">
         <v>45</v>
       </c>
       <c r="P49" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B50" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C50" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D50" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E50" t="s">
+        <v>283</v>
+      </c>
+      <c r="F50" t="n">
+        <v>71</v>
+      </c>
+      <c r="G50" t="n">
+        <v>12577</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.432</v>
+      </c>
+      <c r="I50" t="n">
+        <v>566</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="K50" t="n">
+        <v>590</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="M50" t="s">
         <v>282</v>
       </c>
-      <c r="F50" t="n">
-        <v>70</v>
-      </c>
-      <c r="G50" t="n">
-        <v>12011</v>
-      </c>
-      <c r="H50" t="n">
-        <v>0.412</v>
-      </c>
-      <c r="I50" t="n">
-        <v>487</v>
-      </c>
-      <c r="J50" t="n">
-        <v>0.017</v>
-      </c>
-      <c r="K50" t="n">
-        <v>513.333</v>
-      </c>
-      <c r="L50" t="n">
-        <v>0.018</v>
-      </c>
-      <c r="M50" t="s">
-        <v>281</v>
-      </c>
       <c r="N50" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="O50" t="s">
         <v>74</v>
       </c>
       <c r="P50" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B51" s="1" t="n">
-        <v>43950</v>
+        <v>43951</v>
       </c>
       <c r="C51" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D51" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E51"/>
       <c r="F51" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G51" t="n">
-        <v>219744</v>
+        <v>225899</v>
       </c>
       <c r="H51" t="n">
-        <v>12.824</v>
+        <v>13.184</v>
       </c>
       <c r="I51" t="n">
-        <v>4575</v>
+        <v>4057</v>
       </c>
       <c r="J51" t="n">
-        <v>0.267</v>
+        <v>0.237</v>
       </c>
       <c r="K51" t="n">
-        <v>3803</v>
+        <v>4519.667</v>
       </c>
       <c r="L51" t="n">
-        <v>0.222</v>
+        <v>0.264</v>
       </c>
       <c r="M51" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="N51" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O51" t="s">
         <v>74</v>
       </c>
       <c r="P51" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B52" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C52" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D52" t="s">
         <v>36</v>
       </c>
       <c r="E52"/>
       <c r="F52" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G52" t="n">
-        <v>139898</v>
+        <v>145589</v>
       </c>
       <c r="H52" t="n">
-        <v>29.011</v>
+        <v>30.191</v>
       </c>
       <c r="I52" t="n">
-        <v>5328</v>
+        <v>5691</v>
       </c>
       <c r="J52" t="n">
-        <v>1.105</v>
+        <v>1.18</v>
       </c>
       <c r="K52" t="n">
-        <v>4610.667</v>
+        <v>5628.667</v>
       </c>
       <c r="L52" t="n">
-        <v>0.956</v>
+        <v>1.167</v>
       </c>
       <c r="M52" t="s">
+        <v>294</v>
+      </c>
+      <c r="N52" t="s">
         <v>293</v>
-      </c>
-      <c r="N52" t="s">
-        <v>292</v>
       </c>
       <c r="O52" t="s">
         <v>20</v>
       </c>
       <c r="P52" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B53" s="1" t="n">
-        <v>43950</v>
+        <v>43952</v>
       </c>
       <c r="C53" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D53" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E53"/>
       <c r="F53" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G53" t="n">
-        <v>12828</v>
+        <v>15759</v>
       </c>
       <c r="H53" t="n">
-        <v>0.062</v>
-      </c>
-      <c r="I53" t="n">
-        <v>824</v>
-      </c>
-      <c r="J53" t="n">
-        <v>0.004</v>
-      </c>
+        <v>0.076</v>
+      </c>
+      <c r="I53"/>
+      <c r="J53"/>
       <c r="K53"/>
       <c r="L53"/>
       <c r="M53" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="N53" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="O53" t="s">
         <v>45</v>
       </c>
       <c r="P53" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B54" s="1" t="n">
         <v>43951</v>
       </c>
       <c r="C54" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D54" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E54"/>
       <c r="F54" t="n">
@@ -4528,222 +4531,222 @@
         <v>0.509</v>
       </c>
       <c r="M54" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="N54" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="O54" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="P54" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B55" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C55" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D55" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E55"/>
       <c r="F55" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G55" t="n">
-        <v>182131</v>
+        <v>193859</v>
       </c>
       <c r="H55" t="n">
-        <v>0.825</v>
+        <v>0.878</v>
       </c>
       <c r="I55" t="n">
-        <v>7971</v>
+        <v>11728</v>
       </c>
       <c r="J55" t="n">
-        <v>0.036</v>
+        <v>0.053</v>
       </c>
       <c r="K55" t="n">
-        <v>8302.667</v>
+        <v>9316</v>
       </c>
       <c r="L55" t="n">
-        <v>0.037</v>
+        <v>0.042</v>
       </c>
       <c r="M55" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="N55" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="O55" t="s">
         <v>20</v>
       </c>
       <c r="P55" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B56" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C56" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D56" t="s">
         <v>36</v>
       </c>
       <c r="E56" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F56" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G56" t="n">
-        <v>30749</v>
+        <v>31895</v>
       </c>
       <c r="H56" t="n">
-        <v>7.126</v>
+        <v>7.392</v>
       </c>
       <c r="I56" t="n">
-        <v>912</v>
+        <v>1146</v>
       </c>
       <c r="J56" t="n">
-        <v>0.211</v>
+        <v>0.266</v>
       </c>
       <c r="K56" t="n">
-        <v>971.667</v>
+        <v>1033.333</v>
       </c>
       <c r="L56" t="n">
-        <v>0.225</v>
+        <v>0.239</v>
       </c>
       <c r="M56" t="s">
         <v>36</v>
       </c>
       <c r="N56" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="O56" t="s">
         <v>103</v>
       </c>
       <c r="P56" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B57" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C57" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D57" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E57" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F57" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G57" t="n">
-        <v>9888</v>
+        <v>10327</v>
       </c>
       <c r="H57" t="n">
-        <v>1.386</v>
+        <v>1.448</v>
       </c>
       <c r="I57" t="n">
-        <v>449</v>
+        <v>439</v>
       </c>
       <c r="J57" t="n">
-        <v>0.063</v>
+        <v>0.062</v>
       </c>
       <c r="K57" t="n">
-        <v>486.333</v>
+        <v>483.667</v>
       </c>
       <c r="L57" t="n">
         <v>0.068</v>
       </c>
       <c r="M57" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="N57" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="O57" t="s">
         <v>45</v>
       </c>
       <c r="P57" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B58" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C58" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D58" t="s">
         <v>36</v>
       </c>
       <c r="E58"/>
       <c r="F58" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G58" t="n">
-        <v>318252</v>
+        <v>342498</v>
       </c>
       <c r="H58" t="n">
-        <v>9.652</v>
-      </c>
-      <c r="I58" t="n">
-        <v>50640</v>
-      </c>
+        <v>10.388</v>
+      </c>
+      <c r="I58"/>
       <c r="J58" t="n">
-        <v>1.536</v>
+        <v>0.735</v>
       </c>
       <c r="K58"/>
-      <c r="L58"/>
+      <c r="L58" t="n">
+        <v>1.041</v>
+      </c>
       <c r="M58" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="N58" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="O58" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="P58" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B59" s="1" t="n">
         <v>43951</v>
       </c>
       <c r="C59" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D59" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E59"/>
       <c r="F59" t="n">
@@ -4767,30 +4770,30 @@
         <v>172</v>
       </c>
       <c r="N59" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="O59" t="s">
         <v>74</v>
       </c>
       <c r="P59" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B60" s="1" t="n">
         <v>43952</v>
       </c>
       <c r="C60" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D60" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E60" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F60" t="n">
         <v>58</v>
@@ -4814,325 +4817,325 @@
         <v>0.387</v>
       </c>
       <c r="M60" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="N60" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="O60" t="s">
         <v>45</v>
       </c>
       <c r="P60" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B61" s="1" t="n">
-        <v>43950</v>
+        <v>43951</v>
       </c>
       <c r="C61" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D61" t="s">
         <v>36</v>
       </c>
       <c r="E61"/>
       <c r="F61" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G61" t="n">
-        <v>409961</v>
+        <v>426836</v>
       </c>
       <c r="H61" t="n">
-        <v>40.205</v>
+        <v>41.86</v>
       </c>
       <c r="I61" t="n">
-        <v>13922</v>
+        <v>16061</v>
       </c>
       <c r="J61" t="n">
-        <v>1.365</v>
+        <v>1.575</v>
       </c>
       <c r="K61" t="n">
-        <v>13844.333</v>
+        <v>15421.333</v>
       </c>
       <c r="L61" t="n">
-        <v>1.357</v>
+        <v>1.512</v>
       </c>
       <c r="M61" t="s">
+        <v>343</v>
+      </c>
+      <c r="N61" t="s">
         <v>342</v>
       </c>
-      <c r="N61" t="s">
-        <v>341</v>
-      </c>
       <c r="O61" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="P61" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B62" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C62" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D62" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E62"/>
       <c r="F62" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G62" t="n">
-        <v>97726</v>
+        <v>101728</v>
       </c>
       <c r="H62" t="n">
-        <v>33.92</v>
+        <v>35.309</v>
       </c>
       <c r="I62" t="n">
-        <v>3226</v>
+        <v>4002</v>
       </c>
       <c r="J62" t="n">
-        <v>1.12</v>
+        <v>1.389</v>
       </c>
       <c r="K62" t="n">
-        <v>3039.667</v>
+        <v>3437.667</v>
       </c>
       <c r="L62" t="n">
-        <v>1.055</v>
+        <v>1.193</v>
       </c>
       <c r="M62" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="N62" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="O62" t="s">
         <v>74</v>
       </c>
       <c r="P62" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B63" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C63" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D63" t="s">
+        <v>353</v>
+      </c>
+      <c r="E63" t="s">
+        <v>354</v>
+      </c>
+      <c r="F63" t="n">
+        <v>52</v>
+      </c>
+      <c r="G63" t="n">
+        <v>190540</v>
+      </c>
+      <c r="H63" t="n">
+        <v>9.905</v>
+      </c>
+      <c r="I63" t="n">
+        <v>6852</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.356</v>
+      </c>
+      <c r="K63" t="n">
+        <v>7849</v>
+      </c>
+      <c r="L63" t="n">
+        <v>0.408</v>
+      </c>
+      <c r="M63" t="s">
+        <v>353</v>
+      </c>
+      <c r="N63" t="s">
         <v>352</v>
-      </c>
-      <c r="E63" t="s">
-        <v>353</v>
-      </c>
-      <c r="F63" t="n">
-        <v>51</v>
-      </c>
-      <c r="G63" t="n">
-        <v>183688</v>
-      </c>
-      <c r="H63" t="n">
-        <v>9.548</v>
-      </c>
-      <c r="I63" t="n">
-        <v>8314</v>
-      </c>
-      <c r="J63" t="n">
-        <v>0.432</v>
-      </c>
-      <c r="K63" t="n">
-        <v>11126.333</v>
-      </c>
-      <c r="L63" t="n">
-        <v>0.578</v>
-      </c>
-      <c r="M63" t="s">
-        <v>352</v>
-      </c>
-      <c r="N63" t="s">
-        <v>351</v>
       </c>
       <c r="O63" t="s">
         <v>20</v>
       </c>
       <c r="P63" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B64" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C64" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D64" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E64"/>
       <c r="F64" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G64" t="n">
-        <v>3723807</v>
+        <v>3945518</v>
       </c>
       <c r="H64" t="n">
-        <v>25.517</v>
+        <v>27.036</v>
       </c>
       <c r="I64" t="n">
-        <v>225499</v>
+        <v>221711</v>
       </c>
       <c r="J64" t="n">
-        <v>1.545</v>
+        <v>1.519</v>
       </c>
       <c r="K64" t="n">
-        <v>194849.667</v>
+        <v>213933.667</v>
       </c>
       <c r="L64" t="n">
-        <v>1.335</v>
+        <v>1.466</v>
       </c>
       <c r="M64" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="N64" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="O64" t="s">
         <v>20</v>
       </c>
       <c r="P64" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B65" s="1" t="n">
-        <v>43950</v>
+        <v>43951</v>
       </c>
       <c r="C65" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D65" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E65"/>
       <c r="F65" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G65" t="n">
-        <v>24005</v>
+        <v>25145</v>
       </c>
       <c r="H65" t="n">
-        <v>1.853</v>
+        <v>1.941</v>
       </c>
       <c r="I65" t="n">
-        <v>1705</v>
+        <v>1140</v>
       </c>
       <c r="J65" t="n">
-        <v>0.132</v>
+        <v>0.088</v>
       </c>
       <c r="K65" t="n">
-        <v>1474.667</v>
+        <v>1450</v>
       </c>
       <c r="L65" t="n">
-        <v>0.114</v>
+        <v>0.112</v>
       </c>
       <c r="M65" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="N65" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O65" t="s">
         <v>45</v>
       </c>
       <c r="P65" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B66" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C66" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D66" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E66" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F66" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G66" t="n">
-        <v>12770</v>
+        <v>13960</v>
       </c>
       <c r="H66" t="n">
-        <v>0.763</v>
+        <v>0.834</v>
       </c>
       <c r="I66" t="n">
-        <v>901</v>
+        <v>1190</v>
       </c>
       <c r="J66" t="n">
-        <v>0.054</v>
+        <v>0.071</v>
       </c>
       <c r="K66" t="n">
-        <v>954</v>
+        <v>1084</v>
       </c>
       <c r="L66" t="n">
-        <v>0.057</v>
+        <v>0.065</v>
       </c>
       <c r="M66" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="N66" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="O66" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="P66" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B67" s="1" t="n">
         <v>43952</v>
       </c>
       <c r="C67" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D67" t="s">
         <v>36</v>
       </c>
       <c r="E67" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F67" t="n">
         <v>65</v>
@@ -5159,24 +5162,24 @@
         <v>36</v>
       </c>
       <c r="N67" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="O67" t="s">
         <v>74</v>
       </c>
       <c r="P67" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B68" s="1" t="n">
         <v>43948</v>
       </c>
       <c r="C68" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D68" t="s">
         <v>36</v>
@@ -5199,24 +5202,24 @@
         <v>36</v>
       </c>
       <c r="N68" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="O68" t="s">
         <v>74</v>
       </c>
       <c r="P68" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B69" s="1" t="n">
         <v>43948</v>
       </c>
       <c r="C69" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D69" t="s">
         <v>36</v>
@@ -5239,224 +5242,224 @@
         <v>36</v>
       </c>
       <c r="N69" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="O69" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="P69" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B70" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C70" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D70" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E70"/>
       <c r="F70" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G70" t="n">
-        <v>91072</v>
+        <v>94770</v>
       </c>
       <c r="H70" t="n">
-        <v>16.681</v>
+        <v>17.358</v>
       </c>
       <c r="I70" t="n">
-        <v>5150</v>
+        <v>3698</v>
       </c>
       <c r="J70" t="n">
-        <v>0.943</v>
+        <v>0.677</v>
       </c>
       <c r="K70" t="n">
-        <v>5068.667</v>
+        <v>4477.333</v>
       </c>
       <c r="L70" t="n">
-        <v>0.928</v>
+        <v>0.82</v>
       </c>
       <c r="M70" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="N70" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="O70" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="P70" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B71" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C71" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D71" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E71"/>
       <c r="F71" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G71" t="n">
-        <v>54300</v>
+        <v>55020</v>
       </c>
       <c r="H71" t="n">
-        <v>26.119</v>
+        <v>26.466</v>
       </c>
       <c r="I71" t="n">
-        <v>1352</v>
+        <v>720</v>
       </c>
       <c r="J71" t="n">
-        <v>0.65</v>
+        <v>0.346</v>
       </c>
       <c r="K71" t="n">
-        <v>1336.667</v>
+        <v>1137.667</v>
       </c>
       <c r="L71" t="n">
-        <v>0.643</v>
+        <v>0.547</v>
       </c>
       <c r="M71" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="N71" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="O71" t="s">
         <v>20</v>
       </c>
       <c r="P71" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B72" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C72" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D72" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="E72" t="s">
+        <v>400</v>
+      </c>
+      <c r="F72" t="n">
+        <v>61</v>
+      </c>
+      <c r="G72" t="n">
+        <v>217522</v>
+      </c>
+      <c r="H72" t="n">
+        <v>3.668</v>
+      </c>
+      <c r="I72" t="n">
+        <v>9992</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0.168</v>
+      </c>
+      <c r="K72" t="n">
+        <v>10675</v>
+      </c>
+      <c r="L72" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="M72" t="s">
         <v>399</v>
       </c>
-      <c r="F72" t="n">
-        <v>60</v>
-      </c>
-      <c r="G72" t="n">
-        <v>207530</v>
-      </c>
-      <c r="H72" t="n">
-        <v>3.499</v>
-      </c>
-      <c r="I72" t="n">
-        <v>10403</v>
-      </c>
-      <c r="J72" t="n">
-        <v>0.175</v>
-      </c>
-      <c r="K72" t="n">
-        <v>9686.667</v>
-      </c>
-      <c r="L72" t="n">
-        <v>0.163</v>
-      </c>
-      <c r="M72" t="s">
-        <v>398</v>
-      </c>
       <c r="N72" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="O72" t="s">
         <v>74</v>
       </c>
       <c r="P72" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B73" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C73" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D73" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E73"/>
       <c r="F73" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G73" t="n">
-        <v>623069</v>
+        <v>627562</v>
       </c>
       <c r="H73" t="n">
-        <v>12.153</v>
+        <v>12.241</v>
       </c>
       <c r="I73" t="n">
-        <v>3188</v>
+        <v>4493</v>
       </c>
       <c r="J73" t="n">
-        <v>0.062</v>
+        <v>0.088</v>
       </c>
       <c r="K73" t="n">
-        <v>4851.667</v>
+        <v>4455</v>
       </c>
       <c r="L73" t="n">
-        <v>0.095</v>
+        <v>0.087</v>
       </c>
       <c r="M73" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="N73" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="O73" t="s">
         <v>62</v>
       </c>
       <c r="P73" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B74" s="1" t="n">
         <v>43944</v>
       </c>
       <c r="C74" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D74" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E74" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F74" t="n">
         <v>2</v>
@@ -5472,30 +5475,30 @@
       <c r="K74"/>
       <c r="L74"/>
       <c r="M74" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="N74" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="O74" t="s">
         <v>20</v>
       </c>
       <c r="P74" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B75" s="1" t="n">
         <v>43947</v>
       </c>
       <c r="C75" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D75" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="E75"/>
       <c r="F75" t="n">
@@ -5512,30 +5515,30 @@
       <c r="K75"/>
       <c r="L75"/>
       <c r="M75" t="s">
+        <v>417</v>
+      </c>
+      <c r="N75" t="s">
         <v>416</v>
-      </c>
-      <c r="N75" t="s">
-        <v>415</v>
       </c>
       <c r="O75" t="s">
         <v>74</v>
       </c>
       <c r="P75" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B76" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="C76" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D76" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="E76"/>
       <c r="F76" t="n">
@@ -5556,225 +5559,225 @@
         <v>0.345</v>
       </c>
       <c r="M76" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="N76" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="O76" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="P76" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B77" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C77" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D77" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E77"/>
       <c r="F77" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G77" t="n">
-        <v>63340</v>
+        <v>63713</v>
       </c>
       <c r="H77" t="n">
-        <v>2.659</v>
+        <v>2.675</v>
       </c>
       <c r="I77" t="n">
-        <v>496</v>
+        <v>373</v>
       </c>
       <c r="J77" t="n">
-        <v>0.021</v>
+        <v>0.016</v>
       </c>
       <c r="K77" t="n">
-        <v>552</v>
+        <v>448.333</v>
       </c>
       <c r="L77" t="n">
-        <v>0.023</v>
+        <v>0.019</v>
       </c>
       <c r="M77" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="N77" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="O77" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="P77" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B78" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C78" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D78" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E78"/>
       <c r="F78" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G78" t="n">
-        <v>70535</v>
+        <v>72745</v>
       </c>
       <c r="H78" t="n">
-        <v>1.011</v>
+        <v>1.042</v>
       </c>
       <c r="I78" t="n">
-        <v>4164</v>
+        <v>2210</v>
       </c>
       <c r="J78" t="n">
-        <v>0.06</v>
+        <v>0.032</v>
       </c>
       <c r="K78" t="n">
-        <v>4204.333</v>
+        <v>3575.667</v>
       </c>
       <c r="L78" t="n">
-        <v>0.06</v>
+        <v>0.051</v>
       </c>
       <c r="M78" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="N78" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="O78" t="s">
         <v>74</v>
       </c>
       <c r="P78" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B79" s="1" t="n">
-        <v>43950</v>
+        <v>43951</v>
       </c>
       <c r="C79" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D79" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E79"/>
       <c r="F79" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G79" t="n">
-        <v>22957</v>
+        <v>23526</v>
       </c>
       <c r="H79" t="n">
-        <v>1.942</v>
+        <v>1.991</v>
       </c>
       <c r="I79" t="n">
-        <v>895</v>
+        <v>569</v>
       </c>
       <c r="J79" t="n">
-        <v>0.076</v>
+        <v>0.048</v>
       </c>
       <c r="K79" t="n">
-        <v>625.333</v>
+        <v>683</v>
       </c>
       <c r="L79" t="n">
-        <v>0.053</v>
+        <v>0.058</v>
       </c>
       <c r="M79" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="N79" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="O79" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="P79" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B80" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C80" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D80" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E80"/>
       <c r="F80" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G80" t="n">
-        <v>1033617</v>
+        <v>1075048</v>
       </c>
       <c r="H80" t="n">
-        <v>12.255</v>
+        <v>12.747</v>
       </c>
       <c r="I80" t="n">
-        <v>42004</v>
+        <v>41431</v>
       </c>
       <c r="J80" t="n">
-        <v>0.498</v>
+        <v>0.491</v>
       </c>
       <c r="K80" t="n">
-        <v>38244</v>
+        <v>42311</v>
       </c>
       <c r="L80" t="n">
-        <v>0.454</v>
+        <v>0.502</v>
       </c>
       <c r="M80" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="N80" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="O80" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="P80" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B81" s="1" t="n">
         <v>43951</v>
       </c>
       <c r="C81" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D81" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="E81" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="F81" t="n">
         <v>24</v>
@@ -5798,318 +5801,318 @@
         <v>0.047</v>
       </c>
       <c r="M81" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="N81" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="O81" t="s">
         <v>45</v>
       </c>
       <c r="P81" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B82" s="1" t="n">
-        <v>43951</v>
+        <v>43953</v>
       </c>
       <c r="C82" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D82" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="E82"/>
       <c r="F82" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G82" t="n">
-        <v>111859</v>
+        <v>122752</v>
       </c>
       <c r="H82" t="n">
-        <v>2.558</v>
+        <v>2.807</v>
       </c>
       <c r="I82" t="n">
-        <v>7315</v>
+        <v>4207</v>
       </c>
       <c r="J82" t="n">
-        <v>0.167</v>
+        <v>0.096</v>
       </c>
       <c r="K82" t="n">
-        <v>6113.333</v>
+        <v>6069.333</v>
       </c>
       <c r="L82" t="n">
-        <v>0.14</v>
+        <v>0.139</v>
       </c>
       <c r="M82" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="N82" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="O82" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="P82" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B83" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C83" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D83" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="E83"/>
       <c r="F83" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G83" t="n">
-        <v>687369</v>
+        <v>762279</v>
       </c>
       <c r="H83" t="n">
-        <v>10.125</v>
+        <v>11.229</v>
       </c>
       <c r="I83" t="n">
-        <v>54575</v>
+        <v>73191</v>
       </c>
       <c r="J83" t="n">
-        <v>0.804</v>
+        <v>1.078</v>
       </c>
       <c r="K83" t="n">
-        <v>39200.333</v>
+        <v>53740.333</v>
       </c>
       <c r="L83" t="n">
-        <v>0.578</v>
+        <v>0.792</v>
       </c>
       <c r="M83" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="N83" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="O83" t="s">
         <v>74</v>
       </c>
       <c r="P83" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B84" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C84" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="D84" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="E84"/>
       <c r="F84" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G84" t="n">
-        <v>901905</v>
+        <v>1023824</v>
       </c>
       <c r="H84" t="n">
-        <v>13.286</v>
+        <v>15.082</v>
       </c>
       <c r="I84" t="n">
-        <v>81611</v>
+        <v>122347</v>
       </c>
       <c r="J84" t="n">
-        <v>1.202</v>
+        <v>1.802</v>
       </c>
       <c r="K84" t="n">
-        <v>59201</v>
+        <v>85462.333</v>
       </c>
       <c r="L84" t="n">
-        <v>0.872</v>
+        <v>1.259</v>
       </c>
       <c r="M84" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="N84" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="O84" t="s">
-        <v>20</v>
+        <v>468</v>
       </c>
       <c r="P84" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="B85" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C85" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="D85" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="E85"/>
       <c r="F85" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G85" t="n">
-        <v>6231182</v>
+        <v>6551810</v>
       </c>
       <c r="H85" t="n">
-        <v>18.825</v>
+        <v>19.794</v>
       </c>
       <c r="I85" t="n">
-        <v>206557</v>
+        <v>305118</v>
       </c>
       <c r="J85" t="n">
-        <v>0.624</v>
+        <v>0.922</v>
       </c>
       <c r="K85" t="n">
-        <v>212562.333</v>
+        <v>252027.333</v>
       </c>
       <c r="L85" t="n">
-        <v>0.642</v>
+        <v>0.761</v>
       </c>
       <c r="M85" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="N85" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="O85" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="P85" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="B86" s="1" t="n">
-        <v>43943</v>
+        <v>43944</v>
       </c>
       <c r="C86" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="D86" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="E86"/>
       <c r="F86" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G86" t="n">
-        <v>475478</v>
+        <v>498015</v>
       </c>
       <c r="H86" t="n">
-        <v>1.436</v>
+        <v>1.505</v>
       </c>
       <c r="I86" t="n">
-        <v>19923</v>
+        <v>21420</v>
       </c>
       <c r="J86" t="n">
-        <v>0.06</v>
+        <v>0.065</v>
       </c>
       <c r="K86" t="n">
-        <v>17110</v>
+        <v>19322</v>
       </c>
       <c r="L86" t="n">
-        <v>0.052</v>
+        <v>0.058</v>
       </c>
       <c r="M86" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="N86" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="O86" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="P86" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="B87" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C87" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="D87" t="s">
         <v>101</v>
       </c>
       <c r="E87"/>
       <c r="F87" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G87" t="n">
-        <v>19747</v>
+        <v>20554</v>
       </c>
       <c r="H87" t="n">
-        <v>5.685</v>
+        <v>5.917</v>
       </c>
       <c r="I87" t="n">
-        <v>731</v>
+        <v>807</v>
       </c>
       <c r="J87" t="n">
-        <v>0.21</v>
+        <v>0.232</v>
       </c>
       <c r="K87" t="n">
-        <v>747.333</v>
+        <v>804.667</v>
       </c>
       <c r="L87" t="n">
-        <v>0.215</v>
+        <v>0.231</v>
       </c>
       <c r="M87" t="s">
         <v>101</v>
       </c>
       <c r="N87" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="O87" t="s">
         <v>20</v>
       </c>
       <c r="P87" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="B88" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="C88" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="D88" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="E88"/>
       <c r="F88" t="n">
@@ -6126,64 +6129,64 @@
       <c r="K88"/>
       <c r="L88"/>
       <c r="M88" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="N88" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="O88" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="P88" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="B89" s="1" t="n">
-        <v>43950</v>
+        <v>43951</v>
       </c>
       <c r="C89" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="D89" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="E89"/>
       <c r="F89" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G89" t="n">
-        <v>7642</v>
+        <v>8314</v>
       </c>
       <c r="H89" t="n">
-        <v>0.514</v>
+        <v>0.559</v>
       </c>
       <c r="I89" t="n">
-        <v>355</v>
+        <v>672</v>
       </c>
       <c r="J89" t="n">
-        <v>0.024</v>
+        <v>0.045</v>
       </c>
       <c r="K89" t="n">
-        <v>415.667</v>
+        <v>493.333</v>
       </c>
       <c r="L89" t="n">
-        <v>0.028</v>
+        <v>0.033</v>
       </c>
       <c r="M89" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="N89" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="O89" t="s">
         <v>20</v>
       </c>
       <c r="P89" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testing data for 2020-05-03
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -100,7 +100,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200502151038/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200503141230/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -124,7 +124,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200502151040/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200503141232/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -220,7 +220,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200502151045/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200503141236/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -240,7 +240,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200501173328/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200503141238/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -316,7 +316,7 @@
     <t xml:space="preserve">Croatia - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200502151051/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200503141652/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -391,7 +391,7 @@
     <t xml:space="preserve">Ecuador - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/04/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-30042020-08h00.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/05/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-02052020-08h00.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -404,7 +404,8 @@
   </si>
   <si>
     <t xml:space="preserve">The Government of Ecuador publish daily updates in the form of situation reports and summary infographics. These report the number and status of confirmed cases, deaths and number of samples tested. This data is available daily from 18th March; reports and infographics prior to this date do not include the number of samples tested. But all figures are dated cumulative since 29th February.
-The source reports the number of confirmed ('confirmados') and negative ('descartados') cases, which we sum to get the number of cases tested.</t>
+The source reports the number of confirmed ('confirmados') and negative ('descartados') cases, which we sum to get the number of cases tested.
+On 24 April 2020, the number of tests suddenly jumped from 23,383 to 45,857, because of what we assume to be the inclusion of rapid tests ("pruebas rápidas"), as made clear by the subsequent infographic published on 27 April. We therefore do not include the 24 April infographic in our time series; and from 27 April onwards, we include only PCR tests.</t>
   </si>
   <si>
     <t xml:space="preserve">El Salvador - tests performed</t>
@@ -554,7 +555,7 @@
     <t xml:space="preserve">Outbreak Response Management provides daily situation updates on the total number of people or total samples tested for the coronavirus.
 Using web archives, we reconstruct a time series. Situation updates report the total number of people tested from 28th March, then the total number of samples tested from 18th April. However, the figures given from one period to the other seem to line up correctly, thus we are not certain what the true units are.
 On 24th April, the daily situation update in text format was replaced with an interactive dashboard, still [at the same URL](https://www.ghanahealthservice.org/covid19/). As far we know, this dashboard no longer reports testing data. 
-We are aware of Ghana's [archived situation reports](https://www.ghanahealthservice.org/covid19/archive.php) which provide a breakdown of the total number of tests.</t>
+We are aware of Ghana's [archived situation reports](https://www.ghanahealthservice.org/covid19/archive.php) which provides a breakdown of the total number of tests.</t>
   </si>
   <si>
     <t xml:space="preserve">Greece - tests performed</t>
@@ -785,7 +786,7 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000626512.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000627446.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Implementation status of PCR tests for new coronavirus in Japan (based on the date on which the results were determined). Preliminary data</t>
@@ -848,7 +849,7 @@
     <t xml:space="preserve">Lithuania - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200502151129/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200503141813/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -879,7 +880,7 @@
     <t xml:space="preserve">Malaysia - cases tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200502151137/https://www.moh.gov.my/index.php/pages/view/2019-ncov-wuhan</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200503141827/https://www.moh.gov.my/index.php/pages/view/2019-ncov-wuhan</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1006,7 +1007,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200501155337/http://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200503141847/https://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1045,7 +1046,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200502151159/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200503141854/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1102,7 +1103,7 @@
     <t xml:space="preserve">Peru - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/143593-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-40-459-en-el-peru-comunicado-n-84</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/143615-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-42-534-comunicado-n-85</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1137,7 +1138,7 @@
     <t xml:space="preserve">Poland - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://raw.githubusercontent.com/anuszka/COVID-19-MZ_GOV_PL/master/data/cor.2020.05.01.csv</t>
+    <t xml:space="preserve">https://raw.githubusercontent.com/anuszka/COVID-19-MZ_GOV_PL/master/data/cor.2020.05.03.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1176,7 +1177,7 @@
     <t xml:space="preserve">Qatar - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200502151207/https://www.moph.gov.qa/english/Pages/Coronavirus2019.aspx</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200503141907/https://www.moph.gov.qa/english/Pages/Coronavirus2019.aspx</t>
   </si>
   <si>
     <t xml:space="preserve">Qatar Ministry of Public Health</t>
@@ -1208,7 +1209,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14371</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14373</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1298,7 +1299,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200502151233/https://www.korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200503141916/https://www.korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Center of Health Information and the Office of the Government of the Slovak Republic</t>
@@ -1363,7 +1364,7 @@
     <t xml:space="preserve">South Korea - cases tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367066&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367070&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1380,13 +1381,13 @@
     <t xml:space="preserve">Spain - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mscbs.gob.es/en/gabinete/notasPrensa.do?metodo=detalle&amp;id=4883</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Press release from the Ministerio de Sanidad, Consumo y Bienestar Social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comparing these figures with those collected from Autonomous Communities by CIVIO, the estimate for Madrid included in these figures appears to date back to 14 April (see https://datos.civio.es/dataset/pcr-coronavirus-covid19-espana-comunidades-autonomas/).</t>
+    <t xml:space="preserve">https://www.abc.es/espana/abci-sanchez-somos-quinto-pais-mundo-numero-test-realizados-202005021736_video.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Press conference by Prime Minister</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure given directly by the Prime Minister in a press conference on 2 May 2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministerio de Sanidad, Consumo y Bienestar Social</t>
@@ -1440,7 +1441,7 @@
     <t xml:space="preserve">Taiwan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/bJVsQHE6lCY1CMTi1gMcpQ?typeid=9</t>
+    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/aAUzPjvwik0ZcghByRkokA?typeid=9</t>
   </si>
   <si>
     <t xml:space="preserve">Taiwan Centers for Disease Control (CDC)</t>
@@ -1460,7 +1461,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200502151250/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200503141951/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1501,7 +1502,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200501173455/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200503142006/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1522,7 +1523,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1255973076493369344</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1256338138646994944</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
@@ -1542,7 +1543,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200502151255/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200503142012/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1561,7 +1562,7 @@
     <t xml:space="preserve">United Kingdom - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200501173458/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200503142018/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
@@ -1584,7 +1585,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200501173558/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200503142022/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
   </si>
   <si>
     <t xml:space="preserve">The number of tests performed, including tests posted or delivered but not yet returned and/or processed.</t>
@@ -1652,7 +1653,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-12</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-13</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2176,7 +2177,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -2186,25 +2187,25 @@
       </c>
       <c r="E4"/>
       <c r="F4" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G4" t="n">
-        <v>269619</v>
+        <v>274355</v>
       </c>
       <c r="H4" t="n">
-        <v>29.936</v>
+        <v>30.462</v>
       </c>
       <c r="I4" t="n">
-        <v>5540</v>
+        <v>4736</v>
       </c>
       <c r="J4" t="n">
-        <v>0.615</v>
+        <v>0.526</v>
       </c>
       <c r="K4" t="n">
-        <v>7288.333</v>
+        <v>5985.333</v>
       </c>
       <c r="L4" t="n">
-        <v>0.809</v>
+        <v>0.665</v>
       </c>
       <c r="M4" t="s">
         <v>30</v>
@@ -2224,7 +2225,7 @@
         <v>34</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -2234,25 +2235,25 @@
       </c>
       <c r="E5"/>
       <c r="F5" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G5" t="n">
-        <v>138278</v>
+        <v>143030</v>
       </c>
       <c r="H5" t="n">
-        <v>81.264</v>
+        <v>84.057</v>
       </c>
       <c r="I5" t="n">
-        <v>4196</v>
+        <v>4752</v>
       </c>
       <c r="J5" t="n">
-        <v>2.466</v>
+        <v>2.793</v>
       </c>
       <c r="K5" t="n">
-        <v>3791</v>
+        <v>4445.333</v>
       </c>
       <c r="L5" t="n">
-        <v>2.228</v>
+        <v>2.613</v>
       </c>
       <c r="M5" t="s">
         <v>37</v>
@@ -2360,7 +2361,7 @@
         <v>52</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C8" t="s">
         <v>53</v>
@@ -2370,25 +2371,25 @@
       </c>
       <c r="E8"/>
       <c r="F8" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G8" t="n">
-        <v>327653</v>
+        <v>347936</v>
       </c>
       <c r="H8" t="n">
-        <v>28.271</v>
+        <v>30.021</v>
       </c>
       <c r="I8" t="n">
-        <v>20718</v>
+        <v>21165</v>
       </c>
       <c r="J8" t="n">
-        <v>1.788</v>
+        <v>1.826</v>
       </c>
       <c r="K8" t="n">
-        <v>19130</v>
+        <v>20849</v>
       </c>
       <c r="L8" t="n">
-        <v>1.651</v>
+        <v>1.799</v>
       </c>
       <c r="M8" t="s">
         <v>54</v>
@@ -2408,7 +2409,7 @@
         <v>58</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C9" t="s">
         <v>59</v>
@@ -2420,21 +2421,25 @@
         <v>60</v>
       </c>
       <c r="F9" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G9" t="n">
-        <v>6613</v>
+        <v>7556</v>
       </c>
       <c r="H9" t="n">
-        <v>0.567</v>
-      </c>
-      <c r="I9"/>
+        <v>0.647</v>
+      </c>
+      <c r="I9" t="n">
+        <v>943</v>
+      </c>
       <c r="J9" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="K9"/>
+        <v>0.081</v>
+      </c>
+      <c r="K9" t="n">
+        <v>382.333</v>
+      </c>
       <c r="L9" t="n">
-        <v>0.014</v>
+        <v>0.033</v>
       </c>
       <c r="M9" t="s">
         <v>36</v>
@@ -2454,7 +2459,7 @@
         <v>64</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C10" t="s">
         <v>65</v>
@@ -2464,19 +2469,19 @@
       </c>
       <c r="E10"/>
       <c r="F10" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G10" t="n">
-        <v>47636</v>
+        <v>48618</v>
       </c>
       <c r="H10" t="n">
-        <v>6.856</v>
+        <v>6.997</v>
       </c>
       <c r="I10" t="n">
-        <v>1126</v>
+        <v>982</v>
       </c>
       <c r="J10" t="n">
-        <v>0.162</v>
+        <v>0.141</v>
       </c>
       <c r="K10"/>
       <c r="L10"/>
@@ -2498,7 +2503,7 @@
         <v>70</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>43952</v>
+        <v>43954</v>
       </c>
       <c r="C11" t="s">
         <v>71</v>
@@ -2508,26 +2513,18 @@
       </c>
       <c r="E11"/>
       <c r="F11" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G11" t="n">
-        <v>832222</v>
+        <v>862080</v>
       </c>
       <c r="H11" t="n">
-        <v>22.05</v>
-      </c>
-      <c r="I11" t="n">
-        <v>43939</v>
-      </c>
-      <c r="J11" t="n">
-        <v>1.164</v>
-      </c>
-      <c r="K11" t="n">
-        <v>30454.333</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.807</v>
-      </c>
+        <v>22.841</v>
+      </c>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
       <c r="M11" t="s">
         <v>72</v>
       </c>
@@ -2546,7 +2543,7 @@
         <v>76</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C12" t="s">
         <v>77</v>
@@ -2558,25 +2555,25 @@
         <v>78</v>
       </c>
       <c r="F12" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G12" t="n">
-        <v>189433</v>
+        <v>199400</v>
       </c>
       <c r="H12" t="n">
-        <v>9.91</v>
+        <v>10.431</v>
       </c>
       <c r="I12" t="n">
-        <v>8916</v>
+        <v>9967</v>
       </c>
       <c r="J12" t="n">
-        <v>0.466</v>
+        <v>0.521</v>
       </c>
       <c r="K12" t="n">
-        <v>7756</v>
+        <v>8927</v>
       </c>
       <c r="L12" t="n">
-        <v>0.406</v>
+        <v>0.467</v>
       </c>
       <c r="M12" t="s">
         <v>79</v>
@@ -2596,7 +2593,7 @@
         <v>82</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C13" t="s">
         <v>83</v>
@@ -2606,25 +2603,25 @@
       </c>
       <c r="E13"/>
       <c r="F13" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G13" t="n">
-        <v>108950</v>
+        <v>114602</v>
       </c>
       <c r="H13" t="n">
-        <v>2.141</v>
+        <v>2.252</v>
       </c>
       <c r="I13" t="n">
-        <v>4293</v>
+        <v>5652</v>
       </c>
       <c r="J13" t="n">
-        <v>0.084</v>
+        <v>0.111</v>
       </c>
       <c r="K13" t="n">
-        <v>4621.667</v>
+        <v>4816.333</v>
       </c>
       <c r="L13" t="n">
-        <v>0.091</v>
+        <v>0.095</v>
       </c>
       <c r="M13" t="s">
         <v>84</v>
@@ -2644,7 +2641,7 @@
         <v>88</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C14" t="s">
         <v>89</v>
@@ -2654,25 +2651,25 @@
       </c>
       <c r="E14"/>
       <c r="F14" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G14" t="n">
-        <v>9502</v>
+        <v>9593</v>
       </c>
       <c r="H14" t="n">
-        <v>1.865</v>
+        <v>1.883</v>
       </c>
       <c r="I14" t="n">
-        <v>167</v>
+        <v>91</v>
       </c>
       <c r="J14" t="n">
-        <v>0.033</v>
+        <v>0.018</v>
       </c>
       <c r="K14" t="n">
-        <v>171</v>
+        <v>122.333</v>
       </c>
       <c r="L14" t="n">
-        <v>0.034</v>
+        <v>0.024</v>
       </c>
       <c r="M14" t="s">
         <v>90</v>
@@ -2692,7 +2689,7 @@
         <v>93</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C15" t="s">
         <v>94</v>
@@ -2702,16 +2699,20 @@
       </c>
       <c r="E15"/>
       <c r="F15" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G15" t="n">
-        <v>37557</v>
+        <v>38084</v>
       </c>
       <c r="H15" t="n">
-        <v>9.148</v>
-      </c>
-      <c r="I15"/>
-      <c r="J15"/>
+        <v>9.277</v>
+      </c>
+      <c r="I15" t="n">
+        <v>527</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.128</v>
+      </c>
       <c r="K15"/>
       <c r="L15"/>
       <c r="M15" t="s">
@@ -2732,7 +2733,7 @@
         <v>99</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C16" t="s">
         <v>100</v>
@@ -2744,25 +2745,25 @@
         <v>102</v>
       </c>
       <c r="F16" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G16" t="n">
-        <v>49409</v>
+        <v>51506</v>
       </c>
       <c r="H16" t="n">
-        <v>4.362</v>
+        <v>4.547</v>
       </c>
       <c r="I16" t="n">
-        <v>2062</v>
+        <v>2097</v>
       </c>
       <c r="J16" t="n">
-        <v>0.182</v>
+        <v>0.185</v>
       </c>
       <c r="K16" t="n">
-        <v>1967</v>
+        <v>2054</v>
       </c>
       <c r="L16" t="n">
-        <v>0.174</v>
+        <v>0.181</v>
       </c>
       <c r="M16" t="s">
         <v>101</v>
@@ -2782,7 +2783,7 @@
         <v>105</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C17" t="s">
         <v>106</v>
@@ -2792,25 +2793,25 @@
       </c>
       <c r="E17"/>
       <c r="F17" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G17" t="n">
-        <v>253826</v>
+        <v>257678</v>
       </c>
       <c r="H17" t="n">
-        <v>23.702</v>
+        <v>24.062</v>
       </c>
       <c r="I17" t="n">
-        <v>4192</v>
+        <v>3862</v>
       </c>
       <c r="J17" t="n">
-        <v>0.391</v>
+        <v>0.361</v>
       </c>
       <c r="K17" t="n">
-        <v>6253.667</v>
+        <v>5098</v>
       </c>
       <c r="L17" t="n">
-        <v>0.584</v>
+        <v>0.476</v>
       </c>
       <c r="M17" t="s">
         <v>36</v>
@@ -2876,7 +2877,7 @@
         <v>116</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>43951</v>
+        <v>43953</v>
       </c>
       <c r="C19" t="s">
         <v>117</v>
@@ -2888,25 +2889,25 @@
         <v>119</v>
       </c>
       <c r="F19" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G19" t="n">
-        <v>52848</v>
+        <v>38924</v>
       </c>
       <c r="H19" t="n">
-        <v>2.995</v>
+        <v>2.206</v>
       </c>
       <c r="I19" t="n">
-        <v>663</v>
+        <v>1863</v>
       </c>
       <c r="J19" t="n">
-        <v>0.038</v>
+        <v>0.106</v>
       </c>
       <c r="K19" t="n">
-        <v>1518.667</v>
+        <v>1746.667</v>
       </c>
       <c r="L19" t="n">
-        <v>0.086</v>
+        <v>0.099</v>
       </c>
       <c r="M19" t="s">
         <v>118</v>
@@ -2968,7 +2969,7 @@
         <v>127</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C21" t="s">
         <v>128</v>
@@ -2978,25 +2979,25 @@
       </c>
       <c r="E21"/>
       <c r="F21" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G21" t="n">
-        <v>54464</v>
+        <v>55206</v>
       </c>
       <c r="H21" t="n">
-        <v>41.057</v>
+        <v>41.617</v>
       </c>
       <c r="I21" t="n">
-        <v>697</v>
+        <v>743</v>
       </c>
       <c r="J21" t="n">
-        <v>0.525</v>
+        <v>0.56</v>
       </c>
       <c r="K21" t="n">
-        <v>1096.333</v>
+        <v>823.333</v>
       </c>
       <c r="L21" t="n">
-        <v>0.826</v>
+        <v>0.62</v>
       </c>
       <c r="M21" t="s">
         <v>130</v>
@@ -3064,7 +3065,7 @@
         <v>139</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C23" t="s">
         <v>140</v>
@@ -3074,21 +3075,25 @@
       </c>
       <c r="E23"/>
       <c r="F23" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G23" t="n">
-        <v>97593</v>
+        <v>101750</v>
       </c>
       <c r="H23" t="n">
-        <v>17.614</v>
-      </c>
-      <c r="I23"/>
+        <v>18.364</v>
+      </c>
+      <c r="I23" t="n">
+        <v>2153</v>
+      </c>
       <c r="J23" t="n">
-        <v>0.187</v>
-      </c>
-      <c r="K23"/>
+        <v>0.389</v>
+      </c>
+      <c r="K23" t="n">
+        <v>2860</v>
+      </c>
       <c r="L23" t="n">
-        <v>0.445</v>
+        <v>0.516</v>
       </c>
       <c r="M23" t="s">
         <v>142</v>
@@ -3316,7 +3321,7 @@
         <v>176</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C29" t="s">
         <v>177</v>
@@ -3328,25 +3333,25 @@
         <v>179</v>
       </c>
       <c r="F29" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G29" t="n">
-        <v>79551</v>
+        <v>82010</v>
       </c>
       <c r="H29" t="n">
-        <v>8.235</v>
+        <v>8.489</v>
       </c>
       <c r="I29" t="n">
-        <v>3220</v>
+        <v>2459</v>
       </c>
       <c r="J29" t="n">
-        <v>0.333</v>
+        <v>0.255</v>
       </c>
       <c r="K29" t="n">
-        <v>3083.667</v>
+        <v>3019.667</v>
       </c>
       <c r="L29" t="n">
-        <v>0.319</v>
+        <v>0.313</v>
       </c>
       <c r="M29" t="s">
         <v>178</v>
@@ -3366,7 +3371,7 @@
         <v>183</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C30" t="s">
         <v>184</v>
@@ -3376,25 +3381,21 @@
       </c>
       <c r="E30"/>
       <c r="F30" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G30" t="n">
-        <v>49961</v>
+        <v>50365</v>
       </c>
       <c r="H30" t="n">
-        <v>146.406</v>
-      </c>
-      <c r="I30" t="n">
-        <v>867</v>
-      </c>
+        <v>147.59</v>
+      </c>
+      <c r="I30"/>
       <c r="J30" t="n">
-        <v>2.541</v>
-      </c>
-      <c r="K30" t="n">
-        <v>809.667</v>
-      </c>
+        <v>1.184</v>
+      </c>
+      <c r="K30"/>
       <c r="L30" t="n">
-        <v>2.373</v>
+        <v>1.947</v>
       </c>
       <c r="M30" t="s">
         <v>185</v>
@@ -3460,7 +3461,7 @@
         <v>193</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C32" t="s">
         <v>189</v>
@@ -3472,25 +3473,25 @@
         <v>191</v>
       </c>
       <c r="F32" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G32" t="n">
-        <v>976363</v>
+        <v>1046450</v>
       </c>
       <c r="H32" t="n">
-        <v>0.708</v>
+        <v>0.758</v>
       </c>
       <c r="I32" t="n">
-        <v>73709</v>
+        <v>70087</v>
       </c>
       <c r="J32" t="n">
-        <v>0.053</v>
+        <v>0.051</v>
       </c>
       <c r="K32" t="n">
-        <v>68533</v>
+        <v>72083</v>
       </c>
       <c r="L32" t="n">
-        <v>0.05</v>
+        <v>0.052</v>
       </c>
       <c r="M32" t="s">
         <v>190</v>
@@ -3510,7 +3511,7 @@
         <v>194</v>
       </c>
       <c r="B33" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C33" t="s">
         <v>195</v>
@@ -3520,25 +3521,25 @@
       </c>
       <c r="E33"/>
       <c r="F33" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G33" t="n">
-        <v>79868</v>
+        <v>83012</v>
       </c>
       <c r="H33" t="n">
-        <v>0.292</v>
+        <v>0.303</v>
       </c>
       <c r="I33" t="n">
-        <v>3330</v>
+        <v>3144</v>
       </c>
       <c r="J33" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="K33" t="n">
-        <v>4028</v>
+        <v>3553.667</v>
       </c>
       <c r="L33" t="n">
-        <v>0.015</v>
+        <v>0.013</v>
       </c>
       <c r="M33" t="s">
         <v>196</v>
@@ -3692,7 +3693,7 @@
         <v>215</v>
       </c>
       <c r="B37" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C37" t="s">
         <v>216</v>
@@ -3704,25 +3705,25 @@
         <v>218</v>
       </c>
       <c r="F37" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G37" t="n">
-        <v>1398633</v>
+        <v>1429864</v>
       </c>
       <c r="H37" t="n">
-        <v>23.132</v>
+        <v>23.649</v>
       </c>
       <c r="I37" t="n">
-        <v>43732</v>
+        <v>31231</v>
       </c>
       <c r="J37" t="n">
-        <v>0.723</v>
+        <v>0.517</v>
       </c>
       <c r="K37" t="n">
-        <v>41254</v>
+        <v>38801.333</v>
       </c>
       <c r="L37" t="n">
-        <v>0.682</v>
+        <v>0.642</v>
       </c>
       <c r="M37" t="s">
         <v>219</v>
@@ -3742,7 +3743,7 @@
         <v>222</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C38" t="s">
         <v>216</v>
@@ -3754,25 +3755,25 @@
         <v>218</v>
       </c>
       <c r="F38" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G38" t="n">
-        <v>2053425</v>
+        <v>2108837</v>
       </c>
       <c r="H38" t="n">
-        <v>33.962</v>
+        <v>34.879</v>
       </c>
       <c r="I38" t="n">
-        <v>74208</v>
+        <v>55412</v>
       </c>
       <c r="J38" t="n">
-        <v>1.227</v>
+        <v>0.916</v>
       </c>
       <c r="K38" t="n">
-        <v>68830.333</v>
+        <v>66025.333</v>
       </c>
       <c r="L38" t="n">
-        <v>1.138</v>
+        <v>1.092</v>
       </c>
       <c r="M38" t="s">
         <v>219</v>
@@ -3792,7 +3793,7 @@
         <v>224</v>
       </c>
       <c r="B39" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C39" t="s">
         <v>225</v>
@@ -3804,13 +3805,13 @@
         <v>227</v>
       </c>
       <c r="F39" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G39" t="n">
-        <v>181527</v>
+        <v>183251</v>
       </c>
       <c r="H39" t="n">
-        <v>1.435</v>
+        <v>1.449</v>
       </c>
       <c r="I39"/>
       <c r="J39"/>
@@ -3834,7 +3835,7 @@
         <v>230</v>
       </c>
       <c r="B40" s="1" t="n">
-        <v>43949</v>
+        <v>43951</v>
       </c>
       <c r="C40" t="s">
         <v>231</v>
@@ -3846,25 +3847,25 @@
         <v>232</v>
       </c>
       <c r="F40" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G40" t="n">
-        <v>254703</v>
+        <v>273854</v>
       </c>
       <c r="H40" t="n">
-        <v>2.014</v>
+        <v>2.165</v>
       </c>
       <c r="I40" t="n">
-        <v>4149</v>
+        <v>6636</v>
       </c>
       <c r="J40" t="n">
-        <v>0.033</v>
+        <v>0.052</v>
       </c>
       <c r="K40" t="n">
-        <v>4564.333</v>
+        <v>7305</v>
       </c>
       <c r="L40" t="n">
-        <v>0.036</v>
+        <v>0.058</v>
       </c>
       <c r="M40" t="s">
         <v>226</v>
@@ -3980,7 +3981,7 @@
         <v>244</v>
       </c>
       <c r="B43" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C43" t="s">
         <v>245</v>
@@ -3992,25 +3993,25 @@
         <v>247</v>
       </c>
       <c r="F43" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G43" t="n">
-        <v>63102</v>
+        <v>64245</v>
       </c>
       <c r="H43" t="n">
-        <v>33.455</v>
+        <v>34.061</v>
       </c>
       <c r="I43" t="n">
-        <v>1982</v>
+        <v>1143</v>
       </c>
       <c r="J43" t="n">
-        <v>1.051</v>
+        <v>0.606</v>
       </c>
       <c r="K43" t="n">
-        <v>2763.667</v>
+        <v>2119.667</v>
       </c>
       <c r="L43" t="n">
-        <v>1.465</v>
+        <v>1.124</v>
       </c>
       <c r="M43" t="s">
         <v>246</v>
@@ -4030,7 +4031,7 @@
         <v>249</v>
       </c>
       <c r="B44" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C44" t="s">
         <v>250</v>
@@ -4040,25 +4041,25 @@
       </c>
       <c r="E44"/>
       <c r="F44" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G44" t="n">
-        <v>138270</v>
+        <v>141678</v>
       </c>
       <c r="H44" t="n">
-        <v>50.792</v>
+        <v>52.044</v>
       </c>
       <c r="I44" t="n">
-        <v>5502</v>
+        <v>3408</v>
       </c>
       <c r="J44" t="n">
-        <v>2.021</v>
+        <v>1.252</v>
       </c>
       <c r="K44" t="n">
-        <v>6689.667</v>
+        <v>5374.333</v>
       </c>
       <c r="L44" t="n">
-        <v>2.457</v>
+        <v>1.974</v>
       </c>
       <c r="M44" t="s">
         <v>36</v>
@@ -4126,7 +4127,7 @@
         <v>258</v>
       </c>
       <c r="B46" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C46" t="s">
         <v>259</v>
@@ -4136,19 +4137,19 @@
       </c>
       <c r="E46"/>
       <c r="F46" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G46" t="n">
-        <v>184213</v>
+        <v>195833</v>
       </c>
       <c r="H46" t="n">
-        <v>5.692</v>
+        <v>6.051</v>
       </c>
       <c r="I46" t="n">
-        <v>15429</v>
+        <v>11620</v>
       </c>
       <c r="J46" t="n">
-        <v>0.477</v>
+        <v>0.359</v>
       </c>
       <c r="K46"/>
       <c r="L46"/>
@@ -4183,18 +4184,18 @@
         <v>122</v>
       </c>
       <c r="G47" t="n">
-        <v>75742</v>
+        <v>79255</v>
       </c>
       <c r="H47" t="n">
-        <v>0.587</v>
+        <v>0.615</v>
       </c>
       <c r="I47"/>
       <c r="J47" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K47"/>
       <c r="L47" t="n">
-        <v>0.003</v>
+        <v>0.008</v>
       </c>
       <c r="M47" t="s">
         <v>266</v>
@@ -4314,7 +4315,7 @@
         <v>280</v>
       </c>
       <c r="B50" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C50" t="s">
         <v>281</v>
@@ -4326,25 +4327,25 @@
         <v>283</v>
       </c>
       <c r="F50" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G50" t="n">
-        <v>12577</v>
+        <v>13098</v>
       </c>
       <c r="H50" t="n">
-        <v>0.432</v>
+        <v>0.45</v>
       </c>
       <c r="I50" t="n">
-        <v>566</v>
+        <v>521</v>
       </c>
       <c r="J50" t="n">
-        <v>0.019</v>
+        <v>0.018</v>
       </c>
       <c r="K50" t="n">
-        <v>590</v>
+        <v>524.667</v>
       </c>
       <c r="L50" t="n">
-        <v>0.02</v>
+        <v>0.018</v>
       </c>
       <c r="M50" t="s">
         <v>282</v>
@@ -4412,7 +4413,7 @@
         <v>292</v>
       </c>
       <c r="B52" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C52" t="s">
         <v>293</v>
@@ -4422,25 +4423,25 @@
       </c>
       <c r="E52"/>
       <c r="F52" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G52" t="n">
-        <v>145589</v>
+        <v>150223</v>
       </c>
       <c r="H52" t="n">
-        <v>30.191</v>
+        <v>31.152</v>
       </c>
       <c r="I52" t="n">
-        <v>5691</v>
+        <v>4634</v>
       </c>
       <c r="J52" t="n">
-        <v>1.18</v>
+        <v>0.961</v>
       </c>
       <c r="K52" t="n">
-        <v>5628.667</v>
+        <v>5217.667</v>
       </c>
       <c r="L52" t="n">
-        <v>1.167</v>
+        <v>1.082</v>
       </c>
       <c r="M52" t="s">
         <v>294</v>
@@ -4460,7 +4461,7 @@
         <v>296</v>
       </c>
       <c r="B53" s="1" t="n">
-        <v>43952</v>
+        <v>43954</v>
       </c>
       <c r="C53" t="s">
         <v>297</v>
@@ -4470,13 +4471,13 @@
       </c>
       <c r="E53"/>
       <c r="F53" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G53" t="n">
-        <v>15759</v>
+        <v>16588</v>
       </c>
       <c r="H53" t="n">
-        <v>0.076</v>
+        <v>0.08</v>
       </c>
       <c r="I53"/>
       <c r="J53"/>
@@ -4548,7 +4549,7 @@
         <v>307</v>
       </c>
       <c r="B55" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C55" t="s">
         <v>308</v>
@@ -4558,25 +4559,25 @@
       </c>
       <c r="E55"/>
       <c r="F55" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G55" t="n">
-        <v>193859</v>
+        <v>203025</v>
       </c>
       <c r="H55" t="n">
-        <v>0.878</v>
+        <v>0.919</v>
       </c>
       <c r="I55" t="n">
-        <v>11728</v>
+        <v>9166</v>
       </c>
       <c r="J55" t="n">
-        <v>0.053</v>
+        <v>0.041</v>
       </c>
       <c r="K55" t="n">
-        <v>9316</v>
+        <v>9621.667</v>
       </c>
       <c r="L55" t="n">
-        <v>0.042</v>
+        <v>0.043</v>
       </c>
       <c r="M55" t="s">
         <v>309</v>
@@ -4596,7 +4597,7 @@
         <v>312</v>
       </c>
       <c r="B56" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C56" t="s">
         <v>313</v>
@@ -4608,25 +4609,25 @@
         <v>314</v>
       </c>
       <c r="F56" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G56" t="n">
-        <v>31895</v>
+        <v>33354</v>
       </c>
       <c r="H56" t="n">
-        <v>7.392</v>
+        <v>7.73</v>
       </c>
       <c r="I56" t="n">
-        <v>1146</v>
+        <v>1459</v>
       </c>
       <c r="J56" t="n">
-        <v>0.266</v>
+        <v>0.338</v>
       </c>
       <c r="K56" t="n">
-        <v>1033.333</v>
+        <v>1172.333</v>
       </c>
       <c r="L56" t="n">
-        <v>0.239</v>
+        <v>0.272</v>
       </c>
       <c r="M56" t="s">
         <v>36</v>
@@ -4696,7 +4697,7 @@
         <v>324</v>
       </c>
       <c r="B58" s="1" t="n">
-        <v>43952</v>
+        <v>43954</v>
       </c>
       <c r="C58" t="s">
         <v>325</v>
@@ -4706,22 +4707,18 @@
       </c>
       <c r="E58"/>
       <c r="F58" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G58" t="n">
-        <v>342498</v>
+        <v>355604</v>
       </c>
       <c r="H58" t="n">
-        <v>10.388</v>
+        <v>10.785</v>
       </c>
       <c r="I58"/>
-      <c r="J58" t="n">
-        <v>0.735</v>
-      </c>
+      <c r="J58"/>
       <c r="K58"/>
-      <c r="L58" t="n">
-        <v>1.041</v>
-      </c>
+      <c r="L58"/>
       <c r="M58" t="s">
         <v>326</v>
       </c>
@@ -4740,7 +4737,7 @@
         <v>330</v>
       </c>
       <c r="B59" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C59" t="s">
         <v>331</v>
@@ -4750,22 +4747,26 @@
       </c>
       <c r="E59"/>
       <c r="F59" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G59" t="n">
-        <v>97349</v>
+        <v>103197</v>
       </c>
       <c r="H59" t="n">
-        <v>0.888</v>
+        <v>0.942</v>
       </c>
       <c r="I59" t="n">
-        <v>3962</v>
+        <v>5848</v>
       </c>
       <c r="J59" t="n">
-        <v>0.036</v>
-      </c>
-      <c r="K59"/>
-      <c r="L59"/>
+        <v>0.053</v>
+      </c>
+      <c r="K59" t="n">
+        <v>4776</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0.043</v>
+      </c>
       <c r="M59" t="s">
         <v>172</v>
       </c>
@@ -4784,7 +4785,7 @@
         <v>334</v>
       </c>
       <c r="B60" s="1" t="n">
-        <v>43952</v>
+        <v>43954</v>
       </c>
       <c r="C60" t="s">
         <v>335</v>
@@ -4796,25 +4797,25 @@
         <v>337</v>
       </c>
       <c r="F60" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G60" t="n">
-        <v>354628</v>
+        <v>375948</v>
       </c>
       <c r="H60" t="n">
-        <v>9.37</v>
+        <v>9.933</v>
       </c>
       <c r="I60" t="n">
-        <v>16601</v>
+        <v>9935</v>
       </c>
       <c r="J60" t="n">
-        <v>0.439</v>
+        <v>0.263</v>
       </c>
       <c r="K60" t="n">
-        <v>14628</v>
+        <v>12640.333</v>
       </c>
       <c r="L60" t="n">
-        <v>0.387</v>
+        <v>0.334</v>
       </c>
       <c r="M60" t="s">
         <v>338</v>
@@ -4882,7 +4883,7 @@
         <v>346</v>
       </c>
       <c r="B62" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C62" t="s">
         <v>347</v>
@@ -4892,25 +4893,25 @@
       </c>
       <c r="E62"/>
       <c r="F62" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G62" t="n">
-        <v>101728</v>
+        <v>104435</v>
       </c>
       <c r="H62" t="n">
-        <v>35.309</v>
+        <v>36.249</v>
       </c>
       <c r="I62" t="n">
-        <v>4002</v>
+        <v>2707</v>
       </c>
       <c r="J62" t="n">
-        <v>1.389</v>
+        <v>0.94</v>
       </c>
       <c r="K62" t="n">
-        <v>3437.667</v>
+        <v>3311.667</v>
       </c>
       <c r="L62" t="n">
-        <v>1.193</v>
+        <v>1.15</v>
       </c>
       <c r="M62" t="s">
         <v>348</v>
@@ -4980,7 +4981,7 @@
         <v>356</v>
       </c>
       <c r="B64" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C64" t="s">
         <v>357</v>
@@ -4990,25 +4991,25 @@
       </c>
       <c r="E64"/>
       <c r="F64" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G64" t="n">
-        <v>3945518</v>
+        <v>4099999</v>
       </c>
       <c r="H64" t="n">
-        <v>27.036</v>
+        <v>28.095</v>
       </c>
       <c r="I64" t="n">
-        <v>221711</v>
+        <v>154481</v>
       </c>
       <c r="J64" t="n">
-        <v>1.519</v>
+        <v>1.059</v>
       </c>
       <c r="K64" t="n">
-        <v>213933.667</v>
+        <v>200563.667</v>
       </c>
       <c r="L64" t="n">
-        <v>1.466</v>
+        <v>1.374</v>
       </c>
       <c r="M64" t="s">
         <v>358</v>
@@ -5126,7 +5127,7 @@
         <v>374</v>
       </c>
       <c r="B67" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C67" t="s">
         <v>375</v>
@@ -5138,25 +5139,25 @@
         <v>376</v>
       </c>
       <c r="F67" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G67" t="n">
-        <v>91551</v>
+        <v>96637</v>
       </c>
       <c r="H67" t="n">
-        <v>13.454</v>
+        <v>14.202</v>
       </c>
       <c r="I67" t="n">
-        <v>5906</v>
+        <v>5086</v>
       </c>
       <c r="J67" t="n">
-        <v>0.868</v>
+        <v>0.747</v>
       </c>
       <c r="K67" t="n">
-        <v>6062.667</v>
+        <v>5898.333</v>
       </c>
       <c r="L67" t="n">
-        <v>0.891</v>
+        <v>0.867</v>
       </c>
       <c r="M67" t="s">
         <v>36</v>
@@ -5256,7 +5257,7 @@
         <v>384</v>
       </c>
       <c r="B70" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C70" t="s">
         <v>385</v>
@@ -5266,25 +5267,21 @@
       </c>
       <c r="E70"/>
       <c r="F70" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G70" t="n">
-        <v>94770</v>
+        <v>96220</v>
       </c>
       <c r="H70" t="n">
-        <v>17.358</v>
-      </c>
-      <c r="I70" t="n">
-        <v>3698</v>
-      </c>
+        <v>17.624</v>
+      </c>
+      <c r="I70"/>
       <c r="J70" t="n">
-        <v>0.677</v>
-      </c>
-      <c r="K70" t="n">
-        <v>4477.333</v>
-      </c>
+        <v>0.266</v>
+      </c>
+      <c r="K70"/>
       <c r="L70" t="n">
-        <v>0.82</v>
+        <v>0.629</v>
       </c>
       <c r="M70" t="s">
         <v>387</v>
@@ -5304,7 +5301,7 @@
         <v>391</v>
       </c>
       <c r="B71" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C71" t="s">
         <v>392</v>
@@ -5314,25 +5311,25 @@
       </c>
       <c r="E71"/>
       <c r="F71" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G71" t="n">
-        <v>55020</v>
+        <v>55520</v>
       </c>
       <c r="H71" t="n">
-        <v>26.466</v>
+        <v>26.706</v>
       </c>
       <c r="I71" t="n">
-        <v>720</v>
+        <v>500</v>
       </c>
       <c r="J71" t="n">
-        <v>0.346</v>
+        <v>0.241</v>
       </c>
       <c r="K71" t="n">
-        <v>1137.667</v>
+        <v>857.333</v>
       </c>
       <c r="L71" t="n">
-        <v>0.547</v>
+        <v>0.412</v>
       </c>
       <c r="M71" t="s">
         <v>394</v>
@@ -5352,7 +5349,7 @@
         <v>397</v>
       </c>
       <c r="B72" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C72" t="s">
         <v>398</v>
@@ -5364,25 +5361,25 @@
         <v>400</v>
       </c>
       <c r="F72" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G72" t="n">
-        <v>217522</v>
+        <v>230686</v>
       </c>
       <c r="H72" t="n">
-        <v>3.668</v>
+        <v>3.89</v>
       </c>
       <c r="I72" t="n">
-        <v>9992</v>
+        <v>13164</v>
       </c>
       <c r="J72" t="n">
-        <v>0.168</v>
+        <v>0.222</v>
       </c>
       <c r="K72" t="n">
-        <v>10675</v>
+        <v>11186.333</v>
       </c>
       <c r="L72" t="n">
-        <v>0.18</v>
+        <v>0.188</v>
       </c>
       <c r="M72" t="s">
         <v>399</v>
@@ -5402,7 +5399,7 @@
         <v>403</v>
       </c>
       <c r="B73" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C73" t="s">
         <v>404</v>
@@ -5412,25 +5409,25 @@
       </c>
       <c r="E73"/>
       <c r="F73" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G73" t="n">
-        <v>627562</v>
+        <v>630973</v>
       </c>
       <c r="H73" t="n">
-        <v>12.241</v>
+        <v>12.307</v>
       </c>
       <c r="I73" t="n">
-        <v>4493</v>
+        <v>3411</v>
       </c>
       <c r="J73" t="n">
-        <v>0.088</v>
+        <v>0.067</v>
       </c>
       <c r="K73" t="n">
-        <v>4455</v>
+        <v>3697.333</v>
       </c>
       <c r="L73" t="n">
-        <v>0.087</v>
+        <v>0.072</v>
       </c>
       <c r="M73" t="s">
         <v>405</v>
@@ -5450,7 +5447,7 @@
         <v>408</v>
       </c>
       <c r="B74" s="1" t="n">
-        <v>43944</v>
+        <v>43951</v>
       </c>
       <c r="C74" t="s">
         <v>409</v>
@@ -5462,13 +5459,13 @@
         <v>411</v>
       </c>
       <c r="F74" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G74" t="n">
-        <v>1035522</v>
+        <v>1351130</v>
       </c>
       <c r="H74" t="n">
-        <v>22.148</v>
+        <v>28.898</v>
       </c>
       <c r="I74"/>
       <c r="J74"/>
@@ -5576,7 +5573,7 @@
         <v>425</v>
       </c>
       <c r="B77" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C77" t="s">
         <v>426</v>
@@ -5586,25 +5583,25 @@
       </c>
       <c r="E77"/>
       <c r="F77" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G77" t="n">
-        <v>63713</v>
+        <v>64094</v>
       </c>
       <c r="H77" t="n">
-        <v>2.675</v>
+        <v>2.691</v>
       </c>
       <c r="I77" t="n">
-        <v>373</v>
+        <v>381</v>
       </c>
       <c r="J77" t="n">
         <v>0.016</v>
       </c>
       <c r="K77" t="n">
-        <v>448.333</v>
+        <v>416.667</v>
       </c>
       <c r="L77" t="n">
-        <v>0.019</v>
+        <v>0.018</v>
       </c>
       <c r="M77" t="s">
         <v>427</v>
@@ -5624,7 +5621,7 @@
         <v>431</v>
       </c>
       <c r="B78" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C78" t="s">
         <v>432</v>
@@ -5634,25 +5631,25 @@
       </c>
       <c r="E78"/>
       <c r="F78" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G78" t="n">
-        <v>72745</v>
+        <v>75268</v>
       </c>
       <c r="H78" t="n">
-        <v>1.042</v>
+        <v>1.078</v>
       </c>
       <c r="I78" t="n">
-        <v>2210</v>
+        <v>2523</v>
       </c>
       <c r="J78" t="n">
-        <v>0.032</v>
+        <v>0.036</v>
       </c>
       <c r="K78" t="n">
-        <v>3575.667</v>
+        <v>2965.667</v>
       </c>
       <c r="L78" t="n">
-        <v>0.051</v>
+        <v>0.043</v>
       </c>
       <c r="M78" t="s">
         <v>434</v>
@@ -5672,7 +5669,7 @@
         <v>437</v>
       </c>
       <c r="B79" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C79" t="s">
         <v>438</v>
@@ -5682,25 +5679,25 @@
       </c>
       <c r="E79"/>
       <c r="F79" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G79" t="n">
-        <v>23526</v>
+        <v>24055</v>
       </c>
       <c r="H79" t="n">
-        <v>1.991</v>
+        <v>2.035</v>
       </c>
       <c r="I79" t="n">
-        <v>569</v>
+        <v>529</v>
       </c>
       <c r="J79" t="n">
-        <v>0.048</v>
+        <v>0.045</v>
       </c>
       <c r="K79" t="n">
-        <v>683</v>
+        <v>664.333</v>
       </c>
       <c r="L79" t="n">
-        <v>0.058</v>
+        <v>0.056</v>
       </c>
       <c r="M79" t="s">
         <v>439</v>
@@ -5720,7 +5717,7 @@
         <v>443</v>
       </c>
       <c r="B80" s="1" t="n">
-        <v>43952</v>
+        <v>43954</v>
       </c>
       <c r="C80" t="s">
         <v>444</v>
@@ -5730,26 +5727,18 @@
       </c>
       <c r="E80"/>
       <c r="F80" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G80" t="n">
-        <v>1075048</v>
+        <v>1111366</v>
       </c>
       <c r="H80" t="n">
-        <v>12.747</v>
-      </c>
-      <c r="I80" t="n">
-        <v>41431</v>
-      </c>
-      <c r="J80" t="n">
-        <v>0.491</v>
-      </c>
-      <c r="K80" t="n">
-        <v>42311</v>
-      </c>
-      <c r="L80" t="n">
-        <v>0.502</v>
-      </c>
+        <v>13.177</v>
+      </c>
+      <c r="I80"/>
+      <c r="J80"/>
+      <c r="K80"/>
+      <c r="L80"/>
       <c r="M80" t="s">
         <v>445</v>
       </c>
@@ -5768,7 +5757,7 @@
         <v>449</v>
       </c>
       <c r="B81" s="1" t="n">
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="C81" t="s">
         <v>450</v>
@@ -5780,25 +5769,25 @@
         <v>452</v>
       </c>
       <c r="F81" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G81" t="n">
-        <v>31348</v>
+        <v>33802</v>
       </c>
       <c r="H81" t="n">
-        <v>0.685</v>
+        <v>0.739</v>
       </c>
       <c r="I81" t="n">
-        <v>2071</v>
+        <v>2454</v>
       </c>
       <c r="J81" t="n">
-        <v>0.045</v>
+        <v>0.054</v>
       </c>
       <c r="K81" t="n">
-        <v>2157.667</v>
+        <v>2175.667</v>
       </c>
       <c r="L81" t="n">
-        <v>0.047</v>
+        <v>0.048</v>
       </c>
       <c r="M81" t="s">
         <v>451</v>
@@ -5818,7 +5807,7 @@
         <v>455</v>
       </c>
       <c r="B82" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C82" t="s">
         <v>456</v>
@@ -5828,25 +5817,25 @@
       </c>
       <c r="E82"/>
       <c r="F82" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G82" t="n">
-        <v>122752</v>
+        <v>129723</v>
       </c>
       <c r="H82" t="n">
-        <v>2.807</v>
+        <v>2.966</v>
       </c>
       <c r="I82" t="n">
-        <v>4207</v>
+        <v>6971</v>
       </c>
       <c r="J82" t="n">
-        <v>0.096</v>
+        <v>0.159</v>
       </c>
       <c r="K82" t="n">
-        <v>6069.333</v>
+        <v>5954.667</v>
       </c>
       <c r="L82" t="n">
-        <v>0.139</v>
+        <v>0.136</v>
       </c>
       <c r="M82" t="s">
         <v>457</v>
@@ -5866,7 +5855,7 @@
         <v>461</v>
       </c>
       <c r="B83" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C83" t="s">
         <v>462</v>
@@ -5876,25 +5865,25 @@
       </c>
       <c r="E83"/>
       <c r="F83" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G83" t="n">
-        <v>762279</v>
+        <v>825946</v>
       </c>
       <c r="H83" t="n">
-        <v>11.229</v>
+        <v>12.167</v>
       </c>
       <c r="I83" t="n">
-        <v>73191</v>
+        <v>63667</v>
       </c>
       <c r="J83" t="n">
-        <v>1.078</v>
+        <v>0.938</v>
       </c>
       <c r="K83" t="n">
-        <v>53740.333</v>
+        <v>63811</v>
       </c>
       <c r="L83" t="n">
-        <v>0.792</v>
+        <v>0.94</v>
       </c>
       <c r="M83" t="s">
         <v>463</v>
@@ -5914,7 +5903,7 @@
         <v>466</v>
       </c>
       <c r="B84" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C84" t="s">
         <v>467</v>
@@ -5924,25 +5913,25 @@
       </c>
       <c r="E84"/>
       <c r="F84" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G84" t="n">
-        <v>1023824</v>
+        <v>1129907</v>
       </c>
       <c r="H84" t="n">
-        <v>15.082</v>
+        <v>16.644</v>
       </c>
       <c r="I84" t="n">
-        <v>122347</v>
+        <v>105937</v>
       </c>
       <c r="J84" t="n">
-        <v>1.802</v>
+        <v>1.561</v>
       </c>
       <c r="K84" t="n">
-        <v>85462.333</v>
+        <v>103298.333</v>
       </c>
       <c r="L84" t="n">
-        <v>1.259</v>
+        <v>1.522</v>
       </c>
       <c r="M84" t="s">
         <v>463</v>
@@ -5962,7 +5951,7 @@
         <v>470</v>
       </c>
       <c r="B85" s="1" t="n">
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="C85" t="s">
         <v>471</v>
@@ -5972,25 +5961,25 @@
       </c>
       <c r="E85"/>
       <c r="F85" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G85" t="n">
-        <v>6551810</v>
+        <v>6816347</v>
       </c>
       <c r="H85" t="n">
-        <v>19.794</v>
+        <v>20.593</v>
       </c>
       <c r="I85" t="n">
-        <v>305118</v>
+        <v>264537</v>
       </c>
       <c r="J85" t="n">
-        <v>0.922</v>
+        <v>0.799</v>
       </c>
       <c r="K85" t="n">
-        <v>252027.333</v>
+        <v>263392.333</v>
       </c>
       <c r="L85" t="n">
-        <v>0.761</v>
+        <v>0.796</v>
       </c>
       <c r="M85" t="s">
         <v>472</v>
@@ -6010,7 +5999,7 @@
         <v>476</v>
       </c>
       <c r="B86" s="1" t="n">
-        <v>43944</v>
+        <v>43945</v>
       </c>
       <c r="C86" t="s">
         <v>477</v>
@@ -6020,25 +6009,25 @@
       </c>
       <c r="E86"/>
       <c r="F86" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G86" t="n">
-        <v>498015</v>
+        <v>526054</v>
       </c>
       <c r="H86" t="n">
-        <v>1.505</v>
+        <v>1.589</v>
       </c>
       <c r="I86" t="n">
-        <v>21420</v>
+        <v>23835</v>
       </c>
       <c r="J86" t="n">
-        <v>0.065</v>
+        <v>0.072</v>
       </c>
       <c r="K86" t="n">
-        <v>19322</v>
+        <v>22180.333</v>
       </c>
       <c r="L86" t="n">
-        <v>0.058</v>
+        <v>0.067</v>
       </c>
       <c r="M86" t="s">
         <v>479</v>
@@ -6058,7 +6047,7 @@
         <v>483</v>
       </c>
       <c r="B87" s="1" t="n">
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="C87" t="s">
         <v>484</v>
@@ -6068,25 +6057,25 @@
       </c>
       <c r="E87"/>
       <c r="F87" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G87" t="n">
-        <v>20554</v>
+        <v>21164</v>
       </c>
       <c r="H87" t="n">
-        <v>5.917</v>
+        <v>6.093</v>
       </c>
       <c r="I87" t="n">
-        <v>807</v>
+        <v>610</v>
       </c>
       <c r="J87" t="n">
-        <v>0.232</v>
+        <v>0.176</v>
       </c>
       <c r="K87" t="n">
-        <v>804.667</v>
+        <v>716</v>
       </c>
       <c r="L87" t="n">
-        <v>0.231</v>
+        <v>0.206</v>
       </c>
       <c r="M87" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-05-08
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="594">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -98,7 +98,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/05/coronavirus-covid-19-at-a-glance-6-may-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/05/coronavirus-covid-19-at-a-glance-7-may-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175135/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200508085522/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175139/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200508130052/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -193,7 +193,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-4-maya-vyzdoroveli-i-vypisany-3259-patsientov/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-7-maya-vyzdoroveli-i-vypisany-5067-patsientov/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -247,7 +247,7 @@
   </si>
   <si>
     <t xml:space="preserve">Official testing data from the Bolivian Ministry of Health is reported in [this dashboard](https://www.boliviasegura.gob.bo/datos-oficiales), which provides a breakdown of the cumulative number of confirmed, suspected, and discarded cases to date along with the number of deaths and recoveries. We assume that the number of discarded cases ("casos descartados") refers to the number of cases with negative test results. Under this assumption, we measure the total number of cases tested to date as the sum of the number of confirmed and discarded cases.
-Unfortunately, the official dashboard does not provide a time series of the number of cases tested each day since testing began. Instead, the dashboard only displays a daily snapshot of the total cases tested to date. Since we did not begin monitoring this dashboard until April 15th 2020, we construct a time series dating back to March 21st 2020 using data provided in [this unofficial Github repository](https://github.com/mauforonda/covid19-bolivia), which we have cross-referenced against data in the official dashboard for a sample of dates.</t>
+Unfortunately, the official dashboard does not provide a time series of the number of cases tested each day since testing began. Instead, the dashboard only displays a daily snapshot of the total cases tested to date. Since we did not begin monitoring this dashboard until April 15th 2020, we construct a time series dating back to March 21st 2020 using data provided in [this unofficial GitHub repository](https://github.com/mauforonda/covid19-bolivia), which we have cross-referenced against data in the official dashboard for a sample of dates.</t>
   </si>
   <si>
     <t xml:space="preserve">BRA</t>
@@ -277,7 +277,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175144/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200508085527/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -300,7 +300,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175147/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200508085529/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -336,7 +336,7 @@
     <t xml:space="preserve">https://www.gob.cl/coronavirus/cifrasoficiales/#reportes</t>
   </si>
   <si>
-    <t xml:space="preserve">The Government of Chile release daily reports that include cumulative and daily totals for the number of PCR tests performed across private and public medical establishments. This data is collected by volunteers and [published on Github](https://github.com/jorgeperezrojas/covid19-data). We take our figures from this GitHub, which we regularly audit for accuracy.</t>
+    <t xml:space="preserve">The Government of Chile release daily reports that include cumulative and daily totals for the number of PCR tests performed across private and public medical establishments. This data is collected by volunteers and [published on GitHub](https://github.com/jorgeperezrojas/covid19-data). We take our figures from this GitHub, which we regularly audit for accuracy.</t>
   </si>
   <si>
     <t xml:space="preserve">COL</t>
@@ -388,7 +388,7 @@
     <t xml:space="preserve">Croatia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175452/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200508130102/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -448,7 +448,7 @@
     <t xml:space="preserve">Denmark - People tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/COVID19-overvaagningsrapport-06052020-pp5f</t>
+    <t xml:space="preserve">https://files.ssi.dk/COVID19-overvaagningsrapport-07052020-8t4k</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -475,7 +475,7 @@
     <t xml:space="preserve">Ecuador - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/05/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-04052020-08h00.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/05/INFOGRAFIA-NACIONALCOVI-19-69-COE-NACIONAL-06052020-08h00-2.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -504,7 +504,7 @@
     <t xml:space="preserve">Government of El Salvador</t>
   </si>
   <si>
-    <t xml:space="preserve">updated at 12:10am local time on 2020-05-06.</t>
+    <t xml:space="preserve">updated at 10:35pm local time on 2020-05-06.</t>
   </si>
   <si>
     <t xml:space="preserve">The government of El Salvador publishes an online dashboard with figures and graphs about the epidemic, including the number of tests performed ("pruebas COVID19 realizadas hasta hoy"). No information is given on the geographical scope and number of labs included.</t>
@@ -541,7 +541,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_May-6_-ENG-V4-1.pdf</t>
+    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_May-8_-ENG-V5.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -585,7 +585,7 @@
     <t xml:space="preserve">France - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.santepubliquefrance.fr/content/download/249184/2589560</t>
+    <t xml:space="preserve">https://www.santepubliquefrance.fr/content/download/250807/2596023</t>
   </si>
   <si>
     <t xml:space="preserve">Agence nationale de santé publique</t>
@@ -669,7 +669,7 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200506/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200507/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -771,7 +771,7 @@
   </si>
   <si>
     <t xml:space="preserve">The ICMR reports separate figures for both “samples tested” and “people tested” at press conferences and in press releases (shown separately in the charts above). No other details are provided.
-The press releases from ICMR do not always stay online for very long. The reason for this is unknown, but the releases are being backed up at this [Github repository](https://github.com/datameet/covid19).
+The press releases from ICMR do not always stay online for very long. The reason for this is unknown, but the releases are being backed up at this [GitHub repository](https://github.com/datameet/covid19).
 On some occasions there appear to have been more than one update released per day. Where we are aware of multiple observations for the day, we show the number for the earlier release.</t>
   </si>
   <si>
@@ -804,7 +804,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200506141329/http://irangov.ir/detail/338787</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200507141927/http://irangov.ir/detail/338841</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -856,7 +856,7 @@
     <t xml:space="preserve">https://t.me/s/MOHreport</t>
   </si>
   <si>
-    <t xml:space="preserve">The Israel Ministry of Health publishes COVID-19 updates on its official channel on Telegram. This data is published in a format that is extremely challenging to collect. We rely on the data as collected and made available [on Github](https://github.com/idandrd/israel-covid19-data/blob/master/Corona-Tests.csv).
+    <t xml:space="preserve">The Israel Ministry of Health publishes COVID-19 updates on its official channel on Telegram. This data is published in a format that is extremely challenging to collect. We rely on the data as collected and made available [on GitHub](https://github.com/idandrd/israel-covid19-data/blob/master/Corona-Tests.csv).
 On 19 April 2020, the person who maintains the GitHub repository confirmed to us that the units refer to the number of tests performed, after checking the information with the Ministry of Health.
 No further information on the geographical scope, number of labs, or types of test included are known.</t>
   </si>
@@ -924,7 +924,7 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000627634.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000628517.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Implementation status of PCR tests for new coronavirus in Japan (based on the date on which the results were determined). Preliminary data</t>
@@ -999,7 +999,7 @@
     <t xml:space="preserve">Lithuania - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175614/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200508085626/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -1015,7 +1015,7 @@
     <t xml:space="preserve">Luxembourg - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175621/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200507200422/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg Government situation update</t>
@@ -1036,7 +1036,7 @@
     <t xml:space="preserve">Malaysia - cases tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175630/https://www.moh.gov.my/index.php/pages/view/2019-ncov-wuhan</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200508130208/https://www.moh.gov.my/index.php/pages/view/2019-ncov-wuhan</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1145,10 +1145,10 @@
     <t xml:space="preserve">Netherlands - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-05/COVID-19_WebSite_rapport_20200506_1112.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 6 May 2020 update</t>
+    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-05/COVID-19_WebSite_rapport_20200507_1337_0.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 7 May 2020 update</t>
   </si>
   <si>
     <t xml:space="preserve">Dutch National Institute for Public Health and the Environment</t>
@@ -1184,7 +1184,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506175710/https://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200507200512/https://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1204,7 +1204,7 @@
     <t xml:space="preserve">Norway - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.05.06-dagsrapport-norge-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.05.08-dagsrapport-norge-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Norwegian Institute of Public Health</t>
@@ -1229,7 +1229,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506180000/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200508085712/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1259,7 +1259,7 @@
   <si>
     <t xml:space="preserve">The [Panama Ministry of Health](http://www.minsa.gob.pa) in collaboration with the [Gorgas Memorial Institute for Health Studies](http://www.gorgas.gob.pa) reports the cumulative number of tests performed to date in [this dashboard](http://minsa.gob.pa/coronavirus-covid-19). The reported figures include the total number of positive, negative, and "positive control" test results to date.
 It is unclear whether the total number of tests performed ("pruebas realizadas") refers to the number of people tested or the number of samples tested. The number of reported positive test results is equal to the number of confirmed cases of COVID-19, which suggests that the number of tests performed is equivalent to the number of people tested. However, because the data source does not provide a clear definition, we record the units as "unclear".
-Unfortunately, the Ministry of Health's official dashboard does not provide a time series of the number of tests performed each day since testing began. Instead, the dashboard only displays a daily snapshot of the total number of tests performed to date. Since we did not begin to monitor this dashboard until April 14th 2020, we construct a time series dating back to March 9th 2020 using data provided in [this unofficial Github repository](https://github.com/c0t088/DAP-Panama/blob/master/data_covid_pma_dia.csv), which we have cross-referenced against data in the official Ministry of Health dashboard for a sample of dates.</t>
+Unfortunately, the Ministry of Health's official dashboard does not provide a time series of the number of tests performed each day since testing began. Instead, the dashboard only displays a daily snapshot of the total number of tests performed to date. Since we did not begin to monitor this dashboard until April 14th 2020, we construct a time series dating back to March 9th 2020 using data provided in [this unofficial GitHub repository](https://github.com/c0t088/DAP-Panama/blob/master/data_covid_pma_dia.csv), which we have cross-referenced against data in the official Ministry of Health dashboard for a sample of dates.</t>
   </si>
   <si>
     <t xml:space="preserve">PRY</t>
@@ -1284,7 +1284,7 @@
   </si>
   <si>
     <t xml:space="preserve">The Paraguay Ministry of Public Health and Social Welfare provides press releases of the daily number of samples tested, alongside the number of these samples that tested positive. It is unclear whether these figures include samples for which the results are still pending.
-We construct a time series of the daily number of samples tested using the data stored in [this unofficial Github repository](https://github.com/torresmateo/covidpy-rest). We have cross-checked a sample of the figures reported in this unofficial source against the data reported in official press releases.
+We construct a time series of the daily number of samples tested using the data stored in [this unofficial GitHub repository](https://github.com/torresmateo/covidpy-rest). We have cross-checked a sample of the figures reported in this unofficial source against the data reported in official press releases.
 It is possible that the figures are equivalent to the number of people tested, since the number of positive samples reported tend to be equal to the daily number of confirmed cases that the ministry reports. However, since the ministry uses the language "samples taken" ("muestras tomadas") in its press releases, we interpret the units as "sample tested" rather than "people tested".
 The reported figures are cumulative from March 7th 2020, when the first case in Paraguay was confirmed.</t>
   </si>
@@ -1295,7 +1295,7 @@
     <t xml:space="preserve">Peru - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/147296-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-51-189-en-el-peru-comunicado-n-88</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/151042-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-58-526-en-el-peru-comunicado-n-90</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1336,7 +1336,7 @@
     <t xml:space="preserve">Poland - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://raw.githubusercontent.com/anuszka/COVID-19-MZ_GOV_PL/master/data/cor.2020.05.06.csv</t>
+    <t xml:space="preserve">https://raw.githubusercontent.com/anuszka/COVID-19-MZ_GOV_PL/master/data/cor.2020.05.08.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1381,7 +1381,7 @@
     <t xml:space="preserve">Qatar - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506180008/https://www.moph.gov.qa/english/Pages/Coronavirus2019.aspx</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200508130300/https://www.moph.gov.qa/english/Pages/Coronavirus2019.aspx</t>
   </si>
   <si>
     <t xml:space="preserve">Qatar Ministry of Public Health</t>
@@ -1409,7 +1409,7 @@
     <t xml:space="preserve">Made available by Adrian-Tudor Panescu on Github</t>
   </si>
   <si>
-    <t xml:space="preserve">Data is collected and made available [on Github](https://github.com/adrianp/covid19romania). It includes a cumulative total of tests performed. No information is given on the geographical scope and number of labs included.
+    <t xml:space="preserve">Data is collected and made available [on GitHub](https://github.com/adrianp/covid19romania). It includes a cumulative total of tests performed. No information is given on the geographical scope and number of labs included.
 The main data source is the press office of the Ministry of Internal Affairs, which provides a daily report on most metrics. Data points are also sourced from the Romanian Ministry of Health and the Romanian National Institute of Public Health and occasionally from news outlets.</t>
   </si>
   <si>
@@ -1419,7 +1419,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14386</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14413</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1439,7 +1439,7 @@
     <t xml:space="preserve">Rwanda - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1257748545744113665</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1258101550322536448</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1512,7 +1512,7 @@
     <t xml:space="preserve">https://www.zdravlje.gov.rs/sekcija/345852/covid-19.php</t>
   </si>
   <si>
-    <t xml:space="preserve">Reports are published daily by the Serbian Ministry of Health. The data is collected and aggregated by volunteers and [published on Github](https://github.com/aleksandar-jovicic/COVID19-Serbia). All labs in Serbia are included.</t>
+    <t xml:space="preserve">Reports are published daily by the Serbian Ministry of Health. The data is collected and aggregated by volunteers and [published on GitHub](https://github.com/aleksandar-jovicic/COVID19-Serbia). All labs in Serbia are included.</t>
   </si>
   <si>
     <t xml:space="preserve">SGP</t>
@@ -1546,7 +1546,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506180204/https://korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200508085745/https://korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Center of Health Information and the Office of the Government of the Slovak Republic</t>
@@ -1620,7 +1620,7 @@
     <t xml:space="preserve">South Korea - cases tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367092&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367177&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1640,7 +1640,7 @@
     <t xml:space="preserve">Spain - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/sanidadgob/status/1256993737340747782</t>
+    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/COVID-19_pruebas_diagnosticas.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Consumption and Social Welfare</t>
@@ -1687,9 +1687,6 @@
     <t xml:space="preserve">https://covid-19-schweiz.bagapps.ch/de-3.html</t>
   </si>
   <si>
-    <t xml:space="preserve">BAG dashboard</t>
-  </si>
-  <si>
     <t xml:space="preserve">Federal Office of Public Health</t>
   </si>
   <si>
@@ -1706,7 +1703,7 @@
     <t xml:space="preserve">Taiwan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/DZSBM654J3t3R35Rsh8KJA?typeid=9</t>
+    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/KxbDDNIQs2ZzZcFaecfm7g?typeid=9</t>
   </si>
   <si>
     <t xml:space="preserve">Taiwan Centers for Disease Control (CDC)</t>
@@ -1729,7 +1726,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506180226/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200508085818/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1776,7 +1773,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506180231/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200507200232/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1800,7 +1797,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1257775905147105280</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1258126714259099655</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
@@ -1823,7 +1820,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506180233/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200508085824/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1845,7 +1842,7 @@
     <t xml:space="preserve">United Kingdom - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506180236/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200507200236/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
@@ -1868,7 +1865,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200506180240/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200507200237/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
   </si>
   <si>
     <t xml:space="preserve">The number of tests performed, including tests posted or delivered but not yet returned and/or processed.</t>
@@ -1942,7 +1939,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-16</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-18</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -1981,7 +1978,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1257805665143226377</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1258247862527438848</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -1991,7 +1988,8 @@
   </si>
   <si>
     <t xml:space="preserve">The Zimbabwe Ministry of Health and Child Care provides daily press releases on its website and Twitter account ([@MoHCCZim](https://twitter.com/MoHCCZim)) that report the cumulative number of tests performed to date. The reported figures include positive, negative, and pending test results. It is not clear how many people have been tested, since the reported figures refer only to the number of tests conducted rather than the number of people tested.
-The earliest reported figure that we have been able to find is from March 15th 2020, at which point 14 tests had been conducted.</t>
+The press release for May 6th 2020 reported that 7,808 PCR and 8,244 "rapid screening" tests had been conducted to date. We exclude rapid screening tests from the daily time series that we construct, since we assume that these are antibody tests.
+Prior to May 6th 2020, the press releases either: (a) reported a combined cumulative total of PCR and rapid screening tests without providing a breakdown between the two types of tests; or (b) did not clearly specify whether the reported cumulative total was in reference to PCR tests, antibody tests, or both. For this reason, the daily time series we construct begins on May 6th 2020, at which point the press releases began to clearly indicate that the reported cumulative totals only include PCR tests.</t>
   </si>
 </sst>
 </file>
@@ -2441,7 +2439,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
@@ -2451,31 +2449,31 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H3" t="n">
-        <v>688656</v>
+        <v>722549</v>
       </c>
       <c r="I3" t="n">
-        <v>27.006</v>
+        <v>28.335</v>
       </c>
       <c r="J3" t="n">
-        <v>23900</v>
+        <v>33893</v>
       </c>
       <c r="K3" t="n">
-        <v>0.937</v>
+        <v>1.329</v>
       </c>
       <c r="L3" t="n">
-        <v>18516.333</v>
+        <v>24111.667</v>
       </c>
       <c r="M3" t="n">
-        <v>0.726</v>
+        <v>0.945</v>
       </c>
       <c r="N3" t="n">
-        <v>20606.571</v>
+        <v>22701.143</v>
       </c>
       <c r="O3" t="n">
-        <v>0.808</v>
+        <v>0.89</v>
       </c>
       <c r="P3" t="s">
         <v>29</v>
@@ -2498,7 +2496,7 @@
         <v>33</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
@@ -2508,31 +2506,31 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H4" t="n">
-        <v>292254</v>
+        <v>304069</v>
       </c>
       <c r="I4" t="n">
-        <v>32.45</v>
+        <v>33.761</v>
       </c>
       <c r="J4" t="n">
-        <v>6371</v>
+        <v>6175</v>
       </c>
       <c r="K4" t="n">
-        <v>0.707</v>
+        <v>0.686</v>
       </c>
       <c r="L4" t="n">
-        <v>5966.333</v>
+        <v>6062</v>
       </c>
       <c r="M4" t="n">
-        <v>0.662</v>
+        <v>0.673</v>
       </c>
       <c r="N4" t="n">
-        <v>6357.143</v>
+        <v>5712.857</v>
       </c>
       <c r="O4" t="n">
-        <v>0.706</v>
+        <v>0.634</v>
       </c>
       <c r="P4" t="s">
         <v>36</v>
@@ -2555,7 +2553,7 @@
         <v>41</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D5" t="s">
         <v>42</v>
@@ -2565,31 +2563,31 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H5" t="n">
-        <v>160341</v>
+        <v>170719</v>
       </c>
       <c r="I5" t="n">
-        <v>94.23</v>
+        <v>100.33</v>
       </c>
       <c r="J5" t="n">
-        <v>4840</v>
+        <v>4341</v>
       </c>
       <c r="K5" t="n">
-        <v>2.844</v>
+        <v>2.551</v>
       </c>
       <c r="L5" t="n">
-        <v>5395.333</v>
+        <v>5072.667</v>
       </c>
       <c r="M5" t="n">
-        <v>3.171</v>
+        <v>2.981</v>
       </c>
       <c r="N5" t="n">
-        <v>4776.571</v>
+        <v>5233.857</v>
       </c>
       <c r="O5" t="n">
-        <v>2.807</v>
+        <v>3.076</v>
       </c>
       <c r="P5" t="s">
         <v>44</v>
@@ -2612,7 +2610,7 @@
         <v>49</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D6" t="s">
         <v>50</v>
@@ -2622,31 +2620,31 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H6" t="n">
-        <v>99644</v>
+        <v>105511</v>
       </c>
       <c r="I6" t="n">
-        <v>0.605</v>
+        <v>0.641</v>
       </c>
       <c r="J6" t="n">
-        <v>6241</v>
+        <v>5867</v>
       </c>
       <c r="K6" t="n">
-        <v>0.038</v>
+        <v>0.036</v>
       </c>
       <c r="L6" t="n">
-        <v>6063.333</v>
+        <v>5937.667</v>
       </c>
       <c r="M6" t="n">
-        <v>0.037</v>
+        <v>0.036</v>
       </c>
       <c r="N6" t="n">
-        <v>5706.143</v>
+        <v>5835</v>
       </c>
       <c r="O6" t="n">
-        <v>0.035</v>
+        <v>0.036</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
@@ -2669,7 +2667,7 @@
         <v>56</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>43955</v>
+        <v>43958</v>
       </c>
       <c r="D7" t="s">
         <v>57</v>
@@ -2679,13 +2677,13 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H7" t="n">
-        <v>211369</v>
+        <v>229466</v>
       </c>
       <c r="I7" t="n">
-        <v>22.369</v>
+        <v>24.284</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -2714,7 +2712,7 @@
         <v>62</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>43955</v>
+        <v>43957</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
@@ -2724,31 +2722,31 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H8" t="n">
-        <v>391314</v>
+        <v>424448</v>
       </c>
       <c r="I8" t="n">
-        <v>33.764</v>
+        <v>36.623</v>
       </c>
       <c r="J8" t="n">
-        <v>19721</v>
+        <v>16598</v>
       </c>
       <c r="K8" t="n">
-        <v>1.702</v>
+        <v>1.432</v>
       </c>
       <c r="L8" t="n">
-        <v>15552.667</v>
+        <v>18301</v>
       </c>
       <c r="M8" t="n">
-        <v>1.342</v>
+        <v>1.579</v>
       </c>
       <c r="N8" t="n">
-        <v>18086.286</v>
+        <v>17898.571</v>
       </c>
       <c r="O8" t="n">
-        <v>1.561</v>
+        <v>1.544</v>
       </c>
       <c r="P8" t="s">
         <v>64</v>
@@ -2771,7 +2769,7 @@
         <v>69</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D9" t="s">
         <v>70</v>
@@ -2783,31 +2781,31 @@
         <v>71</v>
       </c>
       <c r="G9" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H9" t="n">
-        <v>7888</v>
+        <v>8167</v>
       </c>
       <c r="I9" t="n">
-        <v>0.676</v>
+        <v>0.7</v>
       </c>
       <c r="J9" t="n">
-        <v>121</v>
+        <v>195</v>
       </c>
       <c r="K9" t="n">
-        <v>0.01</v>
+        <v>0.017</v>
       </c>
       <c r="L9" t="n">
-        <v>110.667</v>
+        <v>133.333</v>
       </c>
       <c r="M9" t="n">
-        <v>0.009</v>
+        <v>0.011</v>
       </c>
       <c r="N9" t="n">
-        <v>252.429</v>
+        <v>230.857</v>
       </c>
       <c r="O9" t="n">
-        <v>0.022</v>
+        <v>0.02</v>
       </c>
       <c r="P9" t="s">
         <v>43</v>
@@ -2875,7 +2873,7 @@
         <v>83</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D11" t="s">
         <v>84</v>
@@ -2885,28 +2883,32 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H11" t="n">
-        <v>51768</v>
+        <v>54328</v>
       </c>
       <c r="I11" t="n">
-        <v>7.45</v>
+        <v>7.819</v>
       </c>
       <c r="J11" t="n">
-        <v>1465</v>
+        <v>1397</v>
       </c>
       <c r="K11" t="n">
-        <v>0.211</v>
+        <v>0.201</v>
       </c>
       <c r="L11" t="n">
-        <v>1050</v>
+        <v>1341.667</v>
       </c>
       <c r="M11" t="n">
-        <v>0.151</v>
-      </c>
-      <c r="N11"/>
-      <c r="O11"/>
+        <v>0.193</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1116.857</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.161</v>
+      </c>
       <c r="P11" t="s">
         <v>86</v>
       </c>
@@ -2928,7 +2930,7 @@
         <v>90</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D12" t="s">
         <v>91</v>
@@ -2938,21 +2940,21 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H12" t="n">
-        <v>942526</v>
+        <v>1005218</v>
       </c>
       <c r="I12" t="n">
-        <v>24.973</v>
+        <v>26.634</v>
       </c>
       <c r="J12"/>
       <c r="K12" t="n">
-        <v>0.052</v>
+        <v>0.088</v>
       </c>
       <c r="L12"/>
       <c r="M12" t="n">
-        <v>0.433</v>
+        <v>0.571</v>
       </c>
       <c r="N12"/>
       <c r="O12"/>
@@ -2977,7 +2979,7 @@
         <v>97</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D13" t="s">
         <v>98</v>
@@ -2989,31 +2991,31 @@
         <v>99</v>
       </c>
       <c r="G13" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H13" t="n">
-        <v>232108</v>
+        <v>244226</v>
       </c>
       <c r="I13" t="n">
-        <v>12.142</v>
+        <v>12.776</v>
       </c>
       <c r="J13" t="n">
-        <v>10013</v>
+        <v>12118</v>
       </c>
       <c r="K13" t="n">
-        <v>0.524</v>
+        <v>0.634</v>
       </c>
       <c r="L13" t="n">
-        <v>8630</v>
+        <v>10031.667</v>
       </c>
       <c r="M13" t="n">
-        <v>0.452</v>
+        <v>0.525</v>
       </c>
       <c r="N13" t="n">
-        <v>8498.429</v>
+        <v>9101.286</v>
       </c>
       <c r="O13" t="n">
-        <v>0.445</v>
+        <v>0.476</v>
       </c>
       <c r="P13" t="s">
         <v>100</v>
@@ -3036,7 +3038,7 @@
         <v>104</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D14" t="s">
         <v>105</v>
@@ -3046,31 +3048,31 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H14" t="n">
-        <v>127105</v>
+        <v>135352</v>
       </c>
       <c r="I14" t="n">
-        <v>2.498</v>
+        <v>2.66</v>
       </c>
       <c r="J14" t="n">
-        <v>4076</v>
+        <v>4242</v>
       </c>
       <c r="K14" t="n">
-        <v>0.08</v>
+        <v>0.083</v>
       </c>
       <c r="L14" t="n">
-        <v>4167.667</v>
+        <v>4107.667</v>
       </c>
       <c r="M14" t="n">
-        <v>0.082</v>
+        <v>0.081</v>
       </c>
       <c r="N14" t="n">
-        <v>4574.286</v>
+        <v>4385</v>
       </c>
       <c r="O14" t="n">
-        <v>0.09</v>
+        <v>0.086</v>
       </c>
       <c r="P14" t="s">
         <v>106</v>
@@ -3093,7 +3095,7 @@
         <v>111</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D15" t="s">
         <v>112</v>
@@ -3103,31 +3105,31 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H15" t="n">
-        <v>9892</v>
+        <v>10375</v>
       </c>
       <c r="I15" t="n">
-        <v>1.942</v>
+        <v>2.037</v>
       </c>
       <c r="J15" t="n">
-        <v>73</v>
+        <v>274</v>
       </c>
       <c r="K15" t="n">
-        <v>0.014</v>
+        <v>0.054</v>
       </c>
       <c r="L15" t="n">
-        <v>99.667</v>
+        <v>185.333</v>
       </c>
       <c r="M15" t="n">
-        <v>0.02</v>
+        <v>0.036</v>
       </c>
       <c r="N15" t="n">
-        <v>129</v>
+        <v>148.571</v>
       </c>
       <c r="O15" t="n">
-        <v>0.025</v>
+        <v>0.029</v>
       </c>
       <c r="P15" t="s">
         <v>113</v>
@@ -3150,7 +3152,7 @@
         <v>117</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D16" t="s">
         <v>118</v>
@@ -3160,25 +3162,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H16" t="n">
-        <v>41053</v>
+        <v>43378</v>
       </c>
       <c r="I16" t="n">
-        <v>10</v>
+        <v>10.566</v>
       </c>
       <c r="J16" t="n">
-        <v>1080</v>
+        <v>1440</v>
       </c>
       <c r="K16" t="n">
-        <v>0.263</v>
+        <v>0.351</v>
       </c>
       <c r="L16" t="n">
-        <v>989.667</v>
+        <v>1135</v>
       </c>
       <c r="M16" t="n">
-        <v>0.241</v>
+        <v>0.277</v>
       </c>
       <c r="N16"/>
       <c r="O16"/>
@@ -3203,7 +3205,7 @@
         <v>124</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>43956</v>
+        <v>43957</v>
       </c>
       <c r="D17" t="s">
         <v>125</v>
@@ -3215,28 +3217,28 @@
         <v>127</v>
       </c>
       <c r="G17" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H17" t="n">
-        <v>59648</v>
+        <v>61613</v>
       </c>
       <c r="I17" t="n">
-        <v>5.266</v>
+        <v>5.44</v>
       </c>
       <c r="J17" t="n">
-        <v>1937</v>
+        <v>1965</v>
       </c>
       <c r="K17" t="n">
-        <v>0.171</v>
+        <v>0.173</v>
       </c>
       <c r="L17" t="n">
-        <v>2034.333</v>
+        <v>2023.667</v>
       </c>
       <c r="M17" t="n">
-        <v>0.179</v>
+        <v>0.178</v>
       </c>
       <c r="N17" t="n">
-        <v>2043.429</v>
+        <v>2038</v>
       </c>
       <c r="O17" t="n">
         <v>0.18</v>
@@ -3262,7 +3264,7 @@
         <v>131</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D18" t="s">
         <v>132</v>
@@ -3272,31 +3274,31 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H18" t="n">
-        <v>278519</v>
+        <v>293992</v>
       </c>
       <c r="I18" t="n">
-        <v>26.008</v>
+        <v>27.453</v>
       </c>
       <c r="J18" t="n">
-        <v>9416</v>
+        <v>7071</v>
       </c>
       <c r="K18" t="n">
-        <v>0.879</v>
+        <v>0.66</v>
       </c>
       <c r="L18" t="n">
-        <v>6879.333</v>
+        <v>8296.333</v>
       </c>
       <c r="M18" t="n">
-        <v>0.642</v>
+        <v>0.775</v>
       </c>
       <c r="N18" t="n">
-        <v>6207.714</v>
+        <v>6335.429</v>
       </c>
       <c r="O18" t="n">
-        <v>0.58</v>
+        <v>0.592</v>
       </c>
       <c r="P18" t="s">
         <v>43</v>
@@ -3319,7 +3321,7 @@
         <v>136</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D19" t="s">
         <v>137</v>
@@ -3331,31 +3333,31 @@
         <v>139</v>
       </c>
       <c r="G19" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H19" t="n">
-        <v>270680</v>
+        <v>284480</v>
       </c>
       <c r="I19" t="n">
-        <v>46.732</v>
+        <v>49.114</v>
       </c>
       <c r="J19" t="n">
-        <v>12942</v>
+        <v>13800</v>
       </c>
       <c r="K19" t="n">
-        <v>2.234</v>
+        <v>2.383</v>
       </c>
       <c r="L19" t="n">
-        <v>12293.667</v>
+        <v>13229.667</v>
       </c>
       <c r="M19" t="n">
-        <v>2.122</v>
+        <v>2.284</v>
       </c>
       <c r="N19" t="n">
-        <v>12945.429</v>
+        <v>13045</v>
       </c>
       <c r="O19" t="n">
-        <v>2.235</v>
+        <v>2.252</v>
       </c>
       <c r="P19" t="s">
         <v>140</v>
@@ -3378,7 +3380,7 @@
         <v>144</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>43955</v>
+        <v>43957</v>
       </c>
       <c r="D20" t="s">
         <v>145</v>
@@ -3390,26 +3392,20 @@
         <v>147</v>
       </c>
       <c r="G20" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H20" t="n">
-        <v>66160</v>
+        <v>63300</v>
       </c>
       <c r="I20" t="n">
-        <v>3.75</v>
+        <v>3.588</v>
       </c>
       <c r="J20"/>
-      <c r="K20" t="n">
-        <v>0.211</v>
-      </c>
+      <c r="K20"/>
       <c r="L20"/>
-      <c r="M20" t="n">
-        <v>0.55</v>
-      </c>
+      <c r="M20"/>
       <c r="N20"/>
-      <c r="O20" t="n">
-        <v>0.284</v>
-      </c>
+      <c r="O20"/>
       <c r="P20" t="s">
         <v>146</v>
       </c>
@@ -3431,7 +3427,7 @@
         <v>151</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>43956</v>
+        <v>43957</v>
       </c>
       <c r="D21" t="s">
         <v>152</v>
@@ -3443,22 +3439,22 @@
         <v>154</v>
       </c>
       <c r="G21" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H21" t="n">
-        <v>33628</v>
+        <v>35411</v>
       </c>
       <c r="I21" t="n">
-        <v>5.185</v>
+        <v>5.459</v>
       </c>
       <c r="J21" t="n">
-        <v>1598</v>
+        <v>1783</v>
       </c>
       <c r="K21" t="n">
-        <v>0.246</v>
+        <v>0.275</v>
       </c>
       <c r="L21" t="n">
-        <v>1677.333</v>
+        <v>1674.667</v>
       </c>
       <c r="M21" t="n">
         <v>0.258</v>
@@ -3486,7 +3482,7 @@
         <v>157</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D22" t="s">
         <v>158</v>
@@ -3496,31 +3492,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H22" t="n">
-        <v>58955</v>
+        <v>61767</v>
       </c>
       <c r="I22" t="n">
-        <v>44.443</v>
+        <v>46.563</v>
       </c>
       <c r="J22" t="n">
-        <v>1541</v>
+        <v>1279</v>
       </c>
       <c r="K22" t="n">
-        <v>1.162</v>
+        <v>0.964</v>
       </c>
       <c r="L22" t="n">
-        <v>1256.667</v>
+        <v>1454.667</v>
       </c>
       <c r="M22" t="n">
-        <v>0.947</v>
+        <v>1.096</v>
       </c>
       <c r="N22" t="n">
-        <v>1112.143</v>
+        <v>1145.429</v>
       </c>
       <c r="O22" t="n">
-        <v>0.838</v>
+        <v>0.863</v>
       </c>
       <c r="P22" t="s">
         <v>160</v>
@@ -3543,7 +3539,7 @@
         <v>165</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D23" t="s">
         <v>166</v>
@@ -3553,16 +3549,20 @@
       </c>
       <c r="F23"/>
       <c r="G23" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H23" t="n">
-        <v>26517</v>
+        <v>30306</v>
       </c>
       <c r="I23" t="n">
-        <v>0.231</v>
-      </c>
-      <c r="J23"/>
-      <c r="K23"/>
+        <v>0.264</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1946</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.017</v>
+      </c>
       <c r="L23"/>
       <c r="M23"/>
       <c r="N23"/>
@@ -3588,7 +3588,7 @@
         <v>171</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>43956</v>
+        <v>43957</v>
       </c>
       <c r="D24" t="s">
         <v>172</v>
@@ -3598,25 +3598,25 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H24" t="n">
-        <v>108112</v>
+        <v>111983</v>
       </c>
       <c r="I24" t="n">
-        <v>19.512</v>
+        <v>20.211</v>
       </c>
       <c r="J24"/>
       <c r="K24" t="n">
-        <v>0.098</v>
+        <v>0.147</v>
       </c>
       <c r="L24"/>
       <c r="M24" t="n">
-        <v>0.184</v>
+        <v>0.319</v>
       </c>
       <c r="N24"/>
       <c r="O24" t="n">
-        <v>0.375</v>
+        <v>0.374</v>
       </c>
       <c r="P24" t="s">
         <v>174</v>
@@ -3639,7 +3639,7 @@
         <v>177</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>43949</v>
+        <v>43956</v>
       </c>
       <c r="D25" t="s">
         <v>178</v>
@@ -3651,13 +3651,13 @@
         <v>180</v>
       </c>
       <c r="G25" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H25" t="n">
-        <v>724574</v>
+        <v>831174</v>
       </c>
       <c r="I25" t="n">
-        <v>11.101</v>
+        <v>12.734</v>
       </c>
       <c r="J25"/>
       <c r="K25"/>
@@ -3733,7 +3733,7 @@
         <v>192</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>43953</v>
+        <v>43955</v>
       </c>
       <c r="D27" t="s">
         <v>193</v>
@@ -3743,20 +3743,16 @@
       </c>
       <c r="F27"/>
       <c r="G27" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H27" t="n">
-        <v>129461</v>
+        <v>135902</v>
       </c>
       <c r="I27" t="n">
-        <v>4.166</v>
-      </c>
-      <c r="J27" t="n">
-        <v>12412</v>
-      </c>
-      <c r="K27" t="n">
-        <v>0.399</v>
-      </c>
+        <v>4.374</v>
+      </c>
+      <c r="J27"/>
+      <c r="K27"/>
       <c r="L27"/>
       <c r="M27"/>
       <c r="N27"/>
@@ -3782,7 +3778,7 @@
         <v>200</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D28" t="s">
         <v>201</v>
@@ -3792,16 +3788,20 @@
       </c>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H28" t="n">
-        <v>87052</v>
+        <v>90043</v>
       </c>
       <c r="I28" t="n">
-        <v>8.352</v>
-      </c>
-      <c r="J28"/>
-      <c r="K28"/>
+        <v>8.639</v>
+      </c>
+      <c r="J28" t="n">
+        <v>2991</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.287</v>
+      </c>
       <c r="L28"/>
       <c r="M28"/>
       <c r="N28"/>
@@ -3827,7 +3827,7 @@
         <v>207</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>43948</v>
+        <v>43956</v>
       </c>
       <c r="D29" t="s">
         <v>208</v>
@@ -3837,13 +3837,13 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H29" t="n">
-        <v>154989</v>
+        <v>168291</v>
       </c>
       <c r="I29" t="n">
-        <v>20.674</v>
+        <v>22.448</v>
       </c>
       <c r="J29"/>
       <c r="K29"/>
@@ -3872,7 +3872,7 @@
         <v>214</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D30" t="s">
         <v>215</v>
@@ -3884,31 +3884,31 @@
         <v>217</v>
       </c>
       <c r="G30" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H30" t="n">
-        <v>86743</v>
+        <v>99058</v>
       </c>
       <c r="I30" t="n">
-        <v>8.979</v>
+        <v>10.254</v>
       </c>
       <c r="J30" t="n">
-        <v>1186</v>
+        <v>5022</v>
       </c>
       <c r="K30" t="n">
-        <v>0.123</v>
+        <v>0.52</v>
       </c>
       <c r="L30" t="n">
-        <v>1577.667</v>
+        <v>4500.333</v>
       </c>
       <c r="M30" t="n">
-        <v>0.164</v>
+        <v>0.466</v>
       </c>
       <c r="N30" t="n">
-        <v>2349</v>
+        <v>3246.714</v>
       </c>
       <c r="O30" t="n">
-        <v>0.243</v>
+        <v>0.336</v>
       </c>
       <c r="P30" t="s">
         <v>216</v>
@@ -3931,7 +3931,7 @@
         <v>222</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D31" t="s">
         <v>223</v>
@@ -3941,25 +3941,31 @@
       </c>
       <c r="F31"/>
       <c r="G31" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H31" t="n">
-        <v>51622</v>
+        <v>52704</v>
       </c>
       <c r="I31" t="n">
-        <v>151.273</v>
-      </c>
-      <c r="J31"/>
+        <v>154.444</v>
+      </c>
+      <c r="J31" t="n">
+        <v>462</v>
+      </c>
       <c r="K31" t="n">
-        <v>0.932</v>
-      </c>
-      <c r="L31"/>
+        <v>1.354</v>
+      </c>
+      <c r="L31" t="n">
+        <v>466.667</v>
+      </c>
       <c r="M31" t="n">
-        <v>1.228</v>
-      </c>
-      <c r="N31"/>
+        <v>1.368</v>
+      </c>
+      <c r="N31" t="n">
+        <v>515.714</v>
+      </c>
       <c r="O31" t="n">
-        <v>1.712</v>
+        <v>1.511</v>
       </c>
       <c r="P31" t="s">
         <v>224</v>
@@ -4033,7 +4039,7 @@
         <v>233</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D33" t="s">
         <v>229</v>
@@ -4045,31 +4051,31 @@
         <v>231</v>
       </c>
       <c r="G33" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H33" t="n">
-        <v>1276781</v>
+        <v>1437788</v>
       </c>
       <c r="I33" t="n">
-        <v>0.925</v>
+        <v>1.042</v>
       </c>
       <c r="J33" t="n">
-        <v>84835</v>
+        <v>80375</v>
       </c>
       <c r="K33" t="n">
-        <v>0.061</v>
+        <v>0.058</v>
       </c>
       <c r="L33" t="n">
-        <v>76777</v>
+        <v>81947.333</v>
       </c>
       <c r="M33" t="n">
+        <v>0.059</v>
+      </c>
+      <c r="N33" t="n">
+        <v>76447.714</v>
+      </c>
+      <c r="O33" t="n">
         <v>0.055</v>
-      </c>
-      <c r="N33" t="n">
-        <v>72288.143</v>
-      </c>
-      <c r="O33" t="n">
-        <v>0.052</v>
       </c>
       <c r="P33" t="s">
         <v>230</v>
@@ -4092,7 +4098,7 @@
         <v>235</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D34" t="s">
         <v>236</v>
@@ -4102,31 +4108,31 @@
       </c>
       <c r="F34"/>
       <c r="G34" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H34" t="n">
-        <v>92976</v>
+        <v>103361</v>
       </c>
       <c r="I34" t="n">
-        <v>0.34</v>
+        <v>0.378</v>
       </c>
       <c r="J34" t="n">
-        <v>4052</v>
+        <v>6644</v>
       </c>
       <c r="K34" t="n">
-        <v>0.015</v>
+        <v>0.024</v>
       </c>
       <c r="L34" t="n">
-        <v>3321.333</v>
+        <v>4812.333</v>
       </c>
       <c r="M34" t="n">
-        <v>0.012</v>
+        <v>0.018</v>
       </c>
       <c r="N34" t="n">
-        <v>3598.857</v>
+        <v>3831.857</v>
       </c>
       <c r="O34" t="n">
-        <v>0.013</v>
+        <v>0.014</v>
       </c>
       <c r="P34" t="s">
         <v>237</v>
@@ -4149,7 +4155,7 @@
         <v>241</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D35" t="s">
         <v>242</v>
@@ -4159,31 +4165,31 @@
       </c>
       <c r="F35"/>
       <c r="G35" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H35" t="n">
-        <v>531275</v>
+        <v>544792</v>
       </c>
       <c r="I35" t="n">
-        <v>6.325</v>
+        <v>6.486</v>
       </c>
       <c r="J35" t="n">
-        <v>11732</v>
+        <v>13517</v>
       </c>
       <c r="K35" t="n">
-        <v>0.14</v>
+        <v>0.161</v>
       </c>
       <c r="L35" t="n">
-        <v>11667.333</v>
+        <v>12168</v>
       </c>
       <c r="M35" t="n">
+        <v>0.145</v>
+      </c>
+      <c r="N35" t="n">
+        <v>11642.429</v>
+      </c>
+      <c r="O35" t="n">
         <v>0.139</v>
-      </c>
-      <c r="N35" t="n">
-        <v>11127</v>
-      </c>
-      <c r="O35" t="n">
-        <v>0.133</v>
       </c>
       <c r="P35" t="s">
         <v>243</v>
@@ -4251,7 +4257,7 @@
         <v>253</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D37" t="s">
         <v>254</v>
@@ -4263,25 +4269,31 @@
         <v>256</v>
       </c>
       <c r="G37" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H37" t="n">
-        <v>413517</v>
+        <v>435790</v>
       </c>
       <c r="I37" t="n">
-        <v>47.775</v>
-      </c>
-      <c r="J37"/>
+        <v>50.348</v>
+      </c>
+      <c r="J37" t="n">
+        <v>8876</v>
+      </c>
       <c r="K37" t="n">
-        <v>0.302</v>
-      </c>
-      <c r="L37"/>
+        <v>1.025</v>
+      </c>
+      <c r="L37" t="n">
+        <v>9003.333</v>
+      </c>
       <c r="M37" t="n">
-        <v>0.803</v>
-      </c>
-      <c r="N37"/>
+        <v>1.04</v>
+      </c>
+      <c r="N37" t="n">
+        <v>8844</v>
+      </c>
       <c r="O37" t="n">
-        <v>0.968</v>
+        <v>1.022</v>
       </c>
       <c r="P37" t="s">
         <v>43</v>
@@ -4304,7 +4316,7 @@
         <v>260</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D38" t="s">
         <v>261</v>
@@ -4316,31 +4328,25 @@
         <v>263</v>
       </c>
       <c r="G38" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H38" t="n">
-        <v>1549892</v>
+        <v>1563557</v>
       </c>
       <c r="I38" t="n">
-        <v>25.634</v>
-      </c>
-      <c r="J38" t="n">
-        <v>37771</v>
-      </c>
+        <v>25.86</v>
+      </c>
+      <c r="J38"/>
       <c r="K38" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="L38" t="n">
-        <v>30993.667</v>
-      </c>
+        <v>0.226</v>
+      </c>
+      <c r="L38"/>
       <c r="M38" t="n">
-        <v>0.513</v>
-      </c>
-      <c r="N38" t="n">
-        <v>33776</v>
-      </c>
+        <v>0.461</v>
+      </c>
+      <c r="N38"/>
       <c r="O38" t="n">
-        <v>0.559</v>
+        <v>0.493</v>
       </c>
       <c r="P38" t="s">
         <v>264</v>
@@ -4363,7 +4369,7 @@
         <v>267</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D39" t="s">
         <v>261</v>
@@ -4375,31 +4381,31 @@
         <v>263</v>
       </c>
       <c r="G39" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H39" t="n">
-        <v>2310929</v>
+        <v>2381288</v>
       </c>
       <c r="I39" t="n">
-        <v>38.221</v>
+        <v>39.385</v>
       </c>
       <c r="J39" t="n">
-        <v>64263</v>
+        <v>70359</v>
       </c>
       <c r="K39" t="n">
-        <v>1.063</v>
+        <v>1.164</v>
       </c>
       <c r="L39" t="n">
-        <v>52385.667</v>
+        <v>63295</v>
       </c>
       <c r="M39" t="n">
-        <v>0.866</v>
+        <v>1.047</v>
       </c>
       <c r="N39" t="n">
-        <v>57166.857</v>
+        <v>57438.714</v>
       </c>
       <c r="O39" t="n">
-        <v>0.945</v>
+        <v>0.95</v>
       </c>
       <c r="P39" t="s">
         <v>264</v>
@@ -4422,7 +4428,7 @@
         <v>270</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D40" t="s">
         <v>271</v>
@@ -4434,13 +4440,13 @@
         <v>273</v>
       </c>
       <c r="G40" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H40" t="n">
-        <v>188927</v>
+        <v>190030</v>
       </c>
       <c r="I40" t="n">
-        <v>1.494</v>
+        <v>1.502</v>
       </c>
       <c r="J40"/>
       <c r="K40"/>
@@ -4469,7 +4475,7 @@
         <v>276</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>43955</v>
+        <v>43957</v>
       </c>
       <c r="D41" t="s">
         <v>277</v>
@@ -4481,31 +4487,31 @@
         <v>278</v>
       </c>
       <c r="G41" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H41" t="n">
-        <v>285356</v>
+        <v>306231</v>
       </c>
       <c r="I41" t="n">
-        <v>2.256</v>
+        <v>2.421</v>
       </c>
       <c r="J41" t="n">
-        <v>2049</v>
+        <v>4281</v>
       </c>
       <c r="K41" t="n">
-        <v>0.016</v>
+        <v>0.034</v>
       </c>
       <c r="L41" t="n">
-        <v>2602.667</v>
+        <v>4110</v>
       </c>
       <c r="M41" t="n">
-        <v>0.02</v>
+        <v>0.032</v>
       </c>
       <c r="N41" t="n">
-        <v>4773.857</v>
+        <v>5450.286</v>
       </c>
       <c r="O41" t="n">
-        <v>0.038</v>
+        <v>0.043</v>
       </c>
       <c r="P41" t="s">
         <v>272</v>
@@ -4528,7 +4534,7 @@
         <v>281</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D42" t="s">
         <v>282</v>
@@ -4538,31 +4544,31 @@
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H42" t="n">
-        <v>336480</v>
+        <v>353843</v>
       </c>
       <c r="I42" t="n">
-        <v>17.92</v>
+        <v>18.845</v>
       </c>
       <c r="J42" t="n">
-        <v>16069</v>
+        <v>17363</v>
       </c>
       <c r="K42" t="n">
-        <v>0.856</v>
+        <v>0.925</v>
       </c>
       <c r="L42" t="n">
-        <v>13448</v>
+        <v>15660.667</v>
       </c>
       <c r="M42" t="n">
-        <v>0.716</v>
+        <v>0.834</v>
       </c>
       <c r="N42" t="n">
-        <v>14866.429</v>
+        <v>14902.286</v>
       </c>
       <c r="O42" t="n">
-        <v>0.792</v>
+        <v>0.794</v>
       </c>
       <c r="P42" t="s">
         <v>283</v>
@@ -4638,7 +4644,7 @@
         <v>293</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D44" t="s">
         <v>294</v>
@@ -4650,31 +4656,31 @@
         <v>296</v>
       </c>
       <c r="G44" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H44" t="n">
-        <v>68627</v>
+        <v>73016</v>
       </c>
       <c r="I44" t="n">
-        <v>36.384</v>
+        <v>38.711</v>
       </c>
       <c r="J44" t="n">
-        <v>2477</v>
+        <v>1947</v>
       </c>
       <c r="K44" t="n">
-        <v>1.313</v>
+        <v>1.032</v>
       </c>
       <c r="L44" t="n">
-        <v>1460.667</v>
+        <v>2288.667</v>
       </c>
       <c r="M44" t="n">
-        <v>0.774</v>
+        <v>1.213</v>
       </c>
       <c r="N44" t="n">
-        <v>1973.714</v>
+        <v>1699.429</v>
       </c>
       <c r="O44" t="n">
-        <v>1.046</v>
+        <v>0.901</v>
       </c>
       <c r="P44" t="s">
         <v>295</v>
@@ -4697,7 +4703,7 @@
         <v>299</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D45" t="s">
         <v>300</v>
@@ -4707,31 +4713,31 @@
       </c>
       <c r="F45"/>
       <c r="G45" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H45" t="n">
-        <v>156493</v>
+        <v>172191</v>
       </c>
       <c r="I45" t="n">
-        <v>57.486</v>
+        <v>63.252</v>
       </c>
       <c r="J45" t="n">
-        <v>7387</v>
+        <v>8103</v>
       </c>
       <c r="K45" t="n">
-        <v>2.714</v>
+        <v>2.977</v>
       </c>
       <c r="L45" t="n">
-        <v>4938.333</v>
+        <v>7695</v>
       </c>
       <c r="M45" t="n">
-        <v>1.814</v>
+        <v>2.827</v>
       </c>
       <c r="N45" t="n">
-        <v>5470.286</v>
+        <v>5631.857</v>
       </c>
       <c r="O45" t="n">
-        <v>2.01</v>
+        <v>2.069</v>
       </c>
       <c r="P45" t="s">
         <v>43</v>
@@ -4754,7 +4760,7 @@
         <v>304</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D46" t="s">
         <v>305</v>
@@ -4764,31 +4770,31 @@
       </c>
       <c r="F46"/>
       <c r="G46" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H46" t="n">
-        <v>50533</v>
+        <v>51883</v>
       </c>
       <c r="I46" t="n">
-        <v>80.727</v>
+        <v>82.883</v>
       </c>
       <c r="J46" t="n">
-        <v>1234</v>
+        <v>1350</v>
       </c>
       <c r="K46" t="n">
-        <v>1.971</v>
+        <v>2.157</v>
       </c>
       <c r="L46" t="n">
-        <v>805</v>
+        <v>1181.333</v>
       </c>
       <c r="M46" t="n">
-        <v>1.286</v>
+        <v>1.887</v>
       </c>
       <c r="N46" t="n">
-        <v>1253.571</v>
+        <v>1320</v>
       </c>
       <c r="O46" t="n">
-        <v>2.003</v>
+        <v>2.109</v>
       </c>
       <c r="P46" t="s">
         <v>306</v>
@@ -4811,7 +4817,7 @@
         <v>310</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D47" t="s">
         <v>311</v>
@@ -4821,28 +4827,32 @@
       </c>
       <c r="F47"/>
       <c r="G47" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H47" t="n">
-        <v>222150</v>
+        <v>239628</v>
       </c>
       <c r="I47" t="n">
-        <v>6.864</v>
+        <v>7.404</v>
       </c>
       <c r="J47" t="n">
-        <v>8930</v>
+        <v>8609</v>
       </c>
       <c r="K47" t="n">
-        <v>0.276</v>
+        <v>0.266</v>
       </c>
       <c r="L47" t="n">
-        <v>8772.333</v>
+        <v>8802.667</v>
       </c>
       <c r="M47" t="n">
-        <v>0.271</v>
-      </c>
-      <c r="N47"/>
-      <c r="O47"/>
+        <v>0.272</v>
+      </c>
+      <c r="N47" t="n">
+        <v>10120.571</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0.313</v>
+      </c>
       <c r="P47" t="s">
         <v>312</v>
       </c>
@@ -4864,7 +4874,7 @@
         <v>317</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D48" t="s">
         <v>318</v>
@@ -4874,13 +4884,13 @@
       </c>
       <c r="F48"/>
       <c r="G48" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H48" t="n">
-        <v>89565</v>
+        <v>98399</v>
       </c>
       <c r="I48" t="n">
-        <v>0.695</v>
+        <v>0.763</v>
       </c>
       <c r="J48"/>
       <c r="K48" t="n">
@@ -4888,11 +4898,11 @@
       </c>
       <c r="L48"/>
       <c r="M48" t="n">
-        <v>0.002</v>
+        <v>0.004</v>
       </c>
       <c r="N48"/>
       <c r="O48" t="n">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="P48" t="s">
         <v>319</v>
@@ -4974,7 +4984,7 @@
         <v>329</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D50" t="s">
         <v>330</v>
@@ -4986,13 +4996,13 @@
         <v>332</v>
       </c>
       <c r="G50" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H50" t="n">
-        <v>9295</v>
+        <v>10227</v>
       </c>
       <c r="I50" t="n">
-        <v>0.171</v>
+        <v>0.188</v>
       </c>
       <c r="J50"/>
       <c r="K50"/>
@@ -5021,7 +5031,7 @@
         <v>336</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D51" t="s">
         <v>337</v>
@@ -5033,31 +5043,31 @@
         <v>339</v>
       </c>
       <c r="G51" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H51" t="n">
-        <v>13850</v>
+        <v>14511</v>
       </c>
       <c r="I51" t="n">
-        <v>0.475</v>
+        <v>0.498</v>
       </c>
       <c r="J51" t="n">
-        <v>210</v>
+        <v>415</v>
       </c>
       <c r="K51" t="n">
-        <v>0.007</v>
+        <v>0.014</v>
       </c>
       <c r="L51" t="n">
-        <v>250.667</v>
+        <v>290.333</v>
       </c>
       <c r="M51" t="n">
-        <v>0.008</v>
+        <v>0.01</v>
       </c>
       <c r="N51" t="n">
-        <v>434.714</v>
+        <v>357.143</v>
       </c>
       <c r="O51" t="n">
-        <v>0.015</v>
+        <v>0.012</v>
       </c>
       <c r="P51" t="s">
         <v>338</v>
@@ -5080,7 +5090,7 @@
         <v>343</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>43956</v>
+        <v>43957</v>
       </c>
       <c r="D52" t="s">
         <v>344</v>
@@ -5090,22 +5100,26 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H52" t="n">
-        <v>243277</v>
+        <v>249655</v>
       </c>
       <c r="I52" t="n">
-        <v>14.198</v>
+        <v>14.57</v>
       </c>
       <c r="J52" t="n">
-        <v>2717</v>
+        <v>3488</v>
       </c>
       <c r="K52" t="n">
-        <v>0.159</v>
-      </c>
-      <c r="L52"/>
-      <c r="M52"/>
+        <v>0.204</v>
+      </c>
+      <c r="L52" t="n">
+        <v>3713.333</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0.217</v>
+      </c>
       <c r="N52"/>
       <c r="O52"/>
       <c r="P52" t="s">
@@ -5129,7 +5143,7 @@
         <v>350</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D53" t="s">
         <v>351</v>
@@ -5139,31 +5153,31 @@
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H53" t="n">
-        <v>160700</v>
+        <v>175835</v>
       </c>
       <c r="I53" t="n">
-        <v>33.325</v>
+        <v>36.463</v>
       </c>
       <c r="J53" t="n">
-        <v>4772</v>
+        <v>7812</v>
       </c>
       <c r="K53" t="n">
-        <v>0.99</v>
+        <v>1.62</v>
       </c>
       <c r="L53" t="n">
-        <v>3492.333</v>
+        <v>6635.667</v>
       </c>
       <c r="M53" t="n">
-        <v>0.724</v>
+        <v>1.376</v>
       </c>
       <c r="N53" t="n">
-        <v>4571</v>
+        <v>5133.857</v>
       </c>
       <c r="O53" t="n">
-        <v>0.948</v>
+        <v>1.065</v>
       </c>
       <c r="P53" t="s">
         <v>352</v>
@@ -5186,7 +5200,7 @@
         <v>355</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D54" t="s">
         <v>356</v>
@@ -5196,25 +5210,25 @@
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H54" t="n">
-        <v>21208</v>
+        <v>22492</v>
       </c>
       <c r="I54" t="n">
-        <v>0.103</v>
+        <v>0.109</v>
       </c>
       <c r="J54" t="n">
-        <v>1696</v>
+        <v>1284</v>
       </c>
       <c r="K54" t="n">
-        <v>0.008</v>
+        <v>0.006</v>
       </c>
       <c r="L54" t="n">
-        <v>1540</v>
+        <v>1318.667</v>
       </c>
       <c r="M54" t="n">
-        <v>0.007</v>
+        <v>0.006</v>
       </c>
       <c r="N54"/>
       <c r="O54"/>
@@ -5239,7 +5253,7 @@
         <v>361</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D55" t="s">
         <v>362</v>
@@ -5249,16 +5263,20 @@
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H55" t="n">
-        <v>188236</v>
+        <v>195921</v>
       </c>
       <c r="I55" t="n">
-        <v>34.722</v>
-      </c>
-      <c r="J55"/>
-      <c r="K55"/>
+        <v>36.14</v>
+      </c>
+      <c r="J55" t="n">
+        <v>3975</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0.733</v>
+      </c>
       <c r="L55"/>
       <c r="M55"/>
       <c r="N55"/>
@@ -5284,7 +5302,7 @@
         <v>368</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D56" t="s">
         <v>369</v>
@@ -5294,31 +5312,31 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H56" t="n">
-        <v>232582</v>
+        <v>257247</v>
       </c>
       <c r="I56" t="n">
-        <v>1.053</v>
+        <v>1.165</v>
       </c>
       <c r="J56" t="n">
-        <v>10178</v>
+        <v>12469</v>
       </c>
       <c r="K56" t="n">
-        <v>0.046</v>
+        <v>0.056</v>
       </c>
       <c r="L56" t="n">
-        <v>9852.333</v>
+        <v>11614.333</v>
       </c>
       <c r="M56" t="n">
-        <v>0.045</v>
+        <v>0.052</v>
       </c>
       <c r="N56" t="n">
-        <v>9524.429</v>
+        <v>10730.857</v>
       </c>
       <c r="O56" t="n">
-        <v>0.043</v>
+        <v>0.048</v>
       </c>
       <c r="P56" t="s">
         <v>370</v>
@@ -5341,7 +5359,7 @@
         <v>374</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D57" t="s">
         <v>375</v>
@@ -5353,31 +5371,31 @@
         <v>376</v>
       </c>
       <c r="G57" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H57" t="n">
-        <v>36483</v>
+        <v>39093</v>
       </c>
       <c r="I57" t="n">
-        <v>8.455</v>
+        <v>9.06</v>
       </c>
       <c r="J57" t="n">
-        <v>927</v>
+        <v>1079</v>
       </c>
       <c r="K57" t="n">
-        <v>0.215</v>
+        <v>0.25</v>
       </c>
       <c r="L57" t="n">
-        <v>1043</v>
+        <v>1179</v>
       </c>
       <c r="M57" t="n">
-        <v>0.242</v>
+        <v>0.273</v>
       </c>
       <c r="N57" t="n">
-        <v>1098.286</v>
+        <v>1192</v>
       </c>
       <c r="O57" t="n">
-        <v>0.254</v>
+        <v>0.276</v>
       </c>
       <c r="P57" t="s">
         <v>43</v>
@@ -5400,7 +5418,7 @@
         <v>380</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D58" t="s">
         <v>381</v>
@@ -5412,31 +5430,31 @@
         <v>383</v>
       </c>
       <c r="G58" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H58" t="n">
-        <v>11898</v>
+        <v>13096</v>
       </c>
       <c r="I58" t="n">
-        <v>1.668</v>
+        <v>1.836</v>
       </c>
       <c r="J58" t="n">
-        <v>458</v>
+        <v>599</v>
       </c>
       <c r="K58" t="n">
+        <v>0.084</v>
+      </c>
+      <c r="L58" t="n">
+        <v>547</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0.077</v>
+      </c>
+      <c r="N58" t="n">
+        <v>456.143</v>
+      </c>
+      <c r="O58" t="n">
         <v>0.064</v>
-      </c>
-      <c r="L58" t="n">
-        <v>382.333</v>
-      </c>
-      <c r="M58" t="n">
-        <v>0.054</v>
-      </c>
-      <c r="N58" t="n">
-        <v>431.714</v>
-      </c>
-      <c r="O58" t="n">
-        <v>0.061</v>
       </c>
       <c r="P58" t="s">
         <v>384</v>
@@ -5459,7 +5477,7 @@
         <v>388</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D59" t="s">
         <v>389</v>
@@ -5469,20 +5487,16 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H59" t="n">
-        <v>406579</v>
+        <v>448020</v>
       </c>
       <c r="I59" t="n">
-        <v>12.331</v>
-      </c>
-      <c r="J59" t="n">
-        <v>21087</v>
-      </c>
-      <c r="K59" t="n">
-        <v>0.64</v>
-      </c>
+        <v>13.588</v>
+      </c>
+      <c r="J59"/>
+      <c r="K59"/>
       <c r="L59"/>
       <c r="M59"/>
       <c r="N59"/>
@@ -5508,7 +5522,7 @@
         <v>395</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>43955</v>
+        <v>43956</v>
       </c>
       <c r="D60" t="s">
         <v>396</v>
@@ -5518,19 +5532,19 @@
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H60" t="n">
-        <v>119512</v>
+        <v>126387</v>
       </c>
       <c r="I60" t="n">
-        <v>1.091</v>
+        <v>1.153</v>
       </c>
       <c r="J60" t="n">
-        <v>6179</v>
+        <v>6875</v>
       </c>
       <c r="K60" t="n">
-        <v>0.056</v>
+        <v>0.063</v>
       </c>
       <c r="L60"/>
       <c r="M60"/>
@@ -5557,7 +5571,7 @@
         <v>400</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D61" t="s">
         <v>401</v>
@@ -5569,31 +5583,31 @@
         <v>403</v>
       </c>
       <c r="G61" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H61" t="n">
-        <v>410468</v>
+        <v>443506</v>
       </c>
       <c r="I61" t="n">
-        <v>10.846</v>
+        <v>11.719</v>
       </c>
       <c r="J61" t="n">
-        <v>16198</v>
+        <v>17512</v>
       </c>
       <c r="K61" t="n">
-        <v>0.428</v>
+        <v>0.463</v>
       </c>
       <c r="L61" t="n">
-        <v>11506.667</v>
+        <v>16412</v>
       </c>
       <c r="M61" t="n">
-        <v>0.304</v>
+        <v>0.434</v>
       </c>
       <c r="N61" t="n">
-        <v>12277.286</v>
+        <v>12696.857</v>
       </c>
       <c r="O61" t="n">
-        <v>0.325</v>
+        <v>0.336</v>
       </c>
       <c r="P61" t="s">
         <v>404</v>
@@ -5616,7 +5630,7 @@
         <v>408</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>43955</v>
+        <v>43956</v>
       </c>
       <c r="D62" t="s">
         <v>409</v>
@@ -5626,31 +5640,31 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H62" t="n">
-        <v>470234</v>
+        <v>485925</v>
       </c>
       <c r="I62" t="n">
-        <v>46.116</v>
+        <v>47.655</v>
       </c>
       <c r="J62" t="n">
-        <v>11532</v>
+        <v>15556</v>
       </c>
       <c r="K62" t="n">
-        <v>1.131</v>
+        <v>1.526</v>
       </c>
       <c r="L62" t="n">
-        <v>10172.333</v>
+        <v>11893.667</v>
       </c>
       <c r="M62" t="n">
-        <v>0.997</v>
+        <v>1.166</v>
       </c>
       <c r="N62" t="n">
-        <v>12808.857</v>
+        <v>12837.714</v>
       </c>
       <c r="O62" t="n">
-        <v>1.256</v>
+        <v>1.259</v>
       </c>
       <c r="P62" t="s">
         <v>410</v>
@@ -5673,7 +5687,7 @@
         <v>414</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D63" t="s">
         <v>415</v>
@@ -5683,31 +5697,31 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H63" t="n">
-        <v>112963</v>
+        <v>120458</v>
       </c>
       <c r="I63" t="n">
-        <v>39.209</v>
+        <v>41.81</v>
       </c>
       <c r="J63" t="n">
-        <v>3201</v>
+        <v>3963</v>
       </c>
       <c r="K63" t="n">
-        <v>1.111</v>
+        <v>1.376</v>
       </c>
       <c r="L63" t="n">
-        <v>2842.667</v>
+        <v>3565.333</v>
       </c>
       <c r="M63" t="n">
-        <v>0.987</v>
+        <v>1.238</v>
       </c>
       <c r="N63" t="n">
-        <v>3078.286</v>
+        <v>3247.429</v>
       </c>
       <c r="O63" t="n">
-        <v>1.069</v>
+        <v>1.127</v>
       </c>
       <c r="P63" t="s">
         <v>416</v>
@@ -5730,7 +5744,7 @@
         <v>420</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D64" t="s">
         <v>421</v>
@@ -5742,31 +5756,31 @@
         <v>423</v>
       </c>
       <c r="G64" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H64" t="n">
-        <v>217139</v>
+        <v>237280</v>
       </c>
       <c r="I64" t="n">
-        <v>11.287</v>
+        <v>12.334</v>
       </c>
       <c r="J64" t="n">
-        <v>11297</v>
+        <v>10667</v>
       </c>
       <c r="K64" t="n">
-        <v>0.587</v>
+        <v>0.554</v>
       </c>
       <c r="L64" t="n">
-        <v>7210.333</v>
+        <v>10479.333</v>
       </c>
       <c r="M64" t="n">
-        <v>0.375</v>
+        <v>0.544</v>
       </c>
       <c r="N64" t="n">
-        <v>7163.714</v>
+        <v>7656</v>
       </c>
       <c r="O64" t="n">
-        <v>0.372</v>
+        <v>0.398</v>
       </c>
       <c r="P64" t="s">
         <v>422</v>
@@ -5789,7 +5803,7 @@
         <v>426</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D65" t="s">
         <v>427</v>
@@ -5799,31 +5813,31 @@
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H65" t="n">
-        <v>4633731</v>
+        <v>4987468</v>
       </c>
       <c r="I65" t="n">
-        <v>31.752</v>
+        <v>34.176</v>
       </c>
       <c r="J65" t="n">
-        <v>173374</v>
+        <v>184276</v>
       </c>
       <c r="K65" t="n">
-        <v>1.188</v>
+        <v>1.263</v>
       </c>
       <c r="L65" t="n">
-        <v>177910.667</v>
+        <v>175703.667</v>
       </c>
       <c r="M65" t="n">
-        <v>1.219</v>
+        <v>1.204</v>
       </c>
       <c r="N65" t="n">
-        <v>190002</v>
+        <v>180523</v>
       </c>
       <c r="O65" t="n">
-        <v>1.302</v>
+        <v>1.237</v>
       </c>
       <c r="P65" t="s">
         <v>428</v>
@@ -5846,7 +5860,7 @@
         <v>432</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>43956</v>
+        <v>43957</v>
       </c>
       <c r="D66" t="s">
         <v>433</v>
@@ -5856,31 +5870,31 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H66" t="n">
-        <v>35992</v>
+        <v>37315</v>
       </c>
       <c r="I66" t="n">
-        <v>2.779</v>
+        <v>2.881</v>
       </c>
       <c r="J66" t="n">
-        <v>896</v>
+        <v>1323</v>
       </c>
       <c r="K66" t="n">
-        <v>0.069</v>
+        <v>0.102</v>
       </c>
       <c r="L66" t="n">
-        <v>896.333</v>
+        <v>988.333</v>
       </c>
       <c r="M66" t="n">
-        <v>0.069</v>
+        <v>0.076</v>
       </c>
       <c r="N66" t="n">
-        <v>1156.571</v>
+        <v>1102</v>
       </c>
       <c r="O66" t="n">
-        <v>0.089</v>
+        <v>0.085</v>
       </c>
       <c r="P66" t="s">
         <v>434</v>
@@ -5903,7 +5917,7 @@
         <v>438</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D67" t="s">
         <v>439</v>
@@ -5913,16 +5927,20 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H67" t="n">
-        <v>389659</v>
+        <v>405685</v>
       </c>
       <c r="I67" t="n">
-        <v>11.193</v>
-      </c>
-      <c r="J67"/>
-      <c r="K67"/>
+        <v>11.653</v>
+      </c>
+      <c r="J67" t="n">
+        <v>16026</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0.46</v>
+      </c>
       <c r="L67"/>
       <c r="M67"/>
       <c r="N67"/>
@@ -5948,7 +5966,7 @@
         <v>442</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D68" t="s">
         <v>443</v>
@@ -5960,31 +5978,31 @@
         <v>445</v>
       </c>
       <c r="G68" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H68" t="n">
-        <v>17461</v>
+        <v>19369</v>
       </c>
       <c r="I68" t="n">
-        <v>1.043</v>
+        <v>1.157</v>
       </c>
       <c r="J68" t="n">
-        <v>1182</v>
+        <v>872</v>
       </c>
       <c r="K68" t="n">
-        <v>0.071</v>
+        <v>0.052</v>
       </c>
       <c r="L68" t="n">
-        <v>897</v>
+        <v>1027</v>
       </c>
       <c r="M68" t="n">
-        <v>0.054</v>
+        <v>0.061</v>
       </c>
       <c r="N68" t="n">
-        <v>964.714</v>
+        <v>941.429</v>
       </c>
       <c r="O68" t="n">
-        <v>0.058</v>
+        <v>0.056</v>
       </c>
       <c r="P68" t="s">
         <v>446</v>
@@ -6007,7 +6025,7 @@
         <v>451</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D69" t="s">
         <v>452</v>
@@ -6019,31 +6037,31 @@
         <v>453</v>
       </c>
       <c r="G69" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H69" t="n">
-        <v>117474</v>
+        <v>122995</v>
       </c>
       <c r="I69" t="n">
-        <v>17.264</v>
+        <v>18.075</v>
       </c>
       <c r="J69" t="n">
-        <v>6196</v>
+        <v>5521</v>
       </c>
       <c r="K69" t="n">
-        <v>0.911</v>
+        <v>0.811</v>
       </c>
       <c r="L69" t="n">
-        <v>5187.667</v>
+        <v>5511.333</v>
       </c>
       <c r="M69" t="n">
-        <v>0.763</v>
+        <v>0.81</v>
       </c>
       <c r="N69" t="n">
-        <v>5504.571</v>
+        <v>5335.714</v>
       </c>
       <c r="O69" t="n">
-        <v>0.809</v>
+        <v>0.784</v>
       </c>
       <c r="P69" t="s">
         <v>43</v>
@@ -6156,7 +6174,7 @@
         <v>465</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D72" t="s">
         <v>466</v>
@@ -6166,31 +6184,31 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H72" t="n">
-        <v>104606</v>
+        <v>114461</v>
       </c>
       <c r="I72" t="n">
-        <v>19.16</v>
+        <v>20.965</v>
       </c>
       <c r="J72" t="n">
-        <v>4742</v>
+        <v>4694</v>
       </c>
       <c r="K72" t="n">
-        <v>0.869</v>
+        <v>0.86</v>
       </c>
       <c r="L72" t="n">
-        <v>2795.333</v>
+        <v>4865.667</v>
       </c>
       <c r="M72" t="n">
-        <v>0.512</v>
+        <v>0.891</v>
       </c>
       <c r="N72" t="n">
-        <v>3324</v>
+        <v>3341.286</v>
       </c>
       <c r="O72" t="n">
-        <v>0.609</v>
+        <v>0.612</v>
       </c>
       <c r="P72" t="s">
         <v>468</v>
@@ -6213,7 +6231,7 @@
         <v>473</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D73" t="s">
         <v>474</v>
@@ -6223,31 +6241,31 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H73" t="n">
-        <v>58923</v>
+        <v>61027</v>
       </c>
       <c r="I73" t="n">
-        <v>28.343</v>
+        <v>29.355</v>
       </c>
       <c r="J73" t="n">
-        <v>1449</v>
+        <v>1049</v>
       </c>
       <c r="K73" t="n">
-        <v>0.697</v>
+        <v>0.505</v>
       </c>
       <c r="L73" t="n">
-        <v>1134.333</v>
+        <v>1184.333</v>
       </c>
       <c r="M73" t="n">
-        <v>0.546</v>
+        <v>0.57</v>
       </c>
       <c r="N73" t="n">
-        <v>1045.143</v>
+        <v>961</v>
       </c>
       <c r="O73" t="n">
-        <v>0.503</v>
+        <v>0.462</v>
       </c>
       <c r="P73" t="s">
         <v>476</v>
@@ -6270,7 +6288,7 @@
         <v>480</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D74" t="s">
         <v>481</v>
@@ -6282,31 +6300,31 @@
         <v>483</v>
       </c>
       <c r="G74" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H74" t="n">
-        <v>268064</v>
+        <v>292153</v>
       </c>
       <c r="I74" t="n">
-        <v>4.52</v>
+        <v>4.926</v>
       </c>
       <c r="J74" t="n">
-        <v>10523</v>
+        <v>12774</v>
       </c>
       <c r="K74" t="n">
-        <v>0.177</v>
+        <v>0.215</v>
       </c>
       <c r="L74" t="n">
-        <v>12459.333</v>
+        <v>11537.333</v>
       </c>
       <c r="M74" t="n">
-        <v>0.21</v>
+        <v>0.194</v>
       </c>
       <c r="N74" t="n">
-        <v>11795.286</v>
+        <v>12089</v>
       </c>
       <c r="O74" t="n">
-        <v>0.199</v>
+        <v>0.204</v>
       </c>
       <c r="P74" t="s">
         <v>482</v>
@@ -6329,7 +6347,7 @@
         <v>487</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D75" t="s">
         <v>488</v>
@@ -6339,25 +6357,31 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H75" t="n">
-        <v>643095</v>
+        <v>654863</v>
       </c>
       <c r="I75" t="n">
-        <v>12.544</v>
-      </c>
-      <c r="J75"/>
+        <v>12.773</v>
+      </c>
+      <c r="J75" t="n">
+        <v>5475</v>
+      </c>
       <c r="K75" t="n">
-        <v>0.056</v>
-      </c>
-      <c r="L75"/>
+        <v>0.107</v>
+      </c>
+      <c r="L75" t="n">
+        <v>4875.333</v>
+      </c>
       <c r="M75" t="n">
-        <v>0.079</v>
-      </c>
-      <c r="N75"/>
+        <v>0.095</v>
+      </c>
+      <c r="N75" t="n">
+        <v>4542</v>
+      </c>
       <c r="O75" t="n">
-        <v>0.081</v>
+        <v>0.089</v>
       </c>
       <c r="P75" t="s">
         <v>489</v>
@@ -6470,7 +6494,7 @@
         <v>505</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D78" t="s">
         <v>506</v>
@@ -6480,679 +6504,673 @@
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H78" t="n">
-        <v>290365</v>
+        <v>301675</v>
       </c>
       <c r="I78" t="n">
-        <v>33.55</v>
+        <v>34.857</v>
       </c>
       <c r="J78"/>
       <c r="K78" t="n">
-        <v>0.153</v>
+        <v>0.131</v>
       </c>
       <c r="L78"/>
       <c r="M78" t="n">
-        <v>0.272</v>
+        <v>0.468</v>
       </c>
       <c r="N78"/>
       <c r="O78" t="n">
-        <v>0.419</v>
+        <v>0.429</v>
       </c>
       <c r="P78" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Q78" t="s">
         <v>506</v>
       </c>
       <c r="R78" t="s">
+        <v>508</v>
+      </c>
+      <c r="S78" t="s">
         <v>509</v>
-      </c>
-      <c r="S78" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
+        <v>510</v>
+      </c>
+      <c r="B79" t="s">
         <v>511</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" s="1" t="n">
+        <v>43958</v>
+      </c>
+      <c r="D79" t="s">
         <v>512</v>
       </c>
-      <c r="C79" s="1" t="n">
-        <v>43956</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>513</v>
-      </c>
-      <c r="E79" t="s">
-        <v>514</v>
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H79" t="n">
-        <v>65589</v>
+        <v>66460</v>
       </c>
       <c r="I79" t="n">
-        <v>2.754</v>
+        <v>2.79</v>
       </c>
       <c r="J79" t="n">
-        <v>631</v>
+        <v>414</v>
       </c>
       <c r="K79" t="n">
-        <v>0.026</v>
+        <v>0.017</v>
       </c>
       <c r="L79" t="n">
-        <v>498.333</v>
+        <v>500.667</v>
       </c>
       <c r="M79" t="n">
         <v>0.021</v>
       </c>
       <c r="N79" t="n">
-        <v>460.143</v>
+        <v>445.714</v>
       </c>
       <c r="O79" t="n">
         <v>0.019</v>
       </c>
       <c r="P79" t="s">
+        <v>513</v>
+      </c>
+      <c r="Q79" t="s">
         <v>514</v>
       </c>
-      <c r="Q79" t="s">
+      <c r="R79" t="s">
         <v>515</v>
       </c>
-      <c r="R79" t="s">
+      <c r="S79" t="s">
         <v>516</v>
-      </c>
-      <c r="S79" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
+        <v>517</v>
+      </c>
+      <c r="B80" t="s">
         <v>518</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" s="1" t="n">
+        <v>43959</v>
+      </c>
+      <c r="D80" t="s">
         <v>519</v>
       </c>
-      <c r="C80" s="1" t="n">
-        <v>43957</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>520</v>
-      </c>
-      <c r="E80" t="s">
-        <v>521</v>
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H80" t="n">
-        <v>86320</v>
+        <v>90016</v>
       </c>
       <c r="I80" t="n">
-        <v>1.237</v>
-      </c>
-      <c r="J80" t="n">
-        <v>3693</v>
-      </c>
+        <v>1.29</v>
+      </c>
+      <c r="J80"/>
       <c r="K80" t="n">
-        <v>0.053</v>
-      </c>
-      <c r="L80" t="n">
-        <v>3684</v>
-      </c>
+        <v>0.003</v>
+      </c>
+      <c r="L80"/>
       <c r="M80" t="n">
-        <v>0.053</v>
-      </c>
-      <c r="N80" t="n">
-        <v>3471.714</v>
-      </c>
+        <v>0.035</v>
+      </c>
+      <c r="N80"/>
       <c r="O80" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="P80" t="s">
+        <v>521</v>
+      </c>
+      <c r="Q80" t="s">
         <v>522</v>
-      </c>
-      <c r="Q80" t="s">
-        <v>523</v>
       </c>
       <c r="R80" t="s">
         <v>94</v>
       </c>
       <c r="S80" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
+        <v>524</v>
+      </c>
+      <c r="B81" t="s">
         <v>525</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" s="1" t="n">
+        <v>43956</v>
+      </c>
+      <c r="D81" t="s">
         <v>526</v>
       </c>
-      <c r="C81" s="1" t="n">
-        <v>43955</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>527</v>
-      </c>
-      <c r="E81" t="s">
-        <v>528</v>
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H81" t="n">
-        <v>25165</v>
+        <v>25555</v>
       </c>
       <c r="I81" t="n">
-        <v>2.129</v>
+        <v>2.162</v>
       </c>
       <c r="J81" t="n">
-        <v>312</v>
+        <v>390</v>
       </c>
       <c r="K81" t="n">
-        <v>0.026</v>
+        <v>0.033</v>
       </c>
       <c r="L81" t="n">
-        <v>370</v>
+        <v>383</v>
       </c>
       <c r="M81" t="n">
-        <v>0.031</v>
+        <v>0.032</v>
       </c>
       <c r="N81" t="n">
-        <v>526.857</v>
+        <v>499</v>
       </c>
       <c r="O81" t="n">
-        <v>0.045</v>
+        <v>0.042</v>
       </c>
       <c r="P81" t="s">
+        <v>527</v>
+      </c>
+      <c r="Q81" t="s">
         <v>528</v>
       </c>
-      <c r="Q81" t="s">
+      <c r="R81" t="s">
         <v>529</v>
       </c>
-      <c r="R81" t="s">
+      <c r="S81" t="s">
         <v>530</v>
-      </c>
-      <c r="S81" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
+        <v>531</v>
+      </c>
+      <c r="B82" t="s">
         <v>532</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" s="1" t="n">
+        <v>43958</v>
+      </c>
+      <c r="D82" t="s">
         <v>533</v>
       </c>
-      <c r="C82" s="1" t="n">
-        <v>43957</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>534</v>
-      </c>
-      <c r="E82" t="s">
-        <v>535</v>
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H82" t="n">
-        <v>1234724</v>
+        <v>1265119</v>
       </c>
       <c r="I82" t="n">
-        <v>14.64</v>
+        <v>15</v>
       </c>
       <c r="J82" t="n">
-        <v>30303</v>
+        <v>30395</v>
       </c>
       <c r="K82" t="n">
-        <v>0.359</v>
+        <v>0.36</v>
       </c>
       <c r="L82" t="n">
-        <v>33119</v>
+        <v>31327</v>
       </c>
       <c r="M82" t="n">
-        <v>0.393</v>
+        <v>0.371</v>
       </c>
       <c r="N82"/>
       <c r="O82"/>
       <c r="P82" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q82" t="s">
         <v>535</v>
       </c>
-      <c r="Q82" t="s">
+      <c r="R82" t="s">
         <v>536</v>
       </c>
-      <c r="R82" t="s">
+      <c r="S82" t="s">
         <v>537</v>
-      </c>
-      <c r="S82" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
+        <v>538</v>
+      </c>
+      <c r="B83" t="s">
         <v>539</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" s="1" t="n">
+        <v>43957</v>
+      </c>
+      <c r="D83" t="s">
         <v>540</v>
       </c>
-      <c r="C83" s="1" t="n">
-        <v>43956</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>541</v>
       </c>
-      <c r="E83" t="s">
+      <c r="F83" t="s">
         <v>542</v>
       </c>
-      <c r="F83" t="s">
+      <c r="G83" t="n">
+        <v>30</v>
+      </c>
+      <c r="H83" t="n">
+        <v>47603</v>
+      </c>
+      <c r="I83" t="n">
+        <v>1.041</v>
+      </c>
+      <c r="J83" t="n">
+        <v>3509</v>
+      </c>
+      <c r="K83" t="n">
+        <v>0.077</v>
+      </c>
+      <c r="L83" t="n">
+        <v>2795.667</v>
+      </c>
+      <c r="M83" t="n">
+        <v>0.061</v>
+      </c>
+      <c r="N83" t="n">
+        <v>2618</v>
+      </c>
+      <c r="O83" t="n">
+        <v>0.057</v>
+      </c>
+      <c r="P83" t="s">
+        <v>541</v>
+      </c>
+      <c r="Q83" t="s">
         <v>543</v>
-      </c>
-      <c r="G83" t="n">
-        <v>29</v>
-      </c>
-      <c r="H83" t="n">
-        <v>44094</v>
-      </c>
-      <c r="I83" t="n">
-        <v>0.964</v>
-      </c>
-      <c r="J83" t="n">
-        <v>2632</v>
-      </c>
-      <c r="K83" t="n">
-        <v>0.058</v>
-      </c>
-      <c r="L83" t="n">
-        <v>2602.667</v>
-      </c>
-      <c r="M83" t="n">
-        <v>0.057</v>
-      </c>
-      <c r="N83" t="n">
-        <v>2402.714</v>
-      </c>
-      <c r="O83" t="n">
-        <v>0.053</v>
-      </c>
-      <c r="P83" t="s">
-        <v>542</v>
-      </c>
-      <c r="Q83" t="s">
-        <v>544</v>
       </c>
       <c r="R83" t="s">
         <v>53</v>
       </c>
       <c r="S83" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
+        <v>545</v>
+      </c>
+      <c r="B84" t="s">
         <v>546</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" s="1" t="n">
+        <v>43959</v>
+      </c>
+      <c r="D84" t="s">
         <v>547</v>
       </c>
-      <c r="C84" s="1" t="n">
-        <v>43957</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>548</v>
-      </c>
-      <c r="E84" t="s">
-        <v>549</v>
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H84" t="n">
-        <v>144283</v>
+        <v>159155</v>
       </c>
       <c r="I84" t="n">
-        <v>3.299</v>
+        <v>3.639</v>
       </c>
       <c r="J84" t="n">
-        <v>4524</v>
+        <v>7586</v>
       </c>
       <c r="K84" t="n">
-        <v>0.103</v>
+        <v>0.173</v>
       </c>
       <c r="L84" t="n">
-        <v>4853.333</v>
+        <v>6465.333</v>
       </c>
       <c r="M84" t="n">
-        <v>0.111</v>
+        <v>0.148</v>
       </c>
       <c r="N84" t="n">
-        <v>5677</v>
+        <v>5801.429</v>
       </c>
       <c r="O84" t="n">
-        <v>0.13</v>
+        <v>0.132</v>
       </c>
       <c r="P84" t="s">
+        <v>548</v>
+      </c>
+      <c r="Q84" t="s">
         <v>549</v>
       </c>
-      <c r="Q84" t="s">
+      <c r="R84" t="s">
         <v>550</v>
       </c>
-      <c r="R84" t="s">
+      <c r="S84" t="s">
         <v>551</v>
-      </c>
-      <c r="S84" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
+        <v>552</v>
+      </c>
+      <c r="B85" t="s">
         <v>553</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" s="1" t="n">
+        <v>43958</v>
+      </c>
+      <c r="D85" t="s">
         <v>554</v>
       </c>
-      <c r="C85" s="1" t="n">
-        <v>43957</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>555</v>
-      </c>
-      <c r="E85" t="s">
-        <v>556</v>
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H85" t="n">
-        <v>1072144</v>
+        <v>1139626</v>
       </c>
       <c r="I85" t="n">
-        <v>15.793</v>
+        <v>16.787</v>
       </c>
       <c r="J85" t="n">
-        <v>57006</v>
+        <v>65092</v>
       </c>
       <c r="K85" t="n">
-        <v>0.84</v>
+        <v>0.959</v>
       </c>
       <c r="L85" t="n">
-        <v>63267</v>
+        <v>63979</v>
       </c>
       <c r="M85" t="n">
-        <v>0.932</v>
+        <v>0.943</v>
       </c>
       <c r="N85" t="n">
-        <v>62518.714</v>
+        <v>64021.143</v>
       </c>
       <c r="O85" t="n">
-        <v>0.921</v>
+        <v>0.943</v>
       </c>
       <c r="P85" t="s">
+        <v>555</v>
+      </c>
+      <c r="Q85" t="s">
         <v>556</v>
-      </c>
-      <c r="Q85" t="s">
-        <v>557</v>
       </c>
       <c r="R85" t="s">
         <v>94</v>
       </c>
       <c r="S85" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B86" t="s">
+        <v>558</v>
+      </c>
+      <c r="C86" s="1" t="n">
+        <v>43958</v>
+      </c>
+      <c r="D86" t="s">
         <v>559</v>
       </c>
-      <c r="C86" s="1" t="n">
-        <v>43957</v>
-      </c>
-      <c r="D86" t="s">
-        <v>560</v>
-      </c>
       <c r="E86" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H86" t="n">
-        <v>1448010</v>
+        <v>1534533</v>
       </c>
       <c r="I86" t="n">
-        <v>21.33</v>
+        <v>22.605</v>
       </c>
       <c r="J86" t="n">
-        <v>69463</v>
+        <v>86583</v>
       </c>
       <c r="K86" t="n">
-        <v>1.023</v>
+        <v>1.275</v>
       </c>
       <c r="L86" t="n">
-        <v>79818.333</v>
+        <v>80284</v>
       </c>
       <c r="M86" t="n">
-        <v>1.176</v>
+        <v>1.182</v>
       </c>
       <c r="N86" t="n">
-        <v>89406.571</v>
+        <v>90116.857</v>
       </c>
       <c r="O86" t="n">
-        <v>1.317</v>
+        <v>1.327</v>
       </c>
       <c r="P86" t="s">
+        <v>555</v>
+      </c>
+      <c r="Q86" t="s">
         <v>556</v>
       </c>
-      <c r="Q86" t="s">
-        <v>557</v>
-      </c>
       <c r="R86" t="s">
+        <v>560</v>
+      </c>
+      <c r="S86" t="s">
         <v>561</v>
-      </c>
-      <c r="S86" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
+        <v>562</v>
+      </c>
+      <c r="B87" t="s">
         <v>563</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" s="1" t="n">
+        <v>43958</v>
+      </c>
+      <c r="D87" t="s">
         <v>564</v>
       </c>
-      <c r="C87" s="1" t="n">
-        <v>43956</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
         <v>565</v>
-      </c>
-      <c r="E87" t="s">
-        <v>566</v>
       </c>
       <c r="F87"/>
       <c r="G87" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H87" t="n">
-        <v>7544328</v>
+        <v>8105513</v>
       </c>
       <c r="I87" t="n">
-        <v>22.792</v>
+        <v>24.488</v>
       </c>
       <c r="J87" t="n">
-        <v>258954</v>
+        <v>318720</v>
       </c>
       <c r="K87" t="n">
-        <v>0.782</v>
+        <v>0.963</v>
       </c>
       <c r="L87" t="n">
-        <v>246362.333</v>
+        <v>273379.667</v>
       </c>
       <c r="M87" t="n">
-        <v>0.744</v>
+        <v>0.826</v>
       </c>
       <c r="N87" t="n">
-        <v>249771.857</v>
+        <v>264249.143</v>
       </c>
       <c r="O87" t="n">
-        <v>0.755</v>
+        <v>0.798</v>
       </c>
       <c r="P87" t="s">
+        <v>565</v>
+      </c>
+      <c r="Q87" t="s">
         <v>566</v>
       </c>
-      <c r="Q87" t="s">
+      <c r="R87" t="s">
         <v>567</v>
       </c>
-      <c r="R87" t="s">
+      <c r="S87" t="s">
         <v>568</v>
-      </c>
-      <c r="S87" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B88" t="s">
+        <v>569</v>
+      </c>
+      <c r="C88" s="1" t="n">
+        <v>43950</v>
+      </c>
+      <c r="D88" t="s">
         <v>570</v>
       </c>
-      <c r="C88" s="1" t="n">
-        <v>43949</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
         <v>571</v>
-      </c>
-      <c r="E88" t="s">
-        <v>572</v>
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H88" t="n">
-        <v>606361</v>
+        <v>629731</v>
       </c>
       <c r="I88" t="n">
-        <v>1.832</v>
+        <v>1.902</v>
       </c>
       <c r="J88" t="n">
-        <v>23063</v>
+        <v>23081</v>
       </c>
       <c r="K88" t="n">
         <v>0.07</v>
       </c>
       <c r="L88" t="n">
-        <v>18202.667</v>
+        <v>23107</v>
       </c>
       <c r="M88" t="n">
-        <v>0.055</v>
+        <v>0.07</v>
       </c>
       <c r="N88" t="n">
-        <v>19781.714</v>
+        <v>20113.714</v>
       </c>
       <c r="O88" t="n">
-        <v>0.06</v>
+        <v>0.061</v>
       </c>
       <c r="P88" t="s">
+        <v>572</v>
+      </c>
+      <c r="Q88" t="s">
         <v>573</v>
       </c>
-      <c r="Q88" t="s">
+      <c r="R88" t="s">
         <v>574</v>
       </c>
-      <c r="R88" t="s">
+      <c r="S88" t="s">
         <v>575</v>
-      </c>
-      <c r="S88" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
+        <v>576</v>
+      </c>
+      <c r="B89" t="s">
         <v>577</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" s="1" t="n">
+        <v>43959</v>
+      </c>
+      <c r="D89" t="s">
         <v>578</v>
-      </c>
-      <c r="C89" s="1" t="n">
-        <v>43957</v>
-      </c>
-      <c r="D89" t="s">
-        <v>579</v>
       </c>
       <c r="E89" t="s">
         <v>126</v>
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H89" t="n">
-        <v>23811</v>
+        <v>25698</v>
       </c>
       <c r="I89" t="n">
-        <v>6.855</v>
+        <v>7.398</v>
       </c>
       <c r="J89" t="n">
-        <v>1006</v>
+        <v>1042</v>
       </c>
       <c r="K89" t="n">
-        <v>0.29</v>
+        <v>0.3</v>
       </c>
       <c r="L89" t="n">
-        <v>882.333</v>
+        <v>964.333</v>
       </c>
       <c r="M89" t="n">
-        <v>0.254</v>
+        <v>0.278</v>
       </c>
       <c r="N89" t="n">
-        <v>810.143</v>
+        <v>850.143</v>
       </c>
       <c r="O89" t="n">
-        <v>0.233</v>
+        <v>0.245</v>
       </c>
       <c r="P89" t="s">
         <v>126</v>
       </c>
       <c r="Q89" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="R89" t="s">
         <v>24</v>
       </c>
       <c r="S89" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
+        <v>581</v>
+      </c>
+      <c r="B90" t="s">
         <v>582</v>
-      </c>
-      <c r="B90" t="s">
-        <v>583</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="D90" t="s">
+        <v>583</v>
+      </c>
+      <c r="E90" t="s">
         <v>584</v>
-      </c>
-      <c r="E90" t="s">
-        <v>585</v>
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
@@ -7171,73 +7189,61 @@
       <c r="N90"/>
       <c r="O90"/>
       <c r="P90" t="s">
+        <v>584</v>
+      </c>
+      <c r="Q90" t="s">
         <v>585</v>
       </c>
-      <c r="Q90" t="s">
+      <c r="R90" t="s">
         <v>586</v>
       </c>
-      <c r="R90" t="s">
+      <c r="S90" t="s">
         <v>587</v>
-      </c>
-      <c r="S90" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
+        <v>588</v>
+      </c>
+      <c r="B91" t="s">
         <v>589</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" s="1" t="n">
+        <v>43957</v>
+      </c>
+      <c r="D91" t="s">
         <v>590</v>
       </c>
-      <c r="C91" s="1" t="n">
-        <v>43956</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>591</v>
-      </c>
-      <c r="E91" t="s">
-        <v>592</v>
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="H91" t="n">
-        <v>14821</v>
+        <v>7808</v>
       </c>
       <c r="I91" t="n">
-        <v>0.997</v>
-      </c>
-      <c r="J91" t="n">
-        <v>1492</v>
-      </c>
-      <c r="K91" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="L91" t="n">
-        <v>1364.667</v>
-      </c>
-      <c r="M91" t="n">
-        <v>0.092</v>
-      </c>
-      <c r="N91" t="n">
-        <v>1076.286</v>
-      </c>
-      <c r="O91" t="n">
-        <v>0.072</v>
-      </c>
+        <v>0.525</v>
+      </c>
+      <c r="J91"/>
+      <c r="K91"/>
+      <c r="L91"/>
+      <c r="M91"/>
+      <c r="N91"/>
+      <c r="O91"/>
       <c r="P91" t="s">
+        <v>591</v>
+      </c>
+      <c r="Q91" t="s">
         <v>592</v>
-      </c>
-      <c r="Q91" t="s">
-        <v>593</v>
       </c>
       <c r="R91" t="s">
         <v>24</v>
       </c>
       <c r="S91" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data for 10th May
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="595">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -77,7 +77,7 @@
     <t xml:space="preserve">Argentina - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/30-04-20_reporte_matutino_covid_19.pdf</t>
+    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/09-05-20_reporte-matutino-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Argentina</t>
@@ -98,7 +98,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/05/coronavirus-covid-19-at-a-glance-7-may-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/05/coronavirus-covid-19-at-a-glance-9-may-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200508085522/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510104642/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200508130052/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200509192849/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -193,7 +193,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-7-maya-vyzdoroveli-i-vypisany-5067-patsientov/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-8-maya-vyzdoroveli-i-vypisany-5-tys-484-patsienta/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -277,7 +277,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200508085527/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510104647/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -300,7 +300,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200508085529/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510104649/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -342,7 +342,7 @@
     <t xml:space="preserve">COL</t>
   </si>
   <si>
-    <t xml:space="preserve">Colombia - samples processed</t>
+    <t xml:space="preserve">Colombia - samples tested</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.ins.gov.co/Noticias/Paginas/Coronavirus.aspx#muestras</t>
@@ -388,7 +388,7 @@
     <t xml:space="preserve">Croatia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200508130102/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200509164031/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -445,10 +445,10 @@
     <t xml:space="preserve">DNK</t>
   </si>
   <si>
-    <t xml:space="preserve">Denmark - People tested</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://files.ssi.dk/COVID19-overvaagningsrapport-07052020-8t4k</t>
+    <t xml:space="preserve">Denmark - people tested</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://files.ssi.dk/COVID19-overvaagningsrapport-09052020-hu51</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -475,7 +475,7 @@
     <t xml:space="preserve">Ecuador - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/05/INFOGRAFIA-NACIONALCOVI-19-69-COE-NACIONAL-06052020-08h00-2.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/05/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-08052020-08h0.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -504,7 +504,7 @@
     <t xml:space="preserve">Government of El Salvador</t>
   </si>
   <si>
-    <t xml:space="preserve">updated at 10:35pm local time on 2020-05-06.</t>
+    <t xml:space="preserve">updated at 12:50pm local time on 2020-05-09.</t>
   </si>
   <si>
     <t xml:space="preserve">The government of El Salvador publishes an online dashboard with figures and graphs about the epidemic, including the number of tests performed ("pruebas COVID19 realizadas hasta hoy"). No information is given on the geographical scope and number of labs included.</t>
@@ -669,7 +669,7 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200507/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200509/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -739,7 +739,7 @@
     <t xml:space="preserve">ISL</t>
   </si>
   <si>
-    <t xml:space="preserve">Iceland - samples</t>
+    <t xml:space="preserve">Iceland - samples tested</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.covid.is/tolulegar-upplysingar</t>
@@ -804,7 +804,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200507141927/http://irangov.ir/detail/338841</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200509000642/http://irangov.ir/detail/338857</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -924,7 +924,7 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000628517.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000628672.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Implementation status of PCR tests for new coronavirus in Japan (based on the date on which the results were determined). Preliminary data</t>
@@ -958,7 +958,7 @@
     <t xml:space="preserve">Kenya - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.go.ke/wp-content/uploads/2020/05/CamScanner-05-05-2020-15.48.16.pdf</t>
+    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1259109013435940866</t>
   </si>
   <si>
     <t xml:space="preserve">Kenya Ministry of Health</t>
@@ -999,7 +999,7 @@
     <t xml:space="preserve">Lithuania - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200508085626/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510104952/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -1015,7 +1015,7 @@
     <t xml:space="preserve">Luxembourg - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200507200422/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200509164113/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg Government situation update</t>
@@ -1036,7 +1036,7 @@
     <t xml:space="preserve">Malaysia - cases tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200508130208/https://www.moh.gov.my/index.php/pages/view/2019-ncov-wuhan</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510105003/https://www.moh.gov.my/index.php/pages/view/2019-ncov-wuhan</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1145,10 +1145,10 @@
     <t xml:space="preserve">Netherlands - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-05/COVID-19_WebSite_rapport_20200507_1337_0.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 7 May 2020 update</t>
+    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-05/COVID-19_WebSite_rapport_20200509_1018.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 9 May 2020 update</t>
   </si>
   <si>
     <t xml:space="preserve">Dutch National Institute for Public Health and the Environment</t>
@@ -1184,7 +1184,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200507200512/https://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200508200455/https://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1229,7 +1229,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200508085712/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510105025/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1295,7 +1295,7 @@
     <t xml:space="preserve">Peru - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/151042-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-58-526-en-el-peru-comunicado-n-90</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/151163-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-65-015-en-el-peru-comunicado-n-95</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1336,7 +1336,7 @@
     <t xml:space="preserve">Poland - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://raw.githubusercontent.com/anuszka/COVID-19-MZ_GOV_PL/master/data/cor.2020.05.08.csv</t>
+    <t xml:space="preserve">https://raw.githubusercontent.com/anuszka/COVID-19-MZ_GOV_PL/master/data/cor.2020.05.09.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1381,7 +1381,7 @@
     <t xml:space="preserve">Qatar - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200508130300/https://www.moph.gov.qa/english/Pages/Coronavirus2019.aspx</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510105040/https://www.moph.gov.qa/english/Pages/Coronavirus2019.aspx</t>
   </si>
   <si>
     <t xml:space="preserve">Qatar Ministry of Public Health</t>
@@ -1419,7 +1419,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14413</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14424</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1439,7 +1439,7 @@
     <t xml:space="preserve">Rwanda - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1258101550322536448</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1259173285348204546</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1546,7 +1546,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200508085745/https://korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510105056/https://korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Center of Health Information and the Office of the Government of the Slovak Republic</t>
@@ -1620,7 +1620,7 @@
     <t xml:space="preserve">South Korea - cases tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367177&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367186&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1640,10 +1640,13 @@
     <t xml:space="preserve">Spain - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/COVID-19_pruebas_diagnosticas.pdf</t>
+    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/COVID-19_pruebas_diagnosticas_07_05_2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Consumption and Social Welfare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corresponding press release: https://www.mscbs.gob.es/gabinete/notasPrensa.do?id=4910</t>
   </si>
   <si>
     <t xml:space="preserve">Ministerio de Sanidad, Consumo y Bienestar Social</t>
@@ -1703,7 +1706,7 @@
     <t xml:space="preserve">Taiwan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/KxbDDNIQs2ZzZcFaecfm7g?typeid=9</t>
+    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/EKvIxtZ0OwCUzeHXum1VBA?typeid=9</t>
   </si>
   <si>
     <t xml:space="preserve">Taiwan Centers for Disease Control (CDC)</t>
@@ -1726,7 +1729,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200508085818/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510105142/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1773,7 +1776,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200507200232/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200509164243/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1797,7 +1800,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1258126714259099655</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1259006502502834181</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
@@ -1820,7 +1823,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200508085824/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200510105147/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1842,7 +1845,7 @@
     <t xml:space="preserve">United Kingdom - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200507200236/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200509164248/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
@@ -1865,7 +1868,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200507200237/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200509164249/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
   </si>
   <si>
     <t xml:space="preserve">The number of tests performed, including tests posted or delivered but not yet returned and/or processed.</t>
@@ -1939,7 +1942,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-18</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-20</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -1978,7 +1981,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1258247862527438848</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1258995561090502657</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -2394,7 +2397,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>43952</v>
+        <v>43960</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -2404,20 +2407,32 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H2" t="n">
-        <v>58685</v>
+        <v>80729</v>
       </c>
       <c r="I2" t="n">
-        <v>1.298</v>
-      </c>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
+        <v>1.786</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2828</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="L2" t="n">
+        <v>2804.667</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.062</v>
+      </c>
+      <c r="N2" t="n">
+        <v>2409</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.053</v>
+      </c>
       <c r="P2" t="s">
         <v>22</v>
       </c>
@@ -2439,7 +2454,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
@@ -2449,31 +2464,31 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H3" t="n">
-        <v>722549</v>
+        <v>795456</v>
       </c>
       <c r="I3" t="n">
-        <v>28.335</v>
+        <v>31.194</v>
       </c>
       <c r="J3" t="n">
-        <v>33893</v>
+        <v>38206</v>
       </c>
       <c r="K3" t="n">
-        <v>1.329</v>
+        <v>1.498</v>
       </c>
       <c r="L3" t="n">
-        <v>24111.667</v>
+        <v>35600</v>
       </c>
       <c r="M3" t="n">
-        <v>0.945</v>
+        <v>1.396</v>
       </c>
       <c r="N3" t="n">
-        <v>22701.143</v>
+        <v>26267.571</v>
       </c>
       <c r="O3" t="n">
-        <v>0.89</v>
+        <v>1.03</v>
       </c>
       <c r="P3" t="s">
         <v>29</v>
@@ -2496,7 +2511,7 @@
         <v>33</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
@@ -2506,31 +2521,31 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H4" t="n">
-        <v>304069</v>
+        <v>316508</v>
       </c>
       <c r="I4" t="n">
-        <v>33.761</v>
+        <v>35.143</v>
       </c>
       <c r="J4" t="n">
-        <v>6175</v>
+        <v>4818</v>
       </c>
       <c r="K4" t="n">
-        <v>0.686</v>
+        <v>0.535</v>
       </c>
       <c r="L4" t="n">
-        <v>6062</v>
+        <v>6204.667</v>
       </c>
       <c r="M4" t="n">
-        <v>0.673</v>
+        <v>0.689</v>
       </c>
       <c r="N4" t="n">
-        <v>5712.857</v>
+        <v>6021.857</v>
       </c>
       <c r="O4" t="n">
-        <v>0.634</v>
+        <v>0.669</v>
       </c>
       <c r="P4" t="s">
         <v>36</v>
@@ -2553,7 +2568,7 @@
         <v>41</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>43959</v>
+        <v>43960</v>
       </c>
       <c r="D5" t="s">
         <v>42</v>
@@ -2563,31 +2578,31 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H5" t="n">
-        <v>170719</v>
+        <v>178353</v>
       </c>
       <c r="I5" t="n">
-        <v>100.33</v>
+        <v>104.816</v>
       </c>
       <c r="J5" t="n">
-        <v>4341</v>
+        <v>6195</v>
       </c>
       <c r="K5" t="n">
-        <v>2.551</v>
+        <v>3.641</v>
       </c>
       <c r="L5" t="n">
-        <v>5072.667</v>
+        <v>6004</v>
       </c>
       <c r="M5" t="n">
-        <v>2.981</v>
+        <v>3.529</v>
       </c>
       <c r="N5" t="n">
-        <v>5233.857</v>
+        <v>5725</v>
       </c>
       <c r="O5" t="n">
-        <v>3.076</v>
+        <v>3.365</v>
       </c>
       <c r="P5" t="s">
         <v>44</v>
@@ -2610,7 +2625,7 @@
         <v>49</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D6" t="s">
         <v>50</v>
@@ -2620,28 +2635,28 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H6" t="n">
-        <v>105511</v>
+        <v>116919</v>
       </c>
       <c r="I6" t="n">
-        <v>0.641</v>
+        <v>0.71</v>
       </c>
       <c r="J6" t="n">
-        <v>5867</v>
+        <v>5465</v>
       </c>
       <c r="K6" t="n">
-        <v>0.036</v>
+        <v>0.033</v>
       </c>
       <c r="L6" t="n">
-        <v>5937.667</v>
+        <v>5758.333</v>
       </c>
       <c r="M6" t="n">
-        <v>0.036</v>
+        <v>0.035</v>
       </c>
       <c r="N6" t="n">
-        <v>5835</v>
+        <v>5836.143</v>
       </c>
       <c r="O6" t="n">
         <v>0.036</v>
@@ -2667,7 +2682,7 @@
         <v>56</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>43958</v>
+        <v>43959</v>
       </c>
       <c r="D7" t="s">
         <v>57</v>
@@ -2677,16 +2692,20 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H7" t="n">
-        <v>229466</v>
+        <v>240146</v>
       </c>
       <c r="I7" t="n">
-        <v>24.284</v>
-      </c>
-      <c r="J7"/>
-      <c r="K7"/>
+        <v>25.414</v>
+      </c>
+      <c r="J7" t="n">
+        <v>10680</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1.13</v>
+      </c>
       <c r="L7"/>
       <c r="M7"/>
       <c r="N7"/>
@@ -2712,7 +2731,7 @@
         <v>62</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
@@ -2722,31 +2741,31 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H8" t="n">
-        <v>424448</v>
+        <v>461303</v>
       </c>
       <c r="I8" t="n">
-        <v>36.623</v>
+        <v>39.803</v>
       </c>
       <c r="J8" t="n">
-        <v>16598</v>
+        <v>21311</v>
       </c>
       <c r="K8" t="n">
-        <v>1.432</v>
+        <v>1.839</v>
       </c>
       <c r="L8" t="n">
-        <v>18301</v>
+        <v>18816.667</v>
       </c>
       <c r="M8" t="n">
-        <v>1.579</v>
+        <v>1.624</v>
       </c>
       <c r="N8" t="n">
-        <v>17898.571</v>
+        <v>17504.143</v>
       </c>
       <c r="O8" t="n">
-        <v>1.544</v>
+        <v>1.51</v>
       </c>
       <c r="P8" t="s">
         <v>64</v>
@@ -2769,7 +2788,7 @@
         <v>69</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D9" t="s">
         <v>70</v>
@@ -2781,31 +2800,31 @@
         <v>71</v>
       </c>
       <c r="G9" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H9" t="n">
-        <v>8167</v>
+        <v>8523</v>
       </c>
       <c r="I9" t="n">
-        <v>0.7</v>
+        <v>0.73</v>
       </c>
       <c r="J9" t="n">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="K9" t="n">
-        <v>0.017</v>
+        <v>0.015</v>
       </c>
       <c r="L9" t="n">
-        <v>133.333</v>
+        <v>183.667</v>
       </c>
       <c r="M9" t="n">
-        <v>0.011</v>
+        <v>0.016</v>
       </c>
       <c r="N9" t="n">
-        <v>230.857</v>
+        <v>138.143</v>
       </c>
       <c r="O9" t="n">
-        <v>0.02</v>
+        <v>0.012</v>
       </c>
       <c r="P9" t="s">
         <v>43</v>
@@ -2873,7 +2892,7 @@
         <v>83</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D11" t="s">
         <v>84</v>
@@ -2883,31 +2902,31 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H11" t="n">
-        <v>54328</v>
+        <v>57231</v>
       </c>
       <c r="I11" t="n">
-        <v>7.819</v>
+        <v>8.237</v>
       </c>
       <c r="J11" t="n">
-        <v>1397</v>
+        <v>1126</v>
       </c>
       <c r="K11" t="n">
-        <v>0.201</v>
+        <v>0.162</v>
       </c>
       <c r="L11" t="n">
-        <v>1341.667</v>
+        <v>1433.333</v>
       </c>
       <c r="M11" t="n">
-        <v>0.193</v>
+        <v>0.206</v>
       </c>
       <c r="N11" t="n">
-        <v>1116.857</v>
+        <v>1230.429</v>
       </c>
       <c r="O11" t="n">
-        <v>0.161</v>
+        <v>0.177</v>
       </c>
       <c r="P11" t="s">
         <v>86</v>
@@ -2930,7 +2949,7 @@
         <v>90</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D12" t="s">
         <v>91</v>
@@ -2940,24 +2959,26 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H12" t="n">
-        <v>1005218</v>
+        <v>1071379</v>
       </c>
       <c r="I12" t="n">
-        <v>26.634</v>
+        <v>28.387</v>
       </c>
       <c r="J12"/>
       <c r="K12" t="n">
-        <v>0.088</v>
+        <v>0.1</v>
       </c>
       <c r="L12"/>
       <c r="M12" t="n">
-        <v>0.571</v>
+        <v>0.614</v>
       </c>
       <c r="N12"/>
-      <c r="O12"/>
+      <c r="O12" t="n">
+        <v>0.673</v>
+      </c>
       <c r="P12" t="s">
         <v>92</v>
       </c>
@@ -2979,7 +3000,7 @@
         <v>97</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D13" t="s">
         <v>98</v>
@@ -2991,31 +3012,31 @@
         <v>99</v>
       </c>
       <c r="G13" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H13" t="n">
-        <v>244226</v>
+        <v>267904</v>
       </c>
       <c r="I13" t="n">
-        <v>12.776</v>
+        <v>14.014</v>
       </c>
       <c r="J13" t="n">
-        <v>12118</v>
+        <v>11943</v>
       </c>
       <c r="K13" t="n">
-        <v>0.634</v>
+        <v>0.625</v>
       </c>
       <c r="L13" t="n">
-        <v>10031.667</v>
+        <v>11932</v>
       </c>
       <c r="M13" t="n">
-        <v>0.525</v>
+        <v>0.624</v>
       </c>
       <c r="N13" t="n">
-        <v>9101.286</v>
+        <v>9786.286</v>
       </c>
       <c r="O13" t="n">
-        <v>0.476</v>
+        <v>0.512</v>
       </c>
       <c r="P13" t="s">
         <v>100</v>
@@ -3038,7 +3059,7 @@
         <v>104</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D14" t="s">
         <v>105</v>
@@ -3048,31 +3069,31 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H14" t="n">
-        <v>135352</v>
+        <v>144912</v>
       </c>
       <c r="I14" t="n">
-        <v>2.66</v>
+        <v>2.848</v>
       </c>
       <c r="J14" t="n">
-        <v>4242</v>
+        <v>5173</v>
       </c>
       <c r="K14" t="n">
-        <v>0.083</v>
+        <v>0.102</v>
       </c>
       <c r="L14" t="n">
-        <v>4107.667</v>
+        <v>4600.667</v>
       </c>
       <c r="M14" t="n">
-        <v>0.081</v>
+        <v>0.09</v>
       </c>
       <c r="N14" t="n">
-        <v>4385</v>
+        <v>4330</v>
       </c>
       <c r="O14" t="n">
-        <v>0.086</v>
+        <v>0.085</v>
       </c>
       <c r="P14" t="s">
         <v>106</v>
@@ -3095,7 +3116,7 @@
         <v>111</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D15" t="s">
         <v>112</v>
@@ -3105,31 +3126,31 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H15" t="n">
-        <v>10375</v>
+        <v>11276</v>
       </c>
       <c r="I15" t="n">
-        <v>2.037</v>
+        <v>2.214</v>
       </c>
       <c r="J15" t="n">
-        <v>274</v>
+        <v>449</v>
       </c>
       <c r="K15" t="n">
-        <v>0.054</v>
+        <v>0.088</v>
       </c>
       <c r="L15" t="n">
-        <v>185.333</v>
+        <v>391.667</v>
       </c>
       <c r="M15" t="n">
-        <v>0.036</v>
+        <v>0.077</v>
       </c>
       <c r="N15" t="n">
-        <v>148.571</v>
+        <v>240.429</v>
       </c>
       <c r="O15" t="n">
-        <v>0.029</v>
+        <v>0.047</v>
       </c>
       <c r="P15" t="s">
         <v>113</v>
@@ -3152,7 +3173,7 @@
         <v>117</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>43959</v>
+        <v>43960</v>
       </c>
       <c r="D16" t="s">
         <v>118</v>
@@ -3162,28 +3183,32 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H16" t="n">
-        <v>43378</v>
+        <v>44218</v>
       </c>
       <c r="I16" t="n">
-        <v>10.566</v>
+        <v>10.771</v>
       </c>
       <c r="J16" t="n">
-        <v>1440</v>
+        <v>840</v>
       </c>
       <c r="K16" t="n">
-        <v>0.351</v>
+        <v>0.205</v>
       </c>
       <c r="L16" t="n">
-        <v>1135</v>
+        <v>1055</v>
       </c>
       <c r="M16" t="n">
-        <v>0.277</v>
-      </c>
-      <c r="N16"/>
-      <c r="O16"/>
+        <v>0.257</v>
+      </c>
+      <c r="N16" t="n">
+        <v>951.571</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.232</v>
+      </c>
       <c r="P16" t="s">
         <v>119</v>
       </c>
@@ -3205,7 +3230,7 @@
         <v>124</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D17" t="s">
         <v>125</v>
@@ -3217,31 +3242,31 @@
         <v>127</v>
       </c>
       <c r="G17" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H17" t="n">
-        <v>61613</v>
+        <v>65509</v>
       </c>
       <c r="I17" t="n">
-        <v>5.44</v>
+        <v>5.784</v>
       </c>
       <c r="J17" t="n">
-        <v>1965</v>
+        <v>1949</v>
       </c>
       <c r="K17" t="n">
-        <v>0.173</v>
+        <v>0.172</v>
       </c>
       <c r="L17" t="n">
-        <v>2023.667</v>
+        <v>1953.667</v>
       </c>
       <c r="M17" t="n">
-        <v>0.178</v>
+        <v>0.172</v>
       </c>
       <c r="N17" t="n">
-        <v>2038</v>
+        <v>2000.429</v>
       </c>
       <c r="O17" t="n">
-        <v>0.18</v>
+        <v>0.176</v>
       </c>
       <c r="P17" t="s">
         <v>126</v>
@@ -3264,7 +3289,7 @@
         <v>131</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D18" t="s">
         <v>132</v>
@@ -3274,31 +3299,31 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H18" t="n">
-        <v>293992</v>
+        <v>302493</v>
       </c>
       <c r="I18" t="n">
-        <v>27.453</v>
+        <v>28.247</v>
       </c>
       <c r="J18" t="n">
-        <v>7071</v>
+        <v>3717</v>
       </c>
       <c r="K18" t="n">
-        <v>0.66</v>
+        <v>0.347</v>
       </c>
       <c r="L18" t="n">
-        <v>8296.333</v>
+        <v>5193.333</v>
       </c>
       <c r="M18" t="n">
-        <v>0.775</v>
+        <v>0.485</v>
       </c>
       <c r="N18" t="n">
-        <v>6335.429</v>
+        <v>6373.143</v>
       </c>
       <c r="O18" t="n">
-        <v>0.592</v>
+        <v>0.595</v>
       </c>
       <c r="P18" t="s">
         <v>43</v>
@@ -3321,7 +3346,7 @@
         <v>136</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D19" t="s">
         <v>137</v>
@@ -3333,31 +3358,31 @@
         <v>139</v>
       </c>
       <c r="G19" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H19" t="n">
-        <v>284480</v>
+        <v>308984</v>
       </c>
       <c r="I19" t="n">
-        <v>49.114</v>
+        <v>53.345</v>
       </c>
       <c r="J19" t="n">
-        <v>13800</v>
+        <v>10496</v>
       </c>
       <c r="K19" t="n">
-        <v>2.383</v>
+        <v>1.812</v>
       </c>
       <c r="L19" t="n">
-        <v>13229.667</v>
+        <v>12768</v>
       </c>
       <c r="M19" t="n">
-        <v>2.284</v>
+        <v>2.204</v>
       </c>
       <c r="N19" t="n">
-        <v>13045</v>
+        <v>12438.857</v>
       </c>
       <c r="O19" t="n">
-        <v>2.252</v>
+        <v>2.147</v>
       </c>
       <c r="P19" t="s">
         <v>140</v>
@@ -3380,7 +3405,7 @@
         <v>144</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D20" t="s">
         <v>145</v>
@@ -3392,16 +3417,18 @@
         <v>147</v>
       </c>
       <c r="G20" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H20" t="n">
-        <v>63300</v>
+        <v>40630</v>
       </c>
       <c r="I20" t="n">
-        <v>3.588</v>
+        <v>2.303</v>
       </c>
       <c r="J20"/>
-      <c r="K20"/>
+      <c r="K20" t="n">
+        <v>-0.212</v>
+      </c>
       <c r="L20"/>
       <c r="M20"/>
       <c r="N20"/>
@@ -3427,7 +3454,7 @@
         <v>151</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D21" t="s">
         <v>152</v>
@@ -3439,26 +3466,22 @@
         <v>154</v>
       </c>
       <c r="G21" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H21" t="n">
-        <v>35411</v>
+        <v>39079</v>
       </c>
       <c r="I21" t="n">
-        <v>5.459</v>
+        <v>6.025</v>
       </c>
       <c r="J21" t="n">
-        <v>1783</v>
+        <v>1773</v>
       </c>
       <c r="K21" t="n">
-        <v>0.275</v>
-      </c>
-      <c r="L21" t="n">
-        <v>1674.667</v>
-      </c>
-      <c r="M21" t="n">
-        <v>0.258</v>
-      </c>
+        <v>0.273</v>
+      </c>
+      <c r="L21"/>
+      <c r="M21"/>
       <c r="N21"/>
       <c r="O21"/>
       <c r="P21" t="s">
@@ -3482,7 +3505,7 @@
         <v>157</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D22" t="s">
         <v>158</v>
@@ -3492,31 +3515,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H22" t="n">
-        <v>61767</v>
+        <v>63372</v>
       </c>
       <c r="I22" t="n">
-        <v>46.563</v>
+        <v>47.772</v>
       </c>
       <c r="J22" t="n">
-        <v>1279</v>
+        <v>654</v>
       </c>
       <c r="K22" t="n">
-        <v>0.964</v>
+        <v>0.493</v>
       </c>
       <c r="L22" t="n">
-        <v>1454.667</v>
+        <v>961.333</v>
       </c>
       <c r="M22" t="n">
-        <v>1.096</v>
+        <v>0.725</v>
       </c>
       <c r="N22" t="n">
-        <v>1145.429</v>
+        <v>1170.714</v>
       </c>
       <c r="O22" t="n">
-        <v>0.863</v>
+        <v>0.882</v>
       </c>
       <c r="P22" t="s">
         <v>160</v>
@@ -3588,7 +3611,7 @@
         <v>171</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D24" t="s">
         <v>172</v>
@@ -3598,25 +3621,25 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H24" t="n">
-        <v>111983</v>
+        <v>119054</v>
       </c>
       <c r="I24" t="n">
-        <v>20.211</v>
+        <v>21.487</v>
       </c>
       <c r="J24"/>
       <c r="K24" t="n">
-        <v>0.147</v>
+        <v>0.116</v>
       </c>
       <c r="L24"/>
       <c r="M24" t="n">
-        <v>0.319</v>
+        <v>0.433</v>
       </c>
       <c r="N24"/>
       <c r="O24" t="n">
-        <v>0.374</v>
+        <v>0.388</v>
       </c>
       <c r="P24" t="s">
         <v>174</v>
@@ -3733,7 +3756,7 @@
         <v>192</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>43955</v>
+        <v>43958</v>
       </c>
       <c r="D27" t="s">
         <v>193</v>
@@ -3743,13 +3766,13 @@
       </c>
       <c r="F27"/>
       <c r="G27" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H27" t="n">
-        <v>135902</v>
+        <v>149948</v>
       </c>
       <c r="I27" t="n">
-        <v>4.374</v>
+        <v>4.826</v>
       </c>
       <c r="J27"/>
       <c r="K27"/>
@@ -3778,7 +3801,7 @@
         <v>200</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D28" t="s">
         <v>201</v>
@@ -3788,22 +3811,26 @@
       </c>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H28" t="n">
-        <v>90043</v>
+        <v>97384</v>
       </c>
       <c r="I28" t="n">
-        <v>8.639</v>
+        <v>9.343</v>
       </c>
       <c r="J28" t="n">
-        <v>2991</v>
+        <v>3093</v>
       </c>
       <c r="K28" t="n">
-        <v>0.287</v>
-      </c>
-      <c r="L28"/>
-      <c r="M28"/>
+        <v>0.297</v>
+      </c>
+      <c r="L28" t="n">
+        <v>3444</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.331</v>
+      </c>
       <c r="N28"/>
       <c r="O28"/>
       <c r="P28" t="s">
@@ -3872,7 +3899,7 @@
         <v>214</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D30" t="s">
         <v>215</v>
@@ -3884,31 +3911,31 @@
         <v>217</v>
       </c>
       <c r="G30" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H30" t="n">
-        <v>99058</v>
+        <v>108257</v>
       </c>
       <c r="I30" t="n">
-        <v>10.254</v>
+        <v>11.206</v>
       </c>
       <c r="J30" t="n">
-        <v>5022</v>
+        <v>4999</v>
       </c>
       <c r="K30" t="n">
-        <v>0.52</v>
+        <v>0.517</v>
       </c>
       <c r="L30" t="n">
-        <v>4500.333</v>
+        <v>4740.333</v>
       </c>
       <c r="M30" t="n">
-        <v>0.466</v>
+        <v>0.491</v>
       </c>
       <c r="N30" t="n">
-        <v>3246.714</v>
+        <v>3749.571</v>
       </c>
       <c r="O30" t="n">
-        <v>0.336</v>
+        <v>0.388</v>
       </c>
       <c r="P30" t="s">
         <v>216</v>
@@ -3931,7 +3958,7 @@
         <v>222</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>43958</v>
+        <v>43959</v>
       </c>
       <c r="D31" t="s">
         <v>223</v>
@@ -3941,31 +3968,31 @@
       </c>
       <c r="F31"/>
       <c r="G31" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H31" t="n">
-        <v>52704</v>
+        <v>53219</v>
       </c>
       <c r="I31" t="n">
-        <v>154.444</v>
+        <v>155.953</v>
       </c>
       <c r="J31" t="n">
-        <v>462</v>
+        <v>515</v>
       </c>
       <c r="K31" t="n">
-        <v>1.354</v>
+        <v>1.509</v>
       </c>
       <c r="L31" t="n">
-        <v>466.667</v>
+        <v>532.333</v>
       </c>
       <c r="M31" t="n">
-        <v>1.368</v>
+        <v>1.56</v>
       </c>
       <c r="N31" t="n">
-        <v>515.714</v>
+        <v>465.429</v>
       </c>
       <c r="O31" t="n">
-        <v>1.511</v>
+        <v>1.364</v>
       </c>
       <c r="P31" t="s">
         <v>224</v>
@@ -4039,7 +4066,7 @@
         <v>233</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D33" t="s">
         <v>229</v>
@@ -4051,31 +4078,31 @@
         <v>231</v>
       </c>
       <c r="G33" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H33" t="n">
-        <v>1437788</v>
+        <v>1609037</v>
       </c>
       <c r="I33" t="n">
-        <v>1.042</v>
+        <v>1.166</v>
       </c>
       <c r="J33" t="n">
-        <v>80375</v>
+        <v>85824</v>
       </c>
       <c r="K33" t="n">
+        <v>0.062</v>
+      </c>
+      <c r="L33" t="n">
+        <v>83874.667</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.061</v>
+      </c>
+      <c r="N33" t="n">
+        <v>80369.571</v>
+      </c>
+      <c r="O33" t="n">
         <v>0.058</v>
-      </c>
-      <c r="L33" t="n">
-        <v>81947.333</v>
-      </c>
-      <c r="M33" t="n">
-        <v>0.059</v>
-      </c>
-      <c r="N33" t="n">
-        <v>76447.714</v>
-      </c>
-      <c r="O33" t="n">
-        <v>0.055</v>
       </c>
       <c r="P33" t="s">
         <v>230</v>
@@ -4098,7 +4125,7 @@
         <v>235</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D34" t="s">
         <v>236</v>
@@ -4108,31 +4135,31 @@
       </c>
       <c r="F34"/>
       <c r="G34" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H34" t="n">
-        <v>103361</v>
+        <v>113452</v>
       </c>
       <c r="I34" t="n">
-        <v>0.378</v>
+        <v>0.415</v>
       </c>
       <c r="J34" t="n">
-        <v>6644</v>
+        <v>4753</v>
       </c>
       <c r="K34" t="n">
-        <v>0.024</v>
+        <v>0.017</v>
       </c>
       <c r="L34" t="n">
-        <v>4812.333</v>
+        <v>5578.333</v>
       </c>
       <c r="M34" t="n">
-        <v>0.018</v>
+        <v>0.02</v>
       </c>
       <c r="N34" t="n">
-        <v>3831.857</v>
+        <v>4348.571</v>
       </c>
       <c r="O34" t="n">
-        <v>0.014</v>
+        <v>0.016</v>
       </c>
       <c r="P34" t="s">
         <v>237</v>
@@ -4155,7 +4182,7 @@
         <v>241</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>43958</v>
+        <v>43959</v>
       </c>
       <c r="D35" t="s">
         <v>242</v>
@@ -4165,31 +4192,31 @@
       </c>
       <c r="F35"/>
       <c r="G35" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H35" t="n">
-        <v>544792</v>
+        <v>558899</v>
       </c>
       <c r="I35" t="n">
-        <v>6.486</v>
+        <v>6.654</v>
       </c>
       <c r="J35" t="n">
-        <v>13517</v>
+        <v>14107</v>
       </c>
       <c r="K35" t="n">
-        <v>0.161</v>
+        <v>0.168</v>
       </c>
       <c r="L35" t="n">
-        <v>12168</v>
+        <v>13118.667</v>
       </c>
       <c r="M35" t="n">
-        <v>0.145</v>
+        <v>0.156</v>
       </c>
       <c r="N35" t="n">
-        <v>11642.429</v>
+        <v>11982.286</v>
       </c>
       <c r="O35" t="n">
-        <v>0.139</v>
+        <v>0.143</v>
       </c>
       <c r="P35" t="s">
         <v>243</v>
@@ -4316,7 +4343,7 @@
         <v>260</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D38" t="s">
         <v>261</v>
@@ -4328,25 +4355,31 @@
         <v>263</v>
       </c>
       <c r="G38" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H38" t="n">
-        <v>1563557</v>
+        <v>1645076</v>
       </c>
       <c r="I38" t="n">
-        <v>25.86</v>
-      </c>
-      <c r="J38"/>
+        <v>27.209</v>
+      </c>
+      <c r="J38" t="n">
+        <v>36091</v>
+      </c>
       <c r="K38" t="n">
-        <v>0.226</v>
-      </c>
-      <c r="L38"/>
+        <v>0.597</v>
+      </c>
+      <c r="L38" t="n">
+        <v>31728</v>
+      </c>
       <c r="M38" t="n">
-        <v>0.461</v>
-      </c>
-      <c r="N38"/>
+        <v>0.525</v>
+      </c>
+      <c r="N38" t="n">
+        <v>30744.571</v>
+      </c>
       <c r="O38" t="n">
-        <v>0.493</v>
+        <v>0.508</v>
       </c>
       <c r="P38" t="s">
         <v>264</v>
@@ -4369,7 +4402,7 @@
         <v>267</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D39" t="s">
         <v>261</v>
@@ -4381,31 +4414,31 @@
         <v>263</v>
       </c>
       <c r="G39" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H39" t="n">
-        <v>2381288</v>
+        <v>2514234</v>
       </c>
       <c r="I39" t="n">
-        <v>39.385</v>
+        <v>41.584</v>
       </c>
       <c r="J39" t="n">
-        <v>70359</v>
+        <v>69171</v>
       </c>
       <c r="K39" t="n">
-        <v>1.164</v>
+        <v>1.144</v>
       </c>
       <c r="L39" t="n">
-        <v>63295</v>
+        <v>67768.333</v>
       </c>
       <c r="M39" t="n">
-        <v>1.047</v>
+        <v>1.121</v>
       </c>
       <c r="N39" t="n">
-        <v>57438.714</v>
+        <v>57913.857</v>
       </c>
       <c r="O39" t="n">
-        <v>0.95</v>
+        <v>0.958</v>
       </c>
       <c r="P39" t="s">
         <v>264</v>
@@ -4428,7 +4461,7 @@
         <v>270</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D40" t="s">
         <v>271</v>
@@ -4440,13 +4473,13 @@
         <v>273</v>
       </c>
       <c r="G40" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H40" t="n">
-        <v>190030</v>
+        <v>211997</v>
       </c>
       <c r="I40" t="n">
-        <v>1.502</v>
+        <v>1.676</v>
       </c>
       <c r="J40"/>
       <c r="K40"/>
@@ -4475,7 +4508,7 @@
         <v>276</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D41" t="s">
         <v>277</v>
@@ -4487,31 +4520,31 @@
         <v>278</v>
       </c>
       <c r="G41" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H41" t="n">
-        <v>306231</v>
+        <v>312728</v>
       </c>
       <c r="I41" t="n">
-        <v>2.421</v>
+        <v>2.473</v>
       </c>
       <c r="J41" t="n">
-        <v>4281</v>
+        <v>6061</v>
       </c>
       <c r="K41" t="n">
-        <v>0.034</v>
+        <v>0.048</v>
       </c>
       <c r="L41" t="n">
-        <v>4110</v>
+        <v>4768.667</v>
       </c>
       <c r="M41" t="n">
-        <v>0.032</v>
+        <v>0.038</v>
       </c>
       <c r="N41" t="n">
-        <v>5450.286</v>
+        <v>5210.143</v>
       </c>
       <c r="O41" t="n">
-        <v>0.043</v>
+        <v>0.041</v>
       </c>
       <c r="P41" t="s">
         <v>272</v>
@@ -4534,7 +4567,7 @@
         <v>281</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D42" t="s">
         <v>282</v>
@@ -4544,31 +4577,31 @@
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H42" t="n">
-        <v>353843</v>
+        <v>385104</v>
       </c>
       <c r="I42" t="n">
-        <v>18.845</v>
+        <v>20.51</v>
       </c>
       <c r="J42" t="n">
-        <v>17363</v>
+        <v>13978</v>
       </c>
       <c r="K42" t="n">
-        <v>0.925</v>
+        <v>0.744</v>
       </c>
       <c r="L42" t="n">
-        <v>15660.667</v>
+        <v>16208</v>
       </c>
       <c r="M42" t="n">
-        <v>0.834</v>
+        <v>0.863</v>
       </c>
       <c r="N42" t="n">
-        <v>14902.286</v>
+        <v>14606</v>
       </c>
       <c r="O42" t="n">
-        <v>0.794</v>
+        <v>0.778</v>
       </c>
       <c r="P42" t="s">
         <v>283</v>
@@ -4591,7 +4624,7 @@
         <v>286</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D43" t="s">
         <v>287</v>
@@ -4601,26 +4634,22 @@
       </c>
       <c r="F43"/>
       <c r="G43" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H43" t="n">
-        <v>25869</v>
+        <v>31041</v>
       </c>
       <c r="I43" t="n">
-        <v>0.481</v>
+        <v>0.577</v>
       </c>
       <c r="J43" t="n">
-        <v>1077</v>
+        <v>1611</v>
       </c>
       <c r="K43" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="L43" t="n">
-        <v>990.667</v>
-      </c>
-      <c r="M43" t="n">
-        <v>0.018</v>
-      </c>
+        <v>0.03</v>
+      </c>
+      <c r="L43"/>
+      <c r="M43"/>
       <c r="N43"/>
       <c r="O43"/>
       <c r="P43" t="s">
@@ -4644,7 +4673,7 @@
         <v>293</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D44" t="s">
         <v>294</v>
@@ -4656,31 +4685,25 @@
         <v>296</v>
       </c>
       <c r="G44" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H44" t="n">
-        <v>73016</v>
+        <v>76592</v>
       </c>
       <c r="I44" t="n">
-        <v>38.711</v>
-      </c>
-      <c r="J44" t="n">
-        <v>1947</v>
-      </c>
+        <v>40.606</v>
+      </c>
+      <c r="J44"/>
       <c r="K44" t="n">
-        <v>1.032</v>
-      </c>
-      <c r="L44" t="n">
-        <v>2288.667</v>
-      </c>
+        <v>0.541</v>
+      </c>
+      <c r="L44"/>
       <c r="M44" t="n">
-        <v>1.213</v>
-      </c>
-      <c r="N44" t="n">
-        <v>1699.429</v>
-      </c>
+        <v>0.976</v>
+      </c>
+      <c r="N44"/>
       <c r="O44" t="n">
-        <v>0.901</v>
+        <v>0.935</v>
       </c>
       <c r="P44" t="s">
         <v>295</v>
@@ -4703,7 +4726,7 @@
         <v>299</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D45" t="s">
         <v>300</v>
@@ -4713,31 +4736,25 @@
       </c>
       <c r="F45"/>
       <c r="G45" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H45" t="n">
-        <v>172191</v>
+        <v>183913</v>
       </c>
       <c r="I45" t="n">
-        <v>63.252</v>
-      </c>
-      <c r="J45" t="n">
-        <v>8103</v>
-      </c>
+        <v>67.558</v>
+      </c>
+      <c r="J45"/>
       <c r="K45" t="n">
-        <v>2.977</v>
-      </c>
-      <c r="L45" t="n">
-        <v>7695</v>
-      </c>
+        <v>1.315</v>
+      </c>
+      <c r="L45"/>
       <c r="M45" t="n">
-        <v>2.827</v>
-      </c>
-      <c r="N45" t="n">
-        <v>5631.857</v>
-      </c>
+        <v>2.427</v>
+      </c>
+      <c r="N45"/>
       <c r="O45" t="n">
-        <v>2.069</v>
+        <v>2.216</v>
       </c>
       <c r="P45" t="s">
         <v>43</v>
@@ -4760,7 +4777,7 @@
         <v>304</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D46" t="s">
         <v>305</v>
@@ -4770,31 +4787,31 @@
       </c>
       <c r="F46"/>
       <c r="G46" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H46" t="n">
-        <v>51883</v>
+        <v>54463</v>
       </c>
       <c r="I46" t="n">
-        <v>82.883</v>
+        <v>87.005</v>
       </c>
       <c r="J46" t="n">
-        <v>1350</v>
+        <v>1206</v>
       </c>
       <c r="K46" t="n">
-        <v>2.157</v>
+        <v>1.927</v>
       </c>
       <c r="L46" t="n">
-        <v>1181.333</v>
+        <v>1310</v>
       </c>
       <c r="M46" t="n">
-        <v>1.887</v>
+        <v>2.093</v>
       </c>
       <c r="N46" t="n">
-        <v>1320</v>
+        <v>1000.429</v>
       </c>
       <c r="O46" t="n">
-        <v>2.109</v>
+        <v>1.598</v>
       </c>
       <c r="P46" t="s">
         <v>306</v>
@@ -4817,7 +4834,7 @@
         <v>310</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D47" t="s">
         <v>311</v>
@@ -4827,32 +4844,20 @@
       </c>
       <c r="F47"/>
       <c r="G47" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H47" t="n">
-        <v>239628</v>
+        <v>256937</v>
       </c>
       <c r="I47" t="n">
-        <v>7.404</v>
-      </c>
-      <c r="J47" t="n">
-        <v>8609</v>
-      </c>
-      <c r="K47" t="n">
-        <v>0.266</v>
-      </c>
-      <c r="L47" t="n">
-        <v>8802.667</v>
-      </c>
-      <c r="M47" t="n">
-        <v>0.272</v>
-      </c>
-      <c r="N47" t="n">
-        <v>10120.571</v>
-      </c>
-      <c r="O47" t="n">
-        <v>0.313</v>
-      </c>
+        <v>7.938</v>
+      </c>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+      <c r="O47"/>
       <c r="P47" t="s">
         <v>312</v>
       </c>
@@ -4874,7 +4879,7 @@
         <v>317</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D48" t="s">
         <v>318</v>
@@ -4884,13 +4889,13 @@
       </c>
       <c r="F48"/>
       <c r="G48" t="n">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="H48" t="n">
-        <v>98399</v>
+        <v>107261</v>
       </c>
       <c r="I48" t="n">
-        <v>0.763</v>
+        <v>0.832</v>
       </c>
       <c r="J48"/>
       <c r="K48" t="n">
@@ -4902,7 +4907,7 @@
       </c>
       <c r="N48"/>
       <c r="O48" t="n">
-        <v>0.01</v>
+        <v>0.014</v>
       </c>
       <c r="P48" t="s">
         <v>319</v>
@@ -4984,7 +4989,7 @@
         <v>329</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>43958</v>
+        <v>43959</v>
       </c>
       <c r="D50" t="s">
         <v>330</v>
@@ -4996,20 +5001,32 @@
         <v>332</v>
       </c>
       <c r="G50" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H50" t="n">
-        <v>10227</v>
+        <v>10848</v>
       </c>
       <c r="I50" t="n">
-        <v>0.188</v>
-      </c>
-      <c r="J50"/>
-      <c r="K50"/>
-      <c r="L50"/>
-      <c r="M50"/>
-      <c r="N50"/>
-      <c r="O50"/>
+        <v>0.199</v>
+      </c>
+      <c r="J50" t="n">
+        <v>582</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="L50" t="n">
+        <v>517.667</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N50" t="n">
+        <v>372.571</v>
+      </c>
+      <c r="O50" t="n">
+        <v>0.007</v>
+      </c>
       <c r="P50" t="s">
         <v>331</v>
       </c>
@@ -5031,7 +5048,7 @@
         <v>336</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D51" t="s">
         <v>337</v>
@@ -5043,31 +5060,31 @@
         <v>339</v>
       </c>
       <c r="G51" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H51" t="n">
-        <v>14511</v>
+        <v>16309</v>
       </c>
       <c r="I51" t="n">
-        <v>0.498</v>
+        <v>0.56</v>
       </c>
       <c r="J51" t="n">
-        <v>415</v>
+        <v>817</v>
       </c>
       <c r="K51" t="n">
-        <v>0.014</v>
+        <v>0.028</v>
       </c>
       <c r="L51" t="n">
-        <v>290.333</v>
+        <v>737.667</v>
       </c>
       <c r="M51" t="n">
-        <v>0.01</v>
+        <v>0.025</v>
       </c>
       <c r="N51" t="n">
-        <v>357.143</v>
+        <v>458.714</v>
       </c>
       <c r="O51" t="n">
-        <v>0.012</v>
+        <v>0.016</v>
       </c>
       <c r="P51" t="s">
         <v>338</v>
@@ -5090,7 +5107,7 @@
         <v>343</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D52" t="s">
         <v>344</v>
@@ -5100,25 +5117,25 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H52" t="n">
-        <v>249655</v>
+        <v>254456</v>
       </c>
       <c r="I52" t="n">
-        <v>14.57</v>
+        <v>14.85</v>
       </c>
       <c r="J52" t="n">
-        <v>3488</v>
+        <v>4442</v>
       </c>
       <c r="K52" t="n">
-        <v>0.204</v>
+        <v>0.259</v>
       </c>
       <c r="L52" t="n">
-        <v>3713.333</v>
+        <v>4035.667</v>
       </c>
       <c r="M52" t="n">
-        <v>0.217</v>
+        <v>0.235</v>
       </c>
       <c r="N52"/>
       <c r="O52"/>
@@ -5143,7 +5160,7 @@
         <v>350</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D53" t="s">
         <v>351</v>
@@ -5153,31 +5170,31 @@
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H53" t="n">
-        <v>175835</v>
+        <v>190326</v>
       </c>
       <c r="I53" t="n">
-        <v>36.463</v>
+        <v>39.468</v>
       </c>
       <c r="J53" t="n">
-        <v>7812</v>
+        <v>7287</v>
       </c>
       <c r="K53" t="n">
-        <v>1.62</v>
+        <v>1.511</v>
       </c>
       <c r="L53" t="n">
-        <v>6635.667</v>
+        <v>7434.333</v>
       </c>
       <c r="M53" t="n">
-        <v>1.376</v>
+        <v>1.542</v>
       </c>
       <c r="N53" t="n">
-        <v>5133.857</v>
+        <v>5729</v>
       </c>
       <c r="O53" t="n">
-        <v>1.065</v>
+        <v>1.188</v>
       </c>
       <c r="P53" t="s">
         <v>352</v>
@@ -5200,7 +5217,7 @@
         <v>355</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>43958</v>
+        <v>43959</v>
       </c>
       <c r="D54" t="s">
         <v>356</v>
@@ -5210,25 +5227,25 @@
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H54" t="n">
-        <v>22492</v>
+        <v>23835</v>
       </c>
       <c r="I54" t="n">
-        <v>0.109</v>
+        <v>0.116</v>
       </c>
       <c r="J54" t="n">
-        <v>1284</v>
+        <v>1343</v>
       </c>
       <c r="K54" t="n">
-        <v>0.006</v>
+        <v>0.007</v>
       </c>
       <c r="L54" t="n">
-        <v>1318.667</v>
+        <v>1441</v>
       </c>
       <c r="M54" t="n">
-        <v>0.006</v>
+        <v>0.007</v>
       </c>
       <c r="N54"/>
       <c r="O54"/>
@@ -5302,7 +5319,7 @@
         <v>368</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D56" t="s">
         <v>369</v>
@@ -5312,31 +5329,31 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H56" t="n">
-        <v>257247</v>
+        <v>283517</v>
       </c>
       <c r="I56" t="n">
-        <v>1.165</v>
+        <v>1.284</v>
       </c>
       <c r="J56" t="n">
-        <v>12469</v>
+        <v>13492</v>
       </c>
       <c r="K56" t="n">
-        <v>0.056</v>
+        <v>0.061</v>
       </c>
       <c r="L56" t="n">
-        <v>11614.333</v>
+        <v>12913</v>
       </c>
       <c r="M56" t="n">
+        <v>0.058</v>
+      </c>
+      <c r="N56" t="n">
+        <v>11498.857</v>
+      </c>
+      <c r="O56" t="n">
         <v>0.052</v>
-      </c>
-      <c r="N56" t="n">
-        <v>10730.857</v>
-      </c>
-      <c r="O56" t="n">
-        <v>0.048</v>
       </c>
       <c r="P56" t="s">
         <v>370</v>
@@ -5359,7 +5376,7 @@
         <v>374</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D57" t="s">
         <v>375</v>
@@ -5371,31 +5388,31 @@
         <v>376</v>
       </c>
       <c r="G57" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H57" t="n">
-        <v>39093</v>
+        <v>41649</v>
       </c>
       <c r="I57" t="n">
-        <v>9.06</v>
+        <v>9.653</v>
       </c>
       <c r="J57" t="n">
-        <v>1079</v>
+        <v>1293</v>
       </c>
       <c r="K57" t="n">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="L57" t="n">
-        <v>1179</v>
+        <v>1211.667</v>
       </c>
       <c r="M57" t="n">
-        <v>0.273</v>
+        <v>0.281</v>
       </c>
       <c r="N57" t="n">
-        <v>1192</v>
+        <v>1185</v>
       </c>
       <c r="O57" t="n">
-        <v>0.276</v>
+        <v>0.275</v>
       </c>
       <c r="P57" t="s">
         <v>43</v>
@@ -5418,7 +5435,7 @@
         <v>380</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D58" t="s">
         <v>381</v>
@@ -5430,31 +5447,31 @@
         <v>383</v>
       </c>
       <c r="G58" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H58" t="n">
-        <v>13096</v>
+        <v>14646</v>
       </c>
       <c r="I58" t="n">
-        <v>1.836</v>
+        <v>2.053</v>
       </c>
       <c r="J58" t="n">
-        <v>599</v>
+        <v>800</v>
       </c>
       <c r="K58" t="n">
-        <v>0.084</v>
+        <v>0.112</v>
       </c>
       <c r="L58" t="n">
-        <v>547</v>
+        <v>716.333</v>
       </c>
       <c r="M58" t="n">
-        <v>0.077</v>
+        <v>0.1</v>
       </c>
       <c r="N58" t="n">
-        <v>456.143</v>
+        <v>554.286</v>
       </c>
       <c r="O58" t="n">
-        <v>0.064</v>
+        <v>0.078</v>
       </c>
       <c r="P58" t="s">
         <v>384</v>
@@ -5477,7 +5494,7 @@
         <v>388</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>43958</v>
+        <v>43961</v>
       </c>
       <c r="D59" t="s">
         <v>389</v>
@@ -5487,13 +5504,13 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H59" t="n">
-        <v>448020</v>
+        <v>494250</v>
       </c>
       <c r="I59" t="n">
-        <v>13.588</v>
+        <v>14.99</v>
       </c>
       <c r="J59"/>
       <c r="K59"/>
@@ -5522,7 +5539,7 @@
         <v>395</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D60" t="s">
         <v>396</v>
@@ -5532,22 +5549,26 @@
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H60" t="n">
-        <v>126387</v>
+        <v>136706</v>
       </c>
       <c r="I60" t="n">
-        <v>1.153</v>
+        <v>1.248</v>
       </c>
       <c r="J60" t="n">
-        <v>6875</v>
+        <v>5216</v>
       </c>
       <c r="K60" t="n">
-        <v>0.063</v>
-      </c>
-      <c r="L60"/>
-      <c r="M60"/>
+        <v>0.048</v>
+      </c>
+      <c r="L60" t="n">
+        <v>5731.333</v>
+      </c>
+      <c r="M60" t="n">
+        <v>0.053</v>
+      </c>
       <c r="N60"/>
       <c r="O60"/>
       <c r="P60" t="s">
@@ -5571,7 +5592,7 @@
         <v>400</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>43959</v>
+        <v>43960</v>
       </c>
       <c r="D61" t="s">
         <v>401</v>
@@ -5583,31 +5604,31 @@
         <v>403</v>
       </c>
       <c r="G61" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H61" t="n">
-        <v>443506</v>
+        <v>460686</v>
       </c>
       <c r="I61" t="n">
-        <v>11.719</v>
+        <v>12.172</v>
       </c>
       <c r="J61" t="n">
-        <v>17512</v>
+        <v>17180</v>
       </c>
       <c r="K61" t="n">
-        <v>0.463</v>
+        <v>0.454</v>
       </c>
       <c r="L61" t="n">
-        <v>16412</v>
+        <v>16739.333</v>
       </c>
       <c r="M61" t="n">
-        <v>0.434</v>
+        <v>0.442</v>
       </c>
       <c r="N61" t="n">
-        <v>12696.857</v>
+        <v>13524.714</v>
       </c>
       <c r="O61" t="n">
-        <v>0.336</v>
+        <v>0.358</v>
       </c>
       <c r="P61" t="s">
         <v>404</v>
@@ -5687,7 +5708,7 @@
         <v>414</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D63" t="s">
         <v>415</v>
@@ -5697,31 +5718,31 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H63" t="n">
-        <v>120458</v>
+        <v>127769</v>
       </c>
       <c r="I63" t="n">
-        <v>41.81</v>
+        <v>44.348</v>
       </c>
       <c r="J63" t="n">
-        <v>3963</v>
+        <v>3215</v>
       </c>
       <c r="K63" t="n">
-        <v>1.376</v>
+        <v>1.116</v>
       </c>
       <c r="L63" t="n">
-        <v>3565.333</v>
+        <v>3758</v>
       </c>
       <c r="M63" t="n">
-        <v>1.238</v>
+        <v>1.305</v>
       </c>
       <c r="N63" t="n">
-        <v>3247.429</v>
+        <v>3333.429</v>
       </c>
       <c r="O63" t="n">
-        <v>1.127</v>
+        <v>1.157</v>
       </c>
       <c r="P63" t="s">
         <v>416</v>
@@ -5744,7 +5765,7 @@
         <v>420</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>43959</v>
+        <v>43960</v>
       </c>
       <c r="D64" t="s">
         <v>421</v>
@@ -5756,31 +5777,31 @@
         <v>423</v>
       </c>
       <c r="G64" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H64" t="n">
-        <v>237280</v>
+        <v>248056</v>
       </c>
       <c r="I64" t="n">
-        <v>12.334</v>
+        <v>12.894</v>
       </c>
       <c r="J64" t="n">
-        <v>10667</v>
+        <v>10776</v>
       </c>
       <c r="K64" t="n">
-        <v>0.554</v>
+        <v>0.56</v>
       </c>
       <c r="L64" t="n">
-        <v>10479.333</v>
+        <v>10305.667</v>
       </c>
       <c r="M64" t="n">
-        <v>0.544</v>
+        <v>0.535</v>
       </c>
       <c r="N64" t="n">
-        <v>7656</v>
+        <v>8216.571</v>
       </c>
       <c r="O64" t="n">
-        <v>0.398</v>
+        <v>0.427</v>
       </c>
       <c r="P64" t="s">
         <v>422</v>
@@ -5803,7 +5824,7 @@
         <v>426</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D65" t="s">
         <v>427</v>
@@ -5813,31 +5834,31 @@
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H65" t="n">
-        <v>4987468</v>
+        <v>5448463</v>
       </c>
       <c r="I65" t="n">
-        <v>34.176</v>
+        <v>37.335</v>
       </c>
       <c r="J65" t="n">
-        <v>184276</v>
+        <v>226499</v>
       </c>
       <c r="K65" t="n">
-        <v>1.263</v>
+        <v>1.552</v>
       </c>
       <c r="L65" t="n">
-        <v>175703.667</v>
+        <v>215090.333</v>
       </c>
       <c r="M65" t="n">
-        <v>1.204</v>
+        <v>1.474</v>
       </c>
       <c r="N65" t="n">
-        <v>180523</v>
+        <v>192637.714</v>
       </c>
       <c r="O65" t="n">
-        <v>1.237</v>
+        <v>1.32</v>
       </c>
       <c r="P65" t="s">
         <v>428</v>
@@ -5860,7 +5881,7 @@
         <v>432</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>43957</v>
+        <v>43960</v>
       </c>
       <c r="D66" t="s">
         <v>433</v>
@@ -5870,31 +5891,31 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H66" t="n">
-        <v>37315</v>
+        <v>41385</v>
       </c>
       <c r="I66" t="n">
-        <v>2.881</v>
+        <v>3.195</v>
       </c>
       <c r="J66" t="n">
-        <v>1323</v>
+        <v>1198</v>
       </c>
       <c r="K66" t="n">
-        <v>0.102</v>
+        <v>0.092</v>
       </c>
       <c r="L66" t="n">
-        <v>988.333</v>
+        <v>1356.667</v>
       </c>
       <c r="M66" t="n">
-        <v>0.076</v>
+        <v>0.104</v>
       </c>
       <c r="N66" t="n">
-        <v>1102</v>
+        <v>1154.571</v>
       </c>
       <c r="O66" t="n">
-        <v>0.085</v>
+        <v>0.089</v>
       </c>
       <c r="P66" t="s">
         <v>434</v>
@@ -5917,7 +5938,7 @@
         <v>438</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D67" t="s">
         <v>439</v>
@@ -5927,22 +5948,26 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H67" t="n">
-        <v>405685</v>
+        <v>433500</v>
       </c>
       <c r="I67" t="n">
-        <v>11.653</v>
+        <v>12.452</v>
       </c>
       <c r="J67" t="n">
-        <v>16026</v>
+        <v>14778</v>
       </c>
       <c r="K67" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="L67"/>
-      <c r="M67"/>
+        <v>0.424</v>
+      </c>
+      <c r="L67" t="n">
+        <v>14613.667</v>
+      </c>
+      <c r="M67" t="n">
+        <v>0.419</v>
+      </c>
       <c r="N67"/>
       <c r="O67"/>
       <c r="P67" t="s">
@@ -5966,7 +5991,7 @@
         <v>442</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>43959</v>
+        <v>43960</v>
       </c>
       <c r="D68" t="s">
         <v>443</v>
@@ -5978,31 +6003,31 @@
         <v>445</v>
       </c>
       <c r="G68" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H68" t="n">
-        <v>19369</v>
+        <v>20217</v>
       </c>
       <c r="I68" t="n">
-        <v>1.157</v>
+        <v>1.207</v>
       </c>
       <c r="J68" t="n">
-        <v>872</v>
+        <v>848</v>
       </c>
       <c r="K68" t="n">
-        <v>0.052</v>
+        <v>0.051</v>
       </c>
       <c r="L68" t="n">
-        <v>1027</v>
+        <v>915.667</v>
       </c>
       <c r="M68" t="n">
-        <v>0.061</v>
+        <v>0.055</v>
       </c>
       <c r="N68" t="n">
-        <v>941.429</v>
+        <v>892.571</v>
       </c>
       <c r="O68" t="n">
-        <v>0.056</v>
+        <v>0.053</v>
       </c>
       <c r="P68" t="s">
         <v>446</v>
@@ -6025,7 +6050,7 @@
         <v>451</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D69" t="s">
         <v>452</v>
@@ -6037,31 +6062,31 @@
         <v>453</v>
       </c>
       <c r="G69" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H69" t="n">
-        <v>122995</v>
+        <v>134533</v>
       </c>
       <c r="I69" t="n">
-        <v>18.075</v>
+        <v>19.771</v>
       </c>
       <c r="J69" t="n">
-        <v>5521</v>
+        <v>5728</v>
       </c>
       <c r="K69" t="n">
-        <v>0.811</v>
+        <v>0.842</v>
       </c>
       <c r="L69" t="n">
-        <v>5511.333</v>
+        <v>5686.333</v>
       </c>
       <c r="M69" t="n">
-        <v>0.81</v>
+        <v>0.836</v>
       </c>
       <c r="N69" t="n">
-        <v>5335.714</v>
+        <v>5413.714</v>
       </c>
       <c r="O69" t="n">
-        <v>0.784</v>
+        <v>0.796</v>
       </c>
       <c r="P69" t="s">
         <v>43</v>
@@ -6174,7 +6199,7 @@
         <v>465</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D72" t="s">
         <v>466</v>
@@ -6184,31 +6209,25 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H72" t="n">
-        <v>114461</v>
+        <v>119859</v>
       </c>
       <c r="I72" t="n">
-        <v>20.965</v>
-      </c>
-      <c r="J72" t="n">
-        <v>4694</v>
-      </c>
+        <v>21.954</v>
+      </c>
+      <c r="J72"/>
       <c r="K72" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="L72" t="n">
-        <v>4865.667</v>
-      </c>
+        <v>0.273</v>
+      </c>
+      <c r="L72"/>
       <c r="M72" t="n">
-        <v>0.891</v>
-      </c>
-      <c r="N72" t="n">
-        <v>3341.286</v>
-      </c>
+        <v>0.616</v>
+      </c>
+      <c r="N72"/>
       <c r="O72" t="n">
-        <v>0.612</v>
+        <v>0.619</v>
       </c>
       <c r="P72" t="s">
         <v>468</v>
@@ -6231,7 +6250,7 @@
         <v>473</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D73" t="s">
         <v>474</v>
@@ -6241,31 +6260,31 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H73" t="n">
-        <v>61027</v>
+        <v>62828</v>
       </c>
       <c r="I73" t="n">
-        <v>29.355</v>
+        <v>30.221</v>
       </c>
       <c r="J73" t="n">
-        <v>1049</v>
+        <v>625</v>
       </c>
       <c r="K73" t="n">
-        <v>0.505</v>
+        <v>0.301</v>
       </c>
       <c r="L73" t="n">
-        <v>1184.333</v>
+        <v>950</v>
       </c>
       <c r="M73" t="n">
-        <v>0.57</v>
+        <v>0.457</v>
       </c>
       <c r="N73" t="n">
-        <v>961</v>
+        <v>1044</v>
       </c>
       <c r="O73" t="n">
-        <v>0.462</v>
+        <v>0.502</v>
       </c>
       <c r="P73" t="s">
         <v>476</v>
@@ -6288,7 +6307,7 @@
         <v>480</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D74" t="s">
         <v>481</v>
@@ -6300,31 +6319,31 @@
         <v>483</v>
       </c>
       <c r="G74" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H74" t="n">
-        <v>292153</v>
+        <v>324079</v>
       </c>
       <c r="I74" t="n">
-        <v>4.926</v>
+        <v>5.464</v>
       </c>
       <c r="J74" t="n">
-        <v>12774</v>
+        <v>16327</v>
       </c>
       <c r="K74" t="n">
-        <v>0.215</v>
+        <v>0.275</v>
       </c>
       <c r="L74" t="n">
-        <v>11537.333</v>
+        <v>14900</v>
       </c>
       <c r="M74" t="n">
-        <v>0.194</v>
+        <v>0.251</v>
       </c>
       <c r="N74" t="n">
-        <v>12089</v>
+        <v>13341.857</v>
       </c>
       <c r="O74" t="n">
-        <v>0.204</v>
+        <v>0.225</v>
       </c>
       <c r="P74" t="s">
         <v>482</v>
@@ -6347,7 +6366,7 @@
         <v>487</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D75" t="s">
         <v>488</v>
@@ -6357,31 +6376,31 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H75" t="n">
-        <v>654863</v>
+        <v>663886</v>
       </c>
       <c r="I75" t="n">
-        <v>12.773</v>
+        <v>12.949</v>
       </c>
       <c r="J75" t="n">
-        <v>5475</v>
+        <v>3856</v>
       </c>
       <c r="K75" t="n">
-        <v>0.107</v>
+        <v>0.075</v>
       </c>
       <c r="L75" t="n">
-        <v>4875.333</v>
+        <v>4832.667</v>
       </c>
       <c r="M75" t="n">
-        <v>0.095</v>
+        <v>0.094</v>
       </c>
       <c r="N75" t="n">
-        <v>4542</v>
+        <v>4701.857</v>
       </c>
       <c r="O75" t="n">
-        <v>0.089</v>
+        <v>0.092</v>
       </c>
       <c r="P75" t="s">
         <v>489</v>
@@ -6404,7 +6423,7 @@
         <v>493</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>43951</v>
+        <v>43958</v>
       </c>
       <c r="D76" t="s">
         <v>494</v>
@@ -6412,15 +6431,17 @@
       <c r="E76" t="s">
         <v>495</v>
       </c>
-      <c r="F76"/>
+      <c r="F76" t="s">
+        <v>496</v>
+      </c>
       <c r="G76" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H76" t="n">
-        <v>1351130</v>
+        <v>1625211</v>
       </c>
       <c r="I76" t="n">
-        <v>28.898</v>
+        <v>34.76</v>
       </c>
       <c r="J76"/>
       <c r="K76"/>
@@ -6429,33 +6450,33 @@
       <c r="N76"/>
       <c r="O76"/>
       <c r="P76" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="Q76" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="R76" t="s">
         <v>24</v>
       </c>
       <c r="S76" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B77" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>43954</v>
       </c>
       <c r="D77" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="E77" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
@@ -6474,151 +6495,151 @@
       <c r="N77"/>
       <c r="O77"/>
       <c r="P77" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q77" t="s">
         <v>502</v>
-      </c>
-      <c r="Q77" t="s">
-        <v>501</v>
       </c>
       <c r="R77" t="s">
         <v>94</v>
       </c>
       <c r="S77" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B78" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D78" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E78" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H78" t="n">
-        <v>301675</v>
+        <v>309595</v>
       </c>
       <c r="I78" t="n">
-        <v>34.857</v>
+        <v>35.772</v>
       </c>
       <c r="J78"/>
       <c r="K78" t="n">
-        <v>0.131</v>
+        <v>0.045</v>
       </c>
       <c r="L78"/>
       <c r="M78" t="n">
-        <v>0.468</v>
+        <v>0.336</v>
       </c>
       <c r="N78"/>
       <c r="O78" t="n">
-        <v>0.429</v>
+        <v>0.434</v>
       </c>
       <c r="P78" t="s">
+        <v>508</v>
+      </c>
+      <c r="Q78" t="s">
         <v>507</v>
       </c>
-      <c r="Q78" t="s">
-        <v>506</v>
-      </c>
       <c r="R78" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="S78" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B79" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D79" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E79" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H79" t="n">
-        <v>66460</v>
+        <v>67133</v>
       </c>
       <c r="I79" t="n">
-        <v>2.79</v>
+        <v>2.819</v>
       </c>
       <c r="J79" t="n">
-        <v>414</v>
+        <v>272</v>
       </c>
       <c r="K79" t="n">
-        <v>0.017</v>
+        <v>0.011</v>
       </c>
       <c r="L79" t="n">
-        <v>500.667</v>
+        <v>362.333</v>
       </c>
       <c r="M79" t="n">
-        <v>0.021</v>
+        <v>0.015</v>
       </c>
       <c r="N79" t="n">
-        <v>445.714</v>
+        <v>434.143</v>
       </c>
       <c r="O79" t="n">
-        <v>0.019</v>
+        <v>0.018</v>
       </c>
       <c r="P79" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="Q79" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="R79" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="S79" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B80" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D80" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="E80" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H80" t="n">
-        <v>90016</v>
+        <v>97177</v>
       </c>
       <c r="I80" t="n">
-        <v>1.29</v>
+        <v>1.392</v>
       </c>
       <c r="J80"/>
       <c r="K80" t="n">
@@ -6630,547 +6651,535 @@
       </c>
       <c r="N80"/>
       <c r="O80" t="n">
-        <v>0.04</v>
+        <v>0.045</v>
       </c>
       <c r="P80" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="Q80" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="R80" t="s">
         <v>94</v>
       </c>
       <c r="S80" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B81" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="D81" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E81" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H81" t="n">
-        <v>25555</v>
+        <v>27420</v>
       </c>
       <c r="I81" t="n">
-        <v>2.162</v>
-      </c>
-      <c r="J81" t="n">
-        <v>390</v>
-      </c>
-      <c r="K81" t="n">
-        <v>0.033</v>
-      </c>
-      <c r="L81" t="n">
-        <v>383</v>
-      </c>
-      <c r="M81" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="N81" t="n">
-        <v>499</v>
-      </c>
-      <c r="O81" t="n">
-        <v>0.042</v>
-      </c>
+        <v>2.32</v>
+      </c>
+      <c r="J81"/>
+      <c r="K81"/>
+      <c r="L81"/>
+      <c r="M81"/>
+      <c r="N81"/>
+      <c r="O81"/>
       <c r="P81" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="Q81" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="R81" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="S81" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B82" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D82" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E82" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H82" t="n">
-        <v>1265119</v>
+        <v>1334411</v>
       </c>
       <c r="I82" t="n">
-        <v>15</v>
+        <v>15.822</v>
       </c>
       <c r="J82" t="n">
-        <v>30395</v>
+        <v>35605</v>
       </c>
       <c r="K82" t="n">
-        <v>0.36</v>
+        <v>0.422</v>
       </c>
       <c r="L82" t="n">
-        <v>31327</v>
+        <v>33229</v>
       </c>
       <c r="M82" t="n">
-        <v>0.371</v>
+        <v>0.394</v>
       </c>
       <c r="N82"/>
       <c r="O82"/>
       <c r="P82" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="Q82" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="R82" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="S82" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B83" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D83" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E83" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="F83" t="s">
+        <v>543</v>
+      </c>
+      <c r="G83" t="n">
+        <v>32</v>
+      </c>
+      <c r="H83" t="n">
+        <v>55203</v>
+      </c>
+      <c r="I83" t="n">
+        <v>1.207</v>
+      </c>
+      <c r="J83" t="n">
+        <v>3161</v>
+      </c>
+      <c r="K83" t="n">
+        <v>0.069</v>
+      </c>
+      <c r="L83" t="n">
+        <v>3493</v>
+      </c>
+      <c r="M83" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="N83" t="n">
+        <v>2967.286</v>
+      </c>
+      <c r="O83" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="P83" t="s">
         <v>542</v>
       </c>
-      <c r="G83" t="n">
-        <v>30</v>
-      </c>
-      <c r="H83" t="n">
-        <v>47603</v>
-      </c>
-      <c r="I83" t="n">
-        <v>1.041</v>
-      </c>
-      <c r="J83" t="n">
-        <v>3509</v>
-      </c>
-      <c r="K83" t="n">
-        <v>0.077</v>
-      </c>
-      <c r="L83" t="n">
-        <v>2795.667</v>
-      </c>
-      <c r="M83" t="n">
-        <v>0.061</v>
-      </c>
-      <c r="N83" t="n">
-        <v>2618</v>
-      </c>
-      <c r="O83" t="n">
-        <v>0.057</v>
-      </c>
-      <c r="P83" t="s">
-        <v>541</v>
-      </c>
       <c r="Q83" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="R83" t="s">
         <v>53</v>
       </c>
       <c r="S83" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B84" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D84" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E84" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H84" t="n">
-        <v>159155</v>
+        <v>176403</v>
       </c>
       <c r="I84" t="n">
-        <v>3.639</v>
+        <v>4.034</v>
       </c>
       <c r="J84" t="n">
-        <v>7586</v>
+        <v>9296</v>
       </c>
       <c r="K84" t="n">
-        <v>0.173</v>
+        <v>0.213</v>
       </c>
       <c r="L84" t="n">
-        <v>6465.333</v>
+        <v>8278</v>
       </c>
       <c r="M84" t="n">
-        <v>0.148</v>
+        <v>0.189</v>
       </c>
       <c r="N84" t="n">
-        <v>5801.429</v>
+        <v>6668.571</v>
       </c>
       <c r="O84" t="n">
-        <v>0.132</v>
+        <v>0.152</v>
       </c>
       <c r="P84" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="Q84" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="R84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="S84" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B85" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D85" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E85" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H85" t="n">
-        <v>1139626</v>
+        <v>1270408</v>
       </c>
       <c r="I85" t="n">
-        <v>16.787</v>
+        <v>18.714</v>
       </c>
       <c r="J85" t="n">
-        <v>65092</v>
+        <v>63339</v>
       </c>
       <c r="K85" t="n">
-        <v>0.959</v>
+        <v>0.933</v>
       </c>
       <c r="L85" t="n">
-        <v>63979</v>
+        <v>65291.333</v>
       </c>
       <c r="M85" t="n">
-        <v>0.943</v>
+        <v>0.962</v>
       </c>
       <c r="N85" t="n">
-        <v>64021.143</v>
+        <v>63153.143</v>
       </c>
       <c r="O85" t="n">
-        <v>0.943</v>
+        <v>0.93</v>
       </c>
       <c r="P85" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="Q85" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="R85" t="s">
         <v>94</v>
       </c>
       <c r="S85" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B86" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D86" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="E86" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H86" t="n">
-        <v>1534533</v>
+        <v>1728443</v>
       </c>
       <c r="I86" t="n">
-        <v>22.605</v>
+        <v>25.461</v>
       </c>
       <c r="J86" t="n">
-        <v>86583</v>
+        <v>96878</v>
       </c>
       <c r="K86" t="n">
-        <v>1.275</v>
+        <v>1.427</v>
       </c>
       <c r="L86" t="n">
-        <v>80284</v>
+        <v>93496.667</v>
       </c>
       <c r="M86" t="n">
-        <v>1.182</v>
+        <v>1.377</v>
       </c>
       <c r="N86" t="n">
-        <v>90116.857</v>
+        <v>85205.857</v>
       </c>
       <c r="O86" t="n">
-        <v>1.327</v>
+        <v>1.255</v>
       </c>
       <c r="P86" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="Q86" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="R86" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="S86" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B87" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="D87" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E87" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="F87"/>
       <c r="G87" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H87" t="n">
-        <v>8105513</v>
+        <v>8709630</v>
       </c>
       <c r="I87" t="n">
-        <v>24.488</v>
+        <v>26.313</v>
       </c>
       <c r="J87" t="n">
-        <v>318720</v>
+        <v>300842</v>
       </c>
       <c r="K87" t="n">
-        <v>0.963</v>
+        <v>0.909</v>
       </c>
       <c r="L87" t="n">
-        <v>273379.667</v>
+        <v>307612.333</v>
       </c>
       <c r="M87" t="n">
-        <v>0.826</v>
+        <v>0.929</v>
       </c>
       <c r="N87" t="n">
-        <v>264249.143</v>
+        <v>272055.571</v>
       </c>
       <c r="O87" t="n">
-        <v>0.798</v>
+        <v>0.822</v>
       </c>
       <c r="P87" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="Q87" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="R87" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="S87" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B88" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>43950</v>
+        <v>43952</v>
       </c>
       <c r="D88" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E88" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H88" t="n">
-        <v>629731</v>
+        <v>695283</v>
       </c>
       <c r="I88" t="n">
-        <v>1.902</v>
+        <v>2.101</v>
       </c>
       <c r="J88" t="n">
-        <v>23081</v>
+        <v>23633</v>
       </c>
       <c r="K88" t="n">
-        <v>0.07</v>
+        <v>0.071</v>
       </c>
       <c r="L88" t="n">
-        <v>23107</v>
+        <v>24423.333</v>
       </c>
       <c r="M88" t="n">
-        <v>0.07</v>
+        <v>0.074</v>
       </c>
       <c r="N88" t="n">
-        <v>20113.714</v>
+        <v>21015.714</v>
       </c>
       <c r="O88" t="n">
-        <v>0.061</v>
+        <v>0.063</v>
       </c>
       <c r="P88" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="Q88" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="R88" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="S88" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B89" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D89" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="E89" t="s">
         <v>126</v>
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H89" t="n">
-        <v>25698</v>
+        <v>27461</v>
       </c>
       <c r="I89" t="n">
-        <v>7.398</v>
+        <v>7.905</v>
       </c>
       <c r="J89" t="n">
-        <v>1042</v>
+        <v>623</v>
       </c>
       <c r="K89" t="n">
-        <v>0.3</v>
+        <v>0.179</v>
       </c>
       <c r="L89" t="n">
-        <v>964.333</v>
+        <v>935</v>
       </c>
       <c r="M89" t="n">
-        <v>0.278</v>
+        <v>0.269</v>
       </c>
       <c r="N89" t="n">
-        <v>850.143</v>
+        <v>899.571</v>
       </c>
       <c r="O89" t="n">
-        <v>0.245</v>
+        <v>0.259</v>
       </c>
       <c r="P89" t="s">
         <v>126</v>
       </c>
       <c r="Q89" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="R89" t="s">
         <v>24</v>
       </c>
       <c r="S89" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B90" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="D90" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="E90" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
@@ -7189,61 +7198,65 @@
       <c r="N90"/>
       <c r="O90"/>
       <c r="P90" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="Q90" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="R90" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="S90" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B91" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>43957</v>
+        <v>43959</v>
       </c>
       <c r="D91" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="E91" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H91" t="n">
-        <v>7808</v>
+        <v>8741</v>
       </c>
       <c r="I91" t="n">
-        <v>0.525</v>
-      </c>
-      <c r="J91"/>
-      <c r="K91"/>
+        <v>0.588</v>
+      </c>
+      <c r="J91" t="n">
+        <v>600</v>
+      </c>
+      <c r="K91" t="n">
+        <v>0.04</v>
+      </c>
       <c r="L91"/>
       <c r="M91"/>
       <c r="N91"/>
       <c r="O91"/>
       <c r="P91" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="Q91" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="R91" t="s">
         <v>24</v>
       </c>
       <c r="S91" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testing data for 2020-05-12
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -77,7 +77,7 @@
     <t xml:space="preserve">Argentina - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/09-05-20_reporte-matutino-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/12-05-20-reporte-matutino-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Argentina</t>
@@ -98,7 +98,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/05/coronavirus-covid-19-at-a-glance-9-may-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/05/coronavirus-covid-19-at-a-glance-12-may-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200510104642/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200512173912/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200509192849/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200512173915/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -193,7 +193,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-8-maya-vyzdoroveli-i-vypisany-5-tys-484-patsienta/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-vyzdoroveli-i-vypisany-6-tys-974-patsienta/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -225,7 +225,12 @@
     <t xml:space="preserve">The data is described both as the number of tests performed and as the number of tested patients.</t>
   </si>
   <si>
-    <t xml:space="preserve">There is some ambiguity as to the units. The testing data are labelled as 'the number of tests performed'. But in the [codebook](https://epistat.sciensano.be/COVID19BE_codebook.pdf) provided alongside the data the testing series is described as 'the number of tested patients'. The date of is the date of laboratory diagnosis, or when not available, the date of sampling is used.</t>
+    <t xml:space="preserve">Sciensano provides a daily time series of the number of tests conducted per day, which is updated retrospectively as new data becomes available each day.
+According to the [dataset codebook](https://epistat.sciensano.be/COVID19BE_codebook.pdf), dates for new testing figures correspond to the date of laboratory diagnosis (or when not available, date of sampling). 
+It appears that the reported testing figures represent the number of people tested, but this is not entirely clear. The official website describes the testing dataset as the "Dataset of total number of tests performed by date", yet the [dataset codebook](https://epistat.sciensano.be/COVID19BE_codebook.pdf) defines the "tests" variable as the "number of tested patients".
+It is also unclear whether the testing figures include antigen tests in addition to PCR tests. In a communication on April 3rd 2020, Sciensano indicates that antigen tests made by Coris Bioconcept may now be used for COVID-19 detection. The communication states that positive antigen test results do not have to be confirmed by a PCR test, but that negative or doubtful cases must be confirmed by a PCR test.
+Official figures reported in Sciensano's daily epidemiological bulletins do not help to clarify these ambiguities. For example, as of May 10th 2020, the [official time series dataset](https://epistat.sciensano.be/covid/covid19_historicaldata.html) reported a cumulative total of 465,201 tests performed between March 1st and May 9th. However, the epidemiological bulletin for [May 10th 2020](https://covid-19.sciensano.be/sites/default/files/Covid19/COVID-19_Daily%20report_20200510%20-%20FR.pdf) states that 325,796 cumulative tests had been performed by laboratories between the beginning of March and May 9th, while an additional 240,305 tests had been performed through the national testing platform (566,101 total tests).
+The bulletin indicates that these figures include both PCR and antigen tests, suggesting that the large discrepancy between the 465,201 figure and the 566,101 figure may be solely due to the fact that the official time series data only includes PCR tests, whereas the official bulletin figures include both PCR and antigen tests. However, it is also possible that the discrepancy is due solely to the fact that the official time series data is reported in terms of "people tested", whereas the bulletin figures represent "tests performed". We have been unable to find official documentation from Sciensano that resolves these ambiguities.</t>
   </si>
   <si>
     <t xml:space="preserve">BOL</t>
@@ -277,7 +282,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200510104647/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200512191641/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -300,7 +305,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200510104649/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200512191644/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -388,7 +393,7 @@
     <t xml:space="preserve">Croatia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200509164031/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200512191650/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -448,7 +453,7 @@
     <t xml:space="preserve">Denmark - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/COVID19-overvaagningsrapport-09052020-hu51</t>
+    <t xml:space="preserve">https://files.ssi.dk/COVID19-overvaagningsrapport-12052020-2-8ft5</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -475,7 +480,7 @@
     <t xml:space="preserve">Ecuador - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/05/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-08052020-08h0.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/05/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-04052020-08h00.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -504,7 +509,7 @@
     <t xml:space="preserve">Government of El Salvador</t>
   </si>
   <si>
-    <t xml:space="preserve">updated at 12:50pm local time on 2020-05-09.</t>
+    <t xml:space="preserve">updated at 11:38pm local time on 2020-05-11.</t>
   </si>
   <si>
     <t xml:space="preserve">The government of El Salvador publishes an online dashboard with figures and graphs about the epidemic, including the number of tests performed ("pruebas COVID19 realizadas hasta hoy"). No information is given on the geographical scope and number of labs included.</t>
@@ -541,7 +546,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_May-8_-ENG-V5.pdf</t>
+    <t xml:space="preserve">https://www.ephi.gov.et/images/confirmed-case-Press-release-May-12--ENG-V1.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -669,7 +674,7 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200509/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200512/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -804,7 +809,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200509000642/http://irangov.ir/detail/338857</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200512153002/http://irangov.ir/detail/339131</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -823,7 +828,7 @@
     <t xml:space="preserve">Ireland - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gov.ie/en/press-release/6f789f-statement-from-the-national-public-health-emergency-team-tuesday-5-m/</t>
+    <t xml:space="preserve">https://www.gov.ie/en/press-release/bc6c86-statement-from-the-national-public-health-emergency-team-tuesday-12-/</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gov.ie/en/publications/?&amp;type=press-releases&amp;organisation=department-of-health</t>
@@ -924,7 +929,7 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000628672.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000629555.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Implementation status of PCR tests for new coronavirus in Japan (based on the date on which the results were determined). Preliminary data</t>
@@ -958,7 +963,7 @@
     <t xml:space="preserve">Kenya - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1259109013435940866</t>
+    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1260187015213187073</t>
   </si>
   <si>
     <t xml:space="preserve">Kenya Ministry of Health</t>
@@ -999,7 +1004,7 @@
     <t xml:space="preserve">Lithuania - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200510104952/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200512191746/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -1015,7 +1020,7 @@
     <t xml:space="preserve">Luxembourg - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200509164113/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200512191747/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg Government situation update</t>
@@ -1036,7 +1041,7 @@
     <t xml:space="preserve">Malaysia - cases tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200510105003/https://www.moh.gov.my/index.php/pages/view/2019-ncov-wuhan</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200511162631/https://www.moh.gov.my/index.php/pages/view/2019-ncov-wuhan</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1091,7 +1096,8 @@
   <si>
     <t xml:space="preserve">The Morocco Ministry of Health provides daily updates of the total number of confirmed cases and the number of cases dismissed following a negative test result. We construct a time series of the cumulative number of cases tested to date using the data stored in [this unofficial GitHub repository](https://github.com/RedaElmar/COVID-19_Morocco). 
 The cumulative number of cases tested to date includes positive and negative test results, while excluding pending results. We have cross-checked a sample of the figures reported in the unofficial source against data reported on the Ministry of Health website.
-The earliest reported figure is from March 2nd 2020, at which point 29 cases had been tested. It is unclear whether March 2nd was the first date on which tests were conducted.</t>
+The earliest reported figure is from March 2nd 2020, at which point 29 cases had been tested. It is unclear whether March 2nd was the first date on which tests were conducted.
+Since 1 May 2020, the [government website dedicated to COVID-19](http://www.covidmaroc.ma/Pages/AccueilAR.aspx) has been down, making it impossible to update our time series.</t>
   </si>
   <si>
     <t xml:space="preserve">MMR</t>
@@ -1145,10 +1151,10 @@
     <t xml:space="preserve">Netherlands - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-05/COVID-19_WebSite_rapport_20200509_1018.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 9 May 2020 update</t>
+    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-05/COVID-19_WebSite_rapport_20200512_1143.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 12 May 2020 update</t>
   </si>
   <si>
     <t xml:space="preserve">Dutch National Institute for Public Health and the Environment</t>
@@ -1184,7 +1190,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200508200455/https://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200512191905/https://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1204,7 +1210,7 @@
     <t xml:space="preserve">Norway - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.05.08-dagsrapport-norge-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.05.12-dagsrapport-norge-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Norwegian Institute of Public Health</t>
@@ -1229,7 +1235,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200510105025/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200512191910/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1295,7 +1301,7 @@
     <t xml:space="preserve">Peru - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/151163-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-65-015-en-el-peru-comunicado-n-95</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/152809-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-72-059-en-el-peru-comunicado-n-98</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1336,7 +1342,7 @@
     <t xml:space="preserve">Poland - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://raw.githubusercontent.com/anuszka/COVID-19-MZ_GOV_PL/master/data/cor.2020.05.09.csv</t>
+    <t xml:space="preserve">https://raw.githubusercontent.com/anuszka/COVID-19-MZ_GOV_PL/master/data/cor.2020.05.12.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1381,7 +1387,7 @@
     <t xml:space="preserve">Qatar - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200510105040/https://www.moph.gov.qa/english/Pages/Coronavirus2019.aspx</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200512191924/https://www.moph.gov.qa/english/Pages/Coronavirus2019.aspx</t>
   </si>
   <si>
     <t xml:space="preserve">Qatar Ministry of Public Health</t>
@@ -1419,7 +1425,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14424</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14429</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1439,7 +1445,7 @@
     <t xml:space="preserve">Rwanda - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1259173285348204546</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1259905287420608513</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1546,7 +1552,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200510105056/https://korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200512191932/https://korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Center of Health Information and the Office of the Government of the Slovak Republic</t>
@@ -1620,7 +1626,7 @@
     <t xml:space="preserve">South Korea - cases tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367186&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367200&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1706,7 +1712,7 @@
     <t xml:space="preserve">Taiwan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/EKvIxtZ0OwCUzeHXum1VBA?typeid=9</t>
+    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/jTbxMFGoCtXzAWcjhfQtaA?typeid=9</t>
   </si>
   <si>
     <t xml:space="preserve">Taiwan Centers for Disease Control (CDC)</t>
@@ -1729,7 +1735,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200510105142/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200511162830/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1776,7 +1782,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200509164243/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200512192345/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1800,13 +1806,13 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1259006502502834181</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1259934362721804290</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
   </si>
   <si>
-    <t xml:space="preserve">We sum the cumulative total provided for the previous day with the daily number of samples tested today.</t>
+    <t xml:space="preserve">We sum the cumulative total provided for the previous day with the daily number of samples tested today. Samples tested today at the Uganda Virus Research Institute. (UVRI)</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.health.go.ug/moh/resources/</t>
@@ -1823,7 +1829,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200510105147/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200512192348/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1845,7 +1851,7 @@
     <t xml:space="preserve">United Kingdom - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200509164248/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200512192350/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
@@ -1868,7 +1874,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200509164249/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200512192351/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
   </si>
   <si>
     <t xml:space="preserve">The number of tests performed, including tests posted or delivered but not yet returned and/or processed.</t>
@@ -1942,7 +1948,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-20</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-22</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -1981,7 +1987,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1258995561090502657</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1260066306474356741</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -2397,7 +2403,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -2407,31 +2413,31 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H2" t="n">
-        <v>80729</v>
+        <v>87547</v>
       </c>
       <c r="I2" t="n">
-        <v>1.786</v>
+        <v>1.937</v>
       </c>
       <c r="J2" t="n">
-        <v>2828</v>
+        <v>2389</v>
       </c>
       <c r="K2" t="n">
-        <v>0.063</v>
+        <v>0.053</v>
       </c>
       <c r="L2" t="n">
-        <v>2804.667</v>
+        <v>2272.667</v>
       </c>
       <c r="M2" t="n">
-        <v>0.062</v>
+        <v>0.05</v>
       </c>
       <c r="N2" t="n">
-        <v>2409</v>
+        <v>2547</v>
       </c>
       <c r="O2" t="n">
-        <v>0.053</v>
+        <v>0.056</v>
       </c>
       <c r="P2" t="s">
         <v>22</v>
@@ -2454,7 +2460,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
@@ -2464,31 +2470,31 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H3" t="n">
-        <v>795456</v>
+        <v>877927</v>
       </c>
       <c r="I3" t="n">
-        <v>31.194</v>
+        <v>34.429</v>
       </c>
       <c r="J3" t="n">
-        <v>38206</v>
+        <v>22808</v>
       </c>
       <c r="K3" t="n">
-        <v>1.498</v>
+        <v>0.894</v>
       </c>
       <c r="L3" t="n">
-        <v>35600</v>
+        <v>27490.333</v>
       </c>
       <c r="M3" t="n">
-        <v>1.396</v>
+        <v>1.078</v>
       </c>
       <c r="N3" t="n">
-        <v>26267.571</v>
+        <v>30453</v>
       </c>
       <c r="O3" t="n">
-        <v>1.03</v>
+        <v>1.194</v>
       </c>
       <c r="P3" t="s">
         <v>29</v>
@@ -2511,7 +2517,7 @@
         <v>33</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>43961</v>
+        <v>43963</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
@@ -2521,31 +2527,31 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H4" t="n">
-        <v>316508</v>
+        <v>329314</v>
       </c>
       <c r="I4" t="n">
-        <v>35.143</v>
+        <v>36.564</v>
       </c>
       <c r="J4" t="n">
-        <v>4818</v>
+        <v>9830</v>
       </c>
       <c r="K4" t="n">
-        <v>0.535</v>
+        <v>1.091</v>
       </c>
       <c r="L4" t="n">
-        <v>6204.667</v>
+        <v>5874.667</v>
       </c>
       <c r="M4" t="n">
+        <v>0.652</v>
+      </c>
+      <c r="N4" t="n">
+        <v>6204.429</v>
+      </c>
+      <c r="O4" t="n">
         <v>0.689</v>
-      </c>
-      <c r="N4" t="n">
-        <v>6021.857</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.669</v>
       </c>
       <c r="P4" t="s">
         <v>36</v>
@@ -2568,7 +2574,7 @@
         <v>41</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D5" t="s">
         <v>42</v>
@@ -2578,31 +2584,31 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H5" t="n">
-        <v>178353</v>
+        <v>197898</v>
       </c>
       <c r="I5" t="n">
-        <v>104.816</v>
+        <v>116.302</v>
       </c>
       <c r="J5" t="n">
-        <v>6195</v>
+        <v>7118</v>
       </c>
       <c r="K5" t="n">
-        <v>3.641</v>
+        <v>4.183</v>
       </c>
       <c r="L5" t="n">
-        <v>6004</v>
+        <v>6515</v>
       </c>
       <c r="M5" t="n">
-        <v>3.529</v>
+        <v>3.829</v>
       </c>
       <c r="N5" t="n">
-        <v>5725</v>
+        <v>6056.714</v>
       </c>
       <c r="O5" t="n">
-        <v>3.365</v>
+        <v>3.559</v>
       </c>
       <c r="P5" t="s">
         <v>44</v>
@@ -2625,7 +2631,7 @@
         <v>49</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D6" t="s">
         <v>50</v>
@@ -2635,31 +2641,31 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H6" t="n">
-        <v>116919</v>
+        <v>136638</v>
       </c>
       <c r="I6" t="n">
-        <v>0.71</v>
+        <v>0.83</v>
       </c>
       <c r="J6" t="n">
-        <v>5465</v>
+        <v>6773</v>
       </c>
       <c r="K6" t="n">
-        <v>0.033</v>
+        <v>0.041</v>
       </c>
       <c r="L6" t="n">
-        <v>5758.333</v>
+        <v>6573</v>
       </c>
       <c r="M6" t="n">
-        <v>0.035</v>
+        <v>0.04</v>
       </c>
       <c r="N6" t="n">
-        <v>5836.143</v>
+        <v>6176.429</v>
       </c>
       <c r="O6" t="n">
-        <v>0.036</v>
+        <v>0.038</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
@@ -2682,7 +2688,7 @@
         <v>56</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>43959</v>
+        <v>43963</v>
       </c>
       <c r="D7" t="s">
         <v>57</v>
@@ -2692,22 +2698,26 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H7" t="n">
-        <v>240146</v>
+        <v>284445</v>
       </c>
       <c r="I7" t="n">
-        <v>25.414</v>
+        <v>30.102</v>
       </c>
       <c r="J7" t="n">
-        <v>10680</v>
+        <v>10385</v>
       </c>
       <c r="K7" t="n">
-        <v>1.13</v>
-      </c>
-      <c r="L7"/>
-      <c r="M7"/>
+        <v>1.099</v>
+      </c>
+      <c r="L7" t="n">
+        <v>10891.333</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1.153</v>
+      </c>
       <c r="N7"/>
       <c r="O7"/>
       <c r="P7" t="s">
@@ -2731,7 +2741,7 @@
         <v>62</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>43959</v>
+        <v>43961</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
@@ -2741,31 +2751,31 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H8" t="n">
-        <v>461303</v>
+        <v>487863</v>
       </c>
       <c r="I8" t="n">
-        <v>39.803</v>
+        <v>42.095</v>
       </c>
       <c r="J8" t="n">
-        <v>21311</v>
+        <v>10044</v>
       </c>
       <c r="K8" t="n">
-        <v>1.839</v>
+        <v>0.867</v>
       </c>
       <c r="L8" t="n">
-        <v>18816.667</v>
+        <v>16559.667</v>
       </c>
       <c r="M8" t="n">
-        <v>1.624</v>
+        <v>1.429</v>
       </c>
       <c r="N8" t="n">
-        <v>17504.143</v>
+        <v>17648.143</v>
       </c>
       <c r="O8" t="n">
-        <v>1.51</v>
+        <v>1.523</v>
       </c>
       <c r="P8" t="s">
         <v>64</v>
@@ -2788,7 +2798,7 @@
         <v>69</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>43960</v>
+        <v>43962</v>
       </c>
       <c r="D9" t="s">
         <v>70</v>
@@ -2800,31 +2810,31 @@
         <v>71</v>
       </c>
       <c r="G9" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H9" t="n">
-        <v>8523</v>
+        <v>8917</v>
       </c>
       <c r="I9" t="n">
-        <v>0.73</v>
+        <v>0.764</v>
       </c>
       <c r="J9" t="n">
-        <v>171</v>
+        <v>275</v>
       </c>
       <c r="K9" t="n">
-        <v>0.015</v>
+        <v>0.024</v>
       </c>
       <c r="L9" t="n">
-        <v>183.667</v>
+        <v>188.333</v>
       </c>
       <c r="M9" t="n">
         <v>0.016</v>
       </c>
       <c r="N9" t="n">
-        <v>138.143</v>
+        <v>164.286</v>
       </c>
       <c r="O9" t="n">
-        <v>0.012</v>
+        <v>0.014</v>
       </c>
       <c r="P9" t="s">
         <v>43</v>
@@ -2892,7 +2902,7 @@
         <v>83</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>43961</v>
+        <v>43963</v>
       </c>
       <c r="D11" t="s">
         <v>84</v>
@@ -2902,31 +2912,31 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H11" t="n">
-        <v>57231</v>
+        <v>58713</v>
       </c>
       <c r="I11" t="n">
-        <v>8.237</v>
+        <v>8.45</v>
       </c>
       <c r="J11" t="n">
-        <v>1126</v>
+        <v>1079</v>
       </c>
       <c r="K11" t="n">
-        <v>0.162</v>
+        <v>0.155</v>
       </c>
       <c r="L11" t="n">
-        <v>1433.333</v>
+        <v>869.333</v>
       </c>
       <c r="M11" t="n">
-        <v>0.206</v>
+        <v>0.125</v>
       </c>
       <c r="N11" t="n">
-        <v>1230.429</v>
+        <v>1201.429</v>
       </c>
       <c r="O11" t="n">
-        <v>0.177</v>
+        <v>0.173</v>
       </c>
       <c r="P11" t="s">
         <v>86</v>
@@ -2949,7 +2959,7 @@
         <v>90</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>43961</v>
+        <v>43963</v>
       </c>
       <c r="D12" t="s">
         <v>91</v>
@@ -2959,25 +2969,31 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H12" t="n">
-        <v>1071379</v>
+        <v>1145683</v>
       </c>
       <c r="I12" t="n">
-        <v>28.387</v>
-      </c>
-      <c r="J12"/>
+        <v>30.356</v>
+      </c>
+      <c r="J12" t="n">
+        <v>26733</v>
+      </c>
       <c r="K12" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="L12"/>
+        <v>0.708</v>
+      </c>
+      <c r="L12" t="n">
+        <v>26029.333</v>
+      </c>
       <c r="M12" t="n">
-        <v>0.614</v>
-      </c>
-      <c r="N12"/>
+        <v>0.69</v>
+      </c>
+      <c r="N12" t="n">
+        <v>29302.286</v>
+      </c>
       <c r="O12" t="n">
-        <v>0.673</v>
+        <v>0.776</v>
       </c>
       <c r="P12" t="s">
         <v>92</v>
@@ -3000,7 +3016,7 @@
         <v>97</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D13" t="s">
         <v>98</v>
@@ -3012,31 +3028,31 @@
         <v>99</v>
       </c>
       <c r="G13" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H13" t="n">
-        <v>267904</v>
+        <v>303340</v>
       </c>
       <c r="I13" t="n">
-        <v>14.014</v>
+        <v>15.868</v>
       </c>
       <c r="J13" t="n">
-        <v>11943</v>
+        <v>9283</v>
       </c>
       <c r="K13" t="n">
-        <v>0.625</v>
+        <v>0.486</v>
       </c>
       <c r="L13" t="n">
-        <v>11932</v>
+        <v>11812</v>
       </c>
       <c r="M13" t="n">
-        <v>0.624</v>
+        <v>0.618</v>
       </c>
       <c r="N13" t="n">
-        <v>9786.286</v>
+        <v>11606.429</v>
       </c>
       <c r="O13" t="n">
-        <v>0.512</v>
+        <v>0.607</v>
       </c>
       <c r="P13" t="s">
         <v>100</v>
@@ -3059,7 +3075,7 @@
         <v>104</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>43960</v>
+        <v>43962</v>
       </c>
       <c r="D14" t="s">
         <v>105</v>
@@ -3069,31 +3085,31 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H14" t="n">
-        <v>144912</v>
+        <v>158933</v>
       </c>
       <c r="I14" t="n">
-        <v>2.848</v>
+        <v>3.124</v>
       </c>
       <c r="J14" t="n">
-        <v>5173</v>
+        <v>7537</v>
       </c>
       <c r="K14" t="n">
-        <v>0.102</v>
+        <v>0.148</v>
       </c>
       <c r="L14" t="n">
-        <v>4600.667</v>
+        <v>6398</v>
       </c>
       <c r="M14" t="n">
-        <v>0.09</v>
+        <v>0.126</v>
       </c>
       <c r="N14" t="n">
-        <v>4330</v>
+        <v>5129.143</v>
       </c>
       <c r="O14" t="n">
-        <v>0.085</v>
+        <v>0.101</v>
       </c>
       <c r="P14" t="s">
         <v>106</v>
@@ -3116,7 +3132,7 @@
         <v>111</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D15" t="s">
         <v>112</v>
@@ -3126,31 +3142,31 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H15" t="n">
-        <v>11276</v>
+        <v>12061</v>
       </c>
       <c r="I15" t="n">
-        <v>2.214</v>
+        <v>2.368</v>
       </c>
       <c r="J15" t="n">
-        <v>449</v>
+        <v>73</v>
       </c>
       <c r="K15" t="n">
-        <v>0.088</v>
+        <v>0.014</v>
       </c>
       <c r="L15" t="n">
-        <v>391.667</v>
+        <v>261.667</v>
       </c>
       <c r="M15" t="n">
-        <v>0.077</v>
+        <v>0.051</v>
       </c>
       <c r="N15" t="n">
-        <v>240.429</v>
+        <v>309.857</v>
       </c>
       <c r="O15" t="n">
-        <v>0.047</v>
+        <v>0.061</v>
       </c>
       <c r="P15" t="s">
         <v>113</v>
@@ -3173,7 +3189,7 @@
         <v>117</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D16" t="s">
         <v>118</v>
@@ -3183,31 +3199,31 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H16" t="n">
-        <v>44218</v>
+        <v>47480</v>
       </c>
       <c r="I16" t="n">
-        <v>10.771</v>
+        <v>11.566</v>
       </c>
       <c r="J16" t="n">
-        <v>840</v>
+        <v>1409</v>
       </c>
       <c r="K16" t="n">
-        <v>0.205</v>
+        <v>0.343</v>
       </c>
       <c r="L16" t="n">
-        <v>1055</v>
+        <v>1087.333</v>
       </c>
       <c r="M16" t="n">
-        <v>0.257</v>
+        <v>0.265</v>
       </c>
       <c r="N16" t="n">
-        <v>951.571</v>
+        <v>1072.429</v>
       </c>
       <c r="O16" t="n">
-        <v>0.232</v>
+        <v>0.261</v>
       </c>
       <c r="P16" t="s">
         <v>119</v>
@@ -3230,7 +3246,7 @@
         <v>124</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>43959</v>
+        <v>43962</v>
       </c>
       <c r="D17" t="s">
         <v>125</v>
@@ -3242,31 +3258,31 @@
         <v>127</v>
       </c>
       <c r="G17" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H17" t="n">
-        <v>65509</v>
+        <v>71157</v>
       </c>
       <c r="I17" t="n">
-        <v>5.784</v>
+        <v>6.282</v>
       </c>
       <c r="J17" t="n">
-        <v>1949</v>
+        <v>1975</v>
       </c>
       <c r="K17" t="n">
-        <v>0.172</v>
+        <v>0.174</v>
       </c>
       <c r="L17" t="n">
-        <v>1953.667</v>
+        <v>1882.667</v>
       </c>
       <c r="M17" t="n">
-        <v>0.172</v>
+        <v>0.166</v>
       </c>
       <c r="N17" t="n">
-        <v>2000.429</v>
+        <v>1920.857</v>
       </c>
       <c r="O17" t="n">
-        <v>0.176</v>
+        <v>0.169</v>
       </c>
       <c r="P17" t="s">
         <v>126</v>
@@ -3289,7 +3305,7 @@
         <v>131</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>43960</v>
+        <v>43962</v>
       </c>
       <c r="D18" t="s">
         <v>132</v>
@@ -3299,31 +3315,31 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H18" t="n">
-        <v>302493</v>
+        <v>314138</v>
       </c>
       <c r="I18" t="n">
-        <v>28.247</v>
+        <v>29.334</v>
       </c>
       <c r="J18" t="n">
-        <v>3717</v>
+        <v>7537</v>
       </c>
       <c r="K18" t="n">
-        <v>0.347</v>
+        <v>0.704</v>
       </c>
       <c r="L18" t="n">
-        <v>5193.333</v>
+        <v>5120.667</v>
       </c>
       <c r="M18" t="n">
-        <v>0.485</v>
+        <v>0.478</v>
       </c>
       <c r="N18" t="n">
-        <v>6373.143</v>
+        <v>6433.571</v>
       </c>
       <c r="O18" t="n">
-        <v>0.595</v>
+        <v>0.601</v>
       </c>
       <c r="P18" t="s">
         <v>43</v>
@@ -3346,7 +3362,7 @@
         <v>136</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D19" t="s">
         <v>137</v>
@@ -3358,31 +3374,31 @@
         <v>139</v>
       </c>
       <c r="G19" t="n">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H19" t="n">
-        <v>308984</v>
+        <v>334260</v>
       </c>
       <c r="I19" t="n">
-        <v>53.345</v>
+        <v>57.709</v>
       </c>
       <c r="J19" t="n">
-        <v>10496</v>
+        <v>7700</v>
       </c>
       <c r="K19" t="n">
-        <v>1.812</v>
+        <v>1.329</v>
       </c>
       <c r="L19" t="n">
-        <v>12768</v>
+        <v>8425.333</v>
       </c>
       <c r="M19" t="n">
-        <v>2.204</v>
+        <v>1.455</v>
       </c>
       <c r="N19" t="n">
-        <v>12438.857</v>
+        <v>10931.714</v>
       </c>
       <c r="O19" t="n">
-        <v>2.147</v>
+        <v>1.887</v>
       </c>
       <c r="P19" t="s">
         <v>140</v>
@@ -3405,7 +3421,7 @@
         <v>144</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>43959</v>
+        <v>43955</v>
       </c>
       <c r="D20" t="s">
         <v>145</v>
@@ -3417,22 +3433,32 @@
         <v>147</v>
       </c>
       <c r="G20" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H20" t="n">
-        <v>40630</v>
+        <v>46260</v>
       </c>
       <c r="I20" t="n">
-        <v>2.303</v>
-      </c>
-      <c r="J20"/>
+        <v>2.622</v>
+      </c>
+      <c r="J20" t="n">
+        <v>2533</v>
+      </c>
       <c r="K20" t="n">
-        <v>-0.212</v>
-      </c>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="N20"/>
-      <c r="O20"/>
+        <v>0.144</v>
+      </c>
+      <c r="L20" t="n">
+        <v>3066.333</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.174</v>
+      </c>
+      <c r="N20" t="n">
+        <v>2160.857</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.123</v>
+      </c>
       <c r="P20" t="s">
         <v>146</v>
       </c>
@@ -3454,7 +3480,7 @@
         <v>151</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>43960</v>
+        <v>43962</v>
       </c>
       <c r="D21" t="s">
         <v>152</v>
@@ -3466,22 +3492,22 @@
         <v>154</v>
       </c>
       <c r="G21" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H21" t="n">
-        <v>39079</v>
+        <v>44926</v>
       </c>
       <c r="I21" t="n">
-        <v>6.025</v>
-      </c>
-      <c r="J21" t="n">
-        <v>1773</v>
-      </c>
+        <v>6.926</v>
+      </c>
+      <c r="J21"/>
       <c r="K21" t="n">
-        <v>0.273</v>
+        <v>0.29</v>
       </c>
       <c r="L21"/>
-      <c r="M21"/>
+      <c r="M21" t="n">
+        <v>0.391</v>
+      </c>
       <c r="N21"/>
       <c r="O21"/>
       <c r="P21" t="s">
@@ -3505,7 +3531,7 @@
         <v>157</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>43960</v>
+        <v>43962</v>
       </c>
       <c r="D22" t="s">
         <v>158</v>
@@ -3515,31 +3541,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H22" t="n">
-        <v>63372</v>
+        <v>64975</v>
       </c>
       <c r="I22" t="n">
-        <v>47.772</v>
+        <v>48.981</v>
       </c>
       <c r="J22" t="n">
-        <v>654</v>
+        <v>1018</v>
       </c>
       <c r="K22" t="n">
-        <v>0.493</v>
+        <v>0.767</v>
       </c>
       <c r="L22" t="n">
-        <v>961.333</v>
+        <v>753</v>
       </c>
       <c r="M22" t="n">
-        <v>0.725</v>
+        <v>0.567</v>
       </c>
       <c r="N22" t="n">
-        <v>1170.714</v>
+        <v>1081.714</v>
       </c>
       <c r="O22" t="n">
-        <v>0.882</v>
+        <v>0.815</v>
       </c>
       <c r="P22" t="s">
         <v>160</v>
@@ -3562,7 +3588,7 @@
         <v>165</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>43959</v>
+        <v>43963</v>
       </c>
       <c r="D23" t="s">
         <v>166</v>
@@ -3572,19 +3598,19 @@
       </c>
       <c r="F23"/>
       <c r="G23" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H23" t="n">
-        <v>30306</v>
+        <v>39048</v>
       </c>
       <c r="I23" t="n">
-        <v>0.264</v>
+        <v>0.34</v>
       </c>
       <c r="J23" t="n">
-        <v>1946</v>
+        <v>2424</v>
       </c>
       <c r="K23" t="n">
-        <v>0.017</v>
+        <v>0.021</v>
       </c>
       <c r="L23"/>
       <c r="M23"/>
@@ -3611,7 +3637,7 @@
         <v>171</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>43959</v>
+        <v>43962</v>
       </c>
       <c r="D24" t="s">
         <v>172</v>
@@ -3621,25 +3647,25 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H24" t="n">
-        <v>119054</v>
+        <v>126327</v>
       </c>
       <c r="I24" t="n">
-        <v>21.487</v>
+        <v>22.8</v>
       </c>
       <c r="J24"/>
       <c r="K24" t="n">
-        <v>0.116</v>
+        <v>0.069</v>
       </c>
       <c r="L24"/>
       <c r="M24" t="n">
-        <v>0.433</v>
+        <v>0.243</v>
       </c>
       <c r="N24"/>
       <c r="O24" t="n">
-        <v>0.388</v>
+        <v>0.432</v>
       </c>
       <c r="P24" t="s">
         <v>174</v>
@@ -3756,7 +3782,7 @@
         <v>192</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>43958</v>
+        <v>43962</v>
       </c>
       <c r="D27" t="s">
         <v>193</v>
@@ -3766,16 +3792,20 @@
       </c>
       <c r="F27"/>
       <c r="G27" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H27" t="n">
-        <v>149948</v>
+        <v>162184</v>
       </c>
       <c r="I27" t="n">
-        <v>4.826</v>
-      </c>
-      <c r="J27"/>
-      <c r="K27"/>
+        <v>5.219</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1683</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.054</v>
+      </c>
       <c r="L27"/>
       <c r="M27"/>
       <c r="N27"/>
@@ -3801,7 +3831,7 @@
         <v>200</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D28" t="s">
         <v>201</v>
@@ -3811,25 +3841,25 @@
       </c>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H28" t="n">
-        <v>97384</v>
+        <v>106054</v>
       </c>
       <c r="I28" t="n">
-        <v>9.343</v>
+        <v>10.175</v>
       </c>
       <c r="J28" t="n">
-        <v>3093</v>
+        <v>6691</v>
       </c>
       <c r="K28" t="n">
-        <v>0.297</v>
+        <v>0.642</v>
       </c>
       <c r="L28" t="n">
-        <v>3444</v>
+        <v>2890</v>
       </c>
       <c r="M28" t="n">
-        <v>0.331</v>
+        <v>0.277</v>
       </c>
       <c r="N28"/>
       <c r="O28"/>
@@ -3899,7 +3929,7 @@
         <v>214</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>43961</v>
+        <v>43963</v>
       </c>
       <c r="D30" t="s">
         <v>215</v>
@@ -3911,31 +3941,31 @@
         <v>217</v>
       </c>
       <c r="G30" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H30" t="n">
-        <v>108257</v>
+        <v>114719</v>
       </c>
       <c r="I30" t="n">
-        <v>11.206</v>
+        <v>11.875</v>
       </c>
       <c r="J30" t="n">
-        <v>4999</v>
+        <v>2554</v>
       </c>
       <c r="K30" t="n">
-        <v>0.517</v>
+        <v>0.264</v>
       </c>
       <c r="L30" t="n">
-        <v>4740.333</v>
+        <v>3820.333</v>
       </c>
       <c r="M30" t="n">
-        <v>0.491</v>
+        <v>0.395</v>
       </c>
       <c r="N30" t="n">
-        <v>3749.571</v>
+        <v>4166</v>
       </c>
       <c r="O30" t="n">
-        <v>0.388</v>
+        <v>0.431</v>
       </c>
       <c r="P30" t="s">
         <v>216</v>
@@ -3958,7 +3988,7 @@
         <v>222</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>43959</v>
+        <v>43962</v>
       </c>
       <c r="D31" t="s">
         <v>223</v>
@@ -3968,31 +3998,31 @@
       </c>
       <c r="F31"/>
       <c r="G31" t="n">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H31" t="n">
-        <v>53219</v>
+        <v>54750</v>
       </c>
       <c r="I31" t="n">
-        <v>155.953</v>
+        <v>160.44</v>
       </c>
       <c r="J31" t="n">
-        <v>515</v>
+        <v>578</v>
       </c>
       <c r="K31" t="n">
-        <v>1.509</v>
+        <v>1.694</v>
       </c>
       <c r="L31" t="n">
-        <v>532.333</v>
+        <v>510.333</v>
       </c>
       <c r="M31" t="n">
-        <v>1.56</v>
+        <v>1.496</v>
       </c>
       <c r="N31" t="n">
-        <v>465.429</v>
+        <v>492.286</v>
       </c>
       <c r="O31" t="n">
-        <v>1.364</v>
+        <v>1.443</v>
       </c>
       <c r="P31" t="s">
         <v>224</v>
@@ -4066,7 +4096,7 @@
         <v>233</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>43961</v>
+        <v>43963</v>
       </c>
       <c r="D33" t="s">
         <v>229</v>
@@ -4078,31 +4108,31 @@
         <v>231</v>
       </c>
       <c r="G33" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H33" t="n">
-        <v>1609037</v>
+        <v>1759579</v>
       </c>
       <c r="I33" t="n">
-        <v>1.166</v>
+        <v>1.275</v>
       </c>
       <c r="J33" t="n">
-        <v>85824</v>
+        <v>85891</v>
       </c>
       <c r="K33" t="n">
         <v>0.062</v>
       </c>
       <c r="L33" t="n">
-        <v>83874.667</v>
+        <v>78788.667</v>
       </c>
       <c r="M33" t="n">
-        <v>0.061</v>
+        <v>0.057</v>
       </c>
       <c r="N33" t="n">
-        <v>80369.571</v>
+        <v>81090.429</v>
       </c>
       <c r="O33" t="n">
-        <v>0.058</v>
+        <v>0.059</v>
       </c>
       <c r="P33" t="s">
         <v>230</v>
@@ -4125,7 +4155,7 @@
         <v>235</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>43961</v>
+        <v>43963</v>
       </c>
       <c r="D34" t="s">
         <v>236</v>
@@ -4135,28 +4165,28 @@
       </c>
       <c r="F34"/>
       <c r="G34" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H34" t="n">
-        <v>113452</v>
+        <v>119728</v>
       </c>
       <c r="I34" t="n">
-        <v>0.415</v>
+        <v>0.438</v>
       </c>
       <c r="J34" t="n">
-        <v>4753</v>
+        <v>3370</v>
       </c>
       <c r="K34" t="n">
-        <v>0.017</v>
+        <v>0.012</v>
       </c>
       <c r="L34" t="n">
-        <v>5578.333</v>
+        <v>3676.333</v>
       </c>
       <c r="M34" t="n">
-        <v>0.02</v>
+        <v>0.013</v>
       </c>
       <c r="N34" t="n">
-        <v>4348.571</v>
+        <v>4400.571</v>
       </c>
       <c r="O34" t="n">
         <v>0.016</v>
@@ -4182,7 +4212,7 @@
         <v>241</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>43959</v>
+        <v>43963</v>
       </c>
       <c r="D35" t="s">
         <v>242</v>
@@ -4192,32 +4222,20 @@
       </c>
       <c r="F35"/>
       <c r="G35" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H35" t="n">
-        <v>558899</v>
+        <v>615477</v>
       </c>
       <c r="I35" t="n">
-        <v>6.654</v>
-      </c>
-      <c r="J35" t="n">
-        <v>14107</v>
-      </c>
-      <c r="K35" t="n">
-        <v>0.168</v>
-      </c>
-      <c r="L35" t="n">
-        <v>13118.667</v>
-      </c>
-      <c r="M35" t="n">
-        <v>0.156</v>
-      </c>
-      <c r="N35" t="n">
-        <v>11982.286</v>
-      </c>
-      <c r="O35" t="n">
-        <v>0.143</v>
-      </c>
+        <v>7.328</v>
+      </c>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
       <c r="P35" t="s">
         <v>243</v>
       </c>
@@ -4239,7 +4257,7 @@
         <v>247</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>43956</v>
+        <v>43963</v>
       </c>
       <c r="D36" t="s">
         <v>248</v>
@@ -4249,13 +4267,13 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H36" t="n">
-        <v>214761</v>
+        <v>258808</v>
       </c>
       <c r="I36" t="n">
-        <v>43.493</v>
+        <v>52.414</v>
       </c>
       <c r="J36"/>
       <c r="K36"/>
@@ -4284,7 +4302,7 @@
         <v>253</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>43958</v>
+        <v>43962</v>
       </c>
       <c r="D37" t="s">
         <v>254</v>
@@ -4296,31 +4314,31 @@
         <v>256</v>
       </c>
       <c r="G37" t="n">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H37" t="n">
-        <v>435790</v>
+        <v>462580</v>
       </c>
       <c r="I37" t="n">
-        <v>50.348</v>
+        <v>53.443</v>
       </c>
       <c r="J37" t="n">
-        <v>8876</v>
+        <v>8291</v>
       </c>
       <c r="K37" t="n">
-        <v>1.025</v>
+        <v>0.958</v>
       </c>
       <c r="L37" t="n">
-        <v>9003.333</v>
+        <v>5704</v>
       </c>
       <c r="M37" t="n">
-        <v>1.04</v>
+        <v>0.659</v>
       </c>
       <c r="N37" t="n">
-        <v>8844</v>
+        <v>7685.714</v>
       </c>
       <c r="O37" t="n">
-        <v>1.022</v>
+        <v>0.888</v>
       </c>
       <c r="P37" t="s">
         <v>43</v>
@@ -4343,7 +4361,7 @@
         <v>260</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D38" t="s">
         <v>261</v>
@@ -4355,31 +4373,31 @@
         <v>263</v>
       </c>
       <c r="G38" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H38" t="n">
-        <v>1645076</v>
+        <v>1741903</v>
       </c>
       <c r="I38" t="n">
-        <v>27.209</v>
+        <v>28.81</v>
       </c>
       <c r="J38" t="n">
-        <v>36091</v>
+        <v>39620</v>
       </c>
       <c r="K38" t="n">
-        <v>0.597</v>
+        <v>0.655</v>
       </c>
       <c r="L38" t="n">
-        <v>31728</v>
+        <v>32275.667</v>
       </c>
       <c r="M38" t="n">
-        <v>0.525</v>
+        <v>0.534</v>
       </c>
       <c r="N38" t="n">
-        <v>30744.571</v>
+        <v>32826</v>
       </c>
       <c r="O38" t="n">
-        <v>0.508</v>
+        <v>0.543</v>
       </c>
       <c r="P38" t="s">
         <v>264</v>
@@ -4402,7 +4420,7 @@
         <v>267</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D39" t="s">
         <v>261</v>
@@ -4414,31 +4432,31 @@
         <v>263</v>
       </c>
       <c r="G39" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H39" t="n">
-        <v>2514234</v>
+        <v>2673655</v>
       </c>
       <c r="I39" t="n">
-        <v>41.584</v>
+        <v>44.221</v>
       </c>
       <c r="J39" t="n">
-        <v>69171</v>
+        <v>67003</v>
       </c>
       <c r="K39" t="n">
-        <v>1.144</v>
+        <v>1.108</v>
       </c>
       <c r="L39" t="n">
-        <v>67768.333</v>
+        <v>53140.333</v>
       </c>
       <c r="M39" t="n">
-        <v>1.121</v>
+        <v>0.879</v>
       </c>
       <c r="N39" t="n">
-        <v>57913.857</v>
+        <v>60998.429</v>
       </c>
       <c r="O39" t="n">
-        <v>0.958</v>
+        <v>1.009</v>
       </c>
       <c r="P39" t="s">
         <v>264</v>
@@ -4461,7 +4479,7 @@
         <v>270</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D40" t="s">
         <v>271</v>
@@ -4473,13 +4491,13 @@
         <v>273</v>
       </c>
       <c r="G40" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H40" t="n">
-        <v>211997</v>
+        <v>223649</v>
       </c>
       <c r="I40" t="n">
-        <v>1.676</v>
+        <v>1.768</v>
       </c>
       <c r="J40"/>
       <c r="K40"/>
@@ -4508,7 +4526,7 @@
         <v>276</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>43958</v>
+        <v>43961</v>
       </c>
       <c r="D41" t="s">
         <v>277</v>
@@ -4520,31 +4538,25 @@
         <v>278</v>
       </c>
       <c r="G41" t="n">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H41" t="n">
-        <v>312728</v>
+        <v>333910</v>
       </c>
       <c r="I41" t="n">
-        <v>2.473</v>
-      </c>
-      <c r="J41" t="n">
-        <v>6061</v>
-      </c>
+        <v>2.64</v>
+      </c>
+      <c r="J41"/>
       <c r="K41" t="n">
-        <v>0.048</v>
-      </c>
-      <c r="L41" t="n">
-        <v>4768.667</v>
-      </c>
+        <v>0.026</v>
+      </c>
+      <c r="L41"/>
       <c r="M41" t="n">
-        <v>0.038</v>
-      </c>
-      <c r="N41" t="n">
-        <v>5210.143</v>
-      </c>
+        <v>0.049</v>
+      </c>
+      <c r="N41"/>
       <c r="O41" t="n">
-        <v>0.041</v>
+        <v>0.044</v>
       </c>
       <c r="P41" t="s">
         <v>272</v>
@@ -4567,7 +4579,7 @@
         <v>281</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D42" t="s">
         <v>282</v>
@@ -4577,31 +4589,31 @@
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H42" t="n">
-        <v>385104</v>
+        <v>422011</v>
       </c>
       <c r="I42" t="n">
-        <v>20.51</v>
+        <v>22.475</v>
       </c>
       <c r="J42" t="n">
-        <v>13978</v>
+        <v>13298</v>
       </c>
       <c r="K42" t="n">
-        <v>0.744</v>
+        <v>0.708</v>
       </c>
       <c r="L42" t="n">
-        <v>16208</v>
+        <v>12302.333</v>
       </c>
       <c r="M42" t="n">
-        <v>0.863</v>
+        <v>0.655</v>
       </c>
       <c r="N42" t="n">
-        <v>14606</v>
+        <v>14514.286</v>
       </c>
       <c r="O42" t="n">
-        <v>0.778</v>
+        <v>0.773</v>
       </c>
       <c r="P42" t="s">
         <v>283</v>
@@ -4624,7 +4636,7 @@
         <v>286</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D43" t="s">
         <v>287</v>
@@ -4634,22 +4646,26 @@
       </c>
       <c r="F43"/>
       <c r="G43" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H43" t="n">
-        <v>31041</v>
+        <v>33916</v>
       </c>
       <c r="I43" t="n">
-        <v>0.577</v>
+        <v>0.631</v>
       </c>
       <c r="J43" t="n">
-        <v>1611</v>
+        <v>978</v>
       </c>
       <c r="K43" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="L43"/>
-      <c r="M43"/>
+        <v>0.018</v>
+      </c>
+      <c r="L43" t="n">
+        <v>958.333</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0.018</v>
+      </c>
       <c r="N43"/>
       <c r="O43"/>
       <c r="P43" t="s">
@@ -4673,7 +4689,7 @@
         <v>293</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>43961</v>
+        <v>43963</v>
       </c>
       <c r="D44" t="s">
         <v>294</v>
@@ -4685,25 +4701,31 @@
         <v>296</v>
       </c>
       <c r="G44" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H44" t="n">
-        <v>76592</v>
+        <v>79047</v>
       </c>
       <c r="I44" t="n">
-        <v>40.606</v>
-      </c>
-      <c r="J44"/>
+        <v>41.908</v>
+      </c>
+      <c r="J44" t="n">
+        <v>1900</v>
+      </c>
       <c r="K44" t="n">
-        <v>0.541</v>
-      </c>
-      <c r="L44"/>
+        <v>1.007</v>
+      </c>
+      <c r="L44" t="n">
+        <v>1158.667</v>
+      </c>
       <c r="M44" t="n">
-        <v>0.976</v>
-      </c>
-      <c r="N44"/>
+        <v>0.614</v>
+      </c>
+      <c r="N44" t="n">
+        <v>1842.429</v>
+      </c>
       <c r="O44" t="n">
-        <v>0.935</v>
+        <v>0.977</v>
       </c>
       <c r="P44" t="s">
         <v>295</v>
@@ -4726,7 +4748,7 @@
         <v>299</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>43961</v>
+        <v>43963</v>
       </c>
       <c r="D45" t="s">
         <v>300</v>
@@ -4736,25 +4758,31 @@
       </c>
       <c r="F45"/>
       <c r="G45" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H45" t="n">
-        <v>183913</v>
+        <v>192386</v>
       </c>
       <c r="I45" t="n">
-        <v>67.558</v>
-      </c>
-      <c r="J45"/>
+        <v>70.671</v>
+      </c>
+      <c r="J45" t="n">
+        <v>5821</v>
+      </c>
       <c r="K45" t="n">
-        <v>1.315</v>
-      </c>
-      <c r="L45"/>
+        <v>2.138</v>
+      </c>
+      <c r="L45" t="n">
+        <v>4018</v>
+      </c>
       <c r="M45" t="n">
-        <v>2.427</v>
-      </c>
-      <c r="N45"/>
+        <v>1.476</v>
+      </c>
+      <c r="N45" t="n">
+        <v>6182.857</v>
+      </c>
       <c r="O45" t="n">
-        <v>2.216</v>
+        <v>2.271</v>
       </c>
       <c r="P45" t="s">
         <v>43</v>
@@ -4777,7 +4805,7 @@
         <v>304</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D46" t="s">
         <v>305</v>
@@ -4787,31 +4815,31 @@
       </c>
       <c r="F46"/>
       <c r="G46" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H46" t="n">
-        <v>54463</v>
+        <v>56394</v>
       </c>
       <c r="I46" t="n">
-        <v>87.005</v>
+        <v>90.09</v>
       </c>
       <c r="J46" t="n">
-        <v>1206</v>
+        <v>979</v>
       </c>
       <c r="K46" t="n">
-        <v>1.927</v>
+        <v>1.564</v>
       </c>
       <c r="L46" t="n">
-        <v>1310</v>
+        <v>643.667</v>
       </c>
       <c r="M46" t="n">
-        <v>2.093</v>
+        <v>1.028</v>
       </c>
       <c r="N46" t="n">
-        <v>1000.429</v>
+        <v>1013.571</v>
       </c>
       <c r="O46" t="n">
-        <v>1.598</v>
+        <v>1.619</v>
       </c>
       <c r="P46" t="s">
         <v>306</v>
@@ -4834,7 +4862,7 @@
         <v>310</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>43961</v>
+        <v>43962</v>
       </c>
       <c r="D47" t="s">
         <v>311</v>
@@ -4844,16 +4872,20 @@
       </c>
       <c r="F47"/>
       <c r="G47" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H47" t="n">
-        <v>256937</v>
+        <v>266048</v>
       </c>
       <c r="I47" t="n">
-        <v>7.938</v>
-      </c>
-      <c r="J47"/>
-      <c r="K47"/>
+        <v>8.22</v>
+      </c>
+      <c r="J47" t="n">
+        <v>9111</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0.281</v>
+      </c>
       <c r="L47"/>
       <c r="M47"/>
       <c r="N47"/>
@@ -4879,7 +4911,7 @@
         <v>317</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>43960</v>
+        <v>43962</v>
       </c>
       <c r="D48" t="s">
         <v>318</v>
@@ -4889,13 +4921,13 @@
       </c>
       <c r="F48"/>
       <c r="G48" t="n">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H48" t="n">
-        <v>107261</v>
+        <v>114125</v>
       </c>
       <c r="I48" t="n">
-        <v>0.832</v>
+        <v>0.885</v>
       </c>
       <c r="J48"/>
       <c r="K48" t="n">
@@ -4903,11 +4935,11 @@
       </c>
       <c r="L48"/>
       <c r="M48" t="n">
-        <v>0.004</v>
+        <v>0.002</v>
       </c>
       <c r="N48"/>
       <c r="O48" t="n">
-        <v>0.014</v>
+        <v>0.013</v>
       </c>
       <c r="P48" t="s">
         <v>319</v>
@@ -4989,7 +5021,7 @@
         <v>329</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>43959</v>
+        <v>43963</v>
       </c>
       <c r="D50" t="s">
         <v>330</v>
@@ -5001,32 +5033,24 @@
         <v>332</v>
       </c>
       <c r="G50" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H50" t="n">
-        <v>10848</v>
+        <v>11822</v>
       </c>
       <c r="I50" t="n">
-        <v>0.199</v>
+        <v>0.217</v>
       </c>
       <c r="J50" t="n">
-        <v>582</v>
+        <v>340</v>
       </c>
       <c r="K50" t="n">
-        <v>0.011</v>
-      </c>
-      <c r="L50" t="n">
-        <v>517.667</v>
-      </c>
-      <c r="M50" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="N50" t="n">
-        <v>372.571</v>
-      </c>
-      <c r="O50" t="n">
-        <v>0.007</v>
-      </c>
+        <v>0.006</v>
+      </c>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+      <c r="O50"/>
       <c r="P50" t="s">
         <v>331</v>
       </c>
@@ -5048,7 +5072,7 @@
         <v>336</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>43960</v>
+        <v>43962</v>
       </c>
       <c r="D51" t="s">
         <v>337</v>
@@ -5060,31 +5084,31 @@
         <v>339</v>
       </c>
       <c r="G51" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H51" t="n">
-        <v>16309</v>
+        <v>17809</v>
       </c>
       <c r="I51" t="n">
-        <v>0.56</v>
+        <v>0.611</v>
       </c>
       <c r="J51" t="n">
-        <v>817</v>
+        <v>911</v>
       </c>
       <c r="K51" t="n">
-        <v>0.028</v>
+        <v>0.031</v>
       </c>
       <c r="L51" t="n">
-        <v>737.667</v>
+        <v>772.333</v>
       </c>
       <c r="M51" t="n">
-        <v>0.025</v>
+        <v>0.026</v>
       </c>
       <c r="N51" t="n">
-        <v>458.714</v>
+        <v>595.571</v>
       </c>
       <c r="O51" t="n">
-        <v>0.016</v>
+        <v>0.02</v>
       </c>
       <c r="P51" t="s">
         <v>338</v>
@@ -5107,7 +5131,7 @@
         <v>343</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>43958</v>
+        <v>43962</v>
       </c>
       <c r="D52" t="s">
         <v>344</v>
@@ -5117,26 +5141,22 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H52" t="n">
-        <v>254456</v>
+        <v>270351</v>
       </c>
       <c r="I52" t="n">
-        <v>14.85</v>
+        <v>15.778</v>
       </c>
       <c r="J52" t="n">
-        <v>4442</v>
+        <v>3192</v>
       </c>
       <c r="K52" t="n">
-        <v>0.259</v>
-      </c>
-      <c r="L52" t="n">
-        <v>4035.667</v>
-      </c>
-      <c r="M52" t="n">
-        <v>0.235</v>
-      </c>
+        <v>0.186</v>
+      </c>
+      <c r="L52"/>
+      <c r="M52"/>
       <c r="N52"/>
       <c r="O52"/>
       <c r="P52" t="s">
@@ -5160,7 +5180,7 @@
         <v>350</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>43960</v>
+        <v>43962</v>
       </c>
       <c r="D53" t="s">
         <v>351</v>
@@ -5170,31 +5190,31 @@
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H53" t="n">
-        <v>190326</v>
+        <v>197084</v>
       </c>
       <c r="I53" t="n">
-        <v>39.468</v>
+        <v>40.87</v>
       </c>
       <c r="J53" t="n">
-        <v>7287</v>
+        <v>2893</v>
       </c>
       <c r="K53" t="n">
-        <v>1.511</v>
+        <v>0.6</v>
       </c>
       <c r="L53" t="n">
-        <v>7434.333</v>
+        <v>4681.667</v>
       </c>
       <c r="M53" t="n">
-        <v>1.542</v>
+        <v>0.971</v>
       </c>
       <c r="N53" t="n">
-        <v>5729</v>
+        <v>5879.429</v>
       </c>
       <c r="O53" t="n">
-        <v>1.188</v>
+        <v>1.219</v>
       </c>
       <c r="P53" t="s">
         <v>352</v>
@@ -5217,7 +5237,7 @@
         <v>355</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>43959</v>
+        <v>43963</v>
       </c>
       <c r="D54" t="s">
         <v>356</v>
@@ -5227,26 +5247,22 @@
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H54" t="n">
-        <v>23835</v>
+        <v>28418</v>
       </c>
       <c r="I54" t="n">
-        <v>0.116</v>
+        <v>0.138</v>
       </c>
       <c r="J54" t="n">
-        <v>1343</v>
+        <v>1340</v>
       </c>
       <c r="K54" t="n">
         <v>0.007</v>
       </c>
-      <c r="L54" t="n">
-        <v>1441</v>
-      </c>
-      <c r="M54" t="n">
-        <v>0.007</v>
-      </c>
+      <c r="L54"/>
+      <c r="M54"/>
       <c r="N54"/>
       <c r="O54"/>
       <c r="P54" t="s">
@@ -5270,7 +5286,7 @@
         <v>361</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>43959</v>
+        <v>43963</v>
       </c>
       <c r="D55" t="s">
         <v>362</v>
@@ -5280,19 +5296,19 @@
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H55" t="n">
-        <v>195921</v>
+        <v>205239</v>
       </c>
       <c r="I55" t="n">
-        <v>36.14</v>
+        <v>37.858</v>
       </c>
       <c r="J55" t="n">
-        <v>3975</v>
+        <v>2488</v>
       </c>
       <c r="K55" t="n">
-        <v>0.733</v>
+        <v>0.459</v>
       </c>
       <c r="L55"/>
       <c r="M55"/>
@@ -5319,7 +5335,7 @@
         <v>368</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>43961</v>
+        <v>43963</v>
       </c>
       <c r="D56" t="s">
         <v>369</v>
@@ -5329,31 +5345,31 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H56" t="n">
-        <v>283517</v>
+        <v>305851</v>
       </c>
       <c r="I56" t="n">
-        <v>1.284</v>
+        <v>1.385</v>
       </c>
       <c r="J56" t="n">
-        <v>13492</v>
+        <v>10957</v>
       </c>
       <c r="K56" t="n">
-        <v>0.061</v>
+        <v>0.05</v>
       </c>
       <c r="L56" t="n">
-        <v>12913</v>
+        <v>11942</v>
       </c>
       <c r="M56" t="n">
-        <v>0.058</v>
+        <v>0.054</v>
       </c>
       <c r="N56" t="n">
-        <v>11498.857</v>
+        <v>11921</v>
       </c>
       <c r="O56" t="n">
-        <v>0.052</v>
+        <v>0.054</v>
       </c>
       <c r="P56" t="s">
         <v>370</v>
@@ -5376,7 +5392,7 @@
         <v>374</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>43960</v>
+        <v>43961</v>
       </c>
       <c r="D57" t="s">
         <v>375</v>
@@ -5388,31 +5404,31 @@
         <v>376</v>
       </c>
       <c r="G57" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H57" t="n">
-        <v>41649</v>
+        <v>42657</v>
       </c>
       <c r="I57" t="n">
-        <v>9.653</v>
+        <v>9.886</v>
       </c>
       <c r="J57" t="n">
-        <v>1293</v>
+        <v>1008</v>
       </c>
       <c r="K57" t="n">
-        <v>0.3</v>
+        <v>0.234</v>
       </c>
       <c r="L57" t="n">
-        <v>1211.667</v>
+        <v>1188</v>
       </c>
       <c r="M57" t="n">
-        <v>0.281</v>
+        <v>0.276</v>
       </c>
       <c r="N57" t="n">
-        <v>1185</v>
+        <v>1171.143</v>
       </c>
       <c r="O57" t="n">
-        <v>0.275</v>
+        <v>0.272</v>
       </c>
       <c r="P57" t="s">
         <v>43</v>
@@ -5494,7 +5510,7 @@
         <v>388</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>43961</v>
+        <v>43963</v>
       </c>
       <c r="D59" t="s">
         <v>389</v>
@@ -5504,16 +5520,20 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H59" t="n">
-        <v>494250</v>
+        <v>532169</v>
       </c>
       <c r="I59" t="n">
-        <v>14.99</v>
-      </c>
-      <c r="J59"/>
-      <c r="K59"/>
+        <v>16.14</v>
+      </c>
+      <c r="J59" t="n">
+        <v>19300</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.585</v>
+      </c>
       <c r="L59"/>
       <c r="M59"/>
       <c r="N59"/>
@@ -5539,7 +5559,7 @@
         <v>395</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>43958</v>
+        <v>43961</v>
       </c>
       <c r="D60" t="s">
         <v>396</v>
@@ -5549,26 +5569,18 @@
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H60" t="n">
-        <v>136706</v>
+        <v>157850</v>
       </c>
       <c r="I60" t="n">
-        <v>1.248</v>
-      </c>
-      <c r="J60" t="n">
-        <v>5216</v>
-      </c>
-      <c r="K60" t="n">
-        <v>0.048</v>
-      </c>
-      <c r="L60" t="n">
-        <v>5731.333</v>
-      </c>
-      <c r="M60" t="n">
-        <v>0.053</v>
-      </c>
+        <v>1.44</v>
+      </c>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="M60"/>
       <c r="N60"/>
       <c r="O60"/>
       <c r="P60" t="s">
@@ -5592,7 +5604,7 @@
         <v>400</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D61" t="s">
         <v>401</v>
@@ -5604,31 +5616,31 @@
         <v>403</v>
       </c>
       <c r="G61" t="n">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H61" t="n">
-        <v>460686</v>
+        <v>507778</v>
       </c>
       <c r="I61" t="n">
-        <v>12.172</v>
+        <v>13.417</v>
       </c>
       <c r="J61" t="n">
-        <v>17180</v>
+        <v>16562</v>
       </c>
       <c r="K61" t="n">
-        <v>0.454</v>
+        <v>0.438</v>
       </c>
       <c r="L61" t="n">
-        <v>16739.333</v>
+        <v>15697.333</v>
       </c>
       <c r="M61" t="n">
-        <v>0.442</v>
+        <v>0.415</v>
       </c>
       <c r="N61" t="n">
-        <v>13524.714</v>
+        <v>16215.429</v>
       </c>
       <c r="O61" t="n">
-        <v>0.358</v>
+        <v>0.429</v>
       </c>
       <c r="P61" t="s">
         <v>404</v>
@@ -5651,7 +5663,7 @@
         <v>408</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>43956</v>
+        <v>43961</v>
       </c>
       <c r="D62" t="s">
         <v>409</v>
@@ -5661,31 +5673,31 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H62" t="n">
-        <v>485925</v>
+        <v>553855</v>
       </c>
       <c r="I62" t="n">
-        <v>47.655</v>
+        <v>54.317</v>
       </c>
       <c r="J62" t="n">
-        <v>15556</v>
+        <v>7472</v>
       </c>
       <c r="K62" t="n">
-        <v>1.526</v>
+        <v>0.733</v>
       </c>
       <c r="L62" t="n">
-        <v>11893.667</v>
+        <v>12041.667</v>
       </c>
       <c r="M62" t="n">
-        <v>1.166</v>
+        <v>1.181</v>
       </c>
       <c r="N62" t="n">
-        <v>12837.714</v>
+        <v>13602</v>
       </c>
       <c r="O62" t="n">
-        <v>1.259</v>
+        <v>1.334</v>
       </c>
       <c r="P62" t="s">
         <v>410</v>
@@ -5708,7 +5720,7 @@
         <v>414</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>43961</v>
+        <v>43963</v>
       </c>
       <c r="D63" t="s">
         <v>415</v>
@@ -5718,31 +5730,31 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H63" t="n">
-        <v>127769</v>
+        <v>135294</v>
       </c>
       <c r="I63" t="n">
-        <v>44.348</v>
+        <v>46.96</v>
       </c>
       <c r="J63" t="n">
-        <v>3215</v>
+        <v>4250</v>
       </c>
       <c r="K63" t="n">
-        <v>1.116</v>
+        <v>1.475</v>
       </c>
       <c r="L63" t="n">
-        <v>3758</v>
+        <v>3580</v>
       </c>
       <c r="M63" t="n">
-        <v>1.305</v>
+        <v>1.243</v>
       </c>
       <c r="N63" t="n">
-        <v>3333.429</v>
+        <v>3647.429</v>
       </c>
       <c r="O63" t="n">
-        <v>1.157</v>
+        <v>1.266</v>
       </c>
       <c r="P63" t="s">
         <v>416</v>
@@ -5765,7 +5777,7 @@
         <v>420</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D64" t="s">
         <v>421</v>
@@ -5777,31 +5789,31 @@
         <v>423</v>
       </c>
       <c r="G64" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H64" t="n">
-        <v>248056</v>
+        <v>269183</v>
       </c>
       <c r="I64" t="n">
-        <v>12.894</v>
+        <v>13.992</v>
       </c>
       <c r="J64" t="n">
-        <v>10776</v>
+        <v>6964</v>
       </c>
       <c r="K64" t="n">
-        <v>0.56</v>
+        <v>0.362</v>
       </c>
       <c r="L64" t="n">
-        <v>10305.667</v>
+        <v>7042.333</v>
       </c>
       <c r="M64" t="n">
-        <v>0.535</v>
+        <v>0.366</v>
       </c>
       <c r="N64" t="n">
-        <v>8216.571</v>
+        <v>9048.714</v>
       </c>
       <c r="O64" t="n">
-        <v>0.427</v>
+        <v>0.47</v>
       </c>
       <c r="P64" t="s">
         <v>422</v>
@@ -5824,7 +5836,7 @@
         <v>426</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>43961</v>
+        <v>43963</v>
       </c>
       <c r="D65" t="s">
         <v>427</v>
@@ -5834,31 +5846,31 @@
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H65" t="n">
-        <v>5448463</v>
+        <v>5805404</v>
       </c>
       <c r="I65" t="n">
-        <v>37.335</v>
+        <v>39.781</v>
       </c>
       <c r="J65" t="n">
-        <v>226499</v>
+        <v>168641</v>
       </c>
       <c r="K65" t="n">
-        <v>1.552</v>
+        <v>1.156</v>
       </c>
       <c r="L65" t="n">
-        <v>215090.333</v>
+        <v>194480</v>
       </c>
       <c r="M65" t="n">
-        <v>1.474</v>
+        <v>1.333</v>
       </c>
       <c r="N65" t="n">
-        <v>192637.714</v>
+        <v>192149.571</v>
       </c>
       <c r="O65" t="n">
-        <v>1.32</v>
+        <v>1.317</v>
       </c>
       <c r="P65" t="s">
         <v>428</v>
@@ -5881,7 +5893,7 @@
         <v>432</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>43960</v>
+        <v>43962</v>
       </c>
       <c r="D66" t="s">
         <v>433</v>
@@ -5891,31 +5903,25 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H66" t="n">
-        <v>41385</v>
+        <v>42805</v>
       </c>
       <c r="I66" t="n">
-        <v>3.195</v>
-      </c>
-      <c r="J66" t="n">
-        <v>1198</v>
-      </c>
+        <v>3.305</v>
+      </c>
+      <c r="J66"/>
       <c r="K66" t="n">
-        <v>0.092</v>
-      </c>
-      <c r="L66" t="n">
-        <v>1356.667</v>
-      </c>
+        <v>0.029</v>
+      </c>
+      <c r="L66"/>
       <c r="M66" t="n">
-        <v>0.104</v>
-      </c>
-      <c r="N66" t="n">
-        <v>1154.571</v>
-      </c>
+        <v>0.067</v>
+      </c>
+      <c r="N66"/>
       <c r="O66" t="n">
-        <v>0.089</v>
+        <v>0.085</v>
       </c>
       <c r="P66" t="s">
         <v>434</v>
@@ -5938,7 +5944,7 @@
         <v>438</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D67" t="s">
         <v>439</v>
@@ -5948,25 +5954,25 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H67" t="n">
-        <v>433500</v>
+        <v>482374</v>
       </c>
       <c r="I67" t="n">
-        <v>12.452</v>
+        <v>13.856</v>
       </c>
       <c r="J67" t="n">
-        <v>14778</v>
+        <v>15005</v>
       </c>
       <c r="K67" t="n">
-        <v>0.424</v>
+        <v>0.431</v>
       </c>
       <c r="L67" t="n">
-        <v>14613.667</v>
+        <v>16291.333</v>
       </c>
       <c r="M67" t="n">
-        <v>0.419</v>
+        <v>0.468</v>
       </c>
       <c r="N67"/>
       <c r="O67"/>
@@ -5991,7 +5997,7 @@
         <v>442</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D68" t="s">
         <v>443</v>
@@ -6003,31 +6009,31 @@
         <v>445</v>
       </c>
       <c r="G68" t="n">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H68" t="n">
-        <v>20217</v>
+        <v>23589</v>
       </c>
       <c r="I68" t="n">
-        <v>1.207</v>
+        <v>1.409</v>
       </c>
       <c r="J68" t="n">
-        <v>848</v>
+        <v>1099</v>
       </c>
       <c r="K68" t="n">
-        <v>0.051</v>
+        <v>0.066</v>
       </c>
       <c r="L68" t="n">
-        <v>915.667</v>
+        <v>1124</v>
       </c>
       <c r="M68" t="n">
-        <v>0.055</v>
+        <v>0.067</v>
       </c>
       <c r="N68" t="n">
-        <v>892.571</v>
+        <v>1043</v>
       </c>
       <c r="O68" t="n">
-        <v>0.053</v>
+        <v>0.062</v>
       </c>
       <c r="P68" t="s">
         <v>446</v>
@@ -6050,7 +6056,7 @@
         <v>451</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D69" t="s">
         <v>452</v>
@@ -6062,31 +6068,31 @@
         <v>453</v>
       </c>
       <c r="G69" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H69" t="n">
-        <v>134533</v>
+        <v>151304</v>
       </c>
       <c r="I69" t="n">
-        <v>19.771</v>
+        <v>22.236</v>
       </c>
       <c r="J69" t="n">
-        <v>5728</v>
+        <v>5700</v>
       </c>
       <c r="K69" t="n">
-        <v>0.842</v>
+        <v>0.838</v>
       </c>
       <c r="L69" t="n">
-        <v>5686.333</v>
+        <v>5590.333</v>
       </c>
       <c r="M69" t="n">
-        <v>0.836</v>
+        <v>0.822</v>
       </c>
       <c r="N69" t="n">
-        <v>5413.714</v>
+        <v>5718</v>
       </c>
       <c r="O69" t="n">
-        <v>0.796</v>
+        <v>0.84</v>
       </c>
       <c r="P69" t="s">
         <v>43</v>
@@ -6199,7 +6205,7 @@
         <v>465</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>43961</v>
+        <v>43963</v>
       </c>
       <c r="D72" t="s">
         <v>466</v>
@@ -6209,25 +6215,31 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H72" t="n">
-        <v>119859</v>
+        <v>122708</v>
       </c>
       <c r="I72" t="n">
-        <v>21.954</v>
-      </c>
-      <c r="J72"/>
+        <v>22.475</v>
+      </c>
+      <c r="J72" t="n">
+        <v>2063</v>
+      </c>
       <c r="K72" t="n">
-        <v>0.273</v>
-      </c>
-      <c r="L72"/>
+        <v>0.378</v>
+      </c>
+      <c r="L72" t="n">
+        <v>1445.667</v>
+      </c>
       <c r="M72" t="n">
-        <v>0.616</v>
-      </c>
-      <c r="N72"/>
+        <v>0.265</v>
+      </c>
+      <c r="N72" t="n">
+        <v>3263.429</v>
+      </c>
       <c r="O72" t="n">
-        <v>0.619</v>
+        <v>0.598</v>
       </c>
       <c r="P72" t="s">
         <v>468</v>
@@ -6250,7 +6262,7 @@
         <v>473</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>43960</v>
+        <v>43962</v>
       </c>
       <c r="D73" t="s">
         <v>474</v>
@@ -6260,31 +6272,31 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H73" t="n">
-        <v>62828</v>
+        <v>64547</v>
       </c>
       <c r="I73" t="n">
-        <v>30.221</v>
+        <v>31.048</v>
       </c>
       <c r="J73" t="n">
-        <v>625</v>
+        <v>1182</v>
       </c>
       <c r="K73" t="n">
-        <v>0.301</v>
+        <v>0.569</v>
       </c>
       <c r="L73" t="n">
-        <v>950</v>
+        <v>781.333</v>
       </c>
       <c r="M73" t="n">
-        <v>0.457</v>
+        <v>0.376</v>
       </c>
       <c r="N73" t="n">
-        <v>1044</v>
+        <v>1010.429</v>
       </c>
       <c r="O73" t="n">
-        <v>0.502</v>
+        <v>0.486</v>
       </c>
       <c r="P73" t="s">
         <v>476</v>
@@ -6307,7 +6319,7 @@
         <v>480</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D74" t="s">
         <v>481</v>
@@ -6319,31 +6331,31 @@
         <v>483</v>
       </c>
       <c r="G74" t="n">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H74" t="n">
-        <v>324079</v>
+        <v>369697</v>
       </c>
       <c r="I74" t="n">
-        <v>5.464</v>
+        <v>6.233</v>
       </c>
       <c r="J74" t="n">
-        <v>16327</v>
+        <v>13630</v>
       </c>
       <c r="K74" t="n">
-        <v>0.275</v>
+        <v>0.23</v>
       </c>
       <c r="L74" t="n">
-        <v>14900</v>
+        <v>15206</v>
       </c>
       <c r="M74" t="n">
-        <v>0.251</v>
+        <v>0.256</v>
       </c>
       <c r="N74" t="n">
-        <v>13341.857</v>
+        <v>14519</v>
       </c>
       <c r="O74" t="n">
-        <v>0.225</v>
+        <v>0.245</v>
       </c>
       <c r="P74" t="s">
         <v>482</v>
@@ -6366,7 +6378,7 @@
         <v>487</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>43961</v>
+        <v>43963</v>
       </c>
       <c r="D75" t="s">
         <v>488</v>
@@ -6376,31 +6388,31 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H75" t="n">
-        <v>663886</v>
+        <v>680890</v>
       </c>
       <c r="I75" t="n">
-        <v>12.949</v>
+        <v>13.281</v>
       </c>
       <c r="J75" t="n">
-        <v>3856</v>
+        <v>12398</v>
       </c>
       <c r="K75" t="n">
-        <v>0.075</v>
+        <v>0.242</v>
       </c>
       <c r="L75" t="n">
-        <v>4832.667</v>
+        <v>6953.333</v>
       </c>
       <c r="M75" t="n">
-        <v>0.094</v>
+        <v>0.136</v>
       </c>
       <c r="N75" t="n">
-        <v>4701.857</v>
+        <v>5807.571</v>
       </c>
       <c r="O75" t="n">
-        <v>0.092</v>
+        <v>0.113</v>
       </c>
       <c r="P75" t="s">
         <v>489</v>
@@ -6470,7 +6482,7 @@
         <v>501</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>43954</v>
+        <v>43961</v>
       </c>
       <c r="D77" t="s">
         <v>502</v>
@@ -6480,13 +6492,13 @@
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H77" t="n">
-        <v>148500</v>
+        <v>177500</v>
       </c>
       <c r="I77" t="n">
-        <v>14.704</v>
+        <v>17.576</v>
       </c>
       <c r="J77"/>
       <c r="K77"/>
@@ -6515,7 +6527,7 @@
         <v>506</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>43960</v>
+        <v>43962</v>
       </c>
       <c r="D78" t="s">
         <v>507</v>
@@ -6525,25 +6537,31 @@
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H78" t="n">
-        <v>309595</v>
+        <v>316851</v>
       </c>
       <c r="I78" t="n">
-        <v>35.772</v>
-      </c>
-      <c r="J78"/>
+        <v>36.611</v>
+      </c>
+      <c r="J78" t="n">
+        <v>2501</v>
+      </c>
       <c r="K78" t="n">
-        <v>0.045</v>
-      </c>
-      <c r="L78"/>
+        <v>0.289</v>
+      </c>
+      <c r="L78" t="n">
+        <v>2350.333</v>
+      </c>
       <c r="M78" t="n">
-        <v>0.336</v>
-      </c>
-      <c r="N78"/>
+        <v>0.272</v>
+      </c>
+      <c r="N78" t="n">
+        <v>3884.143</v>
+      </c>
       <c r="O78" t="n">
-        <v>0.434</v>
+        <v>0.449</v>
       </c>
       <c r="P78" t="s">
         <v>508</v>
@@ -6566,7 +6584,7 @@
         <v>512</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>43960</v>
+        <v>43962</v>
       </c>
       <c r="D79" t="s">
         <v>513</v>
@@ -6576,31 +6594,31 @@
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H79" t="n">
-        <v>67133</v>
+        <v>67758</v>
       </c>
       <c r="I79" t="n">
-        <v>2.819</v>
+        <v>2.845</v>
       </c>
       <c r="J79" t="n">
-        <v>272</v>
+        <v>358</v>
       </c>
       <c r="K79" t="n">
-        <v>0.011</v>
+        <v>0.015</v>
       </c>
       <c r="L79" t="n">
-        <v>362.333</v>
+        <v>299</v>
       </c>
       <c r="M79" t="n">
-        <v>0.015</v>
+        <v>0.012</v>
       </c>
       <c r="N79" t="n">
-        <v>434.143</v>
+        <v>400</v>
       </c>
       <c r="O79" t="n">
-        <v>0.018</v>
+        <v>0.017</v>
       </c>
       <c r="P79" t="s">
         <v>514</v>
@@ -6623,7 +6641,7 @@
         <v>519</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>43961</v>
+        <v>43962</v>
       </c>
       <c r="D80" t="s">
         <v>520</v>
@@ -6633,25 +6651,31 @@
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H80" t="n">
-        <v>97177</v>
+        <v>103858</v>
       </c>
       <c r="I80" t="n">
-        <v>1.392</v>
-      </c>
-      <c r="J80"/>
+        <v>1.488</v>
+      </c>
+      <c r="J80" t="n">
+        <v>3454</v>
+      </c>
       <c r="K80" t="n">
-        <v>0.003</v>
-      </c>
-      <c r="L80"/>
+        <v>0.049</v>
+      </c>
+      <c r="L80" t="n">
+        <v>3404.667</v>
+      </c>
       <c r="M80" t="n">
-        <v>0.035</v>
-      </c>
-      <c r="N80"/>
+        <v>0.049</v>
+      </c>
+      <c r="N80" t="n">
+        <v>3584.286</v>
+      </c>
       <c r="O80" t="n">
-        <v>0.045</v>
+        <v>0.051</v>
       </c>
       <c r="P80" t="s">
         <v>522</v>
@@ -6674,7 +6698,7 @@
         <v>526</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>43958</v>
+        <v>43961</v>
       </c>
       <c r="D81" t="s">
         <v>527</v>
@@ -6684,18 +6708,22 @@
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H81" t="n">
-        <v>27420</v>
+        <v>33266</v>
       </c>
       <c r="I81" t="n">
-        <v>2.32</v>
+        <v>2.815</v>
       </c>
       <c r="J81"/>
-      <c r="K81"/>
+      <c r="K81" t="n">
+        <v>0.038</v>
+      </c>
       <c r="L81"/>
-      <c r="M81"/>
+      <c r="M81" t="n">
+        <v>0.165</v>
+      </c>
       <c r="N81"/>
       <c r="O81"/>
       <c r="P81" t="s">
@@ -6719,7 +6747,7 @@
         <v>533</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D82" t="s">
         <v>534</v>
@@ -6729,28 +6757,32 @@
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H82" t="n">
-        <v>1334411</v>
+        <v>1440671</v>
       </c>
       <c r="I82" t="n">
-        <v>15.822</v>
+        <v>17.082</v>
       </c>
       <c r="J82" t="n">
-        <v>35605</v>
+        <v>37351</v>
       </c>
       <c r="K82" t="n">
-        <v>0.422</v>
+        <v>0.443</v>
       </c>
       <c r="L82" t="n">
-        <v>33229</v>
+        <v>35420</v>
       </c>
       <c r="M82" t="n">
-        <v>0.394</v>
-      </c>
-      <c r="N82"/>
-      <c r="O82"/>
+        <v>0.42</v>
+      </c>
+      <c r="N82" t="n">
+        <v>33750</v>
+      </c>
+      <c r="O82" t="n">
+        <v>0.4</v>
+      </c>
       <c r="P82" t="s">
         <v>535</v>
       </c>
@@ -6772,7 +6804,7 @@
         <v>540</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>43959</v>
+        <v>43962</v>
       </c>
       <c r="D83" t="s">
         <v>541</v>
@@ -6784,31 +6816,31 @@
         <v>543</v>
       </c>
       <c r="G83" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H83" t="n">
-        <v>55203</v>
+        <v>62461</v>
       </c>
       <c r="I83" t="n">
-        <v>1.207</v>
+        <v>1.366</v>
       </c>
       <c r="J83" t="n">
-        <v>3161</v>
+        <v>2854</v>
       </c>
       <c r="K83" t="n">
-        <v>0.069</v>
+        <v>0.062</v>
       </c>
       <c r="L83" t="n">
-        <v>3493</v>
+        <v>2419.333</v>
       </c>
       <c r="M83" t="n">
-        <v>0.076</v>
+        <v>0.053</v>
       </c>
       <c r="N83" t="n">
-        <v>2967.286</v>
+        <v>2909.857</v>
       </c>
       <c r="O83" t="n">
-        <v>0.065</v>
+        <v>0.064</v>
       </c>
       <c r="P83" t="s">
         <v>542</v>
@@ -6831,7 +6863,7 @@
         <v>547</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>43961</v>
+        <v>43963</v>
       </c>
       <c r="D84" t="s">
         <v>548</v>
@@ -6841,31 +6873,31 @@
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H84" t="n">
-        <v>176403</v>
+        <v>187307</v>
       </c>
       <c r="I84" t="n">
-        <v>4.034</v>
+        <v>4.283</v>
       </c>
       <c r="J84" t="n">
-        <v>9296</v>
+        <v>5755</v>
       </c>
       <c r="K84" t="n">
-        <v>0.213</v>
+        <v>0.132</v>
       </c>
       <c r="L84" t="n">
-        <v>8278</v>
+        <v>6733.333</v>
       </c>
       <c r="M84" t="n">
-        <v>0.189</v>
+        <v>0.154</v>
       </c>
       <c r="N84" t="n">
-        <v>6668.571</v>
+        <v>6792.571</v>
       </c>
       <c r="O84" t="n">
-        <v>0.152</v>
+        <v>0.155</v>
       </c>
       <c r="P84" t="s">
         <v>549</v>
@@ -6888,7 +6920,7 @@
         <v>554</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D85" t="s">
         <v>555</v>
@@ -6898,31 +6930,31 @@
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="H85" t="n">
-        <v>1270408</v>
+        <v>1460517</v>
       </c>
       <c r="I85" t="n">
-        <v>18.714</v>
+        <v>21.514</v>
       </c>
       <c r="J85" t="n">
-        <v>63339</v>
+        <v>60410</v>
       </c>
       <c r="K85" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="L85" t="n">
+        <v>63369.667</v>
+      </c>
+      <c r="M85" t="n">
         <v>0.933</v>
       </c>
-      <c r="L85" t="n">
-        <v>65291.333</v>
-      </c>
-      <c r="M85" t="n">
-        <v>0.962</v>
-      </c>
       <c r="N85" t="n">
-        <v>63153.143</v>
+        <v>63284.143</v>
       </c>
       <c r="O85" t="n">
-        <v>0.93</v>
+        <v>0.932</v>
       </c>
       <c r="P85" t="s">
         <v>556</v>
@@ -6945,7 +6977,7 @@
         <v>559</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>43960</v>
+        <v>43963</v>
       </c>
       <c r="D86" t="s">
         <v>560</v>
@@ -6955,31 +6987,31 @@
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H86" t="n">
-        <v>1728443</v>
+        <v>2007146</v>
       </c>
       <c r="I86" t="n">
-        <v>25.461</v>
+        <v>29.566</v>
       </c>
       <c r="J86" t="n">
-        <v>96878</v>
+        <v>85293</v>
       </c>
       <c r="K86" t="n">
-        <v>1.427</v>
+        <v>1.256</v>
       </c>
       <c r="L86" t="n">
-        <v>93496.667</v>
+        <v>92873.333</v>
       </c>
       <c r="M86" t="n">
-        <v>1.377</v>
+        <v>1.368</v>
       </c>
       <c r="N86" t="n">
-        <v>85205.857</v>
+        <v>89796.143</v>
       </c>
       <c r="O86" t="n">
-        <v>1.255</v>
+        <v>1.323</v>
       </c>
       <c r="P86" t="s">
         <v>556</v>
@@ -7002,7 +7034,7 @@
         <v>564</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>43960</v>
+        <v>43962</v>
       </c>
       <c r="D87" t="s">
         <v>565</v>
@@ -7012,31 +7044,31 @@
       </c>
       <c r="F87"/>
       <c r="G87" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H87" t="n">
-        <v>8709630</v>
+        <v>9348458</v>
       </c>
       <c r="I87" t="n">
-        <v>26.313</v>
+        <v>28.243</v>
       </c>
       <c r="J87" t="n">
-        <v>300842</v>
+        <v>388296</v>
       </c>
       <c r="K87" t="n">
-        <v>0.909</v>
+        <v>1.173</v>
       </c>
       <c r="L87" t="n">
-        <v>307612.333</v>
+        <v>319484</v>
       </c>
       <c r="M87" t="n">
-        <v>0.929</v>
+        <v>0.965</v>
       </c>
       <c r="N87" t="n">
-        <v>272055.571</v>
+        <v>294726.286</v>
       </c>
       <c r="O87" t="n">
-        <v>0.822</v>
+        <v>0.891</v>
       </c>
       <c r="P87" t="s">
         <v>566</v>
@@ -7059,7 +7091,7 @@
         <v>570</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>43952</v>
+        <v>43962</v>
       </c>
       <c r="D88" t="s">
         <v>571</v>
@@ -7069,31 +7101,25 @@
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="H88" t="n">
-        <v>695283</v>
+        <v>824957</v>
       </c>
       <c r="I88" t="n">
-        <v>2.101</v>
-      </c>
-      <c r="J88" t="n">
-        <v>23633</v>
-      </c>
+        <v>2.492</v>
+      </c>
+      <c r="J88"/>
       <c r="K88" t="n">
-        <v>0.071</v>
-      </c>
-      <c r="L88" t="n">
-        <v>24423.333</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L88"/>
       <c r="M88" t="n">
-        <v>0.074</v>
-      </c>
-      <c r="N88" t="n">
-        <v>21015.714</v>
-      </c>
+        <v>0.004</v>
+      </c>
+      <c r="N88"/>
       <c r="O88" t="n">
-        <v>0.063</v>
+        <v>0.036</v>
       </c>
       <c r="P88" t="s">
         <v>573</v>
@@ -7116,7 +7142,7 @@
         <v>578</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>43961</v>
+        <v>43962</v>
       </c>
       <c r="D89" t="s">
         <v>579</v>
@@ -7126,31 +7152,31 @@
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H89" t="n">
-        <v>27461</v>
+        <v>28697</v>
       </c>
       <c r="I89" t="n">
-        <v>7.905</v>
+        <v>8.261</v>
       </c>
       <c r="J89" t="n">
-        <v>623</v>
+        <v>1236</v>
       </c>
       <c r="K89" t="n">
-        <v>0.179</v>
+        <v>0.356</v>
       </c>
       <c r="L89" t="n">
-        <v>935</v>
+        <v>999.667</v>
       </c>
       <c r="M89" t="n">
-        <v>0.269</v>
+        <v>0.288</v>
       </c>
       <c r="N89" t="n">
-        <v>899.571</v>
+        <v>965.429</v>
       </c>
       <c r="O89" t="n">
-        <v>0.259</v>
+        <v>0.278</v>
       </c>
       <c r="P89" t="s">
         <v>126</v>
@@ -7218,7 +7244,7 @@
         <v>590</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>43959</v>
+        <v>43962</v>
       </c>
       <c r="D91" t="s">
         <v>591</v>
@@ -7228,22 +7254,26 @@
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H91" t="n">
-        <v>8741</v>
+        <v>10598</v>
       </c>
       <c r="I91" t="n">
-        <v>0.588</v>
+        <v>0.713</v>
       </c>
       <c r="J91" t="n">
-        <v>600</v>
+        <v>726</v>
       </c>
       <c r="K91" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="L91"/>
-      <c r="M91"/>
+        <v>0.049</v>
+      </c>
+      <c r="L91" t="n">
+        <v>619</v>
+      </c>
+      <c r="M91" t="n">
+        <v>0.042</v>
+      </c>
       <c r="N91"/>
       <c r="O91"/>
       <c r="P91" t="s">

</xml_diff>

<commit_message>
Updated testing data for 2020-05-16
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="603">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -98,7 +98,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/05/coronavirus-covid-19-at-a-glance-15-may-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/05/coronavirus-covid-19-at-a-glance-16-may-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200516115932/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200516192434/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -305,7 +305,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200516115941/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200516192440/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -393,7 +393,7 @@
     <t xml:space="preserve">Croatia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200515124712/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200516192446/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -453,7 +453,7 @@
     <t xml:space="preserve">Denmark - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/COVID19-overvaagningsrapport-15052020-fgg8</t>
+    <t xml:space="preserve">https://files.ssi.dk/COVID19-overvaagningsrapport-16052020-12345</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -516,7 +516,7 @@
     <t xml:space="preserve">Government of El Salvador</t>
   </si>
   <si>
-    <t xml:space="preserve">updated at 16:45pm local time on 2020-05-15.</t>
+    <t xml:space="preserve">updated at 12:45pm local time on 2020-05-16.</t>
   </si>
   <si>
     <t xml:space="preserve">The government of El Salvador publishes an online dashboard with figures and graphs about the epidemic, including the number of tests performed ("pruebas COVID19 realizadas hasta hoy"). No information is given on the geographical scope and number of labs included.</t>
@@ -609,7 +609,7 @@
     <t xml:space="preserve">https://www.santepubliquefrance.fr/recherche/#search=COVID-19%20:%20point%20epidemiologique&amp;sort=dat</t>
   </si>
   <si>
-    <t xml:space="preserve">The source publishes epidemiological updates at irregular intervals. The latest update, as of 15th May, was published on the 7th May. The updates include a figure for the number of tests performed (‘Nombre de tests réalisés’). A breakdown into positive and negative results are given, along with a positive test rate.
+    <t xml:space="preserve">The source publishes epidemiological updates at irregular intervals. The latest update with testing figures, as of 16th May, was published on the 7th May. The updates include a figure for the number of tests performed (‘Nombre de tests réalisés’). A breakdown into positive and negative results are given, along with a positive test rate. The most recent epidemiological report, dated 14th May, does not provide the number of laboratory and hospital tests performed.
 The figures in the time series relate to tests performed since 24 February. Since the 24 March update, in addition to the previously reported hospital tests, laboratory tests are also reported. Only the total number of laboratory tests performed between 24 February and 24 March is presented, without a time series. Our figure for 24 March adds the cumulative number of laboratory tests since 24 February (6,500) to the hospital tests figure (101,046). As such 24 March represents a break in the series.</t>
   </si>
   <si>
@@ -692,7 +692,7 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200515/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200516/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -827,7 +827,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200516003830/http://irangov.ir/detail/339275</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200516191022/http://irangov.ir/detail/339329</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -947,7 +947,7 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000630894.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000631066.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Implementation status of PCR tests for new coronavirus in Japan (based on the date on which the results were determined). Preliminary data</t>
@@ -1038,7 +1038,7 @@
     <t xml:space="preserve">Luxembourg - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200515225730/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200516192544/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg Government situation update</t>
@@ -1128,6 +1128,9 @@
   </si>
   <si>
     <t xml:space="preserve">Myanmar Ministry of Health and Sports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This figure is taken from the interactive dashboard and should be updated once the daily PDF situation report becomes available</t>
   </si>
   <si>
     <t xml:space="preserve">https://mohs.gov.mm/Home</t>
@@ -1316,7 +1319,7 @@
     <t xml:space="preserve">Peru - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/154736-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-84-495-en-el-peru-comunicado-n-101</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/156940-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-88-541-en-el-peru-comunicado-n-102</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1352,7 +1355,7 @@
 The total number of individuals tested is the sum of positive, negative, equivocal, and invalid individuals. No definitions of equivocal and invalid individual tests are given, hence our figures only report the sum of individuals who have tested positive or negative.
 The source provides a breakdown of both i) the number of individuals tested and ii) the total tests conducted, by laboratory. We are not aware of any aggregation issues. 
 The DOH used to report the number of cases tested in a previous dashboard, but stopped on 4th April. This previous breakdown of the test results and COVID-19 dashboard have both been removed. We became aware of this new tracker on the 13th April with data 'as of April 11 2020, 12am'. No previous snapshots of the dashboard are available using web archive, therefore the series starts from the 11th April - the earliest date from which we have access to the data. 
-No newly submitted reports as of 14 May. Latest testing data available is from 13 May 2020.</t>
+No newly submitted reports as of 16 May. Latest testing data available is from 13 May 2020.</t>
   </si>
   <si>
     <t xml:space="preserve">POL</t>
@@ -1464,7 +1467,7 @@
     <t xml:space="preserve">Rwanda - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1261348536970391552</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1261712778756329480</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1751,7 +1754,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200516120425/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200516192735/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1818,7 +1821,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200515225910/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200516192739/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1842,13 +1845,13 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1261025109332185089</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1261413937863553025</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
   </si>
   <si>
-    <t xml:space="preserve">We sum the cumulative total provided for the previous day with the daily number of samples tested today. Samples tested today at the Uganda Virus Research Institute. (UVRI)</t>
+    <t xml:space="preserve">We sum the cumulative total provided for the previous day with the daily number of samples tested today.</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.health.go.ug/moh/resources/</t>
@@ -1857,7 +1860,7 @@
     <t xml:space="preserve">The Office of the Director General publishes a daily press release detailing the cumulative number of samples tested to date, on the [MOH official twitter account](https://twitter.com/MinofHealthUG). The earliest press release that lists the cumulative total is 6th April. However, we cannot say with certainty when testing began and the precise date from which cumulative totals begin. 
 After the 14th April, press releases by the Office of the Director General publishes the daily number of samples tested. We sum the cumulative total number of samples tested for the previous day with the daily number of samples tested today. For example, the total number of samples tested on the 15th April is equal to the cumulative total up until the 14th April plus the number of samples tested on the 15th April. 
 For the 18th April, we rely on the figure reported by the MOH official twitter account to calculate our cumulative totals. From the 5th May, we rely on the figures reported by the MOH official twitter account and check figures against press releases where they have been made available by the MOH.  
-We are aware of Uganda's [MOH information portal](https://covid19.gou.go.ug/), however, it only lists the 'cumulative # tested' without specifying more precise units of measurement. Our cumulative totals for the number of samples tested from 19/04 matches the 'cumulative # tested' total in the Uganda information portal for 20/04. This suggests the 'cumulative # tested' refers to the samples tested up until the previous day. However, the cumulative totals diverge from the 29th April.</t>
+We are aware of Uganda's [MOH information portal](https://covid19.gou.go.ug/), however, it only lists the 'cumulative # tested' without specifying more precise units of measurement. Our cumulative totals for the number of samples tested from 19/04 matches the 'cumulative # tested' total in the Uganda information portal for 20/04. This suggests the 'cumulative # tested' refers to the samples tested up until the previous day. However, the cumulative totals calculated via the daily press releases and the MOH information portal diverge from the 29th April.</t>
   </si>
   <si>
     <t xml:space="preserve">UKR</t>
@@ -1888,7 +1891,7 @@
     <t xml:space="preserve">United Kingdom - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200515225915/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200516192745/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
@@ -1911,7 +1914,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200515225916/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200516192746/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
   </si>
   <si>
     <t xml:space="preserve">The number of tests performed, including tests posted or delivered but not yet returned and/or processed.</t>
@@ -2494,7 +2497,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
@@ -2504,31 +2507,31 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H3" t="n">
-        <v>983816</v>
+        <v>1015652</v>
       </c>
       <c r="I3" t="n">
-        <v>38.581</v>
+        <v>39.83</v>
       </c>
       <c r="J3" t="n">
-        <v>40336</v>
+        <v>31836</v>
       </c>
       <c r="K3" t="n">
-        <v>1.582</v>
+        <v>1.248</v>
       </c>
       <c r="L3" t="n">
-        <v>35296.333</v>
+        <v>35542.333</v>
       </c>
       <c r="M3" t="n">
-        <v>1.384</v>
+        <v>1.394</v>
       </c>
       <c r="N3" t="n">
-        <v>32366.571</v>
+        <v>31456.571</v>
       </c>
       <c r="O3" t="n">
-        <v>1.269</v>
+        <v>1.234</v>
       </c>
       <c r="P3" t="s">
         <v>29</v>
@@ -2621,28 +2624,28 @@
         <v>57</v>
       </c>
       <c r="H5" t="n">
-        <v>228573</v>
+        <v>230188</v>
       </c>
       <c r="I5" t="n">
-        <v>134.33</v>
+        <v>135.279</v>
       </c>
       <c r="J5" t="n">
-        <v>6031</v>
+        <v>7646</v>
       </c>
       <c r="K5" t="n">
-        <v>3.544</v>
+        <v>4.493</v>
       </c>
       <c r="L5" t="n">
-        <v>7667.667</v>
+        <v>8206</v>
       </c>
       <c r="M5" t="n">
-        <v>4.506</v>
+        <v>4.822</v>
       </c>
       <c r="N5" t="n">
-        <v>7174.286</v>
+        <v>7405</v>
       </c>
       <c r="O5" t="n">
-        <v>4.216</v>
+        <v>4.352</v>
       </c>
       <c r="P5" t="s">
         <v>44</v>
@@ -2665,7 +2668,7 @@
         <v>49</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D6" t="s">
         <v>50</v>
@@ -2675,31 +2678,31 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H6" t="n">
-        <v>160512</v>
+        <v>167294</v>
       </c>
       <c r="I6" t="n">
-        <v>0.975</v>
+        <v>1.016</v>
       </c>
       <c r="J6" t="n">
-        <v>8582</v>
+        <v>6782</v>
       </c>
       <c r="K6" t="n">
-        <v>0.052</v>
+        <v>0.041</v>
       </c>
       <c r="L6" t="n">
-        <v>7958</v>
+        <v>7585.333</v>
       </c>
       <c r="M6" t="n">
-        <v>0.048</v>
+        <v>0.046</v>
       </c>
       <c r="N6" t="n">
-        <v>7008.286</v>
+        <v>7196.429</v>
       </c>
       <c r="O6" t="n">
-        <v>0.043</v>
+        <v>0.044</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
@@ -3010,22 +3013,28 @@
         <v>58</v>
       </c>
       <c r="H12" t="n">
-        <v>1236670</v>
+        <v>1265502</v>
       </c>
       <c r="I12" t="n">
-        <v>32.766</v>
-      </c>
-      <c r="J12"/>
+        <v>33.53</v>
+      </c>
+      <c r="J12" t="n">
+        <v>32590</v>
+      </c>
       <c r="K12" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="L12"/>
+        <v>0.863</v>
+      </c>
+      <c r="L12" t="n">
+        <v>32040.667</v>
+      </c>
       <c r="M12" t="n">
-        <v>0.595</v>
-      </c>
-      <c r="N12"/>
+        <v>0.849</v>
+      </c>
+      <c r="N12" t="n">
+        <v>28272.429</v>
+      </c>
       <c r="O12" t="n">
-        <v>0.64</v>
+        <v>0.749</v>
       </c>
       <c r="P12" t="s">
         <v>92</v>
@@ -3048,7 +3057,7 @@
         <v>97</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D13" t="s">
         <v>98</v>
@@ -3060,31 +3069,31 @@
         <v>99</v>
       </c>
       <c r="G13" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H13" t="n">
-        <v>341512</v>
+        <v>350325</v>
       </c>
       <c r="I13" t="n">
-        <v>17.865</v>
+        <v>18.326</v>
       </c>
       <c r="J13" t="n">
-        <v>16095</v>
+        <v>8813</v>
       </c>
       <c r="K13" t="n">
-        <v>0.842</v>
+        <v>0.461</v>
       </c>
       <c r="L13" t="n">
-        <v>12724</v>
+        <v>12191.667</v>
       </c>
       <c r="M13" t="n">
-        <v>0.666</v>
+        <v>0.638</v>
       </c>
       <c r="N13" t="n">
-        <v>12221.571</v>
+        <v>11774.429</v>
       </c>
       <c r="O13" t="n">
-        <v>0.64</v>
+        <v>0.616</v>
       </c>
       <c r="P13" t="s">
         <v>100</v>
@@ -3164,7 +3173,7 @@
         <v>111</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D15" t="s">
         <v>112</v>
@@ -3174,31 +3183,31 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H15" t="n">
-        <v>13031</v>
+        <v>13696</v>
       </c>
       <c r="I15" t="n">
-        <v>2.558</v>
+        <v>2.689</v>
       </c>
       <c r="J15" t="n">
-        <v>209</v>
+        <v>665</v>
       </c>
       <c r="K15" t="n">
-        <v>0.041</v>
+        <v>0.131</v>
       </c>
       <c r="L15" t="n">
-        <v>323.333</v>
+        <v>396.333</v>
       </c>
       <c r="M15" t="n">
-        <v>0.064</v>
+        <v>0.078</v>
       </c>
       <c r="N15" t="n">
-        <v>314.857</v>
+        <v>345.714</v>
       </c>
       <c r="O15" t="n">
-        <v>0.062</v>
+        <v>0.068</v>
       </c>
       <c r="P15" t="s">
         <v>113</v>
@@ -3221,7 +3230,7 @@
         <v>117</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D16" t="s">
         <v>118</v>
@@ -3231,31 +3240,31 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H16" t="n">
-        <v>51568</v>
+        <v>52425</v>
       </c>
       <c r="I16" t="n">
-        <v>12.561</v>
+        <v>12.77</v>
       </c>
       <c r="J16" t="n">
-        <v>1228</v>
+        <v>857</v>
       </c>
       <c r="K16" t="n">
+        <v>0.209</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1229.333</v>
+      </c>
+      <c r="M16" t="n">
         <v>0.299</v>
       </c>
-      <c r="L16" t="n">
-        <v>1362.667</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0.332</v>
-      </c>
       <c r="N16" t="n">
-        <v>1170</v>
+        <v>1172.429</v>
       </c>
       <c r="O16" t="n">
-        <v>0.285</v>
+        <v>0.286</v>
       </c>
       <c r="P16" t="s">
         <v>119</v>
@@ -3278,7 +3287,7 @@
         <v>124</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>43965</v>
+        <v>43966</v>
       </c>
       <c r="D17" t="s">
         <v>125</v>
@@ -3290,31 +3299,31 @@
         <v>127</v>
       </c>
       <c r="G17" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H17" t="n">
-        <v>77374</v>
+        <v>79834</v>
       </c>
       <c r="I17" t="n">
-        <v>6.831</v>
+        <v>7.048</v>
       </c>
       <c r="J17" t="n">
-        <v>2232</v>
+        <v>2460</v>
       </c>
       <c r="K17" t="n">
+        <v>0.217</v>
+      </c>
+      <c r="L17" t="n">
+        <v>2235</v>
+      </c>
+      <c r="M17" t="n">
         <v>0.197</v>
       </c>
-      <c r="L17" t="n">
-        <v>2072.333</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0.183</v>
-      </c>
       <c r="N17" t="n">
-        <v>1973.429</v>
+        <v>2046.429</v>
       </c>
       <c r="O17" t="n">
-        <v>0.174</v>
+        <v>0.181</v>
       </c>
       <c r="P17" t="s">
         <v>126</v>
@@ -3394,7 +3403,7 @@
         <v>136</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D19" t="s">
         <v>137</v>
@@ -3406,31 +3415,31 @@
         <v>139</v>
       </c>
       <c r="G19" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H19" t="n">
-        <v>368889</v>
+        <v>379482</v>
       </c>
       <c r="I19" t="n">
-        <v>63.687</v>
+        <v>65.516</v>
       </c>
       <c r="J19" t="n">
-        <v>10903</v>
+        <v>10593</v>
       </c>
       <c r="K19" t="n">
-        <v>1.882</v>
+        <v>1.829</v>
       </c>
       <c r="L19" t="n">
-        <v>11543</v>
+        <v>11256.667</v>
       </c>
       <c r="M19" t="n">
-        <v>1.993</v>
+        <v>1.943</v>
       </c>
       <c r="N19" t="n">
-        <v>10057.286</v>
+        <v>10071.143</v>
       </c>
       <c r="O19" t="n">
-        <v>1.736</v>
+        <v>1.739</v>
       </c>
       <c r="P19" t="s">
         <v>140</v>
@@ -3500,7 +3509,7 @@
         <v>152</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D21" t="s">
         <v>153</v>
@@ -3512,16 +3521,20 @@
         <v>155</v>
       </c>
       <c r="G21" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H21" t="n">
-        <v>51142</v>
+        <v>53412</v>
       </c>
       <c r="I21" t="n">
-        <v>7.885</v>
-      </c>
-      <c r="J21"/>
-      <c r="K21"/>
+        <v>8.235</v>
+      </c>
+      <c r="J21" t="n">
+        <v>2270</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.35</v>
+      </c>
       <c r="L21"/>
       <c r="M21"/>
       <c r="N21"/>
@@ -3657,7 +3670,7 @@
         <v>172</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>43964</v>
+        <v>43966</v>
       </c>
       <c r="D24" t="s">
         <v>173</v>
@@ -3667,25 +3680,25 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H24" t="n">
-        <v>136878</v>
+        <v>143805</v>
       </c>
       <c r="I24" t="n">
-        <v>24.704</v>
+        <v>25.954</v>
       </c>
       <c r="J24"/>
       <c r="K24" t="n">
-        <v>0.215</v>
+        <v>0.123</v>
       </c>
       <c r="L24"/>
       <c r="M24" t="n">
-        <v>0.42</v>
+        <v>0.472</v>
       </c>
       <c r="N24"/>
       <c r="O24" t="n">
-        <v>0.471</v>
+        <v>0.472</v>
       </c>
       <c r="P24" t="s">
         <v>175</v>
@@ -3802,7 +3815,7 @@
         <v>193</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>43964</v>
+        <v>43965</v>
       </c>
       <c r="D27" t="s">
         <v>194</v>
@@ -3814,25 +3827,25 @@
         <v>196</v>
       </c>
       <c r="G27" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H27" t="n">
-        <v>167704</v>
+        <v>171642</v>
       </c>
       <c r="I27" t="n">
-        <v>5.397</v>
+        <v>5.524</v>
       </c>
       <c r="J27" t="n">
-        <v>3252</v>
+        <v>3938</v>
       </c>
       <c r="K27" t="n">
-        <v>0.105</v>
+        <v>0.127</v>
       </c>
       <c r="L27" t="n">
-        <v>2728</v>
+        <v>3479.667</v>
       </c>
       <c r="M27" t="n">
-        <v>0.088</v>
+        <v>0.112</v>
       </c>
       <c r="N27"/>
       <c r="O27"/>
@@ -3857,7 +3870,7 @@
         <v>201</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>43964</v>
+        <v>43965</v>
       </c>
       <c r="D28" t="s">
         <v>194</v>
@@ -3869,25 +3882,25 @@
         <v>202</v>
       </c>
       <c r="G28" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H28" t="n">
-        <v>168685</v>
+        <v>172623</v>
       </c>
       <c r="I28" t="n">
-        <v>5.429</v>
+        <v>5.555</v>
       </c>
       <c r="J28" t="n">
-        <v>3252</v>
+        <v>3938</v>
       </c>
       <c r="K28" t="n">
-        <v>0.105</v>
+        <v>0.127</v>
       </c>
       <c r="L28" t="n">
-        <v>2728</v>
+        <v>3479.667</v>
       </c>
       <c r="M28" t="n">
-        <v>0.088</v>
+        <v>0.112</v>
       </c>
       <c r="N28"/>
       <c r="O28"/>
@@ -3912,7 +3925,7 @@
         <v>204</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D29" t="s">
         <v>205</v>
@@ -3922,31 +3935,31 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H29" t="n">
-        <v>120015</v>
+        <v>126283</v>
       </c>
       <c r="I29" t="n">
-        <v>11.514</v>
+        <v>12.116</v>
       </c>
       <c r="J29" t="n">
-        <v>3782</v>
+        <v>6268</v>
       </c>
       <c r="K29" t="n">
-        <v>0.363</v>
+        <v>0.601</v>
       </c>
       <c r="L29" t="n">
-        <v>4653.667</v>
+        <v>4747</v>
       </c>
       <c r="M29" t="n">
-        <v>0.446</v>
+        <v>0.455</v>
       </c>
       <c r="N29" t="n">
-        <v>3674.857</v>
+        <v>4128.429</v>
       </c>
       <c r="O29" t="n">
-        <v>0.353</v>
+        <v>0.396</v>
       </c>
       <c r="P29" t="s">
         <v>207</v>
@@ -4073,7 +4086,7 @@
         <v>226</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>43965</v>
+        <v>43966</v>
       </c>
       <c r="D32" t="s">
         <v>227</v>
@@ -4083,31 +4096,31 @@
       </c>
       <c r="F32"/>
       <c r="G32" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H32" t="n">
-        <v>56178</v>
+        <v>56701</v>
       </c>
       <c r="I32" t="n">
-        <v>164.624</v>
+        <v>166.157</v>
       </c>
       <c r="J32" t="n">
-        <v>593</v>
+        <v>523</v>
       </c>
       <c r="K32" t="n">
-        <v>1.738</v>
+        <v>1.533</v>
       </c>
       <c r="L32" t="n">
-        <v>476</v>
+        <v>555.667</v>
       </c>
       <c r="M32" t="n">
-        <v>1.395</v>
+        <v>1.629</v>
       </c>
       <c r="N32" t="n">
-        <v>496.286</v>
+        <v>497.429</v>
       </c>
       <c r="O32" t="n">
-        <v>1.454</v>
+        <v>1.458</v>
       </c>
       <c r="P32" t="s">
         <v>228</v>
@@ -4297,7 +4310,7 @@
         <v>245</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D36" t="s">
         <v>246</v>
@@ -4307,25 +4320,25 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H36" t="n">
-        <v>658604</v>
+        <v>672679</v>
       </c>
       <c r="I36" t="n">
-        <v>7.841</v>
+        <v>8.009</v>
       </c>
       <c r="J36" t="n">
-        <v>14832</v>
+        <v>14075</v>
       </c>
       <c r="K36" t="n">
-        <v>0.177</v>
+        <v>0.168</v>
       </c>
       <c r="L36" t="n">
-        <v>14375.667</v>
+        <v>14381.667</v>
       </c>
       <c r="M36" t="n">
-        <v>0.171</v>
+        <v>0.172</v>
       </c>
       <c r="N36"/>
       <c r="O36"/>
@@ -4454,7 +4467,7 @@
         <v>264</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D39" t="s">
         <v>265</v>
@@ -4466,31 +4479,31 @@
         <v>267</v>
       </c>
       <c r="G39" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H39" t="n">
-        <v>1859110</v>
+        <v>1899767</v>
       </c>
       <c r="I39" t="n">
-        <v>30.748</v>
+        <v>31.421</v>
       </c>
       <c r="J39" t="n">
-        <v>39027</v>
+        <v>40657</v>
       </c>
       <c r="K39" t="n">
-        <v>0.645</v>
+        <v>0.672</v>
       </c>
       <c r="L39" t="n">
-        <v>39069</v>
+        <v>40271.667</v>
       </c>
       <c r="M39" t="n">
-        <v>0.646</v>
+        <v>0.666</v>
       </c>
       <c r="N39" t="n">
-        <v>35732.143</v>
+        <v>36384.429</v>
       </c>
       <c r="O39" t="n">
-        <v>0.591</v>
+        <v>0.602</v>
       </c>
       <c r="P39" t="s">
         <v>268</v>
@@ -4513,7 +4526,7 @@
         <v>271</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D40" t="s">
         <v>265</v>
@@ -4525,28 +4538,28 @@
         <v>267</v>
       </c>
       <c r="G40" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H40" t="n">
-        <v>2875680</v>
+        <v>2944859</v>
       </c>
       <c r="I40" t="n">
-        <v>47.562</v>
+        <v>48.706</v>
       </c>
       <c r="J40" t="n">
-        <v>68176</v>
+        <v>69179</v>
       </c>
       <c r="K40" t="n">
-        <v>1.128</v>
+        <v>1.144</v>
       </c>
       <c r="L40" t="n">
-        <v>67341.667</v>
+        <v>69743.667</v>
       </c>
       <c r="M40" t="n">
-        <v>1.114</v>
+        <v>1.154</v>
       </c>
       <c r="N40" t="n">
-        <v>61516.714</v>
+        <v>61517.857</v>
       </c>
       <c r="O40" t="n">
         <v>1.018</v>
@@ -4572,7 +4585,7 @@
         <v>274</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D41" t="s">
         <v>275</v>
@@ -4584,13 +4597,13 @@
         <v>277</v>
       </c>
       <c r="G41" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H41" t="n">
-        <v>230882</v>
+        <v>240368</v>
       </c>
       <c r="I41" t="n">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="J41"/>
       <c r="K41"/>
@@ -4619,7 +4632,7 @@
         <v>280</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>43964</v>
+        <v>43965</v>
       </c>
       <c r="D42" t="s">
         <v>281</v>
@@ -4631,31 +4644,31 @@
         <v>282</v>
       </c>
       <c r="G42" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H42" t="n">
-        <v>357626</v>
+        <v>365074</v>
       </c>
       <c r="I42" t="n">
-        <v>2.828</v>
+        <v>2.886</v>
       </c>
       <c r="J42" t="n">
-        <v>8190</v>
+        <v>6745</v>
       </c>
       <c r="K42" t="n">
-        <v>0.065</v>
+        <v>0.053</v>
       </c>
       <c r="L42" t="n">
-        <v>7755.333</v>
+        <v>7761</v>
       </c>
       <c r="M42" t="n">
         <v>0.061</v>
       </c>
       <c r="N42" t="n">
-        <v>7078.857</v>
+        <v>6999</v>
       </c>
       <c r="O42" t="n">
-        <v>0.056</v>
+        <v>0.055</v>
       </c>
       <c r="P42" t="s">
         <v>276</v>
@@ -4678,7 +4691,7 @@
         <v>285</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D43" t="s">
         <v>286</v>
@@ -4688,31 +4701,31 @@
       </c>
       <c r="F43"/>
       <c r="G43" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H43" t="n">
-        <v>483236</v>
+        <v>505216</v>
       </c>
       <c r="I43" t="n">
-        <v>25.736</v>
+        <v>26.907</v>
       </c>
       <c r="J43" t="n">
-        <v>23500</v>
+        <v>21980</v>
       </c>
       <c r="K43" t="n">
-        <v>1.252</v>
+        <v>1.171</v>
       </c>
       <c r="L43" t="n">
-        <v>20408.333</v>
+        <v>21907</v>
       </c>
       <c r="M43" t="n">
-        <v>1.087</v>
+        <v>1.167</v>
       </c>
       <c r="N43" t="n">
-        <v>16015.714</v>
+        <v>17158.857</v>
       </c>
       <c r="O43" t="n">
-        <v>0.853</v>
+        <v>0.914</v>
       </c>
       <c r="P43" t="s">
         <v>287</v>
@@ -4908,7 +4921,7 @@
         <v>308</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D47" t="s">
         <v>309</v>
@@ -4918,31 +4931,25 @@
       </c>
       <c r="F47"/>
       <c r="G47" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H47" t="n">
-        <v>59987</v>
+        <v>60246</v>
       </c>
       <c r="I47" t="n">
-        <v>95.83</v>
-      </c>
-      <c r="J47" t="n">
-        <v>1260</v>
-      </c>
+        <v>96.243</v>
+      </c>
+      <c r="J47"/>
       <c r="K47" t="n">
-        <v>2.013</v>
-      </c>
-      <c r="L47" t="n">
-        <v>1197.667</v>
-      </c>
+        <v>0.414</v>
+      </c>
+      <c r="L47"/>
       <c r="M47" t="n">
-        <v>1.913</v>
-      </c>
-      <c r="N47" t="n">
-        <v>961.429</v>
-      </c>
+        <v>1.363</v>
+      </c>
+      <c r="N47"/>
       <c r="O47" t="n">
-        <v>1.536</v>
+        <v>1.32</v>
       </c>
       <c r="P47" t="s">
         <v>310</v>
@@ -5120,7 +5127,7 @@
         <v>333</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>43965</v>
+        <v>43967</v>
       </c>
       <c r="D51" t="s">
         <v>334</v>
@@ -5128,65 +5135,55 @@
       <c r="E51" t="s">
         <v>335</v>
       </c>
-      <c r="F51"/>
+      <c r="F51" t="s">
+        <v>336</v>
+      </c>
       <c r="G51" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H51" t="n">
-        <v>12995</v>
+        <v>13634</v>
       </c>
       <c r="I51" t="n">
-        <v>0.239</v>
-      </c>
-      <c r="J51" t="n">
-        <v>513</v>
-      </c>
-      <c r="K51" t="n">
-        <v>0.009</v>
-      </c>
-      <c r="L51" t="n">
-        <v>391</v>
-      </c>
-      <c r="M51" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="N51" t="n">
-        <v>389.857</v>
-      </c>
-      <c r="O51" t="n">
-        <v>0.007</v>
-      </c>
+        <v>0.251</v>
+      </c>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+      <c r="O51"/>
       <c r="P51" t="s">
         <v>335</v>
       </c>
       <c r="Q51" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="R51" t="s">
         <v>53</v>
       </c>
       <c r="S51" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B52" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="D52" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E52" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="F52" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G52" t="n">
         <v>85</v>
@@ -5216,33 +5213,33 @@
         <v>0.041</v>
       </c>
       <c r="P52" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="Q52" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="R52" t="s">
         <v>94</v>
       </c>
       <c r="S52" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B53" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>43965</v>
       </c>
       <c r="D53" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E53" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
@@ -5269,30 +5266,30 @@
       <c r="N53"/>
       <c r="O53"/>
       <c r="P53" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="Q53" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="R53" t="s">
         <v>94</v>
       </c>
       <c r="S53" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B54" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="D54" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E54" t="s">
         <v>43</v>
@@ -5326,33 +5323,33 @@
         <v>1.212</v>
       </c>
       <c r="P54" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q54" t="s">
         <v>355</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>354</v>
       </c>
       <c r="R54" t="s">
         <v>24</v>
       </c>
       <c r="S54" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B55" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>43967</v>
       </c>
       <c r="D55" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E55" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
@@ -5371,33 +5368,33 @@
       <c r="N55"/>
       <c r="O55"/>
       <c r="P55" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="Q55" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="R55" t="s">
         <v>53</v>
       </c>
       <c r="S55" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B56" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="D56" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E56" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
@@ -5424,33 +5421,33 @@
       <c r="N56"/>
       <c r="O56"/>
       <c r="P56" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="Q56" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="R56" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="S56" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B57" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>43967</v>
       </c>
       <c r="D57" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E57" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
@@ -5481,36 +5478,36 @@
         <v>0.058</v>
       </c>
       <c r="P57" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="Q57" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="R57" t="s">
         <v>24</v>
       </c>
       <c r="S57" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B58" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="D58" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="E58" t="s">
         <v>43</v>
       </c>
       <c r="F58" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="G58" t="n">
         <v>68</v>
@@ -5543,33 +5540,33 @@
         <v>43</v>
       </c>
       <c r="Q58" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="R58" t="s">
         <v>128</v>
       </c>
       <c r="S58" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B59" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>43960</v>
       </c>
       <c r="D59" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E59" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="F59" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="G59" t="n">
         <v>62</v>
@@ -5599,81 +5596,85 @@
         <v>0.078</v>
       </c>
       <c r="P59" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="Q59" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="R59" t="s">
         <v>53</v>
       </c>
       <c r="S59" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B60" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D60" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E60" t="s">
         <v>43</v>
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H60" t="n">
-        <v>605383</v>
+        <v>630482</v>
       </c>
       <c r="I60" t="n">
-        <v>18.361</v>
-      </c>
-      <c r="J60"/>
-      <c r="K60"/>
+        <v>19.122</v>
+      </c>
+      <c r="J60" t="n">
+        <v>25099</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0.761</v>
+      </c>
       <c r="L60"/>
       <c r="M60"/>
       <c r="N60"/>
       <c r="O60"/>
       <c r="P60" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="Q60" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="R60" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="S60" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B61" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>43964</v>
       </c>
       <c r="D61" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E61" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F61" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="G61" t="n">
         <v>23</v>
@@ -5698,33 +5699,33 @@
         <v>213</v>
       </c>
       <c r="Q61" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="R61" t="s">
         <v>94</v>
       </c>
       <c r="S61" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B62" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="D62" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E62" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="F62" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="G62" t="n">
         <v>72</v>
@@ -5754,30 +5755,30 @@
         <v>0.501</v>
       </c>
       <c r="P62" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="Q62" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="R62" t="s">
         <v>53</v>
       </c>
       <c r="S62" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B63" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>43964</v>
       </c>
       <c r="D63" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E63" t="s">
         <v>43</v>
@@ -5811,33 +5812,33 @@
         <v>1.376</v>
       </c>
       <c r="P63" t="s">
+        <v>415</v>
+      </c>
+      <c r="Q63" t="s">
         <v>414</v>
       </c>
-      <c r="Q63" t="s">
-        <v>413</v>
-      </c>
       <c r="R63" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="S63" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B64" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>43967</v>
       </c>
       <c r="D64" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E64" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="F64"/>
       <c r="G64" t="n">
@@ -5868,36 +5869,36 @@
         <v>1.396</v>
       </c>
       <c r="P64" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="Q64" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="R64" t="s">
         <v>94</v>
       </c>
       <c r="S64" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B65" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>43965</v>
       </c>
       <c r="D65" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E65" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="F65" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="G65" t="n">
         <v>64</v>
@@ -5927,33 +5928,33 @@
         <v>0.442</v>
       </c>
       <c r="P65" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q65" t="s">
         <v>426</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>425</v>
       </c>
       <c r="R65" t="s">
         <v>24</v>
       </c>
       <c r="S65" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B66" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>43967</v>
       </c>
       <c r="D66" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E66" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
@@ -5984,150 +5985,150 @@
         <v>1.404</v>
       </c>
       <c r="P66" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="Q66" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R66" t="s">
         <v>24</v>
       </c>
       <c r="S66" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B67" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D67" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="E67" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H67" t="n">
-        <v>46198</v>
+        <v>48239</v>
       </c>
       <c r="I67" t="n">
-        <v>3.567</v>
+        <v>3.724</v>
       </c>
       <c r="J67" t="n">
-        <v>1058</v>
+        <v>2041</v>
       </c>
       <c r="K67" t="n">
-        <v>0.082</v>
+        <v>0.158</v>
       </c>
       <c r="L67" t="n">
-        <v>939.667</v>
+        <v>1331.333</v>
       </c>
       <c r="M67" t="n">
-        <v>0.073</v>
+        <v>0.103</v>
       </c>
       <c r="N67" t="n">
-        <v>858.714</v>
+        <v>979.143</v>
       </c>
       <c r="O67" t="n">
-        <v>0.066</v>
+        <v>0.076</v>
       </c>
       <c r="P67" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="Q67" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="R67" t="s">
         <v>53</v>
       </c>
       <c r="S67" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B68" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D68" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E68" t="s">
         <v>43</v>
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H68" t="n">
-        <v>530265</v>
+        <v>548023</v>
       </c>
       <c r="I68" t="n">
-        <v>15.231</v>
+        <v>15.742</v>
       </c>
       <c r="J68" t="n">
-        <v>16678</v>
+        <v>17758</v>
       </c>
       <c r="K68" t="n">
-        <v>0.479</v>
+        <v>0.51</v>
       </c>
       <c r="L68" t="n">
-        <v>15963.667</v>
+        <v>17025</v>
       </c>
       <c r="M68" t="n">
-        <v>0.459</v>
+        <v>0.489</v>
       </c>
       <c r="N68" t="n">
-        <v>15934.714</v>
+        <v>16360.429</v>
       </c>
       <c r="O68" t="n">
-        <v>0.458</v>
+        <v>0.47</v>
       </c>
       <c r="P68" t="s">
         <v>43</v>
       </c>
       <c r="Q68" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="R68" t="s">
         <v>128</v>
       </c>
       <c r="S68" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B69" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C69" s="1" t="n">
         <v>43967</v>
       </c>
       <c r="D69" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E69" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F69" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="G69" t="n">
         <v>75</v>
@@ -6157,89 +6158,89 @@
         <v>0.063</v>
       </c>
       <c r="P69" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="Q69" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="R69" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="S69" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B70" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D70" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="E70" t="s">
         <v>43</v>
       </c>
       <c r="F70" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="G70" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H70" t="n">
-        <v>168670</v>
+        <v>174746</v>
       </c>
       <c r="I70" t="n">
-        <v>24.788</v>
+        <v>25.681</v>
       </c>
       <c r="J70" t="n">
-        <v>5873</v>
+        <v>6076</v>
       </c>
       <c r="K70" t="n">
-        <v>0.863</v>
+        <v>0.893</v>
       </c>
       <c r="L70" t="n">
-        <v>5788.667</v>
+        <v>6047.667</v>
       </c>
       <c r="M70" t="n">
-        <v>0.851</v>
+        <v>0.889</v>
       </c>
       <c r="N70" t="n">
-        <v>5695</v>
+        <v>5744.714</v>
       </c>
       <c r="O70" t="n">
-        <v>0.837</v>
+        <v>0.844</v>
       </c>
       <c r="P70" t="s">
         <v>43</v>
       </c>
       <c r="Q70" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="R70" t="s">
         <v>94</v>
       </c>
       <c r="S70" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B71" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C71" s="1" t="n">
         <v>43961</v>
       </c>
       <c r="D71" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E71" t="s">
         <v>43</v>
@@ -6264,27 +6265,27 @@
         <v>43</v>
       </c>
       <c r="Q71" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="R71" t="s">
         <v>94</v>
       </c>
       <c r="S71" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B72" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>43961</v>
       </c>
       <c r="D72" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E72" t="s">
         <v>43</v>
@@ -6309,30 +6310,30 @@
         <v>43</v>
       </c>
       <c r="Q72" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="R72" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="S72" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B73" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>43967</v>
       </c>
       <c r="D73" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E73" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
@@ -6363,33 +6364,33 @@
         <v>0.566</v>
       </c>
       <c r="P73" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="Q73" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="R73" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="S73" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B74" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="D74" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="E74" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
@@ -6420,36 +6421,36 @@
         <v>0.457</v>
       </c>
       <c r="P74" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="Q74" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="R74" t="s">
         <v>24</v>
       </c>
       <c r="S74" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B75" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="D75" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="E75" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="F75" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="G75" t="n">
         <v>76</v>
@@ -6479,33 +6480,33 @@
         <v>0.274</v>
       </c>
       <c r="P75" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="Q75" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="R75" t="s">
         <v>94</v>
       </c>
       <c r="S75" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B76" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>43967</v>
       </c>
       <c r="D76" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="E76" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
@@ -6536,33 +6537,33 @@
         <v>0.225</v>
       </c>
       <c r="P76" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="Q76" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="R76" t="s">
         <v>73</v>
       </c>
       <c r="S76" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B77" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>43965</v>
       </c>
       <c r="D77" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E77" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
@@ -6581,33 +6582,33 @@
       <c r="N77"/>
       <c r="O77"/>
       <c r="P77" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="Q77" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="R77" t="s">
         <v>24</v>
       </c>
       <c r="S77" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B78" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>43961</v>
       </c>
       <c r="D78" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="E78" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
@@ -6626,90 +6627,90 @@
       <c r="N78"/>
       <c r="O78"/>
       <c r="P78" t="s">
+        <v>507</v>
+      </c>
+      <c r="Q78" t="s">
         <v>506</v>
-      </c>
-      <c r="Q78" t="s">
-        <v>505</v>
       </c>
       <c r="R78" t="s">
         <v>94</v>
       </c>
       <c r="S78" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B79" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="D79" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E79" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
         <v>109</v>
       </c>
       <c r="H79" t="n">
-        <v>339394</v>
+        <v>339347</v>
       </c>
       <c r="I79" t="n">
-        <v>39.215</v>
+        <v>39.21</v>
       </c>
       <c r="J79" t="n">
-        <v>3210</v>
+        <v>3163</v>
       </c>
       <c r="K79" t="n">
-        <v>0.371</v>
+        <v>0.365</v>
       </c>
       <c r="L79" t="n">
-        <v>4785</v>
+        <v>4769.333</v>
       </c>
       <c r="M79" t="n">
-        <v>0.553</v>
+        <v>0.551</v>
       </c>
       <c r="N79" t="n">
-        <v>4224.286</v>
+        <v>4217.571</v>
       </c>
       <c r="O79" t="n">
-        <v>0.488</v>
+        <v>0.487</v>
       </c>
       <c r="P79" t="s">
+        <v>512</v>
+      </c>
+      <c r="Q79" t="s">
         <v>511</v>
       </c>
-      <c r="Q79" t="s">
-        <v>510</v>
-      </c>
       <c r="R79" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="S79" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B80" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="D80" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E80" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
@@ -6740,82 +6741,86 @@
         <v>0.013</v>
       </c>
       <c r="P80" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="Q80" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="R80" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="S80" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B81" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>43967</v>
+        <v>43968</v>
       </c>
       <c r="D81" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="E81" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H81" t="n">
-        <v>118274</v>
+        <v>120659</v>
       </c>
       <c r="I81" t="n">
-        <v>1.694</v>
-      </c>
-      <c r="J81"/>
+        <v>1.729</v>
+      </c>
+      <c r="J81" t="n">
+        <v>2385</v>
+      </c>
       <c r="K81" t="n">
-        <v>0.003</v>
-      </c>
-      <c r="L81"/>
+        <v>0.034</v>
+      </c>
+      <c r="L81" t="n">
+        <v>2084.667</v>
+      </c>
       <c r="M81" t="n">
-        <v>0.033</v>
+        <v>0.03</v>
       </c>
       <c r="N81"/>
       <c r="O81"/>
       <c r="P81" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="Q81" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="R81" t="s">
         <v>94</v>
       </c>
       <c r="S81" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B82" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>43959</v>
       </c>
       <c r="D82" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="E82" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
@@ -6834,33 +6839,33 @@
       <c r="N82"/>
       <c r="O82"/>
       <c r="P82" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="Q82" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="R82" t="s">
         <v>53</v>
       </c>
       <c r="S82" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B83" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C83" s="1" t="n">
         <v>43965</v>
       </c>
       <c r="D83" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E83" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
@@ -6891,149 +6896,149 @@
         <v>0.126</v>
       </c>
       <c r="P83" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="Q83" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="R83" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="S83" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B84" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D84" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E84" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H84" t="n">
-        <v>1547389</v>
+        <v>1589625</v>
       </c>
       <c r="I84" t="n">
-        <v>18.347</v>
+        <v>18.848</v>
       </c>
       <c r="J84" t="n">
-        <v>38565</v>
+        <v>42236</v>
       </c>
       <c r="K84" t="n">
+        <v>0.501</v>
+      </c>
+      <c r="L84" t="n">
+        <v>38540.667</v>
+      </c>
+      <c r="M84" t="n">
         <v>0.457</v>
       </c>
-      <c r="L84" t="n">
-        <v>35572.667</v>
-      </c>
-      <c r="M84" t="n">
-        <v>0.422</v>
-      </c>
       <c r="N84" t="n">
-        <v>35511.857</v>
+        <v>36459.143</v>
       </c>
       <c r="O84" t="n">
-        <v>0.421</v>
+        <v>0.432</v>
       </c>
       <c r="P84" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="Q84" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="R84" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="S84" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B85" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>43965</v>
+        <v>43966</v>
       </c>
       <c r="D85" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="E85" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="F85" t="s">
+        <v>552</v>
+      </c>
+      <c r="G85" t="n">
+        <v>39</v>
+      </c>
+      <c r="H85" t="n">
+        <v>70730</v>
+      </c>
+      <c r="I85" t="n">
+        <v>1.546</v>
+      </c>
+      <c r="J85" t="n">
+        <v>2558</v>
+      </c>
+      <c r="K85" t="n">
+        <v>0.056</v>
+      </c>
+      <c r="L85" t="n">
+        <v>2186</v>
+      </c>
+      <c r="M85" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="N85" t="n">
+        <v>2218.143</v>
+      </c>
+      <c r="O85" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="P85" t="s">
         <v>551</v>
       </c>
-      <c r="G85" t="n">
-        <v>38</v>
-      </c>
-      <c r="H85" t="n">
-        <v>68172</v>
-      </c>
-      <c r="I85" t="n">
-        <v>1.49</v>
-      </c>
-      <c r="J85" t="n">
-        <v>1896</v>
-      </c>
-      <c r="K85" t="n">
-        <v>0.041</v>
-      </c>
-      <c r="L85" t="n">
-        <v>1903.667</v>
-      </c>
-      <c r="M85" t="n">
-        <v>0.041</v>
-      </c>
-      <c r="N85" t="n">
-        <v>2304.286</v>
-      </c>
-      <c r="O85" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="P85" t="s">
-        <v>550</v>
-      </c>
       <c r="Q85" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="R85" t="s">
         <v>53</v>
       </c>
       <c r="S85" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B86" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C86" s="1" t="n">
         <v>43967</v>
       </c>
       <c r="D86" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="E86" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
@@ -7064,151 +7069,151 @@
         <v>0.175</v>
       </c>
       <c r="P86" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="Q86" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="R86" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="S86" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B87" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D87" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="E87" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="F87"/>
       <c r="G87" t="n">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H87" t="n">
-        <v>1663492</v>
+        <v>1742028</v>
       </c>
       <c r="I87" t="n">
-        <v>24.504</v>
+        <v>25.661</v>
       </c>
       <c r="J87" t="n">
-        <v>69590</v>
+        <v>78537</v>
       </c>
       <c r="K87" t="n">
-        <v>1.025</v>
+        <v>1.157</v>
       </c>
       <c r="L87" t="n">
-        <v>67658.333</v>
+        <v>73257</v>
       </c>
       <c r="M87" t="n">
-        <v>0.996</v>
+        <v>1.079</v>
       </c>
       <c r="N87" t="n">
-        <v>65203.286</v>
+        <v>67374.429</v>
       </c>
       <c r="O87" t="n">
-        <v>0.96</v>
+        <v>0.992</v>
       </c>
       <c r="P87" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="Q87" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="R87" t="s">
         <v>94</v>
       </c>
       <c r="S87" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B88" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D88" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="E88" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H88" t="n">
-        <v>2353078</v>
+        <v>2489563</v>
       </c>
       <c r="I88" t="n">
-        <v>34.662</v>
+        <v>36.673</v>
       </c>
       <c r="J88" t="n">
-        <v>133784</v>
+        <v>136486</v>
       </c>
       <c r="K88" t="n">
-        <v>1.971</v>
+        <v>2.011</v>
       </c>
       <c r="L88" t="n">
-        <v>115637</v>
+        <v>132111.333</v>
       </c>
       <c r="M88" t="n">
-        <v>1.703</v>
+        <v>1.946</v>
       </c>
       <c r="N88" t="n">
-        <v>103201.286</v>
+        <v>108859.571</v>
       </c>
       <c r="O88" t="n">
-        <v>1.52</v>
+        <v>1.604</v>
       </c>
       <c r="P88" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="Q88" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="R88" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="S88" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B89" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D89" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="E89" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H89" t="n">
         <v>10720185</v>
@@ -7216,52 +7221,46 @@
       <c r="I89" t="n">
         <v>32.387</v>
       </c>
-      <c r="J89" t="n">
-        <v>378410</v>
-      </c>
+      <c r="J89"/>
       <c r="K89" t="n">
-        <v>1.143</v>
-      </c>
-      <c r="L89" t="n">
-        <v>356593.333</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L89"/>
       <c r="M89" t="n">
-        <v>1.077</v>
-      </c>
-      <c r="N89" t="n">
-        <v>332882.714</v>
-      </c>
+        <v>0.751</v>
+      </c>
+      <c r="N89"/>
       <c r="O89" t="n">
-        <v>1.006</v>
+        <v>0.878</v>
       </c>
       <c r="P89" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="Q89" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="R89" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="S89" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B90" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>43964</v>
       </c>
       <c r="D90" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="E90" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
@@ -7284,30 +7283,30 @@
       <c r="N90"/>
       <c r="O90"/>
       <c r="P90" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="Q90" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="R90" t="s">
         <v>24</v>
       </c>
       <c r="S90" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B91" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C91" s="1" t="n">
         <v>43967</v>
       </c>
       <c r="D91" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="E91" t="s">
         <v>126</v>
@@ -7340,30 +7339,30 @@
         <v>126</v>
       </c>
       <c r="Q91" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="R91" t="s">
         <v>24</v>
       </c>
       <c r="S91" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B92" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="C92" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="D92" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="E92" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
@@ -7382,36 +7381,36 @@
       <c r="N92"/>
       <c r="O92"/>
       <c r="P92" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="Q92" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="R92" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="S92" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B93" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C93" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="D93" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="E93" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="F93" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="G93" t="n">
         <v>9</v>
@@ -7429,16 +7428,16 @@
       <c r="N93"/>
       <c r="O93"/>
       <c r="P93" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="Q93" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="R93" t="s">
         <v>24</v>
       </c>
       <c r="S93" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testing data for 2020-05-19
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="600">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -92,7 +92,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/05/coronavirus-covid-19-at-a-glance-coronavirus-covid-19-at-a-glance-infographic_16.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/05/coronavirus-covid-19-at-a-glance-19-may-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200518181646/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200519110842/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200518181650/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200519110846/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -255,10 +255,7 @@
     <t xml:space="preserve">Brazil - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.saude.gov.br/noticias/agencia-saude/46768-chega-ao-pais-mais-500-mil-testes-de-biologia-molecular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ministry of Health press release</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200519195204/https://covid-insumos.saude.gov.br/paineis/insumos/painel.php</t>
   </si>
   <si>
     <t xml:space="preserve">Brazil Ministry of Health</t>
@@ -267,7 +264,8 @@
     <t xml:space="preserve">https://www.saude.gov.br/noticias/agencia-saude</t>
   </si>
   <si>
-    <t xml:space="preserve">The Ministry of Health press releases published on its website intermittently include figures for the number of tests carried out for a range of respiratory infections, further specifying the figures carried out for the 'specific investigation of COVID-19'. The releases note that 'Tests for coronavirus began to be carried out from February 16 in public and private laboratories'.</t>
+    <t xml:space="preserve">The Ministry of Health press releases published on its website intermittently include figures for the number of tests carried out for a range of respiratory infections, further specifying the figures carried out for the 'specific investigation of COVID-19'. The releases note that 'Tests for coronavirus began to be carried out from February 16 in public and private laboratories'.
+From 6th April, the Ministry of Health intermittently reports the number of PCR and rapid tests separately on its [Panel of beds and inputs](https://covid-insumos.saude.gov.br/paineis/insumos/painel.php) webpage.</t>
   </si>
   <si>
     <t xml:space="preserve">BGR</t>
@@ -276,7 +274,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200517110936/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200519110851/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -299,7 +297,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200518181658/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200519190529/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -387,7 +385,7 @@
     <t xml:space="preserve">Croatia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200518181704/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200519190537/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -447,7 +445,7 @@
     <t xml:space="preserve">Denmark - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/COVID19-overvaagningsrapport-17052020-2-01ui</t>
+    <t xml:space="preserve">https://files.ssi.dk/COVID19-overvaagningsrapport-19052020-d2l8</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -477,7 +475,7 @@
     <t xml:space="preserve">Ecuador - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/05/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-16052020-08h00.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/05/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-19052020-08h00.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -510,7 +508,7 @@
     <t xml:space="preserve">Government of El Salvador</t>
   </si>
   <si>
-    <t xml:space="preserve">updated at 12:48am local time on 2020-05-18.</t>
+    <t xml:space="preserve">updated at 12:43am local time on 2020-05-19.</t>
   </si>
   <si>
     <t xml:space="preserve">The government of El Salvador publishes an online dashboard with figures and graphs about the epidemic, including the number of tests performed ("pruebas COVID19 realizadas hasta hoy"). No information is given on the geographical scope and number of labs included.</t>
@@ -547,7 +545,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_May-18-Eng-V3.pdf</t>
+    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_May-19-Eng-V1.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -686,7 +684,7 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200518/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200519/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -821,7 +819,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200518152946/http://irangov.ir/detail/339482</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200519130712/http://irangov.ir/detail/339563</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -840,7 +838,7 @@
     <t xml:space="preserve">Ireland - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gov.ie/en/press-release/bc6c86-statement-from-the-national-public-health-emergency-team-tuesday-12-/</t>
+    <t xml:space="preserve">https://www.gov.ie/en/press-release/41d42e-statement-from-the-national-public-health-emergency-team-tuesday-19-/</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gov.ie/en/publications/?&amp;type=press-releases&amp;organisation=department-of-health</t>
@@ -920,28 +918,31 @@
     <t xml:space="preserve">Japan - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://github.com/reustle/covid19japan-data</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11399.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
   </si>
   <si>
-    <t xml:space="preserve">Made available by Shane Reustle on Github</t>
+    <t xml:space="preserve">See Table: 国内の発生状況, column 1 '検査実施人数'. Daily change figure provided for this date is not consistent with the cumulative totals for today and the previous day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ministry of Health, Labor and Welfare</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.mhlw.go.jp/stf/houdou/houdou_list_202004.html</t>
   </si>
   <si>
-    <t xml:space="preserve">The Ministry of Health, Labor and Welfare issues daily reports for the total number of people tested. These are collated by a volunteer group on [GitHub](https://github.com/reustle/covid19japan-data/). We take our figures from this group, and regularly audit it for accuracy. Daily changes in the number of people tested are included in parentheses. For the 3rd April, the daily changes do not reconcile with the cumulative totals. Moreover, it is clear that revisions to past data are simply added to the new cumulative total, making the time series of 'daily tests' too erratic to be published.
+    <t xml:space="preserve">The Ministry of Health, Labor and Welfare issues daily reports for the total number of people tested. Daily changes in the number of people tested are included in parentheses. For the 3rd and 21st April, the daily changes do not reconcile with the cumulative totals. Moreover, it is clear that revisions to past data are simply added to the new cumulative total, making the time series of 'daily tests' too erratic to be published.
 This includes two cases where the cumulative number of people tested falls: (1) 19/03 and (2) 25/03. For case (1) see footnote 4 which indicates a past mistake has been noticed and the cumulative figure revised on the date to adjust for this. For case (2), we could not find the associated footnote.
 It isn't clear what exact date these cumulative tests date back to, but it is earlier than 10 Feb when the source reports 938 people had been tested. Prior to the 10 Feb, the press releases provide reports of coronavirus infections for the Diamond Princess cruise ship quarantined in Yokohama port. We do not report these numbers in the time series as it is unclear how they relate to the cumulative totals.
-Google Translate was used while compiling this data so this may affect our interpretation of the data.</t>
+Google translate was used while compiling this data so this may affect our interpretation of the data.</t>
   </si>
   <si>
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000631066.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000631873.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Implementation status of PCR tests for new coronavirus in Japan (based on the date on which the results were determined). Preliminary data</t>
@@ -975,7 +976,7 @@
     <t xml:space="preserve">Kenya - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1262367522122354689</t>
+    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1262726647104581632</t>
   </si>
   <si>
     <t xml:space="preserve">Kenya Ministry of Health</t>
@@ -1016,7 +1017,7 @@
     <t xml:space="preserve">Lithuania - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200517111053/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200519190643/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -1032,7 +1033,7 @@
     <t xml:space="preserve">Luxembourg - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200517200217/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200519190646/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg Government situation update</t>
@@ -1106,10 +1107,8 @@
     <t xml:space="preserve">https://www.sante.gov.ma/Pages/Accueil.aspx</t>
   </si>
   <si>
-    <t xml:space="preserve">The Morocco Ministry of Health provides daily updates of the total number of confirmed cases and the number of cases dismissed following a negative test result. We construct a time series of the cumulative number of cases tested to date using the data stored in [this unofficial GitHub repository](https://github.com/RedaElmar/COVID-19_Morocco). 
-The cumulative number of cases tested to date includes positive and negative test results, while excluding pending results. We have cross-checked a sample of the figures reported in the unofficial source against data reported on the Ministry of Health website.
-The earliest reported figure is from March 2nd 2020, at which point 29 cases had been tested. It is unclear whether March 2nd was the first date on which tests were conducted.
-Since 1 May 2020, the [government website dedicated to COVID-19](http://www.covidmaroc.ma/Pages/AccueilAR.aspx) has been down, making it impossible to update our time series.</t>
+    <t xml:space="preserve">The Morocco Ministry of Health provides daily updates of the total number of confirmed cases and the number of cases dismissed following a negative test result. We construct a time series of the cumulative number of cases tested to date using the data stored in [this unofficial GitHub repository](https://github.com/RedaElmar/COVID-19_Morocco), supplemented by official updates from the Ministry of Health's twitter page ([@Ministere_Sante](https://twitter.com/Ministere_Sante)). We have cross-checked a sample of the figures reported in the unofficial source against official data reported by the Ministry of Health.
+The cumulative number of cases tested to date includes positive and negative test results, while excluding pending results. The earliest reported figure is from February 7th 2020, at which point 9 cases had been tested.</t>
   </si>
   <si>
     <t xml:space="preserve">MMR</t>
@@ -1163,10 +1162,10 @@
     <t xml:space="preserve">Netherlands - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-05/COVID-19_WebSite_rapport_20200518_1121_0.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 18 May 2020 update</t>
+    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-05/COVID-19_WebSite_rapport_20200519_1015_0.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 19 May 2020 update</t>
   </si>
   <si>
     <t xml:space="preserve">Dutch National Institute for Public Health and the Environment</t>
@@ -1202,7 +1201,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200518182025/https://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200519190830/https://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1222,7 +1221,7 @@
     <t xml:space="preserve">Norway - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.05.18-dagsrapport-norge-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.05.19-dagsrapport-norge-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Norwegian Institute of Public Health</t>
@@ -1247,7 +1246,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200518182030/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200519190834/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1313,7 +1312,7 @@
     <t xml:space="preserve">Peru - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/157471-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-92-273-en-el-peru-comunicado-n-103</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/157559-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-99-483-en-el-peru-comunicado-n-105</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1349,7 +1348,7 @@
 The total number of individuals tested is the sum of positive, negative, equivocal, and invalid individuals. No definitions of equivocal and invalid individual tests are given, hence our figures only report the sum of individuals who have tested positive or negative.
 The source provides a breakdown of both i) the number of individuals tested and ii) the total tests conducted, by laboratory. We are not aware of any aggregation issues. 
 The DOH used to report the number of cases tested in a previous dashboard, but stopped on 4th April. This previous breakdown of the test results and COVID-19 dashboard have both been removed. We became aware of this new tracker on the 13th April with data 'as of April 11 2020, 12am'. No previous snapshots of the dashboard are available using web archive, therefore the series starts from the 11th April - the earliest date from which we have access to the data. 
-No newly submitted reports as of 16 May. Latest testing data available is from 13 May 2020.</t>
+No newly submitted reports as of 18 May. Latest testing data available is from 15 May 2020.</t>
   </si>
   <si>
     <t xml:space="preserve">POL</t>
@@ -1358,7 +1357,7 @@
     <t xml:space="preserve">Poland - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://raw.githubusercontent.com/anuszka/COVID-19-MZ_GOV_PL/master/data/cor.2020.05.18.csv</t>
+    <t xml:space="preserve">https://raw.githubusercontent.com/anuszka/COVID-19-MZ_GOV_PL/master/data/cor.2020.05.19.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1403,7 +1402,7 @@
     <t xml:space="preserve">Qatar - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200518181638/https://www.moph.gov.qa/english/Pages/Coronavirus2019.aspx</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200519194531/https://covid19.moph.gov.qa/EN/Pages/default.aspx</t>
   </si>
   <si>
     <t xml:space="preserve">Qatar Ministry of Public Health</t>
@@ -1441,7 +1440,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14479</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14485</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1461,7 +1460,7 @@
     <t xml:space="preserve">Rwanda - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1262071900089528321</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1262441408436285441</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1568,7 +1567,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200517111139/https://korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200519191802/https://korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Center of Health Information and the Office of the Government of the Slovak Republic</t>
@@ -1642,7 +1641,7 @@
     <t xml:space="preserve">South Korea - cases tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367251&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367264&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1725,7 +1724,7 @@
     <t xml:space="preserve">Taiwan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/SXUKk3KipAb5AEMNSwR12w?typeid=9</t>
+    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/c4rwvT--ae8c0wKIWPyTjQ?typeid=9</t>
   </si>
   <si>
     <t xml:space="preserve">Taiwan Centers for Disease Control (CDC)</t>
@@ -1815,7 +1814,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200518182138/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200519191908/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1839,13 +1838,13 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1261748513538551809</t>
+    <t xml:space="preserve">https://www.health.go.ug/cause/update-on-the-covid-19-outbreak-in-uganda-16/</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
   </si>
   <si>
-    <t xml:space="preserve">We sum the cumulative total provided for the previous day with the daily number of samples tested today.</t>
+    <t xml:space="preserve">The MOH did not release daily tests results on 17th April. The cumulative total for 18th April thus takes the total figure as of the 16th April and the daily tests conducted on the 18th April.</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.health.go.ug/moh/resources/</t>
@@ -1863,7 +1862,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200518182140/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200519191911/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1908,7 +1907,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200518182145/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200519192047/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
   </si>
   <si>
     <t xml:space="preserve">The number of tests performed, including tests posted or delivered but not yet returned and/or processed.</t>
@@ -1955,9 +1954,6 @@
     <t xml:space="preserve">United States - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200518182147/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">United States CDC</t>
   </si>
   <si>
@@ -1976,7 +1972,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-28</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-29</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2015,7 +2011,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1261806379716743169</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1262508825690738690</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -2479,7 +2475,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2489,25 +2485,25 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H3" t="n">
-        <v>1062034</v>
+        <v>1085870</v>
       </c>
       <c r="I3" t="n">
-        <v>41.649</v>
+        <v>42.583</v>
       </c>
       <c r="J3" t="n">
-        <v>19908</v>
+        <v>23836</v>
       </c>
       <c r="K3" t="n">
-        <v>0.781</v>
+        <v>0.935</v>
       </c>
       <c r="L3" t="n">
-        <v>29559</v>
+        <v>29706</v>
       </c>
       <c r="M3" t="n">
-        <v>1.159</v>
+        <v>1.165</v>
       </c>
       <c r="N3" t="s">
         <v>27</v>
@@ -2530,7 +2526,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -2540,25 +2536,25 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H4" t="n">
-        <v>365873</v>
+        <v>372435</v>
       </c>
       <c r="I4" t="n">
-        <v>40.624</v>
+        <v>41.352</v>
       </c>
       <c r="J4" t="n">
-        <v>3364</v>
+        <v>6562</v>
       </c>
       <c r="K4" t="n">
-        <v>0.374</v>
+        <v>0.729</v>
       </c>
       <c r="L4" t="n">
-        <v>6627</v>
+        <v>6160</v>
       </c>
       <c r="M4" t="n">
-        <v>0.736</v>
+        <v>0.684</v>
       </c>
       <c r="N4" t="s">
         <v>34</v>
@@ -2581,7 +2577,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2591,25 +2587,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H5" t="n">
-        <v>241132</v>
+        <v>248205</v>
       </c>
       <c r="I5" t="n">
-        <v>141.71</v>
+        <v>145.867</v>
       </c>
       <c r="J5" t="n">
-        <v>4304</v>
+        <v>5174</v>
       </c>
       <c r="K5" t="n">
-        <v>2.529</v>
+        <v>3.041</v>
       </c>
       <c r="L5" t="n">
-        <v>7193</v>
+        <v>7187</v>
       </c>
       <c r="M5" t="n">
-        <v>4.227</v>
+        <v>4.224</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
@@ -2632,7 +2628,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D6" t="s">
         <v>48</v>
@@ -2642,25 +2638,25 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H6" t="n">
-        <v>185196</v>
+        <v>193645</v>
       </c>
       <c r="I6" t="n">
-        <v>1.125</v>
+        <v>1.176</v>
       </c>
       <c r="J6" t="n">
-        <v>9788</v>
+        <v>8449</v>
       </c>
       <c r="K6" t="n">
-        <v>0.059</v>
+        <v>0.051</v>
       </c>
       <c r="L6" t="n">
-        <v>7904</v>
+        <v>8144</v>
       </c>
       <c r="M6" t="n">
-        <v>0.048</v>
+        <v>0.049</v>
       </c>
       <c r="N6" t="s">
         <v>49</v>
@@ -2730,7 +2726,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>43967</v>
+        <v>43968</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
@@ -2740,25 +2736,25 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H8" t="n">
-        <v>569443</v>
+        <v>578746</v>
       </c>
       <c r="I8" t="n">
-        <v>49.134</v>
+        <v>49.937</v>
       </c>
       <c r="J8" t="n">
-        <v>10981</v>
+        <v>7813</v>
       </c>
       <c r="K8" t="n">
-        <v>0.947</v>
+        <v>0.674</v>
       </c>
       <c r="L8" t="n">
-        <v>13685</v>
+        <v>13535</v>
       </c>
       <c r="M8" t="n">
-        <v>1.181</v>
+        <v>1.168</v>
       </c>
       <c r="N8" t="s">
         <v>62</v>
@@ -2781,7 +2777,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>43968</v>
+        <v>43969</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
@@ -2793,25 +2789,25 @@
         <v>69</v>
       </c>
       <c r="G9" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H9" t="n">
-        <v>10174</v>
+        <v>10349</v>
       </c>
       <c r="I9" t="n">
-        <v>0.872</v>
+        <v>0.887</v>
       </c>
       <c r="J9" t="n">
-        <v>262</v>
+        <v>175</v>
       </c>
       <c r="K9" t="n">
-        <v>0.022</v>
+        <v>0.015</v>
       </c>
       <c r="L9" t="n">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="M9" t="n">
-        <v>0.019</v>
+        <v>0.018</v>
       </c>
       <c r="N9" t="s">
         <v>41</v>
@@ -2834,215 +2830,215 @@
         <v>74</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>43941</v>
+        <v>43965</v>
       </c>
       <c r="D10" t="s">
         <v>75</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H10" t="n">
-        <v>132467</v>
+        <v>3081480</v>
       </c>
       <c r="I10" t="n">
-        <v>0.623</v>
+        <v>14.497</v>
       </c>
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10" t="n">
-        <v>5345</v>
+        <v>295084</v>
       </c>
       <c r="M10" t="n">
-        <v>0.025</v>
+        <v>1.388</v>
       </c>
       <c r="N10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O10" t="s">
         <v>77</v>
-      </c>
-      <c r="O10" t="s">
-        <v>78</v>
       </c>
       <c r="P10" t="s">
         <v>22</v>
       </c>
       <c r="Q10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" t="s">
         <v>80</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="1" t="n">
+        <v>43970</v>
+      </c>
+      <c r="D11" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="1" t="n">
-        <v>43968</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>82</v>
-      </c>
-      <c r="E11" t="s">
-        <v>83</v>
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H11" t="n">
-        <v>65574</v>
+        <v>66810</v>
       </c>
       <c r="I11" t="n">
-        <v>9.437</v>
+        <v>9.615</v>
       </c>
       <c r="J11" t="n">
-        <v>1094</v>
+        <v>874</v>
       </c>
       <c r="K11" t="n">
-        <v>0.157</v>
+        <v>0.126</v>
       </c>
       <c r="L11" t="n">
-        <v>1192</v>
+        <v>1157</v>
       </c>
       <c r="M11" t="n">
-        <v>0.172</v>
+        <v>0.167</v>
       </c>
       <c r="N11" t="s">
+        <v>83</v>
+      </c>
+      <c r="O11" t="s">
         <v>84</v>
-      </c>
-      <c r="O11" t="s">
-        <v>85</v>
       </c>
       <c r="P11" t="s">
         <v>22</v>
       </c>
       <c r="Q11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" t="s">
         <v>87</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="1" t="n">
+        <v>43970</v>
+      </c>
+      <c r="D12" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="1" t="n">
-        <v>43969</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>89</v>
-      </c>
-      <c r="E12" t="s">
-        <v>90</v>
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H12" t="n">
-        <v>1319987</v>
+        <v>1336967</v>
       </c>
       <c r="I12" t="n">
-        <v>34.974</v>
+        <v>35.424</v>
       </c>
       <c r="J12" t="n">
-        <v>23292</v>
+        <v>16980</v>
       </c>
       <c r="K12" t="n">
-        <v>0.617</v>
+        <v>0.45</v>
       </c>
       <c r="L12" t="n">
-        <v>28720</v>
+        <v>27326</v>
       </c>
       <c r="M12" t="n">
-        <v>0.761</v>
+        <v>0.724</v>
       </c>
       <c r="N12" t="s">
+        <v>89</v>
+      </c>
+      <c r="O12" t="s">
         <v>90</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>91</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>92</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s">
         <v>94</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="1" t="n">
+        <v>43970</v>
+      </c>
+      <c r="D13" t="s">
         <v>95</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>43969</v>
-      </c>
-      <c r="D13" t="s">
-        <v>96</v>
       </c>
       <c r="E13" t="s">
         <v>41</v>
       </c>
       <c r="F13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" t="n">
+        <v>49</v>
+      </c>
+      <c r="H13" t="n">
+        <v>397200</v>
+      </c>
+      <c r="I13" t="n">
+        <v>20.778</v>
+      </c>
+      <c r="J13" t="n">
+        <v>16189</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.847</v>
+      </c>
+      <c r="L13" t="n">
+        <v>13409</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.701</v>
+      </c>
+      <c r="N13" t="s">
         <v>97</v>
       </c>
-      <c r="G13" t="n">
-        <v>48</v>
-      </c>
-      <c r="H13" t="n">
-        <v>381011</v>
-      </c>
-      <c r="I13" t="n">
-        <v>19.931</v>
-      </c>
-      <c r="J13" t="n">
-        <v>17515</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.916</v>
-      </c>
-      <c r="L13" t="n">
-        <v>12422</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>98</v>
-      </c>
-      <c r="O13" t="s">
-        <v>99</v>
       </c>
       <c r="P13" t="s">
         <v>36</v>
       </c>
       <c r="Q13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" t="s">
         <v>101</v>
-      </c>
-      <c r="B14" t="s">
-        <v>102</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>43968</v>
       </c>
       <c r="D14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" t="s">
         <v>103</v>
-      </c>
-      <c r="E14" t="s">
-        <v>104</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
@@ -3067,546 +3063,550 @@
         <v>0.126</v>
       </c>
       <c r="N14" t="s">
+        <v>103</v>
+      </c>
+      <c r="O14" t="s">
         <v>104</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>105</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>106</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" t="s">
         <v>108</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="1" t="n">
+        <v>43970</v>
+      </c>
+      <c r="D15" t="s">
         <v>109</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>43968</v>
-      </c>
-      <c r="D15" t="s">
-        <v>110</v>
       </c>
       <c r="E15" t="s">
         <v>41</v>
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H15" t="n">
-        <v>14272</v>
+        <v>14616</v>
       </c>
       <c r="I15" t="n">
-        <v>2.802</v>
+        <v>2.869</v>
       </c>
       <c r="J15" t="n">
-        <v>576</v>
+        <v>138</v>
       </c>
       <c r="K15" t="n">
-        <v>0.113</v>
+        <v>0.027</v>
       </c>
       <c r="L15" t="n">
-        <v>343</v>
+        <v>365</v>
       </c>
       <c r="M15" t="n">
-        <v>0.067</v>
+        <v>0.072</v>
       </c>
       <c r="N15" t="s">
+        <v>110</v>
+      </c>
+      <c r="O15" t="s">
         <v>111</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q15" t="s">
         <v>112</v>
-      </c>
-      <c r="P15" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" t="s">
         <v>114</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="1" t="n">
+        <v>43970</v>
+      </c>
+      <c r="D16" t="s">
         <v>115</v>
       </c>
-      <c r="C16" s="1" t="n">
-        <v>43969</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>116</v>
-      </c>
-      <c r="E16" t="s">
-        <v>117</v>
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H16" t="n">
-        <v>54820</v>
+        <v>55800</v>
       </c>
       <c r="I16" t="n">
-        <v>13.354</v>
+        <v>13.592</v>
       </c>
       <c r="J16" t="n">
-        <v>943</v>
+        <v>980</v>
       </c>
       <c r="K16" t="n">
-        <v>0.23</v>
+        <v>0.239</v>
       </c>
       <c r="L16" t="n">
-        <v>1250</v>
+        <v>1189</v>
       </c>
       <c r="M16" t="n">
-        <v>0.304</v>
+        <v>0.29</v>
       </c>
       <c r="N16" t="s">
+        <v>116</v>
+      </c>
+      <c r="O16" t="s">
         <v>117</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>118</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>119</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" t="s">
         <v>121</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="1" t="n">
+        <v>43969</v>
+      </c>
+      <c r="D17" t="s">
         <v>122</v>
       </c>
-      <c r="C17" s="1" t="n">
-        <v>43968</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>123</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>124</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="n">
+        <v>58</v>
+      </c>
+      <c r="H17" t="n">
+        <v>85556</v>
+      </c>
+      <c r="I17" t="n">
+        <v>7.554</v>
+      </c>
+      <c r="J17" t="n">
+        <v>1688</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.149</v>
+      </c>
+      <c r="L17" t="n">
+        <v>2057</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="N17" t="s">
+        <v>123</v>
+      </c>
+      <c r="O17" t="s">
+        <v>122</v>
+      </c>
+      <c r="P17" t="s">
         <v>125</v>
       </c>
-      <c r="G17" t="n">
-        <v>57</v>
-      </c>
-      <c r="H17" t="n">
-        <v>83868</v>
-      </c>
-      <c r="I17" t="n">
-        <v>7.405</v>
-      </c>
-      <c r="J17" t="n">
-        <v>1951</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0.172</v>
-      </c>
-      <c r="L17" t="n">
-        <v>2098</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0.185</v>
-      </c>
-      <c r="N17" t="s">
-        <v>124</v>
-      </c>
-      <c r="O17" t="s">
-        <v>123</v>
-      </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>126</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" t="s">
         <v>128</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" s="1" t="n">
+        <v>43969</v>
+      </c>
+      <c r="D18" t="s">
         <v>129</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>43968</v>
-      </c>
-      <c r="D18" t="s">
-        <v>130</v>
       </c>
       <c r="E18" t="s">
         <v>41</v>
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H18" t="n">
-        <v>356515</v>
+        <v>363963</v>
       </c>
       <c r="I18" t="n">
-        <v>33.291</v>
+        <v>33.987</v>
       </c>
       <c r="J18" t="n">
-        <v>3310</v>
+        <v>7349</v>
       </c>
       <c r="K18" t="n">
-        <v>0.309</v>
+        <v>0.686</v>
       </c>
       <c r="L18" t="n">
-        <v>6477</v>
+        <v>6426</v>
       </c>
       <c r="M18" t="n">
-        <v>0.605</v>
+        <v>0.6</v>
       </c>
       <c r="N18" t="s">
         <v>41</v>
       </c>
       <c r="O18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P18" t="s">
         <v>22</v>
       </c>
       <c r="Q18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" t="s">
         <v>133</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" s="1" t="n">
+        <v>43970</v>
+      </c>
+      <c r="D19" t="s">
         <v>134</v>
       </c>
-      <c r="C19" s="1" t="n">
-        <v>43968</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>135</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>136</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="n">
+        <v>62</v>
+      </c>
+      <c r="H19" t="n">
+        <v>402194</v>
+      </c>
+      <c r="I19" t="n">
+        <v>69.437</v>
+      </c>
+      <c r="J19" t="n">
+        <v>7800</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1.347</v>
+      </c>
+      <c r="L19" t="n">
+        <v>9705</v>
+      </c>
+      <c r="M19" t="n">
+        <v>1.676</v>
+      </c>
+      <c r="N19" t="s">
         <v>137</v>
       </c>
-      <c r="G19" t="n">
-        <v>60</v>
-      </c>
-      <c r="H19" t="n">
-        <v>388703</v>
-      </c>
-      <c r="I19" t="n">
-        <v>67.108</v>
-      </c>
-      <c r="J19" t="n">
-        <v>9221</v>
-      </c>
-      <c r="K19" t="n">
-        <v>1.592</v>
-      </c>
-      <c r="L19" t="n">
-        <v>10124</v>
-      </c>
-      <c r="M19" t="n">
-        <v>1.748</v>
-      </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>138</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q19" t="s">
         <v>139</v>
-      </c>
-      <c r="P19" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" t="s">
         <v>141</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" s="1" t="n">
+        <v>43970</v>
+      </c>
+      <c r="D20" t="s">
         <v>142</v>
       </c>
-      <c r="C20" s="1" t="n">
-        <v>43967</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>143</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>144</v>
       </c>
-      <c r="F20" t="s">
-        <v>145</v>
-      </c>
       <c r="G20" t="n">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="H20" t="n">
-        <v>50020</v>
+        <v>53813</v>
       </c>
       <c r="I20" t="n">
-        <v>2.835</v>
+        <v>3.05</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20" t="n">
-        <v>1217</v>
+        <v>1375</v>
       </c>
       <c r="M20" t="n">
-        <v>0.069</v>
+        <v>0.078</v>
       </c>
       <c r="N20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O20" t="s">
+        <v>145</v>
+      </c>
+      <c r="P20" t="s">
         <v>146</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>147</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" t="s">
         <v>149</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="1" t="n">
+        <v>43969</v>
+      </c>
+      <c r="D21" t="s">
         <v>150</v>
       </c>
-      <c r="C21" s="1" t="n">
-        <v>43968</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>151</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>152</v>
       </c>
-      <c r="F21" t="s">
-        <v>153</v>
-      </c>
       <c r="G21" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H21" t="n">
-        <v>57883</v>
+        <v>60341</v>
       </c>
       <c r="I21" t="n">
-        <v>8.924</v>
+        <v>9.303</v>
       </c>
       <c r="J21" t="n">
-        <v>4471</v>
+        <v>2458</v>
       </c>
       <c r="K21" t="n">
-        <v>0.689</v>
+        <v>0.379</v>
       </c>
       <c r="L21" t="n">
-        <v>2120</v>
+        <v>2202</v>
       </c>
       <c r="M21" t="n">
-        <v>0.327</v>
+        <v>0.339</v>
       </c>
       <c r="N21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P21" t="s">
         <v>22</v>
       </c>
       <c r="Q21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B22" t="s">
         <v>155</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" s="1" t="n">
+        <v>43969</v>
+      </c>
+      <c r="D22" t="s">
         <v>156</v>
       </c>
-      <c r="C22" s="1" t="n">
-        <v>43968</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>157</v>
-      </c>
-      <c r="E22" t="s">
-        <v>158</v>
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H22" t="n">
-        <v>70189</v>
+        <v>71441</v>
       </c>
       <c r="I22" t="n">
-        <v>52.911</v>
+        <v>53.855</v>
       </c>
       <c r="J22" t="n">
-        <v>671</v>
+        <v>1258</v>
       </c>
       <c r="K22" t="n">
-        <v>0.506</v>
+        <v>0.948</v>
       </c>
       <c r="L22" t="n">
-        <v>892</v>
+        <v>927</v>
       </c>
       <c r="M22" t="n">
-        <v>0.672</v>
+        <v>0.699</v>
       </c>
       <c r="N22" t="s">
+        <v>158</v>
+      </c>
+      <c r="O22" t="s">
         <v>159</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>160</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>161</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23" t="s">
         <v>163</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" s="1" t="n">
+        <v>43970</v>
+      </c>
+      <c r="D23" t="s">
         <v>164</v>
       </c>
-      <c r="C23" s="1" t="n">
-        <v>43969</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>165</v>
-      </c>
-      <c r="E23" t="s">
-        <v>166</v>
       </c>
       <c r="F23"/>
       <c r="G23" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H23" t="n">
-        <v>59029</v>
+        <v>62300</v>
       </c>
       <c r="I23" t="n">
-        <v>0.513</v>
-      </c>
-      <c r="J23"/>
-      <c r="K23"/>
+        <v>0.542</v>
+      </c>
+      <c r="J23" t="n">
+        <v>3271</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.028</v>
+      </c>
       <c r="L23" t="n">
-        <v>3201</v>
+        <v>3322</v>
       </c>
       <c r="M23" t="n">
-        <v>0.028</v>
+        <v>0.029</v>
       </c>
       <c r="N23" t="s">
+        <v>165</v>
+      </c>
+      <c r="O23" t="s">
         <v>166</v>
-      </c>
-      <c r="O23" t="s">
-        <v>167</v>
       </c>
       <c r="P23" t="s">
         <v>22</v>
       </c>
       <c r="Q23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
+        <v>168</v>
+      </c>
+      <c r="B24" t="s">
         <v>169</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" s="1" t="n">
+        <v>43968</v>
+      </c>
+      <c r="D24" t="s">
         <v>170</v>
       </c>
-      <c r="C24" s="1" t="n">
-        <v>43966</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>171</v>
-      </c>
-      <c r="E24" t="s">
-        <v>172</v>
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H24" t="n">
-        <v>145959</v>
+        <v>151935</v>
       </c>
       <c r="I24" t="n">
-        <v>26.343</v>
+        <v>27.422</v>
       </c>
       <c r="J24" t="n">
-        <v>2835</v>
+        <v>2017</v>
       </c>
       <c r="K24" t="n">
-        <v>0.512</v>
+        <v>0.364</v>
       </c>
       <c r="L24" t="n">
-        <v>2922</v>
+        <v>3136</v>
       </c>
       <c r="M24" t="n">
-        <v>0.527</v>
+        <v>0.566</v>
       </c>
       <c r="N24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P24" t="s">
         <v>51</v>
       </c>
       <c r="Q24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
+        <v>174</v>
+      </c>
+      <c r="B25" t="s">
         <v>175</v>
-      </c>
-      <c r="B25" t="s">
-        <v>176</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>43956</v>
       </c>
       <c r="D25" t="s">
+        <v>176</v>
+      </c>
+      <c r="E25" t="s">
         <v>177</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>178</v>
-      </c>
-      <c r="F25" t="s">
-        <v>179</v>
       </c>
       <c r="G25" t="n">
         <v>24</v>
@@ -3626,36 +3626,36 @@
         <v>0.233</v>
       </c>
       <c r="N25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P25" t="s">
         <v>22</v>
       </c>
       <c r="Q25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>181</v>
+      </c>
+      <c r="B26" t="s">
         <v>182</v>
-      </c>
-      <c r="B26" t="s">
-        <v>183</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>43961</v>
       </c>
       <c r="D26" t="s">
+        <v>183</v>
+      </c>
+      <c r="E26" t="s">
         <v>184</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>185</v>
-      </c>
-      <c r="F26" t="s">
-        <v>186</v>
       </c>
       <c r="G26" t="n">
         <v>10</v>
@@ -3675,186 +3675,182 @@
         <v>0.652</v>
       </c>
       <c r="N26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O26" t="s">
+        <v>186</v>
+      </c>
+      <c r="P26" t="s">
         <v>187</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>188</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>189</v>
+      </c>
+      <c r="B27" t="s">
         <v>190</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" s="1" t="n">
+        <v>43968</v>
+      </c>
+      <c r="D27" t="s">
         <v>191</v>
       </c>
-      <c r="C27" s="1" t="n">
-        <v>43965</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>192</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>193</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="n">
+        <v>17</v>
+      </c>
+      <c r="H27" t="n">
+        <v>179586</v>
+      </c>
+      <c r="I27" t="n">
+        <v>5.779</v>
+      </c>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27" t="n">
+        <v>2867</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.092</v>
+      </c>
+      <c r="N27" t="s">
         <v>194</v>
       </c>
-      <c r="G27" t="n">
-        <v>15</v>
-      </c>
-      <c r="H27" t="n">
-        <v>171642</v>
-      </c>
-      <c r="I27" t="n">
-        <v>5.524</v>
-      </c>
-      <c r="J27" t="n">
-        <v>3938</v>
-      </c>
-      <c r="K27" t="n">
-        <v>0.127</v>
-      </c>
-      <c r="L27" t="n">
-        <v>3099</v>
-      </c>
-      <c r="M27" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>195</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
         <v>196</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>197</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B28" t="s">
+        <v>198</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>43968</v>
+      </c>
+      <c r="D28" t="s">
+        <v>191</v>
+      </c>
+      <c r="E28" t="s">
+        <v>192</v>
+      </c>
+      <c r="F28" t="s">
         <v>199</v>
       </c>
-      <c r="C28" s="1" t="n">
-        <v>43965</v>
-      </c>
-      <c r="D28" t="s">
-        <v>192</v>
-      </c>
-      <c r="E28" t="s">
-        <v>193</v>
-      </c>
-      <c r="F28" t="s">
-        <v>200</v>
-      </c>
       <c r="G28" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H28" t="n">
-        <v>172623</v>
+        <v>180567</v>
       </c>
       <c r="I28" t="n">
-        <v>5.555</v>
-      </c>
-      <c r="J28" t="n">
-        <v>3938</v>
-      </c>
-      <c r="K28" t="n">
-        <v>0.127</v>
-      </c>
+        <v>5.811</v>
+      </c>
+      <c r="J28"/>
+      <c r="K28"/>
       <c r="L28" t="n">
-        <v>3489</v>
+        <v>2867</v>
       </c>
       <c r="M28" t="n">
-        <v>0.112</v>
+        <v>0.092</v>
       </c>
       <c r="N28" t="s">
+        <v>194</v>
+      </c>
+      <c r="O28" t="s">
         <v>195</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>196</v>
       </c>
-      <c r="P28" t="s">
+      <c r="Q28" t="s">
         <v>197</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
+        <v>200</v>
+      </c>
+      <c r="B29" t="s">
         <v>201</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" s="1" t="n">
+        <v>43970</v>
+      </c>
+      <c r="D29" t="s">
         <v>202</v>
       </c>
-      <c r="C29" s="1" t="n">
-        <v>43969</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>203</v>
-      </c>
-      <c r="E29" t="s">
-        <v>204</v>
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H29" t="n">
-        <v>131684</v>
+        <v>136001</v>
       </c>
       <c r="I29" t="n">
-        <v>12.634</v>
-      </c>
-      <c r="J29"/>
-      <c r="K29"/>
+        <v>13.048</v>
+      </c>
+      <c r="J29" t="n">
+        <v>4317</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.414</v>
+      </c>
       <c r="L29" t="n">
-        <v>4617</v>
+        <v>4278</v>
       </c>
       <c r="M29" t="n">
-        <v>0.443</v>
+        <v>0.41</v>
       </c>
       <c r="N29" t="s">
+        <v>204</v>
+      </c>
+      <c r="O29" t="s">
         <v>205</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q29" t="s">
         <v>206</v>
-      </c>
-      <c r="P29" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>207</v>
+      </c>
+      <c r="B30" t="s">
         <v>208</v>
-      </c>
-      <c r="B30" t="s">
-        <v>209</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>43963</v>
       </c>
       <c r="D30" t="s">
+        <v>209</v>
+      </c>
+      <c r="E30" t="s">
         <v>210</v>
-      </c>
-      <c r="E30" t="s">
-        <v>211</v>
       </c>
       <c r="F30"/>
       <c r="G30" t="n">
@@ -3875,140 +3871,140 @@
         <v>0.261</v>
       </c>
       <c r="N30" t="s">
+        <v>211</v>
+      </c>
+      <c r="O30" t="s">
         <v>212</v>
-      </c>
-      <c r="O30" t="s">
-        <v>213</v>
       </c>
       <c r="P30" t="s">
         <v>22</v>
       </c>
       <c r="Q30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>214</v>
+      </c>
+      <c r="B31" t="s">
         <v>215</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" s="1" t="n">
+        <v>43970</v>
+      </c>
+      <c r="D31" t="s">
         <v>216</v>
       </c>
-      <c r="C31" s="1" t="n">
-        <v>43969</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>217</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>218</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="n">
+        <v>75</v>
+      </c>
+      <c r="H31" t="n">
+        <v>138697</v>
+      </c>
+      <c r="I31" t="n">
+        <v>14.357</v>
+      </c>
+      <c r="J31" t="n">
+        <v>1454</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.151</v>
+      </c>
+      <c r="L31" t="n">
+        <v>3425</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.355</v>
+      </c>
+      <c r="N31" t="s">
+        <v>217</v>
+      </c>
+      <c r="O31" t="s">
         <v>219</v>
       </c>
-      <c r="G31" t="n">
-        <v>74</v>
-      </c>
-      <c r="H31" t="n">
-        <v>137243</v>
-      </c>
-      <c r="I31" t="n">
-        <v>14.207</v>
-      </c>
-      <c r="J31" t="n">
-        <v>2106</v>
-      </c>
-      <c r="K31" t="n">
-        <v>0.218</v>
-      </c>
-      <c r="L31" t="n">
-        <v>3583</v>
-      </c>
-      <c r="M31" t="n">
-        <v>0.371</v>
-      </c>
-      <c r="N31" t="s">
-        <v>218</v>
-      </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>220</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>221</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
+        <v>222</v>
+      </c>
+      <c r="B32" t="s">
         <v>223</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" s="1" t="n">
+        <v>43969</v>
+      </c>
+      <c r="D32" t="s">
         <v>224</v>
       </c>
-      <c r="C32" s="1" t="n">
-        <v>43967</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>225</v>
-      </c>
-      <c r="E32" t="s">
-        <v>226</v>
       </c>
       <c r="F32"/>
       <c r="G32" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H32" t="n">
-        <v>56834</v>
+        <v>57146</v>
       </c>
       <c r="I32" t="n">
-        <v>166.547</v>
+        <v>167.461</v>
       </c>
       <c r="J32" t="n">
-        <v>133</v>
+        <v>305</v>
       </c>
       <c r="K32" t="n">
-        <v>0.39</v>
+        <v>0.894</v>
       </c>
       <c r="L32" t="n">
-        <v>383</v>
+        <v>342</v>
       </c>
       <c r="M32" t="n">
-        <v>1.122</v>
+        <v>1.002</v>
       </c>
       <c r="N32" t="s">
+        <v>225</v>
+      </c>
+      <c r="O32" t="s">
+        <v>224</v>
+      </c>
+      <c r="P32" t="s">
         <v>226</v>
       </c>
-      <c r="O32" t="s">
-        <v>225</v>
-      </c>
-      <c r="P32" t="s">
+      <c r="Q32" t="s">
         <v>227</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
+        <v>228</v>
+      </c>
+      <c r="B33" t="s">
         <v>229</v>
-      </c>
-      <c r="B33" t="s">
-        <v>230</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>43945</v>
       </c>
       <c r="D33" t="s">
+        <v>230</v>
+      </c>
+      <c r="E33" t="s">
         <v>231</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>232</v>
-      </c>
-      <c r="F33" t="s">
-        <v>233</v>
       </c>
       <c r="G33" t="n">
         <v>24</v>
@@ -4032,36 +4028,36 @@
         <v>0.021</v>
       </c>
       <c r="N33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>43969</v>
       </c>
       <c r="D34" t="s">
+        <v>230</v>
+      </c>
+      <c r="E34" t="s">
         <v>231</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>232</v>
-      </c>
-      <c r="F34" t="s">
-        <v>233</v>
       </c>
       <c r="G34" t="n">
         <v>55</v>
@@ -4085,185 +4081,185 @@
         <v>0.065</v>
       </c>
       <c r="N34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O34" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P34" t="s">
         <v>51</v>
       </c>
       <c r="Q34" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
+        <v>235</v>
+      </c>
+      <c r="B35" t="s">
         <v>236</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" s="1" t="n">
+        <v>43970</v>
+      </c>
+      <c r="D35" t="s">
         <v>237</v>
       </c>
-      <c r="C35" s="1" t="n">
-        <v>43969</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>238</v>
-      </c>
-      <c r="E35" t="s">
-        <v>239</v>
       </c>
       <c r="F35"/>
       <c r="G35" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H35" t="n">
-        <v>143035</v>
+        <v>147799</v>
       </c>
       <c r="I35" t="n">
-        <v>0.523</v>
+        <v>0.54</v>
       </c>
       <c r="J35" t="n">
-        <v>2556</v>
+        <v>4764</v>
       </c>
       <c r="K35" t="n">
-        <v>0.009</v>
+        <v>0.017</v>
       </c>
       <c r="L35" t="n">
-        <v>3811</v>
+        <v>4010</v>
       </c>
       <c r="M35" t="n">
-        <v>0.014</v>
+        <v>0.015</v>
       </c>
       <c r="N35" t="s">
+        <v>238</v>
+      </c>
+      <c r="O35" t="s">
         <v>239</v>
-      </c>
-      <c r="O35" t="s">
-        <v>240</v>
       </c>
       <c r="P35" t="s">
         <v>71</v>
       </c>
       <c r="Q35" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
+        <v>241</v>
+      </c>
+      <c r="B36" t="s">
         <v>242</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" s="1" t="n">
+        <v>43970</v>
+      </c>
+      <c r="D36" t="s">
         <v>243</v>
       </c>
-      <c r="C36" s="1" t="n">
-        <v>43969</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>244</v>
-      </c>
-      <c r="E36" t="s">
-        <v>245</v>
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H36" t="n">
-        <v>701640</v>
+        <v>716176</v>
       </c>
       <c r="I36" t="n">
-        <v>8.354</v>
+        <v>8.527</v>
       </c>
       <c r="J36" t="n">
-        <v>14705</v>
+        <v>14536</v>
       </c>
       <c r="K36" t="n">
-        <v>0.175</v>
+        <v>0.173</v>
       </c>
       <c r="L36" t="n">
-        <v>14365</v>
+        <v>14386</v>
       </c>
       <c r="M36" t="n">
         <v>0.171</v>
       </c>
       <c r="N36" t="s">
+        <v>244</v>
+      </c>
+      <c r="O36" t="s">
         <v>245</v>
-      </c>
-      <c r="O36" t="s">
-        <v>246</v>
       </c>
       <c r="P36" t="s">
         <v>22</v>
       </c>
       <c r="Q36" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
+        <v>247</v>
+      </c>
+      <c r="B37" t="s">
         <v>248</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" s="1" t="n">
+        <v>43970</v>
+      </c>
+      <c r="D37" t="s">
         <v>249</v>
       </c>
-      <c r="C37" s="1" t="n">
-        <v>43963</v>
-      </c>
-      <c r="D37" t="s">
-        <v>250</v>
-      </c>
       <c r="E37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F37"/>
       <c r="G37" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H37" t="n">
-        <v>258808</v>
+        <v>295626</v>
       </c>
       <c r="I37" t="n">
-        <v>52.414</v>
+        <v>59.87</v>
       </c>
       <c r="J37"/>
       <c r="K37"/>
       <c r="L37" t="n">
-        <v>6292</v>
+        <v>5260</v>
       </c>
       <c r="M37" t="n">
-        <v>1.274</v>
+        <v>1.065</v>
       </c>
       <c r="N37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O37" t="s">
+        <v>250</v>
+      </c>
+      <c r="P37" t="s">
         <v>251</v>
       </c>
-      <c r="P37" t="s">
+      <c r="Q37" t="s">
         <v>252</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
+        <v>253</v>
+      </c>
+      <c r="B38" t="s">
         <v>254</v>
-      </c>
-      <c r="B38" t="s">
-        <v>255</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>43968</v>
       </c>
       <c r="D38" t="s">
+        <v>255</v>
+      </c>
+      <c r="E38" t="s">
         <v>256</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>257</v>
-      </c>
-      <c r="F38" t="s">
-        <v>258</v>
       </c>
       <c r="G38" t="n">
         <v>87</v>
@@ -4290,165 +4286,165 @@
         <v>41</v>
       </c>
       <c r="O38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P38" t="s">
         <v>22</v>
       </c>
       <c r="Q38" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
+        <v>260</v>
+      </c>
+      <c r="B39" t="s">
         <v>261</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" s="1" t="n">
+        <v>43970</v>
+      </c>
+      <c r="D39" t="s">
         <v>262</v>
       </c>
-      <c r="C39" s="1" t="n">
-        <v>43969</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>263</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>264</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="n">
+        <v>31</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1999599</v>
+      </c>
+      <c r="I39" t="n">
+        <v>33.072</v>
+      </c>
+      <c r="J39" t="n">
+        <v>40226</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.665</v>
+      </c>
+      <c r="L39" t="n">
+        <v>36814</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0.609</v>
+      </c>
+      <c r="N39" t="s">
         <v>265</v>
       </c>
-      <c r="G39" t="n">
-        <v>30</v>
-      </c>
-      <c r="H39" t="n">
-        <v>1959373</v>
-      </c>
-      <c r="I39" t="n">
-        <v>32.407</v>
-      </c>
-      <c r="J39" t="n">
-        <v>26101</v>
-      </c>
-      <c r="K39" t="n">
-        <v>0.432</v>
-      </c>
-      <c r="L39" t="n">
-        <v>36727</v>
-      </c>
-      <c r="M39" t="n">
-        <v>0.607</v>
-      </c>
-      <c r="N39" t="s">
+      <c r="O39" t="s">
         <v>266</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q39" t="s">
         <v>267</v>
-      </c>
-      <c r="P39" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B40" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D40" t="s">
+        <v>262</v>
+      </c>
+      <c r="E40" t="s">
         <v>263</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>264</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="n">
+        <v>86</v>
+      </c>
+      <c r="H40" t="n">
+        <v>3104524</v>
+      </c>
+      <c r="I40" t="n">
+        <v>51.347</v>
+      </c>
+      <c r="J40" t="n">
+        <v>63158</v>
+      </c>
+      <c r="K40" t="n">
+        <v>1.045</v>
+      </c>
+      <c r="L40" t="n">
+        <v>61553</v>
+      </c>
+      <c r="M40" t="n">
+        <v>1.018</v>
+      </c>
+      <c r="N40" t="s">
         <v>265</v>
       </c>
-      <c r="G40" t="n">
-        <v>85</v>
-      </c>
-      <c r="H40" t="n">
-        <v>3041366</v>
-      </c>
-      <c r="I40" t="n">
-        <v>50.302</v>
-      </c>
-      <c r="J40" t="n">
-        <v>36406</v>
-      </c>
-      <c r="K40" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="L40" t="n">
-        <v>62102</v>
-      </c>
-      <c r="M40" t="n">
-        <v>1.027</v>
-      </c>
-      <c r="N40" t="s">
+      <c r="O40" t="s">
         <v>266</v>
-      </c>
-      <c r="O40" t="s">
-        <v>267</v>
       </c>
       <c r="P40" t="s">
         <v>22</v>
       </c>
       <c r="Q40" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
+        <v>270</v>
+      </c>
+      <c r="B41" t="s">
         <v>271</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" s="1" t="n">
+        <v>43970</v>
+      </c>
+      <c r="D41" t="s">
         <v>272</v>
       </c>
-      <c r="C41" s="1" t="n">
-        <v>43969</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>273</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>274</v>
       </c>
-      <c r="F41" t="s">
-        <v>275</v>
-      </c>
       <c r="G41" t="n">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="H41" t="n">
-        <v>250151</v>
+        <v>255675</v>
       </c>
       <c r="I41" t="n">
-        <v>1.978</v>
+        <v>2.022</v>
       </c>
       <c r="J41"/>
       <c r="K41"/>
       <c r="L41" t="n">
-        <v>5760</v>
+        <v>4575</v>
       </c>
       <c r="M41" t="n">
-        <v>0.046</v>
+        <v>0.036</v>
       </c>
       <c r="N41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="O41" t="s">
         <v>276</v>
       </c>
       <c r="P41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q41" t="s">
         <v>277</v>
@@ -4456,46 +4452,46 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B42" t="s">
         <v>278</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>43965</v>
+        <v>43967</v>
       </c>
       <c r="D42" t="s">
         <v>279</v>
       </c>
       <c r="E42" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F42" t="s">
         <v>280</v>
       </c>
       <c r="G42" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H42" t="n">
-        <v>365074</v>
+        <v>402476</v>
       </c>
       <c r="I42" t="n">
-        <v>2.886</v>
+        <v>3.182</v>
       </c>
       <c r="J42" t="n">
-        <v>6745</v>
+        <v>6247</v>
       </c>
       <c r="K42" t="n">
-        <v>0.053</v>
+        <v>0.049</v>
       </c>
       <c r="L42" t="n">
-        <v>6999</v>
+        <v>7063</v>
       </c>
       <c r="M42" t="n">
-        <v>0.055</v>
+        <v>0.056</v>
       </c>
       <c r="N42" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="O42" t="s">
         <v>276</v>
@@ -4515,7 +4511,7 @@
         <v>283</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D43" t="s">
         <v>284</v>
@@ -4525,25 +4521,25 @@
       </c>
       <c r="F43"/>
       <c r="G43" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H43" t="n">
-        <v>540708</v>
+        <v>553062</v>
       </c>
       <c r="I43" t="n">
-        <v>28.797</v>
+        <v>29.455</v>
       </c>
       <c r="J43" t="n">
-        <v>13268</v>
+        <v>12354</v>
       </c>
       <c r="K43" t="n">
-        <v>0.707</v>
+        <v>0.658</v>
       </c>
       <c r="L43" t="n">
-        <v>18856</v>
+        <v>18722</v>
       </c>
       <c r="M43" t="n">
-        <v>1.004</v>
+        <v>0.997</v>
       </c>
       <c r="N43" t="s">
         <v>285</v>
@@ -4566,7 +4562,7 @@
         <v>288</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D44" t="s">
         <v>289</v>
@@ -4576,25 +4572,25 @@
       </c>
       <c r="F44"/>
       <c r="G44" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H44" t="n">
-        <v>44851</v>
+        <v>46784</v>
       </c>
       <c r="I44" t="n">
-        <v>0.834</v>
+        <v>0.87</v>
       </c>
       <c r="J44" t="n">
-        <v>1139</v>
+        <v>1933</v>
       </c>
       <c r="K44" t="n">
-        <v>0.021</v>
+        <v>0.036</v>
       </c>
       <c r="L44" t="n">
-        <v>1702</v>
+        <v>1838</v>
       </c>
       <c r="M44" t="n">
-        <v>0.032</v>
+        <v>0.034</v>
       </c>
       <c r="N44" t="s">
         <v>41</v>
@@ -4617,7 +4613,7 @@
         <v>295</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D45" t="s">
         <v>296</v>
@@ -4629,25 +4625,25 @@
         <v>298</v>
       </c>
       <c r="G45" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H45" t="n">
-        <v>89123</v>
+        <v>90968</v>
       </c>
       <c r="I45" t="n">
-        <v>47.25</v>
+        <v>48.228</v>
       </c>
       <c r="J45" t="n">
-        <v>718</v>
+        <v>1845</v>
       </c>
       <c r="K45" t="n">
-        <v>0.381</v>
+        <v>0.978</v>
       </c>
       <c r="L45" t="n">
-        <v>1711</v>
+        <v>1703</v>
       </c>
       <c r="M45" t="n">
-        <v>0.907</v>
+        <v>0.903</v>
       </c>
       <c r="N45" t="s">
         <v>297</v>
@@ -4670,7 +4666,7 @@
         <v>301</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>43968</v>
+        <v>43970</v>
       </c>
       <c r="D46" t="s">
         <v>302</v>
@@ -4680,25 +4676,21 @@
       </c>
       <c r="F46"/>
       <c r="G46" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H46" t="n">
-        <v>228726</v>
+        <v>237600</v>
       </c>
       <c r="I46" t="n">
-        <v>84.02</v>
-      </c>
-      <c r="J46" t="n">
-        <v>4686</v>
-      </c>
-      <c r="K46" t="n">
-        <v>1.721</v>
-      </c>
+        <v>87.279</v>
+      </c>
+      <c r="J46"/>
+      <c r="K46"/>
       <c r="L46" t="n">
-        <v>6402</v>
+        <v>6459</v>
       </c>
       <c r="M46" t="n">
-        <v>2.352</v>
+        <v>2.373</v>
       </c>
       <c r="N46" t="s">
         <v>41</v>
@@ -4721,7 +4713,7 @@
         <v>306</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>43968</v>
+        <v>43970</v>
       </c>
       <c r="D47" t="s">
         <v>307</v>
@@ -4731,25 +4723,25 @@
       </c>
       <c r="F47"/>
       <c r="G47" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H47" t="n">
-        <v>62153</v>
+        <v>63011</v>
       </c>
       <c r="I47" t="n">
-        <v>99.29</v>
+        <v>100.66</v>
       </c>
       <c r="J47" t="n">
-        <v>1907</v>
+        <v>751</v>
       </c>
       <c r="K47" t="n">
-        <v>3.046</v>
+        <v>1.2</v>
       </c>
       <c r="L47" t="n">
-        <v>986</v>
+        <v>945</v>
       </c>
       <c r="M47" t="n">
-        <v>1.575</v>
+        <v>1.51</v>
       </c>
       <c r="N47" t="s">
         <v>308</v>
@@ -4823,7 +4815,7 @@
         <v>319</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>43967</v>
+        <v>43968</v>
       </c>
       <c r="D49" t="s">
         <v>320</v>
@@ -4833,25 +4825,25 @@
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H49" t="n">
-        <v>144786</v>
+        <v>150198</v>
       </c>
       <c r="I49" t="n">
-        <v>1.123</v>
+        <v>1.165</v>
       </c>
       <c r="J49" t="n">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="K49" t="n">
         <v>0.001</v>
       </c>
       <c r="L49" t="n">
-        <v>2858</v>
+        <v>3179</v>
       </c>
       <c r="M49" t="n">
-        <v>0.022</v>
+        <v>0.025</v>
       </c>
       <c r="N49" t="s">
         <v>321</v>
@@ -4874,7 +4866,7 @@
         <v>324</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>43952</v>
+        <v>43969</v>
       </c>
       <c r="D50" t="s">
         <v>325</v>
@@ -4886,25 +4878,25 @@
         <v>327</v>
       </c>
       <c r="G50" t="n">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="H50" t="n">
-        <v>37006</v>
+        <v>95536</v>
       </c>
       <c r="I50" t="n">
-        <v>1.003</v>
+        <v>2.588</v>
       </c>
       <c r="J50" t="n">
-        <v>2165</v>
+        <v>5579</v>
       </c>
       <c r="K50" t="n">
-        <v>0.059</v>
+        <v>0.151</v>
       </c>
       <c r="L50" t="n">
-        <v>1868</v>
+        <v>3794</v>
       </c>
       <c r="M50" t="n">
-        <v>0.051</v>
+        <v>0.103</v>
       </c>
       <c r="N50" t="s">
         <v>326</v>
@@ -4927,7 +4919,7 @@
         <v>331</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D51" t="s">
         <v>332</v>
@@ -4939,25 +4931,21 @@
         <v>334</v>
       </c>
       <c r="G51" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H51" t="n">
-        <v>14561</v>
+        <v>15137</v>
       </c>
       <c r="I51" t="n">
-        <v>0.268</v>
-      </c>
-      <c r="J51" t="n">
-        <v>562</v>
-      </c>
-      <c r="K51" t="n">
-        <v>0.01</v>
-      </c>
+        <v>0.278</v>
+      </c>
+      <c r="J51"/>
+      <c r="K51"/>
       <c r="L51" t="n">
-        <v>391</v>
+        <v>439</v>
       </c>
       <c r="M51" t="n">
-        <v>0.007</v>
+        <v>0.008</v>
       </c>
       <c r="N51" t="s">
         <v>333</v>
@@ -4980,7 +4968,7 @@
         <v>338</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>43968</v>
+        <v>43969</v>
       </c>
       <c r="D52" t="s">
         <v>339</v>
@@ -4992,25 +4980,25 @@
         <v>341</v>
       </c>
       <c r="G52" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H52" t="n">
-        <v>28161</v>
+        <v>30724</v>
       </c>
       <c r="I52" t="n">
-        <v>0.967</v>
+        <v>1.054</v>
       </c>
       <c r="J52" t="n">
-        <v>1470</v>
+        <v>2563</v>
       </c>
       <c r="K52" t="n">
-        <v>0.05</v>
+        <v>0.088</v>
       </c>
       <c r="L52" t="n">
-        <v>1609</v>
+        <v>1845</v>
       </c>
       <c r="M52" t="n">
-        <v>0.055</v>
+        <v>0.063</v>
       </c>
       <c r="N52" t="s">
         <v>340</v>
@@ -5019,7 +5007,7 @@
         <v>342</v>
       </c>
       <c r="P52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q52" t="s">
         <v>343</v>
@@ -5033,7 +5021,7 @@
         <v>345</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>43968</v>
+        <v>43969</v>
       </c>
       <c r="D53" t="s">
         <v>346</v>
@@ -5043,21 +5031,25 @@
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H53" t="n">
-        <v>297347</v>
+        <v>302395</v>
       </c>
       <c r="I53" t="n">
-        <v>17.353</v>
-      </c>
-      <c r="J53"/>
-      <c r="K53"/>
+        <v>17.648</v>
+      </c>
+      <c r="J53" t="n">
+        <v>2774</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.162</v>
+      </c>
       <c r="L53" t="n">
-        <v>4285</v>
+        <v>4348</v>
       </c>
       <c r="M53" t="n">
-        <v>0.25</v>
+        <v>0.254</v>
       </c>
       <c r="N53" t="s">
         <v>348</v>
@@ -5066,7 +5058,7 @@
         <v>349</v>
       </c>
       <c r="P53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q53" t="s">
         <v>350</v>
@@ -5080,7 +5072,7 @@
         <v>352</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>43968</v>
+        <v>43969</v>
       </c>
       <c r="D54" t="s">
         <v>353</v>
@@ -5090,25 +5082,25 @@
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H54" t="n">
-        <v>230718</v>
+        <v>233843</v>
       </c>
       <c r="I54" t="n">
-        <v>47.845</v>
+        <v>48.493</v>
       </c>
       <c r="J54" t="n">
-        <v>2570</v>
+        <v>3125</v>
       </c>
       <c r="K54" t="n">
-        <v>0.533</v>
+        <v>0.648</v>
       </c>
       <c r="L54" t="n">
-        <v>5218</v>
+        <v>5251</v>
       </c>
       <c r="M54" t="n">
-        <v>1.082</v>
+        <v>1.089</v>
       </c>
       <c r="N54" t="s">
         <v>354</v>
@@ -5131,7 +5123,7 @@
         <v>357</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D55" t="s">
         <v>358</v>
@@ -5141,22 +5133,22 @@
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H55" t="n">
-        <v>35345</v>
+        <v>36899</v>
       </c>
       <c r="I55" t="n">
-        <v>0.171</v>
+        <v>0.179</v>
       </c>
       <c r="J55" t="n">
-        <v>1375</v>
+        <v>1554</v>
       </c>
       <c r="K55" t="n">
-        <v>0.007</v>
+        <v>0.008</v>
       </c>
       <c r="L55" t="n">
-        <v>1181</v>
+        <v>1212</v>
       </c>
       <c r="M55" t="n">
         <v>0.006</v>
@@ -5182,7 +5174,7 @@
         <v>363</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D56" t="s">
         <v>364</v>
@@ -5192,21 +5184,25 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H56" t="n">
-        <v>218039</v>
+        <v>219984</v>
       </c>
       <c r="I56" t="n">
-        <v>40.219</v>
-      </c>
-      <c r="J56"/>
-      <c r="K56"/>
+        <v>40.578</v>
+      </c>
+      <c r="J56" t="n">
+        <v>1945</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0.359</v>
+      </c>
       <c r="L56" t="n">
-        <v>2184</v>
+        <v>2106</v>
       </c>
       <c r="M56" t="n">
-        <v>0.403</v>
+        <v>0.388</v>
       </c>
       <c r="N56" t="s">
         <v>365</v>
@@ -5229,7 +5225,7 @@
         <v>370</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D57" t="s">
         <v>371</v>
@@ -5239,25 +5235,25 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H57" t="n">
-        <v>387335</v>
+        <v>400292</v>
       </c>
       <c r="I57" t="n">
-        <v>1.754</v>
+        <v>1.812</v>
       </c>
       <c r="J57" t="n">
-        <v>13925</v>
+        <v>12957</v>
       </c>
       <c r="K57" t="n">
-        <v>0.063</v>
+        <v>0.059</v>
       </c>
       <c r="L57" t="n">
-        <v>13206</v>
+        <v>13492</v>
       </c>
       <c r="M57" t="n">
-        <v>0.06</v>
+        <v>0.061</v>
       </c>
       <c r="N57" t="s">
         <v>372</v>
@@ -5280,7 +5276,7 @@
         <v>376</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>43967</v>
+        <v>43969</v>
       </c>
       <c r="D58" t="s">
         <v>377</v>
@@ -5292,25 +5288,25 @@
         <v>378</v>
       </c>
       <c r="G58" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H58" t="n">
-        <v>49104</v>
+        <v>51105</v>
       </c>
       <c r="I58" t="n">
-        <v>11.38</v>
+        <v>11.844</v>
       </c>
       <c r="J58" t="n">
-        <v>1336</v>
+        <v>757</v>
       </c>
       <c r="K58" t="n">
-        <v>0.31</v>
+        <v>0.175</v>
       </c>
       <c r="L58" t="n">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="M58" t="n">
-        <v>0.247</v>
+        <v>0.246</v>
       </c>
       <c r="N58" t="s">
         <v>41</v>
@@ -5319,7 +5315,7 @@
         <v>379</v>
       </c>
       <c r="P58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q58" t="s">
         <v>380</v>
@@ -5386,7 +5382,7 @@
         <v>390</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>43968</v>
+        <v>43970</v>
       </c>
       <c r="D60" t="s">
         <v>391</v>
@@ -5396,25 +5392,25 @@
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H60" t="n">
-        <v>650613</v>
+        <v>105627</v>
       </c>
       <c r="I60" t="n">
-        <v>19.732</v>
+        <v>3.204</v>
       </c>
       <c r="J60" t="n">
-        <v>20131</v>
+        <v>2788</v>
       </c>
       <c r="K60" t="n">
-        <v>0.611</v>
+        <v>0.085</v>
       </c>
       <c r="L60" t="n">
-        <v>20812</v>
+        <v>2862</v>
       </c>
       <c r="M60" t="n">
-        <v>0.631</v>
+        <v>0.087</v>
       </c>
       <c r="N60" t="s">
         <v>392</v>
@@ -5437,7 +5433,7 @@
         <v>397</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>43964</v>
+        <v>43966</v>
       </c>
       <c r="D61" t="s">
         <v>398</v>
@@ -5449,34 +5445,30 @@
         <v>400</v>
       </c>
       <c r="G61" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H61" t="n">
-        <v>184617</v>
+        <v>188024</v>
       </c>
       <c r="I61" t="n">
-        <v>1.685</v>
-      </c>
-      <c r="J61" t="n">
-        <v>13009</v>
-      </c>
-      <c r="K61" t="n">
-        <v>0.119</v>
-      </c>
+        <v>1.716</v>
+      </c>
+      <c r="J61"/>
+      <c r="K61"/>
       <c r="L61" t="n">
-        <v>7590</v>
+        <v>6324</v>
       </c>
       <c r="M61" t="n">
-        <v>0.069</v>
+        <v>0.058</v>
       </c>
       <c r="N61" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O61" t="s">
         <v>398</v>
       </c>
       <c r="P61" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q61" t="s">
         <v>401</v>
@@ -5490,7 +5482,7 @@
         <v>403</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D62" t="s">
         <v>404</v>
@@ -5502,25 +5494,25 @@
         <v>406</v>
       </c>
       <c r="G62" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H62" t="n">
-        <v>636046</v>
+        <v>653224</v>
       </c>
       <c r="I62" t="n">
-        <v>16.806</v>
+        <v>17.26</v>
       </c>
       <c r="J62" t="n">
-        <v>15797</v>
+        <v>17178</v>
       </c>
       <c r="K62" t="n">
-        <v>0.417</v>
+        <v>0.454</v>
       </c>
       <c r="L62" t="n">
-        <v>20690</v>
+        <v>20778</v>
       </c>
       <c r="M62" t="n">
-        <v>0.547</v>
+        <v>0.549</v>
       </c>
       <c r="N62" t="s">
         <v>407</v>
@@ -5543,7 +5535,7 @@
         <v>411</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>43965</v>
+        <v>43968</v>
       </c>
       <c r="D63" t="s">
         <v>412</v>
@@ -5553,25 +5545,25 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H63" t="n">
-        <v>618066</v>
+        <v>662375</v>
       </c>
       <c r="I63" t="n">
-        <v>60.614</v>
+        <v>64.96</v>
       </c>
       <c r="J63" t="n">
-        <v>17742</v>
+        <v>8907</v>
       </c>
       <c r="K63" t="n">
-        <v>1.74</v>
+        <v>0.874</v>
       </c>
       <c r="L63" t="n">
-        <v>14331</v>
+        <v>15496</v>
       </c>
       <c r="M63" t="n">
-        <v>1.405</v>
+        <v>1.52</v>
       </c>
       <c r="N63" t="s">
         <v>413</v>
@@ -5594,7 +5586,7 @@
         <v>417</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D64" t="s">
         <v>418</v>
@@ -5604,25 +5596,25 @@
       </c>
       <c r="F64"/>
       <c r="G64" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H64" t="n">
-        <v>161695</v>
+        <v>166182</v>
       </c>
       <c r="I64" t="n">
-        <v>56.123</v>
+        <v>57.681</v>
       </c>
       <c r="J64" t="n">
-        <v>4125</v>
+        <v>4487</v>
       </c>
       <c r="K64" t="n">
-        <v>1.432</v>
+        <v>1.557</v>
       </c>
       <c r="L64" t="n">
-        <v>4379</v>
+        <v>4413</v>
       </c>
       <c r="M64" t="n">
-        <v>1.52</v>
+        <v>1.532</v>
       </c>
       <c r="N64" t="s">
         <v>419</v>
@@ -5631,7 +5623,7 @@
         <v>420</v>
       </c>
       <c r="P64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q64" t="s">
         <v>421</v>
@@ -5698,7 +5690,7 @@
         <v>429</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D66" t="s">
         <v>430</v>
@@ -5708,25 +5700,25 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H66" t="n">
-        <v>7147014</v>
+        <v>7352316</v>
       </c>
       <c r="I66" t="n">
-        <v>48.974</v>
+        <v>50.381</v>
       </c>
       <c r="J66" t="n">
-        <v>230926</v>
+        <v>205302</v>
       </c>
       <c r="K66" t="n">
-        <v>1.582</v>
+        <v>1.407</v>
       </c>
       <c r="L66" t="n">
-        <v>215750</v>
+        <v>220987</v>
       </c>
       <c r="M66" t="n">
-        <v>1.478</v>
+        <v>1.514</v>
       </c>
       <c r="N66" t="s">
         <v>431</v>
@@ -5749,7 +5741,7 @@
         <v>435</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>43968</v>
+        <v>43969</v>
       </c>
       <c r="D67" t="s">
         <v>436</v>
@@ -5759,25 +5751,25 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H67" t="n">
-        <v>49374</v>
+        <v>51118</v>
       </c>
       <c r="I67" t="n">
-        <v>3.812</v>
+        <v>3.947</v>
       </c>
       <c r="J67" t="n">
-        <v>1135</v>
+        <v>1744</v>
       </c>
       <c r="K67" t="n">
-        <v>0.088</v>
+        <v>0.135</v>
       </c>
       <c r="L67" t="n">
-        <v>993</v>
+        <v>1188</v>
       </c>
       <c r="M67" t="n">
-        <v>0.077</v>
+        <v>0.092</v>
       </c>
       <c r="N67" t="s">
         <v>437</v>
@@ -5800,7 +5792,7 @@
         <v>441</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>43968</v>
+        <v>43970</v>
       </c>
       <c r="D68" t="s">
         <v>442</v>
@@ -5810,25 +5802,25 @@
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H68" t="n">
-        <v>586405</v>
+        <v>618084</v>
       </c>
       <c r="I68" t="n">
-        <v>16.844</v>
+        <v>17.754</v>
       </c>
       <c r="J68" t="n">
-        <v>38382</v>
+        <v>16130</v>
       </c>
       <c r="K68" t="n">
-        <v>1.102</v>
+        <v>0.463</v>
       </c>
       <c r="L68" t="n">
-        <v>19537</v>
+        <v>19387</v>
       </c>
       <c r="M68" t="n">
-        <v>0.561</v>
+        <v>0.557</v>
       </c>
       <c r="N68" t="s">
         <v>41</v>
@@ -5837,7 +5829,7 @@
         <v>442</v>
       </c>
       <c r="P68" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q68" t="s">
         <v>443</v>
@@ -5851,7 +5843,7 @@
         <v>445</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D69" t="s">
         <v>446</v>
@@ -5863,25 +5855,25 @@
         <v>448</v>
       </c>
       <c r="G69" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H69" t="n">
-        <v>29506</v>
+        <v>30436</v>
       </c>
       <c r="I69" t="n">
-        <v>1.762</v>
+        <v>1.818</v>
       </c>
       <c r="J69" t="n">
-        <v>1072</v>
+        <v>930</v>
       </c>
       <c r="K69" t="n">
-        <v>0.064</v>
+        <v>0.056</v>
       </c>
       <c r="L69" t="n">
-        <v>1002</v>
+        <v>978</v>
       </c>
       <c r="M69" t="n">
-        <v>0.06</v>
+        <v>0.058</v>
       </c>
       <c r="N69" t="s">
         <v>449</v>
@@ -5904,7 +5896,7 @@
         <v>454</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>43968</v>
+        <v>43970</v>
       </c>
       <c r="D70" t="s">
         <v>455</v>
@@ -5916,25 +5908,25 @@
         <v>456</v>
       </c>
       <c r="G70" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H70" t="n">
-        <v>181272</v>
+        <v>190683</v>
       </c>
       <c r="I70" t="n">
-        <v>26.64</v>
+        <v>28.023</v>
       </c>
       <c r="J70" t="n">
-        <v>6526</v>
+        <v>5298</v>
       </c>
       <c r="K70" t="n">
-        <v>0.959</v>
+        <v>0.779</v>
       </c>
       <c r="L70" t="n">
-        <v>5811</v>
+        <v>5626</v>
       </c>
       <c r="M70" t="n">
-        <v>0.854</v>
+        <v>0.827</v>
       </c>
       <c r="N70" t="s">
         <v>41</v>
@@ -5943,7 +5935,7 @@
         <v>457</v>
       </c>
       <c r="P70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q70" t="s">
         <v>458</v>
@@ -5990,7 +5982,7 @@
         <v>462</v>
       </c>
       <c r="P71" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q71" t="s">
         <v>463</v>
@@ -6051,7 +6043,7 @@
         <v>468</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>43968</v>
+        <v>43970</v>
       </c>
       <c r="D73" t="s">
         <v>469</v>
@@ -6061,25 +6053,25 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H73" t="n">
-        <v>142462</v>
+        <v>145474</v>
       </c>
       <c r="I73" t="n">
-        <v>26.094</v>
+        <v>26.645</v>
       </c>
       <c r="J73" t="n">
-        <v>2476</v>
+        <v>2041</v>
       </c>
       <c r="K73" t="n">
-        <v>0.454</v>
+        <v>0.374</v>
       </c>
       <c r="L73" t="n">
-        <v>3229</v>
+        <v>3252</v>
       </c>
       <c r="M73" t="n">
-        <v>0.591</v>
+        <v>0.596</v>
       </c>
       <c r="N73" t="s">
         <v>471</v>
@@ -6102,7 +6094,7 @@
         <v>476</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>43968</v>
+        <v>43969</v>
       </c>
       <c r="D74" t="s">
         <v>477</v>
@@ -6112,25 +6104,25 @@
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H74" t="n">
-        <v>69842</v>
+        <v>70970</v>
       </c>
       <c r="I74" t="n">
-        <v>33.595</v>
+        <v>34.138</v>
       </c>
       <c r="J74" t="n">
-        <v>479</v>
+        <v>1128</v>
       </c>
       <c r="K74" t="n">
-        <v>0.23</v>
+        <v>0.543</v>
       </c>
       <c r="L74" t="n">
-        <v>925</v>
+        <v>918</v>
       </c>
       <c r="M74" t="n">
-        <v>0.445</v>
+        <v>0.442</v>
       </c>
       <c r="N74" t="s">
         <v>479</v>
@@ -6153,7 +6145,7 @@
         <v>483</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>43968</v>
+        <v>43969</v>
       </c>
       <c r="D75" t="s">
         <v>484</v>
@@ -6165,25 +6157,25 @@
         <v>486</v>
       </c>
       <c r="G75" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H75" t="n">
-        <v>460873</v>
+        <v>475071</v>
       </c>
       <c r="I75" t="n">
-        <v>7.771</v>
+        <v>8.01</v>
       </c>
       <c r="J75" t="n">
-        <v>21314</v>
+        <v>14198</v>
       </c>
       <c r="K75" t="n">
-        <v>0.359</v>
+        <v>0.239</v>
       </c>
       <c r="L75" t="n">
-        <v>17077</v>
+        <v>17001</v>
       </c>
       <c r="M75" t="n">
-        <v>0.288</v>
+        <v>0.287</v>
       </c>
       <c r="N75" t="s">
         <v>485</v>
@@ -6192,7 +6184,7 @@
         <v>487</v>
       </c>
       <c r="P75" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q75" t="s">
         <v>488</v>
@@ -6206,7 +6198,7 @@
         <v>490</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D76" t="s">
         <v>491</v>
@@ -6216,22 +6208,22 @@
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H76" t="n">
-        <v>753211</v>
+        <v>765574</v>
       </c>
       <c r="I76" t="n">
-        <v>14.691</v>
+        <v>14.932</v>
       </c>
       <c r="J76" t="n">
-        <v>5558</v>
+        <v>12363</v>
       </c>
       <c r="K76" t="n">
-        <v>0.108</v>
+        <v>0.241</v>
       </c>
       <c r="L76" t="n">
-        <v>12103</v>
+        <v>12098</v>
       </c>
       <c r="M76" t="n">
         <v>0.236</v>
@@ -6337,7 +6329,7 @@
         <v>504</v>
       </c>
       <c r="P78" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q78" t="s">
         <v>506</v>
@@ -6351,7 +6343,7 @@
         <v>508</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>43967</v>
+        <v>43969</v>
       </c>
       <c r="D79" t="s">
         <v>509</v>
@@ -6361,25 +6353,25 @@
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H79" t="n">
-        <v>344592</v>
+        <v>350091</v>
       </c>
       <c r="I79" t="n">
-        <v>39.816</v>
+        <v>40.451</v>
       </c>
       <c r="J79" t="n">
-        <v>2699</v>
+        <v>2544</v>
       </c>
       <c r="K79" t="n">
-        <v>0.312</v>
+        <v>0.294</v>
       </c>
       <c r="L79" t="n">
-        <v>4518</v>
+        <v>4374</v>
       </c>
       <c r="M79" t="n">
-        <v>0.522</v>
+        <v>0.505</v>
       </c>
       <c r="N79" t="s">
         <v>510</v>
@@ -6402,7 +6394,7 @@
         <v>514</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>43968</v>
+        <v>43969</v>
       </c>
       <c r="D80" t="s">
         <v>515</v>
@@ -6412,25 +6404,25 @@
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H80" t="n">
-        <v>69395</v>
+        <v>69657</v>
       </c>
       <c r="I80" t="n">
-        <v>2.914</v>
+        <v>2.925</v>
       </c>
       <c r="J80" t="n">
-        <v>189</v>
+        <v>262</v>
       </c>
       <c r="K80" t="n">
-        <v>0.008</v>
+        <v>0.011</v>
       </c>
       <c r="L80" t="n">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="M80" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="N80" t="s">
         <v>516</v>
@@ -6490,7 +6482,7 @@
         <v>525</v>
       </c>
       <c r="P81" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q81" t="s">
         <v>526</v>
@@ -6551,7 +6543,7 @@
         <v>533</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>43966</v>
+        <v>43968</v>
       </c>
       <c r="D83" t="s">
         <v>534</v>
@@ -6561,25 +6553,25 @@
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H83" t="n">
-        <v>39778</v>
+        <v>41620</v>
       </c>
       <c r="I83" t="n">
-        <v>3.366</v>
+        <v>3.522</v>
       </c>
       <c r="J83" t="n">
-        <v>1916</v>
+        <v>1061</v>
       </c>
       <c r="K83" t="n">
-        <v>0.162</v>
+        <v>0.09</v>
       </c>
       <c r="L83" t="n">
-        <v>1497</v>
+        <v>1193</v>
       </c>
       <c r="M83" t="n">
-        <v>0.127</v>
+        <v>0.101</v>
       </c>
       <c r="N83" t="s">
         <v>535</v>
@@ -6602,7 +6594,7 @@
         <v>540</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D84" t="s">
         <v>541</v>
@@ -6612,25 +6604,25 @@
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H84" t="n">
-        <v>1650135</v>
+        <v>1675517</v>
       </c>
       <c r="I84" t="n">
-        <v>19.565</v>
+        <v>19.866</v>
       </c>
       <c r="J84" t="n">
-        <v>25141</v>
+        <v>25382</v>
       </c>
       <c r="K84" t="n">
-        <v>0.298</v>
+        <v>0.301</v>
       </c>
       <c r="L84" t="n">
-        <v>35259</v>
+        <v>33549</v>
       </c>
       <c r="M84" t="n">
-        <v>0.418</v>
+        <v>0.398</v>
       </c>
       <c r="N84" t="s">
         <v>542</v>
@@ -6653,7 +6645,7 @@
         <v>547</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>43967</v>
+        <v>43969</v>
       </c>
       <c r="D85" t="s">
         <v>548</v>
@@ -6665,25 +6657,21 @@
         <v>550</v>
       </c>
       <c r="G85" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H85" t="n">
-        <v>72774</v>
+        <v>74098</v>
       </c>
       <c r="I85" t="n">
-        <v>1.591</v>
-      </c>
-      <c r="J85" t="n">
-        <v>2044</v>
-      </c>
-      <c r="K85" t="n">
-        <v>0.045</v>
-      </c>
+        <v>1.62</v>
+      </c>
+      <c r="J85"/>
+      <c r="K85"/>
       <c r="L85" t="n">
-        <v>2144</v>
+        <v>1662</v>
       </c>
       <c r="M85" t="n">
-        <v>0.047</v>
+        <v>0.036</v>
       </c>
       <c r="N85" t="s">
         <v>549</v>
@@ -6706,7 +6694,7 @@
         <v>554</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D86" t="s">
         <v>555</v>
@@ -6716,25 +6704,25 @@
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H86" t="n">
-        <v>232899</v>
+        <v>239961</v>
       </c>
       <c r="I86" t="n">
-        <v>5.325</v>
+        <v>5.487</v>
       </c>
       <c r="J86" t="n">
-        <v>5098</v>
+        <v>7062</v>
       </c>
       <c r="K86" t="n">
-        <v>0.117</v>
+        <v>0.161</v>
       </c>
       <c r="L86" t="n">
-        <v>7335</v>
+        <v>7522</v>
       </c>
       <c r="M86" t="n">
-        <v>0.168</v>
+        <v>0.172</v>
       </c>
       <c r="N86" t="s">
         <v>556</v>
@@ -6794,7 +6782,7 @@
         <v>564</v>
       </c>
       <c r="P87" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q87" t="s">
         <v>565</v>
@@ -6808,7 +6796,7 @@
         <v>566</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D88" t="s">
         <v>567</v>
@@ -6818,25 +6806,25 @@
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H88" t="n">
-        <v>2682716</v>
+        <v>2772552</v>
       </c>
       <c r="I88" t="n">
-        <v>39.518</v>
+        <v>40.841</v>
       </c>
       <c r="J88" t="n">
-        <v>100678</v>
+        <v>89784</v>
       </c>
       <c r="K88" t="n">
-        <v>1.483</v>
+        <v>1.323</v>
       </c>
       <c r="L88" t="n">
-        <v>108707</v>
+        <v>109344</v>
       </c>
       <c r="M88" t="n">
-        <v>1.601</v>
+        <v>1.611</v>
       </c>
       <c r="N88" t="s">
         <v>563</v>
@@ -6859,7 +6847,7 @@
         <v>571</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>43968</v>
+        <v>43969</v>
       </c>
       <c r="D89" t="s">
         <v>572</v>
@@ -6869,25 +6857,25 @@
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H89" t="n">
-        <v>11499203</v>
+        <v>11834508</v>
       </c>
       <c r="I89" t="n">
-        <v>34.741</v>
+        <v>35.754</v>
       </c>
       <c r="J89" t="n">
-        <v>422024</v>
+        <v>338020</v>
       </c>
       <c r="K89" t="n">
-        <v>1.275</v>
+        <v>1.021</v>
       </c>
       <c r="L89" t="n">
-        <v>362720</v>
+        <v>352746</v>
       </c>
       <c r="M89" t="n">
-        <v>1.096</v>
+        <v>1.066</v>
       </c>
       <c r="N89" t="s">
         <v>573</v>
@@ -6910,107 +6898,111 @@
         <v>577</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>43968</v>
+        <v>43969</v>
       </c>
       <c r="D90" t="s">
+        <v>237</v>
+      </c>
+      <c r="E90" t="s">
         <v>578</v>
-      </c>
-      <c r="E90" t="s">
-        <v>579</v>
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H90" t="n">
-        <v>10847778</v>
+        <v>11282781</v>
       </c>
       <c r="I90" t="n">
-        <v>32.772</v>
-      </c>
-      <c r="J90"/>
-      <c r="K90"/>
+        <v>34.087</v>
+      </c>
+      <c r="J90" t="n">
+        <v>435003</v>
+      </c>
+      <c r="K90" t="n">
+        <v>1.314</v>
+      </c>
       <c r="L90"/>
       <c r="M90"/>
       <c r="N90" t="s">
+        <v>578</v>
+      </c>
+      <c r="O90" t="s">
         <v>579</v>
-      </c>
-      <c r="O90" t="s">
-        <v>580</v>
       </c>
       <c r="P90" t="s">
         <v>22</v>
       </c>
       <c r="Q90" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
+        <v>581</v>
+      </c>
+      <c r="B91" t="s">
         <v>582</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" s="1" t="n">
+        <v>43970</v>
+      </c>
+      <c r="D91" t="s">
         <v>583</v>
       </c>
-      <c r="C91" s="1" t="n">
-        <v>43969</v>
-      </c>
-      <c r="D91" t="s">
-        <v>584</v>
-      </c>
       <c r="E91" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H91" t="n">
-        <v>33861</v>
+        <v>34384</v>
       </c>
       <c r="I91" t="n">
-        <v>9.748</v>
+        <v>9.898</v>
       </c>
       <c r="J91" t="n">
-        <v>825</v>
+        <v>523</v>
       </c>
       <c r="K91" t="n">
-        <v>0.237</v>
+        <v>0.151</v>
       </c>
       <c r="L91" t="n">
-        <v>738</v>
+        <v>755</v>
       </c>
       <c r="M91" t="n">
-        <v>0.212</v>
+        <v>0.217</v>
       </c>
       <c r="N91" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O91" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="P91" t="s">
         <v>22</v>
       </c>
       <c r="Q91" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
+        <v>586</v>
+      </c>
+      <c r="B92" t="s">
         <v>587</v>
-      </c>
-      <c r="B92" t="s">
-        <v>588</v>
       </c>
       <c r="C92" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="D92" t="s">
+        <v>588</v>
+      </c>
+      <c r="E92" t="s">
         <v>589</v>
-      </c>
-      <c r="E92" t="s">
-        <v>590</v>
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
@@ -7031,69 +7023,69 @@
         <v>0.112</v>
       </c>
       <c r="N92" t="s">
+        <v>589</v>
+      </c>
+      <c r="O92" t="s">
         <v>590</v>
       </c>
-      <c r="O92" t="s">
+      <c r="P92" t="s">
         <v>591</v>
       </c>
-      <c r="P92" t="s">
+      <c r="Q92" t="s">
         <v>592</v>
-      </c>
-      <c r="Q92" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
+        <v>593</v>
+      </c>
+      <c r="B93" t="s">
         <v>594</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" s="1" t="n">
+        <v>43969</v>
+      </c>
+      <c r="D93" t="s">
         <v>595</v>
       </c>
-      <c r="C93" s="1" t="n">
-        <v>43967</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>596</v>
       </c>
-      <c r="E93" t="s">
+      <c r="F93" t="s">
         <v>597</v>
       </c>
-      <c r="F93" t="s">
+      <c r="G93" t="n">
+        <v>12</v>
+      </c>
+      <c r="H93" t="n">
+        <v>13104</v>
+      </c>
+      <c r="I93" t="n">
+        <v>0.882</v>
+      </c>
+      <c r="J93" t="n">
+        <v>540</v>
+      </c>
+      <c r="K93" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="L93" t="n">
+        <v>358</v>
+      </c>
+      <c r="M93" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="N93" t="s">
+        <v>596</v>
+      </c>
+      <c r="O93" t="s">
         <v>598</v>
-      </c>
-      <c r="G93" t="n">
-        <v>10</v>
-      </c>
-      <c r="H93" t="n">
-        <v>12275</v>
-      </c>
-      <c r="I93" t="n">
-        <v>0.826</v>
-      </c>
-      <c r="J93" t="n">
-        <v>874</v>
-      </c>
-      <c r="K93" t="n">
-        <v>0.059</v>
-      </c>
-      <c r="L93" t="n">
-        <v>383</v>
-      </c>
-      <c r="M93" t="n">
-        <v>0.026</v>
-      </c>
-      <c r="N93" t="s">
-        <v>597</v>
-      </c>
-      <c r="O93" t="s">
-        <v>599</v>
       </c>
       <c r="P93" t="s">
         <v>22</v>
       </c>
       <c r="Q93" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testing data for 2020-05-24
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Argentina - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/22-05-20_reporte_matutino_covid_19.pdf</t>
+    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/23-05-20_reporte-matutino_covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Argentina</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200522161914/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200523150733/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200522192126/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200524003522/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -187,7 +187,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-22-maya-vyzdoroveli-i-vypisany-12-tys-833-patsienta/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-23-maya-vyzdoroveli-i-vypisany-13-tys-528-patsientov/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -278,7 +278,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200522161923/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200524082600/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -301,7 +301,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200522161925/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200524003530/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -389,7 +389,7 @@
     <t xml:space="preserve">Croatia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200522161941/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200523150747/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -449,7 +449,7 @@
     <t xml:space="preserve">Denmark - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200522171325/https://www.ssi.dk/sygdomme-beredskab-og-forskning/sygdomsovervaagning/c/covid19-overvaagning</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200523151920/https://www.ssi.dk/sygdomme-beredskab-og-forskning/sygdomsovervaagning/c/covid19-overvaagning</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -546,7 +546,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_May-22-Eng-V1.pdf</t>
+    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_May-23-Eng-V2.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -685,7 +685,7 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200521/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200523/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -919,13 +919,13 @@
     <t xml:space="preserve">Japan - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11462.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11468.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
   </si>
   <si>
-    <t xml:space="preserve">See Table: 国内の発生状況, column 1 '検査実施人数'. Daily change figure provided for this date is not consistent with the cumulative totals for today and the previous day.</t>
+    <t xml:space="preserve">See Table: 国内の発生状況, column 1 '検査実施人数'.</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare</t>
@@ -943,7 +943,7 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000632897.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000633023.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">The cumulative total reported in the press release now matches the cumulative total calculated from the weekly and daily figures reported by the MOH.</t>
@@ -1019,7 +1019,7 @@
     <t xml:space="preserve">Lithuania - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200522162056/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200523094205/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -1035,7 +1035,7 @@
     <t xml:space="preserve">Luxembourg - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200522162059/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200524003609/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg Government situation update</t>
@@ -1079,13 +1079,13 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/561317043971945/videos/663407067832877/</t>
+    <t xml:space="preserve">https://www.facebook.com/561317043971945/videos/242937120374212/</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Ministry of Health</t>
   </si>
   <si>
-    <t xml:space="preserve">Numbers visible in video at time: 1:40</t>
+    <t xml:space="preserve">Numbers visible in video at time: 0:50</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Ministry of Health Official Facebook page</t>
@@ -1227,7 +1227,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200522162640/https://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200523151817/https://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1272,7 +1272,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200522162646/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200524082815/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1330,7 +1330,7 @@
     <t xml:space="preserve">Peru - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/162379-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-108-769-en-el-peru-comunicado-n-107</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/164292-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-115-754-comunicado-n-109</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1359,14 +1359,13 @@
     <t xml:space="preserve">Department of Health (DOH) Philippines</t>
   </si>
   <si>
-    <t xml:space="preserve">Total individuals tested does not sum to positive + negative + equivocal + invalid individuals, as in past figures of the series.</t>
+    <t xml:space="preserve">The DOH reports the cumulative samples and unique individuals tested.</t>
   </si>
   <si>
     <t xml:space="preserve">The Ministry of Health (MOH) provides a daily snapshot of testing capacity detailing the total number of individuals tested and the total number of tests conducted. 
-The total number of individuals tested is the sum of positive, negative, equivocal, and invalid individuals. No definitions of equivocal and invalid individual tests are given, hence our figures only report the sum of individuals who have tested positive or negative.
+The total number of individuals tested is the sum of positive, negative, equivocal, and invalid individuals. No definitions of equivocal and invalid individual tests are given, hence our figures only report the sum of individuals who have tested positive or negative. From 22nd May, the DOH stopped reporting figures on equivocal and invalid individuals; the DOH provides the cumulative samples and unique indivdiuals tested, where cumulative unique individuals = cumulative positive + cumulative negative individuals. 
 The source provides a breakdown of both i) the number of individuals tested and ii) the total tests conducted, by laboratory. We are not aware of any aggregation issues. 
-The DOH used to report the number of cases tested in a previous dashboard, but stopped on 4th April. This previous breakdown of the test results and COVID-19 dashboard have both been removed. We became aware of this new tracker on the 13th April with data 'as of April 11 2020, 12am'. No previous snapshots of the dashboard are available using web archive, therefore the series starts from the 11th April - the earliest date from which we have access to the data. 
-No newly submitted reports as of 21 May. Latest testing data available is from 15 May 2020.</t>
+The DOH used to report the number of cases tested in a previous dashboard, but stopped on 4th April. This previous breakdown of the test results and COVID-19 dashboard have both been removed. We became aware of this new tracker on the 13th April with data 'as of April 11 2020, 12am'. No previous snapshots of the dashboard are available using web archive, therefore the series starts from the 11th April - the earliest date from which we have access to the data.</t>
   </si>
   <si>
     <t xml:space="preserve">POL</t>
@@ -1375,7 +1374,7 @@
     <t xml:space="preserve">Poland - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://raw.githubusercontent.com/anuszka/COVID-19-MZ_GOV_PL/master/data/cor.2020.05.22.csv</t>
+    <t xml:space="preserve">https://raw.githubusercontent.com/anuszka/COVID-19-MZ_GOV_PL/master/data/cor.2020.05.24.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1420,10 +1419,13 @@
     <t xml:space="preserve">Qatar - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200522174802/https://covid19.moph.gov.qa/EN/Pages/default.aspx</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200523154024/https://covid19.moph.gov.qa/EN/Pages/default.aspx</t>
   </si>
   <si>
     <t xml:space="preserve">Qatar Ministry of Public Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The web archive snapshot does not display the correct figures; displaying test figures for 20th May.</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.moph.gov.qa/</t>
@@ -1458,7 +1460,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14517</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14527</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1503,9 +1505,6 @@
     <t xml:space="preserve">https://covid19.moh.gov.sa/en/</t>
   </si>
   <si>
-    <t xml:space="preserve">There was no update of Saudi Arabia's testing figures on 21st May</t>
-  </si>
-  <si>
     <t xml:space="preserve">The Saudi Arabian Ministry of Health provides a dashboard detailing the total number of tests. Whether units refer to people or tests conducted is unclear.
 The exact date these cumulative figures date back to is also unknown.
 There is no explicit mention of whether the figures include only PCR tests or other kinds of test.</t>
@@ -1588,7 +1587,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200522162657/https://korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200524082827/https://korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Center of Health Information and the Office of the Government of the Slovak Republic</t>
@@ -1662,7 +1661,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367309&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367313&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1745,7 +1744,7 @@
     <t xml:space="preserve">Taiwan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/_JH3cztOCLyrjf4oMVCvdw?typeid=9</t>
+    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/S1_I5sEXF06LuRduBwk-gg?typeid=9</t>
   </si>
   <si>
     <t xml:space="preserve">Taiwan Centers for Disease Control (CDC)</t>
@@ -1768,7 +1767,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200522162756/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200524003803/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1835,7 +1834,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200522192516/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200524003807/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1859,7 +1858,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1263561752576434178</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1263945662338646018</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
@@ -1883,7 +1882,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200522162804/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200524082920/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1928,7 +1927,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200522162807/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200524004223/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
   </si>
   <si>
     <t xml:space="preserve">The number of tests performed, including tests posted or delivered but not yet returned and/or processed.</t>
@@ -1975,7 +1974,7 @@
     <t xml:space="preserve">United States - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200520183014/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200523094405/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
   </si>
   <si>
     <t xml:space="preserve">United States CDC</t>
@@ -1996,7 +1995,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-32</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-33</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2448,7 +2447,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2458,21 +2457,25 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H2" t="n">
-        <v>121278</v>
+        <v>125893</v>
       </c>
       <c r="I2" t="n">
-        <v>2.683</v>
-      </c>
-      <c r="J2"/>
-      <c r="K2"/>
+        <v>2.786</v>
+      </c>
+      <c r="J2" t="n">
+        <v>4615</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.102</v>
+      </c>
       <c r="L2" t="n">
-        <v>3484</v>
+        <v>3647</v>
       </c>
       <c r="M2" t="n">
-        <v>0.077</v>
+        <v>0.081</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -2546,7 +2549,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -2556,21 +2559,25 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H4" t="n">
-        <v>390488</v>
+        <v>396363</v>
       </c>
       <c r="I4" t="n">
-        <v>43.357</v>
-      </c>
-      <c r="J4"/>
-      <c r="K4"/>
+        <v>44.009</v>
+      </c>
+      <c r="J4" t="n">
+        <v>5875</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.652</v>
+      </c>
       <c r="L4" t="n">
-        <v>5591</v>
+        <v>5567</v>
       </c>
       <c r="M4" t="n">
-        <v>0.621</v>
+        <v>0.618</v>
       </c>
       <c r="N4" t="s">
         <v>34</v>
@@ -2593,7 +2600,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2603,21 +2610,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H5" t="n">
-        <v>269179</v>
+        <v>276552</v>
       </c>
       <c r="I5" t="n">
-        <v>158.193</v>
-      </c>
-      <c r="J5"/>
-      <c r="K5"/>
+        <v>162.526</v>
+      </c>
+      <c r="J5" t="n">
+        <v>7373</v>
+      </c>
+      <c r="K5" t="n">
+        <v>4.333</v>
+      </c>
       <c r="L5" t="n">
-        <v>6662</v>
+        <v>6623</v>
       </c>
       <c r="M5" t="n">
-        <v>3.915</v>
+        <v>3.892</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
@@ -2691,7 +2702,7 @@
         <v>54</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D7" t="s">
         <v>55</v>
@@ -2701,21 +2712,25 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H7" t="n">
-        <v>419004</v>
+        <v>434618</v>
       </c>
       <c r="I7" t="n">
-        <v>44.342</v>
-      </c>
-      <c r="J7"/>
-      <c r="K7"/>
+        <v>45.995</v>
+      </c>
+      <c r="J7" t="n">
+        <v>15614</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1.652</v>
+      </c>
       <c r="L7" t="n">
-        <v>13818</v>
+        <v>14032</v>
       </c>
       <c r="M7" t="n">
-        <v>1.462</v>
+        <v>1.485</v>
       </c>
       <c r="N7" t="s">
         <v>56</v>
@@ -2738,7 +2753,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>43971</v>
+        <v>43972</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
@@ -2748,25 +2763,25 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H8" t="n">
-        <v>611701</v>
+        <v>620063</v>
       </c>
       <c r="I8" t="n">
-        <v>52.78</v>
+        <v>53.502</v>
       </c>
       <c r="J8" t="n">
-        <v>12782</v>
+        <v>6895</v>
       </c>
       <c r="K8" t="n">
-        <v>1.103</v>
+        <v>0.595</v>
       </c>
       <c r="L8" t="n">
-        <v>12134</v>
+        <v>11001</v>
       </c>
       <c r="M8" t="n">
-        <v>1.047</v>
+        <v>0.949</v>
       </c>
       <c r="N8" t="s">
         <v>62</v>
@@ -2789,7 +2804,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>43972</v>
+        <v>43974</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
@@ -2801,25 +2816,25 @@
         <v>69</v>
       </c>
       <c r="G9" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H9" t="n">
-        <v>11273</v>
+        <v>12001</v>
       </c>
       <c r="I9" t="n">
-        <v>0.966</v>
+        <v>1.028</v>
       </c>
       <c r="J9" t="n">
-        <v>268</v>
+        <v>336</v>
       </c>
       <c r="K9" t="n">
-        <v>0.023</v>
+        <v>0.029</v>
       </c>
       <c r="L9" t="n">
-        <v>259</v>
+        <v>298</v>
       </c>
       <c r="M9" t="n">
-        <v>0.022</v>
+        <v>0.026</v>
       </c>
       <c r="N9" t="s">
         <v>41</v>
@@ -2889,7 +2904,7 @@
         <v>81</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>43973</v>
+        <v>43975</v>
       </c>
       <c r="D11" t="s">
         <v>82</v>
@@ -2899,21 +2914,25 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H11" t="n">
-        <v>71605</v>
+        <v>74096</v>
       </c>
       <c r="I11" t="n">
-        <v>10.305</v>
-      </c>
-      <c r="J11"/>
-      <c r="K11"/>
+        <v>10.664</v>
+      </c>
+      <c r="J11" t="n">
+        <v>886</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.128</v>
+      </c>
       <c r="L11" t="n">
-        <v>1184</v>
+        <v>1217</v>
       </c>
       <c r="M11" t="n">
-        <v>0.17</v>
+        <v>0.175</v>
       </c>
       <c r="N11" t="s">
         <v>84</v>
@@ -2936,7 +2955,7 @@
         <v>88</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D12" t="s">
         <v>89</v>
@@ -2946,25 +2965,25 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H12" t="n">
-        <v>1401564</v>
+        <v>1431911</v>
       </c>
       <c r="I12" t="n">
-        <v>37.135</v>
+        <v>37.939</v>
       </c>
       <c r="J12" t="n">
-        <v>26514</v>
+        <v>30347</v>
       </c>
       <c r="K12" t="n">
-        <v>0.703</v>
+        <v>0.804</v>
       </c>
       <c r="L12" t="n">
-        <v>24093</v>
+        <v>23773</v>
       </c>
       <c r="M12" t="n">
-        <v>0.638</v>
+        <v>0.63</v>
       </c>
       <c r="N12" t="s">
         <v>90</v>
@@ -2987,7 +3006,7 @@
         <v>95</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D13" t="s">
         <v>96</v>
@@ -2999,25 +3018,25 @@
         <v>97</v>
       </c>
       <c r="G13" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H13" t="n">
-        <v>442093</v>
+        <v>457332</v>
       </c>
       <c r="I13" t="n">
-        <v>23.127</v>
+        <v>23.924</v>
       </c>
       <c r="J13" t="n">
-        <v>16090</v>
+        <v>15239</v>
       </c>
       <c r="K13" t="n">
-        <v>0.842</v>
+        <v>0.797</v>
       </c>
       <c r="L13" t="n">
-        <v>14369</v>
+        <v>15287</v>
       </c>
       <c r="M13" t="n">
-        <v>0.752</v>
+        <v>0.8</v>
       </c>
       <c r="N13" t="s">
         <v>98</v>
@@ -3040,7 +3059,7 @@
         <v>102</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>43972</v>
+        <v>43974</v>
       </c>
       <c r="D14" t="s">
         <v>103</v>
@@ -3050,25 +3069,25 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H14" t="n">
-        <v>222210</v>
+        <v>243119</v>
       </c>
       <c r="I14" t="n">
-        <v>4.367</v>
+        <v>4.778</v>
       </c>
       <c r="J14" t="n">
-        <v>7674</v>
+        <v>7171</v>
       </c>
       <c r="K14" t="n">
-        <v>0.151</v>
+        <v>0.141</v>
       </c>
       <c r="L14" t="n">
-        <v>6451</v>
+        <v>7572</v>
       </c>
       <c r="M14" t="n">
-        <v>0.127</v>
+        <v>0.149</v>
       </c>
       <c r="N14" t="s">
         <v>104</v>
@@ -3142,7 +3161,7 @@
         <v>115</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D16" t="s">
         <v>116</v>
@@ -3152,21 +3171,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H16" t="n">
-        <v>59911</v>
+        <v>60864</v>
       </c>
       <c r="I16" t="n">
-        <v>14.594</v>
-      </c>
-      <c r="J16"/>
-      <c r="K16"/>
+        <v>14.826</v>
+      </c>
+      <c r="J16" t="n">
+        <v>953</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.232</v>
+      </c>
       <c r="L16" t="n">
-        <v>1192</v>
+        <v>1206</v>
       </c>
       <c r="M16" t="n">
-        <v>0.29</v>
+        <v>0.294</v>
       </c>
       <c r="N16" t="s">
         <v>117</v>
@@ -3189,7 +3212,7 @@
         <v>122</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>43972</v>
+        <v>43973</v>
       </c>
       <c r="D17" t="s">
         <v>123</v>
@@ -3201,25 +3224,25 @@
         <v>125</v>
       </c>
       <c r="G17" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H17" t="n">
-        <v>90911</v>
+        <v>92629</v>
       </c>
       <c r="I17" t="n">
-        <v>8.026</v>
+        <v>8.178</v>
       </c>
       <c r="J17" t="n">
-        <v>1880</v>
+        <v>1718</v>
       </c>
       <c r="K17" t="n">
-        <v>0.166</v>
+        <v>0.152</v>
       </c>
       <c r="L17" t="n">
-        <v>1934</v>
+        <v>1828</v>
       </c>
       <c r="M17" t="n">
-        <v>0.171</v>
+        <v>0.161</v>
       </c>
       <c r="N17" t="s">
         <v>124</v>
@@ -3242,7 +3265,7 @@
         <v>129</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>43972</v>
+        <v>43974</v>
       </c>
       <c r="D18" t="s">
         <v>130</v>
@@ -3252,25 +3275,25 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H18" t="n">
-        <v>387127</v>
+        <v>399896</v>
       </c>
       <c r="I18" t="n">
-        <v>36.15</v>
+        <v>37.342</v>
       </c>
       <c r="J18" t="n">
-        <v>7149</v>
+        <v>4952</v>
       </c>
       <c r="K18" t="n">
-        <v>0.668</v>
+        <v>0.462</v>
       </c>
       <c r="L18" t="n">
-        <v>6409</v>
+        <v>6668</v>
       </c>
       <c r="M18" t="n">
-        <v>0.598</v>
+        <v>0.623</v>
       </c>
       <c r="N18" t="s">
         <v>41</v>
@@ -3293,7 +3316,7 @@
         <v>134</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D19" t="s">
         <v>135</v>
@@ -3303,25 +3326,25 @@
       </c>
       <c r="F19"/>
       <c r="G19" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H19" t="n">
-        <v>433971</v>
+        <v>442650</v>
       </c>
       <c r="I19" t="n">
-        <v>74.923</v>
+        <v>76.422</v>
       </c>
       <c r="J19" t="n">
-        <v>8870</v>
+        <v>8679</v>
       </c>
       <c r="K19" t="n">
-        <v>1.531</v>
+        <v>1.498</v>
       </c>
       <c r="L19" t="n">
-        <v>9297</v>
+        <v>9024</v>
       </c>
       <c r="M19" t="n">
-        <v>1.605</v>
+        <v>1.558</v>
       </c>
       <c r="N19" t="s">
         <v>137</v>
@@ -3444,7 +3467,7 @@
         <v>155</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>43972</v>
+        <v>43974</v>
       </c>
       <c r="D22" t="s">
         <v>156</v>
@@ -3454,25 +3477,25 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H22" t="n">
-        <v>74605</v>
+        <v>75780</v>
       </c>
       <c r="I22" t="n">
-        <v>56.24</v>
+        <v>57.126</v>
       </c>
       <c r="J22" t="n">
-        <v>881</v>
+        <v>530</v>
       </c>
       <c r="K22" t="n">
-        <v>0.664</v>
+        <v>0.4</v>
       </c>
       <c r="L22" t="n">
-        <v>932</v>
+        <v>896</v>
       </c>
       <c r="M22" t="n">
-        <v>0.703</v>
+        <v>0.675</v>
       </c>
       <c r="N22" t="s">
         <v>158</v>
@@ -3495,7 +3518,7 @@
         <v>163</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D23" t="s">
         <v>164</v>
@@ -3505,21 +3528,25 @@
       </c>
       <c r="F23"/>
       <c r="G23" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H23" t="n">
-        <v>73164</v>
+        <v>76962</v>
       </c>
       <c r="I23" t="n">
-        <v>0.636</v>
-      </c>
-      <c r="J23"/>
-      <c r="K23"/>
+        <v>0.669</v>
+      </c>
+      <c r="J23" t="n">
+        <v>3798</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.033</v>
+      </c>
       <c r="L23" t="n">
-        <v>3493</v>
+        <v>3544</v>
       </c>
       <c r="M23" t="n">
-        <v>0.03</v>
+        <v>0.031</v>
       </c>
       <c r="N23" t="s">
         <v>165</v>
@@ -3542,7 +3569,7 @@
         <v>169</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>43971</v>
+        <v>43972</v>
       </c>
       <c r="D24" t="s">
         <v>170</v>
@@ -3552,25 +3579,25 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H24" t="n">
-        <v>162217</v>
+        <v>165273</v>
       </c>
       <c r="I24" t="n">
-        <v>29.277</v>
+        <v>29.829</v>
       </c>
       <c r="J24" t="n">
-        <v>2996</v>
+        <v>2554</v>
       </c>
       <c r="K24" t="n">
-        <v>0.541</v>
+        <v>0.461</v>
       </c>
       <c r="L24" t="n">
-        <v>3197</v>
+        <v>3128</v>
       </c>
       <c r="M24" t="n">
-        <v>0.577</v>
+        <v>0.565</v>
       </c>
       <c r="N24" t="s">
         <v>172</v>
@@ -3797,7 +3824,7 @@
         <v>201</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D29" t="s">
         <v>202</v>
@@ -3807,21 +3834,25 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H29" t="n">
-        <v>144078</v>
+        <v>152998</v>
       </c>
       <c r="I29" t="n">
-        <v>13.823</v>
-      </c>
-      <c r="J29"/>
-      <c r="K29"/>
+        <v>14.679</v>
+      </c>
+      <c r="J29" t="n">
+        <v>8920</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.856</v>
+      </c>
       <c r="L29" t="n">
-        <v>3438</v>
+        <v>3816</v>
       </c>
       <c r="M29" t="n">
-        <v>0.33</v>
+        <v>0.366</v>
       </c>
       <c r="N29" t="s">
         <v>204</v>
@@ -3891,7 +3922,7 @@
         <v>215</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>43973</v>
+        <v>43975</v>
       </c>
       <c r="D31" t="s">
         <v>216</v>
@@ -3903,25 +3934,25 @@
         <v>218</v>
       </c>
       <c r="G31" t="n">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H31" t="n">
-        <v>155801</v>
+        <v>162925</v>
       </c>
       <c r="I31" t="n">
-        <v>16.128</v>
+        <v>16.865</v>
       </c>
       <c r="J31" t="n">
-        <v>8290</v>
+        <v>3665</v>
       </c>
       <c r="K31" t="n">
-        <v>0.858</v>
+        <v>0.379</v>
       </c>
       <c r="L31" t="n">
-        <v>4081</v>
+        <v>3970</v>
       </c>
       <c r="M31" t="n">
-        <v>0.422</v>
+        <v>0.411</v>
       </c>
       <c r="N31" t="s">
         <v>217</v>
@@ -3944,7 +3975,7 @@
         <v>223</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>43971</v>
+        <v>43973</v>
       </c>
       <c r="D32" t="s">
         <v>224</v>
@@ -3954,25 +3985,25 @@
       </c>
       <c r="F32"/>
       <c r="G32" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H32" t="n">
-        <v>58184</v>
+        <v>58745</v>
       </c>
       <c r="I32" t="n">
-        <v>170.503</v>
+        <v>172.147</v>
       </c>
       <c r="J32" t="n">
-        <v>597</v>
+        <v>491</v>
       </c>
       <c r="K32" t="n">
-        <v>1.749</v>
+        <v>1.439</v>
       </c>
       <c r="L32" t="n">
-        <v>371</v>
+        <v>292</v>
       </c>
       <c r="M32" t="n">
-        <v>1.087</v>
+        <v>0.856</v>
       </c>
       <c r="N32" t="s">
         <v>225</v>
@@ -4048,7 +4079,7 @@
         <v>234</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>43972</v>
+        <v>43974</v>
       </c>
       <c r="D34" t="s">
         <v>230</v>
@@ -4060,25 +4091,25 @@
         <v>232</v>
       </c>
       <c r="G34" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H34" t="n">
-        <v>2615920</v>
+        <v>2834798</v>
       </c>
       <c r="I34" t="n">
-        <v>1.896</v>
+        <v>2.054</v>
       </c>
       <c r="J34" t="n">
-        <v>103532</v>
+        <v>115364</v>
       </c>
       <c r="K34" t="n">
-        <v>0.075</v>
+        <v>0.084</v>
       </c>
       <c r="L34" t="n">
-        <v>95554</v>
+        <v>100074</v>
       </c>
       <c r="M34" t="n">
-        <v>0.069</v>
+        <v>0.073</v>
       </c>
       <c r="N34" t="s">
         <v>231</v>
@@ -4101,7 +4132,7 @@
         <v>236</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D35" t="s">
         <v>237</v>
@@ -4111,21 +4142,25 @@
       </c>
       <c r="F35"/>
       <c r="G35" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H35" t="n">
-        <v>168969</v>
+        <v>176035</v>
       </c>
       <c r="I35" t="n">
-        <v>0.618</v>
-      </c>
-      <c r="J35"/>
-      <c r="K35"/>
+        <v>0.644</v>
+      </c>
+      <c r="J35" t="n">
+        <v>7066</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.026</v>
+      </c>
       <c r="L35" t="n">
-        <v>5273</v>
+        <v>5758</v>
       </c>
       <c r="M35" t="n">
-        <v>0.019</v>
+        <v>0.021</v>
       </c>
       <c r="N35" t="s">
         <v>238</v>
@@ -4299,7 +4334,7 @@
         <v>261</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D39" t="s">
         <v>262</v>
@@ -4311,25 +4346,25 @@
         <v>264</v>
       </c>
       <c r="G39" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H39" t="n">
-        <v>2121847</v>
+        <v>2164426</v>
       </c>
       <c r="I39" t="n">
-        <v>35.094</v>
+        <v>35.798</v>
       </c>
       <c r="J39" t="n">
-        <v>42987</v>
+        <v>42579</v>
       </c>
       <c r="K39" t="n">
-        <v>0.711</v>
+        <v>0.704</v>
       </c>
       <c r="L39" t="n">
-        <v>37534</v>
+        <v>37808</v>
       </c>
       <c r="M39" t="n">
-        <v>0.621</v>
+        <v>0.625</v>
       </c>
       <c r="N39" t="s">
         <v>265</v>
@@ -4352,7 +4387,7 @@
         <v>268</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D40" t="s">
         <v>262</v>
@@ -4364,25 +4399,25 @@
         <v>264</v>
       </c>
       <c r="G40" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H40" t="n">
-        <v>3318778</v>
+        <v>3391188</v>
       </c>
       <c r="I40" t="n">
-        <v>54.89</v>
+        <v>56.088</v>
       </c>
       <c r="J40" t="n">
-        <v>75380</v>
+        <v>72410</v>
       </c>
       <c r="K40" t="n">
-        <v>1.247</v>
+        <v>1.198</v>
       </c>
       <c r="L40" t="n">
-        <v>63300</v>
+        <v>63761</v>
       </c>
       <c r="M40" t="n">
-        <v>1.047</v>
+        <v>1.055</v>
       </c>
       <c r="N40" t="s">
         <v>265</v>
@@ -4405,7 +4440,7 @@
         <v>271</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D41" t="s">
         <v>272</v>
@@ -4417,21 +4452,21 @@
         <v>274</v>
       </c>
       <c r="G41" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H41" t="n">
-        <v>265502</v>
+        <v>268477</v>
       </c>
       <c r="I41" t="n">
-        <v>2.099</v>
+        <v>2.123</v>
       </c>
       <c r="J41"/>
       <c r="K41"/>
       <c r="L41" t="n">
-        <v>4946</v>
+        <v>4016</v>
       </c>
       <c r="M41" t="n">
-        <v>0.039</v>
+        <v>0.032</v>
       </c>
       <c r="N41" t="s">
         <v>275</v>
@@ -4454,7 +4489,7 @@
         <v>278</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>43971</v>
+        <v>43972</v>
       </c>
       <c r="D42" t="s">
         <v>279</v>
@@ -4466,25 +4501,25 @@
         <v>280</v>
       </c>
       <c r="G42" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H42" t="n">
-        <v>425481</v>
+        <v>432684</v>
       </c>
       <c r="I42" t="n">
-        <v>3.364</v>
+        <v>3.421</v>
       </c>
       <c r="J42" t="n">
-        <v>6135</v>
+        <v>4822</v>
       </c>
       <c r="K42" t="n">
-        <v>0.049</v>
+        <v>0.038</v>
       </c>
       <c r="L42" t="n">
-        <v>6244</v>
+        <v>6065</v>
       </c>
       <c r="M42" t="n">
-        <v>0.049</v>
+        <v>0.048</v>
       </c>
       <c r="N42" t="s">
         <v>275</v>
@@ -4609,7 +4644,7 @@
         <v>295</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>43973</v>
+        <v>43975</v>
       </c>
       <c r="D45" t="s">
         <v>296</v>
@@ -4621,25 +4656,25 @@
         <v>298</v>
       </c>
       <c r="G45" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H45" t="n">
-        <v>96366</v>
+        <v>99049</v>
       </c>
       <c r="I45" t="n">
-        <v>51.09</v>
+        <v>52.512</v>
       </c>
       <c r="J45" t="n">
-        <v>1745</v>
+        <v>1203</v>
       </c>
       <c r="K45" t="n">
-        <v>0.925</v>
+        <v>0.638</v>
       </c>
       <c r="L45" t="n">
-        <v>1562</v>
+        <v>1521</v>
       </c>
       <c r="M45" t="n">
-        <v>0.828</v>
+        <v>0.806</v>
       </c>
       <c r="N45" t="s">
         <v>297</v>
@@ -4662,7 +4697,7 @@
         <v>301</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D46" t="s">
         <v>302</v>
@@ -4672,21 +4707,25 @@
       </c>
       <c r="F46"/>
       <c r="G46" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H46" t="n">
-        <v>259043</v>
+        <v>264882</v>
       </c>
       <c r="I46" t="n">
-        <v>95.156</v>
-      </c>
-      <c r="J46"/>
-      <c r="K46"/>
+        <v>97.301</v>
+      </c>
+      <c r="J46" t="n">
+        <v>5839</v>
+      </c>
+      <c r="K46" t="n">
+        <v>2.145</v>
+      </c>
       <c r="L46" t="n">
-        <v>6114</v>
+        <v>5835</v>
       </c>
       <c r="M46" t="n">
-        <v>2.246</v>
+        <v>2.143</v>
       </c>
       <c r="N46" t="s">
         <v>41</v>
@@ -4709,7 +4748,7 @@
         <v>306</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D47" t="s">
         <v>307</v>
@@ -4719,21 +4758,25 @@
       </c>
       <c r="F47"/>
       <c r="G47" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H47" t="n">
-        <v>65724</v>
+        <v>66653</v>
       </c>
       <c r="I47" t="n">
-        <v>104.994</v>
-      </c>
-      <c r="J47"/>
-      <c r="K47"/>
+        <v>106.479</v>
+      </c>
+      <c r="J47" t="n">
+        <v>929</v>
+      </c>
+      <c r="K47" t="n">
+        <v>1.484</v>
+      </c>
       <c r="L47" t="n">
-        <v>820</v>
+        <v>915</v>
       </c>
       <c r="M47" t="n">
-        <v>1.31</v>
+        <v>1.462</v>
       </c>
       <c r="N47" t="s">
         <v>308</v>
@@ -4803,7 +4846,7 @@
         <v>319</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>43972</v>
+        <v>43973</v>
       </c>
       <c r="D49" t="s">
         <v>320</v>
@@ -4815,25 +4858,25 @@
         <v>322</v>
       </c>
       <c r="G49" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H49" t="n">
-        <v>16846</v>
+        <v>17174</v>
       </c>
       <c r="I49" t="n">
-        <v>31.165</v>
+        <v>31.772</v>
       </c>
       <c r="J49" t="n">
-        <v>495</v>
+        <v>328</v>
       </c>
       <c r="K49" t="n">
-        <v>0.916</v>
+        <v>0.607</v>
       </c>
       <c r="L49" t="n">
-        <v>508</v>
+        <v>498</v>
       </c>
       <c r="M49" t="n">
-        <v>0.94</v>
+        <v>0.921</v>
       </c>
       <c r="N49" t="s">
         <v>323</v>
@@ -4856,7 +4899,7 @@
         <v>327</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>43971</v>
+        <v>43973</v>
       </c>
       <c r="D50" t="s">
         <v>328</v>
@@ -4866,22 +4909,22 @@
       </c>
       <c r="F50"/>
       <c r="G50" t="n">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H50" t="n">
-        <v>168539</v>
+        <v>183992</v>
       </c>
       <c r="I50" t="n">
-        <v>1.307</v>
+        <v>1.427</v>
       </c>
       <c r="J50" t="n">
-        <v>267</v>
+        <v>238</v>
       </c>
       <c r="K50" t="n">
         <v>0.002</v>
       </c>
       <c r="L50" t="n">
-        <v>3079</v>
+        <v>3121</v>
       </c>
       <c r="M50" t="n">
         <v>0.024</v>
@@ -5009,7 +5052,7 @@
         <v>346</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>43972</v>
+        <v>43974</v>
       </c>
       <c r="D53" t="s">
         <v>347</v>
@@ -5021,25 +5064,25 @@
         <v>349</v>
       </c>
       <c r="G53" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H53" t="n">
-        <v>38737</v>
+        <v>45959</v>
       </c>
       <c r="I53" t="n">
-        <v>1.329</v>
+        <v>1.577</v>
       </c>
       <c r="J53" t="n">
-        <v>3243</v>
+        <v>3442</v>
       </c>
       <c r="K53" t="n">
-        <v>0.111</v>
+        <v>0.118</v>
       </c>
       <c r="L53" t="n">
-        <v>2296</v>
+        <v>2753</v>
       </c>
       <c r="M53" t="n">
-        <v>0.079</v>
+        <v>0.094</v>
       </c>
       <c r="N53" t="s">
         <v>348</v>
@@ -5113,7 +5156,7 @@
         <v>360</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>43972</v>
+        <v>43974</v>
       </c>
       <c r="D55" t="s">
         <v>361</v>
@@ -5123,25 +5166,25 @@
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H55" t="n">
-        <v>250246</v>
+        <v>259152</v>
       </c>
       <c r="I55" t="n">
-        <v>51.894</v>
+        <v>53.741</v>
       </c>
       <c r="J55" t="n">
-        <v>5408</v>
+        <v>3302</v>
       </c>
       <c r="K55" t="n">
-        <v>1.121</v>
+        <v>0.685</v>
       </c>
       <c r="L55" t="n">
-        <v>4780</v>
+        <v>4429</v>
       </c>
       <c r="M55" t="n">
-        <v>0.991</v>
+        <v>0.918</v>
       </c>
       <c r="N55" t="s">
         <v>362</v>
@@ -5164,7 +5207,7 @@
         <v>365</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D56" t="s">
         <v>366</v>
@@ -5174,18 +5217,22 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H56" t="n">
-        <v>41907</v>
+        <v>43328</v>
       </c>
       <c r="I56" t="n">
-        <v>0.203</v>
-      </c>
-      <c r="J56"/>
-      <c r="K56"/>
+        <v>0.21</v>
+      </c>
+      <c r="J56" t="n">
+        <v>1421</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0.007</v>
+      </c>
       <c r="L56" t="n">
-        <v>1444</v>
+        <v>1484</v>
       </c>
       <c r="M56" t="n">
         <v>0.007</v>
@@ -5258,7 +5305,7 @@
         <v>378</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>43973</v>
+        <v>43975</v>
       </c>
       <c r="D58" t="s">
         <v>379</v>
@@ -5268,25 +5315,25 @@
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H58" t="n">
-        <v>445987</v>
+        <v>473607</v>
       </c>
       <c r="I58" t="n">
-        <v>2.019</v>
+        <v>2.144</v>
       </c>
       <c r="J58" t="n">
-        <v>16387</v>
+        <v>12915</v>
       </c>
       <c r="K58" t="n">
-        <v>0.074</v>
+        <v>0.058</v>
       </c>
       <c r="L58" t="n">
-        <v>14505</v>
+        <v>14314</v>
       </c>
       <c r="M58" t="n">
-        <v>0.066</v>
+        <v>0.065</v>
       </c>
       <c r="N58" t="s">
         <v>380</v>
@@ -5413,7 +5460,7 @@
         <v>396</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D61" t="s">
         <v>397</v>
@@ -5423,21 +5470,25 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H61" t="n">
-        <v>112353</v>
+        <v>122749</v>
       </c>
       <c r="I61" t="n">
-        <v>3.408</v>
-      </c>
-      <c r="J61"/>
-      <c r="K61"/>
+        <v>3.723</v>
+      </c>
+      <c r="J61" t="n">
+        <v>10396</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0.315</v>
+      </c>
       <c r="L61" t="n">
-        <v>2804</v>
+        <v>3715</v>
       </c>
       <c r="M61" t="n">
-        <v>0.085</v>
+        <v>0.113</v>
       </c>
       <c r="N61" t="s">
         <v>398</v>
@@ -5460,7 +5511,7 @@
         <v>403</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>43966</v>
+        <v>43973</v>
       </c>
       <c r="D62" t="s">
         <v>404</v>
@@ -5472,21 +5523,21 @@
         <v>406</v>
       </c>
       <c r="G62" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H62" t="n">
-        <v>188024</v>
+        <v>265061</v>
       </c>
       <c r="I62" t="n">
-        <v>1.716</v>
+        <v>2.419</v>
       </c>
       <c r="J62"/>
       <c r="K62"/>
       <c r="L62" t="n">
-        <v>6324</v>
+        <v>11005</v>
       </c>
       <c r="M62" t="n">
-        <v>0.058</v>
+        <v>0.1</v>
       </c>
       <c r="N62" t="s">
         <v>210</v>
@@ -5509,7 +5560,7 @@
         <v>409</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D63" t="s">
         <v>410</v>
@@ -5521,25 +5572,25 @@
         <v>412</v>
       </c>
       <c r="G63" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H63" t="n">
-        <v>719571</v>
+        <v>750939</v>
       </c>
       <c r="I63" t="n">
-        <v>19.013</v>
+        <v>19.842</v>
       </c>
       <c r="J63" t="n">
-        <v>22341</v>
+        <v>31368</v>
       </c>
       <c r="K63" t="n">
-        <v>0.59</v>
+        <v>0.829</v>
       </c>
       <c r="L63" t="n">
-        <v>20471</v>
+        <v>21364</v>
       </c>
       <c r="M63" t="n">
-        <v>0.541</v>
+        <v>0.564</v>
       </c>
       <c r="N63" t="s">
         <v>413</v>
@@ -5613,7 +5664,7 @@
         <v>423</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D65" t="s">
         <v>424</v>
@@ -5621,59 +5672,61 @@
       <c r="E65" t="s">
         <v>425</v>
       </c>
-      <c r="F65"/>
+      <c r="F65" t="s">
+        <v>426</v>
+      </c>
       <c r="G65" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H65" t="n">
-        <v>180642</v>
+        <v>184794</v>
       </c>
       <c r="I65" t="n">
-        <v>62.7</v>
+        <v>64.141</v>
       </c>
       <c r="J65" t="n">
-        <v>5160</v>
+        <v>4152</v>
       </c>
       <c r="K65" t="n">
-        <v>1.791</v>
+        <v>1.441</v>
       </c>
       <c r="L65" t="n">
-        <v>4638</v>
+        <v>4584</v>
       </c>
       <c r="M65" t="n">
-        <v>1.61</v>
+        <v>1.591</v>
       </c>
       <c r="N65" t="s">
         <v>425</v>
       </c>
       <c r="O65" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="P65" t="s">
         <v>92</v>
       </c>
       <c r="Q65" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B66" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>43972</v>
       </c>
       <c r="D66" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E66" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="F66" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="G66" t="n">
         <v>71</v>
@@ -5697,80 +5750,84 @@
         <v>0.418</v>
       </c>
       <c r="N66" t="s">
+        <v>432</v>
+      </c>
+      <c r="O66" t="s">
         <v>431</v>
-      </c>
-      <c r="O66" t="s">
-        <v>430</v>
       </c>
       <c r="P66" t="s">
         <v>22</v>
       </c>
       <c r="Q66" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B67" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>43973</v>
+        <v>43975</v>
       </c>
       <c r="D67" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="E67" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H67" t="n">
-        <v>8126626</v>
+        <v>8685305</v>
       </c>
       <c r="I67" t="n">
-        <v>55.687</v>
-      </c>
-      <c r="J67"/>
-      <c r="K67"/>
+        <v>59.515</v>
+      </c>
+      <c r="J67" t="n">
+        <v>282558</v>
+      </c>
+      <c r="K67" t="n">
+        <v>1.936</v>
+      </c>
       <c r="L67" t="n">
-        <v>244668</v>
+        <v>252745</v>
       </c>
       <c r="M67" t="n">
-        <v>1.677</v>
+        <v>1.732</v>
       </c>
       <c r="N67" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="O67" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="P67" t="s">
         <v>22</v>
       </c>
       <c r="Q67" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B68" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C68" s="1" t="n">
         <v>43973</v>
       </c>
       <c r="D68" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="E68" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
@@ -5795,59 +5852,61 @@
         <v>0.108</v>
       </c>
       <c r="N68" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="O68" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="P68" t="s">
         <v>51</v>
       </c>
       <c r="Q68" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B69" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D69" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="E69" t="s">
         <v>41</v>
       </c>
-      <c r="F69" t="s">
-        <v>449</v>
-      </c>
+      <c r="F69"/>
       <c r="G69" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H69" t="n">
-        <v>667057</v>
+        <v>684615</v>
       </c>
       <c r="I69" t="n">
-        <v>19.161</v>
-      </c>
-      <c r="J69"/>
-      <c r="K69"/>
+        <v>19.665</v>
+      </c>
+      <c r="J69" t="n">
+        <v>17558</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0.504</v>
+      </c>
       <c r="L69" t="n">
-        <v>19542</v>
+        <v>19513</v>
       </c>
       <c r="M69" t="n">
-        <v>0.561</v>
+        <v>0.56</v>
       </c>
       <c r="N69" t="s">
         <v>41</v>
       </c>
       <c r="O69" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="P69" t="s">
         <v>126</v>
@@ -5864,7 +5923,7 @@
         <v>452</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D70" t="s">
         <v>453</v>
@@ -5876,22 +5935,22 @@
         <v>455</v>
       </c>
       <c r="G70" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H70" t="n">
-        <v>33892</v>
+        <v>34826</v>
       </c>
       <c r="I70" t="n">
-        <v>2.024</v>
+        <v>2.08</v>
       </c>
       <c r="J70" t="n">
-        <v>1199</v>
+        <v>934</v>
       </c>
       <c r="K70" t="n">
-        <v>0.072</v>
+        <v>0.056</v>
       </c>
       <c r="L70" t="n">
-        <v>1038</v>
+        <v>1030</v>
       </c>
       <c r="M70" t="n">
         <v>0.062</v>
@@ -5917,7 +5976,7 @@
         <v>461</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>43972</v>
+        <v>43974</v>
       </c>
       <c r="D71" t="s">
         <v>462</v>
@@ -5929,25 +5988,25 @@
         <v>463</v>
       </c>
       <c r="G71" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H71" t="n">
-        <v>203799</v>
+        <v>214212</v>
       </c>
       <c r="I71" t="n">
-        <v>29.95</v>
+        <v>31.48</v>
       </c>
       <c r="J71" t="n">
-        <v>6918</v>
+        <v>4415</v>
       </c>
       <c r="K71" t="n">
-        <v>1.017</v>
+        <v>0.649</v>
       </c>
       <c r="L71" t="n">
-        <v>5857</v>
+        <v>5638</v>
       </c>
       <c r="M71" t="n">
-        <v>0.861</v>
+        <v>0.829</v>
       </c>
       <c r="N71" t="s">
         <v>41</v>
@@ -6064,7 +6123,7 @@
         <v>475</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>43973</v>
+        <v>43975</v>
       </c>
       <c r="D74" t="s">
         <v>476</v>
@@ -6074,21 +6133,25 @@
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H74" t="n">
-        <v>154529</v>
+        <v>158414</v>
       </c>
       <c r="I74" t="n">
-        <v>28.304</v>
-      </c>
-      <c r="J74"/>
-      <c r="K74"/>
+        <v>29.015</v>
+      </c>
+      <c r="J74" t="n">
+        <v>1649</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0.302</v>
+      </c>
       <c r="L74" t="n">
-        <v>2661</v>
+        <v>2279</v>
       </c>
       <c r="M74" t="n">
-        <v>0.487</v>
+        <v>0.417</v>
       </c>
       <c r="N74" t="s">
         <v>478</v>
@@ -6111,7 +6174,7 @@
         <v>483</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>43972</v>
+        <v>43974</v>
       </c>
       <c r="D75" t="s">
         <v>484</v>
@@ -6121,25 +6184,25 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H75" t="n">
-        <v>73742</v>
+        <v>74760</v>
       </c>
       <c r="I75" t="n">
-        <v>35.471</v>
+        <v>35.961</v>
       </c>
       <c r="J75" t="n">
-        <v>882</v>
+        <v>341</v>
       </c>
       <c r="K75" t="n">
-        <v>0.424</v>
+        <v>0.164</v>
       </c>
       <c r="L75" t="n">
-        <v>863</v>
+        <v>771</v>
       </c>
       <c r="M75" t="n">
-        <v>0.415</v>
+        <v>0.371</v>
       </c>
       <c r="N75" t="s">
         <v>486</v>
@@ -6162,7 +6225,7 @@
         <v>490</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D76" t="s">
         <v>491</v>
@@ -6174,25 +6237,25 @@
         <v>493</v>
       </c>
       <c r="G76" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H76" t="n">
-        <v>543032</v>
+        <v>564370</v>
       </c>
       <c r="I76" t="n">
-        <v>9.156</v>
+        <v>9.516</v>
       </c>
       <c r="J76" t="n">
-        <v>17599</v>
+        <v>21338</v>
       </c>
       <c r="K76" t="n">
-        <v>0.297</v>
+        <v>0.36</v>
       </c>
       <c r="L76" t="n">
-        <v>17354</v>
+        <v>17830</v>
       </c>
       <c r="M76" t="n">
-        <v>0.293</v>
+        <v>0.301</v>
       </c>
       <c r="N76" t="s">
         <v>492</v>
@@ -6215,7 +6278,7 @@
         <v>497</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D77" t="s">
         <v>498</v>
@@ -6225,21 +6288,25 @@
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H77" t="n">
-        <v>802418</v>
+        <v>814420</v>
       </c>
       <c r="I77" t="n">
-        <v>15.651</v>
-      </c>
-      <c r="J77"/>
-      <c r="K77"/>
+        <v>15.885</v>
+      </c>
+      <c r="J77" t="n">
+        <v>12002</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0.234</v>
+      </c>
       <c r="L77" t="n">
-        <v>10810</v>
+        <v>10539</v>
       </c>
       <c r="M77" t="n">
-        <v>0.211</v>
+        <v>0.206</v>
       </c>
       <c r="N77" t="s">
         <v>499</v>
@@ -6356,7 +6423,7 @@
         <v>515</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>43971</v>
+        <v>43973</v>
       </c>
       <c r="D80" t="s">
         <v>516</v>
@@ -6366,25 +6433,25 @@
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H80" t="n">
-        <v>362612</v>
+        <v>367034</v>
       </c>
       <c r="I80" t="n">
-        <v>41.898</v>
+        <v>42.409</v>
       </c>
       <c r="J80" t="n">
-        <v>4541</v>
+        <v>2043</v>
       </c>
       <c r="K80" t="n">
-        <v>0.525</v>
+        <v>0.236</v>
       </c>
       <c r="L80" t="n">
-        <v>4449</v>
+        <v>3467</v>
       </c>
       <c r="M80" t="n">
-        <v>0.514</v>
+        <v>0.401</v>
       </c>
       <c r="N80" t="s">
         <v>517</v>
@@ -6407,7 +6474,7 @@
         <v>521</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>43972</v>
+        <v>43974</v>
       </c>
       <c r="D81" t="s">
         <v>522</v>
@@ -6417,21 +6484,25 @@
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H81" t="n">
-        <v>70338</v>
+        <v>70697</v>
       </c>
       <c r="I81" t="n">
-        <v>2.953</v>
-      </c>
-      <c r="J81"/>
-      <c r="K81"/>
+        <v>2.968</v>
+      </c>
+      <c r="J81" t="n">
+        <v>171</v>
+      </c>
+      <c r="K81" t="n">
+        <v>0.007</v>
+      </c>
       <c r="L81" t="n">
-        <v>240</v>
+        <v>213</v>
       </c>
       <c r="M81" t="n">
-        <v>0.01</v>
+        <v>0.009</v>
       </c>
       <c r="N81" t="s">
         <v>523</v>
@@ -6454,7 +6525,7 @@
         <v>528</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D82" t="s">
         <v>529</v>
@@ -6464,21 +6535,25 @@
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H82" t="n">
-        <v>147104</v>
+        <v>150455</v>
       </c>
       <c r="I82" t="n">
-        <v>2.108</v>
-      </c>
-      <c r="J82"/>
-      <c r="K82"/>
+        <v>2.156</v>
+      </c>
+      <c r="J82" t="n">
+        <v>3351</v>
+      </c>
+      <c r="K82" t="n">
+        <v>0.048</v>
+      </c>
       <c r="L82" t="n">
-        <v>4148</v>
+        <v>4597</v>
       </c>
       <c r="M82" t="n">
-        <v>0.059</v>
+        <v>0.066</v>
       </c>
       <c r="N82" t="s">
         <v>531</v>
@@ -6548,7 +6623,7 @@
         <v>540</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>43971</v>
+        <v>43973</v>
       </c>
       <c r="D84" t="s">
         <v>541</v>
@@ -6558,25 +6633,25 @@
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H84" t="n">
-        <v>45308</v>
+        <v>47649</v>
       </c>
       <c r="I84" t="n">
-        <v>3.834</v>
+        <v>4.032</v>
       </c>
       <c r="J84" t="n">
-        <v>1585</v>
+        <v>1021</v>
       </c>
       <c r="K84" t="n">
-        <v>0.134</v>
+        <v>0.086</v>
       </c>
       <c r="L84" t="n">
-        <v>1255</v>
+        <v>1124</v>
       </c>
       <c r="M84" t="n">
-        <v>0.106</v>
+        <v>0.095</v>
       </c>
       <c r="N84" t="s">
         <v>542</v>
@@ -6599,7 +6674,7 @@
         <v>547</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D85" t="s">
         <v>548</v>
@@ -6609,21 +6684,25 @@
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H85" t="n">
-        <v>1767495</v>
+        <v>1807673</v>
       </c>
       <c r="I85" t="n">
-        <v>20.957</v>
-      </c>
-      <c r="J85"/>
-      <c r="K85"/>
+        <v>21.433</v>
+      </c>
+      <c r="J85" t="n">
+        <v>40178</v>
+      </c>
+      <c r="K85" t="n">
+        <v>0.476</v>
+      </c>
       <c r="L85" t="n">
-        <v>31444</v>
+        <v>31150</v>
       </c>
       <c r="M85" t="n">
-        <v>0.373</v>
+        <v>0.369</v>
       </c>
       <c r="N85" t="s">
         <v>549</v>
@@ -6646,7 +6725,7 @@
         <v>554</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>43972</v>
+        <v>43973</v>
       </c>
       <c r="D86" t="s">
         <v>555</v>
@@ -6658,25 +6737,25 @@
         <v>557</v>
       </c>
       <c r="G86" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H86" t="n">
-        <v>80552</v>
+        <v>82658</v>
       </c>
       <c r="I86" t="n">
-        <v>1.761</v>
+        <v>1.807</v>
       </c>
       <c r="J86" t="n">
-        <v>2729</v>
+        <v>2106</v>
       </c>
       <c r="K86" t="n">
-        <v>0.06</v>
+        <v>0.046</v>
       </c>
       <c r="L86" t="n">
-        <v>1769</v>
+        <v>1704</v>
       </c>
       <c r="M86" t="n">
-        <v>0.039</v>
+        <v>0.037</v>
       </c>
       <c r="N86" t="s">
         <v>556</v>
@@ -6699,7 +6778,7 @@
         <v>561</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>43973</v>
+        <v>43975</v>
       </c>
       <c r="D87" t="s">
         <v>562</v>
@@ -6709,21 +6788,25 @@
       </c>
       <c r="F87"/>
       <c r="G87" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H87" t="n">
-        <v>267185</v>
+        <v>285626</v>
       </c>
       <c r="I87" t="n">
-        <v>6.109</v>
-      </c>
-      <c r="J87"/>
-      <c r="K87"/>
+        <v>6.531</v>
+      </c>
+      <c r="J87" t="n">
+        <v>7914</v>
+      </c>
+      <c r="K87" t="n">
+        <v>0.181</v>
+      </c>
       <c r="L87" t="n">
-        <v>7939</v>
+        <v>8261</v>
       </c>
       <c r="M87" t="n">
-        <v>0.182</v>
+        <v>0.189</v>
       </c>
       <c r="N87" t="s">
         <v>563</v>
@@ -6797,7 +6880,7 @@
         <v>573</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D89" t="s">
         <v>574</v>
@@ -6807,25 +6890,25 @@
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H89" t="n">
-        <v>3231921</v>
+        <v>3348507</v>
       </c>
       <c r="I89" t="n">
-        <v>47.608</v>
+        <v>49.325</v>
       </c>
       <c r="J89" t="n">
-        <v>140497</v>
+        <v>116585</v>
       </c>
       <c r="K89" t="n">
-        <v>2.07</v>
+        <v>1.717</v>
       </c>
       <c r="L89" t="n">
-        <v>125549</v>
+        <v>122706</v>
       </c>
       <c r="M89" t="n">
-        <v>1.849</v>
+        <v>1.808</v>
       </c>
       <c r="N89" t="s">
         <v>570</v>
@@ -6848,7 +6931,7 @@
         <v>578</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>43972</v>
+        <v>43974</v>
       </c>
       <c r="D90" t="s">
         <v>579</v>
@@ -6858,25 +6941,25 @@
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H90" t="n">
-        <v>13049906</v>
+        <v>13784786</v>
       </c>
       <c r="I90" t="n">
-        <v>39.425</v>
+        <v>41.646</v>
       </c>
       <c r="J90" t="n">
-        <v>402115</v>
+        <v>365728</v>
       </c>
       <c r="K90" t="n">
-        <v>1.215</v>
+        <v>1.105</v>
       </c>
       <c r="L90" t="n">
-        <v>381848</v>
+        <v>389611</v>
       </c>
       <c r="M90" t="n">
-        <v>1.154</v>
+        <v>1.177</v>
       </c>
       <c r="N90" t="s">
         <v>580</v>
@@ -6899,7 +6982,7 @@
         <v>584</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>43970</v>
+        <v>43973</v>
       </c>
       <c r="D91" t="s">
         <v>585</v>
@@ -6909,25 +6992,21 @@
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H91" t="n">
-        <v>12601143</v>
+        <v>13627379</v>
       </c>
       <c r="I91" t="n">
-        <v>38.07</v>
-      </c>
-      <c r="J91" t="n">
-        <v>1318362</v>
-      </c>
-      <c r="K91" t="n">
-        <v>3.983</v>
-      </c>
+        <v>41.17</v>
+      </c>
+      <c r="J91"/>
+      <c r="K91"/>
       <c r="L91" t="n">
-        <v>410895</v>
+        <v>442100</v>
       </c>
       <c r="M91" t="n">
-        <v>1.241</v>
+        <v>1.336</v>
       </c>
       <c r="N91" t="s">
         <v>586</v>
@@ -6950,7 +7029,7 @@
         <v>590</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D92" t="s">
         <v>591</v>
@@ -6960,21 +7039,25 @@
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H92" t="n">
-        <v>35537</v>
+        <v>37178</v>
       </c>
       <c r="I92" t="n">
-        <v>10.23</v>
-      </c>
-      <c r="J92"/>
-      <c r="K92"/>
+        <v>10.703</v>
+      </c>
+      <c r="J92" t="n">
+        <v>1641</v>
+      </c>
+      <c r="K92" t="n">
+        <v>0.472</v>
+      </c>
       <c r="L92" t="n">
-        <v>618</v>
+        <v>708</v>
       </c>
       <c r="M92" t="n">
-        <v>0.178</v>
+        <v>0.204</v>
       </c>
       <c r="N92" t="s">
         <v>124</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-06-03
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Argentina - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/01-06-20_reporte-matutino-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/03-06-20_reporte-matutino-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Argentina</t>
@@ -92,7 +92,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/05/coronavirus-covid-19-at-a-glance-31-may-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/06/coronavirus-covid-19-at-a-glance-2-june-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200601104302/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200603200522/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200601190936/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200603200526/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -187,7 +187,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-1-iyunya-vyzdoroveli-i-vypisany-18-tys-776-patsientov/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-2-iyunya-vyzdoroveli-i-vypisany-19-195-patsientov/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -233,7 +233,7 @@
     <t xml:space="preserve">Bolivia - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4237-bolivia-registra-390-nuevos-contagios-de-coronavirus-y-el-acumulado-llega-a-9-982</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4243-ministerio-de-salud-reporta-460-nuevos-contagios-de-coronavirus-y-33-fallecidos</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -280,7 +280,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200601104307/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200603200557/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -303,7 +303,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200601190941/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200603200615/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -391,7 +391,7 @@
     <t xml:space="preserve">Croatia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200601190948/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200603201313/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -454,7 +454,7 @@
     <t xml:space="preserve">Denmark - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200601180102/https://www.ssi.dk/sygdomme-beredskab-og-forskning/sygdomsovervaagning/c/covid19-overvaagning</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200603172636/https://www.ssi.dk/sygdomme-beredskab-og-forskning/sygdomsovervaagning/c/covid19-overvaagning</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -480,7 +480,7 @@
     <t xml:space="preserve">Ecuador - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/05/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-31052020-08h002.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-02062020-08h00.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -505,7 +505,7 @@
     <t xml:space="preserve">El Salvador - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/2936959489723556</t>
+    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/2942358345850337</t>
   </si>
   <si>
     <t xml:space="preserve">Government of El Salvador</t>
@@ -549,7 +549,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_June-1-Eng_V1.pdf</t>
+    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_June-3-Eng_V2.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -688,7 +688,7 @@
   <si>
     <t xml:space="preserve">Outbreak Response Management provides [daily situation updates](https://www.ghanahealthservice.org/covid19/archive.php) on the total number of people *or* total samples tested for the coronavirus.
 Using web archives, we reconstruct a time series. From 17 March 2020 to 8 May 2020, situation updates sometimes reported the total number of people tested, and other times the total number of samples tested. We are not certain what the true units were during that period.
-From 10 May 2020, the total number of tests and total persons tested figures are reported separately. The situation updates for 27,28,29,30 May do not report the number of people tested.</t>
+From 10 May 2020, the total number of tests and total persons tested figures are reported separately. The situation updates from 27 May onwards do not report the number of people tested.</t>
   </si>
   <si>
     <t xml:space="preserve">Ghana - samples tested</t>
@@ -703,7 +703,7 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200601/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200602/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -841,7 +841,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200531171732/http://irangov.ir/detail/340132</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200603033550/http://irangov.ir/detail/340265</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -860,7 +860,7 @@
     <t xml:space="preserve">Ireland - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gov.ie/en/press-release/78916-statement-from-the-national-public-health-emergency-team-tuesday-26-may/</t>
+    <t xml:space="preserve">https://www.gov.ie/en/press-release/1beb1-statement-from-the-national-public-health-emergency-team-tuesday-2-june/</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gov.ie/en/publications/?&amp;type=press-releases&amp;organisation=department-of-health</t>
@@ -881,7 +881,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/ministry-of-health/corona/corona-virus/</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/20129/covid19-data-israel-27052020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -938,7 +938,7 @@
     <t xml:space="preserve">Japan - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11621.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11664.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -962,7 +962,7 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000635766.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000636597.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">The cumulative total reported in the press release matches the cumulative total calculated from the weekly and daily figures reported by the MOH.</t>
@@ -997,7 +997,7 @@
     <t xml:space="preserve">Kenya - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1267086829985116162</t>
+    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1267805415775121409</t>
   </si>
   <si>
     <t xml:space="preserve">Kenya Ministry of Health</t>
@@ -1038,7 +1038,7 @@
     <t xml:space="preserve">Lithuania - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200601191150/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200603201910/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -1054,7 +1054,7 @@
     <t xml:space="preserve">Luxembourg - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200531165702/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200603201912/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg Government situation update</t>
@@ -1100,13 +1100,13 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/561317043971945/videos/730837957728928/</t>
+    <t xml:space="preserve">https://www.facebook.com/561317043971945/videos/673971883160559/</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Ministry of Health</t>
   </si>
   <si>
-    <t xml:space="preserve">Numbers visible in video at time: 1:30</t>
+    <t xml:space="preserve">Numbers visible in video at time: 1:13</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Ministry of Health Official Facebook page</t>
@@ -1170,9 +1170,6 @@
     <t xml:space="preserve">Myanmar Ministry of Health and Sports</t>
   </si>
   <si>
-    <t xml:space="preserve">This figure is taken from the interactive dashboard and should be updated once the daily PDF situation report becomes available</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://mohs.gov.mm/Home</t>
   </si>
   <si>
@@ -1209,10 +1206,10 @@
     <t xml:space="preserve">Netherlands - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-05/31-5-2020%20COVID-19_WebSite_rapport.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 31 May 2020 update</t>
+    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-06/COVID-19_WebSite_rapport_20200602_1024.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 2 June 2020 update</t>
   </si>
   <si>
     <t xml:space="preserve">Dutch National Institute for Public Health and the Environment</t>
@@ -1248,7 +1245,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200601191454/https://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200603202046/https://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1268,7 +1265,7 @@
     <t xml:space="preserve">Norway - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.05.29-dagsrapport-norge-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.06.03-dagsrapport-norge-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Norwegian Institute of Public Health</t>
@@ -1293,7 +1290,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200601104608/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200603202050/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1351,7 +1348,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/168047-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-164-476-en-el-peru-comunicado-n-117</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/176156-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-178-914-en-el-peru-comunicado-n-120</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1384,8 +1381,8 @@
     <t xml:space="preserve">The Ministry of Health (MOH) provides a daily snapshot of testing capacity detailing the total number of individuals tested and the total number of tests conducted. 
 The total number of individuals tested is the sum of positive, negative, equivocal, and invalid individuals. No definitions of equivocal and invalid individual tests are given, hence our figures only report the sum of individuals who have tested positive or negative. From 22nd May, the DOH stopped reporting figures on equivocal and invalid individuals; the DOH provides the cumulative samples and unique indivdiuals tested, where cumulative unique individuals = cumulative positive + cumulative negative individuals. 
 The source provides a breakdown of both i) the number of individuals tested and ii) the total tests conducted, by laboratory. We are not aware of any aggregation issues. 
-The DOH used to report the number of cases tested in a previous dashboard, but stopped on 4th April. This previous breakdown of the test results and COVID-19 dashboard have both been removed. We became aware of this new tracker on the 13th April with data 'as of April 11 2020, 12am'. No previous snapshots of the dashboard are available using web archive, therefore the series starts from the 11th April - the earliest date from which we have access to the data.  
-No newly submitted report as of 29 May. Latest testing data available is from 28 May.</t>
+The DOH used to report the number of cases tested in a previous dashboard, but stopped on 4th April. This previous breakdown of the test results and COVID-19 dashboard have both been removed. We became aware of this new tracker on the 13th April with data 'as of April 11 2020, 12am'. No previous snapshots of the dashboard are available using web archive, therefore the series starts from the 11th April - the earliest date from which we have access to the data.
+Latest data available until 1st June, as of 3rd June.</t>
   </si>
   <si>
     <t xml:space="preserve">POL</t>
@@ -1394,7 +1391,7 @@
     <t xml:space="preserve">Poland - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://raw.githubusercontent.com/anuszka/COVID-19-MZ_GOV_PL/master/data/cor.2020.06.01.csv</t>
+    <t xml:space="preserve">https://raw.githubusercontent.com/anuszka/COVID-19-MZ_GOV_PL/master/data/cor.2020.06.03.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1477,7 +1474,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14586</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14605</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1497,7 +1494,7 @@
     <t xml:space="preserve">Rwanda - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1266811034104406023</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1267945222819975170</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1579,7 +1576,7 @@
     <t xml:space="preserve">Singapore - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200527192413/https://www.moh.gov.sg/covid-19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200603202128/https://www.moh.gov.sg/covid-19</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.moh.gov.sg/covid-19</t>
@@ -1592,7 +1589,7 @@
     <t xml:space="preserve">Singapore - swabs tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200527192416/https://www.moh.gov.sg/covid-19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200603202130/https://www.moh.gov.sg/covid-19</t>
   </si>
   <si>
     <t xml:space="preserve">The number of swabs tested.</t>
@@ -1604,7 +1601,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200531165819/https://korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200602201741/https://korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Center of Health Information and the Office of the Government of the Slovak Republic</t>
@@ -1678,7 +1675,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367388&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367407&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1761,7 +1758,7 @@
     <t xml:space="preserve">Taiwan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/E8ZwH9zVNq21O-EItgoiEQ?typeid=9</t>
+    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/rWxxHolsA5DEEpJxm5zpoQ?typeid=9</t>
   </si>
   <si>
     <t xml:space="preserve">Taiwan Centers for Disease Control (CDC)</t>
@@ -1784,7 +1781,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200601191602/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200603202218/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1805,10 +1802,13 @@
     <t xml:space="preserve">Thailand - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.who.int/docs/default-source/searo/thailand/2020-05-25-tha-sitrep-85-covid19.pdf?sfvrsn=4fea9246_2</t>
+    <t xml:space="preserve">https://www.who.int/docs/default-source/searo/thailand/2020-06-01-tha-sitrep-88-covid19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">World Health Organization Country Office for Thailand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This figure is approximate. The report states that "Over 420,000 RT-PCR tests have been performed."</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.who.int/thailand/emergencies/novel-coronavirus-2019/situation-reports</t>
@@ -1851,7 +1851,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200601191606/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200603202222/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1875,13 +1875,13 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1267389590316425217/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1267734985693442048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Press Release from the Office of the Director General</t>
   </si>
   <si>
     <t xml:space="preserve">We sum the cumulative total provided for the previous day with the daily number of samples tested today.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Press Release from the Office of the Director General</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.health.go.ug/moh/resources/</t>
@@ -1899,7 +1899,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200601104833/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200603202225/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1930,69 +1930,34 @@
     <t xml:space="preserve">https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public#number-of-cases</t>
   </si>
   <si>
-    <t xml:space="preserve">A time series is not yet released. The figures we provide relate to the daily updates provided for the cumulative total and daily number of people tested. It is not clear the exact date that the cumulative figures date back to.
-We were [informed on 26 April 2020](https://github.com/owid/covid-19-data/issues/29) that the daily changes in cumulative total, which we previously calculated by subtracting one day's running total from the next one, couldn't in fact be calculated in this way, and were provided directly on the page instead. We thus readjusted our time series using [Tom White's archives on GitHub](https://github.com/tomwhite/covid-19-uk-data/tree/master/data/raw), and from 26 April 2020 onwards we collect both figures directly from the official page.
-The UK now provides its figures according to the 'pillars' of it's testing strategy, as follows:
-Pillar 1: swab testing in PHE labs and NHS hospitals for those with a clinical need, and health and care workers
-Pillar 2: swab testing for health, social care and other essential workers and their households
-Pillar 4: serology and swab testing: a national surveillance programme supported by PHE, ONS and Biobank to learn more about the prevalence and spread of the virus
-As of 30 April, there were no people tested under Pillar 4 included in this series.
-(As discussed in the Govenerment's [national testing strategy document](https://www.gov.uk/government/publications/coronavirus-covid-19-scaling-up-testing-programmes), Pillar 3 relates to antibody tests – but these are currently not reported within the figures above).
-The Health Service Journal highlighted in [an article published on 1 May 2020](https://www.hsj.co.uk/quality-and-performance/revealed-how-government-changed-the-rules-to-hit-100000-tests-target/7027544.article) that “the Department of Health and Social Care [was] now including tests that have been posted or delivered to people’s homes in its figures. This means tests which are sent to people are counted before the recipient has provided and returned their sample to a laboratory.” No data is made available by the UK government on how many of these mailed tests have been returned and processed, but this could represent a significant number for recent days. As far as we know, the “People tested” figures are not affected by this issue.</t>
+    <t xml:space="preserve">The figures we provide relate to the daily updates provided for the cumulative total and daily number of people tested. It is not clear the exact date that the cumulative figures date back to. As of 2 June 2020, the sources notes that "reporting on the number of people tested has been temporarily paused to ensure consistent reporting across all pillars. This is due to a small percentage of cases where the same person has had more than one test or tested positive more than once for coronavirus in pillar 2. Corrections will be made to any figures if they have subsequently been found to have an error."</t>
   </si>
   <si>
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200531165920/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of tests performed, including tests posted or delivered but not yet returned and/or processed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A time series is not yet released. The figures we provide relate to the daily updates provided for the cumulative total and daily number of tests performed. It is not clear the exact date that the cumulative figures date back to.
-We were [informed on 26 April 2020](https://github.com/owid/covid-19-data/issues/29) that the daily changes in cumulative total, which we previously calculated by subtracting one day's running total from the next one, couldn't in fact be calculated in this way, and were provided directly on the page instead. We thus readjusted our time series using [Tom White's archives on GitHub](https://github.com/tomwhite/covid-19-uk-data/tree/master/data/raw), and from 26 April 2020 onwards we collect both figures directly from the official page.
-The UK now provides its figures according to the 'pillars' of it's testing strategy, as follows:
-Pillar 1: swab testing in PHE labs and NHS hospitals for those with a clinical need, and health and care workers
-Pillar 2: swab testing for health, social care and other essential workers and their households
-Pillar 4: serology and swab testing: a national surveillance programme supported by PHE, ONS and Biobank to learn more about the prevalence and spread of the virus
-As of 30 April, around 10% of the total number of tests were reported under Pillar 4. How these further breakdown between serology and swab testing is not known.
-As discussed in the Govenerment's [national testing strategy document](https://www.gov.uk/government/publications/coronavirus-covid-19-scaling-up-testing-programmes), Pillar 3 relates to antibody tests – but these are currently not reported within the figures above.
-The Health Service Journal highlighted in [an article published on 1 May 2020](https://www.hsj.co.uk/quality-and-performance/revealed-how-government-changed-the-rules-to-hit-100000-tests-target/7027544.article) that “the Department of Health and Social Care [was] now including tests that have been posted or delivered to people’s homes in its figures. This means tests which are sent to people are counted before the recipient has provided and returned their sample to a laboratory.” No data is made available by the UK government on how many of these mailed tests have been returned and processed, but this could represent a significant number for recent days. As far as we know, the “People tested” figures are not affected by this issue.</t>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/889818/2020-06-03-COVID-19-UK-testing-time-series.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of pillar 1 + pillar 2 (tests processed only)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since early June 2020, the United Kingdom has been publishing a full retrospective time series in CSV format, with testing data going back to 20 March 2020. In our time series for "tests performed", we aggregate the data for the United Kingdom based only on two "pillars":
+- Pillar 1: swab testing in Public Health England (PHE) labs and NHS hospitals for those with a clinical need, and health and care workers;
+- Pillar 2: swab testing for the wider population, as set out in government guidance. For this pillar, we only include "in-person tests", i.e. tests that have not only been mailed out, but also returned and processed.
+These combined criteria mean that our time series starts on 26 April 2020. We do not include other pillars, i.e.
+- Pillar 3: this pillar consists (fully) of serology tests, which we aim not to include;
+- Pillar 4: this pillar consists (partly) of serology tests, which we aim not to include, and positive tests results from this pillar seem not to be included in the government's total for positive cases.
+The source notes that "data on UK tests is updated daily. The figures for test results are compiled from different sources. Daily totals reflect actual counts reported for the previous day. Each day there may be corrections to previous reported figures. This means that previously published daily counts will not necessarily sum to the latest cumulative figure. It also means that today’s cumulative count may not match the previous day’s cumulative count plus today’s daily count."</t>
   </si>
   <si>
     <t xml:space="preserve">USA</t>
   </si>
   <si>
-    <t xml:space="preserve">United States - inconsistent units (COVID Tracking Project)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://covidtracking.com/api/us/daily.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COVID Tracking Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://covidtracking.com/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The data are an aggregation of figures released by individual states. The Project aim to report on the number of people tested, including private labs, but not all states report their figures in this way. The figures for some states appear to include antibody tests in addition to PCR tests.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is a collaborative project launched in order to fill some of the important gaps in the testing figures being collated by the CDC.
-Testing data is gathered from individual states, as reported in state health department websites, data dashboards and press releases from officials.
-As of 26 May, there have been a number of media reports noting that the testing figures released by some states include antibody tests in addition to PCR tests – as discussed in [this article](https://www.theatlantic.com/health/archive/2020/05/cdc-and-states-are-misreporting-covid-19-test-data-pennsylvania-georgia-texas/611935/) in The Atlantic. Our dataset aims to report only PCR tests. But becasue some states do not disaggregate these types of tests we are not currently able to exclude the antibody tests.
-Other differences across states include: some report the number of tests performed, others the number of people tested; some include private labs, others not; some report negative test results, others only positive test results; some include pending tests, others do not (below we show figures that exclude explicitly pending results).
-Moreover, many states do not explicitly provide details about these important factors needed to interpret the data they provide. 
-There are issues in comparing the figures over time. The totals given for early on in the outbreak do not include all states. One significant uncertainty is the extent to which the rapid rise in tests seen from the mid-March in part reflects states beginning to report private lab tests.
-Overall the figures should be seen as providing a general indication of testing output, rather than a specific count of a given indicator. Given the very incomplete coverage and reporting delays of the CDC data, it provides a very important additional perspective.
-The Project documents their work in lots of detail. See the link provided above for full details.</t>
-  </si>
-  <si>
     <t xml:space="preserve">United States - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200530204657/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200603202228/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
   </si>
   <si>
     <t xml:space="preserve">United States CDC</t>
@@ -2015,13 +1980,38 @@
 The CDC previously published a time series that only covered public health labs and did not include private lab tests, which were occurring in significant numbers. Daily figures were provided since 18 January. This data is still visible on [this page of the CDC website](https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/previous-testing-in-us.html).</t>
   </si>
   <si>
+    <t xml:space="preserve">United States - units unclear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://covidtracking.com/api/us/daily.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COVID Tracking Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://covidtracking.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The data are an aggregation of figures released by individual states. The Project aim to report on the number of people tested, including private labs, but not all states report their figures in this way. The figures for some states appear to include antibody tests in addition to PCR tests.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a collaborative project launched in order to fill some of the important gaps in the testing figures being collated by the CDC.
+Testing data is gathered from individual states, as reported in state health department websites, data dashboards and press releases from officials.
+As of 26 May, there have been a number of media reports noting that the testing figures released by some states include antibody tests in addition to PCR tests – as discussed in [this article](https://www.theatlantic.com/health/archive/2020/05/cdc-and-states-are-misreporting-covid-19-test-data-pennsylvania-georgia-texas/611935/) in The Atlantic. Our dataset aims to report only PCR tests. But becasue some states do not disaggregate these types of tests we are not currently able to exclude the antibody tests.
+Other differences across states include: some report the number of tests performed, others the number of people tested; some include private labs, others not; some report negative test results, others only positive test results; some include pending tests, others do not (below we show figures that exclude explicitly pending results).
+Moreover, many states do not explicitly provide details about these important factors needed to interpret the data they provide. 
+There are issues in comparing the figures over time. The totals given for early on in the outbreak do not include all states. One significant uncertainty is the extent to which the rapid rise in tests seen from the mid-March in part reflects states beginning to report private lab tests.
+Overall the figures should be seen as providing a general indication of testing output, rather than a specific count of a given indicator. Given the very incomplete coverage and reporting delays of the CDC data, it provides a very important additional perspective.
+The Project documents their work in lots of detail. See the link provided above for full details.</t>
+  </si>
+  <si>
     <t xml:space="preserve">URY</t>
   </si>
   <si>
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-40</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-42</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2060,7 +2050,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1266843967309713410</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1267885571126505472</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -2470,7 +2460,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2480,25 +2470,21 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H2" t="n">
-        <v>164084</v>
+        <v>172947</v>
       </c>
       <c r="I2" t="n">
-        <v>3.631</v>
-      </c>
-      <c r="J2" t="n">
-        <v>4014</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.089</v>
-      </c>
+        <v>3.827</v>
+      </c>
+      <c r="J2"/>
+      <c r="K2"/>
       <c r="L2" t="n">
-        <v>4435</v>
+        <v>4676</v>
       </c>
       <c r="M2" t="n">
-        <v>0.098</v>
+        <v>0.103</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -2521,7 +2507,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>43982</v>
+        <v>43984</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2531,25 +2517,25 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H3" t="n">
-        <v>1454568</v>
+        <v>1490387</v>
       </c>
       <c r="I3" t="n">
-        <v>57.042</v>
+        <v>58.447</v>
       </c>
       <c r="J3" t="n">
-        <v>26030</v>
+        <v>18167</v>
       </c>
       <c r="K3" t="n">
-        <v>1.021</v>
+        <v>0.712</v>
       </c>
       <c r="L3" t="n">
-        <v>32825</v>
+        <v>28881</v>
       </c>
       <c r="M3" t="n">
-        <v>1.287</v>
+        <v>1.133</v>
       </c>
       <c r="N3" t="s">
         <v>27</v>
@@ -2572,7 +2558,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -2582,25 +2568,25 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H4" t="n">
-        <v>451820</v>
+        <v>462958</v>
       </c>
       <c r="I4" t="n">
-        <v>50.167</v>
+        <v>51.403</v>
       </c>
       <c r="J4" t="n">
-        <v>3286</v>
+        <v>6580</v>
       </c>
       <c r="K4" t="n">
-        <v>0.365</v>
+        <v>0.731</v>
       </c>
       <c r="L4" t="n">
-        <v>6640</v>
+        <v>6322</v>
       </c>
       <c r="M4" t="n">
-        <v>0.737</v>
+        <v>0.702</v>
       </c>
       <c r="N4" t="s">
         <v>34</v>
@@ -2623,7 +2609,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2633,25 +2619,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H5" t="n">
-        <v>323162</v>
+        <v>337773</v>
       </c>
       <c r="I5" t="n">
-        <v>189.918</v>
+        <v>198.505</v>
       </c>
       <c r="J5" t="n">
-        <v>6355</v>
+        <v>7040</v>
       </c>
       <c r="K5" t="n">
-        <v>3.735</v>
+        <v>4.137</v>
       </c>
       <c r="L5" t="n">
-        <v>5611</v>
+        <v>6664</v>
       </c>
       <c r="M5" t="n">
-        <v>3.298</v>
+        <v>3.916</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
@@ -2674,7 +2660,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>43982</v>
+        <v>43984</v>
       </c>
       <c r="D6" t="s">
         <v>48</v>
@@ -2684,25 +2670,25 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H6" t="n">
-        <v>308930</v>
+        <v>333073</v>
       </c>
       <c r="I6" t="n">
-        <v>1.876</v>
+        <v>2.022</v>
       </c>
       <c r="J6" t="n">
-        <v>11876</v>
+        <v>12704</v>
       </c>
       <c r="K6" t="n">
-        <v>0.072</v>
+        <v>0.077</v>
       </c>
       <c r="L6" t="n">
-        <v>9335</v>
+        <v>10662</v>
       </c>
       <c r="M6" t="n">
-        <v>0.057</v>
+        <v>0.065</v>
       </c>
       <c r="N6" t="s">
         <v>49</v>
@@ -2725,7 +2711,7 @@
         <v>54</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>43983</v>
+        <v>43984</v>
       </c>
       <c r="D7" t="s">
         <v>55</v>
@@ -2735,25 +2721,25 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H7" t="n">
-        <v>553377</v>
+        <v>562945</v>
       </c>
       <c r="I7" t="n">
-        <v>58.563</v>
+        <v>59.575</v>
       </c>
       <c r="J7" t="n">
-        <v>12284</v>
+        <v>9568</v>
       </c>
       <c r="K7" t="n">
-        <v>1.3</v>
+        <v>1.013</v>
       </c>
       <c r="L7" t="n">
-        <v>12910</v>
+        <v>12863</v>
       </c>
       <c r="M7" t="n">
-        <v>1.366</v>
+        <v>1.361</v>
       </c>
       <c r="N7" t="s">
         <v>56</v>
@@ -2776,7 +2762,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>43981</v>
+        <v>43983</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
@@ -2786,25 +2772,25 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H8" t="n">
-        <v>698533</v>
+        <v>708996</v>
       </c>
       <c r="I8" t="n">
-        <v>60.272</v>
+        <v>61.175</v>
       </c>
       <c r="J8" t="n">
-        <v>6298</v>
+        <v>3122</v>
       </c>
       <c r="K8" t="n">
-        <v>0.543</v>
+        <v>0.269</v>
       </c>
       <c r="L8" t="n">
-        <v>8851</v>
+        <v>8675</v>
       </c>
       <c r="M8" t="n">
-        <v>0.764</v>
+        <v>0.749</v>
       </c>
       <c r="N8" t="s">
         <v>62</v>
@@ -2827,7 +2813,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>43982</v>
+        <v>43984</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
@@ -2837,25 +2823,25 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H9" t="n">
-        <v>28957</v>
+        <v>31186</v>
       </c>
       <c r="I9" t="n">
-        <v>2.481</v>
+        <v>2.672</v>
       </c>
       <c r="J9" t="n">
-        <v>718</v>
+        <v>1146</v>
       </c>
       <c r="K9" t="n">
-        <v>0.062</v>
+        <v>0.098</v>
       </c>
       <c r="L9" t="n">
-        <v>995</v>
+        <v>1078</v>
       </c>
       <c r="M9" t="n">
-        <v>0.085</v>
+        <v>0.092</v>
       </c>
       <c r="N9" t="s">
         <v>41</v>
@@ -2927,7 +2913,7 @@
         <v>81</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D11" t="s">
         <v>82</v>
@@ -2937,25 +2923,25 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H11" t="n">
-        <v>81694</v>
+        <v>84261</v>
       </c>
       <c r="I11" t="n">
-        <v>11.757</v>
+        <v>12.127</v>
       </c>
       <c r="J11" t="n">
-        <v>346</v>
+        <v>1347</v>
       </c>
       <c r="K11" t="n">
-        <v>0.05</v>
+        <v>0.194</v>
       </c>
       <c r="L11" t="n">
-        <v>1022</v>
+        <v>1124</v>
       </c>
       <c r="M11" t="n">
-        <v>0.147</v>
+        <v>0.162</v>
       </c>
       <c r="N11" t="s">
         <v>84</v>
@@ -2978,7 +2964,7 @@
         <v>88</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D12" t="s">
         <v>89</v>
@@ -2988,25 +2974,25 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H12" t="n">
-        <v>1691297</v>
+        <v>1751547</v>
       </c>
       <c r="I12" t="n">
-        <v>44.812</v>
+        <v>46.408</v>
       </c>
       <c r="J12" t="n">
-        <v>28255</v>
+        <v>30112</v>
       </c>
       <c r="K12" t="n">
-        <v>0.749</v>
+        <v>0.798</v>
       </c>
       <c r="L12" t="n">
-        <v>30219</v>
+        <v>31901</v>
       </c>
       <c r="M12" t="n">
-        <v>0.801</v>
+        <v>0.845</v>
       </c>
       <c r="N12" t="s">
         <v>90</v>
@@ -3029,7 +3015,7 @@
         <v>95</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D13" t="s">
         <v>96</v>
@@ -3041,25 +3027,25 @@
         <v>97</v>
       </c>
       <c r="G13" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H13" t="n">
-        <v>599190</v>
+        <v>628318</v>
       </c>
       <c r="I13" t="n">
-        <v>31.345</v>
+        <v>32.868</v>
       </c>
       <c r="J13" t="n">
-        <v>16750</v>
+        <v>15546</v>
       </c>
       <c r="K13" t="n">
-        <v>0.876</v>
+        <v>0.813</v>
       </c>
       <c r="L13" t="n">
-        <v>15878</v>
+        <v>16256</v>
       </c>
       <c r="M13" t="n">
-        <v>0.831</v>
+        <v>0.85</v>
       </c>
       <c r="N13" t="s">
         <v>98</v>
@@ -3082,7 +3068,7 @@
         <v>102</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>43982</v>
+        <v>43984</v>
       </c>
       <c r="D14" t="s">
         <v>103</v>
@@ -3092,22 +3078,22 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H14" t="n">
-        <v>331817</v>
+        <v>350213</v>
       </c>
       <c r="I14" t="n">
-        <v>6.521</v>
+        <v>6.883</v>
       </c>
       <c r="J14" t="n">
-        <v>12038</v>
+        <v>9071</v>
       </c>
       <c r="K14" t="n">
-        <v>0.237</v>
+        <v>0.178</v>
       </c>
       <c r="L14" t="n">
-        <v>11296</v>
+        <v>11299</v>
       </c>
       <c r="M14" t="n">
         <v>0.222</v>
@@ -3133,7 +3119,7 @@
         <v>109</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>43982</v>
+        <v>43985</v>
       </c>
       <c r="D15" t="s">
         <v>110</v>
@@ -3143,25 +3129,25 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H15" t="n">
-        <v>19176</v>
+        <v>20122</v>
       </c>
       <c r="I15" t="n">
-        <v>3.764</v>
+        <v>3.95</v>
       </c>
       <c r="J15" t="n">
-        <v>515</v>
+        <v>415</v>
       </c>
       <c r="K15" t="n">
-        <v>0.101</v>
+        <v>0.081</v>
       </c>
       <c r="L15" t="n">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="M15" t="n">
-        <v>0.079</v>
+        <v>0.08</v>
       </c>
       <c r="N15" t="s">
         <v>111</v>
@@ -3184,7 +3170,7 @@
         <v>115</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D16" t="s">
         <v>116</v>
@@ -3194,25 +3180,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H16" t="n">
-        <v>66695</v>
+        <v>67814</v>
       </c>
       <c r="I16" t="n">
-        <v>16.246</v>
+        <v>16.519</v>
       </c>
       <c r="J16" t="n">
-        <v>290</v>
+        <v>517</v>
       </c>
       <c r="K16" t="n">
-        <v>0.071</v>
+        <v>0.126</v>
       </c>
       <c r="L16" t="n">
-        <v>610</v>
+        <v>507</v>
       </c>
       <c r="M16" t="n">
-        <v>0.149</v>
+        <v>0.123</v>
       </c>
       <c r="N16" t="s">
         <v>117</v>
@@ -3235,7 +3221,7 @@
         <v>122</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>43982</v>
+        <v>43984</v>
       </c>
       <c r="D17" t="s">
         <v>123</v>
@@ -3247,25 +3233,25 @@
         <v>125</v>
       </c>
       <c r="G17" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H17" t="n">
-        <v>107037</v>
+        <v>110349</v>
       </c>
       <c r="I17" t="n">
-        <v>9.45</v>
+        <v>9.742</v>
       </c>
       <c r="J17" t="n">
-        <v>1763</v>
+        <v>1960</v>
       </c>
       <c r="K17" t="n">
-        <v>0.156</v>
+        <v>0.173</v>
       </c>
       <c r="L17" t="n">
-        <v>1647</v>
+        <v>1710</v>
       </c>
       <c r="M17" t="n">
-        <v>0.145</v>
+        <v>0.151</v>
       </c>
       <c r="N17" t="s">
         <v>124</v>
@@ -3288,7 +3274,7 @@
         <v>130</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>43982</v>
+        <v>43984</v>
       </c>
       <c r="D18" t="s">
         <v>131</v>
@@ -3298,25 +3284,25 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H18" t="n">
-        <v>442866</v>
+        <v>454397</v>
       </c>
       <c r="I18" t="n">
-        <v>41.355</v>
+        <v>42.431</v>
       </c>
       <c r="J18" t="n">
-        <v>2105</v>
+        <v>6116</v>
       </c>
       <c r="K18" t="n">
-        <v>0.197</v>
+        <v>0.571</v>
       </c>
       <c r="L18" t="n">
-        <v>5592</v>
+        <v>5146</v>
       </c>
       <c r="M18" t="n">
-        <v>0.522</v>
+        <v>0.481</v>
       </c>
       <c r="N18" t="s">
         <v>41</v>
@@ -3339,7 +3325,7 @@
         <v>135</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D19" t="s">
         <v>136</v>
@@ -3349,25 +3335,25 @@
       </c>
       <c r="F19"/>
       <c r="G19" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H19" t="n">
-        <v>528982</v>
+        <v>542895</v>
       </c>
       <c r="I19" t="n">
-        <v>91.327</v>
+        <v>93.729</v>
       </c>
       <c r="J19" t="n">
-        <v>6388</v>
+        <v>8113</v>
       </c>
       <c r="K19" t="n">
-        <v>1.103</v>
+        <v>1.401</v>
       </c>
       <c r="L19" t="n">
-        <v>10097</v>
+        <v>8951</v>
       </c>
       <c r="M19" t="n">
-        <v>1.743</v>
+        <v>1.545</v>
       </c>
       <c r="N19" t="s">
         <v>138</v>
@@ -3390,7 +3376,7 @@
         <v>142</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>43982</v>
+        <v>43984</v>
       </c>
       <c r="D20" t="s">
         <v>143</v>
@@ -3402,21 +3388,21 @@
         <v>145</v>
       </c>
       <c r="G20" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H20" t="n">
-        <v>68988</v>
+        <v>72769</v>
       </c>
       <c r="I20" t="n">
-        <v>3.91</v>
+        <v>4.125</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20" t="n">
-        <v>1009</v>
+        <v>1142</v>
       </c>
       <c r="M20" t="n">
-        <v>0.057</v>
+        <v>0.065</v>
       </c>
       <c r="N20" t="s">
         <v>144</v>
@@ -3439,7 +3425,7 @@
         <v>149</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>43981</v>
+        <v>43983</v>
       </c>
       <c r="D21" t="s">
         <v>150</v>
@@ -3449,25 +3435,25 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H21" t="n">
-        <v>89358</v>
+        <v>94272</v>
       </c>
       <c r="I21" t="n">
-        <v>13.777</v>
+        <v>14.534</v>
       </c>
       <c r="J21" t="n">
-        <v>2386</v>
+        <v>2435</v>
       </c>
       <c r="K21" t="n">
-        <v>0.368</v>
+        <v>0.375</v>
       </c>
       <c r="L21" t="n">
-        <v>2392</v>
+        <v>2399</v>
       </c>
       <c r="M21" t="n">
-        <v>0.369</v>
+        <v>0.37</v>
       </c>
       <c r="N21" t="s">
         <v>151</v>
@@ -3490,7 +3476,7 @@
         <v>155</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>43982</v>
+        <v>43984</v>
       </c>
       <c r="D22" t="s">
         <v>156</v>
@@ -3500,25 +3486,25 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H22" t="n">
-        <v>84157</v>
+        <v>86435</v>
       </c>
       <c r="I22" t="n">
-        <v>63.441</v>
+        <v>65.158</v>
       </c>
       <c r="J22" t="n">
-        <v>716</v>
+        <v>1262</v>
       </c>
       <c r="K22" t="n">
-        <v>0.54</v>
+        <v>0.951</v>
       </c>
       <c r="L22" t="n">
-        <v>1082</v>
+        <v>976</v>
       </c>
       <c r="M22" t="n">
-        <v>0.816</v>
+        <v>0.736</v>
       </c>
       <c r="N22" t="s">
         <v>158</v>
@@ -3541,7 +3527,7 @@
         <v>163</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D23" t="s">
         <v>164</v>
@@ -3551,25 +3537,25 @@
       </c>
       <c r="F23"/>
       <c r="G23" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H23" t="n">
-        <v>112377</v>
+        <v>120429</v>
       </c>
       <c r="I23" t="n">
-        <v>0.978</v>
+        <v>1.048</v>
       </c>
       <c r="J23" t="n">
-        <v>2926</v>
+        <v>4120</v>
       </c>
       <c r="K23" t="n">
-        <v>0.025</v>
+        <v>0.036</v>
       </c>
       <c r="L23" t="n">
-        <v>4075</v>
+        <v>4116</v>
       </c>
       <c r="M23" t="n">
-        <v>0.035</v>
+        <v>0.036</v>
       </c>
       <c r="N23" t="s">
         <v>165</v>
@@ -3592,7 +3578,7 @@
         <v>169</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>43981</v>
+        <v>43983</v>
       </c>
       <c r="D24" t="s">
         <v>170</v>
@@ -3602,25 +3588,25 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H24" t="n">
-        <v>185283</v>
+        <v>192410</v>
       </c>
       <c r="I24" t="n">
-        <v>33.44</v>
+        <v>34.727</v>
       </c>
       <c r="J24" t="n">
-        <v>1363</v>
+        <v>1346</v>
       </c>
       <c r="K24" t="n">
-        <v>0.246</v>
+        <v>0.243</v>
       </c>
       <c r="L24" t="n">
-        <v>2172</v>
+        <v>2354</v>
       </c>
       <c r="M24" t="n">
-        <v>0.392</v>
+        <v>0.425</v>
       </c>
       <c r="N24" t="s">
         <v>172</v>
@@ -3843,7 +3829,7 @@
         <v>202</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>43981</v>
+        <v>43982</v>
       </c>
       <c r="D29" t="s">
         <v>195</v>
@@ -3855,25 +3841,25 @@
         <v>203</v>
       </c>
       <c r="G29" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H29" t="n">
-        <v>218425</v>
+        <v>219825</v>
       </c>
       <c r="I29" t="n">
-        <v>7.029</v>
+        <v>7.074</v>
       </c>
       <c r="J29" t="n">
-        <v>3469</v>
+        <v>1400</v>
       </c>
       <c r="K29" t="n">
-        <v>0.112</v>
+        <v>0.045</v>
       </c>
       <c r="L29" t="n">
-        <v>2893</v>
+        <v>2528</v>
       </c>
       <c r="M29" t="n">
-        <v>0.093</v>
+        <v>0.081</v>
       </c>
       <c r="N29" t="s">
         <v>198</v>
@@ -3896,7 +3882,7 @@
         <v>205</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>43983</v>
+        <v>43984</v>
       </c>
       <c r="D30" t="s">
         <v>206</v>
@@ -3906,25 +3892,25 @@
       </c>
       <c r="F30"/>
       <c r="G30" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H30" t="n">
-        <v>182423</v>
+        <v>185590</v>
       </c>
       <c r="I30" t="n">
-        <v>17.502</v>
+        <v>17.806</v>
       </c>
       <c r="J30" t="n">
-        <v>1905</v>
+        <v>3167</v>
       </c>
       <c r="K30" t="n">
-        <v>0.183</v>
+        <v>0.304</v>
       </c>
       <c r="L30" t="n">
-        <v>3912</v>
+        <v>3514</v>
       </c>
       <c r="M30" t="n">
-        <v>0.375</v>
+        <v>0.337</v>
       </c>
       <c r="N30" t="s">
         <v>208</v>
@@ -3994,7 +3980,7 @@
         <v>219</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D32" t="s">
         <v>220</v>
@@ -4006,25 +3992,25 @@
         <v>222</v>
       </c>
       <c r="G32" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H32" t="n">
-        <v>187965</v>
+        <v>191572</v>
       </c>
       <c r="I32" t="n">
-        <v>19.457</v>
+        <v>19.831</v>
       </c>
       <c r="J32" t="n">
-        <v>1985</v>
+        <v>1603</v>
       </c>
       <c r="K32" t="n">
-        <v>0.205</v>
+        <v>0.166</v>
       </c>
       <c r="L32" t="n">
-        <v>3335</v>
+        <v>3087</v>
       </c>
       <c r="M32" t="n">
-        <v>0.345</v>
+        <v>0.32</v>
       </c>
       <c r="N32" t="s">
         <v>221</v>
@@ -4047,7 +4033,7 @@
         <v>227</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>43981</v>
+        <v>43984</v>
       </c>
       <c r="D33" t="s">
         <v>228</v>
@@ -4057,25 +4043,25 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H33" t="n">
-        <v>61081</v>
+        <v>61314</v>
       </c>
       <c r="I33" t="n">
-        <v>178.992</v>
+        <v>179.675</v>
       </c>
       <c r="J33" t="n">
-        <v>97</v>
+        <v>199</v>
       </c>
       <c r="K33" t="n">
-        <v>0.284</v>
+        <v>0.583</v>
       </c>
       <c r="L33" t="n">
-        <v>325</v>
+        <v>249</v>
       </c>
       <c r="M33" t="n">
-        <v>0.952</v>
+        <v>0.73</v>
       </c>
       <c r="N33" t="s">
         <v>229</v>
@@ -4151,7 +4137,7 @@
         <v>238</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>43982</v>
+        <v>43984</v>
       </c>
       <c r="D35" t="s">
         <v>234</v>
@@ -4163,25 +4149,25 @@
         <v>236</v>
       </c>
       <c r="G35" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H35" t="n">
-        <v>3737027</v>
+        <v>3966075</v>
       </c>
       <c r="I35" t="n">
-        <v>2.708</v>
+        <v>2.874</v>
       </c>
       <c r="J35" t="n">
-        <v>125428</v>
+        <v>128868</v>
       </c>
       <c r="K35" t="n">
-        <v>0.091</v>
+        <v>0.093</v>
       </c>
       <c r="L35" t="n">
-        <v>113372</v>
+        <v>119994</v>
       </c>
       <c r="M35" t="n">
-        <v>0.082</v>
+        <v>0.087</v>
       </c>
       <c r="N35" t="s">
         <v>235</v>
@@ -4204,7 +4190,7 @@
         <v>240</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D36" t="s">
         <v>241</v>
@@ -4214,25 +4200,25 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H36" t="n">
-        <v>232113</v>
+        <v>246433</v>
       </c>
       <c r="I36" t="n">
-        <v>0.849</v>
+        <v>0.901</v>
       </c>
       <c r="J36" t="n">
-        <v>8489</v>
+        <v>8486</v>
       </c>
       <c r="K36" t="n">
         <v>0.031</v>
       </c>
       <c r="L36" t="n">
-        <v>6989</v>
+        <v>7274</v>
       </c>
       <c r="M36" t="n">
-        <v>0.026</v>
+        <v>0.027</v>
       </c>
       <c r="N36" t="s">
         <v>242</v>
@@ -4255,7 +4241,7 @@
         <v>247</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>43982</v>
+        <v>43984</v>
       </c>
       <c r="D37" t="s">
         <v>248</v>
@@ -4265,25 +4251,25 @@
       </c>
       <c r="F37"/>
       <c r="G37" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H37" t="n">
-        <v>935894</v>
+        <v>975936</v>
       </c>
       <c r="I37" t="n">
-        <v>11.143</v>
+        <v>11.619</v>
       </c>
       <c r="J37" t="n">
-        <v>19896</v>
+        <v>20071</v>
       </c>
       <c r="K37" t="n">
-        <v>0.237</v>
+        <v>0.239</v>
       </c>
       <c r="L37" t="n">
-        <v>19339</v>
+        <v>19835</v>
       </c>
       <c r="M37" t="n">
-        <v>0.23</v>
+        <v>0.236</v>
       </c>
       <c r="N37" t="s">
         <v>249</v>
@@ -4306,7 +4292,7 @@
         <v>253</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>43977</v>
+        <v>43984</v>
       </c>
       <c r="D38" t="s">
         <v>254</v>
@@ -4316,21 +4302,21 @@
       </c>
       <c r="F38"/>
       <c r="G38" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H38" t="n">
-        <v>325795</v>
+        <v>348416</v>
       </c>
       <c r="I38" t="n">
-        <v>65.98</v>
+        <v>70.561</v>
       </c>
       <c r="J38"/>
       <c r="K38"/>
       <c r="L38" t="n">
-        <v>4310</v>
+        <v>3232</v>
       </c>
       <c r="M38" t="n">
-        <v>0.873</v>
+        <v>0.655</v>
       </c>
       <c r="N38" t="s">
         <v>214</v>
@@ -4353,7 +4339,7 @@
         <v>259</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>43971</v>
+        <v>43978</v>
       </c>
       <c r="D39" t="s">
         <v>260</v>
@@ -4363,25 +4349,25 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="H39" t="n">
-        <v>525728</v>
+        <v>559756</v>
       </c>
       <c r="I39" t="n">
-        <v>60.739</v>
+        <v>64.67</v>
       </c>
       <c r="J39" t="n">
-        <v>5968</v>
+        <v>6642</v>
       </c>
       <c r="K39" t="n">
-        <v>0.69</v>
+        <v>0.767</v>
       </c>
       <c r="L39" t="n">
-        <v>5835</v>
+        <v>4900</v>
       </c>
       <c r="M39" t="n">
-        <v>0.674</v>
+        <v>0.566</v>
       </c>
       <c r="N39" t="s">
         <v>41</v>
@@ -4404,7 +4390,7 @@
         <v>265</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D40" t="s">
         <v>266</v>
@@ -4416,25 +4402,25 @@
         <v>268</v>
       </c>
       <c r="G40" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H40" t="n">
-        <v>2451674</v>
+        <v>2497337</v>
       </c>
       <c r="I40" t="n">
-        <v>40.549</v>
+        <v>41.304</v>
       </c>
       <c r="J40" t="n">
-        <v>18053</v>
+        <v>20035</v>
       </c>
       <c r="K40" t="n">
-        <v>0.299</v>
+        <v>0.331</v>
       </c>
       <c r="L40" t="n">
-        <v>33195</v>
+        <v>29541</v>
       </c>
       <c r="M40" t="n">
-        <v>0.549</v>
+        <v>0.489</v>
       </c>
       <c r="N40" t="s">
         <v>269</v>
@@ -4457,7 +4443,7 @@
         <v>272</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D41" t="s">
         <v>266</v>
@@ -4469,25 +4455,25 @@
         <v>268</v>
       </c>
       <c r="G41" t="n">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H41" t="n">
-        <v>3910133</v>
+        <v>3999591</v>
       </c>
       <c r="I41" t="n">
-        <v>64.671</v>
+        <v>66.151</v>
       </c>
       <c r="J41" t="n">
-        <v>31394</v>
+        <v>37299</v>
       </c>
       <c r="K41" t="n">
-        <v>0.519</v>
+        <v>0.617</v>
       </c>
       <c r="L41" t="n">
-        <v>61126</v>
+        <v>56049</v>
       </c>
       <c r="M41" t="n">
-        <v>1.011</v>
+        <v>0.927</v>
       </c>
       <c r="N41" t="s">
         <v>269</v>
@@ -4510,7 +4496,7 @@
         <v>275</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D42" t="s">
         <v>276</v>
@@ -4522,21 +4508,21 @@
         <v>278</v>
       </c>
       <c r="G42" t="n">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H42" t="n">
-        <v>292569</v>
+        <v>300277</v>
       </c>
       <c r="I42" t="n">
-        <v>2.313</v>
+        <v>2.374</v>
       </c>
       <c r="J42"/>
       <c r="K42"/>
       <c r="L42" t="n">
-        <v>2840</v>
+        <v>3091</v>
       </c>
       <c r="M42" t="n">
-        <v>0.022</v>
+        <v>0.024</v>
       </c>
       <c r="N42" t="s">
         <v>279</v>
@@ -4559,7 +4545,7 @@
         <v>282</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>43981</v>
+        <v>43983</v>
       </c>
       <c r="D43" t="s">
         <v>283</v>
@@ -4571,25 +4557,25 @@
         <v>284</v>
       </c>
       <c r="G43" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H43" t="n">
-        <v>473507</v>
+        <v>489518</v>
       </c>
       <c r="I43" t="n">
-        <v>3.744</v>
+        <v>3.87</v>
       </c>
       <c r="J43" t="n">
-        <v>1547</v>
+        <v>3454</v>
       </c>
       <c r="K43" t="n">
-        <v>0.012</v>
+        <v>0.027</v>
       </c>
       <c r="L43" t="n">
-        <v>3831</v>
+        <v>5138</v>
       </c>
       <c r="M43" t="n">
-        <v>0.03</v>
+        <v>0.041</v>
       </c>
       <c r="N43" t="s">
         <v>279</v>
@@ -4612,7 +4598,7 @@
         <v>287</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>43982</v>
+        <v>43985</v>
       </c>
       <c r="D44" t="s">
         <v>288</v>
@@ -4622,25 +4608,25 @@
       </c>
       <c r="F44"/>
       <c r="G44" t="n">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H44" t="n">
-        <v>812881</v>
+        <v>867286</v>
       </c>
       <c r="I44" t="n">
-        <v>43.292</v>
+        <v>46.189</v>
       </c>
       <c r="J44" t="n">
-        <v>24592</v>
+        <v>23660</v>
       </c>
       <c r="K44" t="n">
-        <v>1.31</v>
+        <v>1.26</v>
       </c>
       <c r="L44" t="n">
-        <v>22238</v>
+        <v>22419</v>
       </c>
       <c r="M44" t="n">
-        <v>1.184</v>
+        <v>1.194</v>
       </c>
       <c r="N44" t="s">
         <v>289</v>
@@ -4663,7 +4649,7 @@
         <v>292</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>43982</v>
+        <v>43984</v>
       </c>
       <c r="D45" t="s">
         <v>293</v>
@@ -4673,21 +4659,25 @@
       </c>
       <c r="F45"/>
       <c r="G45" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H45" t="n">
-        <v>78536</v>
+        <v>82946</v>
       </c>
       <c r="I45" t="n">
-        <v>1.461</v>
-      </c>
-      <c r="J45"/>
-      <c r="K45"/>
+        <v>1.543</v>
+      </c>
+      <c r="J45" t="n">
+        <v>2892</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0.054</v>
+      </c>
       <c r="L45" t="n">
-        <v>2754</v>
+        <v>2669</v>
       </c>
       <c r="M45" t="n">
-        <v>0.051</v>
+        <v>0.05</v>
       </c>
       <c r="N45" t="s">
         <v>41</v>
@@ -4710,7 +4700,7 @@
         <v>299</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D46" t="s">
         <v>300</v>
@@ -4722,25 +4712,25 @@
         <v>302</v>
       </c>
       <c r="G46" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H46" t="n">
-        <v>109723</v>
+        <v>112965</v>
       </c>
       <c r="I46" t="n">
-        <v>58.171</v>
+        <v>59.89</v>
       </c>
       <c r="J46" t="n">
-        <v>652</v>
+        <v>1561</v>
       </c>
       <c r="K46" t="n">
-        <v>0.346</v>
+        <v>0.828</v>
       </c>
       <c r="L46" t="n">
-        <v>1422</v>
+        <v>1345</v>
       </c>
       <c r="M46" t="n">
-        <v>0.754</v>
+        <v>0.713</v>
       </c>
       <c r="N46" t="s">
         <v>301</v>
@@ -4763,7 +4753,7 @@
         <v>305</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D47" t="s">
         <v>306</v>
@@ -4773,25 +4763,25 @@
       </c>
       <c r="F47"/>
       <c r="G47" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H47" t="n">
-        <v>304854</v>
+        <v>315112</v>
       </c>
       <c r="I47" t="n">
-        <v>111.984</v>
+        <v>115.753</v>
       </c>
       <c r="J47" t="n">
-        <v>1995</v>
+        <v>5387</v>
       </c>
       <c r="K47" t="n">
-        <v>0.733</v>
+        <v>1.979</v>
       </c>
       <c r="L47" t="n">
-        <v>4995</v>
+        <v>4840</v>
       </c>
       <c r="M47" t="n">
-        <v>1.835</v>
+        <v>1.778</v>
       </c>
       <c r="N47" t="s">
         <v>41</v>
@@ -4814,7 +4804,7 @@
         <v>310</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>43982</v>
+        <v>43985</v>
       </c>
       <c r="D48" t="s">
         <v>311</v>
@@ -4824,25 +4814,25 @@
       </c>
       <c r="F48"/>
       <c r="G48" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H48" t="n">
-        <v>75432</v>
+        <v>79484</v>
       </c>
       <c r="I48" t="n">
-        <v>120.503</v>
+        <v>126.976</v>
       </c>
       <c r="J48" t="n">
-        <v>1066</v>
+        <v>1458</v>
       </c>
       <c r="K48" t="n">
-        <v>1.703</v>
+        <v>2.329</v>
       </c>
       <c r="L48" t="n">
-        <v>1100</v>
+        <v>1334</v>
       </c>
       <c r="M48" t="n">
-        <v>1.757</v>
+        <v>2.131</v>
       </c>
       <c r="N48" t="s">
         <v>312</v>
@@ -4918,7 +4908,7 @@
         <v>323</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>43981</v>
+        <v>43984</v>
       </c>
       <c r="D50" t="s">
         <v>324</v>
@@ -4930,25 +4920,25 @@
         <v>326</v>
       </c>
       <c r="G50" t="n">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H50" t="n">
-        <v>23127</v>
+        <v>25591</v>
       </c>
       <c r="I50" t="n">
-        <v>42.785</v>
+        <v>47.343</v>
       </c>
       <c r="J50" t="n">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="K50" t="n">
-        <v>1.495</v>
+        <v>1.493</v>
       </c>
       <c r="L50" t="n">
-        <v>765</v>
+        <v>796</v>
       </c>
       <c r="M50" t="n">
-        <v>1.415</v>
+        <v>1.473</v>
       </c>
       <c r="N50" t="s">
         <v>327</v>
@@ -4971,7 +4961,7 @@
         <v>331</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>43980</v>
+        <v>43983</v>
       </c>
       <c r="D51" t="s">
         <v>332</v>
@@ -4981,25 +4971,25 @@
       </c>
       <c r="F51"/>
       <c r="G51" t="n">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H51" t="n">
-        <v>238119</v>
+        <v>250911</v>
       </c>
       <c r="I51" t="n">
-        <v>1.847</v>
+        <v>1.946</v>
       </c>
       <c r="J51" t="n">
-        <v>1414</v>
+        <v>445</v>
       </c>
       <c r="K51" t="n">
-        <v>0.011</v>
+        <v>0.003</v>
       </c>
       <c r="L51" t="n">
-        <v>4076</v>
+        <v>3710</v>
       </c>
       <c r="M51" t="n">
-        <v>0.032</v>
+        <v>0.029</v>
       </c>
       <c r="N51" t="s">
         <v>333</v>
@@ -5075,7 +5065,7 @@
         <v>343</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>43982</v>
+        <v>43983</v>
       </c>
       <c r="D53" t="s">
         <v>344</v>
@@ -5083,72 +5073,74 @@
       <c r="E53" t="s">
         <v>345</v>
       </c>
-      <c r="F53" t="s">
-        <v>346</v>
-      </c>
+      <c r="F53"/>
       <c r="G53" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H53" t="n">
-        <v>24710</v>
+        <v>28251</v>
       </c>
       <c r="I53" t="n">
-        <v>0.454</v>
-      </c>
-      <c r="J53"/>
-      <c r="K53"/>
+        <v>0.519</v>
+      </c>
+      <c r="J53" t="n">
+        <v>1174</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.022</v>
+      </c>
       <c r="L53" t="n">
-        <v>737</v>
+        <v>1134</v>
       </c>
       <c r="M53" t="n">
-        <v>0.014</v>
+        <v>0.021</v>
       </c>
       <c r="N53" t="s">
         <v>345</v>
       </c>
       <c r="O53" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P53" t="s">
         <v>51</v>
       </c>
       <c r="Q53" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
+        <v>348</v>
+      </c>
+      <c r="B54" t="s">
         <v>349</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" s="1" t="n">
+        <v>43982</v>
+      </c>
+      <c r="D54" t="s">
         <v>350</v>
       </c>
-      <c r="C54" s="1" t="n">
-        <v>43981</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>351</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>352</v>
       </c>
-      <c r="F54" t="s">
-        <v>353</v>
-      </c>
       <c r="G54" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H54" t="n">
-        <v>66729</v>
+        <v>69587</v>
       </c>
       <c r="I54" t="n">
-        <v>2.29</v>
+        <v>2.388</v>
       </c>
       <c r="J54" t="n">
-        <v>2575</v>
+        <v>2858</v>
       </c>
       <c r="K54" t="n">
-        <v>0.088</v>
+        <v>0.098</v>
       </c>
       <c r="L54" t="n">
         <v>2967</v>
@@ -5157,287 +5149,291 @@
         <v>0.102</v>
       </c>
       <c r="N54" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="O54" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="P54" t="s">
         <v>92</v>
       </c>
       <c r="Q54" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
+        <v>355</v>
+      </c>
+      <c r="B55" t="s">
         <v>356</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" s="1" t="n">
+        <v>43983</v>
+      </c>
+      <c r="D55" t="s">
         <v>357</v>
       </c>
-      <c r="C55" s="1" t="n">
-        <v>43979</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>358</v>
-      </c>
-      <c r="E55" t="s">
-        <v>359</v>
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H55" t="n">
-        <v>349274</v>
+        <v>359833</v>
       </c>
       <c r="I55" t="n">
-        <v>20.384</v>
+        <v>21</v>
       </c>
       <c r="J55" t="n">
-        <v>4940</v>
+        <v>1903</v>
       </c>
       <c r="K55" t="n">
-        <v>0.288</v>
+        <v>0.111</v>
       </c>
       <c r="L55" t="n">
-        <v>4762</v>
+        <v>3948</v>
       </c>
       <c r="M55" t="n">
-        <v>0.278</v>
+        <v>0.23</v>
       </c>
       <c r="N55" t="s">
+        <v>359</v>
+      </c>
+      <c r="O55" t="s">
         <v>360</v>
-      </c>
-      <c r="O55" t="s">
-        <v>361</v>
       </c>
       <c r="P55" t="s">
         <v>92</v>
       </c>
       <c r="Q55" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>362</v>
+      </c>
+      <c r="B56" t="s">
         <v>363</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" s="1" t="n">
+        <v>43984</v>
+      </c>
+      <c r="D56" t="s">
         <v>364</v>
-      </c>
-      <c r="C56" s="1" t="n">
-        <v>43981</v>
-      </c>
-      <c r="D56" t="s">
-        <v>365</v>
       </c>
       <c r="E56" t="s">
         <v>41</v>
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H56" t="n">
-        <v>280983</v>
+        <v>283525</v>
       </c>
       <c r="I56" t="n">
-        <v>58.268</v>
+        <v>58.795</v>
       </c>
       <c r="J56" t="n">
-        <v>2111</v>
+        <v>1262</v>
       </c>
       <c r="K56" t="n">
-        <v>0.438</v>
+        <v>0.262</v>
       </c>
       <c r="L56" t="n">
-        <v>3119</v>
+        <v>2299</v>
       </c>
       <c r="M56" t="n">
-        <v>0.647</v>
+        <v>0.477</v>
       </c>
       <c r="N56" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="O56" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="P56" t="s">
         <v>22</v>
       </c>
       <c r="Q56" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
+        <v>367</v>
+      </c>
+      <c r="B57" t="s">
         <v>368</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" s="1" t="n">
+        <v>43985</v>
+      </c>
+      <c r="D57" t="s">
         <v>369</v>
       </c>
-      <c r="C57" s="1" t="n">
-        <v>43983</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>370</v>
-      </c>
-      <c r="E57" t="s">
-        <v>371</v>
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H57" t="n">
-        <v>63882</v>
+        <v>69801</v>
       </c>
       <c r="I57" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="J57"/>
-      <c r="K57"/>
+        <v>0.339</v>
+      </c>
+      <c r="J57" t="n">
+        <v>3916</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0.019</v>
+      </c>
       <c r="L57" t="n">
-        <v>2600</v>
+        <v>3037</v>
       </c>
       <c r="M57" t="n">
-        <v>0.013</v>
+        <v>0.015</v>
       </c>
       <c r="N57" t="s">
+        <v>370</v>
+      </c>
+      <c r="O57" t="s">
         <v>371</v>
-      </c>
-      <c r="O57" t="s">
-        <v>372</v>
       </c>
       <c r="P57" t="s">
         <v>51</v>
       </c>
       <c r="Q57" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
+        <v>373</v>
+      </c>
+      <c r="B58" t="s">
         <v>374</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" s="1" t="n">
+        <v>43985</v>
+      </c>
+      <c r="D58" t="s">
         <v>375</v>
       </c>
-      <c r="C58" s="1" t="n">
-        <v>43980</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>376</v>
-      </c>
-      <c r="E58" t="s">
-        <v>377</v>
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H58" t="n">
-        <v>245352</v>
+        <v>252232</v>
       </c>
       <c r="I58" t="n">
-        <v>45.258</v>
+        <v>46.527</v>
       </c>
       <c r="J58" t="n">
-        <v>2754</v>
+        <v>1264</v>
       </c>
       <c r="K58" t="n">
-        <v>0.508</v>
+        <v>0.233</v>
       </c>
       <c r="L58" t="n">
-        <v>2226</v>
+        <v>1767</v>
       </c>
       <c r="M58" t="n">
-        <v>0.411</v>
+        <v>0.326</v>
       </c>
       <c r="N58" t="s">
+        <v>376</v>
+      </c>
+      <c r="O58" t="s">
         <v>377</v>
       </c>
-      <c r="O58" t="s">
+      <c r="P58" t="s">
         <v>378</v>
       </c>
-      <c r="P58" t="s">
+      <c r="Q58" t="s">
         <v>379</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
+        <v>380</v>
+      </c>
+      <c r="B59" t="s">
         <v>381</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" s="1" t="n">
+        <v>43985</v>
+      </c>
+      <c r="D59" t="s">
         <v>382</v>
       </c>
-      <c r="C59" s="1" t="n">
-        <v>43983</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>383</v>
-      </c>
-      <c r="E59" t="s">
-        <v>384</v>
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H59" t="n">
-        <v>561136</v>
+        <v>595344</v>
       </c>
       <c r="I59" t="n">
-        <v>2.54</v>
+        <v>2.695</v>
       </c>
       <c r="J59" t="n">
-        <v>14106</v>
+        <v>17370</v>
       </c>
       <c r="K59" t="n">
-        <v>0.064</v>
+        <v>0.079</v>
       </c>
       <c r="L59" t="n">
-        <v>11069</v>
+        <v>13706</v>
       </c>
       <c r="M59" t="n">
-        <v>0.05</v>
+        <v>0.062</v>
       </c>
       <c r="N59" t="s">
+        <v>383</v>
+      </c>
+      <c r="O59" t="s">
         <v>384</v>
-      </c>
-      <c r="O59" t="s">
-        <v>385</v>
       </c>
       <c r="P59" t="s">
         <v>22</v>
       </c>
       <c r="Q59" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
+        <v>386</v>
+      </c>
+      <c r="B60" t="s">
         <v>387</v>
-      </c>
-      <c r="B60" t="s">
-        <v>388</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>43979</v>
       </c>
       <c r="D60" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E60" t="s">
         <v>41</v>
       </c>
       <c r="F60" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G60" t="n">
         <v>81</v>
@@ -5464,339 +5460,343 @@
         <v>41</v>
       </c>
       <c r="O60" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="P60" t="s">
         <v>127</v>
       </c>
       <c r="Q60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
+        <v>392</v>
+      </c>
+      <c r="B61" t="s">
         <v>393</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" s="1" t="n">
+        <v>43984</v>
+      </c>
+      <c r="D61" t="s">
         <v>394</v>
       </c>
-      <c r="C61" s="1" t="n">
-        <v>43982</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>395</v>
-      </c>
-      <c r="E61" t="s">
-        <v>396</v>
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H61" t="n">
-        <v>30004</v>
+        <v>32106</v>
       </c>
       <c r="I61" t="n">
-        <v>4.207</v>
+        <v>4.501</v>
       </c>
       <c r="J61" t="n">
-        <v>851</v>
+        <v>1272</v>
       </c>
       <c r="K61" t="n">
+        <v>0.178</v>
+      </c>
+      <c r="L61" t="n">
+        <v>848</v>
+      </c>
+      <c r="M61" t="n">
         <v>0.119</v>
       </c>
-      <c r="L61" t="n">
-        <v>742</v>
-      </c>
-      <c r="M61" t="n">
-        <v>0.104</v>
-      </c>
       <c r="N61" t="s">
+        <v>395</v>
+      </c>
+      <c r="O61" t="s">
         <v>396</v>
-      </c>
-      <c r="O61" t="s">
-        <v>397</v>
       </c>
       <c r="P61" t="s">
         <v>51</v>
       </c>
       <c r="Q61" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
+        <v>398</v>
+      </c>
+      <c r="B62" t="s">
         <v>399</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" s="1" t="n">
+        <v>43985</v>
+      </c>
+      <c r="D62" t="s">
         <v>400</v>
-      </c>
-      <c r="C62" s="1" t="n">
-        <v>43983</v>
-      </c>
-      <c r="D62" t="s">
-        <v>401</v>
       </c>
       <c r="E62" t="s">
         <v>41</v>
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H62" t="n">
-        <v>144167</v>
+        <v>152228</v>
       </c>
       <c r="I62" t="n">
-        <v>4.372</v>
+        <v>4.617</v>
       </c>
       <c r="J62" t="n">
-        <v>3562</v>
+        <v>6603</v>
       </c>
       <c r="K62" t="n">
-        <v>0.108</v>
+        <v>0.2</v>
       </c>
       <c r="L62" t="n">
-        <v>2945</v>
+        <v>3539</v>
       </c>
       <c r="M62" t="n">
-        <v>0.089</v>
+        <v>0.107</v>
       </c>
       <c r="N62" t="s">
+        <v>401</v>
+      </c>
+      <c r="O62" t="s">
         <v>402</v>
-      </c>
-      <c r="O62" t="s">
-        <v>403</v>
       </c>
       <c r="P62" t="s">
         <v>92</v>
       </c>
       <c r="Q62" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
+        <v>404</v>
+      </c>
+      <c r="B63" t="s">
         <v>405</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" s="1" t="n">
+        <v>43983</v>
+      </c>
+      <c r="D63" t="s">
         <v>406</v>
       </c>
-      <c r="C63" s="1" t="n">
-        <v>43982</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>407</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>408</v>
       </c>
-      <c r="F63" t="s">
-        <v>409</v>
-      </c>
       <c r="G63" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H63" t="n">
-        <v>328835</v>
+        <v>337306</v>
       </c>
       <c r="I63" t="n">
-        <v>3.001</v>
-      </c>
-      <c r="J63"/>
-      <c r="K63"/>
+        <v>3.078</v>
+      </c>
+      <c r="J63" t="n">
+        <v>8471</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.077</v>
+      </c>
       <c r="L63" t="n">
-        <v>7274</v>
+        <v>7737</v>
       </c>
       <c r="M63" t="n">
-        <v>0.066</v>
+        <v>0.071</v>
       </c>
       <c r="N63" t="s">
         <v>214</v>
       </c>
       <c r="O63" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="P63" t="s">
         <v>92</v>
       </c>
       <c r="Q63" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
+        <v>410</v>
+      </c>
+      <c r="B64" t="s">
         <v>411</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" s="1" t="n">
+        <v>43985</v>
+      </c>
+      <c r="D64" t="s">
         <v>412</v>
       </c>
-      <c r="C64" s="1" t="n">
-        <v>43983</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>413</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>414</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" t="n">
+        <v>91</v>
+      </c>
+      <c r="H64" t="n">
+        <v>967177</v>
+      </c>
+      <c r="I64" t="n">
+        <v>25.555</v>
+      </c>
+      <c r="J64" t="n">
+        <v>21222</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0.561</v>
+      </c>
+      <c r="L64" t="n">
+        <v>20343</v>
+      </c>
+      <c r="M64" t="n">
+        <v>0.538</v>
+      </c>
+      <c r="N64" t="s">
         <v>415</v>
       </c>
-      <c r="G64" t="n">
-        <v>89</v>
-      </c>
-      <c r="H64" t="n">
-        <v>931520</v>
-      </c>
-      <c r="I64" t="n">
-        <v>24.613</v>
-      </c>
-      <c r="J64" t="n">
-        <v>15974</v>
-      </c>
-      <c r="K64" t="n">
-        <v>0.422</v>
-      </c>
-      <c r="L64" t="n">
-        <v>21706</v>
-      </c>
-      <c r="M64" t="n">
-        <v>0.574</v>
-      </c>
-      <c r="N64" t="s">
+      <c r="O64" t="s">
         <v>416</v>
-      </c>
-      <c r="O64" t="s">
-        <v>417</v>
       </c>
       <c r="P64" t="s">
         <v>51</v>
       </c>
       <c r="Q64" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
+        <v>418</v>
+      </c>
+      <c r="B65" t="s">
         <v>419</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" s="1" t="n">
+        <v>43982</v>
+      </c>
+      <c r="D65" t="s">
         <v>420</v>
-      </c>
-      <c r="C65" s="1" t="n">
-        <v>43978</v>
-      </c>
-      <c r="D65" t="s">
-        <v>421</v>
       </c>
       <c r="E65" t="s">
         <v>41</v>
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="H65" t="n">
-        <v>795838</v>
+        <v>847181</v>
       </c>
       <c r="I65" t="n">
-        <v>78.049</v>
+        <v>83.084</v>
       </c>
       <c r="J65" t="n">
-        <v>16897</v>
+        <v>6500</v>
       </c>
       <c r="K65" t="n">
-        <v>1.657</v>
+        <v>0.637</v>
       </c>
       <c r="L65" t="n">
-        <v>12806</v>
+        <v>13532</v>
       </c>
       <c r="M65" t="n">
-        <v>1.256</v>
+        <v>1.327</v>
       </c>
       <c r="N65" t="s">
+        <v>421</v>
+      </c>
+      <c r="O65" t="s">
+        <v>420</v>
+      </c>
+      <c r="P65" t="s">
         <v>422</v>
       </c>
-      <c r="O65" t="s">
-        <v>421</v>
-      </c>
-      <c r="P65" t="s">
+      <c r="Q65" t="s">
         <v>423</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
+        <v>424</v>
+      </c>
+      <c r="B66" t="s">
         <v>425</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" s="1" t="n">
+        <v>43985</v>
+      </c>
+      <c r="D66" t="s">
         <v>426</v>
       </c>
-      <c r="C66" s="1" t="n">
-        <v>43983</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>427</v>
-      </c>
-      <c r="E66" t="s">
-        <v>428</v>
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H66" t="n">
-        <v>225919</v>
+        <v>236437</v>
       </c>
       <c r="I66" t="n">
-        <v>78.415</v>
+        <v>82.066</v>
       </c>
       <c r="J66" t="n">
-        <v>3850</v>
+        <v>5339</v>
       </c>
       <c r="K66" t="n">
-        <v>1.336</v>
+        <v>1.853</v>
       </c>
       <c r="L66" t="n">
-        <v>4776</v>
+        <v>5037</v>
       </c>
       <c r="M66" t="n">
-        <v>1.658</v>
+        <v>1.748</v>
       </c>
       <c r="N66" t="s">
+        <v>427</v>
+      </c>
+      <c r="O66" t="s">
         <v>428</v>
-      </c>
-      <c r="O66" t="s">
-        <v>429</v>
       </c>
       <c r="P66" t="s">
         <v>92</v>
       </c>
       <c r="Q66" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
+        <v>430</v>
+      </c>
+      <c r="B67" t="s">
         <v>431</v>
-      </c>
-      <c r="B67" t="s">
-        <v>432</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>43980</v>
       </c>
       <c r="D67" t="s">
+        <v>432</v>
+      </c>
+      <c r="E67" t="s">
         <v>433</v>
       </c>
-      <c r="E67" t="s">
+      <c r="F67" t="s">
         <v>434</v>
-      </c>
-      <c r="F67" t="s">
-        <v>435</v>
       </c>
       <c r="G67" t="n">
         <v>79</v>
@@ -5820,592 +5820,592 @@
         <v>0.511</v>
       </c>
       <c r="N67" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="O67" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="P67" t="s">
         <v>22</v>
       </c>
       <c r="Q67" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
+        <v>436</v>
+      </c>
+      <c r="B68" t="s">
         <v>437</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" s="1" t="n">
+        <v>43985</v>
+      </c>
+      <c r="D68" t="s">
         <v>438</v>
       </c>
-      <c r="C68" s="1" t="n">
-        <v>43983</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>439</v>
-      </c>
-      <c r="E68" t="s">
-        <v>440</v>
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H68" t="n">
-        <v>10923108</v>
+        <v>11426045</v>
       </c>
       <c r="I68" t="n">
-        <v>74.849</v>
+        <v>78.296</v>
       </c>
       <c r="J68" t="n">
-        <v>279984</v>
+        <v>274423</v>
       </c>
       <c r="K68" t="n">
-        <v>1.919</v>
+        <v>1.88</v>
       </c>
       <c r="L68" t="n">
-        <v>282532</v>
+        <v>287150</v>
       </c>
       <c r="M68" t="n">
-        <v>1.936</v>
+        <v>1.968</v>
       </c>
       <c r="N68" t="s">
+        <v>439</v>
+      </c>
+      <c r="O68" t="s">
         <v>440</v>
-      </c>
-      <c r="O68" t="s">
-        <v>441</v>
       </c>
       <c r="P68" t="s">
         <v>22</v>
       </c>
       <c r="Q68" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
+        <v>442</v>
+      </c>
+      <c r="B69" t="s">
         <v>443</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" s="1" t="n">
+        <v>43984</v>
+      </c>
+      <c r="D69" t="s">
         <v>444</v>
       </c>
-      <c r="C69" s="1" t="n">
-        <v>43981</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>445</v>
-      </c>
-      <c r="E69" t="s">
-        <v>446</v>
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H69" t="n">
-        <v>66976</v>
+        <v>70108</v>
       </c>
       <c r="I69" t="n">
-        <v>5.171</v>
+        <v>5.413</v>
       </c>
       <c r="J69" t="n">
-        <v>1368</v>
+        <v>957</v>
       </c>
       <c r="K69" t="n">
-        <v>0.106</v>
+        <v>0.074</v>
       </c>
       <c r="L69" t="n">
-        <v>1414</v>
+        <v>1381</v>
       </c>
       <c r="M69" t="n">
-        <v>0.109</v>
+        <v>0.107</v>
       </c>
       <c r="N69" t="s">
+        <v>445</v>
+      </c>
+      <c r="O69" t="s">
         <v>446</v>
-      </c>
-      <c r="O69" t="s">
-        <v>447</v>
       </c>
       <c r="P69" t="s">
         <v>51</v>
       </c>
       <c r="Q69" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
+        <v>448</v>
+      </c>
+      <c r="B70" t="s">
         <v>449</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" s="1" t="n">
+        <v>43985</v>
+      </c>
+      <c r="D70" t="s">
         <v>450</v>
-      </c>
-      <c r="C70" s="1" t="n">
-        <v>43983</v>
-      </c>
-      <c r="D70" t="s">
-        <v>451</v>
       </c>
       <c r="E70" t="s">
         <v>41</v>
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H70" t="n">
-        <v>838623</v>
+        <v>870963</v>
       </c>
       <c r="I70" t="n">
-        <v>24.089</v>
+        <v>25.018</v>
       </c>
       <c r="J70" t="n">
-        <v>15854</v>
+        <v>16976</v>
       </c>
       <c r="K70" t="n">
-        <v>0.455</v>
+        <v>0.488</v>
       </c>
       <c r="L70" t="n">
-        <v>16649</v>
+        <v>16671</v>
       </c>
       <c r="M70" t="n">
-        <v>0.478</v>
+        <v>0.479</v>
       </c>
       <c r="N70" t="s">
         <v>41</v>
       </c>
       <c r="O70" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P70" t="s">
         <v>127</v>
       </c>
       <c r="Q70" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
+        <v>452</v>
+      </c>
+      <c r="B71" t="s">
         <v>453</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" s="1" t="n">
+        <v>43985</v>
+      </c>
+      <c r="D71" t="s">
         <v>454</v>
       </c>
-      <c r="C71" s="1" t="n">
-        <v>43983</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>455</v>
       </c>
-      <c r="E71" t="s">
+      <c r="F71" t="s">
         <v>456</v>
       </c>
-      <c r="F71" t="s">
+      <c r="G71" t="n">
+        <v>93</v>
+      </c>
+      <c r="H71" t="n">
+        <v>47647</v>
+      </c>
+      <c r="I71" t="n">
+        <v>2.846</v>
+      </c>
+      <c r="J71" t="n">
+        <v>1549</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0.093</v>
+      </c>
+      <c r="L71" t="n">
+        <v>1333</v>
+      </c>
+      <c r="M71" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="N71" t="s">
         <v>457</v>
       </c>
-      <c r="G71" t="n">
-        <v>91</v>
-      </c>
-      <c r="H71" t="n">
-        <v>44759</v>
-      </c>
-      <c r="I71" t="n">
-        <v>2.673</v>
-      </c>
-      <c r="J71" t="n">
-        <v>1820</v>
-      </c>
-      <c r="K71" t="n">
-        <v>0.109</v>
-      </c>
-      <c r="L71" t="n">
-        <v>1136</v>
-      </c>
-      <c r="M71" t="n">
-        <v>0.068</v>
-      </c>
-      <c r="N71" t="s">
+      <c r="O71" t="s">
         <v>458</v>
       </c>
-      <c r="O71" t="s">
+      <c r="P71" t="s">
         <v>459</v>
       </c>
-      <c r="P71" t="s">
+      <c r="Q71" t="s">
         <v>460</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
+        <v>461</v>
+      </c>
+      <c r="B72" t="s">
         <v>462</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" s="1" t="n">
+        <v>43984</v>
+      </c>
+      <c r="D72" t="s">
         <v>463</v>
-      </c>
-      <c r="C72" s="1" t="n">
-        <v>43982</v>
-      </c>
-      <c r="D72" t="s">
-        <v>464</v>
       </c>
       <c r="E72" t="s">
         <v>41</v>
       </c>
       <c r="F72" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G72" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H72" t="n">
-        <v>245445</v>
+        <v>252132</v>
       </c>
       <c r="I72" t="n">
-        <v>36.07</v>
+        <v>37.053</v>
       </c>
       <c r="J72" t="n">
-        <v>2663</v>
+        <v>4372</v>
       </c>
       <c r="K72" t="n">
-        <v>0.391</v>
+        <v>0.643</v>
       </c>
       <c r="L72" t="n">
-        <v>3941</v>
+        <v>4052</v>
       </c>
       <c r="M72" t="n">
-        <v>0.579</v>
+        <v>0.595</v>
       </c>
       <c r="N72" t="s">
         <v>41</v>
       </c>
       <c r="O72" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="P72" t="s">
         <v>92</v>
       </c>
       <c r="Q72" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
+        <v>467</v>
+      </c>
+      <c r="B73" t="s">
         <v>468</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" s="1" t="n">
+        <v>43983</v>
+      </c>
+      <c r="D73" t="s">
         <v>469</v>
-      </c>
-      <c r="C73" s="1" t="n">
-        <v>43976</v>
-      </c>
-      <c r="D73" t="s">
-        <v>470</v>
       </c>
       <c r="E73" t="s">
         <v>41</v>
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H73" t="n">
-        <v>218996</v>
+        <v>264393</v>
       </c>
       <c r="I73" t="n">
-        <v>37.433</v>
+        <v>45.193</v>
       </c>
       <c r="J73"/>
       <c r="K73"/>
       <c r="L73" t="n">
-        <v>3962</v>
+        <v>6485</v>
       </c>
       <c r="M73" t="n">
-        <v>0.677</v>
+        <v>1.108</v>
       </c>
       <c r="N73" t="s">
         <v>41</v>
       </c>
       <c r="O73" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="P73" t="s">
         <v>92</v>
       </c>
       <c r="Q73" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B74" t="s">
+        <v>472</v>
+      </c>
+      <c r="C74" s="1" t="n">
+        <v>43983</v>
+      </c>
+      <c r="D74" t="s">
         <v>473</v>
-      </c>
-      <c r="C74" s="1" t="n">
-        <v>43976</v>
-      </c>
-      <c r="D74" t="s">
-        <v>474</v>
       </c>
       <c r="E74" t="s">
         <v>41</v>
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H74" t="n">
-        <v>334691</v>
+        <v>408495</v>
       </c>
       <c r="I74" t="n">
-        <v>57.209</v>
+        <v>69.824</v>
       </c>
       <c r="J74"/>
       <c r="K74"/>
       <c r="L74" t="n">
-        <v>5754</v>
+        <v>10543</v>
       </c>
       <c r="M74" t="n">
-        <v>0.984</v>
+        <v>1.802</v>
       </c>
       <c r="N74" t="s">
         <v>41</v>
       </c>
       <c r="O74" t="s">
+        <v>470</v>
+      </c>
+      <c r="P74" t="s">
+        <v>474</v>
+      </c>
+      <c r="Q74" t="s">
         <v>471</v>
-      </c>
-      <c r="P74" t="s">
-        <v>475</v>
-      </c>
-      <c r="Q74" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
+        <v>475</v>
+      </c>
+      <c r="B75" t="s">
         <v>476</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" s="1" t="n">
+        <v>43984</v>
+      </c>
+      <c r="D75" t="s">
         <v>477</v>
       </c>
-      <c r="C75" s="1" t="n">
-        <v>43982</v>
-      </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>478</v>
-      </c>
-      <c r="E75" t="s">
-        <v>479</v>
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H75" t="n">
-        <v>172601</v>
+        <v>179293</v>
       </c>
       <c r="I75" t="n">
-        <v>31.614</v>
+        <v>32.84</v>
       </c>
       <c r="J75" t="n">
-        <v>1606</v>
+        <v>6418</v>
       </c>
       <c r="K75" t="n">
-        <v>0.294</v>
+        <v>1.176</v>
       </c>
       <c r="L75" t="n">
-        <v>2027</v>
+        <v>2681</v>
       </c>
       <c r="M75" t="n">
-        <v>0.371</v>
+        <v>0.491</v>
       </c>
       <c r="N75" t="s">
+        <v>479</v>
+      </c>
+      <c r="O75" t="s">
         <v>480</v>
       </c>
-      <c r="O75" t="s">
+      <c r="P75" t="s">
         <v>481</v>
       </c>
-      <c r="P75" t="s">
+      <c r="Q75" t="s">
         <v>482</v>
-      </c>
-      <c r="Q75" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
+        <v>483</v>
+      </c>
+      <c r="B76" t="s">
         <v>484</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" s="1" t="n">
+        <v>43984</v>
+      </c>
+      <c r="D76" t="s">
         <v>485</v>
       </c>
-      <c r="C76" s="1" t="n">
-        <v>43982</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>486</v>
-      </c>
-      <c r="E76" t="s">
-        <v>487</v>
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H76" t="n">
-        <v>79039</v>
+        <v>80505</v>
       </c>
       <c r="I76" t="n">
-        <v>38.019</v>
+        <v>38.724</v>
       </c>
       <c r="J76" t="n">
-        <v>246</v>
+        <v>807</v>
       </c>
       <c r="K76" t="n">
-        <v>0.118</v>
+        <v>0.388</v>
       </c>
       <c r="L76" t="n">
-        <v>575</v>
+        <v>561</v>
       </c>
       <c r="M76" t="n">
-        <v>0.277</v>
+        <v>0.27</v>
       </c>
       <c r="N76" t="s">
+        <v>487</v>
+      </c>
+      <c r="O76" t="s">
         <v>488</v>
-      </c>
-      <c r="O76" t="s">
-        <v>489</v>
       </c>
       <c r="P76" t="s">
         <v>22</v>
       </c>
       <c r="Q76" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
+        <v>490</v>
+      </c>
+      <c r="B77" t="s">
         <v>491</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" s="1" t="n">
+        <v>43985</v>
+      </c>
+      <c r="D77" t="s">
         <v>492</v>
       </c>
-      <c r="C77" s="1" t="n">
-        <v>43982</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>493</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
         <v>494</v>
       </c>
-      <c r="F77" t="s">
+      <c r="G77" t="n">
+        <v>95</v>
+      </c>
+      <c r="H77" t="n">
+        <v>785979</v>
+      </c>
+      <c r="I77" t="n">
+        <v>13.252</v>
+      </c>
+      <c r="J77" t="n">
+        <v>24445</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0.412</v>
+      </c>
+      <c r="L77" t="n">
+        <v>21569</v>
+      </c>
+      <c r="M77" t="n">
+        <v>0.364</v>
+      </c>
+      <c r="N77" t="s">
+        <v>493</v>
+      </c>
+      <c r="O77" t="s">
         <v>495</v>
-      </c>
-      <c r="G77" t="n">
-        <v>92</v>
-      </c>
-      <c r="H77" t="n">
-        <v>725125</v>
-      </c>
-      <c r="I77" t="n">
-        <v>12.226</v>
-      </c>
-      <c r="J77" t="n">
-        <v>23242</v>
-      </c>
-      <c r="K77" t="n">
-        <v>0.392</v>
-      </c>
-      <c r="L77" t="n">
-        <v>20181</v>
-      </c>
-      <c r="M77" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="N77" t="s">
-        <v>494</v>
-      </c>
-      <c r="O77" t="s">
-        <v>496</v>
       </c>
       <c r="P77" t="s">
         <v>92</v>
       </c>
       <c r="Q77" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
+        <v>497</v>
+      </c>
+      <c r="B78" t="s">
         <v>498</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" s="1" t="n">
+        <v>43985</v>
+      </c>
+      <c r="D78" t="s">
         <v>499</v>
       </c>
-      <c r="C78" s="1" t="n">
-        <v>43983</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>500</v>
-      </c>
-      <c r="E78" t="s">
-        <v>501</v>
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H78" t="n">
-        <v>921391</v>
+        <v>956852</v>
       </c>
       <c r="I78" t="n">
-        <v>17.972</v>
+        <v>18.663</v>
       </c>
       <c r="J78" t="n">
-        <v>10569</v>
+        <v>17001</v>
       </c>
       <c r="K78" t="n">
-        <v>0.206</v>
+        <v>0.332</v>
       </c>
       <c r="L78" t="n">
-        <v>13565</v>
+        <v>14854</v>
       </c>
       <c r="M78" t="n">
-        <v>0.265</v>
+        <v>0.29</v>
       </c>
       <c r="N78" t="s">
+        <v>500</v>
+      </c>
+      <c r="O78" t="s">
         <v>501</v>
-      </c>
-      <c r="O78" t="s">
-        <v>502</v>
       </c>
       <c r="P78" t="s">
         <v>244</v>
       </c>
       <c r="Q78" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
+        <v>503</v>
+      </c>
+      <c r="B79" t="s">
         <v>504</v>
-      </c>
-      <c r="B79" t="s">
-        <v>505</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>43979</v>
       </c>
       <c r="D79" t="s">
+        <v>505</v>
+      </c>
+      <c r="E79" t="s">
         <v>506</v>
-      </c>
-      <c r="E79" t="s">
-        <v>507</v>
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
@@ -6426,254 +6426,256 @@
         <v>0.962</v>
       </c>
       <c r="N79" t="s">
+        <v>507</v>
+      </c>
+      <c r="O79" t="s">
         <v>508</v>
-      </c>
-      <c r="O79" t="s">
-        <v>509</v>
       </c>
       <c r="P79" t="s">
         <v>22</v>
       </c>
       <c r="Q79" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
+        <v>510</v>
+      </c>
+      <c r="B80" t="s">
         <v>511</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" s="1" t="n">
+        <v>43982</v>
+      </c>
+      <c r="D80" t="s">
         <v>512</v>
       </c>
-      <c r="C80" s="1" t="n">
-        <v>43975</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>513</v>
-      </c>
-      <c r="E80" t="s">
-        <v>514</v>
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H80" t="n">
-        <v>239000</v>
+        <v>275500</v>
       </c>
       <c r="I80" t="n">
-        <v>23.665</v>
+        <v>27.279</v>
       </c>
       <c r="J80"/>
       <c r="K80"/>
       <c r="L80" t="n">
-        <v>4143</v>
+        <v>5214</v>
       </c>
       <c r="M80" t="n">
-        <v>0.41</v>
+        <v>0.516</v>
       </c>
       <c r="N80" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="O80" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="P80" t="s">
         <v>92</v>
       </c>
       <c r="Q80" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
+        <v>515</v>
+      </c>
+      <c r="B81" t="s">
         <v>516</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" s="1" t="n">
+        <v>43984</v>
+      </c>
+      <c r="D81" t="s">
         <v>517</v>
       </c>
-      <c r="C81" s="1" t="n">
-        <v>43982</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>518</v>
-      </c>
-      <c r="E81" t="s">
-        <v>519</v>
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H81" t="n">
-        <v>399211</v>
+        <v>404065</v>
       </c>
       <c r="I81" t="n">
-        <v>46.127</v>
+        <v>46.688</v>
       </c>
       <c r="J81" t="n">
-        <v>1254</v>
+        <v>2816</v>
       </c>
       <c r="K81" t="n">
-        <v>0.145</v>
+        <v>0.325</v>
       </c>
       <c r="L81" t="n">
-        <v>3754</v>
+        <v>3065</v>
       </c>
       <c r="M81" t="n">
-        <v>0.434</v>
+        <v>0.354</v>
       </c>
       <c r="N81" t="s">
+        <v>518</v>
+      </c>
+      <c r="O81" t="s">
+        <v>517</v>
+      </c>
+      <c r="P81" t="s">
         <v>519</v>
       </c>
-      <c r="O81" t="s">
-        <v>518</v>
-      </c>
-      <c r="P81" t="s">
+      <c r="Q81" t="s">
         <v>520</v>
-      </c>
-      <c r="Q81" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
+        <v>521</v>
+      </c>
+      <c r="B82" t="s">
         <v>522</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" s="1" t="n">
+        <v>43984</v>
+      </c>
+      <c r="D82" t="s">
         <v>523</v>
       </c>
-      <c r="C82" s="1" t="n">
-        <v>43982</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>524</v>
-      </c>
-      <c r="E82" t="s">
-        <v>525</v>
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H82" t="n">
-        <v>72319</v>
+        <v>72683</v>
       </c>
       <c r="I82" t="n">
-        <v>3.036</v>
+        <v>3.052</v>
       </c>
       <c r="J82" t="n">
-        <v>237</v>
+        <v>176</v>
       </c>
       <c r="K82" t="n">
-        <v>0.01</v>
+        <v>0.007</v>
       </c>
       <c r="L82" t="n">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="M82" t="n">
-        <v>0.009</v>
+        <v>0.008</v>
       </c>
       <c r="N82" t="s">
+        <v>524</v>
+      </c>
+      <c r="O82" t="s">
         <v>525</v>
       </c>
-      <c r="O82" t="s">
+      <c r="P82" t="s">
         <v>526</v>
       </c>
-      <c r="P82" t="s">
+      <c r="Q82" t="s">
         <v>527</v>
-      </c>
-      <c r="Q82" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
+        <v>528</v>
+      </c>
+      <c r="B83" t="s">
         <v>529</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" s="1" t="n">
+        <v>43985</v>
+      </c>
+      <c r="D83" t="s">
         <v>530</v>
       </c>
-      <c r="C83" s="1" t="n">
-        <v>43983</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>531</v>
-      </c>
-      <c r="E83" t="s">
-        <v>532</v>
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H83" t="n">
-        <v>200411</v>
+        <v>212098</v>
       </c>
       <c r="I83" t="n">
-        <v>2.871</v>
+        <v>3.039</v>
       </c>
       <c r="J83" t="n">
-        <v>5500</v>
+        <v>4405</v>
       </c>
       <c r="K83" t="n">
-        <v>0.079</v>
+        <v>0.063</v>
       </c>
       <c r="L83" t="n">
-        <v>5727</v>
+        <v>5150</v>
       </c>
       <c r="M83" t="n">
-        <v>0.082</v>
+        <v>0.074</v>
       </c>
       <c r="N83" t="s">
+        <v>532</v>
+      </c>
+      <c r="O83" t="s">
         <v>533</v>
-      </c>
-      <c r="O83" t="s">
-        <v>534</v>
       </c>
       <c r="P83" t="s">
         <v>92</v>
       </c>
       <c r="Q83" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B84" t="s">
+        <v>535</v>
+      </c>
+      <c r="C84" s="1" t="n">
+        <v>43983</v>
+      </c>
+      <c r="D84" t="s">
         <v>536</v>
       </c>
-      <c r="C84" s="1" t="n">
-        <v>43973</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>537</v>
       </c>
-      <c r="E84" t="s">
+      <c r="F84" t="s">
         <v>538</v>
       </c>
-      <c r="F84"/>
       <c r="G84" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H84" t="n">
-        <v>375453</v>
+        <v>420000</v>
       </c>
       <c r="I84" t="n">
-        <v>5.379</v>
+        <v>6.017</v>
       </c>
       <c r="J84"/>
       <c r="K84"/>
       <c r="L84" t="n">
-        <v>6769</v>
+        <v>4455</v>
       </c>
       <c r="M84" t="n">
-        <v>0.097</v>
+        <v>0.064</v>
       </c>
       <c r="N84" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="O84" t="s">
         <v>539</v>
@@ -6693,7 +6695,7 @@
         <v>542</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>43981</v>
+        <v>43983</v>
       </c>
       <c r="D85" t="s">
         <v>543</v>
@@ -6703,25 +6705,21 @@
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H85" t="n">
-        <v>52503</v>
+        <v>53161</v>
       </c>
       <c r="I85" t="n">
-        <v>4.442</v>
-      </c>
-      <c r="J85" t="n">
-        <v>622</v>
-      </c>
-      <c r="K85" t="n">
-        <v>0.053</v>
-      </c>
+        <v>4.498</v>
+      </c>
+      <c r="J85"/>
+      <c r="K85"/>
       <c r="L85" t="n">
-        <v>670</v>
+        <v>578</v>
       </c>
       <c r="M85" t="n">
-        <v>0.057</v>
+        <v>0.049</v>
       </c>
       <c r="N85" t="s">
         <v>544</v>
@@ -6744,7 +6742,7 @@
         <v>549</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D86" t="s">
         <v>550</v>
@@ -6754,25 +6752,25 @@
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H86" t="n">
-        <v>2070719</v>
+        <v>2155349</v>
       </c>
       <c r="I86" t="n">
-        <v>24.552</v>
+        <v>25.556</v>
       </c>
       <c r="J86" t="n">
-        <v>31525</v>
+        <v>52305</v>
       </c>
       <c r="K86" t="n">
-        <v>0.374</v>
+        <v>0.62</v>
       </c>
       <c r="L86" t="n">
-        <v>30995</v>
+        <v>37243</v>
       </c>
       <c r="M86" t="n">
-        <v>0.368</v>
+        <v>0.442</v>
       </c>
       <c r="N86" t="s">
         <v>551</v>
@@ -6795,38 +6793,40 @@
         <v>556</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>43982</v>
+        <v>43983</v>
       </c>
       <c r="D87" t="s">
         <v>557</v>
       </c>
-      <c r="E87"/>
+      <c r="E87" t="s">
+        <v>558</v>
+      </c>
       <c r="F87" t="s">
+        <v>559</v>
+      </c>
+      <c r="G87" t="n">
+        <v>55</v>
+      </c>
+      <c r="H87" t="n">
+        <v>99427</v>
+      </c>
+      <c r="I87" t="n">
+        <v>2.174</v>
+      </c>
+      <c r="J87" t="n">
+        <v>2222</v>
+      </c>
+      <c r="K87" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="L87" t="n">
+        <v>1808</v>
+      </c>
+      <c r="M87" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N87" t="s">
         <v>558</v>
-      </c>
-      <c r="G87" t="n">
-        <v>54</v>
-      </c>
-      <c r="H87" t="n">
-        <v>97205</v>
-      </c>
-      <c r="I87" t="n">
-        <v>2.125</v>
-      </c>
-      <c r="J87" t="n">
-        <v>1319</v>
-      </c>
-      <c r="K87" t="n">
-        <v>0.029</v>
-      </c>
-      <c r="L87" t="n">
-        <v>1660</v>
-      </c>
-      <c r="M87" t="n">
-        <v>0.036</v>
-      </c>
-      <c r="N87" t="s">
-        <v>559</v>
       </c>
       <c r="O87" t="s">
         <v>560</v>
@@ -6846,7 +6846,7 @@
         <v>563</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D88" t="s">
         <v>564</v>
@@ -6856,21 +6856,25 @@
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H88" t="n">
-        <v>356187</v>
+        <v>381552</v>
       </c>
       <c r="I88" t="n">
-        <v>8.144</v>
-      </c>
-      <c r="J88"/>
-      <c r="K88"/>
+        <v>8.724</v>
+      </c>
+      <c r="J88" t="n">
+        <v>9884</v>
+      </c>
+      <c r="K88" t="n">
+        <v>0.226</v>
+      </c>
       <c r="L88" t="n">
-        <v>9188</v>
+        <v>9860</v>
       </c>
       <c r="M88" t="n">
-        <v>0.21</v>
+        <v>0.225</v>
       </c>
       <c r="N88" t="s">
         <v>565</v>
@@ -6944,7 +6948,7 @@
         <v>575</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>43982</v>
+        <v>43984</v>
       </c>
       <c r="D90" t="s">
         <v>576</v>
@@ -6952,27 +6956,29 @@
       <c r="E90" t="s">
         <v>572</v>
       </c>
-      <c r="F90"/>
+      <c r="F90" t="s">
+        <v>577</v>
+      </c>
       <c r="G90" t="n">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="H90" t="n">
-        <v>4285738</v>
+        <v>3012735</v>
       </c>
       <c r="I90" t="n">
-        <v>63.131</v>
+        <v>44.379</v>
       </c>
       <c r="J90" t="n">
-        <v>115725</v>
+        <v>72689</v>
       </c>
       <c r="K90" t="n">
-        <v>1.705</v>
+        <v>1.071</v>
       </c>
       <c r="L90" t="n">
-        <v>118119</v>
+        <v>65126</v>
       </c>
       <c r="M90" t="n">
-        <v>1.74</v>
+        <v>0.959</v>
       </c>
       <c r="N90" t="s">
         <v>572</v>
@@ -6981,7 +6987,7 @@
         <v>573</v>
       </c>
       <c r="P90" t="s">
-        <v>577</v>
+        <v>22</v>
       </c>
       <c r="Q90" t="s">
         <v>578</v>
@@ -6995,7 +7001,7 @@
         <v>580</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>43982</v>
+        <v>43984</v>
       </c>
       <c r="D91" t="s">
         <v>581</v>
@@ -7005,25 +7011,25 @@
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="H91" t="n">
-        <v>16936891</v>
+        <v>18908412</v>
       </c>
       <c r="I91" t="n">
-        <v>51.168</v>
+        <v>57.125</v>
       </c>
       <c r="J91" t="n">
-        <v>406206</v>
+        <v>1296287</v>
       </c>
       <c r="K91" t="n">
-        <v>1.227</v>
+        <v>3.916</v>
       </c>
       <c r="L91" t="n">
-        <v>396171</v>
+        <v>532075</v>
       </c>
       <c r="M91" t="n">
-        <v>1.197</v>
+        <v>1.607</v>
       </c>
       <c r="N91" t="s">
         <v>582</v>
@@ -7046,7 +7052,7 @@
         <v>586</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>43980</v>
+        <v>43984</v>
       </c>
       <c r="D92" t="s">
         <v>587</v>
@@ -7056,21 +7062,25 @@
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="H92" t="n">
-        <v>16794182</v>
+        <v>17757838</v>
       </c>
       <c r="I92" t="n">
-        <v>50.737</v>
-      </c>
-      <c r="J92"/>
-      <c r="K92"/>
+        <v>53.649</v>
+      </c>
+      <c r="J92" t="n">
+        <v>417156</v>
+      </c>
+      <c r="K92" t="n">
+        <v>1.26</v>
+      </c>
       <c r="L92" t="n">
-        <v>452400</v>
+        <v>407257</v>
       </c>
       <c r="M92" t="n">
-        <v>1.367</v>
+        <v>1.23</v>
       </c>
       <c r="N92" t="s">
         <v>588</v>
@@ -7093,7 +7103,7 @@
         <v>593</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>43982</v>
+        <v>43985</v>
       </c>
       <c r="D93" t="s">
         <v>594</v>
@@ -7103,25 +7113,25 @@
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H93" t="n">
-        <v>43479</v>
+        <v>45226</v>
       </c>
       <c r="I93" t="n">
-        <v>12.517</v>
+        <v>13.019</v>
       </c>
       <c r="J93" t="n">
-        <v>855</v>
+        <v>715</v>
       </c>
       <c r="K93" t="n">
-        <v>0.246</v>
+        <v>0.206</v>
       </c>
       <c r="L93" t="n">
-        <v>831</v>
+        <v>822</v>
       </c>
       <c r="M93" t="n">
-        <v>0.239</v>
+        <v>0.237</v>
       </c>
       <c r="N93" t="s">
         <v>124</v>
@@ -7191,7 +7201,7 @@
         <v>605</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>43981</v>
+        <v>43984</v>
       </c>
       <c r="D95" t="s">
         <v>606</v>
@@ -7201,25 +7211,25 @@
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H95" t="n">
-        <v>17526</v>
+        <v>19290</v>
       </c>
       <c r="I95" t="n">
-        <v>1.179</v>
+        <v>1.298</v>
       </c>
       <c r="J95" t="n">
-        <v>666</v>
+        <v>581</v>
       </c>
       <c r="K95" t="n">
-        <v>0.045</v>
+        <v>0.039</v>
       </c>
       <c r="L95" t="n">
-        <v>313</v>
+        <v>469</v>
       </c>
       <c r="M95" t="n">
-        <v>0.021</v>
+        <v>0.032</v>
       </c>
       <c r="N95" t="s">
         <v>607</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-06-05
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Argentina - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/03-06-20_reporte-matutino-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/05-06-20_reporte-matutino-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Argentina</t>
@@ -92,7 +92,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/06/coronavirus-covid-19-at-a-glance-2-june-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/06/coronavirus-covid-19-at-a-glance-4-june-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200603200522/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200605152528/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200603200526/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200605152532/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -233,7 +233,7 @@
     <t xml:space="preserve">Bolivia - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4243-ministerio-de-salud-reporta-460-nuevos-contagios-de-coronavirus-y-33-fallecidos</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4252-sube-a-12-245-el-numero-de-total-de-contagios-de-coronavirus-en-bolivia-los-casos-descartados-suman-21-701</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -280,7 +280,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200603200557/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200605152539/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -292,7 +292,7 @@
     <t xml:space="preserve">https://coronavirus.bg/</t>
   </si>
   <si>
-    <t xml:space="preserve">Bulgaria's official COVID-19 information portal provides irregular updates of the cumulative number of 'tests done'.
+    <t xml:space="preserve">Bulgaria's official COVID-19 information portal provides irregular updates of the cumulative number of 'PCR tests done'.
 Using web archives we reconstruct the testing time series starting from 11th April.  We cannot say with certainty when testing began, only that the earliest observation available to us begins from the 11th April. For 19th April, we take the figure provided in Bulgaria's [COVID-19 dashboard](https://coronavirus.bg/arcgis/apps/opsdashboard/index.html#/ecacd239ee7e4fba956f7948f586af93) as no snapshot was available using web archives. The test figures provided in the dashboard match the figures provided by the information portal for all other dates available.
 Google Translate was used while compiling this data so this may affect our interpretation of the data.</t>
   </si>
@@ -303,7 +303,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200603200615/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200604194851/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -391,7 +391,7 @@
     <t xml:space="preserve">Croatia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200603201313/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200605152550/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -454,7 +454,7 @@
     <t xml:space="preserve">Denmark - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200603172636/https://www.ssi.dk/sygdomme-beredskab-og-forskning/sygdomsovervaagning/c/covid19-overvaagning</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200605121244/https://www.ssi.dk/sygdomme-beredskab-og-forskning/sygdomsovervaagning/c/covid19-overvaagning</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -480,7 +480,7 @@
     <t xml:space="preserve">Ecuador - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-02062020-08h00.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-03062020-08h00.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -505,7 +505,7 @@
     <t xml:space="preserve">El Salvador - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/2942358345850337</t>
+    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/2947402875345884</t>
   </si>
   <si>
     <t xml:space="preserve">Government of El Salvador</t>
@@ -549,7 +549,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_June-3-Eng_V2.pdf</t>
+    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_June-5-Eng_V1.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -593,13 +593,13 @@
     <t xml:space="preserve">France - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.santepubliquefrance.fr/content/download/256362/2623091</t>
+    <t xml:space="preserve">https://www.santepubliquefrance.fr/content/download/257630/2628879</t>
   </si>
   <si>
     <t xml:space="preserve">National Public Health Agency</t>
   </si>
   <si>
-    <t xml:space="preserve">Dividing 216,891 (weekly total) by 7</t>
+    <t xml:space="preserve">Dividing 236,098 (weekly total) by 7</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.santepubliquefrance.fr/recherche/#search=COVID-19%20:%20point%20epidemiologique&amp;sort=dat</t>
@@ -628,7 +628,7 @@
     <t xml:space="preserve">Germany - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rki.de/DE/Content/InfAZ/N/Neuartiges_Coronavirus/Situationsberichte/2020-05-27-de.pdf?__blob=publicationFile</t>
+    <t xml:space="preserve">https://www.rki.de/DE/Content/InfAZ/N/Neuartiges_Coronavirus/Situationsberichte/2020-06-03-en.pdf?__blob=publicationFile</t>
   </si>
   <si>
     <t xml:space="preserve">Robert Koch Institut</t>
@@ -644,10 +644,11 @@
   </si>
   <si>
     <t xml:space="preserve">To determine how many laboratory tests regarding SARS-CoV-2 are carried out per calendar week in Germany and how many tests are positive or negative, the RKI has started a Germany-wide laboratory query. However, the number of laboratories reporting data seems to vary from week to week.
-The report published on 27 May states that “from the beginning of the collection up to and including calendar week 21/2020”:
-– The cumulative total of samples tested was 3,952,971;
-- For calendar week 21( which ends 24 May), 172 labs reported 344,782 samples tested;
-- For calendar week 20 (which ends 17 May), 181 labs reported 430,882 samples tested;
+The report published on 27 May states that “from the beginning of the collection up to and including calendar week 22/2020”:
+– The cumulative total of samples tested was 4,348,880;
+- For calendar week 22 (which ends 31May), 169 labs reported 392,437 samples tested;
+- For calendar week 21( which ends 24 May), 174 labs reported 346,470 samples tested;
+- For calendar week 20 (which ends 17 May), 182 labs reported 432,666 samples tested;
 - For calendar week 19 (which ends 10 May), 182 labs reported 403,875 samples tested;
 - For calendar week 18 (which ends on 3 May), 175 labs reported 326,788 samples tested;
 - For calendar week 17 (which ends on 26 April), 178 labs reported 363,890 samples tested;
@@ -703,7 +704,7 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200602/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-report-20200604/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -841,7 +842,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200603033550/http://irangov.ir/detail/340265</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200604180455/http://irangov.ir/detail/340321</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -881,7 +882,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/20129/covid19-data-israel-27052020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/20164/covid19-data-israel-28052020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -938,7 +939,7 @@
     <t xml:space="preserve">Japan - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11664.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11719.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -962,7 +963,7 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000636597.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000637302.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">The cumulative total reported in the press release matches the cumulative total calculated from the weekly and daily figures reported by the MOH.</t>
@@ -997,7 +998,7 @@
     <t xml:space="preserve">Kenya - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1267805415775121409</t>
+    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1268563481235787776</t>
   </si>
   <si>
     <t xml:space="preserve">Kenya Ministry of Health</t>
@@ -1038,7 +1039,7 @@
     <t xml:space="preserve">Lithuania - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200603201910/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200605152658/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -1054,7 +1055,7 @@
     <t xml:space="preserve">Luxembourg - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200603201912/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200604195825/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg Government situation update</t>
@@ -1075,20 +1076,21 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/062020/situasi-terkini-01-jun-2020</t>
+    <t xml:space="preserve">https://www.facebook.com/kementeriankesihatanmalaysia/videos/698657040921568</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
   </si>
   <si>
-    <t xml:space="preserve">Jumlah individu disampel' via google translate is interpreted to be the number of individuals sampled. See the 'Taburan Kes' tab at the very bottom of the update.</t>
+    <t xml:space="preserve">Statistics on testing can be see at 20:04 timestamp on the MOH livestream</t>
   </si>
   <si>
     <t xml:space="preserve">http://covid-19.moh.gov.my/terkini</t>
   </si>
   <si>
-    <t xml:space="preserve">The Malaysian Ministry of Health provides daily [situation updates](http://covid-19.moh.gov.my/terkini), including the cumulative number of individuals sampled, available from 19th May. This figure can be found in the infographic titled 'Jumlah Keseluruhan Taburan Kes COVID-19 di Malaysia' labelled as 'Jumlah Individu Disampel'. Since 19th April 2020, we are not aware of the source reporting positive, negative, and pending test figures separately, as was the case before. 
-The situation updates for 27/28 May does not include the infographic detailing the total number of people tested.
+    <t xml:space="preserve">The Malaysian Ministry of Health provides daily [situation updates](http://covid-19.moh.gov.my/terkini), including the cumulative number of individuals sampled, available from 19th May. This figure can be found in the infographic titled 'Jumlah Keseluruhan Taburan Kes COVID-19 di Malaysia' labelled as 'Jumlah Individu Disampel'. Since 19th April 2020, we are not aware of this source reporting positive, negative, and pending test figures separately, as was the case before. 
+The situation updates for 27/28 May and 2 June onwards do not include the infographic detailing the total number of people tested. In these instances, we rely on the MOH daily press conference livestreams uploaded to the official facebook page. The sum of positive and negative tests reported in the livestream match the total people tested figures reported in the situation updates. 
+For 14/15 May, we use the Director General of Health, [daily press statement figures](https://kpkesihatan.com/2020/05/15/kenyataan-akhbar-kpk-15-mei-2020-situasi-semasa-jangkitan-penyakit-coronavirus-2019-covid-19-di-malaysia/). It details the jump in people tested from 14th to 15th May was due to data consolidation efforts and an improved data collection system.
 Prior to 19th May, we relied on MOH web archives to reconstruct the time series. The MOH provided daily updates to the total number of cases tested. It is not clear the exact date these cumulative figures date back to. The earliest release we have been able to find begins from the 14th February. This MOH web archive provides a breakdown of the number of positive, negative, and still pending tests. We report total tests as the sum of positive and negative tests, excluding pending tests. The title of the table indicates that these figures relate to cases. As far as we are aware, cases are equivalent to individuals tested.
 In a previous version of this page, we reported total tests as the sum of positive, negative, and pending tests. However, since April 7th 2020, the source has not reported the number of pending tests each day. For this reason, we have updated the time series so that total tests is equal to the sum of positive and negative tests (excluding pending tests) for all days on which we report data.
 There is no explicit mention of whether the figures include only PCR tests or other kinds of test.</t>
@@ -1100,13 +1102,13 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/561317043971945/videos/673971883160559/</t>
+    <t xml:space="preserve">https://www.facebook.com/561317043971945/videos/2676083566001901/</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Ministry of Health</t>
   </si>
   <si>
-    <t xml:space="preserve">Numbers visible in video at time: 1:13</t>
+    <t xml:space="preserve">Numbers visible in video at time: 2:35</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Ministry of Health Official Facebook page</t>
@@ -1170,6 +1172,9 @@
     <t xml:space="preserve">Myanmar Ministry of Health and Sports</t>
   </si>
   <si>
+    <t xml:space="preserve">This figure is taken from the interactive dashboard and should be updated once the daily PDF situation report becomes available</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://mohs.gov.mm/Home</t>
   </si>
   <si>
@@ -1206,10 +1211,10 @@
     <t xml:space="preserve">Netherlands - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-06/COVID-19_WebSite_rapport_20200602_1024.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 2 June 2020 update</t>
+    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-06/COVID-19_WebSite_rapport_dagelijks20200604_1141.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 4 June 2020 update</t>
   </si>
   <si>
     <t xml:space="preserve">Dutch National Institute for Public Health and the Environment</t>
@@ -1245,7 +1250,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200603202046/https://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200605152829/https://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1265,7 +1270,7 @@
     <t xml:space="preserve">Norway - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.06.03-dagsrapport-norge-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020-06-05-dagsrapport-norge-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Norwegian Institute of Public Health</t>
@@ -1290,7 +1295,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200603202050/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200605152835/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1306,21 +1311,16 @@
     <t xml:space="preserve">PAN</t>
   </si>
   <si>
-    <t xml:space="preserve">Panama - units unclear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/c0t088/DAP-Panama</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Made available by c0t088 on Github</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://minsa.gob.pa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The [Panama Ministry of Health](http://www.minsa.gob.pa) in collaboration with the [Gorgas Memorial Institute for Health Studies](http://www.gorgas.gob.pa) reports the cumulative number of tests performed to date in [this dashboard](http://minsa.gob.pa/coronavirus-covid-19). The reported figures include the total number of positive, negative, and "positive control" test results to date.
-It is unclear whether the total number of tests performed ("pruebas realizadas") refers to the number of people tested or the number of samples tested. The number of reported positive test results is equal to the number of confirmed cases of COVID-19, which suggests that the number of tests performed is equivalent to the number of people tested. However, because the data source does not provide a clear definition, we record the units as "unclear".
-Unfortunately, the Ministry of Health's official dashboard does not provide a time series of the number of tests performed each day since testing began. Instead, the dashboard only displays a daily snapshot of the total number of tests performed to date. Since we did not begin to monitor this dashboard until April 14th 2020, we construct a time series dating back to March 9th 2020 using data provided in [this unofficial GitHub repository](https://github.com/c0t088/DAP-Panama/blob/master/data_covid_pma_dia.csv), which we have cross-referenced against data in the official Ministry of Health dashboard for a sample of dates.</t>
+    <t xml:space="preserve">Panama - tests performed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://minsa.gob.pa/covid-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panama Ministry of Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Panama Ministry of Health reports the cumulative number of tests performed ("pruebas realizadas") on [their official dashboard](http://minsa.gob.pa/covid-19) with a time series dating back to 9 March 2020. The page with testing numbers is not the first one shown but can be navigated to with the arrows at the bottom of the dashboard. The dashboard shows the cumulative number of total, positive, negative, and control tests ("prueba de control") performed. We report here the total of positive and negative numbers because: 1) the time series only includes positive and negative test numbers; and 2) the total they provide seems to include control tests, which we understand to be used for testing quality control.</t>
   </si>
   <si>
     <t xml:space="preserve">PRY</t>
@@ -1348,7 +1348,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/176156-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-178-914-en-el-peru-comunicado-n-120</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/177267-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-183-198-en-el-peru-comunicado-n-121</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1382,7 +1382,7 @@
 The total number of individuals tested is the sum of positive, negative, equivocal, and invalid individuals. No definitions of equivocal and invalid individual tests are given, hence our figures only report the sum of individuals who have tested positive or negative. From 22nd May, the DOH stopped reporting figures on equivocal and invalid individuals; the DOH provides the cumulative samples and unique indivdiuals tested, where cumulative unique individuals = cumulative positive + cumulative negative individuals. 
 The source provides a breakdown of both i) the number of individuals tested and ii) the total tests conducted, by laboratory. We are not aware of any aggregation issues. 
 The DOH used to report the number of cases tested in a previous dashboard, but stopped on 4th April. This previous breakdown of the test results and COVID-19 dashboard have both been removed. We became aware of this new tracker on the 13th April with data 'as of April 11 2020, 12am'. No previous snapshots of the dashboard are available using web archive, therefore the series starts from the 11th April - the earliest date from which we have access to the data.
-Latest data available until 1st June, as of 3rd June.</t>
+Latest data available until 3rd June, as of 5th June.</t>
   </si>
   <si>
     <t xml:space="preserve">POL</t>
@@ -1455,17 +1455,16 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://github.com/adrianp/covid19romania</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-5-iunie-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
   </si>
   <si>
-    <t xml:space="preserve">Made available by Adrian-Tudor Panescu on Github</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data is collected and made available [on GitHub](https://github.com/adrianp/covid19romania). It includes a cumulative total of tests performed. No information is given on the geographical scope and number of labs included.
-The main data source is the press office of the Ministry of Internal Affairs, which provides a daily report on most metrics. Data points are also sourced from the Romanian Ministry of Health and the Romanian National Institute of Public Health and occasionally from news outlets.</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The main data source is the press office of the Ministry of Internal Affairs, which provides a daily report on most metrics, including data on COVID-19 testing (e.g. "Până la această dată, la nivel național, au fost prelucrate 484.782 de teste.")</t>
   </si>
   <si>
     <t xml:space="preserve">RUS</t>
@@ -1474,7 +1473,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14605</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14623</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1494,7 +1493,7 @@
     <t xml:space="preserve">Rwanda - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1267945222819975170</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1268258423898062851</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1601,7 +1600,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200602201741/https://korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200605152917/https://korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Center of Health Information and the Office of the Government of the Slovak Republic</t>
@@ -1675,7 +1674,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367407&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367442&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1758,7 +1757,7 @@
     <t xml:space="preserve">Taiwan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/rWxxHolsA5DEEpJxm5zpoQ?typeid=9</t>
+    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/q_oVMUUh-Gn4ERMn-c5ZnA?typeid=9</t>
   </si>
   <si>
     <t xml:space="preserve">Taiwan Centers for Disease Control (CDC)</t>
@@ -1781,7 +1780,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200603202218/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200605153210/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1851,7 +1850,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200603202222/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200604200117/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1875,13 +1874,13 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1267734985693442048</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1268822086115635200</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
   </si>
   <si>
-    <t xml:space="preserve">We sum the cumulative total provided for the previous day with the daily number of samples tested today.</t>
+    <t xml:space="preserve">The MOH did not release daily test figures for 3rd June. The cumulative total for 4th June thus takes the total figure as of the 2nd June and the daily tests conducted on the 4th June.</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.health.go.ug/moh/resources/</t>
@@ -1899,7 +1898,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200603202225/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200605153218/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1930,13 +1929,13 @@
     <t xml:space="preserve">https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public#number-of-cases</t>
   </si>
   <si>
-    <t xml:space="preserve">The figures we provide relate to the daily updates provided for the cumulative total and daily number of people tested. It is not clear the exact date that the cumulative figures date back to. As of 2 June 2020, the sources notes that "reporting on the number of people tested has been temporarily paused to ensure consistent reporting across all pillars. This is due to a small percentage of cases where the same person has had more than one test or tested positive more than once for coronavirus in pillar 2. Corrections will be made to any figures if they have subsequently been found to have an error."</t>
+    <t xml:space="preserve">The figures we provide relate to the daily updates provided for the cumulative total and daily number of people tested. It is not clear the exact date that the cumulative figures date back to. As of 2 June 2020, the source notes that "reporting on the number of people tested has been temporarily paused to ensure consistent reporting across all pillars. This is due to a small percentage of cases where the same person has had more than one test or tested positive more than once for coronavirus in pillar 2. Corrections will be made to any figures if they have subsequently been found to have an error."</t>
   </si>
   <si>
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/889818/2020-06-03-COVID-19-UK-testing-time-series.csv</t>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/890451/2020-06-05_COVID-19_UK_testing_time_series.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Sum of pillar 1 + pillar 2 (tests processed only)</t>
@@ -1957,7 +1956,7 @@
     <t xml:space="preserve">United States - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200603202228/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200605153221/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
   </si>
   <si>
     <t xml:space="preserve">United States CDC</t>
@@ -2011,7 +2010,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-42</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-44</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2050,7 +2049,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1267885571126505472</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1268307496801898499</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -2460,7 +2459,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2470,21 +2469,25 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H2" t="n">
-        <v>172947</v>
+        <v>183862</v>
       </c>
       <c r="I2" t="n">
-        <v>3.827</v>
-      </c>
-      <c r="J2"/>
-      <c r="K2"/>
+        <v>4.068</v>
+      </c>
+      <c r="J2" t="n">
+        <v>5414</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.12</v>
+      </c>
       <c r="L2" t="n">
-        <v>4676</v>
+        <v>4768</v>
       </c>
       <c r="M2" t="n">
-        <v>0.103</v>
+        <v>0.105</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -2507,7 +2510,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2517,25 +2520,25 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H3" t="n">
-        <v>1490387</v>
+        <v>1546329</v>
       </c>
       <c r="I3" t="n">
-        <v>58.447</v>
+        <v>60.641</v>
       </c>
       <c r="J3" t="n">
-        <v>18167</v>
+        <v>33629</v>
       </c>
       <c r="K3" t="n">
-        <v>0.712</v>
+        <v>1.319</v>
       </c>
       <c r="L3" t="n">
-        <v>28881</v>
+        <v>25555</v>
       </c>
       <c r="M3" t="n">
-        <v>1.133</v>
+        <v>1.002</v>
       </c>
       <c r="N3" t="s">
         <v>27</v>
@@ -2558,7 +2561,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -2568,25 +2571,25 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H4" t="n">
-        <v>462958</v>
+        <v>479449</v>
       </c>
       <c r="I4" t="n">
-        <v>51.403</v>
+        <v>53.234</v>
       </c>
       <c r="J4" t="n">
-        <v>6580</v>
+        <v>7983</v>
       </c>
       <c r="K4" t="n">
-        <v>0.731</v>
+        <v>0.886</v>
       </c>
       <c r="L4" t="n">
-        <v>6322</v>
+        <v>6450</v>
       </c>
       <c r="M4" t="n">
-        <v>0.702</v>
+        <v>0.716</v>
       </c>
       <c r="N4" t="s">
         <v>34</v>
@@ -2609,7 +2612,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2619,25 +2622,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H5" t="n">
-        <v>337773</v>
+        <v>350907</v>
       </c>
       <c r="I5" t="n">
-        <v>198.505</v>
+        <v>206.224</v>
       </c>
       <c r="J5" t="n">
-        <v>7040</v>
+        <v>5570</v>
       </c>
       <c r="K5" t="n">
-        <v>4.137</v>
+        <v>3.273</v>
       </c>
       <c r="L5" t="n">
-        <v>6664</v>
+        <v>6675</v>
       </c>
       <c r="M5" t="n">
-        <v>3.916</v>
+        <v>3.923</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
@@ -2660,7 +2663,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D6" t="s">
         <v>48</v>
@@ -2670,25 +2673,25 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H6" t="n">
-        <v>333073</v>
+        <v>358277</v>
       </c>
       <c r="I6" t="n">
-        <v>2.022</v>
+        <v>2.175</v>
       </c>
       <c r="J6" t="n">
-        <v>12704</v>
+        <v>12694</v>
       </c>
       <c r="K6" t="n">
         <v>0.077</v>
       </c>
       <c r="L6" t="n">
-        <v>10662</v>
+        <v>11786</v>
       </c>
       <c r="M6" t="n">
-        <v>0.065</v>
+        <v>0.072</v>
       </c>
       <c r="N6" t="s">
         <v>49</v>
@@ -2762,7 +2765,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
@@ -2772,25 +2775,25 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H8" t="n">
-        <v>708996</v>
+        <v>724596</v>
       </c>
       <c r="I8" t="n">
-        <v>61.175</v>
+        <v>62.521</v>
       </c>
       <c r="J8" t="n">
-        <v>3122</v>
+        <v>8233</v>
       </c>
       <c r="K8" t="n">
-        <v>0.269</v>
+        <v>0.71</v>
       </c>
       <c r="L8" t="n">
-        <v>8675</v>
+        <v>7219</v>
       </c>
       <c r="M8" t="n">
-        <v>0.749</v>
+        <v>0.623</v>
       </c>
       <c r="N8" t="s">
         <v>62</v>
@@ -2813,7 +2816,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
@@ -2823,25 +2826,25 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H9" t="n">
-        <v>31186</v>
+        <v>33946</v>
       </c>
       <c r="I9" t="n">
-        <v>2.672</v>
+        <v>2.908</v>
       </c>
       <c r="J9" t="n">
-        <v>1146</v>
+        <v>1460</v>
       </c>
       <c r="K9" t="n">
-        <v>0.098</v>
+        <v>0.125</v>
       </c>
       <c r="L9" t="n">
-        <v>1078</v>
+        <v>1108</v>
       </c>
       <c r="M9" t="n">
-        <v>0.092</v>
+        <v>0.095</v>
       </c>
       <c r="N9" t="s">
         <v>41</v>
@@ -2913,7 +2916,7 @@
         <v>81</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D11" t="s">
         <v>82</v>
@@ -2923,25 +2926,25 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H11" t="n">
-        <v>84261</v>
+        <v>87890</v>
       </c>
       <c r="I11" t="n">
-        <v>12.127</v>
+        <v>12.649</v>
       </c>
       <c r="J11" t="n">
-        <v>1347</v>
+        <v>2060</v>
       </c>
       <c r="K11" t="n">
-        <v>0.194</v>
+        <v>0.296</v>
       </c>
       <c r="L11" t="n">
-        <v>1124</v>
+        <v>1214</v>
       </c>
       <c r="M11" t="n">
-        <v>0.162</v>
+        <v>0.175</v>
       </c>
       <c r="N11" t="s">
         <v>84</v>
@@ -2964,7 +2967,7 @@
         <v>88</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>43985</v>
+        <v>43986</v>
       </c>
       <c r="D12" t="s">
         <v>89</v>
@@ -2974,25 +2977,25 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H12" t="n">
-        <v>1751547</v>
+        <v>1787370</v>
       </c>
       <c r="I12" t="n">
-        <v>46.408</v>
+        <v>47.357</v>
       </c>
       <c r="J12" t="n">
-        <v>30112</v>
+        <v>35823</v>
       </c>
       <c r="K12" t="n">
-        <v>0.798</v>
+        <v>0.949</v>
       </c>
       <c r="L12" t="n">
-        <v>31901</v>
+        <v>32595</v>
       </c>
       <c r="M12" t="n">
-        <v>0.845</v>
+        <v>0.864</v>
       </c>
       <c r="N12" t="s">
         <v>90</v>
@@ -3015,7 +3018,7 @@
         <v>95</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>43985</v>
+        <v>43986</v>
       </c>
       <c r="D13" t="s">
         <v>96</v>
@@ -3027,25 +3030,25 @@
         <v>97</v>
       </c>
       <c r="G13" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H13" t="n">
-        <v>628318</v>
+        <v>646458</v>
       </c>
       <c r="I13" t="n">
-        <v>32.868</v>
+        <v>33.817</v>
       </c>
       <c r="J13" t="n">
-        <v>15546</v>
+        <v>18140</v>
       </c>
       <c r="K13" t="n">
-        <v>0.813</v>
+        <v>0.949</v>
       </c>
       <c r="L13" t="n">
-        <v>16256</v>
+        <v>16612</v>
       </c>
       <c r="M13" t="n">
-        <v>0.85</v>
+        <v>0.869</v>
       </c>
       <c r="N13" t="s">
         <v>98</v>
@@ -3068,7 +3071,7 @@
         <v>102</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D14" t="s">
         <v>103</v>
@@ -3078,22 +3081,22 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H14" t="n">
-        <v>350213</v>
+        <v>374592</v>
       </c>
       <c r="I14" t="n">
-        <v>6.883</v>
+        <v>7.362</v>
       </c>
       <c r="J14" t="n">
-        <v>9071</v>
+        <v>12160</v>
       </c>
       <c r="K14" t="n">
-        <v>0.178</v>
+        <v>0.239</v>
       </c>
       <c r="L14" t="n">
-        <v>11299</v>
+        <v>11283</v>
       </c>
       <c r="M14" t="n">
         <v>0.222</v>
@@ -3119,7 +3122,7 @@
         <v>109</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>43985</v>
+        <v>43986</v>
       </c>
       <c r="D15" t="s">
         <v>110</v>
@@ -3129,19 +3132,19 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H15" t="n">
-        <v>20122</v>
+        <v>20498</v>
       </c>
       <c r="I15" t="n">
-        <v>3.95</v>
+        <v>4.024</v>
       </c>
       <c r="J15" t="n">
-        <v>415</v>
+        <v>376</v>
       </c>
       <c r="K15" t="n">
-        <v>0.081</v>
+        <v>0.074</v>
       </c>
       <c r="L15" t="n">
         <v>406</v>
@@ -3170,7 +3173,7 @@
         <v>115</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D16" t="s">
         <v>116</v>
@@ -3180,25 +3183,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H16" t="n">
-        <v>67814</v>
+        <v>68267</v>
       </c>
       <c r="I16" t="n">
-        <v>16.519</v>
+        <v>16.629</v>
       </c>
       <c r="J16" t="n">
-        <v>517</v>
+        <v>270</v>
       </c>
       <c r="K16" t="n">
-        <v>0.126</v>
+        <v>0.066</v>
       </c>
       <c r="L16" t="n">
-        <v>507</v>
+        <v>394</v>
       </c>
       <c r="M16" t="n">
-        <v>0.123</v>
+        <v>0.096</v>
       </c>
       <c r="N16" t="s">
         <v>117</v>
@@ -3221,7 +3224,7 @@
         <v>122</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D17" t="s">
         <v>123</v>
@@ -3233,25 +3236,25 @@
         <v>125</v>
       </c>
       <c r="G17" t="n">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H17" t="n">
-        <v>110349</v>
+        <v>114464</v>
       </c>
       <c r="I17" t="n">
-        <v>9.742</v>
+        <v>10.106</v>
       </c>
       <c r="J17" t="n">
-        <v>1960</v>
+        <v>2015</v>
       </c>
       <c r="K17" t="n">
-        <v>0.173</v>
+        <v>0.178</v>
       </c>
       <c r="L17" t="n">
-        <v>1710</v>
+        <v>1908</v>
       </c>
       <c r="M17" t="n">
-        <v>0.151</v>
+        <v>0.168</v>
       </c>
       <c r="N17" t="s">
         <v>124</v>
@@ -3274,7 +3277,7 @@
         <v>130</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D18" t="s">
         <v>131</v>
@@ -3284,25 +3287,25 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H18" t="n">
-        <v>454397</v>
+        <v>464499</v>
       </c>
       <c r="I18" t="n">
-        <v>42.431</v>
+        <v>43.375</v>
       </c>
       <c r="J18" t="n">
-        <v>6116</v>
+        <v>4537</v>
       </c>
       <c r="K18" t="n">
-        <v>0.571</v>
+        <v>0.424</v>
       </c>
       <c r="L18" t="n">
-        <v>5146</v>
+        <v>4763</v>
       </c>
       <c r="M18" t="n">
-        <v>0.481</v>
+        <v>0.445</v>
       </c>
       <c r="N18" t="s">
         <v>41</v>
@@ -3325,7 +3328,7 @@
         <v>135</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D19" t="s">
         <v>136</v>
@@ -3335,25 +3338,25 @@
       </c>
       <c r="F19"/>
       <c r="G19" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H19" t="n">
-        <v>542895</v>
+        <v>562905</v>
       </c>
       <c r="I19" t="n">
-        <v>93.729</v>
+        <v>97.183</v>
       </c>
       <c r="J19" t="n">
-        <v>8113</v>
+        <v>10017</v>
       </c>
       <c r="K19" t="n">
-        <v>1.401</v>
+        <v>1.729</v>
       </c>
       <c r="L19" t="n">
-        <v>8951</v>
+        <v>8337</v>
       </c>
       <c r="M19" t="n">
-        <v>1.545</v>
+        <v>1.439</v>
       </c>
       <c r="N19" t="s">
         <v>138</v>
@@ -3376,7 +3379,7 @@
         <v>142</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>43984</v>
+        <v>43985</v>
       </c>
       <c r="D20" t="s">
         <v>143</v>
@@ -3388,21 +3391,21 @@
         <v>145</v>
       </c>
       <c r="G20" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H20" t="n">
-        <v>72769</v>
+        <v>74728</v>
       </c>
       <c r="I20" t="n">
-        <v>4.125</v>
+        <v>4.236</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20" t="n">
-        <v>1142</v>
+        <v>1195</v>
       </c>
       <c r="M20" t="n">
-        <v>0.065</v>
+        <v>0.068</v>
       </c>
       <c r="N20" t="s">
         <v>144</v>
@@ -3425,7 +3428,7 @@
         <v>149</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D21" t="s">
         <v>150</v>
@@ -3435,25 +3438,25 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H21" t="n">
-        <v>94272</v>
+        <v>99178</v>
       </c>
       <c r="I21" t="n">
-        <v>14.534</v>
+        <v>15.291</v>
       </c>
       <c r="J21" t="n">
-        <v>2435</v>
+        <v>2531</v>
       </c>
       <c r="K21" t="n">
-        <v>0.375</v>
+        <v>0.39</v>
       </c>
       <c r="L21" t="n">
-        <v>2399</v>
+        <v>2419</v>
       </c>
       <c r="M21" t="n">
-        <v>0.37</v>
+        <v>0.373</v>
       </c>
       <c r="N21" t="s">
         <v>151</v>
@@ -3476,7 +3479,7 @@
         <v>155</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D22" t="s">
         <v>156</v>
@@ -3486,25 +3489,25 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H22" t="n">
-        <v>86435</v>
+        <v>88570</v>
       </c>
       <c r="I22" t="n">
-        <v>65.158</v>
+        <v>66.768</v>
       </c>
       <c r="J22" t="n">
-        <v>1262</v>
+        <v>1122</v>
       </c>
       <c r="K22" t="n">
-        <v>0.951</v>
+        <v>0.846</v>
       </c>
       <c r="L22" t="n">
-        <v>976</v>
+        <v>980</v>
       </c>
       <c r="M22" t="n">
-        <v>0.736</v>
+        <v>0.739</v>
       </c>
       <c r="N22" t="s">
         <v>158</v>
@@ -3527,7 +3530,7 @@
         <v>163</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D23" t="s">
         <v>164</v>
@@ -3537,25 +3540,21 @@
       </c>
       <c r="F23"/>
       <c r="G23" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H23" t="n">
-        <v>120429</v>
+        <v>131368</v>
       </c>
       <c r="I23" t="n">
-        <v>1.048</v>
-      </c>
-      <c r="J23" t="n">
-        <v>4120</v>
-      </c>
-      <c r="K23" t="n">
-        <v>0.036</v>
-      </c>
+        <v>1.143</v>
+      </c>
+      <c r="J23"/>
+      <c r="K23"/>
       <c r="L23" t="n">
-        <v>4116</v>
+        <v>4255</v>
       </c>
       <c r="M23" t="n">
-        <v>0.036</v>
+        <v>0.037</v>
       </c>
       <c r="N23" t="s">
         <v>165</v>
@@ -3578,7 +3577,7 @@
         <v>169</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>43983</v>
+        <v>43984</v>
       </c>
       <c r="D24" t="s">
         <v>170</v>
@@ -3591,22 +3590,22 @@
         <v>98</v>
       </c>
       <c r="H24" t="n">
-        <v>192410</v>
+        <v>194722</v>
       </c>
       <c r="I24" t="n">
-        <v>34.727</v>
+        <v>35.144</v>
       </c>
       <c r="J24" t="n">
-        <v>1346</v>
+        <v>2231</v>
       </c>
       <c r="K24" t="n">
-        <v>0.243</v>
+        <v>0.403</v>
       </c>
       <c r="L24" t="n">
-        <v>2354</v>
+        <v>2177</v>
       </c>
       <c r="M24" t="n">
-        <v>0.425</v>
+        <v>0.393</v>
       </c>
       <c r="N24" t="s">
         <v>172</v>
@@ -3629,7 +3628,7 @@
         <v>175</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>43975</v>
+        <v>43981</v>
       </c>
       <c r="D25" t="s">
         <v>176</v>
@@ -3641,21 +3640,21 @@
         <v>178</v>
       </c>
       <c r="G25" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
       <c r="J25" t="n">
-        <v>30984</v>
+        <v>33728</v>
       </c>
       <c r="K25" t="n">
-        <v>0.475</v>
+        <v>0.517</v>
       </c>
       <c r="L25" t="n">
-        <v>30984</v>
+        <v>33728</v>
       </c>
       <c r="M25" t="n">
-        <v>0.475</v>
+        <v>0.517</v>
       </c>
       <c r="N25" t="s">
         <v>177</v>
@@ -3727,7 +3726,7 @@
         <v>186</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>43975</v>
+        <v>43982</v>
       </c>
       <c r="D27" t="s">
         <v>187</v>
@@ -3739,21 +3738,21 @@
         <v>189</v>
       </c>
       <c r="G27" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H27" t="n">
-        <v>3952971</v>
+        <v>4348880</v>
       </c>
       <c r="I27" t="n">
-        <v>47.181</v>
+        <v>51.906</v>
       </c>
       <c r="J27"/>
       <c r="K27"/>
       <c r="L27" t="n">
-        <v>49255</v>
+        <v>56062</v>
       </c>
       <c r="M27" t="n">
-        <v>0.588</v>
+        <v>0.669</v>
       </c>
       <c r="N27" t="s">
         <v>188</v>
@@ -3829,7 +3828,7 @@
         <v>202</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>43982</v>
+        <v>43984</v>
       </c>
       <c r="D29" t="s">
         <v>195</v>
@@ -3841,25 +3840,25 @@
         <v>203</v>
       </c>
       <c r="G29" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H29" t="n">
-        <v>219825</v>
+        <v>223065</v>
       </c>
       <c r="I29" t="n">
-        <v>7.074</v>
+        <v>7.179</v>
       </c>
       <c r="J29" t="n">
-        <v>1400</v>
+        <v>2912</v>
       </c>
       <c r="K29" t="n">
-        <v>0.045</v>
+        <v>0.094</v>
       </c>
       <c r="L29" t="n">
-        <v>2528</v>
+        <v>2454</v>
       </c>
       <c r="M29" t="n">
-        <v>0.081</v>
+        <v>0.079</v>
       </c>
       <c r="N29" t="s">
         <v>198</v>
@@ -3882,7 +3881,7 @@
         <v>205</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D30" t="s">
         <v>206</v>
@@ -3892,25 +3891,21 @@
       </c>
       <c r="F30"/>
       <c r="G30" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H30" t="n">
-        <v>185590</v>
+        <v>193929</v>
       </c>
       <c r="I30" t="n">
-        <v>17.806</v>
-      </c>
-      <c r="J30" t="n">
-        <v>3167</v>
-      </c>
-      <c r="K30" t="n">
-        <v>0.304</v>
-      </c>
+        <v>18.606</v>
+      </c>
+      <c r="J30"/>
+      <c r="K30"/>
       <c r="L30" t="n">
-        <v>3514</v>
+        <v>3352</v>
       </c>
       <c r="M30" t="n">
-        <v>0.337</v>
+        <v>0.322</v>
       </c>
       <c r="N30" t="s">
         <v>208</v>
@@ -3933,7 +3928,7 @@
         <v>212</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>43977</v>
+        <v>43983</v>
       </c>
       <c r="D31" t="s">
         <v>213</v>
@@ -3943,21 +3938,25 @@
       </c>
       <c r="F31"/>
       <c r="G31" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H31" t="n">
-        <v>222048</v>
+        <v>241992</v>
       </c>
       <c r="I31" t="n">
-        <v>29.618</v>
-      </c>
-      <c r="J31"/>
-      <c r="K31"/>
+        <v>32.279</v>
+      </c>
+      <c r="J31" t="n">
+        <v>3958</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.528</v>
+      </c>
       <c r="L31" t="n">
-        <v>2384</v>
+        <v>2642</v>
       </c>
       <c r="M31" t="n">
-        <v>0.318</v>
+        <v>0.352</v>
       </c>
       <c r="N31" t="s">
         <v>215</v>
@@ -3980,7 +3979,7 @@
         <v>219</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D32" t="s">
         <v>220</v>
@@ -3992,25 +3991,25 @@
         <v>222</v>
       </c>
       <c r="G32" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H32" t="n">
-        <v>191572</v>
+        <v>202606</v>
       </c>
       <c r="I32" t="n">
-        <v>19.831</v>
+        <v>20.973</v>
       </c>
       <c r="J32" t="n">
-        <v>1603</v>
+        <v>6712</v>
       </c>
       <c r="K32" t="n">
-        <v>0.166</v>
+        <v>0.695</v>
       </c>
       <c r="L32" t="n">
-        <v>3087</v>
+        <v>3208</v>
       </c>
       <c r="M32" t="n">
-        <v>0.32</v>
+        <v>0.332</v>
       </c>
       <c r="N32" t="s">
         <v>221</v>
@@ -4033,7 +4032,7 @@
         <v>227</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D33" t="s">
         <v>228</v>
@@ -4043,25 +4042,25 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H33" t="n">
-        <v>61314</v>
+        <v>62189</v>
       </c>
       <c r="I33" t="n">
-        <v>179.675</v>
+        <v>182.239</v>
       </c>
       <c r="J33" t="n">
-        <v>199</v>
+        <v>550</v>
       </c>
       <c r="K33" t="n">
-        <v>0.583</v>
+        <v>1.612</v>
       </c>
       <c r="L33" t="n">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M33" t="n">
-        <v>0.73</v>
+        <v>0.727</v>
       </c>
       <c r="N33" t="s">
         <v>229</v>
@@ -4137,7 +4136,7 @@
         <v>238</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>43984</v>
+        <v>43987</v>
       </c>
       <c r="D35" t="s">
         <v>234</v>
@@ -4149,25 +4148,25 @@
         <v>236</v>
       </c>
       <c r="G35" t="n">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H35" t="n">
-        <v>3966075</v>
+        <v>4386379</v>
       </c>
       <c r="I35" t="n">
-        <v>2.874</v>
+        <v>3.179</v>
       </c>
       <c r="J35" t="n">
-        <v>128868</v>
+        <v>143661</v>
       </c>
       <c r="K35" t="n">
+        <v>0.104</v>
+      </c>
+      <c r="L35" t="n">
+        <v>128934</v>
+      </c>
+      <c r="M35" t="n">
         <v>0.093</v>
-      </c>
-      <c r="L35" t="n">
-        <v>119994</v>
-      </c>
-      <c r="M35" t="n">
-        <v>0.087</v>
       </c>
       <c r="N35" t="s">
         <v>235</v>
@@ -4190,7 +4189,7 @@
         <v>240</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D36" t="s">
         <v>241</v>
@@ -4200,22 +4199,22 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H36" t="n">
-        <v>246433</v>
+        <v>256810</v>
       </c>
       <c r="I36" t="n">
-        <v>0.901</v>
+        <v>0.939</v>
       </c>
       <c r="J36" t="n">
-        <v>8486</v>
+        <v>5074</v>
       </c>
       <c r="K36" t="n">
-        <v>0.031</v>
+        <v>0.019</v>
       </c>
       <c r="L36" t="n">
-        <v>7274</v>
+        <v>7366</v>
       </c>
       <c r="M36" t="n">
         <v>0.027</v>
@@ -4241,7 +4240,7 @@
         <v>247</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D37" t="s">
         <v>248</v>
@@ -4251,25 +4250,25 @@
       </c>
       <c r="F37"/>
       <c r="G37" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H37" t="n">
-        <v>975936</v>
+        <v>1019362</v>
       </c>
       <c r="I37" t="n">
-        <v>11.619</v>
+        <v>12.136</v>
       </c>
       <c r="J37" t="n">
-        <v>20071</v>
+        <v>22353</v>
       </c>
       <c r="K37" t="n">
-        <v>0.239</v>
+        <v>0.266</v>
       </c>
       <c r="L37" t="n">
-        <v>19835</v>
+        <v>20400</v>
       </c>
       <c r="M37" t="n">
-        <v>0.236</v>
+        <v>0.243</v>
       </c>
       <c r="N37" t="s">
         <v>249</v>
@@ -4339,7 +4338,7 @@
         <v>259</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>43978</v>
+        <v>43979</v>
       </c>
       <c r="D39" t="s">
         <v>260</v>
@@ -4349,25 +4348,25 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H39" t="n">
-        <v>559756</v>
+        <v>565161</v>
       </c>
       <c r="I39" t="n">
-        <v>64.67</v>
+        <v>65.295</v>
       </c>
       <c r="J39" t="n">
-        <v>6642</v>
+        <v>5357</v>
       </c>
       <c r="K39" t="n">
-        <v>0.767</v>
+        <v>0.619</v>
       </c>
       <c r="L39" t="n">
-        <v>4900</v>
+        <v>4799</v>
       </c>
       <c r="M39" t="n">
-        <v>0.566</v>
+        <v>0.554</v>
       </c>
       <c r="N39" t="s">
         <v>41</v>
@@ -4390,7 +4389,7 @@
         <v>265</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>43985</v>
+        <v>43986</v>
       </c>
       <c r="D40" t="s">
         <v>266</v>
@@ -4402,25 +4401,25 @@
         <v>268</v>
       </c>
       <c r="G40" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H40" t="n">
-        <v>2497337</v>
+        <v>2524788</v>
       </c>
       <c r="I40" t="n">
-        <v>41.304</v>
+        <v>41.758</v>
       </c>
       <c r="J40" t="n">
-        <v>20035</v>
+        <v>27451</v>
       </c>
       <c r="K40" t="n">
-        <v>0.331</v>
+        <v>0.454</v>
       </c>
       <c r="L40" t="n">
-        <v>29541</v>
+        <v>27771</v>
       </c>
       <c r="M40" t="n">
-        <v>0.489</v>
+        <v>0.459</v>
       </c>
       <c r="N40" t="s">
         <v>269</v>
@@ -4443,7 +4442,7 @@
         <v>272</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>43985</v>
+        <v>43986</v>
       </c>
       <c r="D41" t="s">
         <v>266</v>
@@ -4455,25 +4454,25 @@
         <v>268</v>
       </c>
       <c r="G41" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H41" t="n">
-        <v>3999591</v>
+        <v>4049544</v>
       </c>
       <c r="I41" t="n">
-        <v>66.151</v>
+        <v>66.977</v>
       </c>
       <c r="J41" t="n">
-        <v>37299</v>
+        <v>49953</v>
       </c>
       <c r="K41" t="n">
-        <v>0.617</v>
+        <v>0.826</v>
       </c>
       <c r="L41" t="n">
-        <v>56049</v>
+        <v>52343</v>
       </c>
       <c r="M41" t="n">
-        <v>0.927</v>
+        <v>0.866</v>
       </c>
       <c r="N41" t="s">
         <v>269</v>
@@ -4496,7 +4495,7 @@
         <v>275</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D42" t="s">
         <v>276</v>
@@ -4508,21 +4507,21 @@
         <v>278</v>
       </c>
       <c r="G42" t="n">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H42" t="n">
-        <v>300277</v>
+        <v>307462</v>
       </c>
       <c r="I42" t="n">
-        <v>2.374</v>
+        <v>2.431</v>
       </c>
       <c r="J42"/>
       <c r="K42"/>
       <c r="L42" t="n">
-        <v>3091</v>
+        <v>3243</v>
       </c>
       <c r="M42" t="n">
-        <v>0.024</v>
+        <v>0.026</v>
       </c>
       <c r="N42" t="s">
         <v>279</v>
@@ -4545,7 +4544,7 @@
         <v>282</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D43" t="s">
         <v>283</v>
@@ -4557,25 +4556,25 @@
         <v>284</v>
       </c>
       <c r="G43" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H43" t="n">
-        <v>489518</v>
+        <v>504964</v>
       </c>
       <c r="I43" t="n">
-        <v>3.87</v>
+        <v>3.993</v>
       </c>
       <c r="J43" t="n">
-        <v>3454</v>
+        <v>6999</v>
       </c>
       <c r="K43" t="n">
-        <v>0.027</v>
+        <v>0.055</v>
       </c>
       <c r="L43" t="n">
-        <v>5138</v>
+        <v>5584</v>
       </c>
       <c r="M43" t="n">
-        <v>0.041</v>
+        <v>0.044</v>
       </c>
       <c r="N43" t="s">
         <v>279</v>
@@ -4649,7 +4648,7 @@
         <v>292</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D45" t="s">
         <v>293</v>
@@ -4659,25 +4658,25 @@
       </c>
       <c r="F45"/>
       <c r="G45" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H45" t="n">
-        <v>82946</v>
+        <v>87698</v>
       </c>
       <c r="I45" t="n">
-        <v>1.543</v>
+        <v>1.631</v>
       </c>
       <c r="J45" t="n">
-        <v>2892</v>
+        <v>2640</v>
       </c>
       <c r="K45" t="n">
-        <v>0.054</v>
+        <v>0.049</v>
       </c>
       <c r="L45" t="n">
-        <v>2669</v>
+        <v>2504</v>
       </c>
       <c r="M45" t="n">
-        <v>0.05</v>
+        <v>0.047</v>
       </c>
       <c r="N45" t="s">
         <v>41</v>
@@ -4700,7 +4699,7 @@
         <v>299</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D46" t="s">
         <v>300</v>
@@ -4712,25 +4711,25 @@
         <v>302</v>
       </c>
       <c r="G46" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H46" t="n">
-        <v>112965</v>
+        <v>115461</v>
       </c>
       <c r="I46" t="n">
-        <v>59.89</v>
+        <v>61.213</v>
       </c>
       <c r="J46" t="n">
-        <v>1561</v>
+        <v>1010</v>
       </c>
       <c r="K46" t="n">
-        <v>0.828</v>
+        <v>0.535</v>
       </c>
       <c r="L46" t="n">
-        <v>1345</v>
+        <v>1219</v>
       </c>
       <c r="M46" t="n">
-        <v>0.713</v>
+        <v>0.646</v>
       </c>
       <c r="N46" t="s">
         <v>301</v>
@@ -4753,7 +4752,7 @@
         <v>305</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D47" t="s">
         <v>306</v>
@@ -4763,25 +4762,25 @@
       </c>
       <c r="F47"/>
       <c r="G47" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H47" t="n">
-        <v>315112</v>
+        <v>326294</v>
       </c>
       <c r="I47" t="n">
-        <v>115.753</v>
+        <v>119.86</v>
       </c>
       <c r="J47" t="n">
-        <v>5387</v>
+        <v>5254</v>
       </c>
       <c r="K47" t="n">
-        <v>1.979</v>
+        <v>1.93</v>
       </c>
       <c r="L47" t="n">
-        <v>4840</v>
+        <v>4600</v>
       </c>
       <c r="M47" t="n">
-        <v>1.778</v>
+        <v>1.69</v>
       </c>
       <c r="N47" t="s">
         <v>41</v>
@@ -4804,7 +4803,7 @@
         <v>310</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>43985</v>
+        <v>43986</v>
       </c>
       <c r="D48" t="s">
         <v>311</v>
@@ -4814,25 +4813,25 @@
       </c>
       <c r="F48"/>
       <c r="G48" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H48" t="n">
-        <v>79484</v>
+        <v>82377</v>
       </c>
       <c r="I48" t="n">
-        <v>126.976</v>
+        <v>131.598</v>
       </c>
       <c r="J48" t="n">
-        <v>1458</v>
+        <v>2893</v>
       </c>
       <c r="K48" t="n">
-        <v>2.329</v>
+        <v>4.622</v>
       </c>
       <c r="L48" t="n">
-        <v>1334</v>
+        <v>1611</v>
       </c>
       <c r="M48" t="n">
-        <v>2.131</v>
+        <v>2.574</v>
       </c>
       <c r="N48" t="s">
         <v>312</v>
@@ -4855,7 +4854,7 @@
         <v>316</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>43983</v>
+        <v>43987</v>
       </c>
       <c r="D49" t="s">
         <v>317</v>
@@ -4867,25 +4866,25 @@
         <v>319</v>
       </c>
       <c r="G49" t="n">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="H49" t="n">
-        <v>560738</v>
+        <v>590613</v>
       </c>
       <c r="I49" t="n">
-        <v>17.325</v>
+        <v>18.248</v>
       </c>
       <c r="J49" t="n">
-        <v>7555</v>
+        <v>8127</v>
       </c>
       <c r="K49" t="n">
+        <v>0.251</v>
+      </c>
+      <c r="L49" t="n">
+        <v>7531</v>
+      </c>
+      <c r="M49" t="n">
         <v>0.233</v>
-      </c>
-      <c r="L49" t="n">
-        <v>6767</v>
-      </c>
-      <c r="M49" t="n">
-        <v>0.209</v>
       </c>
       <c r="N49" t="s">
         <v>41</v>
@@ -4908,7 +4907,7 @@
         <v>323</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>43984</v>
+        <v>43985</v>
       </c>
       <c r="D50" t="s">
         <v>324</v>
@@ -4920,25 +4919,25 @@
         <v>326</v>
       </c>
       <c r="G50" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H50" t="n">
-        <v>25591</v>
+        <v>26243</v>
       </c>
       <c r="I50" t="n">
-        <v>47.343</v>
+        <v>48.549</v>
       </c>
       <c r="J50" t="n">
-        <v>807</v>
+        <v>652</v>
       </c>
       <c r="K50" t="n">
-        <v>1.493</v>
+        <v>1.206</v>
       </c>
       <c r="L50" t="n">
-        <v>796</v>
+        <v>772</v>
       </c>
       <c r="M50" t="n">
-        <v>1.473</v>
+        <v>1.428</v>
       </c>
       <c r="N50" t="s">
         <v>327</v>
@@ -4961,7 +4960,7 @@
         <v>331</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D51" t="s">
         <v>332</v>
@@ -4971,25 +4970,25 @@
       </c>
       <c r="F51"/>
       <c r="G51" t="n">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H51" t="n">
-        <v>250911</v>
+        <v>267389</v>
       </c>
       <c r="I51" t="n">
-        <v>1.946</v>
+        <v>2.074</v>
       </c>
       <c r="J51" t="n">
-        <v>445</v>
+        <v>526</v>
       </c>
       <c r="K51" t="n">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="L51" t="n">
-        <v>3710</v>
+        <v>3674</v>
       </c>
       <c r="M51" t="n">
-        <v>0.029</v>
+        <v>0.028</v>
       </c>
       <c r="N51" t="s">
         <v>333</v>
@@ -5065,7 +5064,7 @@
         <v>343</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>43983</v>
+        <v>43986</v>
       </c>
       <c r="D53" t="s">
         <v>344</v>
@@ -5073,382 +5072,378 @@
       <c r="E53" t="s">
         <v>345</v>
       </c>
-      <c r="F53"/>
+      <c r="F53" t="s">
+        <v>346</v>
+      </c>
       <c r="G53" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H53" t="n">
-        <v>28251</v>
+        <v>31701</v>
       </c>
       <c r="I53" t="n">
-        <v>0.519</v>
-      </c>
-      <c r="J53" t="n">
-        <v>1174</v>
-      </c>
-      <c r="K53" t="n">
+        <v>0.583</v>
+      </c>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53" t="n">
+        <v>1173</v>
+      </c>
+      <c r="M53" t="n">
         <v>0.022</v>
-      </c>
-      <c r="L53" t="n">
-        <v>1134</v>
-      </c>
-      <c r="M53" t="n">
-        <v>0.021</v>
       </c>
       <c r="N53" t="s">
         <v>345</v>
       </c>
       <c r="O53" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="P53" t="s">
         <v>51</v>
       </c>
       <c r="Q53" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B54" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>43982</v>
+        <v>43986</v>
       </c>
       <c r="D54" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E54" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="F54" t="s">
+        <v>353</v>
+      </c>
+      <c r="G54" t="n">
+        <v>105</v>
+      </c>
+      <c r="H54" t="n">
+        <v>84134</v>
+      </c>
+      <c r="I54" t="n">
+        <v>2.888</v>
+      </c>
+      <c r="J54" t="n">
+        <v>3867</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="L54" t="n">
+        <v>3317</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0.114</v>
+      </c>
+      <c r="N54" t="s">
         <v>352</v>
       </c>
-      <c r="G54" t="n">
-        <v>101</v>
-      </c>
-      <c r="H54" t="n">
-        <v>69587</v>
-      </c>
-      <c r="I54" t="n">
-        <v>2.388</v>
-      </c>
-      <c r="J54" t="n">
-        <v>2858</v>
-      </c>
-      <c r="K54" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="L54" t="n">
-        <v>2967</v>
-      </c>
-      <c r="M54" t="n">
-        <v>0.102</v>
-      </c>
-      <c r="N54" t="s">
-        <v>351</v>
-      </c>
       <c r="O54" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="P54" t="s">
         <v>92</v>
       </c>
       <c r="Q54" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B55" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D55" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E55" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H55" t="n">
-        <v>359833</v>
+        <v>378912</v>
       </c>
       <c r="I55" t="n">
-        <v>21</v>
+        <v>22.113</v>
       </c>
       <c r="J55" t="n">
-        <v>1903</v>
+        <v>8394</v>
       </c>
       <c r="K55" t="n">
-        <v>0.111</v>
+        <v>0.49</v>
       </c>
       <c r="L55" t="n">
-        <v>3948</v>
+        <v>5188</v>
       </c>
       <c r="M55" t="n">
-        <v>0.23</v>
+        <v>0.303</v>
       </c>
       <c r="N55" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="O55" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="P55" t="s">
         <v>92</v>
       </c>
       <c r="Q55" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B56" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D56" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E56" t="s">
         <v>41</v>
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H56" t="n">
-        <v>283525</v>
+        <v>288987</v>
       </c>
       <c r="I56" t="n">
-        <v>58.795</v>
+        <v>59.928</v>
       </c>
       <c r="J56" t="n">
-        <v>1262</v>
+        <v>2813</v>
       </c>
       <c r="K56" t="n">
-        <v>0.262</v>
+        <v>0.583</v>
       </c>
       <c r="L56" t="n">
-        <v>2299</v>
+        <v>1876</v>
       </c>
       <c r="M56" t="n">
-        <v>0.477</v>
+        <v>0.389</v>
       </c>
       <c r="N56" t="s">
+        <v>366</v>
+      </c>
+      <c r="O56" t="s">
         <v>365</v>
-      </c>
-      <c r="O56" t="s">
-        <v>364</v>
       </c>
       <c r="P56" t="s">
         <v>22</v>
       </c>
       <c r="Q56" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B57" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D57" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E57" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H57" t="n">
-        <v>69801</v>
+        <v>73064</v>
       </c>
       <c r="I57" t="n">
-        <v>0.339</v>
+        <v>0.354</v>
       </c>
       <c r="J57" t="n">
-        <v>3916</v>
+        <v>1728</v>
       </c>
       <c r="K57" t="n">
-        <v>0.019</v>
+        <v>0.008</v>
       </c>
       <c r="L57" t="n">
-        <v>3037</v>
+        <v>2048</v>
       </c>
       <c r="M57" t="n">
-        <v>0.015</v>
+        <v>0.01</v>
       </c>
       <c r="N57" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="O57" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="P57" t="s">
         <v>51</v>
       </c>
       <c r="Q57" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B58" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D58" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E58" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H58" t="n">
-        <v>252232</v>
+        <v>257303</v>
       </c>
       <c r="I58" t="n">
-        <v>46.527</v>
+        <v>47.462</v>
       </c>
       <c r="J58" t="n">
-        <v>1264</v>
+        <v>2590</v>
       </c>
       <c r="K58" t="n">
-        <v>0.233</v>
+        <v>0.478</v>
       </c>
       <c r="L58" t="n">
-        <v>1767</v>
+        <v>1707</v>
       </c>
       <c r="M58" t="n">
-        <v>0.326</v>
+        <v>0.315</v>
       </c>
       <c r="N58" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="O58" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="P58" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="Q58" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B59" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D59" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E59" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H59" t="n">
-        <v>595344</v>
+        <v>638323</v>
       </c>
       <c r="I59" t="n">
-        <v>2.695</v>
+        <v>2.89</v>
       </c>
       <c r="J59" t="n">
-        <v>17370</v>
+        <v>22812</v>
       </c>
       <c r="K59" t="n">
-        <v>0.079</v>
+        <v>0.103</v>
       </c>
       <c r="L59" t="n">
-        <v>13706</v>
+        <v>16901</v>
       </c>
       <c r="M59" t="n">
-        <v>0.062</v>
+        <v>0.077</v>
       </c>
       <c r="N59" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="O59" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="P59" t="s">
         <v>22</v>
       </c>
       <c r="Q59" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B60" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>43979</v>
+        <v>43986</v>
       </c>
       <c r="D60" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E60" t="s">
-        <v>41</v>
-      </c>
-      <c r="F60" t="s">
-        <v>389</v>
-      </c>
+        <v>390</v>
+      </c>
+      <c r="F60"/>
       <c r="G60" t="n">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="H60" t="n">
-        <v>63202</v>
+        <v>70245</v>
       </c>
       <c r="I60" t="n">
-        <v>14.648</v>
+        <v>16.28</v>
       </c>
       <c r="J60" t="n">
-        <v>1307</v>
+        <v>1531</v>
       </c>
       <c r="K60" t="n">
-        <v>0.303</v>
+        <v>0.355</v>
       </c>
       <c r="L60" t="n">
         <v>1325</v>
@@ -5457,13 +5452,13 @@
         <v>0.307</v>
       </c>
       <c r="N60" t="s">
-        <v>41</v>
+        <v>390</v>
       </c>
       <c r="O60" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="P60" t="s">
-        <v>127</v>
+        <v>22</v>
       </c>
       <c r="Q60" t="s">
         <v>391</v>
@@ -5477,7 +5472,7 @@
         <v>393</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D61" t="s">
         <v>394</v>
@@ -5487,25 +5482,25 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H61" t="n">
-        <v>32106</v>
+        <v>34240</v>
       </c>
       <c r="I61" t="n">
-        <v>4.501</v>
+        <v>4.801</v>
       </c>
       <c r="J61" t="n">
-        <v>1272</v>
+        <v>1159</v>
       </c>
       <c r="K61" t="n">
-        <v>0.178</v>
+        <v>0.162</v>
       </c>
       <c r="L61" t="n">
-        <v>848</v>
+        <v>974</v>
       </c>
       <c r="M61" t="n">
-        <v>0.119</v>
+        <v>0.137</v>
       </c>
       <c r="N61" t="s">
         <v>395</v>
@@ -5528,7 +5523,7 @@
         <v>399</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D62" t="s">
         <v>400</v>
@@ -5538,25 +5533,21 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H62" t="n">
-        <v>152228</v>
+        <v>153773</v>
       </c>
       <c r="I62" t="n">
-        <v>4.617</v>
-      </c>
-      <c r="J62" t="n">
-        <v>6603</v>
-      </c>
-      <c r="K62" t="n">
-        <v>0.2</v>
-      </c>
+        <v>4.664</v>
+      </c>
+      <c r="J62"/>
+      <c r="K62"/>
       <c r="L62" t="n">
-        <v>3539</v>
+        <v>2847</v>
       </c>
       <c r="M62" t="n">
-        <v>0.107</v>
+        <v>0.086</v>
       </c>
       <c r="N62" t="s">
         <v>401</v>
@@ -5579,7 +5570,7 @@
         <v>405</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>43983</v>
+        <v>43985</v>
       </c>
       <c r="D63" t="s">
         <v>406</v>
@@ -5591,25 +5582,21 @@
         <v>408</v>
       </c>
       <c r="G63" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H63" t="n">
-        <v>337306</v>
+        <v>357351</v>
       </c>
       <c r="I63" t="n">
-        <v>3.078</v>
-      </c>
-      <c r="J63" t="n">
-        <v>8471</v>
-      </c>
-      <c r="K63" t="n">
-        <v>0.077</v>
-      </c>
+        <v>3.261</v>
+      </c>
+      <c r="J63"/>
+      <c r="K63"/>
       <c r="L63" t="n">
-        <v>7737</v>
+        <v>8561</v>
       </c>
       <c r="M63" t="n">
-        <v>0.071</v>
+        <v>0.078</v>
       </c>
       <c r="N63" t="s">
         <v>214</v>
@@ -5685,7 +5672,7 @@
         <v>419</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>43982</v>
+        <v>43984</v>
       </c>
       <c r="D65" t="s">
         <v>420</v>
@@ -5695,25 +5682,25 @@
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H65" t="n">
-        <v>847181</v>
+        <v>873998</v>
       </c>
       <c r="I65" t="n">
-        <v>83.084</v>
+        <v>85.714</v>
       </c>
       <c r="J65" t="n">
-        <v>6500</v>
+        <v>15344</v>
       </c>
       <c r="K65" t="n">
-        <v>0.637</v>
+        <v>1.505</v>
       </c>
       <c r="L65" t="n">
-        <v>13532</v>
+        <v>13580</v>
       </c>
       <c r="M65" t="n">
-        <v>1.327</v>
+        <v>1.332</v>
       </c>
       <c r="N65" t="s">
         <v>421</v>
@@ -5736,7 +5723,7 @@
         <v>425</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D66" t="s">
         <v>426</v>
@@ -5746,25 +5733,25 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H66" t="n">
-        <v>236437</v>
+        <v>246362</v>
       </c>
       <c r="I66" t="n">
-        <v>82.066</v>
+        <v>85.511</v>
       </c>
       <c r="J66" t="n">
-        <v>5339</v>
+        <v>5276</v>
       </c>
       <c r="K66" t="n">
-        <v>1.853</v>
+        <v>1.831</v>
       </c>
       <c r="L66" t="n">
-        <v>5037</v>
+        <v>4781</v>
       </c>
       <c r="M66" t="n">
-        <v>1.748</v>
+        <v>1.659</v>
       </c>
       <c r="N66" t="s">
         <v>427</v>
@@ -5787,7 +5774,7 @@
         <v>431</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>43980</v>
+        <v>43987</v>
       </c>
       <c r="D67" t="s">
         <v>432</v>
@@ -5795,35 +5782,33 @@
       <c r="E67" t="s">
         <v>433</v>
       </c>
-      <c r="F67" t="s">
-        <v>434</v>
-      </c>
+      <c r="F67"/>
       <c r="G67" t="n">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H67" t="n">
-        <v>421451</v>
+        <v>484782</v>
       </c>
       <c r="I67" t="n">
-        <v>21.908</v>
+        <v>25.2</v>
       </c>
       <c r="J67" t="n">
-        <v>11451</v>
+        <v>11932</v>
       </c>
       <c r="K67" t="n">
-        <v>0.595</v>
+        <v>0.62</v>
       </c>
       <c r="L67" t="n">
-        <v>9829</v>
+        <v>9047</v>
       </c>
       <c r="M67" t="n">
-        <v>0.511</v>
+        <v>0.47</v>
       </c>
       <c r="N67" t="s">
         <v>433</v>
       </c>
       <c r="O67" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="P67" t="s">
         <v>22</v>
@@ -5840,7 +5825,7 @@
         <v>437</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D68" t="s">
         <v>438</v>
@@ -5850,25 +5835,25 @@
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H68" t="n">
-        <v>11426045</v>
+        <v>12053663</v>
       </c>
       <c r="I68" t="n">
-        <v>78.296</v>
+        <v>82.596</v>
       </c>
       <c r="J68" t="n">
-        <v>274423</v>
+        <v>320612</v>
       </c>
       <c r="K68" t="n">
-        <v>1.88</v>
+        <v>2.197</v>
       </c>
       <c r="L68" t="n">
-        <v>287150</v>
+        <v>293372</v>
       </c>
       <c r="M68" t="n">
-        <v>1.968</v>
+        <v>2.01</v>
       </c>
       <c r="N68" t="s">
         <v>439</v>
@@ -5891,7 +5876,7 @@
         <v>443</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>43984</v>
+        <v>43985</v>
       </c>
       <c r="D69" t="s">
         <v>444</v>
@@ -5901,25 +5886,25 @@
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H69" t="n">
-        <v>70108</v>
+        <v>71141</v>
       </c>
       <c r="I69" t="n">
-        <v>5.413</v>
+        <v>5.493</v>
       </c>
       <c r="J69" t="n">
-        <v>957</v>
+        <v>1033</v>
       </c>
       <c r="K69" t="n">
-        <v>0.074</v>
+        <v>0.08</v>
       </c>
       <c r="L69" t="n">
-        <v>1381</v>
+        <v>1234</v>
       </c>
       <c r="M69" t="n">
-        <v>0.107</v>
+        <v>0.095</v>
       </c>
       <c r="N69" t="s">
         <v>445</v>
@@ -5942,7 +5927,7 @@
         <v>449</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>43985</v>
+        <v>43986</v>
       </c>
       <c r="D70" t="s">
         <v>450</v>
@@ -5952,25 +5937,25 @@
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H70" t="n">
-        <v>870963</v>
+        <v>887209</v>
       </c>
       <c r="I70" t="n">
-        <v>25.018</v>
+        <v>25.484</v>
       </c>
       <c r="J70" t="n">
-        <v>16976</v>
+        <v>16246</v>
       </c>
       <c r="K70" t="n">
-        <v>0.488</v>
+        <v>0.467</v>
       </c>
       <c r="L70" t="n">
-        <v>16671</v>
+        <v>16645</v>
       </c>
       <c r="M70" t="n">
-        <v>0.479</v>
+        <v>0.478</v>
       </c>
       <c r="N70" t="s">
         <v>41</v>
@@ -5993,7 +5978,7 @@
         <v>453</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D71" t="s">
         <v>454</v>
@@ -6005,25 +5990,25 @@
         <v>456</v>
       </c>
       <c r="G71" t="n">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H71" t="n">
-        <v>47647</v>
+        <v>50690</v>
       </c>
       <c r="I71" t="n">
-        <v>2.846</v>
+        <v>3.027</v>
       </c>
       <c r="J71" t="n">
-        <v>1549</v>
+        <v>1700</v>
       </c>
       <c r="K71" t="n">
-        <v>0.093</v>
+        <v>0.102</v>
       </c>
       <c r="L71" t="n">
-        <v>1333</v>
+        <v>1449</v>
       </c>
       <c r="M71" t="n">
-        <v>0.08</v>
+        <v>0.087</v>
       </c>
       <c r="N71" t="s">
         <v>457</v>
@@ -6046,7 +6031,7 @@
         <v>462</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D72" t="s">
         <v>463</v>
@@ -6058,25 +6043,25 @@
         <v>464</v>
       </c>
       <c r="G72" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H72" t="n">
-        <v>252132</v>
+        <v>261266</v>
       </c>
       <c r="I72" t="n">
-        <v>37.053</v>
+        <v>38.396</v>
       </c>
       <c r="J72" t="n">
-        <v>4372</v>
+        <v>4024</v>
       </c>
       <c r="K72" t="n">
-        <v>0.643</v>
+        <v>0.591</v>
       </c>
       <c r="L72" t="n">
-        <v>4052</v>
+        <v>3892</v>
       </c>
       <c r="M72" t="n">
-        <v>0.595</v>
+        <v>0.572</v>
       </c>
       <c r="N72" t="s">
         <v>41</v>
@@ -6193,7 +6178,7 @@
         <v>476</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>43984</v>
+        <v>43987</v>
       </c>
       <c r="D75" t="s">
         <v>477</v>
@@ -6203,25 +6188,25 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H75" t="n">
-        <v>179293</v>
+        <v>185596</v>
       </c>
       <c r="I75" t="n">
-        <v>32.84</v>
+        <v>33.994</v>
       </c>
       <c r="J75" t="n">
-        <v>6418</v>
+        <v>1832</v>
       </c>
       <c r="K75" t="n">
-        <v>1.176</v>
+        <v>0.336</v>
       </c>
       <c r="L75" t="n">
-        <v>2681</v>
+        <v>2576</v>
       </c>
       <c r="M75" t="n">
-        <v>0.491</v>
+        <v>0.472</v>
       </c>
       <c r="N75" t="s">
         <v>479</v>
@@ -6244,7 +6229,7 @@
         <v>484</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D76" t="s">
         <v>485</v>
@@ -6254,25 +6239,25 @@
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H76" t="n">
-        <v>80505</v>
+        <v>82161</v>
       </c>
       <c r="I76" t="n">
-        <v>38.724</v>
+        <v>39.521</v>
       </c>
       <c r="J76" t="n">
-        <v>807</v>
+        <v>828</v>
       </c>
       <c r="K76" t="n">
-        <v>0.388</v>
+        <v>0.398</v>
       </c>
       <c r="L76" t="n">
-        <v>561</v>
+        <v>606</v>
       </c>
       <c r="M76" t="n">
-        <v>0.27</v>
+        <v>0.291</v>
       </c>
       <c r="N76" t="s">
         <v>487</v>
@@ -6295,7 +6280,7 @@
         <v>491</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>43985</v>
+        <v>43986</v>
       </c>
       <c r="D77" t="s">
         <v>492</v>
@@ -6307,25 +6292,25 @@
         <v>494</v>
       </c>
       <c r="G77" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H77" t="n">
-        <v>785979</v>
+        <v>820675</v>
       </c>
       <c r="I77" t="n">
-        <v>13.252</v>
+        <v>13.837</v>
       </c>
       <c r="J77" t="n">
-        <v>24445</v>
+        <v>34696</v>
       </c>
       <c r="K77" t="n">
-        <v>0.412</v>
+        <v>0.585</v>
       </c>
       <c r="L77" t="n">
-        <v>21569</v>
+        <v>23565</v>
       </c>
       <c r="M77" t="n">
-        <v>0.364</v>
+        <v>0.397</v>
       </c>
       <c r="N77" t="s">
         <v>493</v>
@@ -6348,7 +6333,7 @@
         <v>498</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D78" t="s">
         <v>499</v>
@@ -6358,25 +6343,25 @@
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H78" t="n">
-        <v>956852</v>
+        <v>990960</v>
       </c>
       <c r="I78" t="n">
-        <v>18.663</v>
+        <v>19.329</v>
       </c>
       <c r="J78" t="n">
-        <v>17001</v>
+        <v>17102</v>
       </c>
       <c r="K78" t="n">
-        <v>0.332</v>
+        <v>0.334</v>
       </c>
       <c r="L78" t="n">
-        <v>14854</v>
+        <v>15120</v>
       </c>
       <c r="M78" t="n">
-        <v>0.29</v>
+        <v>0.295</v>
       </c>
       <c r="N78" t="s">
         <v>500</v>
@@ -6493,7 +6478,7 @@
         <v>516</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D81" t="s">
         <v>517</v>
@@ -6503,25 +6488,25 @@
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H81" t="n">
-        <v>404065</v>
+        <v>415190</v>
       </c>
       <c r="I81" t="n">
-        <v>46.688</v>
+        <v>47.973</v>
       </c>
       <c r="J81" t="n">
-        <v>2816</v>
+        <v>4259</v>
       </c>
       <c r="K81" t="n">
-        <v>0.325</v>
+        <v>0.492</v>
       </c>
       <c r="L81" t="n">
-        <v>3065</v>
+        <v>3332</v>
       </c>
       <c r="M81" t="n">
-        <v>0.354</v>
+        <v>0.385</v>
       </c>
       <c r="N81" t="s">
         <v>518</v>
@@ -6544,7 +6529,7 @@
         <v>522</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D82" t="s">
         <v>523</v>
@@ -6554,22 +6539,22 @@
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H82" t="n">
-        <v>72683</v>
+        <v>73040</v>
       </c>
       <c r="I82" t="n">
-        <v>3.052</v>
+        <v>3.067</v>
       </c>
       <c r="J82" t="n">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="K82" t="n">
         <v>0.007</v>
       </c>
       <c r="L82" t="n">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="M82" t="n">
         <v>0.008</v>
@@ -6595,7 +6580,7 @@
         <v>529</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D83" t="s">
         <v>530</v>
@@ -6605,25 +6590,21 @@
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H83" t="n">
-        <v>212098</v>
+        <v>224386</v>
       </c>
       <c r="I83" t="n">
-        <v>3.039</v>
-      </c>
-      <c r="J83" t="n">
-        <v>4405</v>
-      </c>
-      <c r="K83" t="n">
-        <v>0.063</v>
-      </c>
+        <v>3.215</v>
+      </c>
+      <c r="J83"/>
+      <c r="K83"/>
       <c r="L83" t="n">
-        <v>5150</v>
+        <v>5234</v>
       </c>
       <c r="M83" t="n">
-        <v>0.074</v>
+        <v>0.075</v>
       </c>
       <c r="N83" t="s">
         <v>532</v>
@@ -6742,7 +6723,7 @@
         <v>549</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>43985</v>
+        <v>43986</v>
       </c>
       <c r="D86" t="s">
         <v>550</v>
@@ -6752,25 +6733,25 @@
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H86" t="n">
-        <v>2155349</v>
+        <v>2209583</v>
       </c>
       <c r="I86" t="n">
-        <v>25.556</v>
+        <v>26.199</v>
       </c>
       <c r="J86" t="n">
-        <v>52305</v>
+        <v>54234</v>
       </c>
       <c r="K86" t="n">
-        <v>0.62</v>
+        <v>0.643</v>
       </c>
       <c r="L86" t="n">
-        <v>37243</v>
+        <v>40196</v>
       </c>
       <c r="M86" t="n">
-        <v>0.442</v>
+        <v>0.477</v>
       </c>
       <c r="N86" t="s">
         <v>551</v>
@@ -6793,7 +6774,7 @@
         <v>556</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>43983</v>
+        <v>43986</v>
       </c>
       <c r="D87" t="s">
         <v>557</v>
@@ -6805,25 +6786,21 @@
         <v>559</v>
       </c>
       <c r="G87" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H87" t="n">
-        <v>99427</v>
+        <v>102780</v>
       </c>
       <c r="I87" t="n">
-        <v>2.174</v>
-      </c>
-      <c r="J87" t="n">
-        <v>2222</v>
-      </c>
-      <c r="K87" t="n">
-        <v>0.049</v>
-      </c>
+        <v>2.247</v>
+      </c>
+      <c r="J87"/>
+      <c r="K87"/>
       <c r="L87" t="n">
-        <v>1808</v>
+        <v>1522</v>
       </c>
       <c r="M87" t="n">
-        <v>0.04</v>
+        <v>0.033</v>
       </c>
       <c r="N87" t="s">
         <v>558</v>
@@ -6846,7 +6823,7 @@
         <v>563</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D88" t="s">
         <v>564</v>
@@ -6856,25 +6833,25 @@
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H88" t="n">
-        <v>381552</v>
+        <v>403551</v>
       </c>
       <c r="I88" t="n">
-        <v>8.724</v>
+        <v>9.227</v>
       </c>
       <c r="J88" t="n">
-        <v>9884</v>
+        <v>11235</v>
       </c>
       <c r="K88" t="n">
-        <v>0.226</v>
+        <v>0.257</v>
       </c>
       <c r="L88" t="n">
-        <v>9860</v>
+        <v>9462</v>
       </c>
       <c r="M88" t="n">
-        <v>0.225</v>
+        <v>0.216</v>
       </c>
       <c r="N88" t="s">
         <v>565</v>
@@ -6948,7 +6925,7 @@
         <v>575</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D90" t="s">
         <v>576</v>
@@ -6960,25 +6937,25 @@
         <v>577</v>
       </c>
       <c r="G90" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H90" t="n">
-        <v>3012735</v>
+        <v>3167470</v>
       </c>
       <c r="I90" t="n">
-        <v>44.379</v>
+        <v>46.659</v>
       </c>
       <c r="J90" t="n">
-        <v>72689</v>
+        <v>76608</v>
       </c>
       <c r="K90" t="n">
-        <v>1.071</v>
+        <v>1.128</v>
       </c>
       <c r="L90" t="n">
-        <v>65126</v>
+        <v>68551</v>
       </c>
       <c r="M90" t="n">
-        <v>0.959</v>
+        <v>1.01</v>
       </c>
       <c r="N90" t="s">
         <v>572</v>
@@ -7001,7 +6978,7 @@
         <v>580</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D91" t="s">
         <v>581</v>
@@ -7011,25 +6988,25 @@
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H91" t="n">
-        <v>18908412</v>
+        <v>19811243</v>
       </c>
       <c r="I91" t="n">
-        <v>57.125</v>
+        <v>59.852</v>
       </c>
       <c r="J91" t="n">
-        <v>1296287</v>
+        <v>428963</v>
       </c>
       <c r="K91" t="n">
-        <v>3.916</v>
+        <v>1.296</v>
       </c>
       <c r="L91" t="n">
-        <v>532075</v>
+        <v>504442</v>
       </c>
       <c r="M91" t="n">
-        <v>1.607</v>
+        <v>1.524</v>
       </c>
       <c r="N91" t="s">
         <v>582</v>
@@ -7052,7 +7029,7 @@
         <v>586</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D92" t="s">
         <v>587</v>
@@ -7062,25 +7039,25 @@
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H92" t="n">
-        <v>17757838</v>
+        <v>18680529</v>
       </c>
       <c r="I92" t="n">
-        <v>53.649</v>
+        <v>56.436</v>
       </c>
       <c r="J92" t="n">
-        <v>417156</v>
+        <v>465579</v>
       </c>
       <c r="K92" t="n">
-        <v>1.26</v>
+        <v>1.407</v>
       </c>
       <c r="L92" t="n">
-        <v>407257</v>
+        <v>439041</v>
       </c>
       <c r="M92" t="n">
-        <v>1.23</v>
+        <v>1.326</v>
       </c>
       <c r="N92" t="s">
         <v>588</v>
@@ -7103,7 +7080,7 @@
         <v>593</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D93" t="s">
         <v>594</v>
@@ -7113,25 +7090,25 @@
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H93" t="n">
-        <v>45226</v>
+        <v>46512</v>
       </c>
       <c r="I93" t="n">
-        <v>13.019</v>
+        <v>13.39</v>
       </c>
       <c r="J93" t="n">
-        <v>715</v>
+        <v>735</v>
       </c>
       <c r="K93" t="n">
-        <v>0.206</v>
+        <v>0.212</v>
       </c>
       <c r="L93" t="n">
-        <v>822</v>
+        <v>720</v>
       </c>
       <c r="M93" t="n">
-        <v>0.237</v>
+        <v>0.207</v>
       </c>
       <c r="N93" t="s">
         <v>124</v>
@@ -7201,7 +7178,7 @@
         <v>605</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>43984</v>
+        <v>43985</v>
       </c>
       <c r="D95" t="s">
         <v>606</v>
@@ -7211,25 +7188,25 @@
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H95" t="n">
-        <v>19290</v>
+        <v>20012</v>
       </c>
       <c r="I95" t="n">
-        <v>1.298</v>
+        <v>1.346</v>
       </c>
       <c r="J95" t="n">
-        <v>581</v>
+        <v>722</v>
       </c>
       <c r="K95" t="n">
-        <v>0.039</v>
+        <v>0.049</v>
       </c>
       <c r="L95" t="n">
-        <v>469</v>
+        <v>537</v>
       </c>
       <c r="M95" t="n">
-        <v>0.032</v>
+        <v>0.036</v>
       </c>
       <c r="N95" t="s">
         <v>607</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-06-07
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="609">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Argentina - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/05-06-20_reporte-matutino-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/06-06-20_reporte-matutino-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Argentina</t>
@@ -92,7 +92,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/06/coronavirus-covid-19-at-a-glance-4-june-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/06/coronavirus-covid-19-at-a-glance-5-june-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200605152528/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200607130312/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200605152532/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200607130314/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -280,7 +280,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200605152539/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200607130320/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -303,7 +303,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200604194851/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200607130321/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -391,7 +391,7 @@
     <t xml:space="preserve">Croatia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200605152550/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200607130325/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -454,7 +454,7 @@
     <t xml:space="preserve">Denmark - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200605121244/https://www.ssi.dk/sygdomme-beredskab-og-forskning/sygdomsovervaagning/c/covid19-overvaagning</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200606153440/https://www.ssi.dk/sygdomme-beredskab-og-forskning/sygdomsovervaagning/c/covid19-overvaagning</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -480,7 +480,7 @@
     <t xml:space="preserve">Ecuador - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-03062020-08h00.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-06062020-08h00.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -505,7 +505,7 @@
     <t xml:space="preserve">El Salvador - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/2947402875345884</t>
+    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/2951104881642350</t>
   </si>
   <si>
     <t xml:space="preserve">Government of El Salvador</t>
@@ -606,7 +606,8 @@
   </si>
   <si>
     <t xml:space="preserve">Since 29 May 2020, the National Public Health Agency has replaced its previous weekly updates of the number of tests performed (not updated since 5 May) with the weekly count of people tested.
-For the week between 18 May and 24 May, [the report](https://www.santepubliquefrance.fr/content/download/256362/2623085) states that 216,891 people were tested. This data does not allow us to publish any cumulative total, since no data is available on how many people had been tested prior to 18 May. However, we integrate this data into our "daily tests" time series by dividing 216,891 by 7 days, therefore estimating the daily number of people tested to be 30,984 on average for that week.</t>
+For the week between 18 May and 24 May, [the report](https://www.santepubliquefrance.fr/content/download/256362/2623085) states that 216,891 people were tested. This data does not allow us to publish any cumulative total, since no data is available on how many people had been tested prior to 18 May. However, we integrate this data into our "daily tests" time series by dividing 216,891 by 7 days, therefore estimating the daily number of people tested to be 30,984 on average for that week.
+The [4 June situation report](https://www.santepubliquefrance.fr/content/download/257630/2628879) reports 236,098 people were tested from 24 to 30 May. As the two periods overlap for 24 May, we use the more recent average testing figure for this date.</t>
   </si>
   <si>
     <t xml:space="preserve">France - tests performed</t>
@@ -842,7 +843,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200604180455/http://irangov.ir/detail/340321</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200606165255/http://irangov.ir/detail/340405</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -939,7 +940,7 @@
     <t xml:space="preserve">Japan - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11719.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11739.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -963,10 +964,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000637302.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release matches the cumulative total calculated from the weekly and daily figures reported by the MOH.</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000637521.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (510, 602) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000637521.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11th April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -998,7 +999,7 @@
     <t xml:space="preserve">Kenya - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1268563481235787776</t>
+    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1269290630947143686</t>
   </si>
   <si>
     <t xml:space="preserve">Kenya Ministry of Health</t>
@@ -1055,7 +1056,7 @@
     <t xml:space="preserve">Luxembourg - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200604195825/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200606200221/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg Government situation update</t>
@@ -1076,13 +1077,13 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/kementeriankesihatanmalaysia/videos/698657040921568</t>
+    <t xml:space="preserve">https://www.facebook.com/kementeriankesihatanmalaysia/videos/488938701905775</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
   </si>
   <si>
-    <t xml:space="preserve">Statistics on testing can be see at 20:04 timestamp on the MOH livestream</t>
+    <t xml:space="preserve">Statistics on testing can be see at 17:49 timestamp on the MOH livestream</t>
   </si>
   <si>
     <t xml:space="preserve">http://covid-19.moh.gov.my/terkini</t>
@@ -1172,9 +1173,6 @@
     <t xml:space="preserve">Myanmar Ministry of Health and Sports</t>
   </si>
   <si>
-    <t xml:space="preserve">This figure is taken from the interactive dashboard and should be updated once the daily PDF situation report becomes available</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://mohs.gov.mm/Home</t>
   </si>
   <si>
@@ -1211,10 +1209,10 @@
     <t xml:space="preserve">Netherlands - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-06/COVID-19_WebSite_rapport_dagelijks20200604_1141.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 4 June 2020 update</t>
+    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-06/COVID-19_WebSite_rapport_dagelijks20200606_1025.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 6 June 2020 update</t>
   </si>
   <si>
     <t xml:space="preserve">Dutch National Institute for Public Health and the Environment</t>
@@ -1250,7 +1248,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200605152829/https://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200606200626/https://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1295,7 +1293,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200605152835/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200607132318/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1348,7 +1346,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/177267-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-183-198-en-el-peru-comunicado-n-121</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/183570-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-191-758-en-el-peru-comunicado-n-123</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1381,8 +1379,7 @@
     <t xml:space="preserve">The Ministry of Health (MOH) provides a daily snapshot of testing capacity detailing the total number of individuals tested and the total number of tests conducted. 
 The total number of individuals tested is the sum of positive, negative, equivocal, and invalid individuals. No definitions of equivocal and invalid individual tests are given, hence our figures only report the sum of individuals who have tested positive or negative. From 22nd May, the DOH stopped reporting figures on equivocal and invalid individuals; the DOH provides the cumulative samples and unique indivdiuals tested, where cumulative unique individuals = cumulative positive + cumulative negative individuals. 
 The source provides a breakdown of both i) the number of individuals tested and ii) the total tests conducted, by laboratory. We are not aware of any aggregation issues. 
-The DOH used to report the number of cases tested in a previous dashboard, but stopped on 4th April. This previous breakdown of the test results and COVID-19 dashboard have both been removed. We became aware of this new tracker on the 13th April with data 'as of April 11 2020, 12am'. No previous snapshots of the dashboard are available using web archive, therefore the series starts from the 11th April - the earliest date from which we have access to the data.
-Latest data available until 3rd June, as of 5th June.</t>
+The DOH used to report the number of cases tested in a previous dashboard, but stopped on 4th April. This previous breakdown of the test results and COVID-19 dashboard have both been removed. We became aware of this new tracker on the 13th April with data 'as of April 11 2020, 12am'. No previous snapshots of the dashboard are available using web archive, therefore the series starts from the 11th April - the earliest date from which we have access to the data.</t>
   </si>
   <si>
     <t xml:space="preserve">POL</t>
@@ -1455,7 +1452,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-5-iunie-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-7-iunie-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1473,7 +1470,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14623</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14634</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1493,7 +1490,7 @@
     <t xml:space="preserve">Rwanda - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1268258423898062851</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1269000782919204866</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1600,7 +1597,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200605152917/https://korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200606200638/https://korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Center of Health Information and the Office of the Government of the Slovak Republic</t>
@@ -1674,7 +1671,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367442&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367452&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1757,7 +1754,7 @@
     <t xml:space="preserve">Taiwan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/q_oVMUUh-Gn4ERMn-c5ZnA?typeid=9</t>
+    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/VcdAAClvchXYx-IH8Z2VIg?typeid=9</t>
   </si>
   <si>
     <t xml:space="preserve">Taiwan Centers for Disease Control (CDC)</t>
@@ -1780,7 +1777,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200605153210/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200606200720/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1850,7 +1847,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200604200117/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200606200724/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1874,13 +1871,13 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1268822086115635200</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1269298040814424066</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
   </si>
   <si>
-    <t xml:space="preserve">The MOH did not release daily test figures for 3rd June. The cumulative total for 4th June thus takes the total figure as of the 2nd June and the daily tests conducted on the 4th June.</t>
+    <t xml:space="preserve">We sum the cumulative total provided for the previous day with the daily number of samples tested today.</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.health.go.ug/moh/resources/</t>
@@ -1898,7 +1895,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200605153218/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200607132414/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1935,7 +1932,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/890451/2020-06-05_COVID-19_UK_testing_time_series.csv</t>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/890549/COVID-19_UK_testing_time_series_6_June.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Sum of pillar 1 + pillar 2 (tests processed only)</t>
@@ -1956,7 +1953,7 @@
     <t xml:space="preserve">United States - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200605153221/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200606200727/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
   </si>
   <si>
     <t xml:space="preserve">United States CDC</t>
@@ -2010,7 +2007,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-44</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-46</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2049,7 +2046,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1268307496801898499</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1269065905201459200</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -2459,7 +2456,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>43987</v>
+        <v>43988</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2469,25 +2466,25 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H2" t="n">
-        <v>183862</v>
+        <v>189278</v>
       </c>
       <c r="I2" t="n">
-        <v>4.068</v>
+        <v>4.188</v>
       </c>
       <c r="J2" t="n">
-        <v>5414</v>
+        <v>5416</v>
       </c>
       <c r="K2" t="n">
         <v>0.12</v>
       </c>
       <c r="L2" t="n">
-        <v>4768</v>
+        <v>4857</v>
       </c>
       <c r="M2" t="n">
-        <v>0.105</v>
+        <v>0.107</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -2510,7 +2507,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>43986</v>
+        <v>43987</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2520,25 +2517,25 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H3" t="n">
-        <v>1546329</v>
+        <v>1579192</v>
       </c>
       <c r="I3" t="n">
-        <v>60.641</v>
+        <v>61.929</v>
       </c>
       <c r="J3" t="n">
-        <v>33629</v>
+        <v>32863</v>
       </c>
       <c r="K3" t="n">
-        <v>1.319</v>
+        <v>1.289</v>
       </c>
       <c r="L3" t="n">
-        <v>25555</v>
+        <v>25939</v>
       </c>
       <c r="M3" t="n">
-        <v>1.002</v>
+        <v>1.017</v>
       </c>
       <c r="N3" t="s">
         <v>27</v>
@@ -2561,7 +2558,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>43987</v>
+        <v>43989</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -2571,25 +2568,25 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H4" t="n">
-        <v>479449</v>
+        <v>489597</v>
       </c>
       <c r="I4" t="n">
-        <v>53.234</v>
+        <v>54.361</v>
       </c>
       <c r="J4" t="n">
-        <v>7983</v>
+        <v>3685</v>
       </c>
       <c r="K4" t="n">
-        <v>0.886</v>
+        <v>0.409</v>
       </c>
       <c r="L4" t="n">
-        <v>6450</v>
+        <v>5866</v>
       </c>
       <c r="M4" t="n">
-        <v>0.716</v>
+        <v>0.651</v>
       </c>
       <c r="N4" t="s">
         <v>34</v>
@@ -2612,7 +2609,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>43987</v>
+        <v>43989</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2622,25 +2619,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H5" t="n">
-        <v>350907</v>
+        <v>367056</v>
       </c>
       <c r="I5" t="n">
-        <v>206.224</v>
+        <v>215.714</v>
       </c>
       <c r="J5" t="n">
-        <v>5570</v>
+        <v>5680</v>
       </c>
       <c r="K5" t="n">
-        <v>3.273</v>
+        <v>3.338</v>
       </c>
       <c r="L5" t="n">
-        <v>6675</v>
+        <v>7178</v>
       </c>
       <c r="M5" t="n">
-        <v>3.923</v>
+        <v>4.218</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
@@ -2663,7 +2660,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>43986</v>
+        <v>43988</v>
       </c>
       <c r="D6" t="s">
         <v>48</v>
@@ -2673,25 +2670,25 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H6" t="n">
-        <v>358277</v>
+        <v>384851</v>
       </c>
       <c r="I6" t="n">
-        <v>2.175</v>
+        <v>2.337</v>
       </c>
       <c r="J6" t="n">
-        <v>12694</v>
+        <v>12486</v>
       </c>
       <c r="K6" t="n">
-        <v>0.077</v>
+        <v>0.076</v>
       </c>
       <c r="L6" t="n">
-        <v>11786</v>
+        <v>12542</v>
       </c>
       <c r="M6" t="n">
-        <v>0.072</v>
+        <v>0.076</v>
       </c>
       <c r="N6" t="s">
         <v>49</v>
@@ -2765,7 +2762,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
@@ -2775,25 +2772,25 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H8" t="n">
-        <v>724596</v>
+        <v>741468</v>
       </c>
       <c r="I8" t="n">
-        <v>62.521</v>
+        <v>63.977</v>
       </c>
       <c r="J8" t="n">
-        <v>8233</v>
+        <v>7383</v>
       </c>
       <c r="K8" t="n">
-        <v>0.71</v>
+        <v>0.637</v>
       </c>
       <c r="L8" t="n">
-        <v>7219</v>
+        <v>6883</v>
       </c>
       <c r="M8" t="n">
-        <v>0.623</v>
+        <v>0.594</v>
       </c>
       <c r="N8" t="s">
         <v>62</v>
@@ -2916,7 +2913,7 @@
         <v>81</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>43987</v>
+        <v>43989</v>
       </c>
       <c r="D11" t="s">
         <v>82</v>
@@ -2926,25 +2923,25 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H11" t="n">
-        <v>87890</v>
+        <v>89902</v>
       </c>
       <c r="I11" t="n">
-        <v>12.649</v>
+        <v>12.938</v>
       </c>
       <c r="J11" t="n">
-        <v>2060</v>
+        <v>816</v>
       </c>
       <c r="K11" t="n">
-        <v>0.296</v>
+        <v>0.117</v>
       </c>
       <c r="L11" t="n">
-        <v>1214</v>
+        <v>1222</v>
       </c>
       <c r="M11" t="n">
-        <v>0.175</v>
+        <v>0.176</v>
       </c>
       <c r="N11" t="s">
         <v>84</v>
@@ -2967,7 +2964,7 @@
         <v>88</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>43986</v>
+        <v>43989</v>
       </c>
       <c r="D12" t="s">
         <v>89</v>
@@ -2977,25 +2974,25 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H12" t="n">
-        <v>1787370</v>
+        <v>1868201</v>
       </c>
       <c r="I12" t="n">
-        <v>47.357</v>
+        <v>49.499</v>
       </c>
       <c r="J12" t="n">
-        <v>35823</v>
+        <v>37779</v>
       </c>
       <c r="K12" t="n">
-        <v>0.949</v>
+        <v>1.001</v>
       </c>
       <c r="L12" t="n">
-        <v>32595</v>
+        <v>29308</v>
       </c>
       <c r="M12" t="n">
-        <v>0.864</v>
+        <v>0.777</v>
       </c>
       <c r="N12" t="s">
         <v>90</v>
@@ -3018,7 +3015,7 @@
         <v>95</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>43986</v>
+        <v>43988</v>
       </c>
       <c r="D13" t="s">
         <v>96</v>
@@ -3030,25 +3027,25 @@
         <v>97</v>
       </c>
       <c r="G13" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H13" t="n">
-        <v>646458</v>
+        <v>687510</v>
       </c>
       <c r="I13" t="n">
-        <v>33.817</v>
+        <v>35.965</v>
       </c>
       <c r="J13" t="n">
-        <v>18140</v>
+        <v>18954</v>
       </c>
       <c r="K13" t="n">
-        <v>0.949</v>
+        <v>0.992</v>
       </c>
       <c r="L13" t="n">
-        <v>16612</v>
+        <v>17741</v>
       </c>
       <c r="M13" t="n">
-        <v>0.869</v>
+        <v>0.928</v>
       </c>
       <c r="N13" t="s">
         <v>98</v>
@@ -3071,7 +3068,7 @@
         <v>102</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>43986</v>
+        <v>43988</v>
       </c>
       <c r="D14" t="s">
         <v>103</v>
@@ -3081,25 +3078,25 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H14" t="n">
-        <v>374592</v>
+        <v>399505</v>
       </c>
       <c r="I14" t="n">
-        <v>7.362</v>
+        <v>7.851</v>
       </c>
       <c r="J14" t="n">
-        <v>12160</v>
+        <v>12567</v>
       </c>
       <c r="K14" t="n">
-        <v>0.239</v>
+        <v>0.247</v>
       </c>
       <c r="L14" t="n">
-        <v>11283</v>
+        <v>11389</v>
       </c>
       <c r="M14" t="n">
-        <v>0.222</v>
+        <v>0.224</v>
       </c>
       <c r="N14" t="s">
         <v>104</v>
@@ -3122,7 +3119,7 @@
         <v>109</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>43986</v>
+        <v>43988</v>
       </c>
       <c r="D15" t="s">
         <v>110</v>
@@ -3132,25 +3129,25 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H15" t="n">
-        <v>20498</v>
+        <v>21275</v>
       </c>
       <c r="I15" t="n">
-        <v>4.024</v>
+        <v>4.176</v>
       </c>
       <c r="J15" t="n">
-        <v>376</v>
+        <v>334</v>
       </c>
       <c r="K15" t="n">
-        <v>0.074</v>
+        <v>0.066</v>
       </c>
       <c r="L15" t="n">
-        <v>406</v>
+        <v>373</v>
       </c>
       <c r="M15" t="n">
-        <v>0.08</v>
+        <v>0.073</v>
       </c>
       <c r="N15" t="s">
         <v>111</v>
@@ -3173,7 +3170,7 @@
         <v>115</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>43987</v>
+        <v>43989</v>
       </c>
       <c r="D16" t="s">
         <v>116</v>
@@ -3183,25 +3180,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H16" t="n">
-        <v>68267</v>
+        <v>68740</v>
       </c>
       <c r="I16" t="n">
-        <v>16.629</v>
+        <v>16.744</v>
       </c>
       <c r="J16" t="n">
-        <v>270</v>
+        <v>226</v>
       </c>
       <c r="K16" t="n">
-        <v>0.066</v>
+        <v>0.055</v>
       </c>
       <c r="L16" t="n">
-        <v>394</v>
+        <v>334</v>
       </c>
       <c r="M16" t="n">
-        <v>0.096</v>
+        <v>0.081</v>
       </c>
       <c r="N16" t="s">
         <v>117</v>
@@ -3224,7 +3221,7 @@
         <v>122</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>43986</v>
+        <v>43987</v>
       </c>
       <c r="D17" t="s">
         <v>123</v>
@@ -3236,22 +3233,22 @@
         <v>125</v>
       </c>
       <c r="G17" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H17" t="n">
-        <v>114464</v>
+        <v>116468</v>
       </c>
       <c r="I17" t="n">
-        <v>10.106</v>
+        <v>10.283</v>
       </c>
       <c r="J17" t="n">
-        <v>2015</v>
+        <v>2004</v>
       </c>
       <c r="K17" t="n">
-        <v>0.178</v>
+        <v>0.177</v>
       </c>
       <c r="L17" t="n">
-        <v>1908</v>
+        <v>1906</v>
       </c>
       <c r="M17" t="n">
         <v>0.168</v>
@@ -3277,7 +3274,7 @@
         <v>130</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>43986</v>
+        <v>43988</v>
       </c>
       <c r="D18" t="s">
         <v>131</v>
@@ -3287,25 +3284,25 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H18" t="n">
-        <v>464499</v>
+        <v>471521</v>
       </c>
       <c r="I18" t="n">
-        <v>43.375</v>
+        <v>44.03</v>
       </c>
       <c r="J18" t="n">
-        <v>4537</v>
+        <v>2000</v>
       </c>
       <c r="K18" t="n">
-        <v>0.424</v>
+        <v>0.187</v>
       </c>
       <c r="L18" t="n">
-        <v>4763</v>
+        <v>4316</v>
       </c>
       <c r="M18" t="n">
-        <v>0.445</v>
+        <v>0.403</v>
       </c>
       <c r="N18" t="s">
         <v>41</v>
@@ -3328,7 +3325,7 @@
         <v>135</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>43987</v>
+        <v>43988</v>
       </c>
       <c r="D19" t="s">
         <v>136</v>
@@ -3338,25 +3335,25 @@
       </c>
       <c r="F19"/>
       <c r="G19" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H19" t="n">
-        <v>562905</v>
+        <v>571832</v>
       </c>
       <c r="I19" t="n">
-        <v>97.183</v>
+        <v>98.724</v>
       </c>
       <c r="J19" t="n">
-        <v>10017</v>
+        <v>8927</v>
       </c>
       <c r="K19" t="n">
-        <v>1.729</v>
+        <v>1.541</v>
       </c>
       <c r="L19" t="n">
-        <v>8337</v>
+        <v>8195</v>
       </c>
       <c r="M19" t="n">
-        <v>1.439</v>
+        <v>1.415</v>
       </c>
       <c r="N19" t="s">
         <v>138</v>
@@ -3379,7 +3376,7 @@
         <v>142</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>43985</v>
+        <v>43988</v>
       </c>
       <c r="D20" t="s">
         <v>143</v>
@@ -3391,21 +3388,21 @@
         <v>145</v>
       </c>
       <c r="G20" t="n">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H20" t="n">
-        <v>74728</v>
+        <v>79123</v>
       </c>
       <c r="I20" t="n">
-        <v>4.236</v>
+        <v>4.485</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20" t="n">
-        <v>1195</v>
+        <v>1556</v>
       </c>
       <c r="M20" t="n">
-        <v>0.068</v>
+        <v>0.088</v>
       </c>
       <c r="N20" t="s">
         <v>144</v>
@@ -3428,7 +3425,7 @@
         <v>149</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>43985</v>
+        <v>43986</v>
       </c>
       <c r="D21" t="s">
         <v>150</v>
@@ -3438,22 +3435,22 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H21" t="n">
-        <v>99178</v>
+        <v>101604</v>
       </c>
       <c r="I21" t="n">
-        <v>15.291</v>
+        <v>15.665</v>
       </c>
       <c r="J21" t="n">
-        <v>2531</v>
+        <v>2426</v>
       </c>
       <c r="K21" t="n">
-        <v>0.39</v>
+        <v>0.374</v>
       </c>
       <c r="L21" t="n">
-        <v>2419</v>
+        <v>2422</v>
       </c>
       <c r="M21" t="n">
         <v>0.373</v>
@@ -3479,7 +3476,7 @@
         <v>155</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>43986</v>
+        <v>43988</v>
       </c>
       <c r="D22" t="s">
         <v>156</v>
@@ -3489,25 +3486,25 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H22" t="n">
-        <v>88570</v>
+        <v>90070</v>
       </c>
       <c r="I22" t="n">
-        <v>66.768</v>
+        <v>67.898</v>
       </c>
       <c r="J22" t="n">
-        <v>1122</v>
+        <v>654</v>
       </c>
       <c r="K22" t="n">
-        <v>0.846</v>
+        <v>0.493</v>
       </c>
       <c r="L22" t="n">
-        <v>980</v>
+        <v>948</v>
       </c>
       <c r="M22" t="n">
-        <v>0.739</v>
+        <v>0.715</v>
       </c>
       <c r="N22" t="s">
         <v>158</v>
@@ -3577,7 +3574,7 @@
         <v>169</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>43984</v>
+        <v>43988</v>
       </c>
       <c r="D24" t="s">
         <v>170</v>
@@ -3587,25 +3584,25 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="H24" t="n">
-        <v>194722</v>
+        <v>201077</v>
       </c>
       <c r="I24" t="n">
-        <v>35.144</v>
+        <v>36.291</v>
       </c>
       <c r="J24" t="n">
-        <v>2231</v>
+        <v>408</v>
       </c>
       <c r="K24" t="n">
-        <v>0.403</v>
+        <v>0.074</v>
       </c>
       <c r="L24" t="n">
-        <v>2177</v>
+        <v>1606</v>
       </c>
       <c r="M24" t="n">
-        <v>0.393</v>
+        <v>0.29</v>
       </c>
       <c r="N24" t="s">
         <v>172</v>
@@ -3828,7 +3825,7 @@
         <v>202</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>43984</v>
+        <v>43986</v>
       </c>
       <c r="D29" t="s">
         <v>195</v>
@@ -3840,25 +3837,25 @@
         <v>203</v>
       </c>
       <c r="G29" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H29" t="n">
-        <v>223065</v>
+        <v>229093</v>
       </c>
       <c r="I29" t="n">
-        <v>7.179</v>
+        <v>7.373</v>
       </c>
       <c r="J29" t="n">
-        <v>2912</v>
+        <v>2352</v>
       </c>
       <c r="K29" t="n">
-        <v>0.094</v>
+        <v>0.076</v>
       </c>
       <c r="L29" t="n">
-        <v>2454</v>
+        <v>2496</v>
       </c>
       <c r="M29" t="n">
-        <v>0.079</v>
+        <v>0.08</v>
       </c>
       <c r="N29" t="s">
         <v>198</v>
@@ -3979,7 +3976,7 @@
         <v>219</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>43987</v>
+        <v>43988</v>
       </c>
       <c r="D32" t="s">
         <v>220</v>
@@ -3991,25 +3988,25 @@
         <v>222</v>
       </c>
       <c r="G32" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H32" t="n">
-        <v>202606</v>
+        <v>206853</v>
       </c>
       <c r="I32" t="n">
-        <v>20.973</v>
+        <v>21.413</v>
       </c>
       <c r="J32" t="n">
-        <v>6712</v>
+        <v>4247</v>
       </c>
       <c r="K32" t="n">
-        <v>0.695</v>
+        <v>0.44</v>
       </c>
       <c r="L32" t="n">
-        <v>3208</v>
+        <v>3327</v>
       </c>
       <c r="M32" t="n">
-        <v>0.332</v>
+        <v>0.344</v>
       </c>
       <c r="N32" t="s">
         <v>221</v>
@@ -4032,7 +4029,7 @@
         <v>227</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>43986</v>
+        <v>43987</v>
       </c>
       <c r="D33" t="s">
         <v>228</v>
@@ -4042,25 +4039,25 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H33" t="n">
-        <v>62189</v>
+        <v>62727</v>
       </c>
       <c r="I33" t="n">
-        <v>182.239</v>
+        <v>183.815</v>
       </c>
       <c r="J33" t="n">
-        <v>550</v>
+        <v>538</v>
       </c>
       <c r="K33" t="n">
-        <v>1.612</v>
+        <v>1.577</v>
       </c>
       <c r="L33" t="n">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="M33" t="n">
-        <v>0.727</v>
+        <v>0.73</v>
       </c>
       <c r="N33" t="s">
         <v>229</v>
@@ -4136,7 +4133,7 @@
         <v>238</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>43987</v>
+        <v>43989</v>
       </c>
       <c r="D35" t="s">
         <v>234</v>
@@ -4148,25 +4145,25 @@
         <v>236</v>
       </c>
       <c r="G35" t="n">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H35" t="n">
-        <v>4386379</v>
+        <v>4666386</v>
       </c>
       <c r="I35" t="n">
-        <v>3.179</v>
+        <v>3.381</v>
       </c>
       <c r="J35" t="n">
-        <v>143661</v>
+        <v>142069</v>
       </c>
       <c r="K35" t="n">
-        <v>0.104</v>
+        <v>0.103</v>
       </c>
       <c r="L35" t="n">
-        <v>128934</v>
+        <v>132766</v>
       </c>
       <c r="M35" t="n">
-        <v>0.093</v>
+        <v>0.096</v>
       </c>
       <c r="N35" t="s">
         <v>235</v>
@@ -4189,7 +4186,7 @@
         <v>240</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>43987</v>
+        <v>43989</v>
       </c>
       <c r="D36" t="s">
         <v>241</v>
@@ -4199,25 +4196,25 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H36" t="n">
-        <v>256810</v>
+        <v>269146</v>
       </c>
       <c r="I36" t="n">
-        <v>0.939</v>
+        <v>0.984</v>
       </c>
       <c r="J36" t="n">
-        <v>5074</v>
+        <v>4406</v>
       </c>
       <c r="K36" t="n">
-        <v>0.019</v>
+        <v>0.016</v>
       </c>
       <c r="L36" t="n">
-        <v>7366</v>
+        <v>6503</v>
       </c>
       <c r="M36" t="n">
-        <v>0.027</v>
+        <v>0.024</v>
       </c>
       <c r="N36" t="s">
         <v>242</v>
@@ -4240,7 +4237,7 @@
         <v>247</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>43986</v>
+        <v>43988</v>
       </c>
       <c r="D37" t="s">
         <v>248</v>
@@ -4250,25 +4247,25 @@
       </c>
       <c r="F37"/>
       <c r="G37" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H37" t="n">
-        <v>1019362</v>
+        <v>1060126</v>
       </c>
       <c r="I37" t="n">
-        <v>12.136</v>
+        <v>12.622</v>
       </c>
       <c r="J37" t="n">
-        <v>22353</v>
+        <v>19837</v>
       </c>
       <c r="K37" t="n">
-        <v>0.266</v>
+        <v>0.236</v>
       </c>
       <c r="L37" t="n">
-        <v>20400</v>
+        <v>20590</v>
       </c>
       <c r="M37" t="n">
-        <v>0.243</v>
+        <v>0.245</v>
       </c>
       <c r="N37" t="s">
         <v>249</v>
@@ -4389,7 +4386,7 @@
         <v>265</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>43986</v>
+        <v>43988</v>
       </c>
       <c r="D40" t="s">
         <v>266</v>
@@ -4401,25 +4398,25 @@
         <v>268</v>
       </c>
       <c r="G40" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H40" t="n">
-        <v>2524788</v>
+        <v>2599294</v>
       </c>
       <c r="I40" t="n">
-        <v>41.758</v>
+        <v>42.991</v>
       </c>
       <c r="J40" t="n">
-        <v>27451</v>
+        <v>34036</v>
       </c>
       <c r="K40" t="n">
-        <v>0.454</v>
+        <v>0.563</v>
       </c>
       <c r="L40" t="n">
-        <v>27771</v>
+        <v>27803</v>
       </c>
       <c r="M40" t="n">
-        <v>0.459</v>
+        <v>0.46</v>
       </c>
       <c r="N40" t="s">
         <v>269</v>
@@ -4442,7 +4439,7 @@
         <v>272</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>43986</v>
+        <v>43988</v>
       </c>
       <c r="D41" t="s">
         <v>266</v>
@@ -4454,25 +4451,25 @@
         <v>268</v>
       </c>
       <c r="G41" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H41" t="n">
-        <v>4049544</v>
+        <v>4187057</v>
       </c>
       <c r="I41" t="n">
-        <v>66.977</v>
+        <v>69.251</v>
       </c>
       <c r="J41" t="n">
-        <v>49953</v>
+        <v>72485</v>
       </c>
       <c r="K41" t="n">
-        <v>0.826</v>
+        <v>1.199</v>
       </c>
       <c r="L41" t="n">
-        <v>52343</v>
+        <v>51777</v>
       </c>
       <c r="M41" t="n">
-        <v>0.866</v>
+        <v>0.856</v>
       </c>
       <c r="N41" t="s">
         <v>269</v>
@@ -4495,7 +4492,7 @@
         <v>275</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>43987</v>
+        <v>43989</v>
       </c>
       <c r="D42" t="s">
         <v>276</v>
@@ -4507,21 +4504,21 @@
         <v>278</v>
       </c>
       <c r="G42" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H42" t="n">
-        <v>307462</v>
+        <v>314483</v>
       </c>
       <c r="I42" t="n">
-        <v>2.431</v>
+        <v>2.486</v>
       </c>
       <c r="J42"/>
       <c r="K42"/>
       <c r="L42" t="n">
-        <v>3243</v>
+        <v>3435</v>
       </c>
       <c r="M42" t="n">
-        <v>0.026</v>
+        <v>0.027</v>
       </c>
       <c r="N42" t="s">
         <v>279</v>
@@ -4544,7 +4541,7 @@
         <v>282</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>43985</v>
+        <v>43986</v>
       </c>
       <c r="D43" t="s">
         <v>283</v>
@@ -4556,25 +4553,25 @@
         <v>284</v>
       </c>
       <c r="G43" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H43" t="n">
-        <v>504964</v>
+        <v>510520</v>
       </c>
       <c r="I43" t="n">
-        <v>3.993</v>
+        <v>4.036</v>
       </c>
       <c r="J43" t="n">
-        <v>6999</v>
+        <v>5556</v>
       </c>
       <c r="K43" t="n">
-        <v>0.055</v>
+        <v>0.044</v>
       </c>
       <c r="L43" t="n">
-        <v>5584</v>
+        <v>5496</v>
       </c>
       <c r="M43" t="n">
-        <v>0.044</v>
+        <v>0.043</v>
       </c>
       <c r="N43" t="s">
         <v>279</v>
@@ -4597,7 +4594,7 @@
         <v>287</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>43985</v>
+        <v>43988</v>
       </c>
       <c r="D44" t="s">
         <v>288</v>
@@ -4607,25 +4604,25 @@
       </c>
       <c r="F44"/>
       <c r="G44" t="n">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H44" t="n">
-        <v>867286</v>
+        <v>942576</v>
       </c>
       <c r="I44" t="n">
-        <v>46.189</v>
+        <v>50.199</v>
       </c>
       <c r="J44" t="n">
-        <v>23660</v>
+        <v>26672</v>
       </c>
       <c r="K44" t="n">
-        <v>1.26</v>
+        <v>1.42</v>
       </c>
       <c r="L44" t="n">
-        <v>22419</v>
+        <v>22041</v>
       </c>
       <c r="M44" t="n">
-        <v>1.194</v>
+        <v>1.174</v>
       </c>
       <c r="N44" t="s">
         <v>289</v>
@@ -4648,7 +4645,7 @@
         <v>292</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>43986</v>
+        <v>43988</v>
       </c>
       <c r="D45" t="s">
         <v>293</v>
@@ -4658,25 +4655,25 @@
       </c>
       <c r="F45"/>
       <c r="G45" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H45" t="n">
-        <v>87698</v>
+        <v>94507</v>
       </c>
       <c r="I45" t="n">
-        <v>1.631</v>
+        <v>1.758</v>
       </c>
       <c r="J45" t="n">
-        <v>2640</v>
+        <v>3632</v>
       </c>
       <c r="K45" t="n">
-        <v>0.049</v>
+        <v>0.068</v>
       </c>
       <c r="L45" t="n">
-        <v>2504</v>
+        <v>2605</v>
       </c>
       <c r="M45" t="n">
-        <v>0.047</v>
+        <v>0.048</v>
       </c>
       <c r="N45" t="s">
         <v>41</v>
@@ -4699,7 +4696,7 @@
         <v>299</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>43987</v>
+        <v>43989</v>
       </c>
       <c r="D46" t="s">
         <v>300</v>
@@ -4711,25 +4708,25 @@
         <v>302</v>
       </c>
       <c r="G46" t="n">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H46" t="n">
-        <v>115461</v>
+        <v>117660</v>
       </c>
       <c r="I46" t="n">
-        <v>61.213</v>
+        <v>62.379</v>
       </c>
       <c r="J46" t="n">
-        <v>1010</v>
+        <v>1125</v>
       </c>
       <c r="K46" t="n">
-        <v>0.535</v>
+        <v>0.596</v>
       </c>
       <c r="L46" t="n">
-        <v>1219</v>
+        <v>1227</v>
       </c>
       <c r="M46" t="n">
-        <v>0.646</v>
+        <v>0.651</v>
       </c>
       <c r="N46" t="s">
         <v>301</v>
@@ -4803,7 +4800,7 @@
         <v>310</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>43986</v>
+        <v>43988</v>
       </c>
       <c r="D48" t="s">
         <v>311</v>
@@ -4813,25 +4810,25 @@
       </c>
       <c r="F48"/>
       <c r="G48" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H48" t="n">
-        <v>82377</v>
+        <v>84934</v>
       </c>
       <c r="I48" t="n">
-        <v>131.598</v>
+        <v>135.683</v>
       </c>
       <c r="J48" t="n">
-        <v>2893</v>
+        <v>1261</v>
       </c>
       <c r="K48" t="n">
-        <v>4.622</v>
+        <v>2.014</v>
       </c>
       <c r="L48" t="n">
-        <v>1611</v>
+        <v>1510</v>
       </c>
       <c r="M48" t="n">
-        <v>2.574</v>
+        <v>2.412</v>
       </c>
       <c r="N48" t="s">
         <v>312</v>
@@ -4854,7 +4851,7 @@
         <v>316</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>43987</v>
+        <v>43988</v>
       </c>
       <c r="D49" t="s">
         <v>317</v>
@@ -4866,25 +4863,25 @@
         <v>319</v>
       </c>
       <c r="G49" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H49" t="n">
-        <v>590613</v>
+        <v>599454</v>
       </c>
       <c r="I49" t="n">
-        <v>18.248</v>
+        <v>18.521</v>
       </c>
       <c r="J49" t="n">
-        <v>8127</v>
+        <v>8841</v>
       </c>
       <c r="K49" t="n">
-        <v>0.251</v>
+        <v>0.273</v>
       </c>
       <c r="L49" t="n">
-        <v>7531</v>
+        <v>7584</v>
       </c>
       <c r="M49" t="n">
-        <v>0.233</v>
+        <v>0.234</v>
       </c>
       <c r="N49" t="s">
         <v>41</v>
@@ -4960,7 +4957,7 @@
         <v>331</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>43985</v>
+        <v>43987</v>
       </c>
       <c r="D51" t="s">
         <v>332</v>
@@ -4970,22 +4967,22 @@
       </c>
       <c r="F51"/>
       <c r="G51" t="n">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H51" t="n">
-        <v>267389</v>
+        <v>284046</v>
       </c>
       <c r="I51" t="n">
-        <v>2.074</v>
+        <v>2.203</v>
       </c>
       <c r="J51" t="n">
-        <v>526</v>
+        <v>285</v>
       </c>
       <c r="K51" t="n">
-        <v>0.004</v>
+        <v>0.002</v>
       </c>
       <c r="L51" t="n">
-        <v>3674</v>
+        <v>3651</v>
       </c>
       <c r="M51" t="n">
         <v>0.028</v>
@@ -5064,7 +5061,7 @@
         <v>343</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>43986</v>
+        <v>43987</v>
       </c>
       <c r="D53" t="s">
         <v>344</v>
@@ -5072,260 +5069,262 @@
       <c r="E53" t="s">
         <v>345</v>
       </c>
-      <c r="F53" t="s">
-        <v>346</v>
-      </c>
+      <c r="F53"/>
       <c r="G53" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H53" t="n">
-        <v>31701</v>
+        <v>35432</v>
       </c>
       <c r="I53" t="n">
-        <v>0.583</v>
-      </c>
-      <c r="J53"/>
-      <c r="K53"/>
+        <v>0.651</v>
+      </c>
+      <c r="J53" t="n">
+        <v>1845</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.034</v>
+      </c>
       <c r="L53" t="n">
-        <v>1173</v>
+        <v>1574</v>
       </c>
       <c r="M53" t="n">
-        <v>0.022</v>
+        <v>0.029</v>
       </c>
       <c r="N53" t="s">
         <v>345</v>
       </c>
       <c r="O53" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P53" t="s">
         <v>51</v>
       </c>
       <c r="Q53" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
+        <v>348</v>
+      </c>
+      <c r="B54" t="s">
         <v>349</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" s="1" t="n">
+        <v>43988</v>
+      </c>
+      <c r="D54" t="s">
         <v>350</v>
       </c>
-      <c r="C54" s="1" t="n">
-        <v>43986</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>351</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>352</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="n">
+        <v>107</v>
+      </c>
+      <c r="H54" t="n">
+        <v>92477</v>
+      </c>
+      <c r="I54" t="n">
+        <v>3.174</v>
+      </c>
+      <c r="J54" t="n">
+        <v>4111</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="L54" t="n">
+        <v>3678</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0.126</v>
+      </c>
+      <c r="N54" t="s">
+        <v>351</v>
+      </c>
+      <c r="O54" t="s">
         <v>353</v>
-      </c>
-      <c r="G54" t="n">
-        <v>105</v>
-      </c>
-      <c r="H54" t="n">
-        <v>84134</v>
-      </c>
-      <c r="I54" t="n">
-        <v>2.888</v>
-      </c>
-      <c r="J54" t="n">
-        <v>3867</v>
-      </c>
-      <c r="K54" t="n">
-        <v>0.133</v>
-      </c>
-      <c r="L54" t="n">
-        <v>3317</v>
-      </c>
-      <c r="M54" t="n">
-        <v>0.114</v>
-      </c>
-      <c r="N54" t="s">
-        <v>352</v>
-      </c>
-      <c r="O54" t="s">
-        <v>354</v>
       </c>
       <c r="P54" t="s">
         <v>92</v>
       </c>
       <c r="Q54" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
+        <v>355</v>
+      </c>
+      <c r="B55" t="s">
         <v>356</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" s="1" t="n">
+        <v>43986</v>
+      </c>
+      <c r="D55" t="s">
         <v>357</v>
       </c>
-      <c r="C55" s="1" t="n">
-        <v>43985</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>358</v>
-      </c>
-      <c r="E55" t="s">
-        <v>359</v>
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H55" t="n">
-        <v>378912</v>
+        <v>391624</v>
       </c>
       <c r="I55" t="n">
-        <v>22.113</v>
+        <v>22.855</v>
       </c>
       <c r="J55" t="n">
-        <v>8394</v>
+        <v>9855</v>
       </c>
       <c r="K55" t="n">
-        <v>0.49</v>
+        <v>0.575</v>
       </c>
       <c r="L55" t="n">
-        <v>5188</v>
+        <v>6294</v>
       </c>
       <c r="M55" t="n">
-        <v>0.303</v>
+        <v>0.367</v>
       </c>
       <c r="N55" t="s">
+        <v>359</v>
+      </c>
+      <c r="O55" t="s">
         <v>360</v>
-      </c>
-      <c r="O55" t="s">
-        <v>361</v>
       </c>
       <c r="P55" t="s">
         <v>92</v>
       </c>
       <c r="Q55" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>362</v>
+      </c>
+      <c r="B56" t="s">
         <v>363</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" s="1" t="n">
+        <v>43988</v>
+      </c>
+      <c r="D56" t="s">
         <v>364</v>
-      </c>
-      <c r="C56" s="1" t="n">
-        <v>43986</v>
-      </c>
-      <c r="D56" t="s">
-        <v>365</v>
       </c>
       <c r="E56" t="s">
         <v>41</v>
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H56" t="n">
-        <v>288987</v>
+        <v>294048</v>
       </c>
       <c r="I56" t="n">
-        <v>59.928</v>
+        <v>60.978</v>
       </c>
       <c r="J56" t="n">
-        <v>2813</v>
+        <v>2054</v>
       </c>
       <c r="K56" t="n">
-        <v>0.583</v>
+        <v>0.426</v>
       </c>
       <c r="L56" t="n">
-        <v>1876</v>
+        <v>1866</v>
       </c>
       <c r="M56" t="n">
-        <v>0.389</v>
+        <v>0.387</v>
       </c>
       <c r="N56" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="O56" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="P56" t="s">
         <v>22</v>
       </c>
       <c r="Q56" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
+        <v>367</v>
+      </c>
+      <c r="B57" t="s">
         <v>368</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" s="1" t="n">
+        <v>43988</v>
+      </c>
+      <c r="D57" t="s">
         <v>369</v>
       </c>
-      <c r="C57" s="1" t="n">
-        <v>43987</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>370</v>
-      </c>
-      <c r="E57" t="s">
-        <v>371</v>
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H57" t="n">
-        <v>73064</v>
+        <v>74999</v>
       </c>
       <c r="I57" t="n">
-        <v>0.354</v>
+        <v>0.364</v>
       </c>
       <c r="J57" t="n">
-        <v>1728</v>
+        <v>1935</v>
       </c>
       <c r="K57" t="n">
-        <v>0.008</v>
+        <v>0.009</v>
       </c>
       <c r="L57" t="n">
-        <v>2048</v>
+        <v>2025</v>
       </c>
       <c r="M57" t="n">
         <v>0.01</v>
       </c>
       <c r="N57" t="s">
+        <v>370</v>
+      </c>
+      <c r="O57" t="s">
         <v>371</v>
-      </c>
-      <c r="O57" t="s">
-        <v>372</v>
       </c>
       <c r="P57" t="s">
         <v>51</v>
       </c>
       <c r="Q57" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
+        <v>373</v>
+      </c>
+      <c r="B58" t="s">
         <v>374</v>
-      </c>
-      <c r="B58" t="s">
-        <v>375</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>43987</v>
       </c>
       <c r="D58" t="s">
+        <v>375</v>
+      </c>
+      <c r="E58" t="s">
         <v>376</v>
-      </c>
-      <c r="E58" t="s">
-        <v>377</v>
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
@@ -5350,84 +5349,84 @@
         <v>0.315</v>
       </c>
       <c r="N58" t="s">
+        <v>376</v>
+      </c>
+      <c r="O58" t="s">
         <v>377</v>
       </c>
-      <c r="O58" t="s">
+      <c r="P58" t="s">
         <v>378</v>
       </c>
-      <c r="P58" t="s">
+      <c r="Q58" t="s">
         <v>379</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
+        <v>380</v>
+      </c>
+      <c r="B59" t="s">
         <v>381</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" s="1" t="n">
+        <v>43989</v>
+      </c>
+      <c r="D59" t="s">
         <v>382</v>
       </c>
-      <c r="C59" s="1" t="n">
-        <v>43987</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>383</v>
-      </c>
-      <c r="E59" t="s">
-        <v>384</v>
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H59" t="n">
-        <v>638323</v>
+        <v>683608</v>
       </c>
       <c r="I59" t="n">
-        <v>2.89</v>
+        <v>3.095</v>
       </c>
       <c r="J59" t="n">
-        <v>22812</v>
+        <v>23100</v>
       </c>
       <c r="K59" t="n">
-        <v>0.103</v>
+        <v>0.105</v>
       </c>
       <c r="L59" t="n">
-        <v>16901</v>
+        <v>19511</v>
       </c>
       <c r="M59" t="n">
-        <v>0.077</v>
+        <v>0.088</v>
       </c>
       <c r="N59" t="s">
+        <v>383</v>
+      </c>
+      <c r="O59" t="s">
         <v>384</v>
-      </c>
-      <c r="O59" t="s">
-        <v>385</v>
       </c>
       <c r="P59" t="s">
         <v>22</v>
       </c>
       <c r="Q59" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
+        <v>386</v>
+      </c>
+      <c r="B60" t="s">
         <v>387</v>
-      </c>
-      <c r="B60" t="s">
-        <v>388</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>43986</v>
       </c>
       <c r="D60" t="s">
+        <v>388</v>
+      </c>
+      <c r="E60" t="s">
         <v>389</v>
-      </c>
-      <c r="E60" t="s">
-        <v>390</v>
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
@@ -5452,183 +5451,191 @@
         <v>0.307</v>
       </c>
       <c r="N60" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="O60" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P60" t="s">
         <v>22</v>
       </c>
       <c r="Q60" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
+        <v>391</v>
+      </c>
+      <c r="B61" t="s">
         <v>392</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" s="1" t="n">
+        <v>43987</v>
+      </c>
+      <c r="D61" t="s">
         <v>393</v>
       </c>
-      <c r="C61" s="1" t="n">
-        <v>43986</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>394</v>
-      </c>
-      <c r="E61" t="s">
-        <v>395</v>
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H61" t="n">
-        <v>34240</v>
+        <v>35258</v>
       </c>
       <c r="I61" t="n">
-        <v>4.801</v>
+        <v>4.943</v>
       </c>
       <c r="J61" t="n">
-        <v>1159</v>
+        <v>1018</v>
       </c>
       <c r="K61" t="n">
-        <v>0.162</v>
+        <v>0.143</v>
       </c>
       <c r="L61" t="n">
-        <v>974</v>
+        <v>989</v>
       </c>
       <c r="M61" t="n">
-        <v>0.137</v>
+        <v>0.139</v>
       </c>
       <c r="N61" t="s">
+        <v>394</v>
+      </c>
+      <c r="O61" t="s">
         <v>395</v>
-      </c>
-      <c r="O61" t="s">
-        <v>396</v>
       </c>
       <c r="P61" t="s">
         <v>51</v>
       </c>
       <c r="Q61" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
+        <v>397</v>
+      </c>
+      <c r="B62" t="s">
         <v>398</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" s="1" t="n">
+        <v>43988</v>
+      </c>
+      <c r="D62" t="s">
         <v>399</v>
-      </c>
-      <c r="C62" s="1" t="n">
-        <v>43987</v>
-      </c>
-      <c r="D62" t="s">
-        <v>400</v>
       </c>
       <c r="E62" t="s">
         <v>41</v>
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H62" t="n">
-        <v>153773</v>
+        <v>159169</v>
       </c>
       <c r="I62" t="n">
-        <v>4.664</v>
-      </c>
-      <c r="J62"/>
-      <c r="K62"/>
+        <v>4.827</v>
+      </c>
+      <c r="J62" t="n">
+        <v>5396</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0.164</v>
+      </c>
       <c r="L62" t="n">
-        <v>2847</v>
+        <v>3087</v>
       </c>
       <c r="M62" t="n">
-        <v>0.086</v>
+        <v>0.094</v>
       </c>
       <c r="N62" t="s">
+        <v>400</v>
+      </c>
+      <c r="O62" t="s">
         <v>401</v>
-      </c>
-      <c r="O62" t="s">
-        <v>402</v>
       </c>
       <c r="P62" t="s">
         <v>92</v>
       </c>
       <c r="Q62" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
+        <v>403</v>
+      </c>
+      <c r="B63" t="s">
         <v>404</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" s="1" t="n">
+        <v>43987</v>
+      </c>
+      <c r="D63" t="s">
         <v>405</v>
       </c>
-      <c r="C63" s="1" t="n">
-        <v>43985</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>406</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>407</v>
       </c>
-      <c r="F63" t="s">
-        <v>408</v>
-      </c>
       <c r="G63" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H63" t="n">
-        <v>357351</v>
+        <v>386726</v>
       </c>
       <c r="I63" t="n">
-        <v>3.261</v>
-      </c>
-      <c r="J63"/>
-      <c r="K63"/>
+        <v>3.529</v>
+      </c>
+      <c r="J63" t="n">
+        <v>10385</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.095</v>
+      </c>
       <c r="L63" t="n">
-        <v>8561</v>
+        <v>10603</v>
       </c>
       <c r="M63" t="n">
-        <v>0.078</v>
+        <v>0.097</v>
       </c>
       <c r="N63" t="s">
         <v>214</v>
       </c>
       <c r="O63" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="P63" t="s">
         <v>92</v>
       </c>
       <c r="Q63" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
+        <v>409</v>
+      </c>
+      <c r="B64" t="s">
         <v>410</v>
-      </c>
-      <c r="B64" t="s">
-        <v>411</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>43985</v>
       </c>
       <c r="D64" t="s">
+        <v>411</v>
+      </c>
+      <c r="E64" t="s">
         <v>412</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>413</v>
-      </c>
-      <c r="F64" t="s">
-        <v>414</v>
       </c>
       <c r="G64" t="n">
         <v>91</v>
@@ -5652,30 +5659,30 @@
         <v>0.538</v>
       </c>
       <c r="N64" t="s">
+        <v>414</v>
+      </c>
+      <c r="O64" t="s">
         <v>415</v>
-      </c>
-      <c r="O64" t="s">
-        <v>416</v>
       </c>
       <c r="P64" t="s">
         <v>51</v>
       </c>
       <c r="Q64" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
+        <v>417</v>
+      </c>
+      <c r="B65" t="s">
         <v>418</v>
-      </c>
-      <c r="B65" t="s">
-        <v>419</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>43984</v>
       </c>
       <c r="D65" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E65" t="s">
         <v>41</v>
@@ -5703,391 +5710,391 @@
         <v>1.332</v>
       </c>
       <c r="N65" t="s">
+        <v>420</v>
+      </c>
+      <c r="O65" t="s">
+        <v>419</v>
+      </c>
+      <c r="P65" t="s">
         <v>421</v>
       </c>
-      <c r="O65" t="s">
-        <v>420</v>
-      </c>
-      <c r="P65" t="s">
+      <c r="Q65" t="s">
         <v>422</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
+        <v>423</v>
+      </c>
+      <c r="B66" t="s">
         <v>424</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" s="1" t="n">
+        <v>43988</v>
+      </c>
+      <c r="D66" t="s">
         <v>425</v>
       </c>
-      <c r="C66" s="1" t="n">
-        <v>43987</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>426</v>
-      </c>
-      <c r="E66" t="s">
-        <v>427</v>
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H66" t="n">
-        <v>246362</v>
+        <v>251391</v>
       </c>
       <c r="I66" t="n">
-        <v>85.511</v>
+        <v>87.256</v>
       </c>
       <c r="J66" t="n">
-        <v>5276</v>
+        <v>5029</v>
       </c>
       <c r="K66" t="n">
-        <v>1.831</v>
+        <v>1.746</v>
       </c>
       <c r="L66" t="n">
-        <v>4781</v>
+        <v>4772</v>
       </c>
       <c r="M66" t="n">
-        <v>1.659</v>
+        <v>1.656</v>
       </c>
       <c r="N66" t="s">
+        <v>426</v>
+      </c>
+      <c r="O66" t="s">
         <v>427</v>
-      </c>
-      <c r="O66" t="s">
-        <v>428</v>
       </c>
       <c r="P66" t="s">
         <v>92</v>
       </c>
       <c r="Q66" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
+        <v>429</v>
+      </c>
+      <c r="B67" t="s">
         <v>430</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" s="1" t="n">
+        <v>43989</v>
+      </c>
+      <c r="D67" t="s">
         <v>431</v>
       </c>
-      <c r="C67" s="1" t="n">
-        <v>43987</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>432</v>
-      </c>
-      <c r="E67" t="s">
-        <v>433</v>
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H67" t="n">
-        <v>484782</v>
+        <v>503200</v>
       </c>
       <c r="I67" t="n">
-        <v>25.2</v>
+        <v>26.157</v>
       </c>
       <c r="J67" t="n">
-        <v>11932</v>
+        <v>6792</v>
       </c>
       <c r="K67" t="n">
-        <v>0.62</v>
+        <v>0.353</v>
       </c>
       <c r="L67" t="n">
-        <v>9047</v>
+        <v>9143</v>
       </c>
       <c r="M67" t="n">
-        <v>0.47</v>
+        <v>0.475</v>
       </c>
       <c r="N67" t="s">
+        <v>432</v>
+      </c>
+      <c r="O67" t="s">
         <v>433</v>
-      </c>
-      <c r="O67" t="s">
-        <v>434</v>
       </c>
       <c r="P67" t="s">
         <v>22</v>
       </c>
       <c r="Q67" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
+        <v>435</v>
+      </c>
+      <c r="B68" t="s">
         <v>436</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" s="1" t="n">
+        <v>43989</v>
+      </c>
+      <c r="D68" t="s">
         <v>437</v>
       </c>
-      <c r="C68" s="1" t="n">
-        <v>43987</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>438</v>
-      </c>
-      <c r="E68" t="s">
-        <v>439</v>
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H68" t="n">
-        <v>12053663</v>
+        <v>12721549</v>
       </c>
       <c r="I68" t="n">
-        <v>82.596</v>
+        <v>87.173</v>
       </c>
       <c r="J68" t="n">
-        <v>320612</v>
+        <v>332581</v>
       </c>
       <c r="K68" t="n">
-        <v>2.197</v>
+        <v>2.279</v>
       </c>
       <c r="L68" t="n">
-        <v>293372</v>
+        <v>296918</v>
       </c>
       <c r="M68" t="n">
-        <v>2.01</v>
+        <v>2.035</v>
       </c>
       <c r="N68" t="s">
+        <v>438</v>
+      </c>
+      <c r="O68" t="s">
         <v>439</v>
-      </c>
-      <c r="O68" t="s">
-        <v>440</v>
       </c>
       <c r="P68" t="s">
         <v>22</v>
       </c>
       <c r="Q68" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
+        <v>441</v>
+      </c>
+      <c r="B69" t="s">
         <v>442</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" s="1" t="n">
+        <v>43987</v>
+      </c>
+      <c r="D69" t="s">
         <v>443</v>
       </c>
-      <c r="C69" s="1" t="n">
-        <v>43985</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>444</v>
-      </c>
-      <c r="E69" t="s">
-        <v>445</v>
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H69" t="n">
-        <v>71141</v>
+        <v>74068</v>
       </c>
       <c r="I69" t="n">
-        <v>5.493</v>
+        <v>5.719</v>
       </c>
       <c r="J69" t="n">
-        <v>1033</v>
+        <v>1558</v>
       </c>
       <c r="K69" t="n">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="L69" t="n">
-        <v>1234</v>
+        <v>1209</v>
       </c>
       <c r="M69" t="n">
-        <v>0.095</v>
+        <v>0.093</v>
       </c>
       <c r="N69" t="s">
+        <v>444</v>
+      </c>
+      <c r="O69" t="s">
         <v>445</v>
-      </c>
-      <c r="O69" t="s">
-        <v>446</v>
       </c>
       <c r="P69" t="s">
         <v>51</v>
       </c>
       <c r="Q69" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
+        <v>447</v>
+      </c>
+      <c r="B70" t="s">
         <v>448</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" s="1" t="n">
+        <v>43988</v>
+      </c>
+      <c r="D70" t="s">
         <v>449</v>
-      </c>
-      <c r="C70" s="1" t="n">
-        <v>43986</v>
-      </c>
-      <c r="D70" t="s">
-        <v>450</v>
       </c>
       <c r="E70" t="s">
         <v>41</v>
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H70" t="n">
-        <v>887209</v>
+        <v>933201</v>
       </c>
       <c r="I70" t="n">
-        <v>25.484</v>
+        <v>26.805</v>
       </c>
       <c r="J70" t="n">
-        <v>16246</v>
+        <v>24229</v>
       </c>
       <c r="K70" t="n">
-        <v>0.467</v>
+        <v>0.696</v>
       </c>
       <c r="L70" t="n">
-        <v>16645</v>
+        <v>18090</v>
       </c>
       <c r="M70" t="n">
-        <v>0.478</v>
+        <v>0.52</v>
       </c>
       <c r="N70" t="s">
         <v>41</v>
       </c>
       <c r="O70" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="P70" t="s">
         <v>127</v>
       </c>
       <c r="Q70" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
+        <v>451</v>
+      </c>
+      <c r="B71" t="s">
         <v>452</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" s="1" t="n">
+        <v>43988</v>
+      </c>
+      <c r="D71" t="s">
         <v>453</v>
       </c>
-      <c r="C71" s="1" t="n">
-        <v>43987</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>454</v>
       </c>
-      <c r="E71" t="s">
+      <c r="F71" t="s">
         <v>455</v>
       </c>
-      <c r="F71" t="s">
+      <c r="G71" t="n">
+        <v>96</v>
+      </c>
+      <c r="H71" t="n">
+        <v>51856</v>
+      </c>
+      <c r="I71" t="n">
+        <v>3.097</v>
+      </c>
+      <c r="J71" t="n">
+        <v>1166</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="L71" t="n">
+        <v>1420</v>
+      </c>
+      <c r="M71" t="n">
+        <v>0.085</v>
+      </c>
+      <c r="N71" t="s">
         <v>456</v>
       </c>
-      <c r="G71" t="n">
-        <v>95</v>
-      </c>
-      <c r="H71" t="n">
-        <v>50690</v>
-      </c>
-      <c r="I71" t="n">
-        <v>3.027</v>
-      </c>
-      <c r="J71" t="n">
-        <v>1700</v>
-      </c>
-      <c r="K71" t="n">
-        <v>0.102</v>
-      </c>
-      <c r="L71" t="n">
-        <v>1449</v>
-      </c>
-      <c r="M71" t="n">
-        <v>0.087</v>
-      </c>
-      <c r="N71" t="s">
+      <c r="O71" t="s">
         <v>457</v>
       </c>
-      <c r="O71" t="s">
+      <c r="P71" t="s">
         <v>458</v>
       </c>
-      <c r="P71" t="s">
+      <c r="Q71" t="s">
         <v>459</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
+        <v>460</v>
+      </c>
+      <c r="B72" t="s">
         <v>461</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" s="1" t="n">
+        <v>43988</v>
+      </c>
+      <c r="D72" t="s">
         <v>462</v>
-      </c>
-      <c r="C72" s="1" t="n">
-        <v>43986</v>
-      </c>
-      <c r="D72" t="s">
-        <v>463</v>
       </c>
       <c r="E72" t="s">
         <v>41</v>
       </c>
       <c r="F72" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G72" t="n">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H72" t="n">
-        <v>261266</v>
+        <v>269185</v>
       </c>
       <c r="I72" t="n">
-        <v>38.396</v>
+        <v>39.559</v>
       </c>
       <c r="J72" t="n">
-        <v>4024</v>
+        <v>3124</v>
       </c>
       <c r="K72" t="n">
-        <v>0.591</v>
+        <v>0.459</v>
       </c>
       <c r="L72" t="n">
-        <v>3892</v>
+        <v>3772</v>
       </c>
       <c r="M72" t="n">
-        <v>0.572</v>
+        <v>0.554</v>
       </c>
       <c r="N72" t="s">
         <v>41</v>
       </c>
       <c r="O72" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="P72" t="s">
         <v>92</v>
       </c>
       <c r="Q72" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
+        <v>466</v>
+      </c>
+      <c r="B73" t="s">
         <v>467</v>
-      </c>
-      <c r="B73" t="s">
-        <v>468</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>43983</v>
       </c>
       <c r="D73" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E73" t="s">
         <v>41</v>
@@ -6114,27 +6121,27 @@
         <v>41</v>
       </c>
       <c r="O73" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="P73" t="s">
         <v>92</v>
       </c>
       <c r="Q73" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B74" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>43983</v>
       </c>
       <c r="D74" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E74" t="s">
         <v>41</v>
@@ -6161,236 +6168,236 @@
         <v>41</v>
       </c>
       <c r="O74" t="s">
+        <v>469</v>
+      </c>
+      <c r="P74" t="s">
+        <v>473</v>
+      </c>
+      <c r="Q74" t="s">
         <v>470</v>
-      </c>
-      <c r="P74" t="s">
-        <v>474</v>
-      </c>
-      <c r="Q74" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
+        <v>474</v>
+      </c>
+      <c r="B75" t="s">
         <v>475</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" s="1" t="n">
+        <v>43988</v>
+      </c>
+      <c r="D75" t="s">
         <v>476</v>
       </c>
-      <c r="C75" s="1" t="n">
-        <v>43987</v>
-      </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>477</v>
-      </c>
-      <c r="E75" t="s">
-        <v>478</v>
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H75" t="n">
-        <v>185596</v>
+        <v>188235</v>
       </c>
       <c r="I75" t="n">
-        <v>33.994</v>
+        <v>34.478</v>
       </c>
       <c r="J75" t="n">
-        <v>1832</v>
+        <v>2639</v>
       </c>
       <c r="K75" t="n">
-        <v>0.336</v>
+        <v>0.483</v>
       </c>
       <c r="L75" t="n">
-        <v>2576</v>
+        <v>2463</v>
       </c>
       <c r="M75" t="n">
-        <v>0.472</v>
+        <v>0.451</v>
       </c>
       <c r="N75" t="s">
+        <v>478</v>
+      </c>
+      <c r="O75" t="s">
         <v>479</v>
       </c>
-      <c r="O75" t="s">
+      <c r="P75" t="s">
         <v>480</v>
       </c>
-      <c r="P75" t="s">
+      <c r="Q75" t="s">
         <v>481</v>
-      </c>
-      <c r="Q75" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
+        <v>482</v>
+      </c>
+      <c r="B76" t="s">
         <v>483</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" s="1" t="n">
+        <v>43987</v>
+      </c>
+      <c r="D76" t="s">
         <v>484</v>
       </c>
-      <c r="C76" s="1" t="n">
-        <v>43986</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>485</v>
-      </c>
-      <c r="E76" t="s">
-        <v>486</v>
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H76" t="n">
-        <v>82161</v>
+        <v>82876</v>
       </c>
       <c r="I76" t="n">
-        <v>39.521</v>
+        <v>39.865</v>
       </c>
       <c r="J76" t="n">
-        <v>828</v>
+        <v>715</v>
       </c>
       <c r="K76" t="n">
-        <v>0.398</v>
+        <v>0.344</v>
       </c>
       <c r="L76" t="n">
-        <v>606</v>
+        <v>621</v>
       </c>
       <c r="M76" t="n">
-        <v>0.291</v>
+        <v>0.299</v>
       </c>
       <c r="N76" t="s">
+        <v>486</v>
+      </c>
+      <c r="O76" t="s">
         <v>487</v>
-      </c>
-      <c r="O76" t="s">
-        <v>488</v>
       </c>
       <c r="P76" t="s">
         <v>22</v>
       </c>
       <c r="Q76" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
+        <v>489</v>
+      </c>
+      <c r="B77" t="s">
         <v>490</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" s="1" t="n">
+        <v>43988</v>
+      </c>
+      <c r="D77" t="s">
         <v>491</v>
       </c>
-      <c r="C77" s="1" t="n">
-        <v>43986</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>492</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
         <v>493</v>
       </c>
-      <c r="F77" t="s">
+      <c r="G77" t="n">
+        <v>98</v>
+      </c>
+      <c r="H77" t="n">
+        <v>891668</v>
+      </c>
+      <c r="I77" t="n">
+        <v>15.034</v>
+      </c>
+      <c r="J77" t="n">
+        <v>40797</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0.688</v>
+      </c>
+      <c r="L77" t="n">
+        <v>27112</v>
+      </c>
+      <c r="M77" t="n">
+        <v>0.457</v>
+      </c>
+      <c r="N77" t="s">
+        <v>492</v>
+      </c>
+      <c r="O77" t="s">
         <v>494</v>
-      </c>
-      <c r="G77" t="n">
-        <v>96</v>
-      </c>
-      <c r="H77" t="n">
-        <v>820675</v>
-      </c>
-      <c r="I77" t="n">
-        <v>13.837</v>
-      </c>
-      <c r="J77" t="n">
-        <v>34696</v>
-      </c>
-      <c r="K77" t="n">
-        <v>0.585</v>
-      </c>
-      <c r="L77" t="n">
-        <v>23565</v>
-      </c>
-      <c r="M77" t="n">
-        <v>0.397</v>
-      </c>
-      <c r="N77" t="s">
-        <v>493</v>
-      </c>
-      <c r="O77" t="s">
-        <v>495</v>
       </c>
       <c r="P77" t="s">
         <v>92</v>
       </c>
       <c r="Q77" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
+        <v>496</v>
+      </c>
+      <c r="B78" t="s">
         <v>497</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" s="1" t="n">
+        <v>43989</v>
+      </c>
+      <c r="D78" t="s">
         <v>498</v>
       </c>
-      <c r="C78" s="1" t="n">
-        <v>43987</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>499</v>
-      </c>
-      <c r="E78" t="s">
-        <v>500</v>
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H78" t="n">
-        <v>990960</v>
+        <v>1012769</v>
       </c>
       <c r="I78" t="n">
-        <v>19.329</v>
+        <v>19.754</v>
       </c>
       <c r="J78" t="n">
-        <v>17102</v>
+        <v>7464</v>
       </c>
       <c r="K78" t="n">
-        <v>0.334</v>
+        <v>0.146</v>
       </c>
       <c r="L78" t="n">
-        <v>15120</v>
+        <v>14564</v>
       </c>
       <c r="M78" t="n">
-        <v>0.295</v>
+        <v>0.284</v>
       </c>
       <c r="N78" t="s">
+        <v>499</v>
+      </c>
+      <c r="O78" t="s">
         <v>500</v>
-      </c>
-      <c r="O78" t="s">
-        <v>501</v>
       </c>
       <c r="P78" t="s">
         <v>244</v>
       </c>
       <c r="Q78" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
+        <v>502</v>
+      </c>
+      <c r="B79" t="s">
         <v>503</v>
-      </c>
-      <c r="B79" t="s">
-        <v>504</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>43979</v>
       </c>
       <c r="D79" t="s">
+        <v>504</v>
+      </c>
+      <c r="E79" t="s">
         <v>505</v>
-      </c>
-      <c r="E79" t="s">
-        <v>506</v>
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
@@ -6411,33 +6418,33 @@
         <v>0.962</v>
       </c>
       <c r="N79" t="s">
+        <v>506</v>
+      </c>
+      <c r="O79" t="s">
         <v>507</v>
-      </c>
-      <c r="O79" t="s">
-        <v>508</v>
       </c>
       <c r="P79" t="s">
         <v>22</v>
       </c>
       <c r="Q79" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
+        <v>509</v>
+      </c>
+      <c r="B80" t="s">
         <v>510</v>
-      </c>
-      <c r="B80" t="s">
-        <v>511</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>43982</v>
       </c>
       <c r="D80" t="s">
+        <v>511</v>
+      </c>
+      <c r="E80" t="s">
         <v>512</v>
-      </c>
-      <c r="E80" t="s">
-        <v>513</v>
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
@@ -6458,185 +6465,189 @@
         <v>0.516</v>
       </c>
       <c r="N80" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="O80" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="P80" t="s">
         <v>92</v>
       </c>
       <c r="Q80" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
+        <v>514</v>
+      </c>
+      <c r="B81" t="s">
         <v>515</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" s="1" t="n">
+        <v>43988</v>
+      </c>
+      <c r="D81" t="s">
         <v>516</v>
       </c>
-      <c r="C81" s="1" t="n">
-        <v>43986</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>517</v>
-      </c>
-      <c r="E81" t="s">
-        <v>518</v>
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="H81" t="n">
-        <v>415190</v>
+        <v>423468</v>
       </c>
       <c r="I81" t="n">
-        <v>47.973</v>
+        <v>48.93</v>
       </c>
       <c r="J81" t="n">
-        <v>4259</v>
+        <v>2530</v>
       </c>
       <c r="K81" t="n">
-        <v>0.492</v>
+        <v>0.292</v>
       </c>
       <c r="L81" t="n">
-        <v>3332</v>
+        <v>3607</v>
       </c>
       <c r="M81" t="n">
-        <v>0.385</v>
+        <v>0.417</v>
       </c>
       <c r="N81" t="s">
+        <v>517</v>
+      </c>
+      <c r="O81" t="s">
+        <v>516</v>
+      </c>
+      <c r="P81" t="s">
         <v>518</v>
       </c>
-      <c r="O81" t="s">
-        <v>517</v>
-      </c>
-      <c r="P81" t="s">
+      <c r="Q81" t="s">
         <v>519</v>
-      </c>
-      <c r="Q81" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
+        <v>520</v>
+      </c>
+      <c r="B82" t="s">
         <v>521</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" s="1" t="n">
+        <v>43988</v>
+      </c>
+      <c r="D82" t="s">
         <v>522</v>
       </c>
-      <c r="C82" s="1" t="n">
-        <v>43986</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>523</v>
-      </c>
-      <c r="E82" t="s">
-        <v>524</v>
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H82" t="n">
-        <v>73040</v>
+        <v>73359</v>
       </c>
       <c r="I82" t="n">
-        <v>3.067</v>
+        <v>3.08</v>
       </c>
       <c r="J82" t="n">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="K82" t="n">
-        <v>0.007</v>
+        <v>0.006</v>
       </c>
       <c r="L82" t="n">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M82" t="n">
         <v>0.008</v>
       </c>
       <c r="N82" t="s">
+        <v>523</v>
+      </c>
+      <c r="O82" t="s">
         <v>524</v>
       </c>
-      <c r="O82" t="s">
+      <c r="P82" t="s">
         <v>525</v>
       </c>
-      <c r="P82" t="s">
+      <c r="Q82" t="s">
         <v>526</v>
-      </c>
-      <c r="Q82" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
+        <v>527</v>
+      </c>
+      <c r="B83" t="s">
         <v>528</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" s="1" t="n">
+        <v>43988</v>
+      </c>
+      <c r="D83" t="s">
         <v>529</v>
       </c>
-      <c r="C83" s="1" t="n">
-        <v>43987</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>530</v>
-      </c>
-      <c r="E83" t="s">
-        <v>531</v>
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H83" t="n">
-        <v>224386</v>
+        <v>228349</v>
       </c>
       <c r="I83" t="n">
-        <v>3.215</v>
-      </c>
-      <c r="J83"/>
-      <c r="K83"/>
+        <v>3.271</v>
+      </c>
+      <c r="J83" t="n">
+        <v>3963</v>
+      </c>
+      <c r="K83" t="n">
+        <v>0.057</v>
+      </c>
       <c r="L83" t="n">
-        <v>5234</v>
+        <v>5204</v>
       </c>
       <c r="M83" t="n">
         <v>0.075</v>
       </c>
       <c r="N83" t="s">
+        <v>531</v>
+      </c>
+      <c r="O83" t="s">
         <v>532</v>
-      </c>
-      <c r="O83" t="s">
-        <v>533</v>
       </c>
       <c r="P83" t="s">
         <v>92</v>
       </c>
       <c r="Q83" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B84" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C84" s="1" t="n">
         <v>43983</v>
       </c>
       <c r="D84" t="s">
+        <v>535</v>
+      </c>
+      <c r="E84" t="s">
         <v>536</v>
       </c>
-      <c r="E84" t="s">
+      <c r="F84" t="s">
         <v>537</v>
-      </c>
-      <c r="F84" t="s">
-        <v>538</v>
       </c>
       <c r="G84" t="n">
         <v>9</v>
@@ -6656,33 +6667,33 @@
         <v>0.064</v>
       </c>
       <c r="N84" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="O84" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="P84" t="s">
         <v>51</v>
       </c>
       <c r="Q84" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
+        <v>540</v>
+      </c>
+      <c r="B85" t="s">
         <v>541</v>
-      </c>
-      <c r="B85" t="s">
-        <v>542</v>
       </c>
       <c r="C85" s="1" t="n">
         <v>43983</v>
       </c>
       <c r="D85" t="s">
+        <v>542</v>
+      </c>
+      <c r="E85" t="s">
         <v>543</v>
-      </c>
-      <c r="E85" t="s">
-        <v>544</v>
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
@@ -6703,184 +6714,188 @@
         <v>0.049</v>
       </c>
       <c r="N85" t="s">
+        <v>543</v>
+      </c>
+      <c r="O85" t="s">
         <v>544</v>
       </c>
-      <c r="O85" t="s">
+      <c r="P85" t="s">
         <v>545</v>
       </c>
-      <c r="P85" t="s">
+      <c r="Q85" t="s">
         <v>546</v>
-      </c>
-      <c r="Q85" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
+        <v>547</v>
+      </c>
+      <c r="B86" t="s">
         <v>548</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" s="1" t="n">
+        <v>43988</v>
+      </c>
+      <c r="D86" t="s">
         <v>549</v>
       </c>
-      <c r="C86" s="1" t="n">
-        <v>43986</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="E86" t="s">
         <v>550</v>
-      </c>
-      <c r="E86" t="s">
-        <v>551</v>
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H86" t="n">
-        <v>2209583</v>
+        <v>2303258</v>
       </c>
       <c r="I86" t="n">
-        <v>26.199</v>
+        <v>27.31</v>
       </c>
       <c r="J86" t="n">
-        <v>54234</v>
+        <v>35846</v>
       </c>
       <c r="K86" t="n">
-        <v>0.643</v>
+        <v>0.425</v>
       </c>
       <c r="L86" t="n">
-        <v>40196</v>
+        <v>42809</v>
       </c>
       <c r="M86" t="n">
-        <v>0.477</v>
+        <v>0.508</v>
       </c>
       <c r="N86" t="s">
+        <v>550</v>
+      </c>
+      <c r="O86" t="s">
         <v>551</v>
       </c>
-      <c r="O86" t="s">
+      <c r="P86" t="s">
         <v>552</v>
       </c>
-      <c r="P86" t="s">
+      <c r="Q86" t="s">
         <v>553</v>
-      </c>
-      <c r="Q86" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
+        <v>554</v>
+      </c>
+      <c r="B87" t="s">
         <v>555</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" s="1" t="n">
+        <v>43987</v>
+      </c>
+      <c r="D87" t="s">
         <v>556</v>
       </c>
-      <c r="C87" s="1" t="n">
-        <v>43986</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
         <v>557</v>
       </c>
-      <c r="E87" t="s">
+      <c r="F87" t="s">
         <v>558</v>
       </c>
-      <c r="F87" t="s">
+      <c r="G87" t="n">
+        <v>58</v>
+      </c>
+      <c r="H87" t="n">
+        <v>104090</v>
+      </c>
+      <c r="I87" t="n">
+        <v>2.276</v>
+      </c>
+      <c r="J87" t="n">
+        <v>1310</v>
+      </c>
+      <c r="K87" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="L87" t="n">
+        <v>1434</v>
+      </c>
+      <c r="M87" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="N87" t="s">
+        <v>557</v>
+      </c>
+      <c r="O87" t="s">
         <v>559</v>
-      </c>
-      <c r="G87" t="n">
-        <v>57</v>
-      </c>
-      <c r="H87" t="n">
-        <v>102780</v>
-      </c>
-      <c r="I87" t="n">
-        <v>2.247</v>
-      </c>
-      <c r="J87"/>
-      <c r="K87"/>
-      <c r="L87" t="n">
-        <v>1522</v>
-      </c>
-      <c r="M87" t="n">
-        <v>0.033</v>
-      </c>
-      <c r="N87" t="s">
-        <v>558</v>
-      </c>
-      <c r="O87" t="s">
-        <v>560</v>
       </c>
       <c r="P87" t="s">
         <v>51</v>
       </c>
       <c r="Q87" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
+        <v>561</v>
+      </c>
+      <c r="B88" t="s">
         <v>562</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" s="1" t="n">
+        <v>43989</v>
+      </c>
+      <c r="D88" t="s">
         <v>563</v>
       </c>
-      <c r="C88" s="1" t="n">
-        <v>43987</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
         <v>564</v>
-      </c>
-      <c r="E88" t="s">
-        <v>565</v>
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H88" t="n">
-        <v>403551</v>
+        <v>424046</v>
       </c>
       <c r="I88" t="n">
-        <v>9.227</v>
+        <v>9.696</v>
       </c>
       <c r="J88" t="n">
-        <v>11235</v>
+        <v>9504</v>
       </c>
       <c r="K88" t="n">
-        <v>0.257</v>
+        <v>0.217</v>
       </c>
       <c r="L88" t="n">
-        <v>9462</v>
+        <v>10259</v>
       </c>
       <c r="M88" t="n">
-        <v>0.216</v>
+        <v>0.235</v>
       </c>
       <c r="N88" t="s">
+        <v>564</v>
+      </c>
+      <c r="O88" t="s">
         <v>565</v>
       </c>
-      <c r="O88" t="s">
+      <c r="P88" t="s">
         <v>566</v>
       </c>
-      <c r="P88" t="s">
+      <c r="Q88" t="s">
         <v>567</v>
-      </c>
-      <c r="Q88" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
+        <v>568</v>
+      </c>
+      <c r="B89" t="s">
         <v>569</v>
-      </c>
-      <c r="B89" t="s">
-        <v>570</v>
       </c>
       <c r="C89" s="1" t="n">
         <v>43973</v>
       </c>
       <c r="D89" t="s">
+        <v>570</v>
+      </c>
+      <c r="E89" t="s">
         <v>571</v>
-      </c>
-      <c r="E89" t="s">
-        <v>572</v>
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
@@ -6905,239 +6920,239 @@
         <v>1.012</v>
       </c>
       <c r="N89" t="s">
+        <v>571</v>
+      </c>
+      <c r="O89" t="s">
         <v>572</v>
-      </c>
-      <c r="O89" t="s">
-        <v>573</v>
       </c>
       <c r="P89" t="s">
         <v>92</v>
       </c>
       <c r="Q89" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B90" t="s">
+        <v>574</v>
+      </c>
+      <c r="C90" s="1" t="n">
+        <v>43987</v>
+      </c>
+      <c r="D90" t="s">
         <v>575</v>
       </c>
-      <c r="C90" s="1" t="n">
-        <v>43986</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
+        <v>571</v>
+      </c>
+      <c r="F90" t="s">
         <v>576</v>
       </c>
-      <c r="E90" t="s">
+      <c r="G90" t="n">
+        <v>41</v>
+      </c>
+      <c r="H90" t="n">
+        <v>3250401</v>
+      </c>
+      <c r="I90" t="n">
+        <v>47.88</v>
+      </c>
+      <c r="J90" t="n">
+        <v>82389</v>
+      </c>
+      <c r="K90" t="n">
+        <v>1.214</v>
+      </c>
+      <c r="L90" t="n">
+        <v>69249</v>
+      </c>
+      <c r="M90" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="N90" t="s">
+        <v>571</v>
+      </c>
+      <c r="O90" t="s">
         <v>572</v>
-      </c>
-      <c r="F90" t="s">
-        <v>577</v>
-      </c>
-      <c r="G90" t="n">
-        <v>40</v>
-      </c>
-      <c r="H90" t="n">
-        <v>3167470</v>
-      </c>
-      <c r="I90" t="n">
-        <v>46.659</v>
-      </c>
-      <c r="J90" t="n">
-        <v>76608</v>
-      </c>
-      <c r="K90" t="n">
-        <v>1.128</v>
-      </c>
-      <c r="L90" t="n">
-        <v>68551</v>
-      </c>
-      <c r="M90" t="n">
-        <v>1.01</v>
-      </c>
-      <c r="N90" t="s">
-        <v>572</v>
-      </c>
-      <c r="O90" t="s">
-        <v>573</v>
       </c>
       <c r="P90" t="s">
         <v>22</v>
       </c>
       <c r="Q90" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
+        <v>578</v>
+      </c>
+      <c r="B91" t="s">
         <v>579</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" s="1" t="n">
+        <v>43987</v>
+      </c>
+      <c r="D91" t="s">
         <v>580</v>
       </c>
-      <c r="C91" s="1" t="n">
-        <v>43986</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>581</v>
-      </c>
-      <c r="E91" t="s">
-        <v>582</v>
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H91" t="n">
-        <v>19811243</v>
+        <v>20384850</v>
       </c>
       <c r="I91" t="n">
-        <v>59.852</v>
+        <v>61.585</v>
       </c>
       <c r="J91" t="n">
-        <v>428963</v>
+        <v>573607</v>
       </c>
       <c r="K91" t="n">
-        <v>1.296</v>
+        <v>1.733</v>
       </c>
       <c r="L91" t="n">
-        <v>504442</v>
+        <v>512953</v>
       </c>
       <c r="M91" t="n">
-        <v>1.524</v>
+        <v>1.55</v>
       </c>
       <c r="N91" t="s">
+        <v>581</v>
+      </c>
+      <c r="O91" t="s">
         <v>582</v>
       </c>
-      <c r="O91" t="s">
+      <c r="P91" t="s">
         <v>583</v>
       </c>
-      <c r="P91" t="s">
+      <c r="Q91" t="s">
         <v>584</v>
-      </c>
-      <c r="Q91" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B92" t="s">
+        <v>585</v>
+      </c>
+      <c r="C92" s="1" t="n">
+        <v>43988</v>
+      </c>
+      <c r="D92" t="s">
         <v>586</v>
       </c>
-      <c r="C92" s="1" t="n">
-        <v>43986</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>587</v>
-      </c>
-      <c r="E92" t="s">
-        <v>588</v>
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H92" t="n">
-        <v>18680529</v>
+        <v>19778873</v>
       </c>
       <c r="I92" t="n">
-        <v>56.436</v>
+        <v>59.754</v>
       </c>
       <c r="J92" t="n">
-        <v>465579</v>
+        <v>547429</v>
       </c>
       <c r="K92" t="n">
-        <v>1.407</v>
+        <v>1.654</v>
       </c>
       <c r="L92" t="n">
-        <v>439041</v>
+        <v>464027</v>
       </c>
       <c r="M92" t="n">
-        <v>1.326</v>
+        <v>1.402</v>
       </c>
       <c r="N92" t="s">
+        <v>587</v>
+      </c>
+      <c r="O92" t="s">
         <v>588</v>
       </c>
-      <c r="O92" t="s">
+      <c r="P92" t="s">
         <v>589</v>
       </c>
-      <c r="P92" t="s">
+      <c r="Q92" t="s">
         <v>590</v>
-      </c>
-      <c r="Q92" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
+        <v>591</v>
+      </c>
+      <c r="B93" t="s">
         <v>592</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" s="1" t="n">
+        <v>43989</v>
+      </c>
+      <c r="D93" t="s">
         <v>593</v>
-      </c>
-      <c r="C93" s="1" t="n">
-        <v>43987</v>
-      </c>
-      <c r="D93" t="s">
-        <v>594</v>
       </c>
       <c r="E93" t="s">
         <v>124</v>
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H93" t="n">
-        <v>46512</v>
+        <v>48029</v>
       </c>
       <c r="I93" t="n">
-        <v>13.39</v>
+        <v>13.826</v>
       </c>
       <c r="J93" t="n">
-        <v>735</v>
+        <v>596</v>
       </c>
       <c r="K93" t="n">
-        <v>0.212</v>
+        <v>0.172</v>
       </c>
       <c r="L93" t="n">
-        <v>720</v>
+        <v>650</v>
       </c>
       <c r="M93" t="n">
-        <v>0.207</v>
+        <v>0.187</v>
       </c>
       <c r="N93" t="s">
         <v>124</v>
       </c>
       <c r="O93" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="P93" t="s">
         <v>22</v>
       </c>
       <c r="Q93" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
+        <v>596</v>
+      </c>
+      <c r="B94" t="s">
         <v>597</v>
-      </c>
-      <c r="B94" t="s">
-        <v>598</v>
       </c>
       <c r="C94" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="D94" t="s">
+        <v>598</v>
+      </c>
+      <c r="E94" t="s">
         <v>599</v>
-      </c>
-      <c r="E94" t="s">
-        <v>600</v>
       </c>
       <c r="F94"/>
       <c r="G94" t="n">
@@ -7158,67 +7173,67 @@
         <v>0.112</v>
       </c>
       <c r="N94" t="s">
+        <v>599</v>
+      </c>
+      <c r="O94" t="s">
         <v>600</v>
       </c>
-      <c r="O94" t="s">
+      <c r="P94" t="s">
         <v>601</v>
       </c>
-      <c r="P94" t="s">
+      <c r="Q94" t="s">
         <v>602</v>
-      </c>
-      <c r="Q94" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
+        <v>603</v>
+      </c>
+      <c r="B95" t="s">
         <v>604</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" s="1" t="n">
+        <v>43987</v>
+      </c>
+      <c r="D95" t="s">
         <v>605</v>
       </c>
-      <c r="C95" s="1" t="n">
-        <v>43985</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>606</v>
-      </c>
-      <c r="E95" t="s">
-        <v>607</v>
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H95" t="n">
-        <v>20012</v>
+        <v>21000</v>
       </c>
       <c r="I95" t="n">
-        <v>1.346</v>
+        <v>1.413</v>
       </c>
       <c r="J95" t="n">
-        <v>722</v>
+        <v>598</v>
       </c>
       <c r="K95" t="n">
-        <v>0.049</v>
+        <v>0.04</v>
       </c>
       <c r="L95" t="n">
-        <v>537</v>
+        <v>591</v>
       </c>
       <c r="M95" t="n">
-        <v>0.036</v>
+        <v>0.04</v>
       </c>
       <c r="N95" t="s">
+        <v>606</v>
+      </c>
+      <c r="O95" t="s">
         <v>607</v>
-      </c>
-      <c r="O95" t="s">
-        <v>608</v>
       </c>
       <c r="P95" t="s">
         <v>22</v>
       </c>
       <c r="Q95" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testing data for 2020-06-09
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="610">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Argentina - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/06-06-20_reporte-matutino-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/09-06-20_reporte-matutino-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Argentina</t>
@@ -92,7 +92,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/06/coronavirus-covid-19-at-a-glance-5-june-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/06/coronavirus-covid-19-at-a-glance-8-june-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200607130312/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200609200149/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200607130314/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200609200151/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -154,9 +154,9 @@
     <t xml:space="preserve">The source reports the 'number of assessments' conducted. It is unclear whether this refers to the total number of tests conducted, or the number of people tested.</t>
   </si>
   <si>
-    <t xml:space="preserve">The Bahrainian Ministry of Health publishes frequent updates (not daily, but with high frequency) on the number of confirmed cases, status of existing cases and number of assessments conducted.
+    <t xml:space="preserve">The Bahrainian Ministry of Health publishes frequent updates on the number of confirmed cases, status of existing cases and number of assessments conducted.
 These figures represent the cumulative tests to that given date. It is not clear whether this refers to the total number of tests conducted, or the number of people tested.
-These updates are not provided daily – typically every few days, so a daily time-series is not available. However, using web archives we can construct a time-series of tests conducted over time based on these frequent updates. It is not clear when testing first began; data is only available from 5th March where it was reported that 5334 tests had been conducted.</t>
+Using web archives we can construct a time-series of tests conducted over time based on these frequent updates. It is not clear when testing first began; data is only available from 5th March where it was reported that 5334 tests had been conducted.</t>
   </si>
   <si>
     <t xml:space="preserve">BGD</t>
@@ -187,7 +187,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-2-iyunya-vyzdoroveli-i-vypisany-19-195-patsientov/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-8-iyunya-vyzdoroveli-i-vypisany-23-tys-880-patsientov/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -233,7 +233,7 @@
     <t xml:space="preserve">Bolivia - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4252-sube-a-12-245-el-numero-de-total-de-contagios-de-coronavirus-en-bolivia-los-casos-descartados-suman-21-701</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4271-ministerio-de-salud-reporta-306-nuevos-contagios-de-coronavirus-y-10-fallecidos</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -280,7 +280,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200607130320/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200609200157/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -303,7 +303,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200607130321/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200609200159/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -391,7 +391,7 @@
     <t xml:space="preserve">Croatia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200607130325/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200609200210/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -454,7 +454,7 @@
     <t xml:space="preserve">Denmark - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200606153440/https://www.ssi.dk/sygdomme-beredskab-og-forskning/sygdomsovervaagning/c/covid19-overvaagning</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200609210201/https://www.ssi.dk/sygdomme-beredskab-og-forskning/sygdomsovervaagning/c/covid19-overvaagning</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -480,7 +480,7 @@
     <t xml:space="preserve">Ecuador - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-06062020-08h00.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-08062020-08h00.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -505,7 +505,7 @@
     <t xml:space="preserve">El Salvador - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/2951104881642350</t>
+    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/2958451900907648</t>
   </si>
   <si>
     <t xml:space="preserve">Government of El Salvador</t>
@@ -549,7 +549,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_June-5-Eng_V1.pdf</t>
+    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_June-9-Eng_V1.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -577,8 +577,7 @@
     <t xml:space="preserve">Finnish Department of Health and Welfare COVID-19 data dashboard</t>
   </si>
   <si>
-    <t xml:space="preserve">The Finnish Department of Health and Welfare publishes a dashboard of confirmed cases, deaths and samples tested.
-The dashboard provides daily figures and cumulative test numbers on a separate tab. We have copied this time-series as presented in the original source. It's important to note that when figures exceed 1000, the Finnish Department of Health and Welfare report samples to the nearest hundred (e.g. 1.6k). 
+    <t xml:space="preserve">The Finnish Department of Health and Welfare publishes a dashboard of confirmed cases, deaths and samples tested. The dashboard provides both daily and cumulative test numbers. We extract the complete daily time series using the [official API](https://thl.fi/fi/tilastot-ja-data/aineistot-ja-palvelut/avoin-data/varmistetut-koronatapaukset-suomessa-covid-19-).
 Further descriptions of the testing data are provided [here](https://thl.fi/fi/web/infektiotaudit-ja-rokotukset/ajankohtaista/ajankohtaista-koronaviruksesta-covid-19/tilannekatsaus-koronaviruksesta). In this document it notes that:
 - "Public and private sector laboratories report to THL (health authority) the number of samples tested per hospital district"
 - "The actual number of infections in Finland is probably higher than reported, as not all mild symptoms have been tested so far and no information is available on the number of asymptomatic infections."
@@ -705,7 +704,7 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-report-20200604/</t>
+    <t xml:space="preserve">https://eody.gov.gr/wp-content/uploads/2020/06/covid-gr-daily-report-20200609.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -808,7 +807,8 @@
   <si>
     <t xml:space="preserve">The ICMR reports separate figures for both “samples tested” and “people tested” at press conferences and in press releases (shown separately in the charts above). No other details are provided.
 The press releases from ICMR do not always stay online for very long. The reason for this is unknown, but the releases are being backed up at this [GitHub repository](https://github.com/datameet/covid19).
-On some occasions there appear to have been more than one update released per day. Where we are aware of multiple observations for the day, we show the number for the earlier release.</t>
+On some occasions there appear to have been more than one update released per day. Where we are aware of multiple observations for the day, we show the number for the earlier release.
+The ICMR website does not explicitly state whether the reported figures refer to PCR tests only. From contextual information, it appears that the reported figures may also include samples that were tested using a TrueNat non-PCR test. ICMR communications on [May 21st 2020](https://www.icmr.gov.in/pdf/press_realease_files/ICMR_Press_Release_TruNat_21052020.pdf) and [April 19th 2020](https://www.icmr.gov.in/pdf/covid/labs/Additional_guidance_on_TrueNat_based_COVID19_testing.pdf) indicate that TrueNat tests are being used in diagnostic testing. These TrueNat tests likely account for a small minority of all samples tested.</t>
   </si>
   <si>
     <t xml:space="preserve">India - samples tested</t>
@@ -843,7 +843,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200606165255/http://irangov.ir/detail/340405</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200608164008/http://irangov.ir/detail/340523</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -862,7 +862,7 @@
     <t xml:space="preserve">Ireland - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gov.ie/en/press-release/1beb1-statement-from-the-national-public-health-emergency-team-tuesday-2-june/</t>
+    <t xml:space="preserve">https://www.gov.ie/en/press-release/b8a62-statement-from-the-national-public-health-emergency-team-tuesday-9-june/</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gov.ie/en/publications/?&amp;type=press-releases&amp;organisation=department-of-health</t>
@@ -883,7 +883,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/20164/covid19-data-israel-28052020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/20359/covid19-data-israel-02062020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -940,7 +940,7 @@
     <t xml:space="preserve">Japan - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11739.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11774.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -964,10 +964,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000637521.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release (510, 602) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000637521.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000638336.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (514, 315) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000637887.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11th April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -999,7 +999,7 @@
     <t xml:space="preserve">Kenya - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1269290630947143686</t>
+    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1269625118482993152</t>
   </si>
   <si>
     <t xml:space="preserve">Kenya Ministry of Health</t>
@@ -1040,7 +1040,7 @@
     <t xml:space="preserve">Lithuania - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200605152658/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200609202712/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -1056,7 +1056,7 @@
     <t xml:space="preserve">Luxembourg - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200606200221/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200609202720/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg Government situation update</t>
@@ -1077,13 +1077,13 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/kementeriankesihatanmalaysia/videos/488938701905775</t>
+    <t xml:space="preserve">https://www.facebook.com/373560576236/videos/558621301493247</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
   </si>
   <si>
-    <t xml:space="preserve">Statistics on testing can be see at 17:49 timestamp on the MOH livestream</t>
+    <t xml:space="preserve">Statistics on testing can be see at 35:09 timestamp on the MOH livestream</t>
   </si>
   <si>
     <t xml:space="preserve">http://covid-19.moh.gov.my/terkini</t>
@@ -1103,13 +1103,13 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/561317043971945/videos/2676083566001901/</t>
+    <t xml:space="preserve">https://www.facebook.com/561317043971945/videos/2853180084804153/</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Ministry of Health</t>
   </si>
   <si>
-    <t xml:space="preserve">Numbers visible in video at time: 2:35</t>
+    <t xml:space="preserve">Numbers visible in video at time: 1:07</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Ministry of Health Official Facebook page</t>
@@ -1134,7 +1134,7 @@
   </si>
   <si>
     <t xml:space="preserve">The Mexican Health Secretary publishes a dataset on [datos.gob.mx](https://datos.gob.mx/busca/dataset/informacion-referente-a-casos-covid-19-en-mexico), the open data platform of the Mexican government.
-The file can be downloaded in CSV format, and gives detailed information on each case (1 row per case). The RESULTADO column gives the status of the case, with 1 = CONFIRMED and 2 = NEGATIVE. The resulting tally can also be found on the [government's COVID-19 dashboard](https://coronavirus.gob.mx/datos/).
+The file can be downloaded in CSV format, and gives detailed information on each case (1 row per case). The RESULTADO column gives the status of the case, with 1 = CONFIRMED and 2 = NEGATIVE. The resulting tally can also be found on the [government's COVID-19 dashboard](https://coronavirus.gob.mx/datos/). We do not include pending tests (RESULTADO = 3).
 While geographical coverage is complete, there is a time lag in the publication of the data, and recent days systematically show temporary low figures. Data starts on 1 January 2020; we do not know if this is because tests started on that date or because earlier data is not available.
 The notes to the data provide the following note "Information from the Epidemiological Surveillance System for Viral Respiratory Diseases, reported by the 475 viral respiratory disease monitoring units (USMER) throughout the country in the entire health sector (IMSS, ISSSTE, SEDENA, SEMAR, ETC).... Preliminary data subject to validation by the Ministry of Health through the General Directorate of Epidemiology. The information contained corresponds only to the data obtained from the epidemiological study of a suspected case of viral respiratory disease at the time it is identified in the medical units of the Health Sector". (via Google translate)</t>
   </si>
@@ -1209,10 +1209,10 @@
     <t xml:space="preserve">Netherlands - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-06/COVID-19_WebSite_rapport_dagelijks20200606_1025.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 6 June 2020 update</t>
+    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-06/COVID-19_WebSite_rapport_dagelijks20200608_1021.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dutch National Institute for Public Health and the Environment - 8 June 2020 update</t>
   </si>
   <si>
     <t xml:space="preserve">Dutch National Institute for Public Health and the Environment</t>
@@ -1248,7 +1248,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200606200626/https://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200609202905/https://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1268,7 +1268,7 @@
     <t xml:space="preserve">Norway - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020-06-05-dagsrapport-norge-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.06.09---dagsrapport-norge-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Norwegian Institute of Public Health</t>
@@ -1293,7 +1293,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200607132318/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200609202908/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1312,10 +1312,13 @@
     <t xml:space="preserve">Panama - tests performed</t>
   </si>
   <si>
+    <t xml:space="preserve">http://minsa.gob.pa/covid-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panama Ministry of Health</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://minsa.gob.pa/covid-19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panama Ministry of Health</t>
   </si>
   <si>
     <t xml:space="preserve">The Panama Ministry of Health reports the cumulative number of tests performed ("pruebas realizadas") on [their official dashboard](http://minsa.gob.pa/covid-19) with a time series dating back to 9 March 2020. The page with testing numbers is not the first one shown but can be navigated to with the arrows at the bottom of the dashboard. The dashboard shows the cumulative number of total, positive, negative, and control tests ("prueba de control") performed. We report here the total of positive and negative numbers because: 1) the time series only includes positive and negative test numbers; and 2) the total they provide seems to include control tests, which we understand to be used for testing quality control.</t>
@@ -1346,7 +1349,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/183570-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-191-758-en-el-peru-comunicado-n-123</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/185100-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-203-736-en-el-peru-comunicado-n-126</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1452,7 +1455,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-7-iunie-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-9-iunie-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1470,7 +1473,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14634</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14653</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1490,7 +1493,7 @@
     <t xml:space="preserve">Rwanda - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1269000782919204866</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1269689516522160128</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1597,7 +1600,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200606200638/https://korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200609203740/https://korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Center of Health Information and the Office of the Government of the Slovak Republic</t>
@@ -1671,7 +1674,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367452&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367472&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1691,7 +1694,7 @@
     <t xml:space="preserve">Spain - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/COVID-19_pruebas_diagnosticas_28_05_2020.pdf</t>
+    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/COVID-19_pruebas_diagnosticas_04_06_2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Consumption and Social Welfare</t>
@@ -1777,7 +1780,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200606200720/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200609203821/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1804,7 +1807,7 @@
     <t xml:space="preserve">World Health Organization Country Office for Thailand</t>
   </si>
   <si>
-    <t xml:space="preserve">This figure is approximate. The report states that "Over 420,000 RT-PCR tests have been performed."</t>
+    <t xml:space="preserve">This figure is approximate. The report states that "By 5th June more than 468,000 tests for COVID-19 had been performed..."</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.who.int/thailand/emergencies/novel-coronavirus-2019/situation-reports</t>
@@ -1847,7 +1850,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200606200724/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200609203827/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1871,7 +1874,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1269298040814424066</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1270267232887672832</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
@@ -1895,7 +1898,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200607132414/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200609203829/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1932,7 +1935,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/890549/COVID-19_UK_testing_time_series_6_June.csv</t>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/891086/2020-06-09_COVID-19_UK_testing_time_series.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Sum of pillar 1 + pillar 2 (tests processed only)</t>
@@ -1953,7 +1956,7 @@
     <t xml:space="preserve">United States - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200606200727/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200609203831/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
   </si>
   <si>
     <t xml:space="preserve">United States CDC</t>
@@ -2007,7 +2010,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-46</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-48</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2046,7 +2049,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1269065905201459200</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1269368825193119746</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -2456,7 +2459,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>43988</v>
+        <v>43991</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2466,25 +2469,25 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H2" t="n">
-        <v>189278</v>
+        <v>203051</v>
       </c>
       <c r="I2" t="n">
-        <v>4.188</v>
+        <v>4.493</v>
       </c>
       <c r="J2" t="n">
-        <v>5416</v>
+        <v>4531</v>
       </c>
       <c r="K2" t="n">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="L2" t="n">
-        <v>4857</v>
+        <v>4934</v>
       </c>
       <c r="M2" t="n">
-        <v>0.107</v>
+        <v>0.109</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -2507,7 +2510,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>43987</v>
+        <v>43990</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2517,25 +2520,25 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H3" t="n">
-        <v>1579192</v>
+        <v>1633515</v>
       </c>
       <c r="I3" t="n">
-        <v>61.929</v>
+        <v>64.06</v>
       </c>
       <c r="J3" t="n">
-        <v>32863</v>
+        <v>16053</v>
       </c>
       <c r="K3" t="n">
-        <v>1.289</v>
+        <v>0.63</v>
       </c>
       <c r="L3" t="n">
-        <v>25939</v>
+        <v>23042</v>
       </c>
       <c r="M3" t="n">
-        <v>1.017</v>
+        <v>0.904</v>
       </c>
       <c r="N3" t="s">
         <v>27</v>
@@ -2558,7 +2561,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -2568,25 +2571,25 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H4" t="n">
-        <v>489597</v>
+        <v>500921</v>
       </c>
       <c r="I4" t="n">
-        <v>54.361</v>
+        <v>55.618</v>
       </c>
       <c r="J4" t="n">
-        <v>3685</v>
+        <v>6160</v>
       </c>
       <c r="K4" t="n">
-        <v>0.409</v>
+        <v>0.684</v>
       </c>
       <c r="L4" t="n">
-        <v>5866</v>
+        <v>6363</v>
       </c>
       <c r="M4" t="n">
-        <v>0.651</v>
+        <v>0.706</v>
       </c>
       <c r="N4" t="s">
         <v>34</v>
@@ -2609,7 +2612,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2619,25 +2622,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H5" t="n">
-        <v>367056</v>
+        <v>378235</v>
       </c>
       <c r="I5" t="n">
-        <v>215.714</v>
+        <v>222.284</v>
       </c>
       <c r="J5" t="n">
-        <v>5680</v>
+        <v>3873</v>
       </c>
       <c r="K5" t="n">
-        <v>3.338</v>
+        <v>2.276</v>
       </c>
       <c r="L5" t="n">
-        <v>7178</v>
+        <v>6786</v>
       </c>
       <c r="M5" t="n">
-        <v>4.218</v>
+        <v>3.988</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
@@ -2660,7 +2663,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>43988</v>
+        <v>43990</v>
       </c>
       <c r="D6" t="s">
         <v>48</v>
@@ -2670,25 +2673,25 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H6" t="n">
-        <v>384851</v>
+        <v>410931</v>
       </c>
       <c r="I6" t="n">
-        <v>2.337</v>
+        <v>2.495</v>
       </c>
       <c r="J6" t="n">
-        <v>12486</v>
+        <v>12944</v>
       </c>
       <c r="K6" t="n">
-        <v>0.076</v>
+        <v>0.079</v>
       </c>
       <c r="L6" t="n">
-        <v>12542</v>
+        <v>12937</v>
       </c>
       <c r="M6" t="n">
-        <v>0.076</v>
+        <v>0.079</v>
       </c>
       <c r="N6" t="s">
         <v>49</v>
@@ -2711,7 +2714,7 @@
         <v>54</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>43984</v>
+        <v>43990</v>
       </c>
       <c r="D7" t="s">
         <v>55</v>
@@ -2721,25 +2724,25 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H7" t="n">
-        <v>562945</v>
+        <v>632993</v>
       </c>
       <c r="I7" t="n">
-        <v>59.575</v>
+        <v>66.988</v>
       </c>
       <c r="J7" t="n">
-        <v>9568</v>
+        <v>10680</v>
       </c>
       <c r="K7" t="n">
-        <v>1.013</v>
+        <v>1.13</v>
       </c>
       <c r="L7" t="n">
-        <v>12863</v>
+        <v>11374</v>
       </c>
       <c r="M7" t="n">
-        <v>1.361</v>
+        <v>1.204</v>
       </c>
       <c r="N7" t="s">
         <v>56</v>
@@ -2762,7 +2765,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>43987</v>
+        <v>43989</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
@@ -2772,25 +2775,25 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H8" t="n">
-        <v>741468</v>
+        <v>756888</v>
       </c>
       <c r="I8" t="n">
-        <v>63.977</v>
+        <v>65.307</v>
       </c>
       <c r="J8" t="n">
-        <v>7383</v>
+        <v>4936</v>
       </c>
       <c r="K8" t="n">
-        <v>0.637</v>
+        <v>0.426</v>
       </c>
       <c r="L8" t="n">
-        <v>6883</v>
+        <v>7355</v>
       </c>
       <c r="M8" t="n">
-        <v>0.594</v>
+        <v>0.635</v>
       </c>
       <c r="N8" t="s">
         <v>62</v>
@@ -2813,7 +2816,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>43986</v>
+        <v>43990</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
@@ -2823,25 +2826,25 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="H9" t="n">
-        <v>33946</v>
+        <v>38092</v>
       </c>
       <c r="I9" t="n">
-        <v>2.908</v>
+        <v>3.263</v>
       </c>
       <c r="J9" t="n">
-        <v>1460</v>
+        <v>816</v>
       </c>
       <c r="K9" t="n">
-        <v>0.125</v>
+        <v>0.07</v>
       </c>
       <c r="L9" t="n">
-        <v>1108</v>
+        <v>1150</v>
       </c>
       <c r="M9" t="n">
-        <v>0.095</v>
+        <v>0.099</v>
       </c>
       <c r="N9" t="s">
         <v>41</v>
@@ -2913,7 +2916,7 @@
         <v>81</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D11" t="s">
         <v>82</v>
@@ -2923,25 +2926,25 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H11" t="n">
-        <v>89902</v>
+        <v>91735</v>
       </c>
       <c r="I11" t="n">
-        <v>12.938</v>
+        <v>13.202</v>
       </c>
       <c r="J11" t="n">
-        <v>816</v>
+        <v>1406</v>
       </c>
       <c r="K11" t="n">
-        <v>0.117</v>
+        <v>0.202</v>
       </c>
       <c r="L11" t="n">
-        <v>1222</v>
+        <v>1260</v>
       </c>
       <c r="M11" t="n">
-        <v>0.176</v>
+        <v>0.181</v>
       </c>
       <c r="N11" t="s">
         <v>84</v>
@@ -2964,7 +2967,7 @@
         <v>88</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D12" t="s">
         <v>89</v>
@@ -2974,25 +2977,25 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H12" t="n">
-        <v>1868201</v>
+        <v>1930065</v>
       </c>
       <c r="I12" t="n">
-        <v>49.499</v>
+        <v>51.138</v>
       </c>
       <c r="J12" t="n">
-        <v>37779</v>
+        <v>33319</v>
       </c>
       <c r="K12" t="n">
-        <v>1.001</v>
+        <v>0.883</v>
       </c>
       <c r="L12" t="n">
-        <v>29308</v>
+        <v>29804</v>
       </c>
       <c r="M12" t="n">
-        <v>0.777</v>
+        <v>0.79</v>
       </c>
       <c r="N12" t="s">
         <v>90</v>
@@ -3015,7 +3018,7 @@
         <v>95</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>43988</v>
+        <v>43991</v>
       </c>
       <c r="D13" t="s">
         <v>96</v>
@@ -3027,25 +3030,25 @@
         <v>97</v>
       </c>
       <c r="G13" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H13" t="n">
-        <v>687510</v>
+        <v>746592</v>
       </c>
       <c r="I13" t="n">
-        <v>35.965</v>
+        <v>39.055</v>
       </c>
       <c r="J13" t="n">
-        <v>18954</v>
+        <v>17777</v>
       </c>
       <c r="K13" t="n">
-        <v>0.992</v>
+        <v>0.93</v>
       </c>
       <c r="L13" t="n">
-        <v>17741</v>
+        <v>19117</v>
       </c>
       <c r="M13" t="n">
-        <v>0.928</v>
+        <v>1</v>
       </c>
       <c r="N13" t="s">
         <v>98</v>
@@ -3068,7 +3071,7 @@
         <v>102</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>43988</v>
+        <v>43990</v>
       </c>
       <c r="D14" t="s">
         <v>103</v>
@@ -3078,25 +3081,25 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H14" t="n">
-        <v>399505</v>
+        <v>421723</v>
       </c>
       <c r="I14" t="n">
-        <v>7.851</v>
+        <v>8.288</v>
       </c>
       <c r="J14" t="n">
-        <v>12567</v>
+        <v>11004</v>
       </c>
       <c r="K14" t="n">
-        <v>0.247</v>
+        <v>0.216</v>
       </c>
       <c r="L14" t="n">
-        <v>11389</v>
+        <v>11512</v>
       </c>
       <c r="M14" t="n">
-        <v>0.224</v>
+        <v>0.226</v>
       </c>
       <c r="N14" t="s">
         <v>104</v>
@@ -3119,7 +3122,7 @@
         <v>109</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>43988</v>
+        <v>43991</v>
       </c>
       <c r="D15" t="s">
         <v>110</v>
@@ -3129,25 +3132,25 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H15" t="n">
-        <v>21275</v>
+        <v>21933</v>
       </c>
       <c r="I15" t="n">
-        <v>4.176</v>
+        <v>4.306</v>
       </c>
       <c r="J15" t="n">
-        <v>334</v>
+        <v>229</v>
       </c>
       <c r="K15" t="n">
-        <v>0.066</v>
+        <v>0.045</v>
       </c>
       <c r="L15" t="n">
-        <v>373</v>
+        <v>318</v>
       </c>
       <c r="M15" t="n">
-        <v>0.073</v>
+        <v>0.062</v>
       </c>
       <c r="N15" t="s">
         <v>111</v>
@@ -3170,7 +3173,7 @@
         <v>115</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D16" t="s">
         <v>116</v>
@@ -3180,25 +3183,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H16" t="n">
-        <v>68740</v>
+        <v>69115</v>
       </c>
       <c r="I16" t="n">
-        <v>16.744</v>
+        <v>16.836</v>
       </c>
       <c r="J16" t="n">
-        <v>226</v>
+        <v>249</v>
       </c>
       <c r="K16" t="n">
-        <v>0.055</v>
+        <v>0.061</v>
       </c>
       <c r="L16" t="n">
-        <v>334</v>
+        <v>260</v>
       </c>
       <c r="M16" t="n">
-        <v>0.081</v>
+        <v>0.063</v>
       </c>
       <c r="N16" t="s">
         <v>117</v>
@@ -3221,7 +3224,7 @@
         <v>122</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>43987</v>
+        <v>43990</v>
       </c>
       <c r="D17" t="s">
         <v>123</v>
@@ -3233,25 +3236,25 @@
         <v>125</v>
       </c>
       <c r="G17" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H17" t="n">
-        <v>116468</v>
+        <v>122603</v>
       </c>
       <c r="I17" t="n">
-        <v>10.283</v>
+        <v>10.824</v>
       </c>
       <c r="J17" t="n">
-        <v>2004</v>
+        <v>2067</v>
       </c>
       <c r="K17" t="n">
-        <v>0.177</v>
+        <v>0.182</v>
       </c>
       <c r="L17" t="n">
-        <v>1906</v>
+        <v>2031</v>
       </c>
       <c r="M17" t="n">
-        <v>0.168</v>
+        <v>0.179</v>
       </c>
       <c r="N17" t="s">
         <v>124</v>
@@ -3274,7 +3277,7 @@
         <v>130</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>43988</v>
+        <v>43990</v>
       </c>
       <c r="D18" t="s">
         <v>131</v>
@@ -3284,25 +3287,25 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H18" t="n">
-        <v>471521</v>
+        <v>478825</v>
       </c>
       <c r="I18" t="n">
-        <v>44.03</v>
+        <v>44.712</v>
       </c>
       <c r="J18" t="n">
-        <v>2000</v>
+        <v>4571</v>
       </c>
       <c r="K18" t="n">
-        <v>0.187</v>
+        <v>0.427</v>
       </c>
       <c r="L18" t="n">
-        <v>4316</v>
+        <v>4242</v>
       </c>
       <c r="M18" t="n">
-        <v>0.403</v>
+        <v>0.396</v>
       </c>
       <c r="N18" t="s">
         <v>41</v>
@@ -3325,7 +3328,7 @@
         <v>135</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>43988</v>
+        <v>43991</v>
       </c>
       <c r="D19" t="s">
         <v>136</v>
@@ -3335,25 +3338,25 @@
       </c>
       <c r="F19"/>
       <c r="G19" t="n">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H19" t="n">
-        <v>571832</v>
+        <v>594790</v>
       </c>
       <c r="I19" t="n">
-        <v>98.724</v>
+        <v>102.688</v>
       </c>
       <c r="J19" t="n">
-        <v>8927</v>
+        <v>9766</v>
       </c>
       <c r="K19" t="n">
-        <v>1.541</v>
+        <v>1.686</v>
       </c>
       <c r="L19" t="n">
-        <v>8195</v>
+        <v>8573</v>
       </c>
       <c r="M19" t="n">
-        <v>1.415</v>
+        <v>1.48</v>
       </c>
       <c r="N19" t="s">
         <v>138</v>
@@ -3376,7 +3379,7 @@
         <v>142</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>43988</v>
+        <v>43990</v>
       </c>
       <c r="D20" t="s">
         <v>143</v>
@@ -3388,21 +3391,21 @@
         <v>145</v>
       </c>
       <c r="G20" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H20" t="n">
-        <v>79123</v>
+        <v>80796</v>
       </c>
       <c r="I20" t="n">
-        <v>4.485</v>
+        <v>4.579</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20" t="n">
-        <v>1556</v>
+        <v>1339</v>
       </c>
       <c r="M20" t="n">
-        <v>0.088</v>
+        <v>0.076</v>
       </c>
       <c r="N20" t="s">
         <v>144</v>
@@ -3425,7 +3428,7 @@
         <v>149</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>43986</v>
+        <v>43989</v>
       </c>
       <c r="D21" t="s">
         <v>150</v>
@@ -3435,25 +3438,25 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="H21" t="n">
-        <v>101604</v>
+        <v>108924</v>
       </c>
       <c r="I21" t="n">
-        <v>15.665</v>
+        <v>16.793</v>
       </c>
       <c r="J21" t="n">
-        <v>2426</v>
+        <v>2376</v>
       </c>
       <c r="K21" t="n">
-        <v>0.374</v>
+        <v>0.366</v>
       </c>
       <c r="L21" t="n">
-        <v>2422</v>
+        <v>2441</v>
       </c>
       <c r="M21" t="n">
-        <v>0.373</v>
+        <v>0.376</v>
       </c>
       <c r="N21" t="s">
         <v>151</v>
@@ -3476,7 +3479,7 @@
         <v>155</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>43988</v>
+        <v>43990</v>
       </c>
       <c r="D22" t="s">
         <v>156</v>
@@ -3486,25 +3489,25 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H22" t="n">
-        <v>90070</v>
+        <v>91734</v>
       </c>
       <c r="I22" t="n">
-        <v>67.898</v>
+        <v>69.153</v>
       </c>
       <c r="J22" t="n">
-        <v>654</v>
+        <v>1121</v>
       </c>
       <c r="K22" t="n">
-        <v>0.493</v>
+        <v>0.845</v>
       </c>
       <c r="L22" t="n">
-        <v>948</v>
+        <v>938</v>
       </c>
       <c r="M22" t="n">
-        <v>0.715</v>
+        <v>0.707</v>
       </c>
       <c r="N22" t="s">
         <v>158</v>
@@ -3527,7 +3530,7 @@
         <v>163</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>43987</v>
+        <v>43991</v>
       </c>
       <c r="D23" t="s">
         <v>164</v>
@@ -3537,21 +3540,25 @@
       </c>
       <c r="F23"/>
       <c r="G23" t="n">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H23" t="n">
-        <v>131368</v>
+        <v>152334</v>
       </c>
       <c r="I23" t="n">
-        <v>1.143</v>
-      </c>
-      <c r="J23"/>
-      <c r="K23"/>
+        <v>1.325</v>
+      </c>
+      <c r="J23" t="n">
+        <v>4599</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.04</v>
+      </c>
       <c r="L23" t="n">
-        <v>4255</v>
+        <v>5146</v>
       </c>
       <c r="M23" t="n">
-        <v>0.037</v>
+        <v>0.045</v>
       </c>
       <c r="N23" t="s">
         <v>165</v>
@@ -3574,7 +3581,7 @@
         <v>169</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>43988</v>
+        <v>43989</v>
       </c>
       <c r="D24" t="s">
         <v>170</v>
@@ -3584,25 +3591,25 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H24" t="n">
-        <v>201077</v>
+        <v>205494</v>
       </c>
       <c r="I24" t="n">
-        <v>36.291</v>
+        <v>37.088</v>
       </c>
       <c r="J24" t="n">
-        <v>408</v>
+        <v>640</v>
       </c>
       <c r="K24" t="n">
-        <v>0.074</v>
+        <v>0.116</v>
       </c>
       <c r="L24" t="n">
-        <v>1606</v>
+        <v>2061</v>
       </c>
       <c r="M24" t="n">
-        <v>0.29</v>
+        <v>0.372</v>
       </c>
       <c r="N24" t="s">
         <v>172</v>
@@ -3825,7 +3832,7 @@
         <v>202</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>43986</v>
+        <v>43987</v>
       </c>
       <c r="D29" t="s">
         <v>195</v>
@@ -3837,25 +3844,25 @@
         <v>203</v>
       </c>
       <c r="G29" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H29" t="n">
-        <v>229093</v>
+        <v>233734</v>
       </c>
       <c r="I29" t="n">
-        <v>7.373</v>
+        <v>7.522</v>
       </c>
       <c r="J29" t="n">
-        <v>2352</v>
+        <v>4641</v>
       </c>
       <c r="K29" t="n">
-        <v>0.076</v>
+        <v>0.149</v>
       </c>
       <c r="L29" t="n">
-        <v>2496</v>
+        <v>2683</v>
       </c>
       <c r="M29" t="n">
-        <v>0.08</v>
+        <v>0.086</v>
       </c>
       <c r="N29" t="s">
         <v>198</v>
@@ -3878,7 +3885,7 @@
         <v>205</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>43986</v>
+        <v>43991</v>
       </c>
       <c r="D30" t="s">
         <v>206</v>
@@ -3888,21 +3895,25 @@
       </c>
       <c r="F30"/>
       <c r="G30" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H30" t="n">
-        <v>193929</v>
+        <v>231759</v>
       </c>
       <c r="I30" t="n">
-        <v>18.606</v>
-      </c>
-      <c r="J30"/>
-      <c r="K30"/>
+        <v>22.235</v>
+      </c>
+      <c r="J30" t="n">
+        <v>2240</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.215</v>
+      </c>
       <c r="L30" t="n">
-        <v>3352</v>
+        <v>6596</v>
       </c>
       <c r="M30" t="n">
-        <v>0.322</v>
+        <v>0.633</v>
       </c>
       <c r="N30" t="s">
         <v>208</v>
@@ -3976,7 +3987,7 @@
         <v>219</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>43988</v>
+        <v>43989</v>
       </c>
       <c r="D32" t="s">
         <v>220</v>
@@ -3988,25 +3999,25 @@
         <v>222</v>
       </c>
       <c r="G32" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H32" t="n">
-        <v>206853</v>
+        <v>210202</v>
       </c>
       <c r="I32" t="n">
-        <v>21.413</v>
+        <v>21.759</v>
       </c>
       <c r="J32" t="n">
-        <v>4247</v>
+        <v>3349</v>
       </c>
       <c r="K32" t="n">
-        <v>0.44</v>
+        <v>0.347</v>
       </c>
       <c r="L32" t="n">
-        <v>3327</v>
+        <v>3460</v>
       </c>
       <c r="M32" t="n">
-        <v>0.344</v>
+        <v>0.358</v>
       </c>
       <c r="N32" t="s">
         <v>221</v>
@@ -4029,7 +4040,7 @@
         <v>227</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>43987</v>
+        <v>43990</v>
       </c>
       <c r="D33" t="s">
         <v>228</v>
@@ -4039,25 +4050,25 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H33" t="n">
-        <v>62727</v>
+        <v>62829</v>
       </c>
       <c r="I33" t="n">
-        <v>183.815</v>
+        <v>184.114</v>
       </c>
       <c r="J33" t="n">
-        <v>538</v>
+        <v>68</v>
       </c>
       <c r="K33" t="n">
-        <v>1.577</v>
+        <v>0.199</v>
       </c>
       <c r="L33" t="n">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="M33" t="n">
-        <v>0.73</v>
+        <v>0.718</v>
       </c>
       <c r="N33" t="s">
         <v>229</v>
@@ -4133,7 +4144,7 @@
         <v>238</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D35" t="s">
         <v>234</v>
@@ -4145,25 +4156,25 @@
         <v>236</v>
       </c>
       <c r="G35" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H35" t="n">
-        <v>4666386</v>
+        <v>4916116</v>
       </c>
       <c r="I35" t="n">
-        <v>3.381</v>
+        <v>3.562</v>
       </c>
       <c r="J35" t="n">
-        <v>142069</v>
+        <v>141682</v>
       </c>
       <c r="K35" t="n">
         <v>0.103</v>
       </c>
       <c r="L35" t="n">
-        <v>132766</v>
+        <v>135720</v>
       </c>
       <c r="M35" t="n">
-        <v>0.096</v>
+        <v>0.098</v>
       </c>
       <c r="N35" t="s">
         <v>235</v>
@@ -4186,7 +4197,7 @@
         <v>240</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D36" t="s">
         <v>241</v>
@@ -4196,25 +4207,25 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H36" t="n">
-        <v>269146</v>
+        <v>281653</v>
       </c>
       <c r="I36" t="n">
-        <v>0.984</v>
+        <v>1.03</v>
       </c>
       <c r="J36" t="n">
-        <v>4406</v>
+        <v>7223</v>
       </c>
       <c r="K36" t="n">
-        <v>0.016</v>
+        <v>0.026</v>
       </c>
       <c r="L36" t="n">
-        <v>6503</v>
+        <v>6244</v>
       </c>
       <c r="M36" t="n">
-        <v>0.024</v>
+        <v>0.023</v>
       </c>
       <c r="N36" t="s">
         <v>242</v>
@@ -4237,7 +4248,7 @@
         <v>247</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>43988</v>
+        <v>43989</v>
       </c>
       <c r="D37" t="s">
         <v>248</v>
@@ -4247,25 +4258,25 @@
       </c>
       <c r="F37"/>
       <c r="G37" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H37" t="n">
-        <v>1060126</v>
+        <v>1084857</v>
       </c>
       <c r="I37" t="n">
-        <v>12.622</v>
+        <v>12.916</v>
       </c>
       <c r="J37" t="n">
-        <v>19837</v>
+        <v>24731</v>
       </c>
       <c r="K37" t="n">
-        <v>0.236</v>
+        <v>0.294</v>
       </c>
       <c r="L37" t="n">
-        <v>20590</v>
+        <v>21280</v>
       </c>
       <c r="M37" t="n">
-        <v>0.245</v>
+        <v>0.253</v>
       </c>
       <c r="N37" t="s">
         <v>249</v>
@@ -4288,7 +4299,7 @@
         <v>253</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>43984</v>
+        <v>43991</v>
       </c>
       <c r="D38" t="s">
         <v>254</v>
@@ -4298,21 +4309,21 @@
       </c>
       <c r="F38"/>
       <c r="G38" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H38" t="n">
-        <v>348416</v>
+        <v>367780</v>
       </c>
       <c r="I38" t="n">
-        <v>70.561</v>
+        <v>74.483</v>
       </c>
       <c r="J38"/>
       <c r="K38"/>
       <c r="L38" t="n">
-        <v>3232</v>
+        <v>2766</v>
       </c>
       <c r="M38" t="n">
-        <v>0.655</v>
+        <v>0.56</v>
       </c>
       <c r="N38" t="s">
         <v>214</v>
@@ -4335,7 +4346,7 @@
         <v>259</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>43979</v>
+        <v>43984</v>
       </c>
       <c r="D39" t="s">
         <v>260</v>
@@ -4345,25 +4356,25 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="H39" t="n">
-        <v>565161</v>
+        <v>593579</v>
       </c>
       <c r="I39" t="n">
-        <v>65.295</v>
+        <v>68.578</v>
       </c>
       <c r="J39" t="n">
-        <v>5357</v>
+        <v>11736</v>
       </c>
       <c r="K39" t="n">
-        <v>0.619</v>
+        <v>1.356</v>
       </c>
       <c r="L39" t="n">
-        <v>4799</v>
+        <v>5786</v>
       </c>
       <c r="M39" t="n">
-        <v>0.554</v>
+        <v>0.668</v>
       </c>
       <c r="N39" t="s">
         <v>41</v>
@@ -4386,7 +4397,7 @@
         <v>265</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>43988</v>
+        <v>43991</v>
       </c>
       <c r="D40" t="s">
         <v>266</v>
@@ -4398,25 +4409,25 @@
         <v>268</v>
       </c>
       <c r="G40" t="n">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H40" t="n">
-        <v>2599294</v>
+        <v>2675689</v>
       </c>
       <c r="I40" t="n">
-        <v>42.991</v>
+        <v>44.254</v>
       </c>
       <c r="J40" t="n">
-        <v>34036</v>
+        <v>32200</v>
       </c>
       <c r="K40" t="n">
-        <v>0.563</v>
+        <v>0.533</v>
       </c>
       <c r="L40" t="n">
-        <v>27803</v>
+        <v>28341</v>
       </c>
       <c r="M40" t="n">
-        <v>0.46</v>
+        <v>0.469</v>
       </c>
       <c r="N40" t="s">
         <v>269</v>
@@ -4439,7 +4450,7 @@
         <v>272</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>43988</v>
+        <v>43991</v>
       </c>
       <c r="D41" t="s">
         <v>266</v>
@@ -4451,25 +4462,25 @@
         <v>268</v>
       </c>
       <c r="G41" t="n">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H41" t="n">
-        <v>4187057</v>
+        <v>4318650</v>
       </c>
       <c r="I41" t="n">
-        <v>69.251</v>
+        <v>71.428</v>
       </c>
       <c r="J41" t="n">
-        <v>72485</v>
+        <v>55003</v>
       </c>
       <c r="K41" t="n">
-        <v>1.199</v>
+        <v>0.91</v>
       </c>
       <c r="L41" t="n">
-        <v>51777</v>
+        <v>50908</v>
       </c>
       <c r="M41" t="n">
-        <v>0.856</v>
+        <v>0.842</v>
       </c>
       <c r="N41" t="s">
         <v>269</v>
@@ -4492,7 +4503,7 @@
         <v>275</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D42" t="s">
         <v>276</v>
@@ -4504,21 +4515,21 @@
         <v>278</v>
       </c>
       <c r="G42" t="n">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H42" t="n">
-        <v>314483</v>
+        <v>321053</v>
       </c>
       <c r="I42" t="n">
-        <v>2.486</v>
+        <v>2.538</v>
       </c>
       <c r="J42"/>
       <c r="K42"/>
       <c r="L42" t="n">
-        <v>3435</v>
+        <v>3524</v>
       </c>
       <c r="M42" t="n">
-        <v>0.027</v>
+        <v>0.028</v>
       </c>
       <c r="N42" t="s">
         <v>279</v>
@@ -4541,7 +4552,7 @@
         <v>282</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>43986</v>
+        <v>43988</v>
       </c>
       <c r="D43" t="s">
         <v>283</v>
@@ -4553,25 +4564,25 @@
         <v>284</v>
       </c>
       <c r="G43" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H43" t="n">
-        <v>510520</v>
+        <v>525692</v>
       </c>
       <c r="I43" t="n">
-        <v>4.036</v>
+        <v>4.156</v>
       </c>
       <c r="J43" t="n">
-        <v>5556</v>
+        <v>5974</v>
       </c>
       <c r="K43" t="n">
-        <v>0.044</v>
+        <v>0.047</v>
       </c>
       <c r="L43" t="n">
-        <v>5496</v>
+        <v>5924</v>
       </c>
       <c r="M43" t="n">
-        <v>0.043</v>
+        <v>0.047</v>
       </c>
       <c r="N43" t="s">
         <v>279</v>
@@ -4594,7 +4605,7 @@
         <v>287</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>43988</v>
+        <v>43989</v>
       </c>
       <c r="D44" t="s">
         <v>288</v>
@@ -4604,25 +4615,25 @@
       </c>
       <c r="F44"/>
       <c r="G44" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H44" t="n">
-        <v>942576</v>
+        <v>965089</v>
       </c>
       <c r="I44" t="n">
-        <v>50.199</v>
+        <v>51.398</v>
       </c>
       <c r="J44" t="n">
-        <v>26672</v>
+        <v>22513</v>
       </c>
       <c r="K44" t="n">
-        <v>1.42</v>
+        <v>1.199</v>
       </c>
       <c r="L44" t="n">
-        <v>22041</v>
+        <v>21744</v>
       </c>
       <c r="M44" t="n">
-        <v>1.174</v>
+        <v>1.158</v>
       </c>
       <c r="N44" t="s">
         <v>289</v>
@@ -4645,7 +4656,7 @@
         <v>292</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>43988</v>
+        <v>43989</v>
       </c>
       <c r="D45" t="s">
         <v>293</v>
@@ -4655,25 +4666,25 @@
       </c>
       <c r="F45"/>
       <c r="G45" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H45" t="n">
-        <v>94507</v>
+        <v>97340</v>
       </c>
       <c r="I45" t="n">
-        <v>1.758</v>
+        <v>1.81</v>
       </c>
       <c r="J45" t="n">
-        <v>3632</v>
+        <v>2833</v>
       </c>
       <c r="K45" t="n">
-        <v>0.068</v>
+        <v>0.053</v>
       </c>
       <c r="L45" t="n">
-        <v>2605</v>
+        <v>2686</v>
       </c>
       <c r="M45" t="n">
-        <v>0.048</v>
+        <v>0.05</v>
       </c>
       <c r="N45" t="s">
         <v>41</v>
@@ -4696,7 +4707,7 @@
         <v>299</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D46" t="s">
         <v>300</v>
@@ -4708,25 +4719,25 @@
         <v>302</v>
       </c>
       <c r="G46" t="n">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H46" t="n">
-        <v>117660</v>
+        <v>120052</v>
       </c>
       <c r="I46" t="n">
-        <v>62.379</v>
+        <v>63.647</v>
       </c>
       <c r="J46" t="n">
-        <v>1125</v>
+        <v>1730</v>
       </c>
       <c r="K46" t="n">
-        <v>0.596</v>
+        <v>0.917</v>
       </c>
       <c r="L46" t="n">
-        <v>1227</v>
+        <v>1235</v>
       </c>
       <c r="M46" t="n">
-        <v>0.651</v>
+        <v>0.655</v>
       </c>
       <c r="N46" t="s">
         <v>301</v>
@@ -4749,7 +4760,7 @@
         <v>305</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>43987</v>
+        <v>43991</v>
       </c>
       <c r="D47" t="s">
         <v>306</v>
@@ -4759,25 +4770,25 @@
       </c>
       <c r="F47"/>
       <c r="G47" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H47" t="n">
-        <v>326294</v>
+        <v>340073</v>
       </c>
       <c r="I47" t="n">
-        <v>119.86</v>
+        <v>124.922</v>
       </c>
       <c r="J47" t="n">
-        <v>5254</v>
+        <v>4387</v>
       </c>
       <c r="K47" t="n">
-        <v>1.93</v>
+        <v>1.612</v>
       </c>
       <c r="L47" t="n">
-        <v>4600</v>
+        <v>4335</v>
       </c>
       <c r="M47" t="n">
-        <v>1.69</v>
+        <v>1.592</v>
       </c>
       <c r="N47" t="s">
         <v>41</v>
@@ -4800,7 +4811,7 @@
         <v>310</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>43988</v>
+        <v>43991</v>
       </c>
       <c r="D48" t="s">
         <v>311</v>
@@ -4810,25 +4821,25 @@
       </c>
       <c r="F48"/>
       <c r="G48" t="n">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H48" t="n">
-        <v>84934</v>
+        <v>88914</v>
       </c>
       <c r="I48" t="n">
-        <v>135.683</v>
+        <v>142.041</v>
       </c>
       <c r="J48" t="n">
-        <v>1261</v>
+        <v>680</v>
       </c>
       <c r="K48" t="n">
-        <v>2.014</v>
+        <v>1.086</v>
       </c>
       <c r="L48" t="n">
-        <v>1510</v>
+        <v>1555</v>
       </c>
       <c r="M48" t="n">
-        <v>2.412</v>
+        <v>2.484</v>
       </c>
       <c r="N48" t="s">
         <v>312</v>
@@ -4851,7 +4862,7 @@
         <v>316</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>43988</v>
+        <v>43991</v>
       </c>
       <c r="D49" t="s">
         <v>317</v>
@@ -4863,22 +4874,22 @@
         <v>319</v>
       </c>
       <c r="G49" t="n">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H49" t="n">
-        <v>599454</v>
+        <v>620320</v>
       </c>
       <c r="I49" t="n">
-        <v>18.521</v>
+        <v>19.166</v>
       </c>
       <c r="J49" t="n">
-        <v>8841</v>
+        <v>6081</v>
       </c>
       <c r="K49" t="n">
-        <v>0.273</v>
+        <v>0.188</v>
       </c>
       <c r="L49" t="n">
-        <v>7584</v>
+        <v>7576</v>
       </c>
       <c r="M49" t="n">
         <v>0.234</v>
@@ -4904,7 +4915,7 @@
         <v>323</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>43985</v>
+        <v>43989</v>
       </c>
       <c r="D50" t="s">
         <v>324</v>
@@ -4916,25 +4927,25 @@
         <v>326</v>
       </c>
       <c r="G50" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H50" t="n">
-        <v>26243</v>
+        <v>29582</v>
       </c>
       <c r="I50" t="n">
-        <v>48.549</v>
+        <v>54.727</v>
       </c>
       <c r="J50" t="n">
-        <v>652</v>
+        <v>875</v>
       </c>
       <c r="K50" t="n">
-        <v>1.206</v>
+        <v>1.619</v>
       </c>
       <c r="L50" t="n">
-        <v>772</v>
+        <v>822</v>
       </c>
       <c r="M50" t="n">
-        <v>1.428</v>
+        <v>1.521</v>
       </c>
       <c r="N50" t="s">
         <v>327</v>
@@ -4957,7 +4968,7 @@
         <v>331</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>43987</v>
+        <v>43989</v>
       </c>
       <c r="D51" t="s">
         <v>332</v>
@@ -4967,25 +4978,25 @@
       </c>
       <c r="F51"/>
       <c r="G51" t="n">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H51" t="n">
-        <v>284046</v>
+        <v>297963</v>
       </c>
       <c r="I51" t="n">
-        <v>2.203</v>
+        <v>2.311</v>
       </c>
       <c r="J51" t="n">
-        <v>285</v>
+        <v>222</v>
       </c>
       <c r="K51" t="n">
         <v>0.002</v>
       </c>
       <c r="L51" t="n">
-        <v>3651</v>
+        <v>4323</v>
       </c>
       <c r="M51" t="n">
-        <v>0.028</v>
+        <v>0.034</v>
       </c>
       <c r="N51" t="s">
         <v>333</v>
@@ -5061,7 +5072,7 @@
         <v>343</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>43987</v>
+        <v>43989</v>
       </c>
       <c r="D53" t="s">
         <v>344</v>
@@ -5071,25 +5082,25 @@
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H53" t="n">
-        <v>35432</v>
+        <v>39211</v>
       </c>
       <c r="I53" t="n">
-        <v>0.651</v>
+        <v>0.721</v>
       </c>
       <c r="J53" t="n">
-        <v>1845</v>
+        <v>1892</v>
       </c>
       <c r="K53" t="n">
-        <v>0.034</v>
+        <v>0.035</v>
       </c>
       <c r="L53" t="n">
-        <v>1574</v>
+        <v>1733</v>
       </c>
       <c r="M53" t="n">
-        <v>0.029</v>
+        <v>0.032</v>
       </c>
       <c r="N53" t="s">
         <v>345</v>
@@ -5112,7 +5123,7 @@
         <v>349</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>43988</v>
+        <v>43989</v>
       </c>
       <c r="D54" t="s">
         <v>350</v>
@@ -5124,25 +5135,25 @@
         <v>352</v>
       </c>
       <c r="G54" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H54" t="n">
-        <v>92477</v>
+        <v>96205</v>
       </c>
       <c r="I54" t="n">
-        <v>3.174</v>
+        <v>3.302</v>
       </c>
       <c r="J54" t="n">
-        <v>4111</v>
+        <v>3728</v>
       </c>
       <c r="K54" t="n">
-        <v>0.141</v>
+        <v>0.128</v>
       </c>
       <c r="L54" t="n">
-        <v>3678</v>
+        <v>3803</v>
       </c>
       <c r="M54" t="n">
-        <v>0.126</v>
+        <v>0.131</v>
       </c>
       <c r="N54" t="s">
         <v>351</v>
@@ -5165,7 +5176,7 @@
         <v>356</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>43986</v>
+        <v>43989</v>
       </c>
       <c r="D55" t="s">
         <v>357</v>
@@ -5175,25 +5186,21 @@
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H55" t="n">
-        <v>391624</v>
+        <v>414550</v>
       </c>
       <c r="I55" t="n">
-        <v>22.855</v>
-      </c>
-      <c r="J55" t="n">
-        <v>9855</v>
-      </c>
-      <c r="K55" t="n">
-        <v>0.575</v>
-      </c>
+        <v>24.193</v>
+      </c>
+      <c r="J55"/>
+      <c r="K55"/>
       <c r="L55" t="n">
-        <v>6294</v>
+        <v>7512</v>
       </c>
       <c r="M55" t="n">
-        <v>0.367</v>
+        <v>0.438</v>
       </c>
       <c r="N55" t="s">
         <v>359</v>
@@ -5216,7 +5223,7 @@
         <v>363</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>43988</v>
+        <v>43990</v>
       </c>
       <c r="D56" t="s">
         <v>364</v>
@@ -5226,25 +5233,25 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H56" t="n">
-        <v>294048</v>
+        <v>295901</v>
       </c>
       <c r="I56" t="n">
-        <v>60.978</v>
+        <v>61.362</v>
       </c>
       <c r="J56" t="n">
-        <v>2054</v>
+        <v>1053</v>
       </c>
       <c r="K56" t="n">
-        <v>0.426</v>
+        <v>0.218</v>
       </c>
       <c r="L56" t="n">
-        <v>1866</v>
+        <v>1948</v>
       </c>
       <c r="M56" t="n">
-        <v>0.387</v>
+        <v>0.404</v>
       </c>
       <c r="N56" t="s">
         <v>365</v>
@@ -5267,7 +5274,7 @@
         <v>368</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>43988</v>
+        <v>43991</v>
       </c>
       <c r="D57" t="s">
         <v>369</v>
@@ -5277,22 +5284,22 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H57" t="n">
-        <v>74999</v>
+        <v>79948</v>
       </c>
       <c r="I57" t="n">
-        <v>0.364</v>
+        <v>0.388</v>
       </c>
       <c r="J57" t="n">
-        <v>1935</v>
+        <v>1704</v>
       </c>
       <c r="K57" t="n">
-        <v>0.009</v>
+        <v>0.008</v>
       </c>
       <c r="L57" t="n">
-        <v>2025</v>
+        <v>2009</v>
       </c>
       <c r="M57" t="n">
         <v>0.01</v>
@@ -5318,7 +5325,7 @@
         <v>374</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>43987</v>
+        <v>43991</v>
       </c>
       <c r="D58" t="s">
         <v>375</v>
@@ -5328,25 +5335,25 @@
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H58" t="n">
-        <v>257303</v>
+        <v>264390</v>
       </c>
       <c r="I58" t="n">
-        <v>47.462</v>
+        <v>48.769</v>
       </c>
       <c r="J58" t="n">
-        <v>2590</v>
+        <v>2154</v>
       </c>
       <c r="K58" t="n">
-        <v>0.478</v>
+        <v>0.397</v>
       </c>
       <c r="L58" t="n">
-        <v>1707</v>
+        <v>1917</v>
       </c>
       <c r="M58" t="n">
-        <v>0.315</v>
+        <v>0.354</v>
       </c>
       <c r="N58" t="s">
         <v>376</v>
@@ -5369,7 +5376,7 @@
         <v>381</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D59" t="s">
         <v>382</v>
@@ -5379,25 +5386,25 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H59" t="n">
-        <v>683608</v>
+        <v>730453</v>
       </c>
       <c r="I59" t="n">
-        <v>3.095</v>
+        <v>3.307</v>
       </c>
       <c r="J59" t="n">
-        <v>23100</v>
+        <v>24620</v>
       </c>
       <c r="K59" t="n">
-        <v>0.105</v>
+        <v>0.111</v>
       </c>
       <c r="L59" t="n">
-        <v>19511</v>
+        <v>21783</v>
       </c>
       <c r="M59" t="n">
-        <v>0.088</v>
+        <v>0.099</v>
       </c>
       <c r="N59" t="s">
         <v>383</v>
@@ -5420,7 +5427,7 @@
         <v>387</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>43986</v>
+        <v>43990</v>
       </c>
       <c r="D60" t="s">
         <v>388</v>
@@ -5430,212 +5437,208 @@
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H60" t="n">
-        <v>70245</v>
+        <v>76713</v>
       </c>
       <c r="I60" t="n">
-        <v>16.28</v>
+        <v>17.779</v>
       </c>
       <c r="J60" t="n">
-        <v>1531</v>
+        <v>1656</v>
       </c>
       <c r="K60" t="n">
-        <v>0.355</v>
+        <v>0.384</v>
       </c>
       <c r="L60" t="n">
-        <v>1325</v>
+        <v>1493</v>
       </c>
       <c r="M60" t="n">
-        <v>0.307</v>
+        <v>0.346</v>
       </c>
       <c r="N60" t="s">
         <v>389</v>
       </c>
       <c r="O60" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="P60" t="s">
         <v>22</v>
       </c>
       <c r="Q60" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B61" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>43987</v>
+        <v>43989</v>
       </c>
       <c r="D61" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E61" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H61" t="n">
-        <v>35258</v>
+        <v>37532</v>
       </c>
       <c r="I61" t="n">
-        <v>4.943</v>
+        <v>5.262</v>
       </c>
       <c r="J61" t="n">
-        <v>1018</v>
+        <v>1159</v>
       </c>
       <c r="K61" t="n">
-        <v>0.143</v>
+        <v>0.162</v>
       </c>
       <c r="L61" t="n">
-        <v>989</v>
+        <v>1075</v>
       </c>
       <c r="M61" t="n">
-        <v>0.139</v>
+        <v>0.151</v>
       </c>
       <c r="N61" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="O61" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="P61" t="s">
         <v>51</v>
       </c>
       <c r="Q61" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B62" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>43988</v>
+        <v>43991</v>
       </c>
       <c r="D62" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E62" t="s">
         <v>41</v>
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H62" t="n">
-        <v>159169</v>
+        <v>171719</v>
       </c>
       <c r="I62" t="n">
-        <v>4.827</v>
-      </c>
-      <c r="J62" t="n">
-        <v>5396</v>
-      </c>
-      <c r="K62" t="n">
-        <v>0.164</v>
-      </c>
+        <v>5.208</v>
+      </c>
+      <c r="J62"/>
+      <c r="K62"/>
       <c r="L62" t="n">
-        <v>3087</v>
+        <v>3728</v>
       </c>
       <c r="M62" t="n">
-        <v>0.094</v>
+        <v>0.113</v>
       </c>
       <c r="N62" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="O62" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="P62" t="s">
         <v>92</v>
       </c>
       <c r="Q62" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B63" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>43987</v>
+        <v>43989</v>
       </c>
       <c r="D63" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E63" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="F63" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="G63" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H63" t="n">
-        <v>386726</v>
+        <v>406344</v>
       </c>
       <c r="I63" t="n">
-        <v>3.529</v>
+        <v>3.708</v>
       </c>
       <c r="J63" t="n">
-        <v>10385</v>
+        <v>10472</v>
       </c>
       <c r="K63" t="n">
-        <v>0.095</v>
+        <v>0.096</v>
       </c>
       <c r="L63" t="n">
-        <v>10603</v>
+        <v>11073</v>
       </c>
       <c r="M63" t="n">
-        <v>0.097</v>
+        <v>0.101</v>
       </c>
       <c r="N63" t="s">
         <v>214</v>
       </c>
       <c r="O63" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="P63" t="s">
         <v>92</v>
       </c>
       <c r="Q63" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B64" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>43985</v>
       </c>
       <c r="D64" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E64" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="F64" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="G64" t="n">
         <v>91</v>
@@ -5659,30 +5662,30 @@
         <v>0.538</v>
       </c>
       <c r="N64" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="O64" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="P64" t="s">
         <v>51</v>
       </c>
       <c r="Q64" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B65" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>43984</v>
       </c>
       <c r="D65" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E65" t="s">
         <v>41</v>
@@ -5710,391 +5713,391 @@
         <v>1.332</v>
       </c>
       <c r="N65" t="s">
+        <v>421</v>
+      </c>
+      <c r="O65" t="s">
         <v>420</v>
       </c>
-      <c r="O65" t="s">
-        <v>419</v>
-      </c>
       <c r="P65" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="Q65" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B66" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>43988</v>
+        <v>43991</v>
       </c>
       <c r="D66" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E66" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H66" t="n">
-        <v>251391</v>
+        <v>265035</v>
       </c>
       <c r="I66" t="n">
-        <v>87.256</v>
+        <v>91.992</v>
       </c>
       <c r="J66" t="n">
-        <v>5029</v>
+        <v>5389</v>
       </c>
       <c r="K66" t="n">
-        <v>1.746</v>
+        <v>1.87</v>
       </c>
       <c r="L66" t="n">
-        <v>4772</v>
+        <v>4848</v>
       </c>
       <c r="M66" t="n">
-        <v>1.656</v>
+        <v>1.683</v>
       </c>
       <c r="N66" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="O66" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="P66" t="s">
         <v>92</v>
       </c>
       <c r="Q66" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B67" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D67" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E67" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H67" t="n">
-        <v>503200</v>
+        <v>511295</v>
       </c>
       <c r="I67" t="n">
-        <v>26.157</v>
+        <v>26.578</v>
       </c>
       <c r="J67" t="n">
-        <v>6792</v>
+        <v>5180</v>
       </c>
       <c r="K67" t="n">
-        <v>0.353</v>
+        <v>0.269</v>
       </c>
       <c r="L67" t="n">
-        <v>9143</v>
+        <v>8567</v>
       </c>
       <c r="M67" t="n">
-        <v>0.475</v>
+        <v>0.445</v>
       </c>
       <c r="N67" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="O67" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="P67" t="s">
         <v>22</v>
       </c>
       <c r="Q67" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B68" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D68" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="E68" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H68" t="n">
-        <v>12721549</v>
+        <v>13254678</v>
       </c>
       <c r="I68" t="n">
-        <v>87.173</v>
+        <v>90.826</v>
       </c>
       <c r="J68" t="n">
-        <v>332581</v>
+        <v>238655</v>
       </c>
       <c r="K68" t="n">
-        <v>2.279</v>
+        <v>1.635</v>
       </c>
       <c r="L68" t="n">
-        <v>296918</v>
+        <v>300437</v>
       </c>
       <c r="M68" t="n">
-        <v>2.035</v>
+        <v>2.059</v>
       </c>
       <c r="N68" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="O68" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="P68" t="s">
         <v>22</v>
       </c>
       <c r="Q68" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B69" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>43987</v>
+        <v>43989</v>
       </c>
       <c r="D69" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E69" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H69" t="n">
-        <v>74068</v>
+        <v>76331</v>
       </c>
       <c r="I69" t="n">
-        <v>5.719</v>
+        <v>5.893</v>
       </c>
       <c r="J69" t="n">
-        <v>1558</v>
+        <v>1318</v>
       </c>
       <c r="K69" t="n">
-        <v>0.12</v>
+        <v>0.102</v>
       </c>
       <c r="L69" t="n">
-        <v>1209</v>
+        <v>1180</v>
       </c>
       <c r="M69" t="n">
-        <v>0.093</v>
+        <v>0.091</v>
       </c>
       <c r="N69" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="O69" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="P69" t="s">
         <v>51</v>
       </c>
       <c r="Q69" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B70" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>43988</v>
+        <v>43991</v>
       </c>
       <c r="D70" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E70" t="s">
         <v>41</v>
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H70" t="n">
-        <v>933201</v>
+        <v>997673</v>
       </c>
       <c r="I70" t="n">
-        <v>26.805</v>
+        <v>28.657</v>
       </c>
       <c r="J70" t="n">
-        <v>24229</v>
+        <v>20858</v>
       </c>
       <c r="K70" t="n">
-        <v>0.696</v>
+        <v>0.599</v>
       </c>
       <c r="L70" t="n">
-        <v>18090</v>
+        <v>20527</v>
       </c>
       <c r="M70" t="n">
-        <v>0.52</v>
+        <v>0.59</v>
       </c>
       <c r="N70" t="s">
         <v>41</v>
       </c>
       <c r="O70" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="P70" t="s">
         <v>127</v>
       </c>
       <c r="Q70" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B71" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>43988</v>
+        <v>43990</v>
       </c>
       <c r="D71" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E71" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="F71" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="G71" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H71" t="n">
-        <v>51856</v>
+        <v>54132</v>
       </c>
       <c r="I71" t="n">
-        <v>3.097</v>
+        <v>3.233</v>
       </c>
       <c r="J71" t="n">
-        <v>1166</v>
+        <v>1010</v>
       </c>
       <c r="K71" t="n">
-        <v>0.07</v>
+        <v>0.06</v>
       </c>
       <c r="L71" t="n">
-        <v>1420</v>
+        <v>1339</v>
       </c>
       <c r="M71" t="n">
-        <v>0.085</v>
+        <v>0.08</v>
       </c>
       <c r="N71" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="O71" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="P71" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="Q71" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B72" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>43988</v>
+        <v>43990</v>
       </c>
       <c r="D72" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E72" t="s">
         <v>41</v>
       </c>
       <c r="F72" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="G72" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H72" t="n">
-        <v>269185</v>
+        <v>276810</v>
       </c>
       <c r="I72" t="n">
-        <v>39.559</v>
+        <v>40.68</v>
       </c>
       <c r="J72" t="n">
-        <v>3124</v>
+        <v>4308</v>
       </c>
       <c r="K72" t="n">
-        <v>0.459</v>
+        <v>0.633</v>
       </c>
       <c r="L72" t="n">
-        <v>3772</v>
+        <v>4150</v>
       </c>
       <c r="M72" t="n">
-        <v>0.554</v>
+        <v>0.61</v>
       </c>
       <c r="N72" t="s">
         <v>41</v>
       </c>
       <c r="O72" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="P72" t="s">
         <v>92</v>
       </c>
       <c r="Q72" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B73" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>43983</v>
       </c>
       <c r="D73" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E73" t="s">
         <v>41</v>
@@ -6121,27 +6124,27 @@
         <v>41</v>
       </c>
       <c r="O73" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="P73" t="s">
         <v>92</v>
       </c>
       <c r="Q73" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B74" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>43983</v>
       </c>
       <c r="D74" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="E74" t="s">
         <v>41</v>
@@ -6168,381 +6171,381 @@
         <v>41</v>
       </c>
       <c r="O74" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="P74" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="Q74" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B75" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>43988</v>
+        <v>43991</v>
       </c>
       <c r="D75" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E75" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H75" t="n">
-        <v>188235</v>
+        <v>190426</v>
       </c>
       <c r="I75" t="n">
-        <v>34.478</v>
+        <v>34.879</v>
       </c>
       <c r="J75" t="n">
-        <v>2639</v>
+        <v>851</v>
       </c>
       <c r="K75" t="n">
-        <v>0.483</v>
+        <v>0.156</v>
       </c>
       <c r="L75" t="n">
-        <v>2463</v>
+        <v>1590</v>
       </c>
       <c r="M75" t="n">
-        <v>0.451</v>
+        <v>0.291</v>
       </c>
       <c r="N75" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="O75" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="P75" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="Q75" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B76" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>43987</v>
+        <v>43990</v>
       </c>
       <c r="D76" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E76" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H76" t="n">
-        <v>82876</v>
+        <v>84130</v>
       </c>
       <c r="I76" t="n">
-        <v>39.865</v>
+        <v>40.468</v>
       </c>
       <c r="J76" t="n">
-        <v>715</v>
+        <v>814</v>
       </c>
       <c r="K76" t="n">
-        <v>0.344</v>
+        <v>0.392</v>
       </c>
       <c r="L76" t="n">
-        <v>621</v>
+        <v>633</v>
       </c>
       <c r="M76" t="n">
-        <v>0.299</v>
+        <v>0.304</v>
       </c>
       <c r="N76" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="O76" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="P76" t="s">
         <v>22</v>
       </c>
       <c r="Q76" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B77" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>43988</v>
+        <v>43990</v>
       </c>
       <c r="D77" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E77" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F77" t="s">
+        <v>494</v>
+      </c>
+      <c r="G77" t="n">
+        <v>100</v>
+      </c>
+      <c r="H77" t="n">
+        <v>943059</v>
+      </c>
+      <c r="I77" t="n">
+        <v>15.901</v>
+      </c>
+      <c r="J77" t="n">
+        <v>22995</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0.388</v>
+      </c>
+      <c r="L77" t="n">
+        <v>28617</v>
+      </c>
+      <c r="M77" t="n">
+        <v>0.483</v>
+      </c>
+      <c r="N77" t="s">
         <v>493</v>
       </c>
-      <c r="G77" t="n">
-        <v>98</v>
-      </c>
-      <c r="H77" t="n">
-        <v>891668</v>
-      </c>
-      <c r="I77" t="n">
-        <v>15.034</v>
-      </c>
-      <c r="J77" t="n">
-        <v>40797</v>
-      </c>
-      <c r="K77" t="n">
-        <v>0.688</v>
-      </c>
-      <c r="L77" t="n">
-        <v>27112</v>
-      </c>
-      <c r="M77" t="n">
-        <v>0.457</v>
-      </c>
-      <c r="N77" t="s">
-        <v>492</v>
-      </c>
       <c r="O77" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="P77" t="s">
         <v>92</v>
       </c>
       <c r="Q77" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B78" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D78" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E78" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H78" t="n">
-        <v>1012769</v>
+        <v>1035997</v>
       </c>
       <c r="I78" t="n">
-        <v>19.754</v>
+        <v>20.207</v>
       </c>
       <c r="J78" t="n">
-        <v>7464</v>
+        <v>17783</v>
       </c>
       <c r="K78" t="n">
-        <v>0.146</v>
+        <v>0.347</v>
       </c>
       <c r="L78" t="n">
-        <v>14564</v>
+        <v>13735</v>
       </c>
       <c r="M78" t="n">
-        <v>0.284</v>
+        <v>0.268</v>
       </c>
       <c r="N78" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="O78" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="P78" t="s">
         <v>244</v>
       </c>
       <c r="Q78" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B79" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>43979</v>
+        <v>43986</v>
       </c>
       <c r="D79" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="E79" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H79" t="n">
-        <v>2536234</v>
+        <v>2822880</v>
       </c>
       <c r="I79" t="n">
-        <v>54.245</v>
+        <v>60.376</v>
       </c>
       <c r="J79"/>
       <c r="K79"/>
       <c r="L79" t="n">
-        <v>44962</v>
+        <v>40949</v>
       </c>
       <c r="M79" t="n">
-        <v>0.962</v>
+        <v>0.876</v>
       </c>
       <c r="N79" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="O79" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="P79" t="s">
         <v>22</v>
       </c>
       <c r="Q79" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B80" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>43982</v>
+        <v>43989</v>
       </c>
       <c r="D80" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="E80" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H80" t="n">
-        <v>275500</v>
+        <v>325000</v>
       </c>
       <c r="I80" t="n">
-        <v>27.279</v>
+        <v>32.181</v>
       </c>
       <c r="J80"/>
       <c r="K80"/>
       <c r="L80" t="n">
-        <v>5214</v>
+        <v>7029</v>
       </c>
       <c r="M80" t="n">
-        <v>0.516</v>
+        <v>0.696</v>
       </c>
       <c r="N80" t="s">
+        <v>513</v>
+      </c>
+      <c r="O80" t="s">
         <v>512</v>
-      </c>
-      <c r="O80" t="s">
-        <v>511</v>
       </c>
       <c r="P80" t="s">
         <v>92</v>
       </c>
       <c r="Q80" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B81" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>43988</v>
+        <v>43990</v>
       </c>
       <c r="D81" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E81" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H81" t="n">
-        <v>423468</v>
+        <v>428973</v>
       </c>
       <c r="I81" t="n">
-        <v>48.93</v>
+        <v>49.566</v>
       </c>
       <c r="J81" t="n">
-        <v>2530</v>
+        <v>3269</v>
       </c>
       <c r="K81" t="n">
-        <v>0.292</v>
+        <v>0.378</v>
       </c>
       <c r="L81" t="n">
-        <v>3607</v>
+        <v>3905</v>
       </c>
       <c r="M81" t="n">
-        <v>0.417</v>
+        <v>0.451</v>
       </c>
       <c r="N81" t="s">
+        <v>518</v>
+      </c>
+      <c r="O81" t="s">
         <v>517</v>
       </c>
-      <c r="O81" t="s">
-        <v>516</v>
-      </c>
       <c r="P81" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="Q81" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B82" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>43988</v>
       </c>
       <c r="D82" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E82" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
@@ -6567,133 +6570,133 @@
         <v>0.008</v>
       </c>
       <c r="N82" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="O82" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="P82" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="Q82" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B83" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>43988</v>
+        <v>43991</v>
       </c>
       <c r="D83" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="E83" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H83" t="n">
-        <v>228349</v>
+        <v>243464</v>
       </c>
       <c r="I83" t="n">
-        <v>3.271</v>
+        <v>3.488</v>
       </c>
       <c r="J83" t="n">
-        <v>3963</v>
+        <v>6523</v>
       </c>
       <c r="K83" t="n">
-        <v>0.057</v>
+        <v>0.093</v>
       </c>
       <c r="L83" t="n">
-        <v>5204</v>
+        <v>5110</v>
       </c>
       <c r="M83" t="n">
-        <v>0.075</v>
+        <v>0.073</v>
       </c>
       <c r="N83" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="O83" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="P83" t="s">
         <v>92</v>
       </c>
       <c r="Q83" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B84" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>43983</v>
+        <v>43987</v>
       </c>
       <c r="D84" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E84" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="F84" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="G84" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H84" t="n">
-        <v>420000</v>
+        <v>468000</v>
       </c>
       <c r="I84" t="n">
-        <v>6.017</v>
+        <v>6.705</v>
       </c>
       <c r="J84"/>
       <c r="K84"/>
       <c r="L84" t="n">
-        <v>4455</v>
+        <v>8766</v>
       </c>
       <c r="M84" t="n">
-        <v>0.064</v>
+        <v>0.126</v>
       </c>
       <c r="N84" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="O84" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="P84" t="s">
         <v>51</v>
       </c>
       <c r="Q84" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B85" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C85" s="1" t="n">
         <v>43983</v>
       </c>
       <c r="D85" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E85" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
@@ -6714,188 +6717,188 @@
         <v>0.049</v>
       </c>
       <c r="N85" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="O85" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="P85" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="Q85" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B86" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>43988</v>
+        <v>43991</v>
       </c>
       <c r="D86" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="E86" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H86" t="n">
-        <v>2303258</v>
+        <v>2415179</v>
       </c>
       <c r="I86" t="n">
-        <v>27.31</v>
+        <v>28.637</v>
       </c>
       <c r="J86" t="n">
-        <v>35846</v>
+        <v>37225</v>
       </c>
       <c r="K86" t="n">
-        <v>0.425</v>
+        <v>0.441</v>
       </c>
       <c r="L86" t="n">
-        <v>42809</v>
+        <v>44591</v>
       </c>
       <c r="M86" t="n">
-        <v>0.508</v>
+        <v>0.529</v>
       </c>
       <c r="N86" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="O86" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="P86" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="Q86" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B87" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>43987</v>
+        <v>43990</v>
       </c>
       <c r="D87" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="E87" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="F87" t="s">
+        <v>559</v>
+      </c>
+      <c r="G87" t="n">
+        <v>61</v>
+      </c>
+      <c r="H87" t="n">
+        <v>112678</v>
+      </c>
+      <c r="I87" t="n">
+        <v>2.463</v>
+      </c>
+      <c r="J87" t="n">
+        <v>2336</v>
+      </c>
+      <c r="K87" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="L87" t="n">
+        <v>1893</v>
+      </c>
+      <c r="M87" t="n">
+        <v>0.041</v>
+      </c>
+      <c r="N87" t="s">
         <v>558</v>
       </c>
-      <c r="G87" t="n">
-        <v>58</v>
-      </c>
-      <c r="H87" t="n">
-        <v>104090</v>
-      </c>
-      <c r="I87" t="n">
-        <v>2.276</v>
-      </c>
-      <c r="J87" t="n">
-        <v>1310</v>
-      </c>
-      <c r="K87" t="n">
-        <v>0.029</v>
-      </c>
-      <c r="L87" t="n">
-        <v>1434</v>
-      </c>
-      <c r="M87" t="n">
-        <v>0.031</v>
-      </c>
-      <c r="N87" t="s">
-        <v>557</v>
-      </c>
       <c r="O87" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="P87" t="s">
         <v>51</v>
       </c>
       <c r="Q87" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B88" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D88" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="E88" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H88" t="n">
-        <v>424046</v>
+        <v>437444</v>
       </c>
       <c r="I88" t="n">
-        <v>9.696</v>
+        <v>10.002</v>
       </c>
       <c r="J88" t="n">
-        <v>9504</v>
+        <v>6359</v>
       </c>
       <c r="K88" t="n">
-        <v>0.217</v>
+        <v>0.145</v>
       </c>
       <c r="L88" t="n">
-        <v>10259</v>
+        <v>9397</v>
       </c>
       <c r="M88" t="n">
-        <v>0.235</v>
+        <v>0.215</v>
       </c>
       <c r="N88" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="O88" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="P88" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="Q88" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B89" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C89" s="1" t="n">
         <v>43973</v>
       </c>
       <c r="D89" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E89" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
@@ -6920,239 +6923,235 @@
         <v>1.012</v>
       </c>
       <c r="N89" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="O89" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="P89" t="s">
         <v>92</v>
       </c>
       <c r="Q89" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B90" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>43987</v>
+        <v>43990</v>
       </c>
       <c r="D90" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="E90" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="F90" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="G90" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H90" t="n">
-        <v>3250401</v>
+        <v>3477545</v>
       </c>
       <c r="I90" t="n">
-        <v>47.88</v>
+        <v>51.226</v>
       </c>
       <c r="J90" t="n">
-        <v>82389</v>
+        <v>45981</v>
       </c>
       <c r="K90" t="n">
-        <v>1.214</v>
+        <v>0.677</v>
       </c>
       <c r="L90" t="n">
-        <v>69249</v>
+        <v>76628</v>
       </c>
       <c r="M90" t="n">
-        <v>1.02</v>
+        <v>1.129</v>
       </c>
       <c r="N90" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="O90" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="P90" t="s">
         <v>22</v>
       </c>
       <c r="Q90" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B91" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>43987</v>
+        <v>43990</v>
       </c>
       <c r="D91" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="E91" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H91" t="n">
-        <v>20384850</v>
+        <v>20814269</v>
       </c>
       <c r="I91" t="n">
-        <v>61.585</v>
-      </c>
-      <c r="J91" t="n">
-        <v>573607</v>
-      </c>
-      <c r="K91" t="n">
-        <v>1.733</v>
-      </c>
+        <v>62.882</v>
+      </c>
+      <c r="J91"/>
+      <c r="K91"/>
       <c r="L91" t="n">
-        <v>512953</v>
+        <v>457449</v>
       </c>
       <c r="M91" t="n">
-        <v>1.55</v>
+        <v>1.382</v>
       </c>
       <c r="N91" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="O91" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="P91" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="Q91" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B92" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>43988</v>
+        <v>43990</v>
       </c>
       <c r="D92" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="E92" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H92" t="n">
-        <v>19778873</v>
+        <v>20615303</v>
       </c>
       <c r="I92" t="n">
-        <v>59.754</v>
+        <v>62.281</v>
       </c>
       <c r="J92" t="n">
-        <v>547429</v>
+        <v>379625</v>
       </c>
       <c r="K92" t="n">
-        <v>1.654</v>
+        <v>1.147</v>
       </c>
       <c r="L92" t="n">
-        <v>464027</v>
+        <v>464453</v>
       </c>
       <c r="M92" t="n">
-        <v>1.402</v>
+        <v>1.403</v>
       </c>
       <c r="N92" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="O92" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="P92" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q92" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B93" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D93" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="E93" t="s">
         <v>124</v>
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H93" t="n">
-        <v>48029</v>
+        <v>48896</v>
       </c>
       <c r="I93" t="n">
-        <v>13.826</v>
+        <v>14.076</v>
       </c>
       <c r="J93" t="n">
-        <v>596</v>
+        <v>464</v>
       </c>
       <c r="K93" t="n">
-        <v>0.172</v>
+        <v>0.134</v>
       </c>
       <c r="L93" t="n">
-        <v>650</v>
+        <v>626</v>
       </c>
       <c r="M93" t="n">
-        <v>0.187</v>
+        <v>0.18</v>
       </c>
       <c r="N93" t="s">
         <v>124</v>
       </c>
       <c r="O93" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="P93" t="s">
         <v>22</v>
       </c>
       <c r="Q93" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B94" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C94" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="D94" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="E94" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="F94"/>
       <c r="G94" t="n">
@@ -7173,67 +7172,67 @@
         <v>0.112</v>
       </c>
       <c r="N94" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="O94" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="P94" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="Q94" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B95" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>43987</v>
+        <v>43988</v>
       </c>
       <c r="D95" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="E95" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H95" t="n">
-        <v>21000</v>
+        <v>21354</v>
       </c>
       <c r="I95" t="n">
-        <v>1.413</v>
+        <v>1.437</v>
       </c>
       <c r="J95" t="n">
-        <v>598</v>
+        <v>354</v>
       </c>
       <c r="K95" t="n">
-        <v>0.04</v>
+        <v>0.024</v>
       </c>
       <c r="L95" t="n">
-        <v>591</v>
+        <v>547</v>
       </c>
       <c r="M95" t="n">
-        <v>0.04</v>
+        <v>0.037</v>
       </c>
       <c r="N95" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="O95" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="P95" t="s">
         <v>22</v>
       </c>
       <c r="Q95" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>